<commit_message>
Registree stats backup on Tue 13 Apr 2021 21:20:48 SAST
</commit_message>
<xml_diff>
--- a/static/docs/registrees_list.xlsx
+++ b/static/docs/registrees_list.xlsx
@@ -451,7 +451,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>MD410 Registrees as of 13/04/2021 18:59</t>
+          <t>MD410 Registrees as of 13/04/2021 21:20</t>
         </is>
       </c>
     </row>
@@ -7795,7 +7795,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Registrees as of 13/04/2021 18:59</t>
+          <t>410E Registrees as of 13/04/2021 21:20</t>
         </is>
       </c>
     </row>
@@ -11029,7 +11029,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Registrees as of 13/04/2021 18:59</t>
+          <t>410W Registrees as of 13/04/2021 21:20</t>
         </is>
       </c>
     </row>
@@ -15097,7 +15097,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Voting details as of 13/04/2021 18:59</t>
+          <t>410E Voting details as of 13/04/2021 21:20</t>
         </is>
       </c>
     </row>
@@ -15434,7 +15434,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Voting details as of 13/04/2021 18:59</t>
+          <t>410W Voting details as of 13/04/2021 21:20</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Registree stats backup on Tue 13 Apr 2021 21:27:29 SAST
</commit_message>
<xml_diff>
--- a/static/docs/registrees_list.xlsx
+++ b/static/docs/registrees_list.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F231"/>
+  <dimension ref="A1:F232"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,7 +451,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>MD410 Registrees as of 13/04/2021 21:20</t>
+          <t>MD410 Registrees as of 13/04/2021 21:27</t>
         </is>
       </c>
     </row>
@@ -3306,22 +3306,22 @@
     <row r="91" ht="25" customHeight="1">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>Kienast</t>
+          <t>Khoza</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
         <is>
-          <t>Margie</t>
+          <t>Faniso</t>
         </is>
       </c>
       <c r="C91" s="3" t="inlineStr">
         <is>
-          <t>Edenvale</t>
+          <t>The Wilds</t>
         </is>
       </c>
       <c r="D91" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E91" s="3" t="inlineStr">
@@ -3338,17 +3338,17 @@
     <row r="92" ht="25" customHeight="1">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>Kimari</t>
+          <t>Kienast</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
         <is>
-          <t>Joyce</t>
+          <t>Margie</t>
         </is>
       </c>
       <c r="C92" s="3" t="inlineStr">
         <is>
-          <t>Eden</t>
+          <t>Edenvale</t>
         </is>
       </c>
       <c r="D92" s="3" t="inlineStr">
@@ -3370,17 +3370,17 @@
     <row r="93" ht="25" customHeight="1">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>King</t>
+          <t>Kimari</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
         <is>
-          <t>Ian</t>
+          <t>Joyce</t>
         </is>
       </c>
       <c r="C93" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Eden</t>
         </is>
       </c>
       <c r="D93" s="3" t="inlineStr">
@@ -3390,7 +3390,7 @@
       </c>
       <c r="E93" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F93" s="3" t="inlineStr">
@@ -3407,7 +3407,7 @@
       </c>
       <c r="B94" s="3" t="inlineStr">
         <is>
-          <t>Sandy</t>
+          <t>Ian</t>
         </is>
       </c>
       <c r="C94" s="3" t="inlineStr">
@@ -3434,17 +3434,17 @@
     <row r="95" ht="25" customHeight="1">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>Koekemoer</t>
+          <t>King</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
         <is>
-          <t>Christa</t>
+          <t>Sandy</t>
         </is>
       </c>
       <c r="C95" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D95" s="3" t="inlineStr">
@@ -3454,7 +3454,7 @@
       </c>
       <c r="E95" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F95" s="3" t="inlineStr">
@@ -3466,22 +3466,22 @@
     <row r="96" ht="25" customHeight="1">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>Koloko</t>
+          <t>Koekemoer</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
         <is>
-          <t>Muya</t>
+          <t>Christa</t>
         </is>
       </c>
       <c r="C96" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D96" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E96" s="3" t="inlineStr">
@@ -3491,34 +3491,34 @@
       </c>
       <c r="F96" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="97" ht="25" customHeight="1">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>Kruger</t>
+          <t>Koloko</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
         <is>
-          <t>Zwaai</t>
+          <t>Muya</t>
         </is>
       </c>
       <c r="C97" s="3" t="inlineStr">
         <is>
-          <t>Sedgefield</t>
+          <t>Durbanville</t>
         </is>
       </c>
       <c r="D97" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E97" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F97" s="3" t="inlineStr">
@@ -3530,17 +3530,17 @@
     <row r="98" ht="25" customHeight="1">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>Laas</t>
+          <t>Kruger</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
         <is>
-          <t>Natalie</t>
+          <t>Zwaai</t>
         </is>
       </c>
       <c r="C98" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Sedgefield</t>
         </is>
       </c>
       <c r="D98" s="3" t="inlineStr">
@@ -3550,29 +3550,29 @@
       </c>
       <c r="E98" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F98" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="99" ht="25" customHeight="1">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>Lakay</t>
+          <t>Laas</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
         <is>
-          <t>Bevil</t>
+          <t>Natalie</t>
         </is>
       </c>
       <c r="C99" s="3" t="inlineStr">
         <is>
-          <t>Mitchells Plain</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D99" s="3" t="inlineStr">
@@ -3582,29 +3582,29 @@
       </c>
       <c r="E99" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F99" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="100" ht="25" customHeight="1">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>Lang</t>
+          <t>Lakay</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
         <is>
-          <t>Paula</t>
+          <t>Bevil</t>
         </is>
       </c>
       <c r="C100" s="3" t="inlineStr">
         <is>
-          <t>Gordons Bay</t>
+          <t>Mitchells Plain</t>
         </is>
       </c>
       <c r="D100" s="3" t="inlineStr">
@@ -3631,7 +3631,7 @@
       </c>
       <c r="B101" s="3" t="inlineStr">
         <is>
-          <t>Jimmy</t>
+          <t>Paula</t>
         </is>
       </c>
       <c r="C101" s="3" t="inlineStr">
@@ -3646,7 +3646,7 @@
       </c>
       <c r="E101" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F101" s="3" t="inlineStr">
@@ -3658,22 +3658,22 @@
     <row r="102" ht="25" customHeight="1">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>Langton</t>
+          <t>Lang</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
         <is>
-          <t>Evelyn May</t>
+          <t>Jimmy</t>
         </is>
       </c>
       <c r="C102" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Gordons Bay</t>
         </is>
       </c>
       <c r="D102" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E102" s="3" t="inlineStr">
@@ -3683,29 +3683,29 @@
       </c>
       <c r="F102" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="103" ht="25" customHeight="1">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>Laubscher</t>
+          <t>Langton</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
         <is>
-          <t>Herman</t>
+          <t>Evelyn May</t>
         </is>
       </c>
       <c r="C103" s="3" t="inlineStr">
         <is>
-          <t>Ceres</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D103" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E103" s="3" t="inlineStr">
@@ -3715,24 +3715,24 @@
       </c>
       <c r="F103" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="104" ht="25" customHeight="1">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>Lautenbach</t>
+          <t>Laubscher</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
         <is>
-          <t>Steven</t>
+          <t>Herman</t>
         </is>
       </c>
       <c r="C104" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Ceres</t>
         </is>
       </c>
       <c r="D104" s="3" t="inlineStr">
@@ -3742,29 +3742,29 @@
       </c>
       <c r="E104" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F104" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="105" ht="25" customHeight="1">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>Lee</t>
+          <t>Lautenbach</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
         <is>
-          <t>Heather</t>
+          <t>Steven</t>
         </is>
       </c>
       <c r="C105" s="3" t="inlineStr">
         <is>
-          <t>Cape Of Good Hope</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D105" s="3" t="inlineStr">
@@ -3779,24 +3779,24 @@
       </c>
       <c r="F105" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="106" ht="25" customHeight="1">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>Logan</t>
+          <t>Lee</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
         <is>
-          <t>Graeme</t>
+          <t>Heather</t>
         </is>
       </c>
       <c r="C106" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Cape Of Good Hope</t>
         </is>
       </c>
       <c r="D106" s="3" t="inlineStr">
@@ -3806,34 +3806,34 @@
       </c>
       <c r="E106" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F106" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="107" ht="25" customHeight="1">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>Louw</t>
+          <t>Logan</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
         <is>
-          <t>Erika</t>
+          <t>Graeme</t>
         </is>
       </c>
       <c r="C107" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D107" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E107" s="3" t="inlineStr">
@@ -3843,29 +3843,29 @@
       </c>
       <c r="F107" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="108" ht="25" customHeight="1">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>Love</t>
+          <t>Louw</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
         <is>
-          <t>Dee</t>
+          <t>Erika</t>
         </is>
       </c>
       <c r="C108" s="3" t="inlineStr">
         <is>
-          <t>Cowies Hill</t>
+          <t>Durbanville</t>
         </is>
       </c>
       <c r="D108" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E108" s="3" t="inlineStr">
@@ -3875,24 +3875,24 @@
       </c>
       <c r="F108" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="109" ht="25" customHeight="1">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>Lucas</t>
+          <t>Love</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
         <is>
-          <t>Rashmiya</t>
+          <t>Dee</t>
         </is>
       </c>
       <c r="C109" s="3" t="inlineStr">
         <is>
-          <t>Mitchells Plain</t>
+          <t>Cowies Hill</t>
         </is>
       </c>
       <c r="D109" s="3" t="inlineStr">
@@ -3907,24 +3907,24 @@
       </c>
       <c r="F109" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="110" ht="25" customHeight="1">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>Luck</t>
+          <t>Lucas</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
         <is>
-          <t>Zarina</t>
+          <t>Rashmiya</t>
         </is>
       </c>
       <c r="C110" s="3" t="inlineStr">
         <is>
-          <t>Newcastle</t>
+          <t>Mitchells Plain</t>
         </is>
       </c>
       <c r="D110" s="3" t="inlineStr">
@@ -3939,29 +3939,29 @@
       </c>
       <c r="F110" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="111" ht="25" customHeight="1">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>MARCHANT</t>
+          <t>Luck</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
         <is>
-          <t>Richard</t>
+          <t>Zarina</t>
         </is>
       </c>
       <c r="C111" s="3" t="inlineStr">
         <is>
-          <t>The Wilds</t>
+          <t>Newcastle</t>
         </is>
       </c>
       <c r="D111" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E111" s="3" t="inlineStr">
@@ -3978,22 +3978,22 @@
     <row r="112" ht="25" customHeight="1">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>MAYTHAM</t>
+          <t>MARCHANT</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
         <is>
-          <t>LANCE</t>
+          <t>Richard</t>
         </is>
       </c>
       <c r="C112" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>The Wilds</t>
         </is>
       </c>
       <c r="D112" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E112" s="3" t="inlineStr">
@@ -4003,7 +4003,7 @@
       </c>
       <c r="F112" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -4015,7 +4015,7 @@
       </c>
       <c r="B113" s="3" t="inlineStr">
         <is>
-          <t>ROSEMARIE</t>
+          <t>LANCE</t>
         </is>
       </c>
       <c r="C113" s="3" t="inlineStr">
@@ -4042,17 +4042,17 @@
     <row r="114" ht="25" customHeight="1">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>MILLS</t>
+          <t>MAYTHAM</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
         <is>
-          <t>BERNICE</t>
+          <t>ROSEMARIE</t>
         </is>
       </c>
       <c r="C114" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D114" s="3" t="inlineStr">
@@ -4062,29 +4062,29 @@
       </c>
       <c r="E114" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F114" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="115" ht="25" customHeight="1">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>MacRobert</t>
+          <t>MILLS</t>
         </is>
       </c>
       <c r="B115" s="3" t="inlineStr">
         <is>
-          <t>Pam</t>
+          <t>BERNICE</t>
         </is>
       </c>
       <c r="C115" s="3" t="inlineStr">
         <is>
-          <t>Groote Schuur</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D115" s="3" t="inlineStr">
@@ -4094,39 +4094,39 @@
       </c>
       <c r="E115" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F115" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="116" ht="25" customHeight="1">
       <c r="A116" s="3" t="inlineStr">
         <is>
-          <t>Mangwende</t>
+          <t>MacRobert</t>
         </is>
       </c>
       <c r="B116" s="3" t="inlineStr">
         <is>
-          <t>Sharon</t>
+          <t>Pam</t>
         </is>
       </c>
       <c r="C116" s="3" t="inlineStr">
         <is>
-          <t>Cape Town</t>
+          <t>Groote Schuur</t>
         </is>
       </c>
       <c r="D116" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E116" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F116" s="3" t="inlineStr">
@@ -4138,22 +4138,22 @@
     <row r="117" ht="25" customHeight="1">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>Mare</t>
+          <t>Mangwende</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
         <is>
-          <t>Beaulieu</t>
+          <t>Sharon</t>
         </is>
       </c>
       <c r="C117" s="3" t="inlineStr">
         <is>
-          <t>Benoni Lakes</t>
+          <t>Cape Town</t>
         </is>
       </c>
       <c r="D117" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E117" s="3" t="inlineStr">
@@ -4163,19 +4163,19 @@
       </c>
       <c r="F117" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="118" ht="25" customHeight="1">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>Maré</t>
+          <t>Mare</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
         <is>
-          <t>Nick</t>
+          <t>Beaulieu</t>
         </is>
       </c>
       <c r="C118" s="3" t="inlineStr">
@@ -4190,7 +4190,7 @@
       </c>
       <c r="E118" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F118" s="3" t="inlineStr">
@@ -4202,17 +4202,17 @@
     <row r="119" ht="25" customHeight="1">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>McDonald</t>
+          <t>Maré</t>
         </is>
       </c>
       <c r="B119" s="3" t="inlineStr">
         <is>
-          <t>Rochelle</t>
+          <t>Nick</t>
         </is>
       </c>
       <c r="C119" s="3" t="inlineStr">
         <is>
-          <t>Vereeniging</t>
+          <t>Benoni Lakes</t>
         </is>
       </c>
       <c r="D119" s="3" t="inlineStr">
@@ -4222,7 +4222,7 @@
       </c>
       <c r="E119" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F119" s="3" t="inlineStr">
@@ -4234,17 +4234,17 @@
     <row r="120" ht="25" customHeight="1">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>McPherson</t>
+          <t>McDonald</t>
         </is>
       </c>
       <c r="B120" s="3" t="inlineStr">
         <is>
-          <t>Stuart</t>
+          <t>Rochelle</t>
         </is>
       </c>
       <c r="C120" s="3" t="inlineStr">
         <is>
-          <t>Newlands</t>
+          <t>Vereeniging</t>
         </is>
       </c>
       <c r="D120" s="3" t="inlineStr">
@@ -4259,24 +4259,24 @@
       </c>
       <c r="F120" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="121" ht="25" customHeight="1">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>Mccullough</t>
+          <t>McPherson</t>
         </is>
       </c>
       <c r="B121" s="3" t="inlineStr">
         <is>
-          <t>David</t>
+          <t>Stuart</t>
         </is>
       </c>
       <c r="C121" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Newlands</t>
         </is>
       </c>
       <c r="D121" s="3" t="inlineStr">
@@ -4286,29 +4286,29 @@
       </c>
       <c r="E121" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F121" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="122" ht="25" customHeight="1">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>Meyer</t>
+          <t>Mccullough</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
         <is>
-          <t>Denis</t>
+          <t>David</t>
         </is>
       </c>
       <c r="C122" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D122" s="3" t="inlineStr">
@@ -4318,7 +4318,7 @@
       </c>
       <c r="E122" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F122" s="3" t="inlineStr">
@@ -4330,17 +4330,17 @@
     <row r="123" ht="25" customHeight="1">
       <c r="A123" s="3" t="inlineStr">
         <is>
-          <t>Michas</t>
+          <t>Meyer</t>
         </is>
       </c>
       <c r="B123" s="3" t="inlineStr">
         <is>
-          <t>Roy</t>
+          <t>Denis</t>
         </is>
       </c>
       <c r="C123" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D123" s="3" t="inlineStr">
@@ -4367,7 +4367,7 @@
       </c>
       <c r="B124" s="3" t="inlineStr">
         <is>
-          <t>Dawn</t>
+          <t>Roy</t>
         </is>
       </c>
       <c r="C124" s="3" t="inlineStr">
@@ -4382,7 +4382,7 @@
       </c>
       <c r="E124" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F124" s="3" t="inlineStr">
@@ -4394,17 +4394,17 @@
     <row r="125" ht="25" customHeight="1">
       <c r="A125" s="3" t="inlineStr">
         <is>
-          <t>Mills</t>
+          <t>Michas</t>
         </is>
       </c>
       <c r="B125" s="3" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>Dawn</t>
         </is>
       </c>
       <c r="C125" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D125" s="3" t="inlineStr">
@@ -4414,7 +4414,7 @@
       </c>
       <c r="E125" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F125" s="3" t="inlineStr">
@@ -4426,17 +4426,17 @@
     <row r="126" ht="25" customHeight="1">
       <c r="A126" s="3" t="inlineStr">
         <is>
-          <t>Mitchell</t>
+          <t>Mills</t>
         </is>
       </c>
       <c r="B126" s="3" t="inlineStr">
         <is>
-          <t>Alana</t>
+          <t>Patrick</t>
         </is>
       </c>
       <c r="C126" s="3" t="inlineStr">
         <is>
-          <t>Rustenburg</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D126" s="3" t="inlineStr">
@@ -4446,7 +4446,7 @@
       </c>
       <c r="E126" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F126" s="3" t="inlineStr">
@@ -4463,7 +4463,7 @@
       </c>
       <c r="B127" s="3" t="inlineStr">
         <is>
-          <t>Juan</t>
+          <t>Alana</t>
         </is>
       </c>
       <c r="C127" s="3" t="inlineStr">
@@ -4478,7 +4478,7 @@
       </c>
       <c r="E127" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F127" s="3" t="inlineStr">
@@ -4490,17 +4490,17 @@
     <row r="128" ht="25" customHeight="1">
       <c r="A128" s="3" t="inlineStr">
         <is>
-          <t>Mkhize</t>
+          <t>Mitchell</t>
         </is>
       </c>
       <c r="B128" s="3" t="inlineStr">
         <is>
-          <t>Virginia</t>
+          <t>Juan</t>
         </is>
       </c>
       <c r="C128" s="3" t="inlineStr">
         <is>
-          <t>Cape Town</t>
+          <t>Rustenburg</t>
         </is>
       </c>
       <c r="D128" s="3" t="inlineStr">
@@ -4510,39 +4510,39 @@
       </c>
       <c r="E128" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F128" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="129" ht="25" customHeight="1">
       <c r="A129" s="3" t="inlineStr">
         <is>
-          <t>Moeller</t>
+          <t>Mkhize</t>
         </is>
       </c>
       <c r="B129" s="3" t="inlineStr">
         <is>
-          <t>Frauke E.</t>
+          <t>Virginia</t>
         </is>
       </c>
       <c r="C129" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Cape Town</t>
         </is>
       </c>
       <c r="D129" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E129" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F129" s="3" t="inlineStr">
@@ -4554,27 +4554,27 @@
     <row r="130" ht="25" customHeight="1">
       <c r="A130" s="3" t="inlineStr">
         <is>
-          <t>Moses</t>
+          <t>Moeller</t>
         </is>
       </c>
       <c r="B130" s="3" t="inlineStr">
         <is>
-          <t>Bernadine</t>
+          <t>Frauke E.</t>
         </is>
       </c>
       <c r="C130" s="3" t="inlineStr">
         <is>
-          <t>Cape Town</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D130" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E130" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F130" s="3" t="inlineStr">
@@ -4586,27 +4586,27 @@
     <row r="131" ht="25" customHeight="1">
       <c r="A131" s="3" t="inlineStr">
         <is>
-          <t>Mostert</t>
+          <t>Moses</t>
         </is>
       </c>
       <c r="B131" s="3" t="inlineStr">
         <is>
-          <t>Jacques</t>
+          <t>Bernadine</t>
         </is>
       </c>
       <c r="C131" s="3" t="inlineStr">
         <is>
-          <t>Merriman</t>
+          <t>Cape Town</t>
         </is>
       </c>
       <c r="D131" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E131" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F131" s="3" t="inlineStr">
@@ -4618,22 +4618,22 @@
     <row r="132" ht="25" customHeight="1">
       <c r="A132" s="3" t="inlineStr">
         <is>
-          <t>Murray</t>
+          <t>Mostert</t>
         </is>
       </c>
       <c r="B132" s="3" t="inlineStr">
         <is>
-          <t>Suzanne</t>
+          <t>Jacques</t>
         </is>
       </c>
       <c r="C132" s="3" t="inlineStr">
         <is>
-          <t>Vereeniging</t>
+          <t>Merriman</t>
         </is>
       </c>
       <c r="D132" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E132" s="3" t="inlineStr">
@@ -4643,7 +4643,7 @@
       </c>
       <c r="F132" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -4655,7 +4655,7 @@
       </c>
       <c r="B133" s="3" t="inlineStr">
         <is>
-          <t>Gary</t>
+          <t>Suzanne</t>
         </is>
       </c>
       <c r="C133" s="3" t="inlineStr">
@@ -4682,17 +4682,17 @@
     <row r="134" ht="25" customHeight="1">
       <c r="A134" s="3" t="inlineStr">
         <is>
-          <t>Myburg</t>
+          <t>Murray</t>
         </is>
       </c>
       <c r="B134" s="3" t="inlineStr">
         <is>
-          <t>Pieter</t>
+          <t>Gary</t>
         </is>
       </c>
       <c r="C134" s="3" t="inlineStr">
         <is>
-          <t>Wellington</t>
+          <t>Vereeniging</t>
         </is>
       </c>
       <c r="D134" s="3" t="inlineStr">
@@ -4707,71 +4707,71 @@
       </c>
       <c r="F134" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="135" ht="25" customHeight="1">
       <c r="A135" s="3" t="inlineStr">
         <is>
-          <t>Naude</t>
+          <t>Myburg</t>
         </is>
       </c>
       <c r="B135" s="3" t="inlineStr">
         <is>
-          <t>Cornette</t>
+          <t>Pieter</t>
         </is>
       </c>
       <c r="C135" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Wellington</t>
         </is>
       </c>
       <c r="D135" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E135" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F135" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="136" ht="25" customHeight="1">
       <c r="A136" s="3" t="inlineStr">
         <is>
-          <t>Nel</t>
+          <t>Naude</t>
         </is>
       </c>
       <c r="B136" s="3" t="inlineStr">
         <is>
-          <t>Pieter</t>
+          <t>Cornette</t>
         </is>
       </c>
       <c r="C136" s="3" t="inlineStr">
         <is>
-          <t>George</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D136" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E136" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F136" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -4783,12 +4783,12 @@
       </c>
       <c r="B137" s="3" t="inlineStr">
         <is>
-          <t>Tillie</t>
+          <t>Pieter</t>
         </is>
       </c>
       <c r="C137" s="3" t="inlineStr">
         <is>
-          <t>Eden</t>
+          <t>George</t>
         </is>
       </c>
       <c r="D137" s="3" t="inlineStr">
@@ -4810,17 +4810,17 @@
     <row r="138" ht="25" customHeight="1">
       <c r="A138" s="3" t="inlineStr">
         <is>
-          <t>Newlands</t>
+          <t>Nel</t>
         </is>
       </c>
       <c r="B138" s="3" t="inlineStr">
         <is>
-          <t>Mike</t>
+          <t>Tillie</t>
         </is>
       </c>
       <c r="C138" s="3" t="inlineStr">
         <is>
-          <t>Port Alfred</t>
+          <t>Eden</t>
         </is>
       </c>
       <c r="D138" s="3" t="inlineStr">
@@ -4835,24 +4835,24 @@
       </c>
       <c r="F138" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="139" ht="25" customHeight="1">
       <c r="A139" s="3" t="inlineStr">
         <is>
-          <t>Niehaus</t>
+          <t>Newlands</t>
         </is>
       </c>
       <c r="B139" s="3" t="inlineStr">
         <is>
-          <t>Angela</t>
+          <t>Mike</t>
         </is>
       </c>
       <c r="C139" s="3" t="inlineStr">
         <is>
-          <t>Bergvliet</t>
+          <t>Port Alfred</t>
         </is>
       </c>
       <c r="D139" s="3" t="inlineStr">
@@ -4867,24 +4867,24 @@
       </c>
       <c r="F139" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="140" ht="25" customHeight="1">
       <c r="A140" s="3" t="inlineStr">
         <is>
-          <t>Oberholzer</t>
+          <t>Niehaus</t>
         </is>
       </c>
       <c r="B140" s="3" t="inlineStr">
         <is>
-          <t>PDG Bokkie</t>
+          <t>Angela</t>
         </is>
       </c>
       <c r="C140" s="3" t="inlineStr">
         <is>
-          <t>Uitenhage</t>
+          <t>Bergvliet</t>
         </is>
       </c>
       <c r="D140" s="3" t="inlineStr">
@@ -4899,24 +4899,24 @@
       </c>
       <c r="F140" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="141" ht="25" customHeight="1">
       <c r="A141" s="3" t="inlineStr">
         <is>
-          <t>PORTEOUS</t>
+          <t>Oberholzer</t>
         </is>
       </c>
       <c r="B141" s="3" t="inlineStr">
         <is>
-          <t>BRIAN</t>
+          <t>PDG Bokkie</t>
         </is>
       </c>
       <c r="C141" s="3" t="inlineStr">
         <is>
-          <t>Hibberdene</t>
+          <t>Uitenhage</t>
         </is>
       </c>
       <c r="D141" s="3" t="inlineStr">
@@ -4938,17 +4938,17 @@
     <row r="142" ht="25" customHeight="1">
       <c r="A142" s="3" t="inlineStr">
         <is>
-          <t>Pantoleon</t>
+          <t>PORTEOUS</t>
         </is>
       </c>
       <c r="B142" s="3" t="inlineStr">
         <is>
-          <t>Teresa</t>
+          <t>BRIAN</t>
         </is>
       </c>
       <c r="C142" s="3" t="inlineStr">
         <is>
-          <t>Vereeniging</t>
+          <t>Hibberdene</t>
         </is>
       </c>
       <c r="D142" s="3" t="inlineStr">
@@ -4970,17 +4970,17 @@
     <row r="143" ht="25" customHeight="1">
       <c r="A143" s="3" t="inlineStr">
         <is>
-          <t>Peters</t>
+          <t>Pantoleon</t>
         </is>
       </c>
       <c r="B143" s="3" t="inlineStr">
         <is>
-          <t>Maureen</t>
+          <t>Teresa</t>
         </is>
       </c>
       <c r="C143" s="3" t="inlineStr">
         <is>
-          <t>Ceres</t>
+          <t>Vereeniging</t>
         </is>
       </c>
       <c r="D143" s="3" t="inlineStr">
@@ -4995,24 +4995,24 @@
       </c>
       <c r="F143" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="144" ht="25" customHeight="1">
       <c r="A144" s="3" t="inlineStr">
         <is>
-          <t>Pillay</t>
+          <t>Peters</t>
         </is>
       </c>
       <c r="B144" s="3" t="inlineStr">
         <is>
-          <t>Sundru</t>
+          <t>Maureen</t>
         </is>
       </c>
       <c r="C144" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>Ceres</t>
         </is>
       </c>
       <c r="D144" s="3" t="inlineStr">
@@ -5022,7 +5022,7 @@
       </c>
       <c r="E144" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F144" s="3" t="inlineStr">
@@ -5039,12 +5039,12 @@
       </c>
       <c r="B145" s="3" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>Sundru</t>
         </is>
       </c>
       <c r="C145" s="3" t="inlineStr">
         <is>
-          <t>Tygerberg Hills</t>
+          <t>Durbanville</t>
         </is>
       </c>
       <c r="D145" s="3" t="inlineStr">
@@ -5054,7 +5054,7 @@
       </c>
       <c r="E145" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F145" s="3" t="inlineStr">
@@ -5066,17 +5066,17 @@
     <row r="146" ht="25" customHeight="1">
       <c r="A146" s="3" t="inlineStr">
         <is>
-          <t>Polkinghorne</t>
+          <t>Pillay</t>
         </is>
       </c>
       <c r="B146" s="3" t="inlineStr">
         <is>
-          <t>Tracey</t>
+          <t>Patrick</t>
         </is>
       </c>
       <c r="C146" s="3" t="inlineStr">
         <is>
-          <t>Kensington</t>
+          <t>Tygerberg Hills</t>
         </is>
       </c>
       <c r="D146" s="3" t="inlineStr">
@@ -5091,7 +5091,7 @@
       </c>
       <c r="F146" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -5103,7 +5103,7 @@
       </c>
       <c r="B147" s="3" t="inlineStr">
         <is>
-          <t>Gavin</t>
+          <t>Tracey</t>
         </is>
       </c>
       <c r="C147" s="3" t="inlineStr">
@@ -5118,7 +5118,7 @@
       </c>
       <c r="E147" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F147" s="3" t="inlineStr">
@@ -5130,22 +5130,22 @@
     <row r="148" ht="25" customHeight="1">
       <c r="A148" s="3" t="inlineStr">
         <is>
-          <t>Pretorius</t>
+          <t>Polkinghorne</t>
         </is>
       </c>
       <c r="B148" s="3" t="inlineStr">
         <is>
-          <t>Sheldon Edmund</t>
+          <t>Gavin</t>
         </is>
       </c>
       <c r="C148" s="3" t="inlineStr">
         <is>
-          <t>Merriman</t>
+          <t>Kensington</t>
         </is>
       </c>
       <c r="D148" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E148" s="3" t="inlineStr">
@@ -5155,29 +5155,29 @@
       </c>
       <c r="F148" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="149" ht="25" customHeight="1">
       <c r="A149" s="3" t="inlineStr">
         <is>
-          <t>Ras</t>
+          <t>Pretorius</t>
         </is>
       </c>
       <c r="B149" s="3" t="inlineStr">
         <is>
-          <t>Mary-Anne</t>
+          <t>Sheldon Edmund</t>
         </is>
       </c>
       <c r="C149" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Merriman</t>
         </is>
       </c>
       <c r="D149" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E149" s="3" t="inlineStr">
@@ -5199,7 +5199,7 @@
       </c>
       <c r="B150" s="3" t="inlineStr">
         <is>
-          <t>Leon Jacobus</t>
+          <t>Mary-Anne</t>
         </is>
       </c>
       <c r="C150" s="3" t="inlineStr">
@@ -5219,24 +5219,24 @@
       </c>
       <c r="F150" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="151" ht="25" customHeight="1">
       <c r="A151" s="3" t="inlineStr">
         <is>
-          <t>Reniers</t>
+          <t>Ras</t>
         </is>
       </c>
       <c r="B151" s="3" t="inlineStr">
         <is>
-          <t>Hugo</t>
+          <t>Leon Jacobus</t>
         </is>
       </c>
       <c r="C151" s="3" t="inlineStr">
         <is>
-          <t>Nelspruit</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D151" s="3" t="inlineStr">
@@ -5246,7 +5246,7 @@
       </c>
       <c r="E151" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F151" s="3" t="inlineStr">
@@ -5258,17 +5258,17 @@
     <row r="152" ht="25" customHeight="1">
       <c r="A152" s="3" t="inlineStr">
         <is>
-          <t>Roman</t>
+          <t>Reniers</t>
         </is>
       </c>
       <c r="B152" s="3" t="inlineStr">
         <is>
-          <t>Sandy</t>
+          <t>Hugo</t>
         </is>
       </c>
       <c r="C152" s="3" t="inlineStr">
         <is>
-          <t>Bergvliet</t>
+          <t>Nelspruit</t>
         </is>
       </c>
       <c r="D152" s="3" t="inlineStr">
@@ -5278,29 +5278,29 @@
       </c>
       <c r="E152" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F152" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="153" ht="25" customHeight="1">
       <c r="A153" s="3" t="inlineStr">
         <is>
-          <t>Rossouw</t>
+          <t>Roman</t>
         </is>
       </c>
       <c r="B153" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Sandy</t>
         </is>
       </c>
       <c r="C153" s="3" t="inlineStr">
         <is>
-          <t>Tokai</t>
+          <t>Bergvliet</t>
         </is>
       </c>
       <c r="D153" s="3" t="inlineStr">
@@ -5310,7 +5310,7 @@
       </c>
       <c r="E153" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F153" s="3" t="inlineStr">
@@ -5322,17 +5322,17 @@
     <row r="154" ht="25" customHeight="1">
       <c r="A154" s="3" t="inlineStr">
         <is>
-          <t>Rothner</t>
+          <t>Rossouw</t>
         </is>
       </c>
       <c r="B154" s="3" t="inlineStr">
         <is>
-          <t>Andrea</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C154" s="3" t="inlineStr">
         <is>
-          <t>Eden</t>
+          <t>Tokai</t>
         </is>
       </c>
       <c r="D154" s="3" t="inlineStr">
@@ -5342,7 +5342,7 @@
       </c>
       <c r="E154" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F154" s="3" t="inlineStr">
@@ -5354,17 +5354,17 @@
     <row r="155" ht="25" customHeight="1">
       <c r="A155" s="3" t="inlineStr">
         <is>
-          <t>Roux</t>
+          <t>Rothner</t>
         </is>
       </c>
       <c r="B155" s="3" t="inlineStr">
         <is>
-          <t>Anthonie Petrus</t>
+          <t>Andrea</t>
         </is>
       </c>
       <c r="C155" s="3" t="inlineStr">
         <is>
-          <t>Moorreesburg</t>
+          <t>Eden</t>
         </is>
       </c>
       <c r="D155" s="3" t="inlineStr">
@@ -5374,7 +5374,7 @@
       </c>
       <c r="E155" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F155" s="3" t="inlineStr">
@@ -5386,17 +5386,17 @@
     <row r="156" ht="25" customHeight="1">
       <c r="A156" s="3" t="inlineStr">
         <is>
-          <t>Russell</t>
+          <t>Roux</t>
         </is>
       </c>
       <c r="B156" s="3" t="inlineStr">
         <is>
-          <t>Ingrid</t>
+          <t>Anthonie Petrus</t>
         </is>
       </c>
       <c r="C156" s="3" t="inlineStr">
         <is>
-          <t>Fish Hoek</t>
+          <t>Moorreesburg</t>
         </is>
       </c>
       <c r="D156" s="3" t="inlineStr">
@@ -5418,27 +5418,27 @@
     <row r="157" ht="25" customHeight="1">
       <c r="A157" s="3" t="inlineStr">
         <is>
-          <t>SNYMAN</t>
+          <t>Russell</t>
         </is>
       </c>
       <c r="B157" s="3" t="inlineStr">
         <is>
-          <t>LYN</t>
+          <t>Ingrid</t>
         </is>
       </c>
       <c r="C157" s="3" t="inlineStr">
         <is>
-          <t>Deep South</t>
+          <t>Fish Hoek</t>
         </is>
       </c>
       <c r="D157" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E157" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F157" s="3" t="inlineStr">
@@ -5450,27 +5450,27 @@
     <row r="158" ht="25" customHeight="1">
       <c r="A158" s="3" t="inlineStr">
         <is>
-          <t>STEENBERG</t>
+          <t>SNYMAN</t>
         </is>
       </c>
       <c r="B158" s="3" t="inlineStr">
         <is>
-          <t>TIM</t>
+          <t>LYN</t>
         </is>
       </c>
       <c r="C158" s="3" t="inlineStr">
         <is>
-          <t>Wellington</t>
+          <t>Deep South</t>
         </is>
       </c>
       <c r="D158" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E158" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F158" s="3" t="inlineStr">
@@ -5482,17 +5482,17 @@
     <row r="159" ht="25" customHeight="1">
       <c r="A159" s="3" t="inlineStr">
         <is>
-          <t>Sabatier</t>
+          <t>STEENBERG</t>
         </is>
       </c>
       <c r="B159" s="3" t="inlineStr">
         <is>
-          <t>Rodney</t>
+          <t>TIM</t>
         </is>
       </c>
       <c r="C159" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Wellington</t>
         </is>
       </c>
       <c r="D159" s="3" t="inlineStr">
@@ -5507,24 +5507,24 @@
       </c>
       <c r="F159" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="160" ht="25" customHeight="1">
       <c r="A160" s="3" t="inlineStr">
         <is>
-          <t>Sampie</t>
+          <t>Sabatier</t>
         </is>
       </c>
       <c r="B160" s="3" t="inlineStr">
         <is>
-          <t>Sharon</t>
+          <t>Rodney</t>
         </is>
       </c>
       <c r="C160" s="3" t="inlineStr">
         <is>
-          <t>Bergvliet</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D160" s="3" t="inlineStr">
@@ -5539,24 +5539,24 @@
       </c>
       <c r="F160" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="161" ht="25" customHeight="1">
       <c r="A161" s="3" t="inlineStr">
         <is>
-          <t>Schatz</t>
+          <t>Sampie</t>
         </is>
       </c>
       <c r="B161" s="3" t="inlineStr">
         <is>
-          <t>Vera</t>
+          <t>Sharon</t>
         </is>
       </c>
       <c r="C161" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Bergvliet</t>
         </is>
       </c>
       <c r="D161" s="3" t="inlineStr">
@@ -5583,7 +5583,7 @@
       </c>
       <c r="B162" s="3" t="inlineStr">
         <is>
-          <t>Frank</t>
+          <t>Vera</t>
         </is>
       </c>
       <c r="C162" s="3" t="inlineStr">
@@ -5610,17 +5610,17 @@
     <row r="163" ht="25" customHeight="1">
       <c r="A163" s="3" t="inlineStr">
         <is>
-          <t>Searle</t>
+          <t>Schatz</t>
         </is>
       </c>
       <c r="B163" s="3" t="inlineStr">
         <is>
-          <t>Francis</t>
+          <t>Frank</t>
         </is>
       </c>
       <c r="C163" s="3" t="inlineStr">
         <is>
-          <t>Kouga</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D163" s="3" t="inlineStr">
@@ -5635,7 +5635,7 @@
       </c>
       <c r="F163" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -5647,7 +5647,7 @@
       </c>
       <c r="B164" s="3" t="inlineStr">
         <is>
-          <t>Gloria</t>
+          <t>Francis</t>
         </is>
       </c>
       <c r="C164" s="3" t="inlineStr">
@@ -5662,7 +5662,7 @@
       </c>
       <c r="E164" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F164" s="3" t="inlineStr">
@@ -5674,17 +5674,17 @@
     <row r="165" ht="25" customHeight="1">
       <c r="A165" s="3" t="inlineStr">
         <is>
-          <t>Sell</t>
+          <t>Searle</t>
         </is>
       </c>
       <c r="B165" s="3" t="inlineStr">
         <is>
-          <t>Ami</t>
+          <t>Gloria</t>
         </is>
       </c>
       <c r="C165" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Kouga</t>
         </is>
       </c>
       <c r="D165" s="3" t="inlineStr">
@@ -5699,24 +5699,24 @@
       </c>
       <c r="F165" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="166" ht="25" customHeight="1">
       <c r="A166" s="3" t="inlineStr">
         <is>
-          <t>Simpson</t>
+          <t>Sell</t>
         </is>
       </c>
       <c r="B166" s="3" t="inlineStr">
         <is>
-          <t>Beryl</t>
+          <t>Ami</t>
         </is>
       </c>
       <c r="C166" s="3" t="inlineStr">
         <is>
-          <t>Cape Town</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D166" s="3" t="inlineStr">
@@ -5738,17 +5738,17 @@
     <row r="167" ht="25" customHeight="1">
       <c r="A167" s="3" t="inlineStr">
         <is>
-          <t>Sircoulomb</t>
+          <t>Simpson</t>
         </is>
       </c>
       <c r="B167" s="3" t="inlineStr">
         <is>
-          <t>Kenlis</t>
+          <t>Beryl</t>
         </is>
       </c>
       <c r="C167" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Cape Town</t>
         </is>
       </c>
       <c r="D167" s="3" t="inlineStr">
@@ -5775,7 +5775,7 @@
       </c>
       <c r="B168" s="3" t="inlineStr">
         <is>
-          <t>Holger</t>
+          <t>Kenlis</t>
         </is>
       </c>
       <c r="C168" s="3" t="inlineStr">
@@ -5802,12 +5802,12 @@
     <row r="169" ht="25" customHeight="1">
       <c r="A169" s="3" t="inlineStr">
         <is>
-          <t>Smeer</t>
+          <t>Sircoulomb</t>
         </is>
       </c>
       <c r="B169" s="3" t="inlineStr">
         <is>
-          <t>Hennie</t>
+          <t>Holger</t>
         </is>
       </c>
       <c r="C169" s="3" t="inlineStr">
@@ -5817,12 +5817,12 @@
       </c>
       <c r="D169" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E169" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F169" s="3" t="inlineStr">
@@ -5834,22 +5834,22 @@
     <row r="170" ht="25" customHeight="1">
       <c r="A170" s="3" t="inlineStr">
         <is>
-          <t>Smit</t>
+          <t>Smeer</t>
         </is>
       </c>
       <c r="B170" s="3" t="inlineStr">
         <is>
-          <t>Sue</t>
+          <t>Hennie</t>
         </is>
       </c>
       <c r="C170" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D170" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E170" s="3" t="inlineStr">
@@ -5859,7 +5859,7 @@
       </c>
       <c r="F170" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -5871,12 +5871,12 @@
       </c>
       <c r="B171" s="3" t="inlineStr">
         <is>
-          <t>Herman</t>
+          <t>Sue</t>
         </is>
       </c>
       <c r="C171" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D171" s="3" t="inlineStr">
@@ -5886,29 +5886,29 @@
       </c>
       <c r="E171" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F171" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="172" ht="25" customHeight="1">
       <c r="A172" s="3" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Smit</t>
         </is>
       </c>
       <c r="B172" s="3" t="inlineStr">
         <is>
-          <t>Jeff</t>
+          <t>Herman</t>
         </is>
       </c>
       <c r="C172" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D172" s="3" t="inlineStr">
@@ -5923,7 +5923,7 @@
       </c>
       <c r="F172" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -5935,12 +5935,12 @@
       </c>
       <c r="B173" s="3" t="inlineStr">
         <is>
-          <t>Bennie</t>
+          <t>Jeff</t>
         </is>
       </c>
       <c r="C173" s="3" t="inlineStr">
         <is>
-          <t>Wellington</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D173" s="3" t="inlineStr">
@@ -5950,12 +5950,12 @@
       </c>
       <c r="E173" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F173" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -5967,12 +5967,12 @@
       </c>
       <c r="B174" s="3" t="inlineStr">
         <is>
-          <t>Carmen Dolores</t>
+          <t>Bennie</t>
         </is>
       </c>
       <c r="C174" s="3" t="inlineStr">
         <is>
-          <t>Tokai</t>
+          <t>Wellington</t>
         </is>
       </c>
       <c r="D174" s="3" t="inlineStr">
@@ -5982,7 +5982,7 @@
       </c>
       <c r="E174" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F174" s="3" t="inlineStr">
@@ -5999,7 +5999,7 @@
       </c>
       <c r="B175" s="3" t="inlineStr">
         <is>
-          <t>David John</t>
+          <t>Carmen Dolores</t>
         </is>
       </c>
       <c r="C175" s="3" t="inlineStr">
@@ -6026,17 +6026,17 @@
     <row r="176" ht="25" customHeight="1">
       <c r="A176" s="3" t="inlineStr">
         <is>
-          <t>Sochen</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="B176" s="3" t="inlineStr">
         <is>
-          <t>Diana</t>
+          <t>David John</t>
         </is>
       </c>
       <c r="C176" s="3" t="inlineStr">
         <is>
-          <t>Sea Point</t>
+          <t>Tokai</t>
         </is>
       </c>
       <c r="D176" s="3" t="inlineStr">
@@ -6046,7 +6046,7 @@
       </c>
       <c r="E176" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F176" s="3" t="inlineStr">
@@ -6058,49 +6058,49 @@
     <row r="177" ht="25" customHeight="1">
       <c r="A177" s="3" t="inlineStr">
         <is>
-          <t>Steyn</t>
+          <t>Sochen</t>
         </is>
       </c>
       <c r="B177" s="3" t="inlineStr">
         <is>
-          <t>Elna</t>
+          <t>Diana</t>
         </is>
       </c>
       <c r="C177" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Sea Point</t>
         </is>
       </c>
       <c r="D177" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E177" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F177" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="178" ht="25" customHeight="1">
       <c r="A178" s="3" t="inlineStr">
         <is>
-          <t>Strauss</t>
+          <t>Steyn</t>
         </is>
       </c>
       <c r="B178" s="3" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>Elna</t>
         </is>
       </c>
       <c r="C178" s="3" t="inlineStr">
         <is>
-          <t>Kuilsriver</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D178" s="3" t="inlineStr">
@@ -6115,29 +6115,29 @@
       </c>
       <c r="F178" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="179" ht="25" customHeight="1">
       <c r="A179" s="3" t="inlineStr">
         <is>
-          <t>Sturges</t>
+          <t>Strauss</t>
         </is>
       </c>
       <c r="B179" s="3" t="inlineStr">
         <is>
-          <t>Trevor</t>
+          <t>Patrick</t>
         </is>
       </c>
       <c r="C179" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Kuilsriver</t>
         </is>
       </c>
       <c r="D179" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E179" s="3" t="inlineStr">
@@ -6147,24 +6147,24 @@
       </c>
       <c r="F179" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="180" ht="25" customHeight="1">
       <c r="A180" s="3" t="inlineStr">
         <is>
-          <t>Talbot</t>
+          <t>Sturges</t>
         </is>
       </c>
       <c r="B180" s="3" t="inlineStr">
         <is>
-          <t>Lauryn</t>
+          <t>Trevor</t>
         </is>
       </c>
       <c r="C180" s="3" t="inlineStr">
         <is>
-          <t>Benoni Lakes</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D180" s="3" t="inlineStr">
@@ -6186,17 +6186,17 @@
     <row r="181" ht="25" customHeight="1">
       <c r="A181" s="3" t="inlineStr">
         <is>
-          <t>Theron</t>
+          <t>Talbot</t>
         </is>
       </c>
       <c r="B181" s="3" t="inlineStr">
         <is>
-          <t>Pierre</t>
+          <t>Lauryn</t>
         </is>
       </c>
       <c r="C181" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Benoni Lakes</t>
         </is>
       </c>
       <c r="D181" s="3" t="inlineStr">
@@ -6223,7 +6223,7 @@
       </c>
       <c r="B182" s="3" t="inlineStr">
         <is>
-          <t>Moira</t>
+          <t>Pierre</t>
         </is>
       </c>
       <c r="C182" s="3" t="inlineStr">
@@ -6250,22 +6250,22 @@
     <row r="183" ht="25" customHeight="1">
       <c r="A183" s="3" t="inlineStr">
         <is>
-          <t>Toye</t>
+          <t>Theron</t>
         </is>
       </c>
       <c r="B183" s="3" t="inlineStr">
         <is>
-          <t>Omolayo</t>
+          <t>Moira</t>
         </is>
       </c>
       <c r="C183" s="3" t="inlineStr">
         <is>
-          <t>The Wilds</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D183" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E183" s="3" t="inlineStr">
@@ -6282,22 +6282,22 @@
     <row r="184" ht="25" customHeight="1">
       <c r="A184" s="3" t="inlineStr">
         <is>
-          <t>Tshikala</t>
+          <t>Toye</t>
         </is>
       </c>
       <c r="B184" s="3" t="inlineStr">
         <is>
-          <t>David Alex</t>
+          <t>Omolayo</t>
         </is>
       </c>
       <c r="C184" s="3" t="inlineStr">
         <is>
-          <t>Athlone</t>
+          <t>The Wilds</t>
         </is>
       </c>
       <c r="D184" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E184" s="3" t="inlineStr">
@@ -6307,24 +6307,24 @@
       </c>
       <c r="F184" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="185" ht="25" customHeight="1">
       <c r="A185" s="3" t="inlineStr">
         <is>
-          <t>Tuckett</t>
+          <t>Tshikala</t>
         </is>
       </c>
       <c r="B185" s="3" t="inlineStr">
         <is>
-          <t>Alistair</t>
+          <t>David Alex</t>
         </is>
       </c>
       <c r="C185" s="3" t="inlineStr">
         <is>
-          <t>Roodepoort Clearwater Cyber</t>
+          <t>Athlone</t>
         </is>
       </c>
       <c r="D185" s="3" t="inlineStr">
@@ -6339,7 +6339,7 @@
       </c>
       <c r="F185" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -6351,7 +6351,7 @@
       </c>
       <c r="B186" s="3" t="inlineStr">
         <is>
-          <t>Rowan</t>
+          <t>Alistair</t>
         </is>
       </c>
       <c r="C186" s="3" t="inlineStr">
@@ -6366,7 +6366,7 @@
       </c>
       <c r="E186" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F186" s="3" t="inlineStr">
@@ -6383,7 +6383,7 @@
       </c>
       <c r="B187" s="3" t="inlineStr">
         <is>
-          <t>Gail</t>
+          <t>Rowan</t>
         </is>
       </c>
       <c r="C187" s="3" t="inlineStr">
@@ -6398,7 +6398,7 @@
       </c>
       <c r="E187" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F187" s="3" t="inlineStr">
@@ -6410,17 +6410,17 @@
     <row r="188" ht="25" customHeight="1">
       <c r="A188" s="3" t="inlineStr">
         <is>
-          <t>VAN BREDA</t>
+          <t>Tuckett</t>
         </is>
       </c>
       <c r="B188" s="3" t="inlineStr">
         <is>
-          <t>HILARY LISE</t>
+          <t>Gail</t>
         </is>
       </c>
       <c r="C188" s="3" t="inlineStr">
         <is>
-          <t>Cape Town</t>
+          <t>Roodepoort Clearwater Cyber</t>
         </is>
       </c>
       <c r="D188" s="3" t="inlineStr">
@@ -6435,39 +6435,39 @@
       </c>
       <c r="F188" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="189" ht="25" customHeight="1">
       <c r="A189" s="3" t="inlineStr">
         <is>
-          <t>VAN DER MERWE</t>
+          <t>VAN BREDA</t>
         </is>
       </c>
       <c r="B189" s="3" t="inlineStr">
         <is>
-          <t>PATRICIA</t>
+          <t>HILARY LISE</t>
         </is>
       </c>
       <c r="C189" s="3" t="inlineStr">
         <is>
-          <t>East London Port Rex</t>
+          <t>Cape Town</t>
         </is>
       </c>
       <c r="D189" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E189" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F189" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -6479,17 +6479,17 @@
       </c>
       <c r="B190" s="3" t="inlineStr">
         <is>
-          <t>MARINA</t>
+          <t>PATRICIA</t>
         </is>
       </c>
       <c r="C190" s="3" t="inlineStr">
         <is>
-          <t>Malmesbury</t>
+          <t>East London Port Rex</t>
         </is>
       </c>
       <c r="D190" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E190" s="3" t="inlineStr">
@@ -6499,56 +6499,56 @@
       </c>
       <c r="F190" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="191" ht="25" customHeight="1">
       <c r="A191" s="3" t="inlineStr">
         <is>
-          <t>Valadao</t>
+          <t>VAN DER MERWE</t>
         </is>
       </c>
       <c r="B191" s="3" t="inlineStr">
         <is>
-          <t>Tracy</t>
+          <t>MARINA</t>
         </is>
       </c>
       <c r="C191" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Malmesbury</t>
         </is>
       </c>
       <c r="D191" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E191" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F191" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="192" ht="25" customHeight="1">
       <c r="A192" s="3" t="inlineStr">
         <is>
-          <t>Van Niekerk</t>
+          <t>Valadao</t>
         </is>
       </c>
       <c r="B192" s="3" t="inlineStr">
         <is>
-          <t>Riaan</t>
+          <t>Tracy</t>
         </is>
       </c>
       <c r="C192" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D192" s="3" t="inlineStr">
@@ -6570,59 +6570,59 @@
     <row r="193" ht="25" customHeight="1">
       <c r="A193" s="3" t="inlineStr">
         <is>
-          <t>Van Rensburg</t>
+          <t>Van Niekerk</t>
         </is>
       </c>
       <c r="B193" s="3" t="inlineStr">
         <is>
-          <t>Neville</t>
+          <t>Riaan</t>
         </is>
       </c>
       <c r="C193" s="3" t="inlineStr">
         <is>
-          <t>Moorreesburg</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D193" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E193" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F193" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="194" ht="25" customHeight="1">
       <c r="A194" s="3" t="inlineStr">
         <is>
-          <t>Van Romburgh</t>
+          <t>Van Rensburg</t>
         </is>
       </c>
       <c r="B194" s="3" t="inlineStr">
         <is>
-          <t>Lorna</t>
+          <t>Neville</t>
         </is>
       </c>
       <c r="C194" s="3" t="inlineStr">
         <is>
-          <t>Fish Hoek</t>
+          <t>Moorreesburg</t>
         </is>
       </c>
       <c r="D194" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E194" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F194" s="3" t="inlineStr">
@@ -6634,17 +6634,17 @@
     <row r="195" ht="25" customHeight="1">
       <c r="A195" s="3" t="inlineStr">
         <is>
-          <t>Van Wyk-Nelson</t>
+          <t>Van Romburgh</t>
         </is>
       </c>
       <c r="B195" s="3" t="inlineStr">
         <is>
-          <t>Edith</t>
+          <t>Lorna</t>
         </is>
       </c>
       <c r="C195" s="3" t="inlineStr">
         <is>
-          <t>Kuilsriver</t>
+          <t>Fish Hoek</t>
         </is>
       </c>
       <c r="D195" s="3" t="inlineStr">
@@ -6666,22 +6666,22 @@
     <row r="196" ht="25" customHeight="1">
       <c r="A196" s="3" t="inlineStr">
         <is>
-          <t>Van de Merwe</t>
+          <t>Van Wyk-Nelson</t>
         </is>
       </c>
       <c r="B196" s="3" t="inlineStr">
         <is>
-          <t>Marina</t>
+          <t>Edith</t>
         </is>
       </c>
       <c r="C196" s="3" t="inlineStr">
         <is>
-          <t>Malmesbury</t>
+          <t>Kuilsriver</t>
         </is>
       </c>
       <c r="D196" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E196" s="3" t="inlineStr">
@@ -6698,54 +6698,54 @@
     <row r="197" ht="25" customHeight="1">
       <c r="A197" s="3" t="inlineStr">
         <is>
-          <t>Venter</t>
+          <t>Van de Merwe</t>
         </is>
       </c>
       <c r="B197" s="3" t="inlineStr">
         <is>
-          <t>Louis</t>
+          <t>Marina</t>
         </is>
       </c>
       <c r="C197" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Malmesbury</t>
         </is>
       </c>
       <c r="D197" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E197" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F197" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="198" ht="25" customHeight="1">
       <c r="A198" s="3" t="inlineStr">
         <is>
-          <t>Volker</t>
+          <t>Venter</t>
         </is>
       </c>
       <c r="B198" s="3" t="inlineStr">
         <is>
-          <t>Russell</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="C198" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D198" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E198" s="3" t="inlineStr">
@@ -6762,96 +6762,96 @@
     <row r="199" ht="25" customHeight="1">
       <c r="A199" s="3" t="inlineStr">
         <is>
-          <t>Von Mollendorf</t>
+          <t>Volker</t>
         </is>
       </c>
       <c r="B199" s="3" t="inlineStr">
         <is>
-          <t>Rinette</t>
+          <t>Russell</t>
         </is>
       </c>
       <c r="C199" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>King William's Town</t>
         </is>
       </c>
       <c r="D199" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E199" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F199" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="200" ht="25" customHeight="1">
       <c r="A200" s="3" t="inlineStr">
         <is>
-          <t>Warman</t>
+          <t>Von Mollendorf</t>
         </is>
       </c>
       <c r="B200" s="3" t="inlineStr">
         <is>
-          <t>Alastair</t>
+          <t>Rinette</t>
         </is>
       </c>
       <c r="C200" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Durbanville</t>
         </is>
       </c>
       <c r="D200" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E200" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F200" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="201" ht="25" customHeight="1">
       <c r="A201" s="3" t="inlineStr">
         <is>
-          <t>Watson</t>
+          <t>Warman</t>
         </is>
       </c>
       <c r="B201" s="3" t="inlineStr">
         <is>
-          <t>Allan</t>
+          <t>Alastair</t>
         </is>
       </c>
       <c r="C201" s="3" t="inlineStr">
         <is>
-          <t>Sea Point</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D201" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E201" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F201" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -6863,22 +6863,22 @@
       </c>
       <c r="B202" s="3" t="inlineStr">
         <is>
-          <t>Alison</t>
+          <t>Allan</t>
         </is>
       </c>
       <c r="C202" s="3" t="inlineStr">
         <is>
-          <t>Sedgefield</t>
+          <t>Sea Point</t>
         </is>
       </c>
       <c r="D202" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E202" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F202" s="3" t="inlineStr">
@@ -6890,27 +6890,27 @@
     <row r="203" ht="25" customHeight="1">
       <c r="A203" s="3" t="inlineStr">
         <is>
-          <t>Williams</t>
+          <t>Watson</t>
         </is>
       </c>
       <c r="B203" s="3" t="inlineStr">
         <is>
-          <t>Johanna</t>
+          <t>Alison</t>
         </is>
       </c>
       <c r="C203" s="3" t="inlineStr">
         <is>
-          <t>Mitchells Plain</t>
+          <t>Sedgefield</t>
         </is>
       </c>
       <c r="D203" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E203" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F203" s="3" t="inlineStr">
@@ -6922,22 +6922,22 @@
     <row r="204" ht="25" customHeight="1">
       <c r="A204" s="3" t="inlineStr">
         <is>
-          <t>Wills</t>
+          <t>Williams</t>
         </is>
       </c>
       <c r="B204" s="3" t="inlineStr">
         <is>
-          <t>Geila</t>
+          <t>Johanna</t>
         </is>
       </c>
       <c r="C204" s="3" t="inlineStr">
         <is>
-          <t>Athlone</t>
+          <t>Mitchells Plain</t>
         </is>
       </c>
       <c r="D204" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E204" s="3" t="inlineStr">
@@ -6954,17 +6954,17 @@
     <row r="205" ht="25" customHeight="1">
       <c r="A205" s="3" t="inlineStr">
         <is>
-          <t>Wilter-Sturges</t>
+          <t>Wills</t>
         </is>
       </c>
       <c r="B205" s="3" t="inlineStr">
         <is>
-          <t>Meredith</t>
+          <t>Geila</t>
         </is>
       </c>
       <c r="C205" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Athlone</t>
         </is>
       </c>
       <c r="D205" s="3" t="inlineStr">
@@ -6979,24 +6979,24 @@
       </c>
       <c r="F205" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="206" ht="25" customHeight="1">
       <c r="A206" s="3" t="inlineStr">
         <is>
-          <t>Wright</t>
+          <t>Wilter-Sturges</t>
         </is>
       </c>
       <c r="B206" s="3" t="inlineStr">
         <is>
-          <t>Rocky</t>
+          <t>Meredith</t>
         </is>
       </c>
       <c r="C206" s="3" t="inlineStr">
         <is>
-          <t>Table View</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D206" s="3" t="inlineStr">
@@ -7006,29 +7006,29 @@
       </c>
       <c r="E206" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F206" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="207" ht="25" customHeight="1">
       <c r="A207" s="3" t="inlineStr">
         <is>
-          <t>Young</t>
+          <t>Wright</t>
         </is>
       </c>
       <c r="B207" s="3" t="inlineStr">
         <is>
-          <t>Judy</t>
+          <t>Rocky</t>
         </is>
       </c>
       <c r="C207" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>Table View</t>
         </is>
       </c>
       <c r="D207" s="3" t="inlineStr">
@@ -7038,7 +7038,7 @@
       </c>
       <c r="E207" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F207" s="3" t="inlineStr">
@@ -7050,17 +7050,17 @@
     <row r="208" ht="25" customHeight="1">
       <c r="A208" s="3" t="inlineStr">
         <is>
-          <t>de Kock</t>
+          <t>Young</t>
         </is>
       </c>
       <c r="B208" s="3" t="inlineStr">
         <is>
-          <t>Engela</t>
+          <t>Judy</t>
         </is>
       </c>
       <c r="C208" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Durbanville</t>
         </is>
       </c>
       <c r="D208" s="3" t="inlineStr">
@@ -7070,7 +7070,7 @@
       </c>
       <c r="E208" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F208" s="3" t="inlineStr">
@@ -7087,7 +7087,7 @@
       </c>
       <c r="B209" s="3" t="inlineStr">
         <is>
-          <t>Francois</t>
+          <t>Engela</t>
         </is>
       </c>
       <c r="C209" s="3" t="inlineStr">
@@ -7114,54 +7114,54 @@
     <row r="210" ht="25" customHeight="1">
       <c r="A210" s="3" t="inlineStr">
         <is>
-          <t>de Silva</t>
+          <t>de Kock</t>
         </is>
       </c>
       <c r="B210" s="3" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Francois</t>
         </is>
       </c>
       <c r="C210" s="3" t="inlineStr">
         <is>
-          <t>Edenvale</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D210" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E210" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F210" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="211" ht="25" customHeight="1">
       <c r="A211" s="3" t="inlineStr">
         <is>
-          <t>du Toit</t>
+          <t>de Silva</t>
         </is>
       </c>
       <c r="B211" s="3" t="inlineStr">
         <is>
-          <t>Desiree</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="C211" s="3" t="inlineStr">
         <is>
-          <t>Ramsgate</t>
+          <t>Edenvale</t>
         </is>
       </c>
       <c r="D211" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E211" s="3" t="inlineStr">
@@ -7178,59 +7178,59 @@
     <row r="212" ht="25" customHeight="1">
       <c r="A212" s="3" t="inlineStr">
         <is>
-          <t>stier</t>
+          <t>du Toit</t>
         </is>
       </c>
       <c r="B212" s="3" t="inlineStr">
         <is>
-          <t>RORY</t>
+          <t>Desiree</t>
         </is>
       </c>
       <c r="C212" s="3" t="inlineStr">
         <is>
-          <t>Deep South</t>
+          <t>Ramsgate</t>
         </is>
       </c>
       <c r="D212" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E212" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F212" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="213" ht="25" customHeight="1">
       <c r="A213" s="3" t="inlineStr">
         <is>
-          <t>van Blerk</t>
+          <t>stier</t>
         </is>
       </c>
       <c r="B213" s="3" t="inlineStr">
         <is>
-          <t>Carl</t>
+          <t>RORY</t>
         </is>
       </c>
       <c r="C213" s="3" t="inlineStr">
         <is>
-          <t>Eden</t>
+          <t>Deep South</t>
         </is>
       </c>
       <c r="D213" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E213" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F213" s="3" t="inlineStr">
@@ -7242,17 +7242,17 @@
     <row r="214" ht="25" customHeight="1">
       <c r="A214" s="3" t="inlineStr">
         <is>
-          <t>van Heerden</t>
+          <t>van Blerk</t>
         </is>
       </c>
       <c r="B214" s="3" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Carl</t>
         </is>
       </c>
       <c r="C214" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Eden</t>
         </is>
       </c>
       <c r="D214" s="3" t="inlineStr">
@@ -7267,7 +7267,7 @@
       </c>
       <c r="F214" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -7279,7 +7279,7 @@
       </c>
       <c r="B215" s="3" t="inlineStr">
         <is>
-          <t>Sandy</t>
+          <t>Sydney</t>
         </is>
       </c>
       <c r="C215" s="3" t="inlineStr">
@@ -7294,7 +7294,7 @@
       </c>
       <c r="E215" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F215" s="3" t="inlineStr">
@@ -7311,12 +7311,12 @@
       </c>
       <c r="B216" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Sandy</t>
         </is>
       </c>
       <c r="C216" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D216" s="3" t="inlineStr">
@@ -7338,17 +7338,17 @@
     <row r="217" ht="25" customHeight="1">
       <c r="A217" s="3" t="inlineStr">
         <is>
-          <t>van Rensburg</t>
+          <t>van Heerden</t>
         </is>
       </c>
       <c r="B217" s="3" t="inlineStr">
         <is>
-          <t>Johan</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C217" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D217" s="3" t="inlineStr">
@@ -7363,7 +7363,7 @@
       </c>
       <c r="F217" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -7375,7 +7375,7 @@
       </c>
       <c r="B218" s="3" t="inlineStr">
         <is>
-          <t>Anne</t>
+          <t>Johan</t>
         </is>
       </c>
       <c r="C218" s="3" t="inlineStr">
@@ -7390,7 +7390,7 @@
       </c>
       <c r="E218" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F218" s="3" t="inlineStr">
@@ -7402,17 +7402,17 @@
     <row r="219" ht="25" customHeight="1">
       <c r="A219" s="3" t="inlineStr">
         <is>
-          <t>van Wulven</t>
+          <t>van Rensburg</t>
         </is>
       </c>
       <c r="B219" s="3" t="inlineStr">
         <is>
-          <t>Jeannie</t>
+          <t>Anne</t>
         </is>
       </c>
       <c r="C219" s="3" t="inlineStr">
         <is>
-          <t>Tygerberg Hills</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D219" s="3" t="inlineStr">
@@ -7422,7 +7422,7 @@
       </c>
       <c r="E219" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F219" s="3" t="inlineStr">
@@ -7439,7 +7439,7 @@
       </c>
       <c r="B220" s="3" t="inlineStr">
         <is>
-          <t>Alan</t>
+          <t>Jeannie</t>
         </is>
       </c>
       <c r="C220" s="3" t="inlineStr">
@@ -7454,7 +7454,7 @@
       </c>
       <c r="E220" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F220" s="3" t="inlineStr">
@@ -7471,7 +7471,7 @@
       </c>
       <c r="B221" s="3" t="inlineStr">
         <is>
-          <t>Deon</t>
+          <t>Alan</t>
         </is>
       </c>
       <c r="C221" s="3" t="inlineStr">
@@ -7498,17 +7498,17 @@
     <row r="222" ht="25" customHeight="1">
       <c r="A222" s="3" t="inlineStr">
         <is>
-          <t>van Wyk</t>
+          <t>van Wulven</t>
         </is>
       </c>
       <c r="B222" s="3" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>Deon</t>
         </is>
       </c>
       <c r="C222" s="3" t="inlineStr">
         <is>
-          <t>North Durban</t>
+          <t>Tygerberg Hills</t>
         </is>
       </c>
       <c r="D222" s="3" t="inlineStr">
@@ -7523,7 +7523,7 @@
       </c>
       <c r="F222" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -7535,12 +7535,12 @@
       </c>
       <c r="B223" s="3" t="inlineStr">
         <is>
-          <t>Lindie</t>
+          <t>Kim</t>
         </is>
       </c>
       <c r="C223" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>North Durban</t>
         </is>
       </c>
       <c r="D223" s="3" t="inlineStr">
@@ -7567,12 +7567,12 @@
       </c>
       <c r="B224" s="3" t="inlineStr">
         <is>
-          <t>Willem</t>
+          <t>Lindie</t>
         </is>
       </c>
       <c r="C224" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D224" s="3" t="inlineStr">
@@ -7599,12 +7599,12 @@
       </c>
       <c r="B225" s="3" t="inlineStr">
         <is>
-          <t>Patricia</t>
+          <t>Willem</t>
         </is>
       </c>
       <c r="C225" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D225" s="3" t="inlineStr">
@@ -7626,27 +7626,27 @@
     <row r="226" ht="25" customHeight="1">
       <c r="A226" s="3" t="inlineStr">
         <is>
-          <t>van der Merwe</t>
+          <t>van Wyk</t>
         </is>
       </c>
       <c r="B226" s="3" t="inlineStr">
         <is>
-          <t>Ingrid</t>
+          <t>Patricia</t>
         </is>
       </c>
       <c r="C226" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D226" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E226" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F226" s="3" t="inlineStr">
@@ -7658,22 +7658,22 @@
     <row r="227" ht="25" customHeight="1">
       <c r="A227" s="3" t="inlineStr">
         <is>
-          <t>van der Westhuizen</t>
+          <t>van der Merwe</t>
         </is>
       </c>
       <c r="B227" s="3" t="inlineStr">
         <is>
-          <t>Hennie</t>
+          <t>Ingrid</t>
         </is>
       </c>
       <c r="C227" s="3" t="inlineStr">
         <is>
-          <t>Helderberg</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D227" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E227" s="3" t="inlineStr">
@@ -7683,24 +7683,24 @@
       </c>
       <c r="F227" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="228" ht="25" customHeight="1">
       <c r="A228" s="3" t="inlineStr">
         <is>
-          <t>von der Decken</t>
+          <t>van der Westhuizen</t>
         </is>
       </c>
       <c r="B228" s="3" t="inlineStr">
         <is>
-          <t>Brian</t>
+          <t>Hennie</t>
         </is>
       </c>
       <c r="C228" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Helderberg</t>
         </is>
       </c>
       <c r="D228" s="3" t="inlineStr">
@@ -7715,51 +7715,83 @@
       </c>
       <c r="F228" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="229" ht="25" customHeight="1">
       <c r="A229" s="3" t="inlineStr">
         <is>
+          <t>von der Decken</t>
+        </is>
+      </c>
+      <c r="B229" s="3" t="inlineStr">
+        <is>
+          <t>Brian</t>
+        </is>
+      </c>
+      <c r="C229" s="3" t="inlineStr">
+        <is>
+          <t>King William's Town</t>
+        </is>
+      </c>
+      <c r="D229" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E229" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F229" s="3" t="inlineStr">
+        <is>
+          <t>410E</t>
+        </is>
+      </c>
+    </row>
+    <row r="230" ht="25" customHeight="1">
+      <c r="A230" s="3" t="inlineStr">
+        <is>
           <t>‘t Hart</t>
         </is>
       </c>
-      <c r="B229" s="3" t="inlineStr">
+      <c r="B230" s="3" t="inlineStr">
         <is>
           <t>Michelle</t>
         </is>
       </c>
-      <c r="C229" s="3" t="inlineStr">
+      <c r="C230" s="3" t="inlineStr">
         <is>
           <t>Benoni Lakes</t>
         </is>
       </c>
-      <c r="D229" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E229" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F229" s="3" t="inlineStr">
+      <c r="D230" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E230" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F230" s="3" t="inlineStr">
         <is>
           <t>410E</t>
-        </is>
-      </c>
-    </row>
-    <row r="230">
-      <c r="A230" s="1" t="inlineStr">
-        <is>
-          <t>Number of attendees: 227</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="inlineStr">
+        <is>
+          <t>Number of attendees: 228</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" s="1" t="inlineStr">
         <is>
           <t>Number of voters: 109</t>
         </is>
@@ -7795,7 +7827,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Registrees as of 13/04/2021 21:20</t>
+          <t>410E Registrees as of 13/04/2021 21:27</t>
         </is>
       </c>
     </row>
@@ -11029,7 +11061,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Registrees as of 13/04/2021 21:20</t>
+          <t>410W Registrees as of 13/04/2021 21:27</t>
         </is>
       </c>
     </row>
@@ -15097,7 +15129,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Voting details as of 13/04/2021 21:20</t>
+          <t>410E Voting details as of 13/04/2021 21:27</t>
         </is>
       </c>
     </row>
@@ -15434,7 +15466,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Voting details as of 13/04/2021 21:20</t>
+          <t>410W Voting details as of 13/04/2021 21:27</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Registree stats backup on Wed 14 Apr 2021 14:25:22 SAST
</commit_message>
<xml_diff>
--- a/static/docs/registrees_list.xlsx
+++ b/static/docs/registrees_list.xlsx
@@ -451,7 +451,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>MD410 Registrees as of 13/04/2021 22:42</t>
+          <t>MD410 Registrees as of 14/04/2021 14:25</t>
         </is>
       </c>
     </row>
@@ -7841,7 +7841,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E121"/>
+  <dimension ref="A1:E122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7859,7 +7859,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Registrees as of 13/04/2021 22:42</t>
+          <t>410E Registrees as of 14/04/2021 14:25</t>
         </is>
       </c>
     </row>
@@ -10323,22 +10323,22 @@
     <row r="93" ht="25" customHeight="1">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>Tuckett</t>
+          <t>Toye</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
         <is>
-          <t>Alistair</t>
+          <t>Omolayo</t>
         </is>
       </c>
       <c r="C93" s="3" t="inlineStr">
         <is>
-          <t>Roodepoort Clearwater Cyber</t>
+          <t>The Wilds</t>
         </is>
       </c>
       <c r="D93" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E93" s="3" t="inlineStr">
@@ -10355,7 +10355,7 @@
       </c>
       <c r="B94" s="3" t="inlineStr">
         <is>
-          <t>Rowan</t>
+          <t>Alistair</t>
         </is>
       </c>
       <c r="C94" s="3" t="inlineStr">
@@ -10370,7 +10370,7 @@
       </c>
       <c r="E94" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -10382,7 +10382,7 @@
       </c>
       <c r="B95" s="3" t="inlineStr">
         <is>
-          <t>Gail</t>
+          <t>Rowan</t>
         </is>
       </c>
       <c r="C95" s="3" t="inlineStr">
@@ -10397,29 +10397,29 @@
       </c>
       <c r="E95" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="96" ht="25" customHeight="1">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>Uchytil</t>
+          <t>Tuckett</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
         <is>
-          <t>Jiri</t>
+          <t>Gail</t>
         </is>
       </c>
       <c r="C96" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Roodepoort Clearwater Cyber</t>
         </is>
       </c>
       <c r="D96" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E96" s="3" t="inlineStr">
@@ -10431,17 +10431,17 @@
     <row r="97" ht="25" customHeight="1">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>VAN DER MERWE</t>
+          <t>Uchytil</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
         <is>
-          <t>PATRICIA</t>
+          <t>Jiri</t>
         </is>
       </c>
       <c r="C97" s="3" t="inlineStr">
         <is>
-          <t>East London Port Rex</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D97" s="3" t="inlineStr">
@@ -10451,24 +10451,24 @@
       </c>
       <c r="E97" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="98" ht="25" customHeight="1">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>Van Niekerk</t>
+          <t>VAN DER MERWE</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
         <is>
-          <t>Riaan</t>
+          <t>PATRICIA</t>
         </is>
       </c>
       <c r="C98" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>East London Port Rex</t>
         </is>
       </c>
       <c r="D98" s="3" t="inlineStr">
@@ -10478,24 +10478,24 @@
       </c>
       <c r="E98" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="99" ht="25" customHeight="1">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>Venter</t>
+          <t>Van Niekerk</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
         <is>
-          <t>Louis</t>
+          <t>Riaan</t>
         </is>
       </c>
       <c r="C99" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D99" s="3" t="inlineStr">
@@ -10505,29 +10505,29 @@
       </c>
       <c r="E99" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="100" ht="25" customHeight="1">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>Volker</t>
+          <t>Venter</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
         <is>
-          <t>Russell</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="C100" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D100" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E100" s="3" t="inlineStr">
@@ -10539,17 +10539,17 @@
     <row r="101" ht="25" customHeight="1">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>Warman</t>
+          <t>Volker</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
         <is>
-          <t>Alastair</t>
+          <t>Russell</t>
         </is>
       </c>
       <c r="C101" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>King William's Town</t>
         </is>
       </c>
       <c r="D101" s="3" t="inlineStr">
@@ -10566,17 +10566,17 @@
     <row r="102" ht="25" customHeight="1">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>Williamson</t>
+          <t>Warman</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
         <is>
-          <t>Neville</t>
+          <t>Alastair</t>
         </is>
       </c>
       <c r="C102" s="3" t="inlineStr">
         <is>
-          <t>Port Alfred</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D102" s="3" t="inlineStr">
@@ -10586,24 +10586,24 @@
       </c>
       <c r="E102" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="103" ht="25" customHeight="1">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>Wilter-Sturges</t>
+          <t>Williamson</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
         <is>
-          <t>Meredith</t>
+          <t>Neville</t>
         </is>
       </c>
       <c r="C103" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Port Alfred</t>
         </is>
       </c>
       <c r="D103" s="3" t="inlineStr">
@@ -10620,17 +10620,17 @@
     <row r="104" ht="25" customHeight="1">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>Zucker</t>
+          <t>Wilter-Sturges</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
         <is>
-          <t>Leonie</t>
+          <t>Meredith</t>
         </is>
       </c>
       <c r="C104" s="3" t="inlineStr">
         <is>
-          <t>Milnerton</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D104" s="3" t="inlineStr">
@@ -10640,61 +10640,61 @@
       </c>
       <c r="E104" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="105" ht="25" customHeight="1">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>de Silva</t>
+          <t>Zucker</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Leonie</t>
         </is>
       </c>
       <c r="C105" s="3" t="inlineStr">
         <is>
-          <t>Edenvale</t>
+          <t>Milnerton</t>
         </is>
       </c>
       <c r="D105" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E105" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="106" ht="25" customHeight="1">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>du Plooy</t>
+          <t>de Silva</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
         <is>
-          <t>Tammy</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="C106" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Edenvale</t>
         </is>
       </c>
       <c r="D106" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E106" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -10706,7 +10706,7 @@
       </c>
       <c r="B107" s="3" t="inlineStr">
         <is>
-          <t>Marc</t>
+          <t>Tammy</t>
         </is>
       </c>
       <c r="C107" s="3" t="inlineStr">
@@ -10728,17 +10728,17 @@
     <row r="108" ht="25" customHeight="1">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>du Toit</t>
+          <t>du Plooy</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
         <is>
-          <t>Desiree</t>
+          <t>Marc</t>
         </is>
       </c>
       <c r="C108" s="3" t="inlineStr">
         <is>
-          <t>Ramsgate</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D108" s="3" t="inlineStr">
@@ -10748,24 +10748,24 @@
       </c>
       <c r="E108" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="109" ht="25" customHeight="1">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>le Roux</t>
+          <t>du Toit</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
         <is>
-          <t>Jeanette</t>
+          <t>Desiree</t>
         </is>
       </c>
       <c r="C109" s="3" t="inlineStr">
         <is>
-          <t>Gonubie</t>
+          <t>Ramsgate</t>
         </is>
       </c>
       <c r="D109" s="3" t="inlineStr">
@@ -10782,17 +10782,17 @@
     <row r="110" ht="25" customHeight="1">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>van Heerden</t>
+          <t>le Roux</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Jeanette</t>
         </is>
       </c>
       <c r="C110" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Gonubie</t>
         </is>
       </c>
       <c r="D110" s="3" t="inlineStr">
@@ -10814,7 +10814,7 @@
       </c>
       <c r="B111" s="3" t="inlineStr">
         <is>
-          <t>Sandy</t>
+          <t>Sydney</t>
         </is>
       </c>
       <c r="C111" s="3" t="inlineStr">
@@ -10829,7 +10829,7 @@
       </c>
       <c r="E111" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -10841,12 +10841,12 @@
       </c>
       <c r="B112" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Sandy</t>
         </is>
       </c>
       <c r="C112" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D112" s="3" t="inlineStr">
@@ -10863,17 +10863,17 @@
     <row r="113" ht="25" customHeight="1">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>van Wyk</t>
+          <t>van Heerden</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C113" s="3" t="inlineStr">
         <is>
-          <t>North Durban</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D113" s="3" t="inlineStr">
@@ -10883,7 +10883,7 @@
       </c>
       <c r="E113" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -10895,12 +10895,12 @@
       </c>
       <c r="B114" s="3" t="inlineStr">
         <is>
-          <t>Lindie</t>
+          <t>Kim</t>
         </is>
       </c>
       <c r="C114" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>North Durban</t>
         </is>
       </c>
       <c r="D114" s="3" t="inlineStr">
@@ -10922,12 +10922,12 @@
       </c>
       <c r="B115" s="3" t="inlineStr">
         <is>
-          <t>Willem</t>
+          <t>Lindie</t>
         </is>
       </c>
       <c r="C115" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D115" s="3" t="inlineStr">
@@ -10949,12 +10949,12 @@
       </c>
       <c r="B116" s="3" t="inlineStr">
         <is>
-          <t>Patricia</t>
+          <t>Willem</t>
         </is>
       </c>
       <c r="C116" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D116" s="3" t="inlineStr">
@@ -10971,49 +10971,49 @@
     <row r="117" ht="25" customHeight="1">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>van der Merwe</t>
+          <t>van Wyk</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
         <is>
-          <t>Ingrid</t>
+          <t>Patricia</t>
         </is>
       </c>
       <c r="C117" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D117" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E117" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="118" ht="25" customHeight="1">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>von der Decken</t>
+          <t>van der Merwe</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
         <is>
-          <t>Brian</t>
+          <t>Ingrid</t>
         </is>
       </c>
       <c r="C118" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D118" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E118" s="3" t="inlineStr">
@@ -11025,39 +11025,66 @@
     <row r="119" ht="25" customHeight="1">
       <c r="A119" s="3" t="inlineStr">
         <is>
+          <t>von der Decken</t>
+        </is>
+      </c>
+      <c r="B119" s="3" t="inlineStr">
+        <is>
+          <t>Brian</t>
+        </is>
+      </c>
+      <c r="C119" s="3" t="inlineStr">
+        <is>
+          <t>King William's Town</t>
+        </is>
+      </c>
+      <c r="D119" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E119" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="120" ht="25" customHeight="1">
+      <c r="A120" s="3" t="inlineStr">
+        <is>
           <t>‘t Hart</t>
         </is>
       </c>
-      <c r="B119" s="3" t="inlineStr">
+      <c r="B120" s="3" t="inlineStr">
         <is>
           <t>Michelle</t>
         </is>
       </c>
-      <c r="C119" s="3" t="inlineStr">
+      <c r="C120" s="3" t="inlineStr">
         <is>
           <t>Benoni Lakes</t>
         </is>
       </c>
-      <c r="D119" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E119" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" s="1" t="inlineStr">
-        <is>
-          <t>Number of attendees: 117</t>
+      <c r="D120" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E120" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="inlineStr">
+        <is>
+          <t>Number of attendees: 118</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="inlineStr">
         <is>
           <t>Number of voters: 60</t>
         </is>
@@ -11093,7 +11120,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Registrees as of 13/04/2021 22:42</t>
+          <t>410W Registrees as of 14/04/2021 14:25</t>
         </is>
       </c>
     </row>
@@ -15188,7 +15215,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Voting details as of 13/04/2021 22:42</t>
+          <t>410E Voting details as of 14/04/2021 14:25</t>
         </is>
       </c>
     </row>
@@ -15525,7 +15552,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Voting details as of 13/04/2021 22:42</t>
+          <t>410W Voting details as of 14/04/2021 14:25</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Registree stats backup on Sun 18 Apr 2021 21:32:10 SAST
</commit_message>
<xml_diff>
--- a/static/docs/registrees_list.xlsx
+++ b/static/docs/registrees_list.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F233"/>
+  <dimension ref="A1:F234"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,7 +451,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>MD410 Registrees as of 16/04/2021 09:40</t>
+          <t>MD410 Registrees as of 18/04/2021 21:32</t>
         </is>
       </c>
     </row>
@@ -5002,17 +5002,17 @@
     <row r="144" ht="25" customHeight="1">
       <c r="A144" s="3" t="inlineStr">
         <is>
-          <t>Pantoleon</t>
+          <t>Paijmans</t>
         </is>
       </c>
       <c r="B144" s="3" t="inlineStr">
         <is>
-          <t>Teresa</t>
+          <t>Bronwyn Anne</t>
         </is>
       </c>
       <c r="C144" s="3" t="inlineStr">
         <is>
-          <t>Vereeniging</t>
+          <t>Cowies Hill</t>
         </is>
       </c>
       <c r="D144" s="3" t="inlineStr">
@@ -5022,7 +5022,7 @@
       </c>
       <c r="E144" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F144" s="3" t="inlineStr">
@@ -5034,17 +5034,17 @@
     <row r="145" ht="25" customHeight="1">
       <c r="A145" s="3" t="inlineStr">
         <is>
-          <t>Peters</t>
+          <t>Pantoleon</t>
         </is>
       </c>
       <c r="B145" s="3" t="inlineStr">
         <is>
-          <t>Maureen</t>
+          <t>Teresa</t>
         </is>
       </c>
       <c r="C145" s="3" t="inlineStr">
         <is>
-          <t>Ceres</t>
+          <t>Vereeniging</t>
         </is>
       </c>
       <c r="D145" s="3" t="inlineStr">
@@ -5059,24 +5059,24 @@
       </c>
       <c r="F145" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="146" ht="25" customHeight="1">
       <c r="A146" s="3" t="inlineStr">
         <is>
-          <t>Pillay</t>
+          <t>Peters</t>
         </is>
       </c>
       <c r="B146" s="3" t="inlineStr">
         <is>
-          <t>Sundru</t>
+          <t>Maureen</t>
         </is>
       </c>
       <c r="C146" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>Ceres</t>
         </is>
       </c>
       <c r="D146" s="3" t="inlineStr">
@@ -5086,7 +5086,7 @@
       </c>
       <c r="E146" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F146" s="3" t="inlineStr">
@@ -5103,12 +5103,12 @@
       </c>
       <c r="B147" s="3" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>Sundru</t>
         </is>
       </c>
       <c r="C147" s="3" t="inlineStr">
         <is>
-          <t>Tygerberg Hills</t>
+          <t>Durbanville</t>
         </is>
       </c>
       <c r="D147" s="3" t="inlineStr">
@@ -5118,7 +5118,7 @@
       </c>
       <c r="E147" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F147" s="3" t="inlineStr">
@@ -5130,17 +5130,17 @@
     <row r="148" ht="25" customHeight="1">
       <c r="A148" s="3" t="inlineStr">
         <is>
-          <t>Polkinghorne</t>
+          <t>Pillay</t>
         </is>
       </c>
       <c r="B148" s="3" t="inlineStr">
         <is>
-          <t>Tracey</t>
+          <t>Patrick</t>
         </is>
       </c>
       <c r="C148" s="3" t="inlineStr">
         <is>
-          <t>Kensington</t>
+          <t>Tygerberg Hills</t>
         </is>
       </c>
       <c r="D148" s="3" t="inlineStr">
@@ -5155,7 +5155,7 @@
       </c>
       <c r="F148" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -5167,7 +5167,7 @@
       </c>
       <c r="B149" s="3" t="inlineStr">
         <is>
-          <t>Gavin</t>
+          <t>Tracey</t>
         </is>
       </c>
       <c r="C149" s="3" t="inlineStr">
@@ -5182,7 +5182,7 @@
       </c>
       <c r="E149" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F149" s="3" t="inlineStr">
@@ -5194,22 +5194,22 @@
     <row r="150" ht="25" customHeight="1">
       <c r="A150" s="3" t="inlineStr">
         <is>
-          <t>Pretorius</t>
+          <t>Polkinghorne</t>
         </is>
       </c>
       <c r="B150" s="3" t="inlineStr">
         <is>
-          <t>Sheldon Edmund</t>
+          <t>Gavin</t>
         </is>
       </c>
       <c r="C150" s="3" t="inlineStr">
         <is>
-          <t>Merriman</t>
+          <t>Kensington</t>
         </is>
       </c>
       <c r="D150" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E150" s="3" t="inlineStr">
@@ -5219,29 +5219,29 @@
       </c>
       <c r="F150" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="151" ht="25" customHeight="1">
       <c r="A151" s="3" t="inlineStr">
         <is>
-          <t>Ras</t>
+          <t>Pretorius</t>
         </is>
       </c>
       <c r="B151" s="3" t="inlineStr">
         <is>
-          <t>Mary-Anne</t>
+          <t>Sheldon Edmund</t>
         </is>
       </c>
       <c r="C151" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Merriman</t>
         </is>
       </c>
       <c r="D151" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E151" s="3" t="inlineStr">
@@ -5263,7 +5263,7 @@
       </c>
       <c r="B152" s="3" t="inlineStr">
         <is>
-          <t>Leon Jacobus</t>
+          <t>Mary-Anne</t>
         </is>
       </c>
       <c r="C152" s="3" t="inlineStr">
@@ -5283,24 +5283,24 @@
       </c>
       <c r="F152" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="153" ht="25" customHeight="1">
       <c r="A153" s="3" t="inlineStr">
         <is>
-          <t>Reniers</t>
+          <t>Ras</t>
         </is>
       </c>
       <c r="B153" s="3" t="inlineStr">
         <is>
-          <t>Hugo</t>
+          <t>Leon Jacobus</t>
         </is>
       </c>
       <c r="C153" s="3" t="inlineStr">
         <is>
-          <t>Nelspruit</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D153" s="3" t="inlineStr">
@@ -5310,7 +5310,7 @@
       </c>
       <c r="E153" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F153" s="3" t="inlineStr">
@@ -5322,17 +5322,17 @@
     <row r="154" ht="25" customHeight="1">
       <c r="A154" s="3" t="inlineStr">
         <is>
-          <t>Roman</t>
+          <t>Reniers</t>
         </is>
       </c>
       <c r="B154" s="3" t="inlineStr">
         <is>
-          <t>Sandy</t>
+          <t>Hugo</t>
         </is>
       </c>
       <c r="C154" s="3" t="inlineStr">
         <is>
-          <t>Bergvliet</t>
+          <t>Nelspruit</t>
         </is>
       </c>
       <c r="D154" s="3" t="inlineStr">
@@ -5342,29 +5342,29 @@
       </c>
       <c r="E154" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F154" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="155" ht="25" customHeight="1">
       <c r="A155" s="3" t="inlineStr">
         <is>
-          <t>Rossouw</t>
+          <t>Roman</t>
         </is>
       </c>
       <c r="B155" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Sandy</t>
         </is>
       </c>
       <c r="C155" s="3" t="inlineStr">
         <is>
-          <t>Tokai</t>
+          <t>Bergvliet</t>
         </is>
       </c>
       <c r="D155" s="3" t="inlineStr">
@@ -5374,7 +5374,7 @@
       </c>
       <c r="E155" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F155" s="3" t="inlineStr">
@@ -5386,17 +5386,17 @@
     <row r="156" ht="25" customHeight="1">
       <c r="A156" s="3" t="inlineStr">
         <is>
-          <t>Rothner</t>
+          <t>Rossouw</t>
         </is>
       </c>
       <c r="B156" s="3" t="inlineStr">
         <is>
-          <t>Andrea</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C156" s="3" t="inlineStr">
         <is>
-          <t>Eden</t>
+          <t>Tokai</t>
         </is>
       </c>
       <c r="D156" s="3" t="inlineStr">
@@ -5406,7 +5406,7 @@
       </c>
       <c r="E156" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F156" s="3" t="inlineStr">
@@ -5418,17 +5418,17 @@
     <row r="157" ht="25" customHeight="1">
       <c r="A157" s="3" t="inlineStr">
         <is>
-          <t>Roux</t>
+          <t>Rothner</t>
         </is>
       </c>
       <c r="B157" s="3" t="inlineStr">
         <is>
-          <t>Anthonie Petrus</t>
+          <t>Andrea</t>
         </is>
       </c>
       <c r="C157" s="3" t="inlineStr">
         <is>
-          <t>Moorreesburg</t>
+          <t>Eden</t>
         </is>
       </c>
       <c r="D157" s="3" t="inlineStr">
@@ -5438,7 +5438,7 @@
       </c>
       <c r="E157" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F157" s="3" t="inlineStr">
@@ -5450,17 +5450,17 @@
     <row r="158" ht="25" customHeight="1">
       <c r="A158" s="3" t="inlineStr">
         <is>
-          <t>Russell</t>
+          <t>Roux</t>
         </is>
       </c>
       <c r="B158" s="3" t="inlineStr">
         <is>
-          <t>Ingrid</t>
+          <t>Anthonie Petrus</t>
         </is>
       </c>
       <c r="C158" s="3" t="inlineStr">
         <is>
-          <t>Fish Hoek</t>
+          <t>Moorreesburg</t>
         </is>
       </c>
       <c r="D158" s="3" t="inlineStr">
@@ -5482,27 +5482,27 @@
     <row r="159" ht="25" customHeight="1">
       <c r="A159" s="3" t="inlineStr">
         <is>
-          <t>SNYMAN</t>
+          <t>Russell</t>
         </is>
       </c>
       <c r="B159" s="3" t="inlineStr">
         <is>
-          <t>LYN</t>
+          <t>Ingrid</t>
         </is>
       </c>
       <c r="C159" s="3" t="inlineStr">
         <is>
-          <t>Deep South</t>
+          <t>Fish Hoek</t>
         </is>
       </c>
       <c r="D159" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E159" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F159" s="3" t="inlineStr">
@@ -5514,27 +5514,27 @@
     <row r="160" ht="25" customHeight="1">
       <c r="A160" s="3" t="inlineStr">
         <is>
-          <t>STEENBERG</t>
+          <t>SNYMAN</t>
         </is>
       </c>
       <c r="B160" s="3" t="inlineStr">
         <is>
-          <t>TIM</t>
+          <t>LYN</t>
         </is>
       </c>
       <c r="C160" s="3" t="inlineStr">
         <is>
-          <t>Wellington</t>
+          <t>Deep South</t>
         </is>
       </c>
       <c r="D160" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E160" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F160" s="3" t="inlineStr">
@@ -5546,17 +5546,17 @@
     <row r="161" ht="25" customHeight="1">
       <c r="A161" s="3" t="inlineStr">
         <is>
-          <t>Sabatier</t>
+          <t>STEENBERG</t>
         </is>
       </c>
       <c r="B161" s="3" t="inlineStr">
         <is>
-          <t>Rodney</t>
+          <t>TIM</t>
         </is>
       </c>
       <c r="C161" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Wellington</t>
         </is>
       </c>
       <c r="D161" s="3" t="inlineStr">
@@ -5571,24 +5571,24 @@
       </c>
       <c r="F161" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="162" ht="25" customHeight="1">
       <c r="A162" s="3" t="inlineStr">
         <is>
-          <t>Sampie</t>
+          <t>Sabatier</t>
         </is>
       </c>
       <c r="B162" s="3" t="inlineStr">
         <is>
-          <t>Sharon</t>
+          <t>Rodney</t>
         </is>
       </c>
       <c r="C162" s="3" t="inlineStr">
         <is>
-          <t>Bergvliet</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D162" s="3" t="inlineStr">
@@ -5603,24 +5603,24 @@
       </c>
       <c r="F162" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="163" ht="25" customHeight="1">
       <c r="A163" s="3" t="inlineStr">
         <is>
-          <t>Schatz</t>
+          <t>Sampie</t>
         </is>
       </c>
       <c r="B163" s="3" t="inlineStr">
         <is>
-          <t>Vera</t>
+          <t>Sharon</t>
         </is>
       </c>
       <c r="C163" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Bergvliet</t>
         </is>
       </c>
       <c r="D163" s="3" t="inlineStr">
@@ -5647,7 +5647,7 @@
       </c>
       <c r="B164" s="3" t="inlineStr">
         <is>
-          <t>Frank</t>
+          <t>Vera</t>
         </is>
       </c>
       <c r="C164" s="3" t="inlineStr">
@@ -5674,17 +5674,17 @@
     <row r="165" ht="25" customHeight="1">
       <c r="A165" s="3" t="inlineStr">
         <is>
-          <t>Searle</t>
+          <t>Schatz</t>
         </is>
       </c>
       <c r="B165" s="3" t="inlineStr">
         <is>
-          <t>Francis</t>
+          <t>Frank</t>
         </is>
       </c>
       <c r="C165" s="3" t="inlineStr">
         <is>
-          <t>Kouga</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D165" s="3" t="inlineStr">
@@ -5699,7 +5699,7 @@
       </c>
       <c r="F165" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -5711,7 +5711,7 @@
       </c>
       <c r="B166" s="3" t="inlineStr">
         <is>
-          <t>Gloria</t>
+          <t>Francis</t>
         </is>
       </c>
       <c r="C166" s="3" t="inlineStr">
@@ -5726,7 +5726,7 @@
       </c>
       <c r="E166" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F166" s="3" t="inlineStr">
@@ -5738,17 +5738,17 @@
     <row r="167" ht="25" customHeight="1">
       <c r="A167" s="3" t="inlineStr">
         <is>
-          <t>Sell</t>
+          <t>Searle</t>
         </is>
       </c>
       <c r="B167" s="3" t="inlineStr">
         <is>
-          <t>Ami</t>
+          <t>Gloria</t>
         </is>
       </c>
       <c r="C167" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Kouga</t>
         </is>
       </c>
       <c r="D167" s="3" t="inlineStr">
@@ -5763,24 +5763,24 @@
       </c>
       <c r="F167" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="168" ht="25" customHeight="1">
       <c r="A168" s="3" t="inlineStr">
         <is>
-          <t>Simpson</t>
+          <t>Sell</t>
         </is>
       </c>
       <c r="B168" s="3" t="inlineStr">
         <is>
-          <t>Beryl</t>
+          <t>Ami</t>
         </is>
       </c>
       <c r="C168" s="3" t="inlineStr">
         <is>
-          <t>Cape Town</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D168" s="3" t="inlineStr">
@@ -5802,17 +5802,17 @@
     <row r="169" ht="25" customHeight="1">
       <c r="A169" s="3" t="inlineStr">
         <is>
-          <t>Sircoulomb</t>
+          <t>Simpson</t>
         </is>
       </c>
       <c r="B169" s="3" t="inlineStr">
         <is>
-          <t>Kenlis</t>
+          <t>Beryl</t>
         </is>
       </c>
       <c r="C169" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Cape Town</t>
         </is>
       </c>
       <c r="D169" s="3" t="inlineStr">
@@ -5839,7 +5839,7 @@
       </c>
       <c r="B170" s="3" t="inlineStr">
         <is>
-          <t>Holger</t>
+          <t>Kenlis</t>
         </is>
       </c>
       <c r="C170" s="3" t="inlineStr">
@@ -5866,12 +5866,12 @@
     <row r="171" ht="25" customHeight="1">
       <c r="A171" s="3" t="inlineStr">
         <is>
-          <t>Smeer</t>
+          <t>Sircoulomb</t>
         </is>
       </c>
       <c r="B171" s="3" t="inlineStr">
         <is>
-          <t>Hennie</t>
+          <t>Holger</t>
         </is>
       </c>
       <c r="C171" s="3" t="inlineStr">
@@ -5881,12 +5881,12 @@
       </c>
       <c r="D171" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E171" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F171" s="3" t="inlineStr">
@@ -5898,22 +5898,22 @@
     <row r="172" ht="25" customHeight="1">
       <c r="A172" s="3" t="inlineStr">
         <is>
-          <t>Smit</t>
+          <t>Smeer</t>
         </is>
       </c>
       <c r="B172" s="3" t="inlineStr">
         <is>
-          <t>Sue</t>
+          <t>Hennie</t>
         </is>
       </c>
       <c r="C172" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D172" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E172" s="3" t="inlineStr">
@@ -5923,7 +5923,7 @@
       </c>
       <c r="F172" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -5935,12 +5935,12 @@
       </c>
       <c r="B173" s="3" t="inlineStr">
         <is>
-          <t>Herman</t>
+          <t>Sue</t>
         </is>
       </c>
       <c r="C173" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D173" s="3" t="inlineStr">
@@ -5950,29 +5950,29 @@
       </c>
       <c r="E173" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F173" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="174" ht="25" customHeight="1">
       <c r="A174" s="3" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Smit</t>
         </is>
       </c>
       <c r="B174" s="3" t="inlineStr">
         <is>
-          <t>Jeff</t>
+          <t>Herman</t>
         </is>
       </c>
       <c r="C174" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D174" s="3" t="inlineStr">
@@ -5987,7 +5987,7 @@
       </c>
       <c r="F174" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -5999,12 +5999,12 @@
       </c>
       <c r="B175" s="3" t="inlineStr">
         <is>
-          <t>Bennie</t>
+          <t>Jeff</t>
         </is>
       </c>
       <c r="C175" s="3" t="inlineStr">
         <is>
-          <t>Wellington</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D175" s="3" t="inlineStr">
@@ -6014,12 +6014,12 @@
       </c>
       <c r="E175" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F175" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -6031,12 +6031,12 @@
       </c>
       <c r="B176" s="3" t="inlineStr">
         <is>
-          <t>Carmen Dolores</t>
+          <t>Bennie</t>
         </is>
       </c>
       <c r="C176" s="3" t="inlineStr">
         <is>
-          <t>Tokai</t>
+          <t>Wellington</t>
         </is>
       </c>
       <c r="D176" s="3" t="inlineStr">
@@ -6046,7 +6046,7 @@
       </c>
       <c r="E176" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F176" s="3" t="inlineStr">
@@ -6063,7 +6063,7 @@
       </c>
       <c r="B177" s="3" t="inlineStr">
         <is>
-          <t>David John</t>
+          <t>Carmen Dolores</t>
         </is>
       </c>
       <c r="C177" s="3" t="inlineStr">
@@ -6090,17 +6090,17 @@
     <row r="178" ht="25" customHeight="1">
       <c r="A178" s="3" t="inlineStr">
         <is>
-          <t>Sochen</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="B178" s="3" t="inlineStr">
         <is>
-          <t>Diana</t>
+          <t>David John</t>
         </is>
       </c>
       <c r="C178" s="3" t="inlineStr">
         <is>
-          <t>Sea Point</t>
+          <t>Tokai</t>
         </is>
       </c>
       <c r="D178" s="3" t="inlineStr">
@@ -6110,7 +6110,7 @@
       </c>
       <c r="E178" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F178" s="3" t="inlineStr">
@@ -6122,49 +6122,49 @@
     <row r="179" ht="25" customHeight="1">
       <c r="A179" s="3" t="inlineStr">
         <is>
-          <t>Steyn</t>
+          <t>Sochen</t>
         </is>
       </c>
       <c r="B179" s="3" t="inlineStr">
         <is>
-          <t>Elna</t>
+          <t>Diana</t>
         </is>
       </c>
       <c r="C179" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Sea Point</t>
         </is>
       </c>
       <c r="D179" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E179" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F179" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="180" ht="25" customHeight="1">
       <c r="A180" s="3" t="inlineStr">
         <is>
-          <t>Strauss</t>
+          <t>Steyn</t>
         </is>
       </c>
       <c r="B180" s="3" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>Elna</t>
         </is>
       </c>
       <c r="C180" s="3" t="inlineStr">
         <is>
-          <t>Kuilsriver</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D180" s="3" t="inlineStr">
@@ -6179,29 +6179,29 @@
       </c>
       <c r="F180" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="181" ht="25" customHeight="1">
       <c r="A181" s="3" t="inlineStr">
         <is>
-          <t>Sturges</t>
+          <t>Strauss</t>
         </is>
       </c>
       <c r="B181" s="3" t="inlineStr">
         <is>
-          <t>Trevor</t>
+          <t>Patrick</t>
         </is>
       </c>
       <c r="C181" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Kuilsriver</t>
         </is>
       </c>
       <c r="D181" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E181" s="3" t="inlineStr">
@@ -6211,24 +6211,24 @@
       </c>
       <c r="F181" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="182" ht="25" customHeight="1">
       <c r="A182" s="3" t="inlineStr">
         <is>
-          <t>Talbot</t>
+          <t>Sturges</t>
         </is>
       </c>
       <c r="B182" s="3" t="inlineStr">
         <is>
-          <t>Lauryn</t>
+          <t>Trevor</t>
         </is>
       </c>
       <c r="C182" s="3" t="inlineStr">
         <is>
-          <t>Benoni Lakes</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D182" s="3" t="inlineStr">
@@ -6250,17 +6250,17 @@
     <row r="183" ht="25" customHeight="1">
       <c r="A183" s="3" t="inlineStr">
         <is>
-          <t>Theron</t>
+          <t>Talbot</t>
         </is>
       </c>
       <c r="B183" s="3" t="inlineStr">
         <is>
-          <t>Pierre</t>
+          <t>Lauryn</t>
         </is>
       </c>
       <c r="C183" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Benoni Lakes</t>
         </is>
       </c>
       <c r="D183" s="3" t="inlineStr">
@@ -6287,7 +6287,7 @@
       </c>
       <c r="B184" s="3" t="inlineStr">
         <is>
-          <t>Moira</t>
+          <t>Pierre</t>
         </is>
       </c>
       <c r="C184" s="3" t="inlineStr">
@@ -6314,22 +6314,22 @@
     <row r="185" ht="25" customHeight="1">
       <c r="A185" s="3" t="inlineStr">
         <is>
-          <t>Toye</t>
+          <t>Theron</t>
         </is>
       </c>
       <c r="B185" s="3" t="inlineStr">
         <is>
-          <t>Omolayo</t>
+          <t>Moira</t>
         </is>
       </c>
       <c r="C185" s="3" t="inlineStr">
         <is>
-          <t>The Wilds</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D185" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E185" s="3" t="inlineStr">
@@ -6346,22 +6346,22 @@
     <row r="186" ht="25" customHeight="1">
       <c r="A186" s="3" t="inlineStr">
         <is>
-          <t>Tshikala</t>
+          <t>Toye</t>
         </is>
       </c>
       <c r="B186" s="3" t="inlineStr">
         <is>
-          <t>David Alex</t>
+          <t>Omolayo</t>
         </is>
       </c>
       <c r="C186" s="3" t="inlineStr">
         <is>
-          <t>Athlone</t>
+          <t>The Wilds</t>
         </is>
       </c>
       <c r="D186" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E186" s="3" t="inlineStr">
@@ -6371,24 +6371,24 @@
       </c>
       <c r="F186" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="187" ht="25" customHeight="1">
       <c r="A187" s="3" t="inlineStr">
         <is>
-          <t>Tuckett</t>
+          <t>Tshikala</t>
         </is>
       </c>
       <c r="B187" s="3" t="inlineStr">
         <is>
-          <t>Alistair</t>
+          <t>David Alex</t>
         </is>
       </c>
       <c r="C187" s="3" t="inlineStr">
         <is>
-          <t>Roodepoort Clearwater Cyber</t>
+          <t>Athlone</t>
         </is>
       </c>
       <c r="D187" s="3" t="inlineStr">
@@ -6403,7 +6403,7 @@
       </c>
       <c r="F187" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -6415,7 +6415,7 @@
       </c>
       <c r="B188" s="3" t="inlineStr">
         <is>
-          <t>Rowan</t>
+          <t>Alistair</t>
         </is>
       </c>
       <c r="C188" s="3" t="inlineStr">
@@ -6430,7 +6430,7 @@
       </c>
       <c r="E188" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F188" s="3" t="inlineStr">
@@ -6447,7 +6447,7 @@
       </c>
       <c r="B189" s="3" t="inlineStr">
         <is>
-          <t>Gail</t>
+          <t>Rowan</t>
         </is>
       </c>
       <c r="C189" s="3" t="inlineStr">
@@ -6462,7 +6462,7 @@
       </c>
       <c r="E189" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F189" s="3" t="inlineStr">
@@ -6474,17 +6474,17 @@
     <row r="190" ht="25" customHeight="1">
       <c r="A190" s="3" t="inlineStr">
         <is>
-          <t>VAN BREDA</t>
+          <t>Tuckett</t>
         </is>
       </c>
       <c r="B190" s="3" t="inlineStr">
         <is>
-          <t>HILARY LISE</t>
+          <t>Gail</t>
         </is>
       </c>
       <c r="C190" s="3" t="inlineStr">
         <is>
-          <t>Cape Town</t>
+          <t>Roodepoort Clearwater Cyber</t>
         </is>
       </c>
       <c r="D190" s="3" t="inlineStr">
@@ -6499,39 +6499,39 @@
       </c>
       <c r="F190" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="191" ht="25" customHeight="1">
       <c r="A191" s="3" t="inlineStr">
         <is>
-          <t>VAN DER MERWE</t>
+          <t>VAN BREDA</t>
         </is>
       </c>
       <c r="B191" s="3" t="inlineStr">
         <is>
-          <t>PATRICIA</t>
+          <t>HILARY LISE</t>
         </is>
       </c>
       <c r="C191" s="3" t="inlineStr">
         <is>
-          <t>East London Port Rex</t>
+          <t>Cape Town</t>
         </is>
       </c>
       <c r="D191" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E191" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F191" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -6543,17 +6543,17 @@
       </c>
       <c r="B192" s="3" t="inlineStr">
         <is>
-          <t>MARINA</t>
+          <t>PATRICIA</t>
         </is>
       </c>
       <c r="C192" s="3" t="inlineStr">
         <is>
-          <t>Malmesbury</t>
+          <t>East London Port Rex</t>
         </is>
       </c>
       <c r="D192" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E192" s="3" t="inlineStr">
@@ -6563,56 +6563,56 @@
       </c>
       <c r="F192" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="193" ht="25" customHeight="1">
       <c r="A193" s="3" t="inlineStr">
         <is>
-          <t>Valadao</t>
+          <t>VAN DER MERWE</t>
         </is>
       </c>
       <c r="B193" s="3" t="inlineStr">
         <is>
-          <t>Tracy</t>
+          <t>MARINA</t>
         </is>
       </c>
       <c r="C193" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Malmesbury</t>
         </is>
       </c>
       <c r="D193" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E193" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F193" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="194" ht="25" customHeight="1">
       <c r="A194" s="3" t="inlineStr">
         <is>
-          <t>Van Niekerk</t>
+          <t>Valadao</t>
         </is>
       </c>
       <c r="B194" s="3" t="inlineStr">
         <is>
-          <t>Riaan</t>
+          <t>Tracy</t>
         </is>
       </c>
       <c r="C194" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D194" s="3" t="inlineStr">
@@ -6634,59 +6634,59 @@
     <row r="195" ht="25" customHeight="1">
       <c r="A195" s="3" t="inlineStr">
         <is>
-          <t>Van Rensburg</t>
+          <t>Van Niekerk</t>
         </is>
       </c>
       <c r="B195" s="3" t="inlineStr">
         <is>
-          <t>Neville</t>
+          <t>Riaan</t>
         </is>
       </c>
       <c r="C195" s="3" t="inlineStr">
         <is>
-          <t>Moorreesburg</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D195" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E195" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F195" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="196" ht="25" customHeight="1">
       <c r="A196" s="3" t="inlineStr">
         <is>
-          <t>Van Romburgh</t>
+          <t>Van Rensburg</t>
         </is>
       </c>
       <c r="B196" s="3" t="inlineStr">
         <is>
-          <t>Lorna</t>
+          <t>Neville</t>
         </is>
       </c>
       <c r="C196" s="3" t="inlineStr">
         <is>
-          <t>Fish Hoek</t>
+          <t>Moorreesburg</t>
         </is>
       </c>
       <c r="D196" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E196" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F196" s="3" t="inlineStr">
@@ -6698,17 +6698,17 @@
     <row r="197" ht="25" customHeight="1">
       <c r="A197" s="3" t="inlineStr">
         <is>
-          <t>Van Wyk-Nelson</t>
+          <t>Van Romburgh</t>
         </is>
       </c>
       <c r="B197" s="3" t="inlineStr">
         <is>
-          <t>Edith</t>
+          <t>Lorna</t>
         </is>
       </c>
       <c r="C197" s="3" t="inlineStr">
         <is>
-          <t>Kuilsriver</t>
+          <t>Fish Hoek</t>
         </is>
       </c>
       <c r="D197" s="3" t="inlineStr">
@@ -6730,22 +6730,22 @@
     <row r="198" ht="25" customHeight="1">
       <c r="A198" s="3" t="inlineStr">
         <is>
-          <t>Van de Merwe</t>
+          <t>Van Wyk-Nelson</t>
         </is>
       </c>
       <c r="B198" s="3" t="inlineStr">
         <is>
-          <t>Marina</t>
+          <t>Edith</t>
         </is>
       </c>
       <c r="C198" s="3" t="inlineStr">
         <is>
-          <t>Malmesbury</t>
+          <t>Kuilsriver</t>
         </is>
       </c>
       <c r="D198" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E198" s="3" t="inlineStr">
@@ -6762,54 +6762,54 @@
     <row r="199" ht="25" customHeight="1">
       <c r="A199" s="3" t="inlineStr">
         <is>
-          <t>Venter</t>
+          <t>Van de Merwe</t>
         </is>
       </c>
       <c r="B199" s="3" t="inlineStr">
         <is>
-          <t>Louis</t>
+          <t>Marina</t>
         </is>
       </c>
       <c r="C199" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Malmesbury</t>
         </is>
       </c>
       <c r="D199" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E199" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F199" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="200" ht="25" customHeight="1">
       <c r="A200" s="3" t="inlineStr">
         <is>
-          <t>Volker</t>
+          <t>Venter</t>
         </is>
       </c>
       <c r="B200" s="3" t="inlineStr">
         <is>
-          <t>Russell</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="C200" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D200" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E200" s="3" t="inlineStr">
@@ -6826,96 +6826,96 @@
     <row r="201" ht="25" customHeight="1">
       <c r="A201" s="3" t="inlineStr">
         <is>
-          <t>Von Mollendorf</t>
+          <t>Volker</t>
         </is>
       </c>
       <c r="B201" s="3" t="inlineStr">
         <is>
-          <t>Rinette</t>
+          <t>Russell</t>
         </is>
       </c>
       <c r="C201" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>King William's Town</t>
         </is>
       </c>
       <c r="D201" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E201" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F201" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="202" ht="25" customHeight="1">
       <c r="A202" s="3" t="inlineStr">
         <is>
-          <t>Warman</t>
+          <t>Von Mollendorf</t>
         </is>
       </c>
       <c r="B202" s="3" t="inlineStr">
         <is>
-          <t>Alastair</t>
+          <t>Rinette</t>
         </is>
       </c>
       <c r="C202" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Durbanville</t>
         </is>
       </c>
       <c r="D202" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E202" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F202" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="203" ht="25" customHeight="1">
       <c r="A203" s="3" t="inlineStr">
         <is>
-          <t>Watson</t>
+          <t>Warman</t>
         </is>
       </c>
       <c r="B203" s="3" t="inlineStr">
         <is>
-          <t>Allan</t>
+          <t>Alastair</t>
         </is>
       </c>
       <c r="C203" s="3" t="inlineStr">
         <is>
-          <t>Sea Point</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D203" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E203" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F203" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -6927,22 +6927,22 @@
       </c>
       <c r="B204" s="3" t="inlineStr">
         <is>
-          <t>Alison</t>
+          <t>Allan</t>
         </is>
       </c>
       <c r="C204" s="3" t="inlineStr">
         <is>
-          <t>Sedgefield</t>
+          <t>Sea Point</t>
         </is>
       </c>
       <c r="D204" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E204" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F204" s="3" t="inlineStr">
@@ -6954,27 +6954,27 @@
     <row r="205" ht="25" customHeight="1">
       <c r="A205" s="3" t="inlineStr">
         <is>
-          <t>Williams</t>
+          <t>Watson</t>
         </is>
       </c>
       <c r="B205" s="3" t="inlineStr">
         <is>
-          <t>Johanna</t>
+          <t>Alison</t>
         </is>
       </c>
       <c r="C205" s="3" t="inlineStr">
         <is>
-          <t>Mitchells Plain</t>
+          <t>Sedgefield</t>
         </is>
       </c>
       <c r="D205" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E205" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F205" s="3" t="inlineStr">
@@ -6986,22 +6986,22 @@
     <row r="206" ht="25" customHeight="1">
       <c r="A206" s="3" t="inlineStr">
         <is>
-          <t>Wills</t>
+          <t>Williams</t>
         </is>
       </c>
       <c r="B206" s="3" t="inlineStr">
         <is>
-          <t>Geila</t>
+          <t>Johanna</t>
         </is>
       </c>
       <c r="C206" s="3" t="inlineStr">
         <is>
-          <t>Athlone</t>
+          <t>Mitchells Plain</t>
         </is>
       </c>
       <c r="D206" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E206" s="3" t="inlineStr">
@@ -7018,17 +7018,17 @@
     <row r="207" ht="25" customHeight="1">
       <c r="A207" s="3" t="inlineStr">
         <is>
-          <t>Wilter-Sturges</t>
+          <t>Wills</t>
         </is>
       </c>
       <c r="B207" s="3" t="inlineStr">
         <is>
-          <t>Meredith</t>
+          <t>Geila</t>
         </is>
       </c>
       <c r="C207" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Athlone</t>
         </is>
       </c>
       <c r="D207" s="3" t="inlineStr">
@@ -7043,24 +7043,24 @@
       </c>
       <c r="F207" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="208" ht="25" customHeight="1">
       <c r="A208" s="3" t="inlineStr">
         <is>
-          <t>Wright</t>
+          <t>Wilter-Sturges</t>
         </is>
       </c>
       <c r="B208" s="3" t="inlineStr">
         <is>
-          <t>Rocky</t>
+          <t>Meredith</t>
         </is>
       </c>
       <c r="C208" s="3" t="inlineStr">
         <is>
-          <t>Table View</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D208" s="3" t="inlineStr">
@@ -7070,29 +7070,29 @@
       </c>
       <c r="E208" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F208" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="209" ht="25" customHeight="1">
       <c r="A209" s="3" t="inlineStr">
         <is>
-          <t>Young</t>
+          <t>Wright</t>
         </is>
       </c>
       <c r="B209" s="3" t="inlineStr">
         <is>
-          <t>Judy</t>
+          <t>Rocky</t>
         </is>
       </c>
       <c r="C209" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>Table View</t>
         </is>
       </c>
       <c r="D209" s="3" t="inlineStr">
@@ -7102,7 +7102,7 @@
       </c>
       <c r="E209" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F209" s="3" t="inlineStr">
@@ -7114,17 +7114,17 @@
     <row r="210" ht="25" customHeight="1">
       <c r="A210" s="3" t="inlineStr">
         <is>
-          <t>de Kock</t>
+          <t>Young</t>
         </is>
       </c>
       <c r="B210" s="3" t="inlineStr">
         <is>
-          <t>Engela</t>
+          <t>Judy</t>
         </is>
       </c>
       <c r="C210" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Durbanville</t>
         </is>
       </c>
       <c r="D210" s="3" t="inlineStr">
@@ -7134,7 +7134,7 @@
       </c>
       <c r="E210" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F210" s="3" t="inlineStr">
@@ -7151,7 +7151,7 @@
       </c>
       <c r="B211" s="3" t="inlineStr">
         <is>
-          <t>Francois</t>
+          <t>Engela</t>
         </is>
       </c>
       <c r="C211" s="3" t="inlineStr">
@@ -7178,54 +7178,54 @@
     <row r="212" ht="25" customHeight="1">
       <c r="A212" s="3" t="inlineStr">
         <is>
-          <t>de Silva</t>
+          <t>de Kock</t>
         </is>
       </c>
       <c r="B212" s="3" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Francois</t>
         </is>
       </c>
       <c r="C212" s="3" t="inlineStr">
         <is>
-          <t>Edenvale</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D212" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E212" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F212" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="213" ht="25" customHeight="1">
       <c r="A213" s="3" t="inlineStr">
         <is>
-          <t>du Toit</t>
+          <t>de Silva</t>
         </is>
       </c>
       <c r="B213" s="3" t="inlineStr">
         <is>
-          <t>Desiree</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="C213" s="3" t="inlineStr">
         <is>
-          <t>Ramsgate</t>
+          <t>Edenvale</t>
         </is>
       </c>
       <c r="D213" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E213" s="3" t="inlineStr">
@@ -7242,59 +7242,59 @@
     <row r="214" ht="25" customHeight="1">
       <c r="A214" s="3" t="inlineStr">
         <is>
-          <t>stier</t>
+          <t>du Toit</t>
         </is>
       </c>
       <c r="B214" s="3" t="inlineStr">
         <is>
-          <t>RORY</t>
+          <t>Desiree</t>
         </is>
       </c>
       <c r="C214" s="3" t="inlineStr">
         <is>
-          <t>Deep South</t>
+          <t>Ramsgate</t>
         </is>
       </c>
       <c r="D214" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E214" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F214" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="215" ht="25" customHeight="1">
       <c r="A215" s="3" t="inlineStr">
         <is>
-          <t>van Blerk</t>
+          <t>stier</t>
         </is>
       </c>
       <c r="B215" s="3" t="inlineStr">
         <is>
-          <t>Carl</t>
+          <t>RORY</t>
         </is>
       </c>
       <c r="C215" s="3" t="inlineStr">
         <is>
-          <t>Eden</t>
+          <t>Deep South</t>
         </is>
       </c>
       <c r="D215" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E215" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F215" s="3" t="inlineStr">
@@ -7306,17 +7306,17 @@
     <row r="216" ht="25" customHeight="1">
       <c r="A216" s="3" t="inlineStr">
         <is>
-          <t>van Heerden</t>
+          <t>van Blerk</t>
         </is>
       </c>
       <c r="B216" s="3" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Carl</t>
         </is>
       </c>
       <c r="C216" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Eden</t>
         </is>
       </c>
       <c r="D216" s="3" t="inlineStr">
@@ -7331,7 +7331,7 @@
       </c>
       <c r="F216" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -7343,7 +7343,7 @@
       </c>
       <c r="B217" s="3" t="inlineStr">
         <is>
-          <t>Sandy</t>
+          <t>Sydney</t>
         </is>
       </c>
       <c r="C217" s="3" t="inlineStr">
@@ -7358,7 +7358,7 @@
       </c>
       <c r="E217" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F217" s="3" t="inlineStr">
@@ -7375,12 +7375,12 @@
       </c>
       <c r="B218" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Sandy</t>
         </is>
       </c>
       <c r="C218" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D218" s="3" t="inlineStr">
@@ -7402,17 +7402,17 @@
     <row r="219" ht="25" customHeight="1">
       <c r="A219" s="3" t="inlineStr">
         <is>
-          <t>van Rensburg</t>
+          <t>van Heerden</t>
         </is>
       </c>
       <c r="B219" s="3" t="inlineStr">
         <is>
-          <t>Johan</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C219" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D219" s="3" t="inlineStr">
@@ -7427,7 +7427,7 @@
       </c>
       <c r="F219" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -7439,7 +7439,7 @@
       </c>
       <c r="B220" s="3" t="inlineStr">
         <is>
-          <t>Anne</t>
+          <t>Johan</t>
         </is>
       </c>
       <c r="C220" s="3" t="inlineStr">
@@ -7454,7 +7454,7 @@
       </c>
       <c r="E220" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F220" s="3" t="inlineStr">
@@ -7466,17 +7466,17 @@
     <row r="221" ht="25" customHeight="1">
       <c r="A221" s="3" t="inlineStr">
         <is>
-          <t>van Wulven</t>
+          <t>van Rensburg</t>
         </is>
       </c>
       <c r="B221" s="3" t="inlineStr">
         <is>
-          <t>Jeannie</t>
+          <t>Anne</t>
         </is>
       </c>
       <c r="C221" s="3" t="inlineStr">
         <is>
-          <t>Tygerberg Hills</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D221" s="3" t="inlineStr">
@@ -7486,7 +7486,7 @@
       </c>
       <c r="E221" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F221" s="3" t="inlineStr">
@@ -7503,7 +7503,7 @@
       </c>
       <c r="B222" s="3" t="inlineStr">
         <is>
-          <t>Alan</t>
+          <t>Jeannie</t>
         </is>
       </c>
       <c r="C222" s="3" t="inlineStr">
@@ -7518,7 +7518,7 @@
       </c>
       <c r="E222" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F222" s="3" t="inlineStr">
@@ -7535,7 +7535,7 @@
       </c>
       <c r="B223" s="3" t="inlineStr">
         <is>
-          <t>Deon</t>
+          <t>Alan</t>
         </is>
       </c>
       <c r="C223" s="3" t="inlineStr">
@@ -7562,17 +7562,17 @@
     <row r="224" ht="25" customHeight="1">
       <c r="A224" s="3" t="inlineStr">
         <is>
-          <t>van Wyk</t>
+          <t>van Wulven</t>
         </is>
       </c>
       <c r="B224" s="3" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>Deon</t>
         </is>
       </c>
       <c r="C224" s="3" t="inlineStr">
         <is>
-          <t>North Durban</t>
+          <t>Tygerberg Hills</t>
         </is>
       </c>
       <c r="D224" s="3" t="inlineStr">
@@ -7587,7 +7587,7 @@
       </c>
       <c r="F224" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -7599,12 +7599,12 @@
       </c>
       <c r="B225" s="3" t="inlineStr">
         <is>
-          <t>Lindie</t>
+          <t>Kim</t>
         </is>
       </c>
       <c r="C225" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>North Durban</t>
         </is>
       </c>
       <c r="D225" s="3" t="inlineStr">
@@ -7631,12 +7631,12 @@
       </c>
       <c r="B226" s="3" t="inlineStr">
         <is>
-          <t>Willem</t>
+          <t>Lindie</t>
         </is>
       </c>
       <c r="C226" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D226" s="3" t="inlineStr">
@@ -7663,12 +7663,12 @@
       </c>
       <c r="B227" s="3" t="inlineStr">
         <is>
-          <t>Patricia</t>
+          <t>Willem</t>
         </is>
       </c>
       <c r="C227" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D227" s="3" t="inlineStr">
@@ -7690,27 +7690,27 @@
     <row r="228" ht="25" customHeight="1">
       <c r="A228" s="3" t="inlineStr">
         <is>
-          <t>van der Merwe</t>
+          <t>van Wyk</t>
         </is>
       </c>
       <c r="B228" s="3" t="inlineStr">
         <is>
-          <t>Ingrid</t>
+          <t>Patricia</t>
         </is>
       </c>
       <c r="C228" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D228" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E228" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F228" s="3" t="inlineStr">
@@ -7722,22 +7722,22 @@
     <row r="229" ht="25" customHeight="1">
       <c r="A229" s="3" t="inlineStr">
         <is>
-          <t>van der Westhuizen</t>
+          <t>van der Merwe</t>
         </is>
       </c>
       <c r="B229" s="3" t="inlineStr">
         <is>
-          <t>Hennie</t>
+          <t>Ingrid</t>
         </is>
       </c>
       <c r="C229" s="3" t="inlineStr">
         <is>
-          <t>Helderberg</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D229" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E229" s="3" t="inlineStr">
@@ -7747,24 +7747,24 @@
       </c>
       <c r="F229" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="230" ht="25" customHeight="1">
       <c r="A230" s="3" t="inlineStr">
         <is>
-          <t>von der Decken</t>
+          <t>van der Westhuizen</t>
         </is>
       </c>
       <c r="B230" s="3" t="inlineStr">
         <is>
-          <t>Brian</t>
+          <t>Hennie</t>
         </is>
       </c>
       <c r="C230" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Helderberg</t>
         </is>
       </c>
       <c r="D230" s="3" t="inlineStr">
@@ -7779,51 +7779,83 @@
       </c>
       <c r="F230" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="231" ht="25" customHeight="1">
       <c r="A231" s="3" t="inlineStr">
         <is>
+          <t>von der Decken</t>
+        </is>
+      </c>
+      <c r="B231" s="3" t="inlineStr">
+        <is>
+          <t>Brian</t>
+        </is>
+      </c>
+      <c r="C231" s="3" t="inlineStr">
+        <is>
+          <t>King William's Town</t>
+        </is>
+      </c>
+      <c r="D231" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E231" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F231" s="3" t="inlineStr">
+        <is>
+          <t>410E</t>
+        </is>
+      </c>
+    </row>
+    <row r="232" ht="25" customHeight="1">
+      <c r="A232" s="3" t="inlineStr">
+        <is>
           <t>‘t Hart</t>
         </is>
       </c>
-      <c r="B231" s="3" t="inlineStr">
+      <c r="B232" s="3" t="inlineStr">
         <is>
           <t>Michelle</t>
         </is>
       </c>
-      <c r="C231" s="3" t="inlineStr">
+      <c r="C232" s="3" t="inlineStr">
         <is>
           <t>Benoni Lakes</t>
         </is>
       </c>
-      <c r="D231" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E231" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F231" s="3" t="inlineStr">
+      <c r="D232" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E232" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F232" s="3" t="inlineStr">
         <is>
           <t>410E</t>
-        </is>
-      </c>
-    </row>
-    <row r="232">
-      <c r="A232" s="1" t="inlineStr">
-        <is>
-          <t>Number of attendees: 229</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="inlineStr">
+        <is>
+          <t>Number of attendees: 230</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" s="1" t="inlineStr">
         <is>
           <t>Number of voters: 109</t>
         </is>
@@ -7841,7 +7873,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E124"/>
+  <dimension ref="A1:E125"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7859,7 +7891,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Registrees as of 16/04/2021 09:40</t>
+          <t>410E Registrees as of 18/04/2021 21:32</t>
         </is>
       </c>
     </row>
@@ -9864,17 +9896,17 @@
     <row r="76" ht="25" customHeight="1">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>Pantoleon</t>
+          <t>Paijmans</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
         <is>
-          <t>Teresa</t>
+          <t>Bronwyn Anne</t>
         </is>
       </c>
       <c r="C76" s="3" t="inlineStr">
         <is>
-          <t>Vereeniging</t>
+          <t>Cowies Hill</t>
         </is>
       </c>
       <c r="D76" s="3" t="inlineStr">
@@ -9884,24 +9916,24 @@
       </c>
       <c r="E76" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="77" ht="25" customHeight="1">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>Polkinghorne</t>
+          <t>Pantoleon</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
         <is>
-          <t>Tracey</t>
+          <t>Teresa</t>
         </is>
       </c>
       <c r="C77" s="3" t="inlineStr">
         <is>
-          <t>Kensington</t>
+          <t>Vereeniging</t>
         </is>
       </c>
       <c r="D77" s="3" t="inlineStr">
@@ -9923,7 +9955,7 @@
       </c>
       <c r="B78" s="3" t="inlineStr">
         <is>
-          <t>Gavin</t>
+          <t>Tracey</t>
         </is>
       </c>
       <c r="C78" s="3" t="inlineStr">
@@ -9938,24 +9970,24 @@
       </c>
       <c r="E78" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="79" ht="25" customHeight="1">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>Ras</t>
+          <t>Polkinghorne</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
         <is>
-          <t>Leon Jacobus</t>
+          <t>Gavin</t>
         </is>
       </c>
       <c r="C79" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Kensington</t>
         </is>
       </c>
       <c r="D79" s="3" t="inlineStr">
@@ -9972,17 +10004,17 @@
     <row r="80" ht="25" customHeight="1">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>Reniers</t>
+          <t>Ras</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
         <is>
-          <t>Hugo</t>
+          <t>Leon Jacobus</t>
         </is>
       </c>
       <c r="C80" s="3" t="inlineStr">
         <is>
-          <t>Nelspruit</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D80" s="3" t="inlineStr">
@@ -9992,24 +10024,24 @@
       </c>
       <c r="E80" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="81" ht="25" customHeight="1">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>Sabatier</t>
+          <t>Reniers</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
         <is>
-          <t>Rodney</t>
+          <t>Hugo</t>
         </is>
       </c>
       <c r="C81" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Nelspruit</t>
         </is>
       </c>
       <c r="D81" s="3" t="inlineStr">
@@ -10026,17 +10058,17 @@
     <row r="82" ht="25" customHeight="1">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>Searle</t>
+          <t>Sabatier</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
         <is>
-          <t>Francis</t>
+          <t>Rodney</t>
         </is>
       </c>
       <c r="C82" s="3" t="inlineStr">
         <is>
-          <t>Kouga</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D82" s="3" t="inlineStr">
@@ -10058,7 +10090,7 @@
       </c>
       <c r="B83" s="3" t="inlineStr">
         <is>
-          <t>Gloria</t>
+          <t>Francis</t>
         </is>
       </c>
       <c r="C83" s="3" t="inlineStr">
@@ -10073,24 +10105,24 @@
       </c>
       <c r="E83" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="84" ht="25" customHeight="1">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>Smit</t>
+          <t>Searle</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
         <is>
-          <t>Sue</t>
+          <t>Gloria</t>
         </is>
       </c>
       <c r="C84" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Kouga</t>
         </is>
       </c>
       <c r="D84" s="3" t="inlineStr">
@@ -10100,24 +10132,24 @@
       </c>
       <c r="E84" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="85" ht="25" customHeight="1">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Smit</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
         <is>
-          <t>Jeff</t>
+          <t>Sue</t>
         </is>
       </c>
       <c r="C85" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D85" s="3" t="inlineStr">
@@ -10127,24 +10159,24 @@
       </c>
       <c r="E85" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="86" ht="25" customHeight="1">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>Stander</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
         <is>
-          <t>Max</t>
+          <t>Jeff</t>
         </is>
       </c>
       <c r="C86" s="3" t="inlineStr">
         <is>
-          <t>Port Alfred</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D86" s="3" t="inlineStr">
@@ -10154,7 +10186,7 @@
       </c>
       <c r="E86" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -10166,12 +10198,12 @@
       </c>
       <c r="B87" s="3" t="inlineStr">
         <is>
-          <t>Ashley</t>
+          <t>Max</t>
         </is>
       </c>
       <c r="C87" s="3" t="inlineStr">
         <is>
-          <t>Krugersdorp</t>
+          <t>Port Alfred</t>
         </is>
       </c>
       <c r="D87" s="3" t="inlineStr">
@@ -10193,7 +10225,7 @@
       </c>
       <c r="B88" s="3" t="inlineStr">
         <is>
-          <t>Brett Jason</t>
+          <t>Ashley</t>
         </is>
       </c>
       <c r="C88" s="3" t="inlineStr">
@@ -10208,29 +10240,29 @@
       </c>
       <c r="E88" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="89" ht="25" customHeight="1">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>Steyn</t>
+          <t>Stander</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
         <is>
-          <t>Elna</t>
+          <t>Brett Jason</t>
         </is>
       </c>
       <c r="C89" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Krugersdorp</t>
         </is>
       </c>
       <c r="D89" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E89" s="3" t="inlineStr">
@@ -10242,22 +10274,22 @@
     <row r="90" ht="25" customHeight="1">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>Sturges</t>
+          <t>Steyn</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
         <is>
-          <t>Trevor</t>
+          <t>Elna</t>
         </is>
       </c>
       <c r="C90" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D90" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E90" s="3" t="inlineStr">
@@ -10269,17 +10301,17 @@
     <row r="91" ht="25" customHeight="1">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>Talbot</t>
+          <t>Sturges</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
         <is>
-          <t>Lauryn</t>
+          <t>Trevor</t>
         </is>
       </c>
       <c r="C91" s="3" t="inlineStr">
         <is>
-          <t>Benoni Lakes</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D91" s="3" t="inlineStr">
@@ -10296,17 +10328,17 @@
     <row r="92" ht="25" customHeight="1">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>Theron</t>
+          <t>Talbot</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
         <is>
-          <t>Pierre</t>
+          <t>Lauryn</t>
         </is>
       </c>
       <c r="C92" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Benoni Lakes</t>
         </is>
       </c>
       <c r="D92" s="3" t="inlineStr">
@@ -10328,7 +10360,7 @@
       </c>
       <c r="B93" s="3" t="inlineStr">
         <is>
-          <t>Moira</t>
+          <t>Pierre</t>
         </is>
       </c>
       <c r="C93" s="3" t="inlineStr">
@@ -10350,17 +10382,17 @@
     <row r="94" ht="25" customHeight="1">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>Townsend</t>
+          <t>Theron</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
         <is>
-          <t>Diane</t>
+          <t>Moira</t>
         </is>
       </c>
       <c r="C94" s="3" t="inlineStr">
         <is>
-          <t>Benoni Lakes</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D94" s="3" t="inlineStr">
@@ -10377,22 +10409,22 @@
     <row r="95" ht="25" customHeight="1">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>Toye</t>
+          <t>Townsend</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
         <is>
-          <t>Omolayo</t>
+          <t>Diane</t>
         </is>
       </c>
       <c r="C95" s="3" t="inlineStr">
         <is>
-          <t>The Wilds</t>
+          <t>Benoni Lakes</t>
         </is>
       </c>
       <c r="D95" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E95" s="3" t="inlineStr">
@@ -10404,22 +10436,22 @@
     <row r="96" ht="25" customHeight="1">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>Tuckett</t>
+          <t>Toye</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
         <is>
-          <t>Alistair</t>
+          <t>Omolayo</t>
         </is>
       </c>
       <c r="C96" s="3" t="inlineStr">
         <is>
-          <t>Roodepoort Clearwater Cyber</t>
+          <t>The Wilds</t>
         </is>
       </c>
       <c r="D96" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E96" s="3" t="inlineStr">
@@ -10436,7 +10468,7 @@
       </c>
       <c r="B97" s="3" t="inlineStr">
         <is>
-          <t>Rowan</t>
+          <t>Alistair</t>
         </is>
       </c>
       <c r="C97" s="3" t="inlineStr">
@@ -10451,7 +10483,7 @@
       </c>
       <c r="E97" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -10463,7 +10495,7 @@
       </c>
       <c r="B98" s="3" t="inlineStr">
         <is>
-          <t>Gail</t>
+          <t>Rowan</t>
         </is>
       </c>
       <c r="C98" s="3" t="inlineStr">
@@ -10478,29 +10510,29 @@
       </c>
       <c r="E98" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="99" ht="25" customHeight="1">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>Uchytil</t>
+          <t>Tuckett</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
         <is>
-          <t>Jiri</t>
+          <t>Gail</t>
         </is>
       </c>
       <c r="C99" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Roodepoort Clearwater Cyber</t>
         </is>
       </c>
       <c r="D99" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E99" s="3" t="inlineStr">
@@ -10512,17 +10544,17 @@
     <row r="100" ht="25" customHeight="1">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>VAN DER MERWE</t>
+          <t>Uchytil</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
         <is>
-          <t>PATRICIA</t>
+          <t>Jiri</t>
         </is>
       </c>
       <c r="C100" s="3" t="inlineStr">
         <is>
-          <t>East London Port Rex</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D100" s="3" t="inlineStr">
@@ -10532,24 +10564,24 @@
       </c>
       <c r="E100" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="101" ht="25" customHeight="1">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>Van Niekerk</t>
+          <t>VAN DER MERWE</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
         <is>
-          <t>Riaan</t>
+          <t>PATRICIA</t>
         </is>
       </c>
       <c r="C101" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>East London Port Rex</t>
         </is>
       </c>
       <c r="D101" s="3" t="inlineStr">
@@ -10559,24 +10591,24 @@
       </c>
       <c r="E101" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="102" ht="25" customHeight="1">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>Venter</t>
+          <t>Van Niekerk</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
         <is>
-          <t>Louis</t>
+          <t>Riaan</t>
         </is>
       </c>
       <c r="C102" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D102" s="3" t="inlineStr">
@@ -10586,29 +10618,29 @@
       </c>
       <c r="E102" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="103" ht="25" customHeight="1">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>Volker</t>
+          <t>Venter</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
         <is>
-          <t>Russell</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="C103" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D103" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E103" s="3" t="inlineStr">
@@ -10620,17 +10652,17 @@
     <row r="104" ht="25" customHeight="1">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>Warman</t>
+          <t>Volker</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
         <is>
-          <t>Alastair</t>
+          <t>Russell</t>
         </is>
       </c>
       <c r="C104" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>King William's Town</t>
         </is>
       </c>
       <c r="D104" s="3" t="inlineStr">
@@ -10647,17 +10679,17 @@
     <row r="105" ht="25" customHeight="1">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>Williamson</t>
+          <t>Warman</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
         <is>
-          <t>Neville</t>
+          <t>Alastair</t>
         </is>
       </c>
       <c r="C105" s="3" t="inlineStr">
         <is>
-          <t>Port Alfred</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D105" s="3" t="inlineStr">
@@ -10667,24 +10699,24 @@
       </c>
       <c r="E105" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="106" ht="25" customHeight="1">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>Wilter-Sturges</t>
+          <t>Williamson</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
         <is>
-          <t>Meredith</t>
+          <t>Neville</t>
         </is>
       </c>
       <c r="C106" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Port Alfred</t>
         </is>
       </c>
       <c r="D106" s="3" t="inlineStr">
@@ -10701,17 +10733,17 @@
     <row r="107" ht="25" customHeight="1">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>Zucker</t>
+          <t>Wilter-Sturges</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
         <is>
-          <t>Leonie</t>
+          <t>Meredith</t>
         </is>
       </c>
       <c r="C107" s="3" t="inlineStr">
         <is>
-          <t>Milnerton</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D107" s="3" t="inlineStr">
@@ -10721,61 +10753,61 @@
       </c>
       <c r="E107" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="108" ht="25" customHeight="1">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>de Silva</t>
+          <t>Zucker</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Leonie</t>
         </is>
       </c>
       <c r="C108" s="3" t="inlineStr">
         <is>
-          <t>Edenvale</t>
+          <t>Milnerton</t>
         </is>
       </c>
       <c r="D108" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E108" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="109" ht="25" customHeight="1">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>du Plooy</t>
+          <t>de Silva</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
         <is>
-          <t>Tammy</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="C109" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Edenvale</t>
         </is>
       </c>
       <c r="D109" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E109" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -10787,7 +10819,7 @@
       </c>
       <c r="B110" s="3" t="inlineStr">
         <is>
-          <t>Marc</t>
+          <t>Tammy</t>
         </is>
       </c>
       <c r="C110" s="3" t="inlineStr">
@@ -10809,17 +10841,17 @@
     <row r="111" ht="25" customHeight="1">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>du Toit</t>
+          <t>du Plooy</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
         <is>
-          <t>Desiree</t>
+          <t>Marc</t>
         </is>
       </c>
       <c r="C111" s="3" t="inlineStr">
         <is>
-          <t>Ramsgate</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D111" s="3" t="inlineStr">
@@ -10829,24 +10861,24 @@
       </c>
       <c r="E111" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="112" ht="25" customHeight="1">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>le Roux</t>
+          <t>du Toit</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
         <is>
-          <t>Jeanette</t>
+          <t>Desiree</t>
         </is>
       </c>
       <c r="C112" s="3" t="inlineStr">
         <is>
-          <t>Gonubie</t>
+          <t>Ramsgate</t>
         </is>
       </c>
       <c r="D112" s="3" t="inlineStr">
@@ -10863,17 +10895,17 @@
     <row r="113" ht="25" customHeight="1">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>van Heerden</t>
+          <t>le Roux</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Jeanette</t>
         </is>
       </c>
       <c r="C113" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Gonubie</t>
         </is>
       </c>
       <c r="D113" s="3" t="inlineStr">
@@ -10895,7 +10927,7 @@
       </c>
       <c r="B114" s="3" t="inlineStr">
         <is>
-          <t>Sandy</t>
+          <t>Sydney</t>
         </is>
       </c>
       <c r="C114" s="3" t="inlineStr">
@@ -10910,7 +10942,7 @@
       </c>
       <c r="E114" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -10922,12 +10954,12 @@
       </c>
       <c r="B115" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Sandy</t>
         </is>
       </c>
       <c r="C115" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D115" s="3" t="inlineStr">
@@ -10944,17 +10976,17 @@
     <row r="116" ht="25" customHeight="1">
       <c r="A116" s="3" t="inlineStr">
         <is>
-          <t>van Wyk</t>
+          <t>van Heerden</t>
         </is>
       </c>
       <c r="B116" s="3" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C116" s="3" t="inlineStr">
         <is>
-          <t>North Durban</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D116" s="3" t="inlineStr">
@@ -10964,7 +10996,7 @@
       </c>
       <c r="E116" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -10976,12 +11008,12 @@
       </c>
       <c r="B117" s="3" t="inlineStr">
         <is>
-          <t>Lindie</t>
+          <t>Kim</t>
         </is>
       </c>
       <c r="C117" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>North Durban</t>
         </is>
       </c>
       <c r="D117" s="3" t="inlineStr">
@@ -11003,12 +11035,12 @@
       </c>
       <c r="B118" s="3" t="inlineStr">
         <is>
-          <t>Willem</t>
+          <t>Lindie</t>
         </is>
       </c>
       <c r="C118" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D118" s="3" t="inlineStr">
@@ -11030,12 +11062,12 @@
       </c>
       <c r="B119" s="3" t="inlineStr">
         <is>
-          <t>Patricia</t>
+          <t>Willem</t>
         </is>
       </c>
       <c r="C119" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D119" s="3" t="inlineStr">
@@ -11052,49 +11084,49 @@
     <row r="120" ht="25" customHeight="1">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>van der Merwe</t>
+          <t>van Wyk</t>
         </is>
       </c>
       <c r="B120" s="3" t="inlineStr">
         <is>
-          <t>Ingrid</t>
+          <t>Patricia</t>
         </is>
       </c>
       <c r="C120" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D120" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E120" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="121" ht="25" customHeight="1">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>von der Decken</t>
+          <t>van der Merwe</t>
         </is>
       </c>
       <c r="B121" s="3" t="inlineStr">
         <is>
-          <t>Brian</t>
+          <t>Ingrid</t>
         </is>
       </c>
       <c r="C121" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D121" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E121" s="3" t="inlineStr">
@@ -11106,39 +11138,66 @@
     <row r="122" ht="25" customHeight="1">
       <c r="A122" s="3" t="inlineStr">
         <is>
+          <t>von der Decken</t>
+        </is>
+      </c>
+      <c r="B122" s="3" t="inlineStr">
+        <is>
+          <t>Brian</t>
+        </is>
+      </c>
+      <c r="C122" s="3" t="inlineStr">
+        <is>
+          <t>King William's Town</t>
+        </is>
+      </c>
+      <c r="D122" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E122" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="123" ht="25" customHeight="1">
+      <c r="A123" s="3" t="inlineStr">
+        <is>
           <t>‘t Hart</t>
         </is>
       </c>
-      <c r="B122" s="3" t="inlineStr">
+      <c r="B123" s="3" t="inlineStr">
         <is>
           <t>Michelle</t>
         </is>
       </c>
-      <c r="C122" s="3" t="inlineStr">
+      <c r="C123" s="3" t="inlineStr">
         <is>
           <t>Benoni Lakes</t>
         </is>
       </c>
-      <c r="D122" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E122" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" s="1" t="inlineStr">
-        <is>
-          <t>Number of attendees: 120</t>
+      <c r="D123" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E123" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="inlineStr">
+        <is>
+          <t>Number of attendees: 121</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="1" t="inlineStr">
         <is>
           <t>Number of voters: 60</t>
         </is>
@@ -11174,7 +11233,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Registrees as of 16/04/2021 09:40</t>
+          <t>410W Registrees as of 18/04/2021 21:32</t>
         </is>
       </c>
     </row>
@@ -15215,7 +15274,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Voting details as of 16/04/2021 09:40</t>
+          <t>410E Voting details as of 18/04/2021 21:32</t>
         </is>
       </c>
     </row>
@@ -15552,7 +15611,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Voting details as of 16/04/2021 09:40</t>
+          <t>410W Voting details as of 18/04/2021 21:32</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Registree stats backup on Mon 19 Apr 2021 10:15:44 SAST
</commit_message>
<xml_diff>
--- a/static/docs/registrees_list.xlsx
+++ b/static/docs/registrees_list.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F234"/>
+  <dimension ref="A1:F236"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,7 +451,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>MD410 Registrees as of 18/04/2021 21:32</t>
+          <t>MD410 Registrees as of 19/04/2021 10:15</t>
         </is>
       </c>
     </row>
@@ -4906,17 +4906,17 @@
     <row r="141" ht="25" customHeight="1">
       <c r="A141" s="3" t="inlineStr">
         <is>
-          <t>Niehaus</t>
+          <t>Ngobozana</t>
         </is>
       </c>
       <c r="B141" s="3" t="inlineStr">
         <is>
-          <t>Angela</t>
+          <t>Sphiwe</t>
         </is>
       </c>
       <c r="C141" s="3" t="inlineStr">
         <is>
-          <t>Bergvliet</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D141" s="3" t="inlineStr">
@@ -4926,29 +4926,29 @@
       </c>
       <c r="E141" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F141" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="142" ht="25" customHeight="1">
       <c r="A142" s="3" t="inlineStr">
         <is>
-          <t>Oberholzer</t>
+          <t>Niehaus</t>
         </is>
       </c>
       <c r="B142" s="3" t="inlineStr">
         <is>
-          <t>PDG Bokkie</t>
+          <t>Angela</t>
         </is>
       </c>
       <c r="C142" s="3" t="inlineStr">
         <is>
-          <t>Uitenhage</t>
+          <t>Bergvliet</t>
         </is>
       </c>
       <c r="D142" s="3" t="inlineStr">
@@ -4963,24 +4963,24 @@
       </c>
       <c r="F142" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="143" ht="25" customHeight="1">
       <c r="A143" s="3" t="inlineStr">
         <is>
-          <t>PORTEOUS</t>
+          <t>Oberholzer</t>
         </is>
       </c>
       <c r="B143" s="3" t="inlineStr">
         <is>
-          <t>BRIAN</t>
+          <t>PDG Bokkie</t>
         </is>
       </c>
       <c r="C143" s="3" t="inlineStr">
         <is>
-          <t>Hibberdene</t>
+          <t>Uitenhage</t>
         </is>
       </c>
       <c r="D143" s="3" t="inlineStr">
@@ -5002,17 +5002,17 @@
     <row r="144" ht="25" customHeight="1">
       <c r="A144" s="3" t="inlineStr">
         <is>
-          <t>Paijmans</t>
+          <t>PORTEOUS</t>
         </is>
       </c>
       <c r="B144" s="3" t="inlineStr">
         <is>
-          <t>Bronwyn Anne</t>
+          <t>BRIAN</t>
         </is>
       </c>
       <c r="C144" s="3" t="inlineStr">
         <is>
-          <t>Cowies Hill</t>
+          <t>Hibberdene</t>
         </is>
       </c>
       <c r="D144" s="3" t="inlineStr">
@@ -5022,7 +5022,7 @@
       </c>
       <c r="E144" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F144" s="3" t="inlineStr">
@@ -5034,17 +5034,17 @@
     <row r="145" ht="25" customHeight="1">
       <c r="A145" s="3" t="inlineStr">
         <is>
-          <t>Pantoleon</t>
+          <t>Paijmans</t>
         </is>
       </c>
       <c r="B145" s="3" t="inlineStr">
         <is>
-          <t>Teresa</t>
+          <t>Bronwyn Anne</t>
         </is>
       </c>
       <c r="C145" s="3" t="inlineStr">
         <is>
-          <t>Vereeniging</t>
+          <t>Cowies Hill</t>
         </is>
       </c>
       <c r="D145" s="3" t="inlineStr">
@@ -5054,7 +5054,7 @@
       </c>
       <c r="E145" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F145" s="3" t="inlineStr">
@@ -5066,17 +5066,17 @@
     <row r="146" ht="25" customHeight="1">
       <c r="A146" s="3" t="inlineStr">
         <is>
-          <t>Peters</t>
+          <t>Pantoleon</t>
         </is>
       </c>
       <c r="B146" s="3" t="inlineStr">
         <is>
-          <t>Maureen</t>
+          <t>Teresa</t>
         </is>
       </c>
       <c r="C146" s="3" t="inlineStr">
         <is>
-          <t>Ceres</t>
+          <t>Vereeniging</t>
         </is>
       </c>
       <c r="D146" s="3" t="inlineStr">
@@ -5091,24 +5091,24 @@
       </c>
       <c r="F146" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="147" ht="25" customHeight="1">
       <c r="A147" s="3" t="inlineStr">
         <is>
-          <t>Pillay</t>
+          <t>Peters</t>
         </is>
       </c>
       <c r="B147" s="3" t="inlineStr">
         <is>
-          <t>Sundru</t>
+          <t>Maureen</t>
         </is>
       </c>
       <c r="C147" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>Ceres</t>
         </is>
       </c>
       <c r="D147" s="3" t="inlineStr">
@@ -5118,7 +5118,7 @@
       </c>
       <c r="E147" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F147" s="3" t="inlineStr">
@@ -5135,12 +5135,12 @@
       </c>
       <c r="B148" s="3" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>Sundru</t>
         </is>
       </c>
       <c r="C148" s="3" t="inlineStr">
         <is>
-          <t>Tygerberg Hills</t>
+          <t>Durbanville</t>
         </is>
       </c>
       <c r="D148" s="3" t="inlineStr">
@@ -5150,7 +5150,7 @@
       </c>
       <c r="E148" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F148" s="3" t="inlineStr">
@@ -5162,17 +5162,17 @@
     <row r="149" ht="25" customHeight="1">
       <c r="A149" s="3" t="inlineStr">
         <is>
-          <t>Polkinghorne</t>
+          <t>Pillay</t>
         </is>
       </c>
       <c r="B149" s="3" t="inlineStr">
         <is>
-          <t>Tracey</t>
+          <t>Patrick</t>
         </is>
       </c>
       <c r="C149" s="3" t="inlineStr">
         <is>
-          <t>Kensington</t>
+          <t>Tygerberg Hills</t>
         </is>
       </c>
       <c r="D149" s="3" t="inlineStr">
@@ -5187,7 +5187,7 @@
       </c>
       <c r="F149" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -5199,7 +5199,7 @@
       </c>
       <c r="B150" s="3" t="inlineStr">
         <is>
-          <t>Gavin</t>
+          <t>Tracey</t>
         </is>
       </c>
       <c r="C150" s="3" t="inlineStr">
@@ -5214,7 +5214,7 @@
       </c>
       <c r="E150" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F150" s="3" t="inlineStr">
@@ -5226,22 +5226,22 @@
     <row r="151" ht="25" customHeight="1">
       <c r="A151" s="3" t="inlineStr">
         <is>
-          <t>Pretorius</t>
+          <t>Polkinghorne</t>
         </is>
       </c>
       <c r="B151" s="3" t="inlineStr">
         <is>
-          <t>Sheldon Edmund</t>
+          <t>Gavin</t>
         </is>
       </c>
       <c r="C151" s="3" t="inlineStr">
         <is>
-          <t>Merriman</t>
+          <t>Kensington</t>
         </is>
       </c>
       <c r="D151" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E151" s="3" t="inlineStr">
@@ -5251,29 +5251,29 @@
       </c>
       <c r="F151" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="152" ht="25" customHeight="1">
       <c r="A152" s="3" t="inlineStr">
         <is>
-          <t>Ras</t>
+          <t>Pretorius</t>
         </is>
       </c>
       <c r="B152" s="3" t="inlineStr">
         <is>
-          <t>Mary-Anne</t>
+          <t>Sheldon Edmund</t>
         </is>
       </c>
       <c r="C152" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Merriman</t>
         </is>
       </c>
       <c r="D152" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E152" s="3" t="inlineStr">
@@ -5295,7 +5295,7 @@
       </c>
       <c r="B153" s="3" t="inlineStr">
         <is>
-          <t>Leon Jacobus</t>
+          <t>Mary-Anne</t>
         </is>
       </c>
       <c r="C153" s="3" t="inlineStr">
@@ -5315,24 +5315,24 @@
       </c>
       <c r="F153" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="154" ht="25" customHeight="1">
       <c r="A154" s="3" t="inlineStr">
         <is>
-          <t>Reniers</t>
+          <t>Ras</t>
         </is>
       </c>
       <c r="B154" s="3" t="inlineStr">
         <is>
-          <t>Hugo</t>
+          <t>Leon Jacobus</t>
         </is>
       </c>
       <c r="C154" s="3" t="inlineStr">
         <is>
-          <t>Nelspruit</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D154" s="3" t="inlineStr">
@@ -5342,7 +5342,7 @@
       </c>
       <c r="E154" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F154" s="3" t="inlineStr">
@@ -5354,17 +5354,17 @@
     <row r="155" ht="25" customHeight="1">
       <c r="A155" s="3" t="inlineStr">
         <is>
-          <t>Roman</t>
+          <t>Reniers</t>
         </is>
       </c>
       <c r="B155" s="3" t="inlineStr">
         <is>
-          <t>Sandy</t>
+          <t>Hugo</t>
         </is>
       </c>
       <c r="C155" s="3" t="inlineStr">
         <is>
-          <t>Bergvliet</t>
+          <t>Nelspruit</t>
         </is>
       </c>
       <c r="D155" s="3" t="inlineStr">
@@ -5374,29 +5374,29 @@
       </c>
       <c r="E155" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F155" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="156" ht="25" customHeight="1">
       <c r="A156" s="3" t="inlineStr">
         <is>
-          <t>Rossouw</t>
+          <t>Roman</t>
         </is>
       </c>
       <c r="B156" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Sandy</t>
         </is>
       </c>
       <c r="C156" s="3" t="inlineStr">
         <is>
-          <t>Tokai</t>
+          <t>Bergvliet</t>
         </is>
       </c>
       <c r="D156" s="3" t="inlineStr">
@@ -5406,7 +5406,7 @@
       </c>
       <c r="E156" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F156" s="3" t="inlineStr">
@@ -5418,17 +5418,17 @@
     <row r="157" ht="25" customHeight="1">
       <c r="A157" s="3" t="inlineStr">
         <is>
-          <t>Rothner</t>
+          <t>Rossouw</t>
         </is>
       </c>
       <c r="B157" s="3" t="inlineStr">
         <is>
-          <t>Andrea</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C157" s="3" t="inlineStr">
         <is>
-          <t>Eden</t>
+          <t>Tokai</t>
         </is>
       </c>
       <c r="D157" s="3" t="inlineStr">
@@ -5438,7 +5438,7 @@
       </c>
       <c r="E157" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F157" s="3" t="inlineStr">
@@ -5450,17 +5450,17 @@
     <row r="158" ht="25" customHeight="1">
       <c r="A158" s="3" t="inlineStr">
         <is>
-          <t>Roux</t>
+          <t>Rothner</t>
         </is>
       </c>
       <c r="B158" s="3" t="inlineStr">
         <is>
-          <t>Anthonie Petrus</t>
+          <t>Andrea</t>
         </is>
       </c>
       <c r="C158" s="3" t="inlineStr">
         <is>
-          <t>Moorreesburg</t>
+          <t>Eden</t>
         </is>
       </c>
       <c r="D158" s="3" t="inlineStr">
@@ -5470,7 +5470,7 @@
       </c>
       <c r="E158" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F158" s="3" t="inlineStr">
@@ -5482,17 +5482,17 @@
     <row r="159" ht="25" customHeight="1">
       <c r="A159" s="3" t="inlineStr">
         <is>
-          <t>Russell</t>
+          <t>Roux</t>
         </is>
       </c>
       <c r="B159" s="3" t="inlineStr">
         <is>
-          <t>Ingrid</t>
+          <t>Anthonie Petrus</t>
         </is>
       </c>
       <c r="C159" s="3" t="inlineStr">
         <is>
-          <t>Fish Hoek</t>
+          <t>Moorreesburg</t>
         </is>
       </c>
       <c r="D159" s="3" t="inlineStr">
@@ -5514,27 +5514,27 @@
     <row r="160" ht="25" customHeight="1">
       <c r="A160" s="3" t="inlineStr">
         <is>
-          <t>SNYMAN</t>
+          <t>Russell</t>
         </is>
       </c>
       <c r="B160" s="3" t="inlineStr">
         <is>
-          <t>LYN</t>
+          <t>Ingrid</t>
         </is>
       </c>
       <c r="C160" s="3" t="inlineStr">
         <is>
-          <t>Deep South</t>
+          <t>Fish Hoek</t>
         </is>
       </c>
       <c r="D160" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E160" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F160" s="3" t="inlineStr">
@@ -5546,27 +5546,27 @@
     <row r="161" ht="25" customHeight="1">
       <c r="A161" s="3" t="inlineStr">
         <is>
-          <t>STEENBERG</t>
+          <t>SNYMAN</t>
         </is>
       </c>
       <c r="B161" s="3" t="inlineStr">
         <is>
-          <t>TIM</t>
+          <t>LYN</t>
         </is>
       </c>
       <c r="C161" s="3" t="inlineStr">
         <is>
-          <t>Wellington</t>
+          <t>Deep South</t>
         </is>
       </c>
       <c r="D161" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E161" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F161" s="3" t="inlineStr">
@@ -5578,17 +5578,17 @@
     <row r="162" ht="25" customHeight="1">
       <c r="A162" s="3" t="inlineStr">
         <is>
-          <t>Sabatier</t>
+          <t>STEENBERG</t>
         </is>
       </c>
       <c r="B162" s="3" t="inlineStr">
         <is>
-          <t>Rodney</t>
+          <t>TIM</t>
         </is>
       </c>
       <c r="C162" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Wellington</t>
         </is>
       </c>
       <c r="D162" s="3" t="inlineStr">
@@ -5603,24 +5603,24 @@
       </c>
       <c r="F162" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="163" ht="25" customHeight="1">
       <c r="A163" s="3" t="inlineStr">
         <is>
-          <t>Sampie</t>
+          <t>Sabatier</t>
         </is>
       </c>
       <c r="B163" s="3" t="inlineStr">
         <is>
-          <t>Sharon</t>
+          <t>Rodney</t>
         </is>
       </c>
       <c r="C163" s="3" t="inlineStr">
         <is>
-          <t>Bergvliet</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D163" s="3" t="inlineStr">
@@ -5635,24 +5635,24 @@
       </c>
       <c r="F163" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="164" ht="25" customHeight="1">
       <c r="A164" s="3" t="inlineStr">
         <is>
-          <t>Schatz</t>
+          <t>Sampie</t>
         </is>
       </c>
       <c r="B164" s="3" t="inlineStr">
         <is>
-          <t>Vera</t>
+          <t>Sharon</t>
         </is>
       </c>
       <c r="C164" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Bergvliet</t>
         </is>
       </c>
       <c r="D164" s="3" t="inlineStr">
@@ -5679,7 +5679,7 @@
       </c>
       <c r="B165" s="3" t="inlineStr">
         <is>
-          <t>Frank</t>
+          <t>Vera</t>
         </is>
       </c>
       <c r="C165" s="3" t="inlineStr">
@@ -5706,17 +5706,17 @@
     <row r="166" ht="25" customHeight="1">
       <c r="A166" s="3" t="inlineStr">
         <is>
-          <t>Searle</t>
+          <t>Schatz</t>
         </is>
       </c>
       <c r="B166" s="3" t="inlineStr">
         <is>
-          <t>Francis</t>
+          <t>Frank</t>
         </is>
       </c>
       <c r="C166" s="3" t="inlineStr">
         <is>
-          <t>Kouga</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D166" s="3" t="inlineStr">
@@ -5731,7 +5731,7 @@
       </c>
       <c r="F166" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -5743,7 +5743,7 @@
       </c>
       <c r="B167" s="3" t="inlineStr">
         <is>
-          <t>Gloria</t>
+          <t>Francis</t>
         </is>
       </c>
       <c r="C167" s="3" t="inlineStr">
@@ -5758,7 +5758,7 @@
       </c>
       <c r="E167" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F167" s="3" t="inlineStr">
@@ -5770,17 +5770,17 @@
     <row r="168" ht="25" customHeight="1">
       <c r="A168" s="3" t="inlineStr">
         <is>
-          <t>Sell</t>
+          <t>Searle</t>
         </is>
       </c>
       <c r="B168" s="3" t="inlineStr">
         <is>
-          <t>Ami</t>
+          <t>Gloria</t>
         </is>
       </c>
       <c r="C168" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Kouga</t>
         </is>
       </c>
       <c r="D168" s="3" t="inlineStr">
@@ -5795,24 +5795,24 @@
       </c>
       <c r="F168" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="169" ht="25" customHeight="1">
       <c r="A169" s="3" t="inlineStr">
         <is>
-          <t>Simpson</t>
+          <t>Sell</t>
         </is>
       </c>
       <c r="B169" s="3" t="inlineStr">
         <is>
-          <t>Beryl</t>
+          <t>Ami</t>
         </is>
       </c>
       <c r="C169" s="3" t="inlineStr">
         <is>
-          <t>Cape Town</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D169" s="3" t="inlineStr">
@@ -5834,17 +5834,17 @@
     <row r="170" ht="25" customHeight="1">
       <c r="A170" s="3" t="inlineStr">
         <is>
-          <t>Sircoulomb</t>
+          <t>Simpson</t>
         </is>
       </c>
       <c r="B170" s="3" t="inlineStr">
         <is>
-          <t>Kenlis</t>
+          <t>Beryl</t>
         </is>
       </c>
       <c r="C170" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Cape Town</t>
         </is>
       </c>
       <c r="D170" s="3" t="inlineStr">
@@ -5871,7 +5871,7 @@
       </c>
       <c r="B171" s="3" t="inlineStr">
         <is>
-          <t>Holger</t>
+          <t>Kenlis</t>
         </is>
       </c>
       <c r="C171" s="3" t="inlineStr">
@@ -5898,12 +5898,12 @@
     <row r="172" ht="25" customHeight="1">
       <c r="A172" s="3" t="inlineStr">
         <is>
-          <t>Smeer</t>
+          <t>Sircoulomb</t>
         </is>
       </c>
       <c r="B172" s="3" t="inlineStr">
         <is>
-          <t>Hennie</t>
+          <t>Holger</t>
         </is>
       </c>
       <c r="C172" s="3" t="inlineStr">
@@ -5913,12 +5913,12 @@
       </c>
       <c r="D172" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E172" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F172" s="3" t="inlineStr">
@@ -5930,22 +5930,22 @@
     <row r="173" ht="25" customHeight="1">
       <c r="A173" s="3" t="inlineStr">
         <is>
-          <t>Smit</t>
+          <t>Smeer</t>
         </is>
       </c>
       <c r="B173" s="3" t="inlineStr">
         <is>
-          <t>Sue</t>
+          <t>Hennie</t>
         </is>
       </c>
       <c r="C173" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D173" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E173" s="3" t="inlineStr">
@@ -5955,7 +5955,7 @@
       </c>
       <c r="F173" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -5967,12 +5967,12 @@
       </c>
       <c r="B174" s="3" t="inlineStr">
         <is>
-          <t>Herman</t>
+          <t>Sue</t>
         </is>
       </c>
       <c r="C174" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D174" s="3" t="inlineStr">
@@ -5982,29 +5982,29 @@
       </c>
       <c r="E174" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F174" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="175" ht="25" customHeight="1">
       <c r="A175" s="3" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Smit</t>
         </is>
       </c>
       <c r="B175" s="3" t="inlineStr">
         <is>
-          <t>Jeff</t>
+          <t>Herman</t>
         </is>
       </c>
       <c r="C175" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D175" s="3" t="inlineStr">
@@ -6019,7 +6019,7 @@
       </c>
       <c r="F175" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -6031,12 +6031,12 @@
       </c>
       <c r="B176" s="3" t="inlineStr">
         <is>
-          <t>Bennie</t>
+          <t>Jeff</t>
         </is>
       </c>
       <c r="C176" s="3" t="inlineStr">
         <is>
-          <t>Wellington</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D176" s="3" t="inlineStr">
@@ -6046,12 +6046,12 @@
       </c>
       <c r="E176" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F176" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -6063,12 +6063,12 @@
       </c>
       <c r="B177" s="3" t="inlineStr">
         <is>
-          <t>Carmen Dolores</t>
+          <t>Bennie</t>
         </is>
       </c>
       <c r="C177" s="3" t="inlineStr">
         <is>
-          <t>Tokai</t>
+          <t>Wellington</t>
         </is>
       </c>
       <c r="D177" s="3" t="inlineStr">
@@ -6078,7 +6078,7 @@
       </c>
       <c r="E177" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F177" s="3" t="inlineStr">
@@ -6095,7 +6095,7 @@
       </c>
       <c r="B178" s="3" t="inlineStr">
         <is>
-          <t>David John</t>
+          <t>Carmen Dolores</t>
         </is>
       </c>
       <c r="C178" s="3" t="inlineStr">
@@ -6122,17 +6122,17 @@
     <row r="179" ht="25" customHeight="1">
       <c r="A179" s="3" t="inlineStr">
         <is>
-          <t>Sochen</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="B179" s="3" t="inlineStr">
         <is>
-          <t>Diana</t>
+          <t>David John</t>
         </is>
       </c>
       <c r="C179" s="3" t="inlineStr">
         <is>
-          <t>Sea Point</t>
+          <t>Tokai</t>
         </is>
       </c>
       <c r="D179" s="3" t="inlineStr">
@@ -6142,7 +6142,7 @@
       </c>
       <c r="E179" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F179" s="3" t="inlineStr">
@@ -6154,49 +6154,49 @@
     <row r="180" ht="25" customHeight="1">
       <c r="A180" s="3" t="inlineStr">
         <is>
-          <t>Steyn</t>
+          <t>Sochen</t>
         </is>
       </c>
       <c r="B180" s="3" t="inlineStr">
         <is>
-          <t>Elna</t>
+          <t>Diana</t>
         </is>
       </c>
       <c r="C180" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Sea Point</t>
         </is>
       </c>
       <c r="D180" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E180" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F180" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="181" ht="25" customHeight="1">
       <c r="A181" s="3" t="inlineStr">
         <is>
-          <t>Strauss</t>
+          <t>Steyn</t>
         </is>
       </c>
       <c r="B181" s="3" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>Elna</t>
         </is>
       </c>
       <c r="C181" s="3" t="inlineStr">
         <is>
-          <t>Kuilsriver</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D181" s="3" t="inlineStr">
@@ -6211,29 +6211,29 @@
       </c>
       <c r="F181" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="182" ht="25" customHeight="1">
       <c r="A182" s="3" t="inlineStr">
         <is>
-          <t>Sturges</t>
+          <t>Strauss</t>
         </is>
       </c>
       <c r="B182" s="3" t="inlineStr">
         <is>
-          <t>Trevor</t>
+          <t>Patrick</t>
         </is>
       </c>
       <c r="C182" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Kuilsriver</t>
         </is>
       </c>
       <c r="D182" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E182" s="3" t="inlineStr">
@@ -6243,24 +6243,24 @@
       </c>
       <c r="F182" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="183" ht="25" customHeight="1">
       <c r="A183" s="3" t="inlineStr">
         <is>
-          <t>Talbot</t>
+          <t>Sturges</t>
         </is>
       </c>
       <c r="B183" s="3" t="inlineStr">
         <is>
-          <t>Lauryn</t>
+          <t>Trevor</t>
         </is>
       </c>
       <c r="C183" s="3" t="inlineStr">
         <is>
-          <t>Benoni Lakes</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D183" s="3" t="inlineStr">
@@ -6282,17 +6282,17 @@
     <row r="184" ht="25" customHeight="1">
       <c r="A184" s="3" t="inlineStr">
         <is>
-          <t>Theron</t>
+          <t>Talbot</t>
         </is>
       </c>
       <c r="B184" s="3" t="inlineStr">
         <is>
-          <t>Pierre</t>
+          <t>Lauryn</t>
         </is>
       </c>
       <c r="C184" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Benoni Lakes</t>
         </is>
       </c>
       <c r="D184" s="3" t="inlineStr">
@@ -6319,7 +6319,7 @@
       </c>
       <c r="B185" s="3" t="inlineStr">
         <is>
-          <t>Moira</t>
+          <t>Pierre</t>
         </is>
       </c>
       <c r="C185" s="3" t="inlineStr">
@@ -6346,22 +6346,22 @@
     <row r="186" ht="25" customHeight="1">
       <c r="A186" s="3" t="inlineStr">
         <is>
-          <t>Toye</t>
+          <t>Theron</t>
         </is>
       </c>
       <c r="B186" s="3" t="inlineStr">
         <is>
-          <t>Omolayo</t>
+          <t>Moira</t>
         </is>
       </c>
       <c r="C186" s="3" t="inlineStr">
         <is>
-          <t>The Wilds</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D186" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E186" s="3" t="inlineStr">
@@ -6378,22 +6378,22 @@
     <row r="187" ht="25" customHeight="1">
       <c r="A187" s="3" t="inlineStr">
         <is>
-          <t>Tshikala</t>
+          <t>Toye</t>
         </is>
       </c>
       <c r="B187" s="3" t="inlineStr">
         <is>
-          <t>David Alex</t>
+          <t>Omolayo</t>
         </is>
       </c>
       <c r="C187" s="3" t="inlineStr">
         <is>
-          <t>Athlone</t>
+          <t>The Wilds</t>
         </is>
       </c>
       <c r="D187" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E187" s="3" t="inlineStr">
@@ -6403,24 +6403,24 @@
       </c>
       <c r="F187" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="188" ht="25" customHeight="1">
       <c r="A188" s="3" t="inlineStr">
         <is>
-          <t>Tuckett</t>
+          <t>Tshikala</t>
         </is>
       </c>
       <c r="B188" s="3" t="inlineStr">
         <is>
-          <t>Alistair</t>
+          <t>David Alex</t>
         </is>
       </c>
       <c r="C188" s="3" t="inlineStr">
         <is>
-          <t>Roodepoort Clearwater Cyber</t>
+          <t>Athlone</t>
         </is>
       </c>
       <c r="D188" s="3" t="inlineStr">
@@ -6435,7 +6435,7 @@
       </c>
       <c r="F188" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -6447,7 +6447,7 @@
       </c>
       <c r="B189" s="3" t="inlineStr">
         <is>
-          <t>Rowan</t>
+          <t>Alistair</t>
         </is>
       </c>
       <c r="C189" s="3" t="inlineStr">
@@ -6462,7 +6462,7 @@
       </c>
       <c r="E189" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F189" s="3" t="inlineStr">
@@ -6479,7 +6479,7 @@
       </c>
       <c r="B190" s="3" t="inlineStr">
         <is>
-          <t>Gail</t>
+          <t>Rowan</t>
         </is>
       </c>
       <c r="C190" s="3" t="inlineStr">
@@ -6494,7 +6494,7 @@
       </c>
       <c r="E190" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F190" s="3" t="inlineStr">
@@ -6506,17 +6506,17 @@
     <row r="191" ht="25" customHeight="1">
       <c r="A191" s="3" t="inlineStr">
         <is>
-          <t>VAN BREDA</t>
+          <t>Tuckett</t>
         </is>
       </c>
       <c r="B191" s="3" t="inlineStr">
         <is>
-          <t>HILARY LISE</t>
+          <t>Gail</t>
         </is>
       </c>
       <c r="C191" s="3" t="inlineStr">
         <is>
-          <t>Cape Town</t>
+          <t>Roodepoort Clearwater Cyber</t>
         </is>
       </c>
       <c r="D191" s="3" t="inlineStr">
@@ -6531,39 +6531,39 @@
       </c>
       <c r="F191" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="192" ht="25" customHeight="1">
       <c r="A192" s="3" t="inlineStr">
         <is>
-          <t>VAN DER MERWE</t>
+          <t>VAN BREDA</t>
         </is>
       </c>
       <c r="B192" s="3" t="inlineStr">
         <is>
-          <t>PATRICIA</t>
+          <t>HILARY LISE</t>
         </is>
       </c>
       <c r="C192" s="3" t="inlineStr">
         <is>
-          <t>East London Port Rex</t>
+          <t>Cape Town</t>
         </is>
       </c>
       <c r="D192" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E192" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F192" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -6575,17 +6575,17 @@
       </c>
       <c r="B193" s="3" t="inlineStr">
         <is>
-          <t>MARINA</t>
+          <t>PATRICIA</t>
         </is>
       </c>
       <c r="C193" s="3" t="inlineStr">
         <is>
-          <t>Malmesbury</t>
+          <t>East London Port Rex</t>
         </is>
       </c>
       <c r="D193" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E193" s="3" t="inlineStr">
@@ -6595,56 +6595,56 @@
       </c>
       <c r="F193" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="194" ht="25" customHeight="1">
       <c r="A194" s="3" t="inlineStr">
         <is>
-          <t>Valadao</t>
+          <t>VAN DER MERWE</t>
         </is>
       </c>
       <c r="B194" s="3" t="inlineStr">
         <is>
-          <t>Tracy</t>
+          <t>MARINA</t>
         </is>
       </c>
       <c r="C194" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Malmesbury</t>
         </is>
       </c>
       <c r="D194" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E194" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F194" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="195" ht="25" customHeight="1">
       <c r="A195" s="3" t="inlineStr">
         <is>
-          <t>Van Niekerk</t>
+          <t>Valadao</t>
         </is>
       </c>
       <c r="B195" s="3" t="inlineStr">
         <is>
-          <t>Riaan</t>
+          <t>Tracy</t>
         </is>
       </c>
       <c r="C195" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D195" s="3" t="inlineStr">
@@ -6666,54 +6666,54 @@
     <row r="196" ht="25" customHeight="1">
       <c r="A196" s="3" t="inlineStr">
         <is>
-          <t>Van Rensburg</t>
+          <t>Van Niekerk</t>
         </is>
       </c>
       <c r="B196" s="3" t="inlineStr">
         <is>
-          <t>Neville</t>
+          <t>Riaan</t>
         </is>
       </c>
       <c r="C196" s="3" t="inlineStr">
         <is>
-          <t>Moorreesburg</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D196" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E196" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F196" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="197" ht="25" customHeight="1">
       <c r="A197" s="3" t="inlineStr">
         <is>
-          <t>Van Romburgh</t>
+          <t>Van Nieuwenhuyzen</t>
         </is>
       </c>
       <c r="B197" s="3" t="inlineStr">
         <is>
-          <t>Lorna</t>
+          <t>Hilgardt</t>
         </is>
       </c>
       <c r="C197" s="3" t="inlineStr">
         <is>
-          <t>Fish Hoek</t>
+          <t>Worcester</t>
         </is>
       </c>
       <c r="D197" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E197" s="3" t="inlineStr">
@@ -6723,34 +6723,34 @@
       </c>
       <c r="F197" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="198" ht="25" customHeight="1">
       <c r="A198" s="3" t="inlineStr">
         <is>
-          <t>Van Wyk-Nelson</t>
+          <t>Van Rensburg</t>
         </is>
       </c>
       <c r="B198" s="3" t="inlineStr">
         <is>
-          <t>Edith</t>
+          <t>Neville</t>
         </is>
       </c>
       <c r="C198" s="3" t="inlineStr">
         <is>
-          <t>Kuilsriver</t>
+          <t>Moorreesburg</t>
         </is>
       </c>
       <c r="D198" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E198" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F198" s="3" t="inlineStr">
@@ -6762,22 +6762,22 @@
     <row r="199" ht="25" customHeight="1">
       <c r="A199" s="3" t="inlineStr">
         <is>
-          <t>Van de Merwe</t>
+          <t>Van Romburgh</t>
         </is>
       </c>
       <c r="B199" s="3" t="inlineStr">
         <is>
-          <t>Marina</t>
+          <t>Lorna</t>
         </is>
       </c>
       <c r="C199" s="3" t="inlineStr">
         <is>
-          <t>Malmesbury</t>
+          <t>Fish Hoek</t>
         </is>
       </c>
       <c r="D199" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E199" s="3" t="inlineStr">
@@ -6794,17 +6794,17 @@
     <row r="200" ht="25" customHeight="1">
       <c r="A200" s="3" t="inlineStr">
         <is>
-          <t>Venter</t>
+          <t>Van Wyk-Nelson</t>
         </is>
       </c>
       <c r="B200" s="3" t="inlineStr">
         <is>
-          <t>Louis</t>
+          <t>Edith</t>
         </is>
       </c>
       <c r="C200" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Kuilsriver</t>
         </is>
       </c>
       <c r="D200" s="3" t="inlineStr">
@@ -6814,29 +6814,29 @@
       </c>
       <c r="E200" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F200" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="201" ht="25" customHeight="1">
       <c r="A201" s="3" t="inlineStr">
         <is>
-          <t>Volker</t>
+          <t>Van de Merwe</t>
         </is>
       </c>
       <c r="B201" s="3" t="inlineStr">
         <is>
-          <t>Russell</t>
+          <t>Marina</t>
         </is>
       </c>
       <c r="C201" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Malmesbury</t>
         </is>
       </c>
       <c r="D201" s="3" t="inlineStr">
@@ -6846,29 +6846,29 @@
       </c>
       <c r="E201" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F201" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="202" ht="25" customHeight="1">
       <c r="A202" s="3" t="inlineStr">
         <is>
-          <t>Von Mollendorf</t>
+          <t>Venter</t>
         </is>
       </c>
       <c r="B202" s="3" t="inlineStr">
         <is>
-          <t>Rinette</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="C202" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D202" s="3" t="inlineStr">
@@ -6878,29 +6878,29 @@
       </c>
       <c r="E202" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F202" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="203" ht="25" customHeight="1">
       <c r="A203" s="3" t="inlineStr">
         <is>
-          <t>Warman</t>
+          <t>Volker</t>
         </is>
       </c>
       <c r="B203" s="3" t="inlineStr">
         <is>
-          <t>Alastair</t>
+          <t>Russell</t>
         </is>
       </c>
       <c r="C203" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>King William's Town</t>
         </is>
       </c>
       <c r="D203" s="3" t="inlineStr">
@@ -6922,17 +6922,17 @@
     <row r="204" ht="25" customHeight="1">
       <c r="A204" s="3" t="inlineStr">
         <is>
-          <t>Watson</t>
+          <t>Von Mollendorf</t>
         </is>
       </c>
       <c r="B204" s="3" t="inlineStr">
         <is>
-          <t>Allan</t>
+          <t>Rinette</t>
         </is>
       </c>
       <c r="C204" s="3" t="inlineStr">
         <is>
-          <t>Sea Point</t>
+          <t>Durbanville</t>
         </is>
       </c>
       <c r="D204" s="3" t="inlineStr">
@@ -6954,17 +6954,17 @@
     <row r="205" ht="25" customHeight="1">
       <c r="A205" s="3" t="inlineStr">
         <is>
-          <t>Watson</t>
+          <t>Warman</t>
         </is>
       </c>
       <c r="B205" s="3" t="inlineStr">
         <is>
-          <t>Alison</t>
+          <t>Alastair</t>
         </is>
       </c>
       <c r="C205" s="3" t="inlineStr">
         <is>
-          <t>Sedgefield</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D205" s="3" t="inlineStr">
@@ -6979,24 +6979,24 @@
       </c>
       <c r="F205" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="206" ht="25" customHeight="1">
       <c r="A206" s="3" t="inlineStr">
         <is>
-          <t>Williams</t>
+          <t>Watson</t>
         </is>
       </c>
       <c r="B206" s="3" t="inlineStr">
         <is>
-          <t>Johanna</t>
+          <t>Allan</t>
         </is>
       </c>
       <c r="C206" s="3" t="inlineStr">
         <is>
-          <t>Mitchells Plain</t>
+          <t>Sea Point</t>
         </is>
       </c>
       <c r="D206" s="3" t="inlineStr">
@@ -7018,17 +7018,17 @@
     <row r="207" ht="25" customHeight="1">
       <c r="A207" s="3" t="inlineStr">
         <is>
-          <t>Wills</t>
+          <t>Watson</t>
         </is>
       </c>
       <c r="B207" s="3" t="inlineStr">
         <is>
-          <t>Geila</t>
+          <t>Alison</t>
         </is>
       </c>
       <c r="C207" s="3" t="inlineStr">
         <is>
-          <t>Athlone</t>
+          <t>Sedgefield</t>
         </is>
       </c>
       <c r="D207" s="3" t="inlineStr">
@@ -7038,7 +7038,7 @@
       </c>
       <c r="E207" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F207" s="3" t="inlineStr">
@@ -7050,22 +7050,22 @@
     <row r="208" ht="25" customHeight="1">
       <c r="A208" s="3" t="inlineStr">
         <is>
-          <t>Wilter-Sturges</t>
+          <t>Williams</t>
         </is>
       </c>
       <c r="B208" s="3" t="inlineStr">
         <is>
-          <t>Meredith</t>
+          <t>Johanna</t>
         </is>
       </c>
       <c r="C208" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Mitchells Plain</t>
         </is>
       </c>
       <c r="D208" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E208" s="3" t="inlineStr">
@@ -7075,24 +7075,24 @@
       </c>
       <c r="F208" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="209" ht="25" customHeight="1">
       <c r="A209" s="3" t="inlineStr">
         <is>
-          <t>Wright</t>
+          <t>Wills</t>
         </is>
       </c>
       <c r="B209" s="3" t="inlineStr">
         <is>
-          <t>Rocky</t>
+          <t>Geila</t>
         </is>
       </c>
       <c r="C209" s="3" t="inlineStr">
         <is>
-          <t>Table View</t>
+          <t>Athlone</t>
         </is>
       </c>
       <c r="D209" s="3" t="inlineStr">
@@ -7102,7 +7102,7 @@
       </c>
       <c r="E209" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F209" s="3" t="inlineStr">
@@ -7114,17 +7114,17 @@
     <row r="210" ht="25" customHeight="1">
       <c r="A210" s="3" t="inlineStr">
         <is>
-          <t>Young</t>
+          <t>Wilter-Sturges</t>
         </is>
       </c>
       <c r="B210" s="3" t="inlineStr">
         <is>
-          <t>Judy</t>
+          <t>Meredith</t>
         </is>
       </c>
       <c r="C210" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D210" s="3" t="inlineStr">
@@ -7139,24 +7139,24 @@
       </c>
       <c r="F210" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="211" ht="25" customHeight="1">
       <c r="A211" s="3" t="inlineStr">
         <is>
-          <t>de Kock</t>
+          <t>Wright</t>
         </is>
       </c>
       <c r="B211" s="3" t="inlineStr">
         <is>
-          <t>Engela</t>
+          <t>Rocky</t>
         </is>
       </c>
       <c r="C211" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Table View</t>
         </is>
       </c>
       <c r="D211" s="3" t="inlineStr">
@@ -7178,17 +7178,17 @@
     <row r="212" ht="25" customHeight="1">
       <c r="A212" s="3" t="inlineStr">
         <is>
-          <t>de Kock</t>
+          <t>Young</t>
         </is>
       </c>
       <c r="B212" s="3" t="inlineStr">
         <is>
-          <t>Francois</t>
+          <t>Judy</t>
         </is>
       </c>
       <c r="C212" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Durbanville</t>
         </is>
       </c>
       <c r="D212" s="3" t="inlineStr">
@@ -7198,7 +7198,7 @@
       </c>
       <c r="E212" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F212" s="3" t="inlineStr">
@@ -7210,49 +7210,49 @@
     <row r="213" ht="25" customHeight="1">
       <c r="A213" s="3" t="inlineStr">
         <is>
-          <t>de Silva</t>
+          <t>de Kock</t>
         </is>
       </c>
       <c r="B213" s="3" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Engela</t>
         </is>
       </c>
       <c r="C213" s="3" t="inlineStr">
         <is>
-          <t>Edenvale</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D213" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E213" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F213" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="214" ht="25" customHeight="1">
       <c r="A214" s="3" t="inlineStr">
         <is>
-          <t>du Toit</t>
+          <t>de Kock</t>
         </is>
       </c>
       <c r="B214" s="3" t="inlineStr">
         <is>
-          <t>Desiree</t>
+          <t>Francois</t>
         </is>
       </c>
       <c r="C214" s="3" t="inlineStr">
         <is>
-          <t>Ramsgate</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D214" s="3" t="inlineStr">
@@ -7262,29 +7262,29 @@
       </c>
       <c r="E214" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F214" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="215" ht="25" customHeight="1">
       <c r="A215" s="3" t="inlineStr">
         <is>
-          <t>stier</t>
+          <t>de Silva</t>
         </is>
       </c>
       <c r="B215" s="3" t="inlineStr">
         <is>
-          <t>RORY</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="C215" s="3" t="inlineStr">
         <is>
-          <t>Deep South</t>
+          <t>Edenvale</t>
         </is>
       </c>
       <c r="D215" s="3" t="inlineStr">
@@ -7294,29 +7294,29 @@
       </c>
       <c r="E215" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F215" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="216" ht="25" customHeight="1">
       <c r="A216" s="3" t="inlineStr">
         <is>
-          <t>van Blerk</t>
+          <t>du Toit</t>
         </is>
       </c>
       <c r="B216" s="3" t="inlineStr">
         <is>
-          <t>Carl</t>
+          <t>Desiree</t>
         </is>
       </c>
       <c r="C216" s="3" t="inlineStr">
         <is>
-          <t>Eden</t>
+          <t>Ramsgate</t>
         </is>
       </c>
       <c r="D216" s="3" t="inlineStr">
@@ -7331,56 +7331,56 @@
       </c>
       <c r="F216" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="217" ht="25" customHeight="1">
       <c r="A217" s="3" t="inlineStr">
         <is>
-          <t>van Heerden</t>
+          <t>stier</t>
         </is>
       </c>
       <c r="B217" s="3" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>RORY</t>
         </is>
       </c>
       <c r="C217" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Deep South</t>
         </is>
       </c>
       <c r="D217" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E217" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F217" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="218" ht="25" customHeight="1">
       <c r="A218" s="3" t="inlineStr">
         <is>
-          <t>van Heerden</t>
+          <t>van Blerk</t>
         </is>
       </c>
       <c r="B218" s="3" t="inlineStr">
         <is>
-          <t>Sandy</t>
+          <t>Carl</t>
         </is>
       </c>
       <c r="C218" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Eden</t>
         </is>
       </c>
       <c r="D218" s="3" t="inlineStr">
@@ -7390,12 +7390,12 @@
       </c>
       <c r="E218" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F218" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -7407,12 +7407,12 @@
       </c>
       <c r="B219" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Sydney</t>
         </is>
       </c>
       <c r="C219" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D219" s="3" t="inlineStr">
@@ -7422,7 +7422,7 @@
       </c>
       <c r="E219" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F219" s="3" t="inlineStr">
@@ -7434,17 +7434,17 @@
     <row r="220" ht="25" customHeight="1">
       <c r="A220" s="3" t="inlineStr">
         <is>
-          <t>van Rensburg</t>
+          <t>van Heerden</t>
         </is>
       </c>
       <c r="B220" s="3" t="inlineStr">
         <is>
-          <t>Johan</t>
+          <t>Sandy</t>
         </is>
       </c>
       <c r="C220" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D220" s="3" t="inlineStr">
@@ -7459,24 +7459,24 @@
       </c>
       <c r="F220" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="221" ht="25" customHeight="1">
       <c r="A221" s="3" t="inlineStr">
         <is>
-          <t>van Rensburg</t>
+          <t>van Heerden</t>
         </is>
       </c>
       <c r="B221" s="3" t="inlineStr">
         <is>
-          <t>Anne</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C221" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D221" s="3" t="inlineStr">
@@ -7486,29 +7486,29 @@
       </c>
       <c r="E221" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F221" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="222" ht="25" customHeight="1">
       <c r="A222" s="3" t="inlineStr">
         <is>
-          <t>van Wulven</t>
+          <t>van Rensburg</t>
         </is>
       </c>
       <c r="B222" s="3" t="inlineStr">
         <is>
-          <t>Jeannie</t>
+          <t>Johan</t>
         </is>
       </c>
       <c r="C222" s="3" t="inlineStr">
         <is>
-          <t>Tygerberg Hills</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D222" s="3" t="inlineStr">
@@ -7530,17 +7530,17 @@
     <row r="223" ht="25" customHeight="1">
       <c r="A223" s="3" t="inlineStr">
         <is>
-          <t>van Wulven</t>
+          <t>van Rensburg</t>
         </is>
       </c>
       <c r="B223" s="3" t="inlineStr">
         <is>
-          <t>Alan</t>
+          <t>Anne</t>
         </is>
       </c>
       <c r="C223" s="3" t="inlineStr">
         <is>
-          <t>Tygerberg Hills</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D223" s="3" t="inlineStr">
@@ -7567,7 +7567,7 @@
       </c>
       <c r="B224" s="3" t="inlineStr">
         <is>
-          <t>Deon</t>
+          <t>Jeannie</t>
         </is>
       </c>
       <c r="C224" s="3" t="inlineStr">
@@ -7582,7 +7582,7 @@
       </c>
       <c r="E224" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F224" s="3" t="inlineStr">
@@ -7594,17 +7594,17 @@
     <row r="225" ht="25" customHeight="1">
       <c r="A225" s="3" t="inlineStr">
         <is>
-          <t>van Wyk</t>
+          <t>van Wulven</t>
         </is>
       </c>
       <c r="B225" s="3" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>Alan</t>
         </is>
       </c>
       <c r="C225" s="3" t="inlineStr">
         <is>
-          <t>North Durban</t>
+          <t>Tygerberg Hills</t>
         </is>
       </c>
       <c r="D225" s="3" t="inlineStr">
@@ -7619,24 +7619,24 @@
       </c>
       <c r="F225" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="226" ht="25" customHeight="1">
       <c r="A226" s="3" t="inlineStr">
         <is>
-          <t>van Wyk</t>
+          <t>van Wulven</t>
         </is>
       </c>
       <c r="B226" s="3" t="inlineStr">
         <is>
-          <t>Lindie</t>
+          <t>Deon</t>
         </is>
       </c>
       <c r="C226" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Tygerberg Hills</t>
         </is>
       </c>
       <c r="D226" s="3" t="inlineStr">
@@ -7651,7 +7651,7 @@
       </c>
       <c r="F226" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -7663,12 +7663,12 @@
       </c>
       <c r="B227" s="3" t="inlineStr">
         <is>
-          <t>Willem</t>
+          <t>Kim</t>
         </is>
       </c>
       <c r="C227" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>North Durban</t>
         </is>
       </c>
       <c r="D227" s="3" t="inlineStr">
@@ -7695,7 +7695,7 @@
       </c>
       <c r="B228" s="3" t="inlineStr">
         <is>
-          <t>Patricia</t>
+          <t>Lindie</t>
         </is>
       </c>
       <c r="C228" s="3" t="inlineStr">
@@ -7722,27 +7722,27 @@
     <row r="229" ht="25" customHeight="1">
       <c r="A229" s="3" t="inlineStr">
         <is>
-          <t>van der Merwe</t>
+          <t>van Wyk</t>
         </is>
       </c>
       <c r="B229" s="3" t="inlineStr">
         <is>
-          <t>Ingrid</t>
+          <t>Willem</t>
         </is>
       </c>
       <c r="C229" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D229" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E229" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F229" s="3" t="inlineStr">
@@ -7754,17 +7754,17 @@
     <row r="230" ht="25" customHeight="1">
       <c r="A230" s="3" t="inlineStr">
         <is>
-          <t>van der Westhuizen</t>
+          <t>van Wyk</t>
         </is>
       </c>
       <c r="B230" s="3" t="inlineStr">
         <is>
-          <t>Hennie</t>
+          <t>Patricia</t>
         </is>
       </c>
       <c r="C230" s="3" t="inlineStr">
         <is>
-          <t>Helderberg</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D230" s="3" t="inlineStr">
@@ -7774,34 +7774,34 @@
       </c>
       <c r="E230" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F230" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="231" ht="25" customHeight="1">
       <c r="A231" s="3" t="inlineStr">
         <is>
-          <t>von der Decken</t>
+          <t>van der Merwe</t>
         </is>
       </c>
       <c r="B231" s="3" t="inlineStr">
         <is>
-          <t>Brian</t>
+          <t>Ingrid</t>
         </is>
       </c>
       <c r="C231" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D231" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E231" s="3" t="inlineStr">
@@ -7818,44 +7818,108 @@
     <row r="232" ht="25" customHeight="1">
       <c r="A232" s="3" t="inlineStr">
         <is>
+          <t>van der Westhuizen</t>
+        </is>
+      </c>
+      <c r="B232" s="3" t="inlineStr">
+        <is>
+          <t>Hennie</t>
+        </is>
+      </c>
+      <c r="C232" s="3" t="inlineStr">
+        <is>
+          <t>Helderberg</t>
+        </is>
+      </c>
+      <c r="D232" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E232" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F232" s="3" t="inlineStr">
+        <is>
+          <t>410W</t>
+        </is>
+      </c>
+    </row>
+    <row r="233" ht="25" customHeight="1">
+      <c r="A233" s="3" t="inlineStr">
+        <is>
+          <t>von der Decken</t>
+        </is>
+      </c>
+      <c r="B233" s="3" t="inlineStr">
+        <is>
+          <t>Brian</t>
+        </is>
+      </c>
+      <c r="C233" s="3" t="inlineStr">
+        <is>
+          <t>King William's Town</t>
+        </is>
+      </c>
+      <c r="D233" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E233" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F233" s="3" t="inlineStr">
+        <is>
+          <t>410E</t>
+        </is>
+      </c>
+    </row>
+    <row r="234" ht="25" customHeight="1">
+      <c r="A234" s="3" t="inlineStr">
+        <is>
           <t>‘t Hart</t>
         </is>
       </c>
-      <c r="B232" s="3" t="inlineStr">
+      <c r="B234" s="3" t="inlineStr">
         <is>
           <t>Michelle</t>
         </is>
       </c>
-      <c r="C232" s="3" t="inlineStr">
+      <c r="C234" s="3" t="inlineStr">
         <is>
           <t>Benoni Lakes</t>
         </is>
       </c>
-      <c r="D232" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E232" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F232" s="3" t="inlineStr">
+      <c r="D234" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E234" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F234" s="3" t="inlineStr">
         <is>
           <t>410E</t>
         </is>
       </c>
     </row>
-    <row r="233">
-      <c r="A233" s="1" t="inlineStr">
-        <is>
-          <t>Number of attendees: 230</t>
-        </is>
-      </c>
-    </row>
-    <row r="234">
-      <c r="A234" s="1" t="inlineStr">
+    <row r="235">
+      <c r="A235" s="1" t="inlineStr">
+        <is>
+          <t>Number of attendees: 232</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" s="1" t="inlineStr">
         <is>
           <t>Number of voters: 109</t>
         </is>
@@ -7873,7 +7937,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E125"/>
+  <dimension ref="A1:E127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7891,7 +7955,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Registrees as of 18/04/2021 21:32</t>
+          <t>410E Registrees as of 19/04/2021 10:15</t>
         </is>
       </c>
     </row>
@@ -9842,17 +9906,17 @@
     <row r="74" ht="25" customHeight="1">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>Oberholzer</t>
+          <t>Ngobozana</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
         <is>
-          <t>PDG Bokkie</t>
+          <t>Sphiwe</t>
         </is>
       </c>
       <c r="C74" s="3" t="inlineStr">
         <is>
-          <t>Uitenhage</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D74" s="3" t="inlineStr">
@@ -9862,24 +9926,24 @@
       </c>
       <c r="E74" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="75" ht="25" customHeight="1">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>PORTEOUS</t>
+          <t>Oberholzer</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
         <is>
-          <t>BRIAN</t>
+          <t>PDG Bokkie</t>
         </is>
       </c>
       <c r="C75" s="3" t="inlineStr">
         <is>
-          <t>Hibberdene</t>
+          <t>Uitenhage</t>
         </is>
       </c>
       <c r="D75" s="3" t="inlineStr">
@@ -9896,17 +9960,17 @@
     <row r="76" ht="25" customHeight="1">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>Paijmans</t>
+          <t>PORTEOUS</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
         <is>
-          <t>Bronwyn Anne</t>
+          <t>BRIAN</t>
         </is>
       </c>
       <c r="C76" s="3" t="inlineStr">
         <is>
-          <t>Cowies Hill</t>
+          <t>Hibberdene</t>
         </is>
       </c>
       <c r="D76" s="3" t="inlineStr">
@@ -9916,24 +9980,24 @@
       </c>
       <c r="E76" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="77" ht="25" customHeight="1">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>Pantoleon</t>
+          <t>Paijmans</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
         <is>
-          <t>Teresa</t>
+          <t>Bronwyn Anne</t>
         </is>
       </c>
       <c r="C77" s="3" t="inlineStr">
         <is>
-          <t>Vereeniging</t>
+          <t>Cowies Hill</t>
         </is>
       </c>
       <c r="D77" s="3" t="inlineStr">
@@ -9943,24 +10007,24 @@
       </c>
       <c r="E77" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="78" ht="25" customHeight="1">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>Polkinghorne</t>
+          <t>Pantoleon</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
         <is>
-          <t>Tracey</t>
+          <t>Teresa</t>
         </is>
       </c>
       <c r="C78" s="3" t="inlineStr">
         <is>
-          <t>Kensington</t>
+          <t>Vereeniging</t>
         </is>
       </c>
       <c r="D78" s="3" t="inlineStr">
@@ -9982,7 +10046,7 @@
       </c>
       <c r="B79" s="3" t="inlineStr">
         <is>
-          <t>Gavin</t>
+          <t>Tracey</t>
         </is>
       </c>
       <c r="C79" s="3" t="inlineStr">
@@ -9997,24 +10061,24 @@
       </c>
       <c r="E79" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="80" ht="25" customHeight="1">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>Ras</t>
+          <t>Polkinghorne</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
         <is>
-          <t>Leon Jacobus</t>
+          <t>Gavin</t>
         </is>
       </c>
       <c r="C80" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Kensington</t>
         </is>
       </c>
       <c r="D80" s="3" t="inlineStr">
@@ -10031,17 +10095,17 @@
     <row r="81" ht="25" customHeight="1">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>Reniers</t>
+          <t>Ras</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
         <is>
-          <t>Hugo</t>
+          <t>Leon Jacobus</t>
         </is>
       </c>
       <c r="C81" s="3" t="inlineStr">
         <is>
-          <t>Nelspruit</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D81" s="3" t="inlineStr">
@@ -10051,24 +10115,24 @@
       </c>
       <c r="E81" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="82" ht="25" customHeight="1">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>Sabatier</t>
+          <t>Reniers</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
         <is>
-          <t>Rodney</t>
+          <t>Hugo</t>
         </is>
       </c>
       <c r="C82" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Nelspruit</t>
         </is>
       </c>
       <c r="D82" s="3" t="inlineStr">
@@ -10085,17 +10149,17 @@
     <row r="83" ht="25" customHeight="1">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>Searle</t>
+          <t>Sabatier</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
         <is>
-          <t>Francis</t>
+          <t>Rodney</t>
         </is>
       </c>
       <c r="C83" s="3" t="inlineStr">
         <is>
-          <t>Kouga</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D83" s="3" t="inlineStr">
@@ -10117,7 +10181,7 @@
       </c>
       <c r="B84" s="3" t="inlineStr">
         <is>
-          <t>Gloria</t>
+          <t>Francis</t>
         </is>
       </c>
       <c r="C84" s="3" t="inlineStr">
@@ -10132,24 +10196,24 @@
       </c>
       <c r="E84" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="85" ht="25" customHeight="1">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>Smit</t>
+          <t>Searle</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
         <is>
-          <t>Sue</t>
+          <t>Gloria</t>
         </is>
       </c>
       <c r="C85" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Kouga</t>
         </is>
       </c>
       <c r="D85" s="3" t="inlineStr">
@@ -10159,24 +10223,24 @@
       </c>
       <c r="E85" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="86" ht="25" customHeight="1">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Smit</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
         <is>
-          <t>Jeff</t>
+          <t>Sue</t>
         </is>
       </c>
       <c r="C86" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D86" s="3" t="inlineStr">
@@ -10186,24 +10250,24 @@
       </c>
       <c r="E86" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="87" ht="25" customHeight="1">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>Stander</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
         <is>
-          <t>Max</t>
+          <t>Jeff</t>
         </is>
       </c>
       <c r="C87" s="3" t="inlineStr">
         <is>
-          <t>Port Alfred</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D87" s="3" t="inlineStr">
@@ -10213,7 +10277,7 @@
       </c>
       <c r="E87" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -10225,12 +10289,12 @@
       </c>
       <c r="B88" s="3" t="inlineStr">
         <is>
-          <t>Ashley</t>
+          <t>Max</t>
         </is>
       </c>
       <c r="C88" s="3" t="inlineStr">
         <is>
-          <t>Krugersdorp</t>
+          <t>Port Alfred</t>
         </is>
       </c>
       <c r="D88" s="3" t="inlineStr">
@@ -10252,7 +10316,7 @@
       </c>
       <c r="B89" s="3" t="inlineStr">
         <is>
-          <t>Brett Jason</t>
+          <t>Ashley</t>
         </is>
       </c>
       <c r="C89" s="3" t="inlineStr">
@@ -10267,29 +10331,29 @@
       </c>
       <c r="E89" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="90" ht="25" customHeight="1">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>Steyn</t>
+          <t>Stander</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
         <is>
-          <t>Elna</t>
+          <t>Brett Jason</t>
         </is>
       </c>
       <c r="C90" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Krugersdorp</t>
         </is>
       </c>
       <c r="D90" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E90" s="3" t="inlineStr">
@@ -10301,22 +10365,22 @@
     <row r="91" ht="25" customHeight="1">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>Sturges</t>
+          <t>Steyn</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
         <is>
-          <t>Trevor</t>
+          <t>Elna</t>
         </is>
       </c>
       <c r="C91" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D91" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E91" s="3" t="inlineStr">
@@ -10328,17 +10392,17 @@
     <row r="92" ht="25" customHeight="1">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>Talbot</t>
+          <t>Sturges</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
         <is>
-          <t>Lauryn</t>
+          <t>Trevor</t>
         </is>
       </c>
       <c r="C92" s="3" t="inlineStr">
         <is>
-          <t>Benoni Lakes</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D92" s="3" t="inlineStr">
@@ -10355,17 +10419,17 @@
     <row r="93" ht="25" customHeight="1">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>Theron</t>
+          <t>Talbot</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
         <is>
-          <t>Pierre</t>
+          <t>Lauryn</t>
         </is>
       </c>
       <c r="C93" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Benoni Lakes</t>
         </is>
       </c>
       <c r="D93" s="3" t="inlineStr">
@@ -10387,7 +10451,7 @@
       </c>
       <c r="B94" s="3" t="inlineStr">
         <is>
-          <t>Moira</t>
+          <t>Pierre</t>
         </is>
       </c>
       <c r="C94" s="3" t="inlineStr">
@@ -10409,17 +10473,17 @@
     <row r="95" ht="25" customHeight="1">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>Townsend</t>
+          <t>Theron</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
         <is>
-          <t>Diane</t>
+          <t>Moira</t>
         </is>
       </c>
       <c r="C95" s="3" t="inlineStr">
         <is>
-          <t>Benoni Lakes</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D95" s="3" t="inlineStr">
@@ -10436,22 +10500,22 @@
     <row r="96" ht="25" customHeight="1">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>Toye</t>
+          <t>Townsend</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
         <is>
-          <t>Omolayo</t>
+          <t>Diane</t>
         </is>
       </c>
       <c r="C96" s="3" t="inlineStr">
         <is>
-          <t>The Wilds</t>
+          <t>Benoni Lakes</t>
         </is>
       </c>
       <c r="D96" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E96" s="3" t="inlineStr">
@@ -10463,22 +10527,22 @@
     <row r="97" ht="25" customHeight="1">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>Tuckett</t>
+          <t>Toye</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
         <is>
-          <t>Alistair</t>
+          <t>Omolayo</t>
         </is>
       </c>
       <c r="C97" s="3" t="inlineStr">
         <is>
-          <t>Roodepoort Clearwater Cyber</t>
+          <t>The Wilds</t>
         </is>
       </c>
       <c r="D97" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E97" s="3" t="inlineStr">
@@ -10495,7 +10559,7 @@
       </c>
       <c r="B98" s="3" t="inlineStr">
         <is>
-          <t>Rowan</t>
+          <t>Alistair</t>
         </is>
       </c>
       <c r="C98" s="3" t="inlineStr">
@@ -10510,7 +10574,7 @@
       </c>
       <c r="E98" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -10522,7 +10586,7 @@
       </c>
       <c r="B99" s="3" t="inlineStr">
         <is>
-          <t>Gail</t>
+          <t>Rowan</t>
         </is>
       </c>
       <c r="C99" s="3" t="inlineStr">
@@ -10537,29 +10601,29 @@
       </c>
       <c r="E99" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="100" ht="25" customHeight="1">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>Uchytil</t>
+          <t>Tuckett</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
         <is>
-          <t>Jiri</t>
+          <t>Gail</t>
         </is>
       </c>
       <c r="C100" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Roodepoort Clearwater Cyber</t>
         </is>
       </c>
       <c r="D100" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E100" s="3" t="inlineStr">
@@ -10571,17 +10635,17 @@
     <row r="101" ht="25" customHeight="1">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>VAN DER MERWE</t>
+          <t>Uchytil</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
         <is>
-          <t>PATRICIA</t>
+          <t>Jiri</t>
         </is>
       </c>
       <c r="C101" s="3" t="inlineStr">
         <is>
-          <t>East London Port Rex</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D101" s="3" t="inlineStr">
@@ -10591,24 +10655,24 @@
       </c>
       <c r="E101" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="102" ht="25" customHeight="1">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>Van Niekerk</t>
+          <t>VAN DER MERWE</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
         <is>
-          <t>Riaan</t>
+          <t>PATRICIA</t>
         </is>
       </c>
       <c r="C102" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>East London Port Rex</t>
         </is>
       </c>
       <c r="D102" s="3" t="inlineStr">
@@ -10618,24 +10682,24 @@
       </c>
       <c r="E102" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="103" ht="25" customHeight="1">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>Venter</t>
+          <t>Van Niekerk</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
         <is>
-          <t>Louis</t>
+          <t>Riaan</t>
         </is>
       </c>
       <c r="C103" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D103" s="3" t="inlineStr">
@@ -10645,24 +10709,24 @@
       </c>
       <c r="E103" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="104" ht="25" customHeight="1">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>Volker</t>
+          <t>Van Nieuwenhuyzen</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
         <is>
-          <t>Russell</t>
+          <t>Hilgardt</t>
         </is>
       </c>
       <c r="C104" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Worcester</t>
         </is>
       </c>
       <c r="D104" s="3" t="inlineStr">
@@ -10672,29 +10736,29 @@
       </c>
       <c r="E104" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="105" ht="25" customHeight="1">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>Warman</t>
+          <t>Venter</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
         <is>
-          <t>Alastair</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="C105" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D105" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E105" s="3" t="inlineStr">
@@ -10706,17 +10770,17 @@
     <row r="106" ht="25" customHeight="1">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>Williamson</t>
+          <t>Volker</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
         <is>
-          <t>Neville</t>
+          <t>Russell</t>
         </is>
       </c>
       <c r="C106" s="3" t="inlineStr">
         <is>
-          <t>Port Alfred</t>
+          <t>King William's Town</t>
         </is>
       </c>
       <c r="D106" s="3" t="inlineStr">
@@ -10726,24 +10790,24 @@
       </c>
       <c r="E106" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="107" ht="25" customHeight="1">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>Wilter-Sturges</t>
+          <t>Warman</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
         <is>
-          <t>Meredith</t>
+          <t>Alastair</t>
         </is>
       </c>
       <c r="C107" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D107" s="3" t="inlineStr">
@@ -10753,24 +10817,24 @@
       </c>
       <c r="E107" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="108" ht="25" customHeight="1">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>Zucker</t>
+          <t>Williamson</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
         <is>
-          <t>Leonie</t>
+          <t>Neville</t>
         </is>
       </c>
       <c r="C108" s="3" t="inlineStr">
         <is>
-          <t>Milnerton</t>
+          <t>Port Alfred</t>
         </is>
       </c>
       <c r="D108" s="3" t="inlineStr">
@@ -10780,29 +10844,29 @@
       </c>
       <c r="E108" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="109" ht="25" customHeight="1">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>de Silva</t>
+          <t>Wilter-Sturges</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Meredith</t>
         </is>
       </c>
       <c r="C109" s="3" t="inlineStr">
         <is>
-          <t>Edenvale</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D109" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E109" s="3" t="inlineStr">
@@ -10814,17 +10878,17 @@
     <row r="110" ht="25" customHeight="1">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>du Plooy</t>
+          <t>Zucker</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
         <is>
-          <t>Tammy</t>
+          <t>Leonie</t>
         </is>
       </c>
       <c r="C110" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Milnerton</t>
         </is>
       </c>
       <c r="D110" s="3" t="inlineStr">
@@ -10841,44 +10905,44 @@
     <row r="111" ht="25" customHeight="1">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>du Plooy</t>
+          <t>de Silva</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
         <is>
-          <t>Marc</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="C111" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Edenvale</t>
         </is>
       </c>
       <c r="D111" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E111" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="112" ht="25" customHeight="1">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>du Toit</t>
+          <t>du Plooy</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
         <is>
-          <t>Desiree</t>
+          <t>Tammy</t>
         </is>
       </c>
       <c r="C112" s="3" t="inlineStr">
         <is>
-          <t>Ramsgate</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D112" s="3" t="inlineStr">
@@ -10888,24 +10952,24 @@
       </c>
       <c r="E112" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="113" ht="25" customHeight="1">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>le Roux</t>
+          <t>du Plooy</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
         <is>
-          <t>Jeanette</t>
+          <t>Marc</t>
         </is>
       </c>
       <c r="C113" s="3" t="inlineStr">
         <is>
-          <t>Gonubie</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D113" s="3" t="inlineStr">
@@ -10915,24 +10979,24 @@
       </c>
       <c r="E113" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="114" ht="25" customHeight="1">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>van Heerden</t>
+          <t>du Toit</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Desiree</t>
         </is>
       </c>
       <c r="C114" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Ramsgate</t>
         </is>
       </c>
       <c r="D114" s="3" t="inlineStr">
@@ -10949,17 +11013,17 @@
     <row r="115" ht="25" customHeight="1">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>van Heerden</t>
+          <t>le Roux</t>
         </is>
       </c>
       <c r="B115" s="3" t="inlineStr">
         <is>
-          <t>Sandy</t>
+          <t>Jeanette</t>
         </is>
       </c>
       <c r="C115" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Gonubie</t>
         </is>
       </c>
       <c r="D115" s="3" t="inlineStr">
@@ -10969,7 +11033,7 @@
       </c>
       <c r="E115" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -10981,12 +11045,12 @@
       </c>
       <c r="B116" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Sydney</t>
         </is>
       </c>
       <c r="C116" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D116" s="3" t="inlineStr">
@@ -10996,24 +11060,24 @@
       </c>
       <c r="E116" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="117" ht="25" customHeight="1">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>van Wyk</t>
+          <t>van Heerden</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>Sandy</t>
         </is>
       </c>
       <c r="C117" s="3" t="inlineStr">
         <is>
-          <t>North Durban</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D117" s="3" t="inlineStr">
@@ -11023,24 +11087,24 @@
       </c>
       <c r="E117" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="118" ht="25" customHeight="1">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>van Wyk</t>
+          <t>van Heerden</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
         <is>
-          <t>Lindie</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C118" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D118" s="3" t="inlineStr">
@@ -11050,7 +11114,7 @@
       </c>
       <c r="E118" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -11062,12 +11126,12 @@
       </c>
       <c r="B119" s="3" t="inlineStr">
         <is>
-          <t>Willem</t>
+          <t>Kim</t>
         </is>
       </c>
       <c r="C119" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>North Durban</t>
         </is>
       </c>
       <c r="D119" s="3" t="inlineStr">
@@ -11089,7 +11153,7 @@
       </c>
       <c r="B120" s="3" t="inlineStr">
         <is>
-          <t>Patricia</t>
+          <t>Lindie</t>
         </is>
       </c>
       <c r="C120" s="3" t="inlineStr">
@@ -11111,44 +11175,44 @@
     <row r="121" ht="25" customHeight="1">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>van der Merwe</t>
+          <t>van Wyk</t>
         </is>
       </c>
       <c r="B121" s="3" t="inlineStr">
         <is>
-          <t>Ingrid</t>
+          <t>Willem</t>
         </is>
       </c>
       <c r="C121" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D121" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E121" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="122" ht="25" customHeight="1">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>von der Decken</t>
+          <t>van Wyk</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
         <is>
-          <t>Brian</t>
+          <t>Patricia</t>
         </is>
       </c>
       <c r="C122" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D122" s="3" t="inlineStr">
@@ -11158,46 +11222,100 @@
       </c>
       <c r="E122" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="123" ht="25" customHeight="1">
       <c r="A123" s="3" t="inlineStr">
         <is>
+          <t>van der Merwe</t>
+        </is>
+      </c>
+      <c r="B123" s="3" t="inlineStr">
+        <is>
+          <t>Ingrid</t>
+        </is>
+      </c>
+      <c r="C123" s="3" t="inlineStr">
+        <is>
+          <t>Letaba Tzaneen</t>
+        </is>
+      </c>
+      <c r="D123" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="E123" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="124" ht="25" customHeight="1">
+      <c r="A124" s="3" t="inlineStr">
+        <is>
+          <t>von der Decken</t>
+        </is>
+      </c>
+      <c r="B124" s="3" t="inlineStr">
+        <is>
+          <t>Brian</t>
+        </is>
+      </c>
+      <c r="C124" s="3" t="inlineStr">
+        <is>
+          <t>King William's Town</t>
+        </is>
+      </c>
+      <c r="D124" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E124" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="125" ht="25" customHeight="1">
+      <c r="A125" s="3" t="inlineStr">
+        <is>
           <t>‘t Hart</t>
         </is>
       </c>
-      <c r="B123" s="3" t="inlineStr">
+      <c r="B125" s="3" t="inlineStr">
         <is>
           <t>Michelle</t>
         </is>
       </c>
-      <c r="C123" s="3" t="inlineStr">
+      <c r="C125" s="3" t="inlineStr">
         <is>
           <t>Benoni Lakes</t>
         </is>
       </c>
-      <c r="D123" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E123" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" s="1" t="inlineStr">
-        <is>
-          <t>Number of attendees: 121</t>
-        </is>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" s="1" t="inlineStr">
+      <c r="D125" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E125" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="1" t="inlineStr">
+        <is>
+          <t>Number of attendees: 123</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="inlineStr">
         <is>
           <t>Number of voters: 60</t>
         </is>
@@ -11233,7 +11351,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Registrees as of 18/04/2021 21:32</t>
+          <t>410W Registrees as of 19/04/2021 10:15</t>
         </is>
       </c>
     </row>
@@ -15274,7 +15392,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Voting details as of 18/04/2021 21:32</t>
+          <t>410E Voting details as of 19/04/2021 10:15</t>
         </is>
       </c>
     </row>
@@ -15611,7 +15729,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Voting details as of 18/04/2021 21:32</t>
+          <t>410W Voting details as of 19/04/2021 10:15</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Registree stats backup on Tue 20 Apr 2021 08:45:05 SAST
</commit_message>
<xml_diff>
--- a/static/docs/registrees_list.xlsx
+++ b/static/docs/registrees_list.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F236"/>
+  <dimension ref="A1:F237"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,7 +451,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>MD410 Registrees as of 19/04/2021 10:15</t>
+          <t>MD410 Registrees as of 20/04/2021 08:45</t>
         </is>
       </c>
     </row>
@@ -6250,17 +6250,17 @@
     <row r="183" ht="25" customHeight="1">
       <c r="A183" s="3" t="inlineStr">
         <is>
-          <t>Sturges</t>
+          <t>Strydom</t>
         </is>
       </c>
       <c r="B183" s="3" t="inlineStr">
         <is>
-          <t>Trevor</t>
+          <t>Melinda Lee</t>
         </is>
       </c>
       <c r="C183" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D183" s="3" t="inlineStr">
@@ -6282,17 +6282,17 @@
     <row r="184" ht="25" customHeight="1">
       <c r="A184" s="3" t="inlineStr">
         <is>
-          <t>Talbot</t>
+          <t>Sturges</t>
         </is>
       </c>
       <c r="B184" s="3" t="inlineStr">
         <is>
-          <t>Lauryn</t>
+          <t>Trevor</t>
         </is>
       </c>
       <c r="C184" s="3" t="inlineStr">
         <is>
-          <t>Benoni Lakes</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D184" s="3" t="inlineStr">
@@ -6314,17 +6314,17 @@
     <row r="185" ht="25" customHeight="1">
       <c r="A185" s="3" t="inlineStr">
         <is>
-          <t>Theron</t>
+          <t>Talbot</t>
         </is>
       </c>
       <c r="B185" s="3" t="inlineStr">
         <is>
-          <t>Pierre</t>
+          <t>Lauryn</t>
         </is>
       </c>
       <c r="C185" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Benoni Lakes</t>
         </is>
       </c>
       <c r="D185" s="3" t="inlineStr">
@@ -6351,7 +6351,7 @@
       </c>
       <c r="B186" s="3" t="inlineStr">
         <is>
-          <t>Moira</t>
+          <t>Pierre</t>
         </is>
       </c>
       <c r="C186" s="3" t="inlineStr">
@@ -6378,22 +6378,22 @@
     <row r="187" ht="25" customHeight="1">
       <c r="A187" s="3" t="inlineStr">
         <is>
-          <t>Toye</t>
+          <t>Theron</t>
         </is>
       </c>
       <c r="B187" s="3" t="inlineStr">
         <is>
-          <t>Omolayo</t>
+          <t>Moira</t>
         </is>
       </c>
       <c r="C187" s="3" t="inlineStr">
         <is>
-          <t>The Wilds</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D187" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E187" s="3" t="inlineStr">
@@ -6410,22 +6410,22 @@
     <row r="188" ht="25" customHeight="1">
       <c r="A188" s="3" t="inlineStr">
         <is>
-          <t>Tshikala</t>
+          <t>Toye</t>
         </is>
       </c>
       <c r="B188" s="3" t="inlineStr">
         <is>
-          <t>David Alex</t>
+          <t>Omolayo</t>
         </is>
       </c>
       <c r="C188" s="3" t="inlineStr">
         <is>
-          <t>Athlone</t>
+          <t>The Wilds</t>
         </is>
       </c>
       <c r="D188" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E188" s="3" t="inlineStr">
@@ -6435,24 +6435,24 @@
       </c>
       <c r="F188" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="189" ht="25" customHeight="1">
       <c r="A189" s="3" t="inlineStr">
         <is>
-          <t>Tuckett</t>
+          <t>Tshikala</t>
         </is>
       </c>
       <c r="B189" s="3" t="inlineStr">
         <is>
-          <t>Alistair</t>
+          <t>David Alex</t>
         </is>
       </c>
       <c r="C189" s="3" t="inlineStr">
         <is>
-          <t>Roodepoort Clearwater Cyber</t>
+          <t>Athlone</t>
         </is>
       </c>
       <c r="D189" s="3" t="inlineStr">
@@ -6467,7 +6467,7 @@
       </c>
       <c r="F189" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -6479,7 +6479,7 @@
       </c>
       <c r="B190" s="3" t="inlineStr">
         <is>
-          <t>Rowan</t>
+          <t>Alistair</t>
         </is>
       </c>
       <c r="C190" s="3" t="inlineStr">
@@ -6494,7 +6494,7 @@
       </c>
       <c r="E190" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F190" s="3" t="inlineStr">
@@ -6511,7 +6511,7 @@
       </c>
       <c r="B191" s="3" t="inlineStr">
         <is>
-          <t>Gail</t>
+          <t>Rowan</t>
         </is>
       </c>
       <c r="C191" s="3" t="inlineStr">
@@ -6526,7 +6526,7 @@
       </c>
       <c r="E191" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F191" s="3" t="inlineStr">
@@ -6538,17 +6538,17 @@
     <row r="192" ht="25" customHeight="1">
       <c r="A192" s="3" t="inlineStr">
         <is>
-          <t>VAN BREDA</t>
+          <t>Tuckett</t>
         </is>
       </c>
       <c r="B192" s="3" t="inlineStr">
         <is>
-          <t>HILARY LISE</t>
+          <t>Gail</t>
         </is>
       </c>
       <c r="C192" s="3" t="inlineStr">
         <is>
-          <t>Cape Town</t>
+          <t>Roodepoort Clearwater Cyber</t>
         </is>
       </c>
       <c r="D192" s="3" t="inlineStr">
@@ -6563,39 +6563,39 @@
       </c>
       <c r="F192" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="193" ht="25" customHeight="1">
       <c r="A193" s="3" t="inlineStr">
         <is>
-          <t>VAN DER MERWE</t>
+          <t>VAN BREDA</t>
         </is>
       </c>
       <c r="B193" s="3" t="inlineStr">
         <is>
-          <t>PATRICIA</t>
+          <t>HILARY LISE</t>
         </is>
       </c>
       <c r="C193" s="3" t="inlineStr">
         <is>
-          <t>East London Port Rex</t>
+          <t>Cape Town</t>
         </is>
       </c>
       <c r="D193" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E193" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F193" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -6607,17 +6607,17 @@
       </c>
       <c r="B194" s="3" t="inlineStr">
         <is>
-          <t>MARINA</t>
+          <t>PATRICIA</t>
         </is>
       </c>
       <c r="C194" s="3" t="inlineStr">
         <is>
-          <t>Malmesbury</t>
+          <t>East London Port Rex</t>
         </is>
       </c>
       <c r="D194" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E194" s="3" t="inlineStr">
@@ -6627,56 +6627,56 @@
       </c>
       <c r="F194" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="195" ht="25" customHeight="1">
       <c r="A195" s="3" t="inlineStr">
         <is>
-          <t>Valadao</t>
+          <t>VAN DER MERWE</t>
         </is>
       </c>
       <c r="B195" s="3" t="inlineStr">
         <is>
-          <t>Tracy</t>
+          <t>MARINA</t>
         </is>
       </c>
       <c r="C195" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Malmesbury</t>
         </is>
       </c>
       <c r="D195" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E195" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F195" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="196" ht="25" customHeight="1">
       <c r="A196" s="3" t="inlineStr">
         <is>
-          <t>Van Niekerk</t>
+          <t>Valadao</t>
         </is>
       </c>
       <c r="B196" s="3" t="inlineStr">
         <is>
-          <t>Riaan</t>
+          <t>Tracy</t>
         </is>
       </c>
       <c r="C196" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D196" s="3" t="inlineStr">
@@ -6698,22 +6698,22 @@
     <row r="197" ht="25" customHeight="1">
       <c r="A197" s="3" t="inlineStr">
         <is>
-          <t>Van Nieuwenhuyzen</t>
+          <t>Van Niekerk</t>
         </is>
       </c>
       <c r="B197" s="3" t="inlineStr">
         <is>
-          <t>Hilgardt</t>
+          <t>Riaan</t>
         </is>
       </c>
       <c r="C197" s="3" t="inlineStr">
         <is>
-          <t>Worcester</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D197" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E197" s="3" t="inlineStr">
@@ -6730,17 +6730,17 @@
     <row r="198" ht="25" customHeight="1">
       <c r="A198" s="3" t="inlineStr">
         <is>
-          <t>Van Rensburg</t>
+          <t>Van Nieuwenhuyzen</t>
         </is>
       </c>
       <c r="B198" s="3" t="inlineStr">
         <is>
-          <t>Neville</t>
+          <t>Hilgardt</t>
         </is>
       </c>
       <c r="C198" s="3" t="inlineStr">
         <is>
-          <t>Moorreesburg</t>
+          <t>Worcester</t>
         </is>
       </c>
       <c r="D198" s="3" t="inlineStr">
@@ -6750,39 +6750,39 @@
       </c>
       <c r="E198" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F198" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="199" ht="25" customHeight="1">
       <c r="A199" s="3" t="inlineStr">
         <is>
-          <t>Van Romburgh</t>
+          <t>Van Rensburg</t>
         </is>
       </c>
       <c r="B199" s="3" t="inlineStr">
         <is>
-          <t>Lorna</t>
+          <t>Neville</t>
         </is>
       </c>
       <c r="C199" s="3" t="inlineStr">
         <is>
-          <t>Fish Hoek</t>
+          <t>Moorreesburg</t>
         </is>
       </c>
       <c r="D199" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E199" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F199" s="3" t="inlineStr">
@@ -6794,17 +6794,17 @@
     <row r="200" ht="25" customHeight="1">
       <c r="A200" s="3" t="inlineStr">
         <is>
-          <t>Van Wyk-Nelson</t>
+          <t>Van Romburgh</t>
         </is>
       </c>
       <c r="B200" s="3" t="inlineStr">
         <is>
-          <t>Edith</t>
+          <t>Lorna</t>
         </is>
       </c>
       <c r="C200" s="3" t="inlineStr">
         <is>
-          <t>Kuilsriver</t>
+          <t>Fish Hoek</t>
         </is>
       </c>
       <c r="D200" s="3" t="inlineStr">
@@ -6826,22 +6826,22 @@
     <row r="201" ht="25" customHeight="1">
       <c r="A201" s="3" t="inlineStr">
         <is>
-          <t>Van de Merwe</t>
+          <t>Van Wyk-Nelson</t>
         </is>
       </c>
       <c r="B201" s="3" t="inlineStr">
         <is>
-          <t>Marina</t>
+          <t>Edith</t>
         </is>
       </c>
       <c r="C201" s="3" t="inlineStr">
         <is>
-          <t>Malmesbury</t>
+          <t>Kuilsriver</t>
         </is>
       </c>
       <c r="D201" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E201" s="3" t="inlineStr">
@@ -6858,54 +6858,54 @@
     <row r="202" ht="25" customHeight="1">
       <c r="A202" s="3" t="inlineStr">
         <is>
-          <t>Venter</t>
+          <t>Van de Merwe</t>
         </is>
       </c>
       <c r="B202" s="3" t="inlineStr">
         <is>
-          <t>Louis</t>
+          <t>Marina</t>
         </is>
       </c>
       <c r="C202" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Malmesbury</t>
         </is>
       </c>
       <c r="D202" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E202" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F202" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="203" ht="25" customHeight="1">
       <c r="A203" s="3" t="inlineStr">
         <is>
-          <t>Volker</t>
+          <t>Venter</t>
         </is>
       </c>
       <c r="B203" s="3" t="inlineStr">
         <is>
-          <t>Russell</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="C203" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D203" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E203" s="3" t="inlineStr">
@@ -6922,96 +6922,96 @@
     <row r="204" ht="25" customHeight="1">
       <c r="A204" s="3" t="inlineStr">
         <is>
-          <t>Von Mollendorf</t>
+          <t>Volker</t>
         </is>
       </c>
       <c r="B204" s="3" t="inlineStr">
         <is>
-          <t>Rinette</t>
+          <t>Russell</t>
         </is>
       </c>
       <c r="C204" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>King William's Town</t>
         </is>
       </c>
       <c r="D204" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E204" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F204" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="205" ht="25" customHeight="1">
       <c r="A205" s="3" t="inlineStr">
         <is>
-          <t>Warman</t>
+          <t>Von Mollendorf</t>
         </is>
       </c>
       <c r="B205" s="3" t="inlineStr">
         <is>
-          <t>Alastair</t>
+          <t>Rinette</t>
         </is>
       </c>
       <c r="C205" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Durbanville</t>
         </is>
       </c>
       <c r="D205" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E205" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F205" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="206" ht="25" customHeight="1">
       <c r="A206" s="3" t="inlineStr">
         <is>
-          <t>Watson</t>
+          <t>Warman</t>
         </is>
       </c>
       <c r="B206" s="3" t="inlineStr">
         <is>
-          <t>Allan</t>
+          <t>Alastair</t>
         </is>
       </c>
       <c r="C206" s="3" t="inlineStr">
         <is>
-          <t>Sea Point</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D206" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E206" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F206" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -7023,22 +7023,22 @@
       </c>
       <c r="B207" s="3" t="inlineStr">
         <is>
-          <t>Alison</t>
+          <t>Allan</t>
         </is>
       </c>
       <c r="C207" s="3" t="inlineStr">
         <is>
-          <t>Sedgefield</t>
+          <t>Sea Point</t>
         </is>
       </c>
       <c r="D207" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E207" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F207" s="3" t="inlineStr">
@@ -7050,27 +7050,27 @@
     <row r="208" ht="25" customHeight="1">
       <c r="A208" s="3" t="inlineStr">
         <is>
-          <t>Williams</t>
+          <t>Watson</t>
         </is>
       </c>
       <c r="B208" s="3" t="inlineStr">
         <is>
-          <t>Johanna</t>
+          <t>Alison</t>
         </is>
       </c>
       <c r="C208" s="3" t="inlineStr">
         <is>
-          <t>Mitchells Plain</t>
+          <t>Sedgefield</t>
         </is>
       </c>
       <c r="D208" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E208" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F208" s="3" t="inlineStr">
@@ -7082,22 +7082,22 @@
     <row r="209" ht="25" customHeight="1">
       <c r="A209" s="3" t="inlineStr">
         <is>
-          <t>Wills</t>
+          <t>Williams</t>
         </is>
       </c>
       <c r="B209" s="3" t="inlineStr">
         <is>
-          <t>Geila</t>
+          <t>Johanna</t>
         </is>
       </c>
       <c r="C209" s="3" t="inlineStr">
         <is>
-          <t>Athlone</t>
+          <t>Mitchells Plain</t>
         </is>
       </c>
       <c r="D209" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E209" s="3" t="inlineStr">
@@ -7114,17 +7114,17 @@
     <row r="210" ht="25" customHeight="1">
       <c r="A210" s="3" t="inlineStr">
         <is>
-          <t>Wilter-Sturges</t>
+          <t>Wills</t>
         </is>
       </c>
       <c r="B210" s="3" t="inlineStr">
         <is>
-          <t>Meredith</t>
+          <t>Geila</t>
         </is>
       </c>
       <c r="C210" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Athlone</t>
         </is>
       </c>
       <c r="D210" s="3" t="inlineStr">
@@ -7139,24 +7139,24 @@
       </c>
       <c r="F210" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="211" ht="25" customHeight="1">
       <c r="A211" s="3" t="inlineStr">
         <is>
-          <t>Wright</t>
+          <t>Wilter-Sturges</t>
         </is>
       </c>
       <c r="B211" s="3" t="inlineStr">
         <is>
-          <t>Rocky</t>
+          <t>Meredith</t>
         </is>
       </c>
       <c r="C211" s="3" t="inlineStr">
         <is>
-          <t>Table View</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D211" s="3" t="inlineStr">
@@ -7166,29 +7166,29 @@
       </c>
       <c r="E211" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F211" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="212" ht="25" customHeight="1">
       <c r="A212" s="3" t="inlineStr">
         <is>
-          <t>Young</t>
+          <t>Wright</t>
         </is>
       </c>
       <c r="B212" s="3" t="inlineStr">
         <is>
-          <t>Judy</t>
+          <t>Rocky</t>
         </is>
       </c>
       <c r="C212" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>Table View</t>
         </is>
       </c>
       <c r="D212" s="3" t="inlineStr">
@@ -7198,7 +7198,7 @@
       </c>
       <c r="E212" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F212" s="3" t="inlineStr">
@@ -7210,17 +7210,17 @@
     <row r="213" ht="25" customHeight="1">
       <c r="A213" s="3" t="inlineStr">
         <is>
-          <t>de Kock</t>
+          <t>Young</t>
         </is>
       </c>
       <c r="B213" s="3" t="inlineStr">
         <is>
-          <t>Engela</t>
+          <t>Judy</t>
         </is>
       </c>
       <c r="C213" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Durbanville</t>
         </is>
       </c>
       <c r="D213" s="3" t="inlineStr">
@@ -7230,7 +7230,7 @@
       </c>
       <c r="E213" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F213" s="3" t="inlineStr">
@@ -7247,7 +7247,7 @@
       </c>
       <c r="B214" s="3" t="inlineStr">
         <is>
-          <t>Francois</t>
+          <t>Engela</t>
         </is>
       </c>
       <c r="C214" s="3" t="inlineStr">
@@ -7274,54 +7274,54 @@
     <row r="215" ht="25" customHeight="1">
       <c r="A215" s="3" t="inlineStr">
         <is>
-          <t>de Silva</t>
+          <t>de Kock</t>
         </is>
       </c>
       <c r="B215" s="3" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Francois</t>
         </is>
       </c>
       <c r="C215" s="3" t="inlineStr">
         <is>
-          <t>Edenvale</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D215" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E215" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F215" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="216" ht="25" customHeight="1">
       <c r="A216" s="3" t="inlineStr">
         <is>
-          <t>du Toit</t>
+          <t>de Silva</t>
         </is>
       </c>
       <c r="B216" s="3" t="inlineStr">
         <is>
-          <t>Desiree</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="C216" s="3" t="inlineStr">
         <is>
-          <t>Ramsgate</t>
+          <t>Edenvale</t>
         </is>
       </c>
       <c r="D216" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E216" s="3" t="inlineStr">
@@ -7338,59 +7338,59 @@
     <row r="217" ht="25" customHeight="1">
       <c r="A217" s="3" t="inlineStr">
         <is>
-          <t>stier</t>
+          <t>du Toit</t>
         </is>
       </c>
       <c r="B217" s="3" t="inlineStr">
         <is>
-          <t>RORY</t>
+          <t>Desiree</t>
         </is>
       </c>
       <c r="C217" s="3" t="inlineStr">
         <is>
-          <t>Deep South</t>
+          <t>Ramsgate</t>
         </is>
       </c>
       <c r="D217" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E217" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F217" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="218" ht="25" customHeight="1">
       <c r="A218" s="3" t="inlineStr">
         <is>
-          <t>van Blerk</t>
+          <t>stier</t>
         </is>
       </c>
       <c r="B218" s="3" t="inlineStr">
         <is>
-          <t>Carl</t>
+          <t>RORY</t>
         </is>
       </c>
       <c r="C218" s="3" t="inlineStr">
         <is>
-          <t>Eden</t>
+          <t>Deep South</t>
         </is>
       </c>
       <c r="D218" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E218" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F218" s="3" t="inlineStr">
@@ -7402,17 +7402,17 @@
     <row r="219" ht="25" customHeight="1">
       <c r="A219" s="3" t="inlineStr">
         <is>
-          <t>van Heerden</t>
+          <t>van Blerk</t>
         </is>
       </c>
       <c r="B219" s="3" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Carl</t>
         </is>
       </c>
       <c r="C219" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Eden</t>
         </is>
       </c>
       <c r="D219" s="3" t="inlineStr">
@@ -7427,7 +7427,7 @@
       </c>
       <c r="F219" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -7439,7 +7439,7 @@
       </c>
       <c r="B220" s="3" t="inlineStr">
         <is>
-          <t>Sandy</t>
+          <t>Sydney</t>
         </is>
       </c>
       <c r="C220" s="3" t="inlineStr">
@@ -7454,7 +7454,7 @@
       </c>
       <c r="E220" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F220" s="3" t="inlineStr">
@@ -7471,12 +7471,12 @@
       </c>
       <c r="B221" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Sandy</t>
         </is>
       </c>
       <c r="C221" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D221" s="3" t="inlineStr">
@@ -7498,17 +7498,17 @@
     <row r="222" ht="25" customHeight="1">
       <c r="A222" s="3" t="inlineStr">
         <is>
-          <t>van Rensburg</t>
+          <t>van Heerden</t>
         </is>
       </c>
       <c r="B222" s="3" t="inlineStr">
         <is>
-          <t>Johan</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C222" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D222" s="3" t="inlineStr">
@@ -7523,7 +7523,7 @@
       </c>
       <c r="F222" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -7535,7 +7535,7 @@
       </c>
       <c r="B223" s="3" t="inlineStr">
         <is>
-          <t>Anne</t>
+          <t>Johan</t>
         </is>
       </c>
       <c r="C223" s="3" t="inlineStr">
@@ -7550,7 +7550,7 @@
       </c>
       <c r="E223" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F223" s="3" t="inlineStr">
@@ -7562,17 +7562,17 @@
     <row r="224" ht="25" customHeight="1">
       <c r="A224" s="3" t="inlineStr">
         <is>
-          <t>van Wulven</t>
+          <t>van Rensburg</t>
         </is>
       </c>
       <c r="B224" s="3" t="inlineStr">
         <is>
-          <t>Jeannie</t>
+          <t>Anne</t>
         </is>
       </c>
       <c r="C224" s="3" t="inlineStr">
         <is>
-          <t>Tygerberg Hills</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D224" s="3" t="inlineStr">
@@ -7582,7 +7582,7 @@
       </c>
       <c r="E224" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F224" s="3" t="inlineStr">
@@ -7599,7 +7599,7 @@
       </c>
       <c r="B225" s="3" t="inlineStr">
         <is>
-          <t>Alan</t>
+          <t>Jeannie</t>
         </is>
       </c>
       <c r="C225" s="3" t="inlineStr">
@@ -7614,7 +7614,7 @@
       </c>
       <c r="E225" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F225" s="3" t="inlineStr">
@@ -7631,7 +7631,7 @@
       </c>
       <c r="B226" s="3" t="inlineStr">
         <is>
-          <t>Deon</t>
+          <t>Alan</t>
         </is>
       </c>
       <c r="C226" s="3" t="inlineStr">
@@ -7658,17 +7658,17 @@
     <row r="227" ht="25" customHeight="1">
       <c r="A227" s="3" t="inlineStr">
         <is>
-          <t>van Wyk</t>
+          <t>van Wulven</t>
         </is>
       </c>
       <c r="B227" s="3" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>Deon</t>
         </is>
       </c>
       <c r="C227" s="3" t="inlineStr">
         <is>
-          <t>North Durban</t>
+          <t>Tygerberg Hills</t>
         </is>
       </c>
       <c r="D227" s="3" t="inlineStr">
@@ -7683,7 +7683,7 @@
       </c>
       <c r="F227" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -7695,12 +7695,12 @@
       </c>
       <c r="B228" s="3" t="inlineStr">
         <is>
-          <t>Lindie</t>
+          <t>Kim</t>
         </is>
       </c>
       <c r="C228" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>North Durban</t>
         </is>
       </c>
       <c r="D228" s="3" t="inlineStr">
@@ -7727,12 +7727,12 @@
       </c>
       <c r="B229" s="3" t="inlineStr">
         <is>
-          <t>Willem</t>
+          <t>Lindie</t>
         </is>
       </c>
       <c r="C229" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D229" s="3" t="inlineStr">
@@ -7759,12 +7759,12 @@
       </c>
       <c r="B230" s="3" t="inlineStr">
         <is>
-          <t>Patricia</t>
+          <t>Willem</t>
         </is>
       </c>
       <c r="C230" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D230" s="3" t="inlineStr">
@@ -7786,27 +7786,27 @@
     <row r="231" ht="25" customHeight="1">
       <c r="A231" s="3" t="inlineStr">
         <is>
-          <t>van der Merwe</t>
+          <t>van Wyk</t>
         </is>
       </c>
       <c r="B231" s="3" t="inlineStr">
         <is>
-          <t>Ingrid</t>
+          <t>Patricia</t>
         </is>
       </c>
       <c r="C231" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D231" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E231" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F231" s="3" t="inlineStr">
@@ -7818,22 +7818,22 @@
     <row r="232" ht="25" customHeight="1">
       <c r="A232" s="3" t="inlineStr">
         <is>
-          <t>van der Westhuizen</t>
+          <t>van der Merwe</t>
         </is>
       </c>
       <c r="B232" s="3" t="inlineStr">
         <is>
-          <t>Hennie</t>
+          <t>Ingrid</t>
         </is>
       </c>
       <c r="C232" s="3" t="inlineStr">
         <is>
-          <t>Helderberg</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D232" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E232" s="3" t="inlineStr">
@@ -7843,24 +7843,24 @@
       </c>
       <c r="F232" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="233" ht="25" customHeight="1">
       <c r="A233" s="3" t="inlineStr">
         <is>
-          <t>von der Decken</t>
+          <t>van der Westhuizen</t>
         </is>
       </c>
       <c r="B233" s="3" t="inlineStr">
         <is>
-          <t>Brian</t>
+          <t>Hennie</t>
         </is>
       </c>
       <c r="C233" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Helderberg</t>
         </is>
       </c>
       <c r="D233" s="3" t="inlineStr">
@@ -7875,51 +7875,83 @@
       </c>
       <c r="F233" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="234" ht="25" customHeight="1">
       <c r="A234" s="3" t="inlineStr">
         <is>
+          <t>von der Decken</t>
+        </is>
+      </c>
+      <c r="B234" s="3" t="inlineStr">
+        <is>
+          <t>Brian</t>
+        </is>
+      </c>
+      <c r="C234" s="3" t="inlineStr">
+        <is>
+          <t>King William's Town</t>
+        </is>
+      </c>
+      <c r="D234" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E234" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F234" s="3" t="inlineStr">
+        <is>
+          <t>410E</t>
+        </is>
+      </c>
+    </row>
+    <row r="235" ht="25" customHeight="1">
+      <c r="A235" s="3" t="inlineStr">
+        <is>
           <t>‘t Hart</t>
         </is>
       </c>
-      <c r="B234" s="3" t="inlineStr">
+      <c r="B235" s="3" t="inlineStr">
         <is>
           <t>Michelle</t>
         </is>
       </c>
-      <c r="C234" s="3" t="inlineStr">
+      <c r="C235" s="3" t="inlineStr">
         <is>
           <t>Benoni Lakes</t>
         </is>
       </c>
-      <c r="D234" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E234" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F234" s="3" t="inlineStr">
+      <c r="D235" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E235" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F235" s="3" t="inlineStr">
         <is>
           <t>410E</t>
-        </is>
-      </c>
-    </row>
-    <row r="235">
-      <c r="A235" s="1" t="inlineStr">
-        <is>
-          <t>Number of attendees: 232</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="inlineStr">
+        <is>
+          <t>Number of attendees: 233</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" s="1" t="inlineStr">
         <is>
           <t>Number of voters: 109</t>
         </is>
@@ -7955,7 +7987,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Registrees as of 19/04/2021 10:15</t>
+          <t>410E Registrees as of 20/04/2021 08:45</t>
         </is>
       </c>
     </row>
@@ -11351,7 +11383,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Registrees as of 19/04/2021 10:15</t>
+          <t>410W Registrees as of 20/04/2021 08:45</t>
         </is>
       </c>
     </row>
@@ -15392,7 +15424,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Voting details as of 19/04/2021 10:15</t>
+          <t>410E Voting details as of 20/04/2021 08:45</t>
         </is>
       </c>
     </row>
@@ -15729,7 +15761,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Voting details as of 19/04/2021 10:15</t>
+          <t>410W Voting details as of 20/04/2021 08:45</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Registree stats backup on Tue 20 Apr 2021 11:11:12 SAST
</commit_message>
<xml_diff>
--- a/static/docs/registrees_list.xlsx
+++ b/static/docs/registrees_list.xlsx
@@ -451,7 +451,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>MD410 Registrees as of 20/04/2021 08:45</t>
+          <t>MD410 Registrees as of 20/04/2021 11:11</t>
         </is>
       </c>
     </row>
@@ -7987,7 +7987,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Registrees as of 20/04/2021 08:45</t>
+          <t>410E Registrees as of 20/04/2021 11:11</t>
         </is>
       </c>
     </row>
@@ -11383,7 +11383,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Registrees as of 20/04/2021 08:45</t>
+          <t>410W Registrees as of 20/04/2021 11:11</t>
         </is>
       </c>
     </row>
@@ -15424,7 +15424,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Voting details as of 20/04/2021 08:45</t>
+          <t>410E Voting details as of 20/04/2021 11:11</t>
         </is>
       </c>
     </row>
@@ -15761,7 +15761,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Voting details as of 20/04/2021 08:45</t>
+          <t>410W Voting details as of 20/04/2021 11:11</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Registree stats backup on Tue 20 Apr 2021 11:25:46 SAST
</commit_message>
<xml_diff>
--- a/static/docs/registrees_list.xlsx
+++ b/static/docs/registrees_list.xlsx
@@ -451,7 +451,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>MD410 Registrees as of 20/04/2021 11:11</t>
+          <t>MD410 Registrees as of 20/04/2021 11:25</t>
         </is>
       </c>
     </row>
@@ -766,7 +766,7 @@
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F11" s="3" t="inlineStr">
@@ -1758,7 +1758,7 @@
       </c>
       <c r="E42" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F42" s="3" t="inlineStr">
@@ -3102,7 +3102,7 @@
       </c>
       <c r="E84" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F84" s="3" t="inlineStr">
@@ -3198,7 +3198,7 @@
       </c>
       <c r="E87" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F87" s="3" t="inlineStr">
@@ -4606,7 +4606,7 @@
       </c>
       <c r="E131" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F131" s="3" t="inlineStr">
@@ -4766,7 +4766,7 @@
       </c>
       <c r="E136" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F136" s="3" t="inlineStr">
@@ -5694,7 +5694,7 @@
       </c>
       <c r="E165" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F165" s="3" t="inlineStr">
@@ -5918,7 +5918,7 @@
       </c>
       <c r="E172" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F172" s="3" t="inlineStr">
@@ -5950,7 +5950,7 @@
       </c>
       <c r="E173" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F173" s="3" t="inlineStr">
@@ -7550,7 +7550,7 @@
       </c>
       <c r="E223" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F223" s="3" t="inlineStr">
@@ -7614,7 +7614,7 @@
       </c>
       <c r="E225" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F225" s="3" t="inlineStr">
@@ -7953,7 +7953,7 @@
     <row r="237">
       <c r="A237" s="1" t="inlineStr">
         <is>
-          <t>Number of voters: 109</t>
+          <t>Number of voters: 102</t>
         </is>
       </c>
     </row>
@@ -7987,7 +7987,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Registrees as of 20/04/2021 11:11</t>
+          <t>410E Registrees as of 20/04/2021 11:25</t>
         </is>
       </c>
     </row>
@@ -11383,7 +11383,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Registrees as of 20/04/2021 11:11</t>
+          <t>410W Registrees as of 20/04/2021 11:25</t>
         </is>
       </c>
     </row>
@@ -11680,7 +11680,7 @@
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -11707,7 +11707,7 @@
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -12166,7 +12166,7 @@
       </c>
       <c r="E30" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -12247,7 +12247,7 @@
       </c>
       <c r="E33" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -12409,7 +12409,7 @@
       </c>
       <c r="E39" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -12544,7 +12544,7 @@
       </c>
       <c r="E44" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -12895,7 +12895,7 @@
       </c>
       <c r="E57" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -12976,7 +12976,7 @@
       </c>
       <c r="E60" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -13030,7 +13030,7 @@
       </c>
       <c r="E62" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -13138,7 +13138,7 @@
       </c>
       <c r="E66" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -13624,7 +13624,7 @@
       </c>
       <c r="E84" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -13759,7 +13759,7 @@
       </c>
       <c r="E89" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -13948,7 +13948,7 @@
       </c>
       <c r="E96" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -13975,7 +13975,7 @@
       </c>
       <c r="E97" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -14326,7 +14326,7 @@
       </c>
       <c r="E110" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -14461,7 +14461,7 @@
       </c>
       <c r="E115" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -15109,7 +15109,7 @@
       </c>
       <c r="E139" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -15244,7 +15244,7 @@
       </c>
       <c r="E144" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -15298,7 +15298,7 @@
       </c>
       <c r="E146" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -15393,7 +15393,7 @@
     <row r="151">
       <c r="A151" s="1" t="inlineStr">
         <is>
-          <t>Number of voters: 67</t>
+          <t>Number of voters: 54</t>
         </is>
       </c>
     </row>
@@ -15424,7 +15424,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Voting details as of 20/04/2021 11:11</t>
+          <t>410E Voting details as of 20/04/2021 11:25</t>
         </is>
       </c>
     </row>
@@ -15761,7 +15761,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Voting details as of 20/04/2021 11:11</t>
+          <t>410W Voting details as of 20/04/2021 11:25</t>
         </is>
       </c>
     </row>
@@ -15834,7 +15834,7 @@
         </is>
       </c>
       <c r="B8" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" ht="25" customHeight="1">
@@ -15930,7 +15930,7 @@
     <row r="18" ht="25" customHeight="1">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>Kuilsriver</t>
+          <t>Malgas</t>
         </is>
       </c>
       <c r="B18" s="3" t="n">
@@ -15940,7 +15940,7 @@
     <row r="19" ht="25" customHeight="1">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>Malgas</t>
+          <t>Malmesbury</t>
         </is>
       </c>
       <c r="B19" s="3" t="n">
@@ -15950,37 +15950,37 @@
     <row r="20" ht="25" customHeight="1">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>Malmesbury</t>
+          <t>Merriman</t>
         </is>
       </c>
       <c r="B20" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" ht="25" customHeight="1">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>Merriman</t>
+          <t>Milnerton</t>
         </is>
       </c>
       <c r="B21" s="3" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" ht="25" customHeight="1">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>Milnerton</t>
+          <t>Mitchells Plain</t>
         </is>
       </c>
       <c r="B22" s="3" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" ht="25" customHeight="1">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>Mitchells Plain</t>
+          <t>Moorreesburg</t>
         </is>
       </c>
       <c r="B23" s="3" t="n">
@@ -15990,7 +15990,7 @@
     <row r="24" ht="25" customHeight="1">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>Moorreesburg</t>
+          <t>Newlands</t>
         </is>
       </c>
       <c r="B24" s="3" t="n">
@@ -16000,17 +16000,17 @@
     <row r="25" ht="25" customHeight="1">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>Newlands</t>
+          <t>Rehoboth</t>
         </is>
       </c>
       <c r="B25" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" ht="25" customHeight="1">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>Rehoboth</t>
+          <t>Sea Point</t>
         </is>
       </c>
       <c r="B26" s="3" t="n">
@@ -16020,37 +16020,37 @@
     <row r="27" ht="25" customHeight="1">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>Sea Point</t>
+          <t>Sedgefield</t>
         </is>
       </c>
       <c r="B27" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" ht="25" customHeight="1">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>Sedgefield</t>
+          <t>Stellenbosch</t>
         </is>
       </c>
       <c r="B28" s="3" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" ht="25" customHeight="1">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>Stellenbosch</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="B29" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" ht="25" customHeight="1">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Table View</t>
         </is>
       </c>
       <c r="B30" s="3" t="n">
@@ -16060,7 +16060,7 @@
     <row r="31" ht="25" customHeight="1">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>Table View</t>
+          <t>Tokai</t>
         </is>
       </c>
       <c r="B31" s="3" t="n">
@@ -16070,11 +16070,11 @@
     <row r="32" ht="25" customHeight="1">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>Tokai</t>
+          <t>Tsumeb</t>
         </is>
       </c>
       <c r="B32" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" ht="25" customHeight="1">
@@ -16084,7 +16084,7 @@
         </is>
       </c>
       <c r="B33" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" ht="25" customHeight="1">
@@ -16094,7 +16094,7 @@
         </is>
       </c>
       <c r="B34" s="3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" ht="25" customHeight="1">
@@ -16104,7 +16104,7 @@
         </is>
       </c>
       <c r="B35" s="3" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" ht="25" customHeight="1">
@@ -16114,7 +16114,7 @@
         </is>
       </c>
       <c r="B36" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37">
@@ -16127,7 +16127,7 @@
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>Number of voters: 70</t>
+          <t>Number of voters: 55</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Registree stats backup on Tue 20 Apr 2021 15:16:31 SAST
</commit_message>
<xml_diff>
--- a/static/docs/registrees_list.xlsx
+++ b/static/docs/registrees_list.xlsx
@@ -451,7 +451,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>MD410 Registrees as of 20/04/2021 11:25</t>
+          <t>MD410 Registrees as of 20/04/2021 15:16</t>
         </is>
       </c>
     </row>
@@ -7969,7 +7969,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E127"/>
+  <dimension ref="A1:E126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7987,7 +7987,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Registrees as of 20/04/2021 11:25</t>
+          <t>410E Registrees as of 20/04/2021 15:16</t>
         </is>
       </c>
     </row>
@@ -10910,54 +10910,54 @@
     <row r="110" ht="25" customHeight="1">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>Zucker</t>
+          <t>de Silva</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
         <is>
-          <t>Leonie</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="C110" s="3" t="inlineStr">
         <is>
-          <t>Milnerton</t>
+          <t>Edenvale</t>
         </is>
       </c>
       <c r="D110" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E110" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="111" ht="25" customHeight="1">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>de Silva</t>
+          <t>du Plooy</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Tammy</t>
         </is>
       </c>
       <c r="C111" s="3" t="inlineStr">
         <is>
-          <t>Edenvale</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D111" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E111" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -10969,7 +10969,7 @@
       </c>
       <c r="B112" s="3" t="inlineStr">
         <is>
-          <t>Tammy</t>
+          <t>Marc</t>
         </is>
       </c>
       <c r="C112" s="3" t="inlineStr">
@@ -10991,17 +10991,17 @@
     <row r="113" ht="25" customHeight="1">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>du Plooy</t>
+          <t>du Toit</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
         <is>
-          <t>Marc</t>
+          <t>Desiree</t>
         </is>
       </c>
       <c r="C113" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Ramsgate</t>
         </is>
       </c>
       <c r="D113" s="3" t="inlineStr">
@@ -11011,24 +11011,24 @@
       </c>
       <c r="E113" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="114" ht="25" customHeight="1">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>du Toit</t>
+          <t>le Roux</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
         <is>
-          <t>Desiree</t>
+          <t>Jeanette</t>
         </is>
       </c>
       <c r="C114" s="3" t="inlineStr">
         <is>
-          <t>Ramsgate</t>
+          <t>Gonubie</t>
         </is>
       </c>
       <c r="D114" s="3" t="inlineStr">
@@ -11045,17 +11045,17 @@
     <row r="115" ht="25" customHeight="1">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>le Roux</t>
+          <t>van Heerden</t>
         </is>
       </c>
       <c r="B115" s="3" t="inlineStr">
         <is>
-          <t>Jeanette</t>
+          <t>Sydney</t>
         </is>
       </c>
       <c r="C115" s="3" t="inlineStr">
         <is>
-          <t>Gonubie</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D115" s="3" t="inlineStr">
@@ -11077,7 +11077,7 @@
       </c>
       <c r="B116" s="3" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Sandy</t>
         </is>
       </c>
       <c r="C116" s="3" t="inlineStr">
@@ -11092,7 +11092,7 @@
       </c>
       <c r="E116" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -11104,12 +11104,12 @@
       </c>
       <c r="B117" s="3" t="inlineStr">
         <is>
-          <t>Sandy</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C117" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D117" s="3" t="inlineStr">
@@ -11126,17 +11126,17 @@
     <row r="118" ht="25" customHeight="1">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>van Heerden</t>
+          <t>van Wyk</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Kim</t>
         </is>
       </c>
       <c r="C118" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>North Durban</t>
         </is>
       </c>
       <c r="D118" s="3" t="inlineStr">
@@ -11146,7 +11146,7 @@
       </c>
       <c r="E118" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -11158,12 +11158,12 @@
       </c>
       <c r="B119" s="3" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>Lindie</t>
         </is>
       </c>
       <c r="C119" s="3" t="inlineStr">
         <is>
-          <t>North Durban</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D119" s="3" t="inlineStr">
@@ -11185,12 +11185,12 @@
       </c>
       <c r="B120" s="3" t="inlineStr">
         <is>
-          <t>Lindie</t>
+          <t>Willem</t>
         </is>
       </c>
       <c r="C120" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D120" s="3" t="inlineStr">
@@ -11212,12 +11212,12 @@
       </c>
       <c r="B121" s="3" t="inlineStr">
         <is>
-          <t>Willem</t>
+          <t>Patricia</t>
         </is>
       </c>
       <c r="C121" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D121" s="3" t="inlineStr">
@@ -11234,49 +11234,49 @@
     <row r="122" ht="25" customHeight="1">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>van Wyk</t>
+          <t>van der Merwe</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
         <is>
-          <t>Patricia</t>
+          <t>Ingrid</t>
         </is>
       </c>
       <c r="C122" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D122" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E122" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="123" ht="25" customHeight="1">
       <c r="A123" s="3" t="inlineStr">
         <is>
-          <t>van der Merwe</t>
+          <t>von der Decken</t>
         </is>
       </c>
       <c r="B123" s="3" t="inlineStr">
         <is>
-          <t>Ingrid</t>
+          <t>Brian</t>
         </is>
       </c>
       <c r="C123" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>King William's Town</t>
         </is>
       </c>
       <c r="D123" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E123" s="3" t="inlineStr">
@@ -11288,17 +11288,17 @@
     <row r="124" ht="25" customHeight="1">
       <c r="A124" s="3" t="inlineStr">
         <is>
-          <t>von der Decken</t>
+          <t>‘t Hart</t>
         </is>
       </c>
       <c r="B124" s="3" t="inlineStr">
         <is>
-          <t>Brian</t>
+          <t>Michelle</t>
         </is>
       </c>
       <c r="C124" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Benoni Lakes</t>
         </is>
       </c>
       <c r="D124" s="3" t="inlineStr">
@@ -11308,48 +11308,21 @@
       </c>
       <c r="E124" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
-        </is>
-      </c>
-    </row>
-    <row r="125" ht="25" customHeight="1">
-      <c r="A125" s="3" t="inlineStr">
-        <is>
-          <t>‘t Hart</t>
-        </is>
-      </c>
-      <c r="B125" s="3" t="inlineStr">
-        <is>
-          <t>Michelle</t>
-        </is>
-      </c>
-      <c r="C125" s="3" t="inlineStr">
-        <is>
-          <t>Benoni Lakes</t>
-        </is>
-      </c>
-      <c r="D125" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E125" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="1" t="inlineStr">
+        <is>
+          <t>Number of attendees: 122</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="inlineStr">
         <is>
-          <t>Number of attendees: 123</t>
-        </is>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" s="1" t="inlineStr">
-        <is>
-          <t>Number of voters: 60</t>
+          <t>Number of voters: 59</t>
         </is>
       </c>
     </row>
@@ -11365,7 +11338,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E151"/>
+  <dimension ref="A1:E152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11383,7 +11356,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Registrees as of 20/04/2021 11:25</t>
+          <t>410W Registrees as of 20/04/2021 15:16</t>
         </is>
       </c>
     </row>
@@ -12335,17 +12308,17 @@
     <row r="37" ht="25" customHeight="1">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>Fourie</t>
+          <t>Fouché</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
         <is>
-          <t>Michele</t>
+          <t>Jéan</t>
         </is>
       </c>
       <c r="C37" s="3" t="inlineStr">
         <is>
-          <t>Merriman</t>
+          <t>Worcester</t>
         </is>
       </c>
       <c r="D37" s="3" t="inlineStr">
@@ -12355,19 +12328,19 @@
       </c>
       <c r="E37" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="38" ht="25" customHeight="1">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>Fox</t>
+          <t>Fourie</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
         <is>
-          <t>Clive</t>
+          <t>Michele</t>
         </is>
       </c>
       <c r="C38" s="3" t="inlineStr">
@@ -12382,7 +12355,7 @@
       </c>
       <c r="E38" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -12394,7 +12367,7 @@
       </c>
       <c r="B39" s="3" t="inlineStr">
         <is>
-          <t>Pat</t>
+          <t>Clive</t>
         </is>
       </c>
       <c r="C39" s="3" t="inlineStr">
@@ -12409,24 +12382,24 @@
       </c>
       <c r="E39" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="40" ht="25" customHeight="1">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>Georges</t>
+          <t>Fox</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
         <is>
-          <t>Allison</t>
+          <t>Pat</t>
         </is>
       </c>
       <c r="C40" s="3" t="inlineStr">
         <is>
-          <t>Cape Of Good Hope</t>
+          <t>Merriman</t>
         </is>
       </c>
       <c r="D40" s="3" t="inlineStr">
@@ -12443,17 +12416,17 @@
     <row r="41" ht="25" customHeight="1">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>Grater</t>
+          <t>Georges</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
         <is>
-          <t>Viv</t>
+          <t>Allison</t>
         </is>
       </c>
       <c r="C41" s="3" t="inlineStr">
         <is>
-          <t>Sedgefield</t>
+          <t>Cape Of Good Hope</t>
         </is>
       </c>
       <c r="D41" s="3" t="inlineStr">
@@ -12463,110 +12436,110 @@
       </c>
       <c r="E41" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="42" ht="25" customHeight="1">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>Gray</t>
+          <t>Grater</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
         <is>
-          <t>Brian</t>
+          <t>Viv</t>
         </is>
       </c>
       <c r="C42" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>Sedgefield</t>
         </is>
       </c>
       <c r="D42" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E42" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="43" ht="25" customHeight="1">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>Grobler</t>
+          <t>Gray</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
         <is>
-          <t>Matty</t>
+          <t>Brian</t>
         </is>
       </c>
       <c r="C43" s="3" t="inlineStr">
         <is>
-          <t>Henties Bay</t>
+          <t>Durbanville</t>
         </is>
       </c>
       <c r="D43" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E43" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="44" ht="25" customHeight="1">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>Groenewoud</t>
+          <t>Grobler</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
         <is>
-          <t>Christiana</t>
+          <t>Matty</t>
         </is>
       </c>
       <c r="C44" s="3" t="inlineStr">
         <is>
-          <t>Milnerton</t>
+          <t>Henties Bay</t>
         </is>
       </c>
       <c r="D44" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E44" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="45" ht="25" customHeight="1">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>Groves</t>
+          <t>Groenewoud</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
         <is>
-          <t>Mattheus</t>
+          <t>Christiana</t>
         </is>
       </c>
       <c r="C45" s="3" t="inlineStr">
         <is>
-          <t>Sedgefield</t>
+          <t>Milnerton</t>
         </is>
       </c>
       <c r="D45" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E45" s="3" t="inlineStr">
@@ -12578,22 +12551,22 @@
     <row r="46" ht="25" customHeight="1">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>Gunter</t>
+          <t>Groves</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
         <is>
-          <t>Glyn</t>
+          <t>Mattheus</t>
         </is>
       </c>
       <c r="C46" s="3" t="inlineStr">
         <is>
-          <t>Malmesbury</t>
+          <t>Sedgefield</t>
         </is>
       </c>
       <c r="D46" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E46" s="3" t="inlineStr">
@@ -12605,22 +12578,22 @@
     <row r="47" ht="25" customHeight="1">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>Haywood</t>
+          <t>Gunter</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
         <is>
-          <t>Barbara</t>
+          <t>Glyn</t>
         </is>
       </c>
       <c r="C47" s="3" t="inlineStr">
         <is>
-          <t>Eden</t>
+          <t>Malmesbury</t>
         </is>
       </c>
       <c r="D47" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E47" s="3" t="inlineStr">
@@ -12632,17 +12605,17 @@
     <row r="48" ht="25" customHeight="1">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>Hendricks</t>
+          <t>Haywood</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
         <is>
-          <t>Zarina</t>
+          <t>Barbara</t>
         </is>
       </c>
       <c r="C48" s="3" t="inlineStr">
         <is>
-          <t>Athlone</t>
+          <t>Eden</t>
         </is>
       </c>
       <c r="D48" s="3" t="inlineStr">
@@ -12652,51 +12625,51 @@
       </c>
       <c r="E48" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="49" ht="25" customHeight="1">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>Hendriks</t>
+          <t>Hendricks</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
         <is>
-          <t>ELIZABETH</t>
+          <t>Zarina</t>
         </is>
       </c>
       <c r="C49" s="3" t="inlineStr">
         <is>
-          <t>Table View</t>
+          <t>Athlone</t>
         </is>
       </c>
       <c r="D49" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E49" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="50" ht="25" customHeight="1">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>Hess</t>
+          <t>Hendriks</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
         <is>
-          <t>Dorothy</t>
+          <t>ELIZABETH</t>
         </is>
       </c>
       <c r="C50" s="3" t="inlineStr">
         <is>
-          <t>Kuilsriver</t>
+          <t>Table View</t>
         </is>
       </c>
       <c r="D50" s="3" t="inlineStr">
@@ -12713,22 +12686,22 @@
     <row r="51" ht="25" customHeight="1">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>Hoffmann</t>
+          <t>Hess</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
         <is>
-          <t>Ellen G W</t>
+          <t>Dorothy</t>
         </is>
       </c>
       <c r="C51" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Kuilsriver</t>
         </is>
       </c>
       <c r="D51" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E51" s="3" t="inlineStr">
@@ -12740,17 +12713,17 @@
     <row r="52" ht="25" customHeight="1">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Hoffmann</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
         <is>
-          <t>Liz</t>
+          <t>Ellen G W</t>
         </is>
       </c>
       <c r="C52" s="3" t="inlineStr">
         <is>
-          <t>Table View</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D52" s="3" t="inlineStr">
@@ -12760,7 +12733,7 @@
       </c>
       <c r="E52" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -12772,7 +12745,7 @@
       </c>
       <c r="B53" s="3" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>Liz</t>
         </is>
       </c>
       <c r="C53" s="3" t="inlineStr">
@@ -12787,34 +12760,34 @@
       </c>
       <c r="E53" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="54" ht="25" customHeight="1">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>Jacobs</t>
+          <t>Houston</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
         <is>
-          <t>Dawid</t>
+          <t>John</t>
         </is>
       </c>
       <c r="C54" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>Table View</t>
         </is>
       </c>
       <c r="D54" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E54" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -12826,39 +12799,39 @@
       </c>
       <c r="B55" s="3" t="inlineStr">
         <is>
-          <t>Jean</t>
+          <t>Dawid</t>
         </is>
       </c>
       <c r="C55" s="3" t="inlineStr">
         <is>
-          <t>Mitchells Plain</t>
+          <t>Durbanville</t>
         </is>
       </c>
       <c r="D55" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E55" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="56" ht="25" customHeight="1">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>Jacobson</t>
+          <t>Jacobs</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
         <is>
-          <t>WOLSLEY</t>
+          <t>Jean</t>
         </is>
       </c>
       <c r="C56" s="3" t="inlineStr">
         <is>
-          <t>Cape Town</t>
+          <t>Mitchells Plain</t>
         </is>
       </c>
       <c r="D56" s="3" t="inlineStr">
@@ -12868,51 +12841,51 @@
       </c>
       <c r="E56" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="57" ht="25" customHeight="1">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>Jeniker</t>
+          <t>Jacobson</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
         <is>
-          <t>Tristan</t>
+          <t>WOLSLEY</t>
         </is>
       </c>
       <c r="C57" s="3" t="inlineStr">
         <is>
-          <t>Merriman</t>
+          <t>Cape Town</t>
         </is>
       </c>
       <c r="D57" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E57" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="58" ht="25" customHeight="1">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>Jonathan</t>
+          <t>Jeniker</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
         <is>
-          <t>Grant</t>
+          <t>Tristan</t>
         </is>
       </c>
       <c r="C58" s="3" t="inlineStr">
         <is>
-          <t>Gordons Bay</t>
+          <t>Merriman</t>
         </is>
       </c>
       <c r="D58" s="3" t="inlineStr">
@@ -12922,83 +12895,83 @@
       </c>
       <c r="E58" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="59" ht="25" customHeight="1">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>Kahn</t>
+          <t>Jonathan</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
         <is>
-          <t>Michelle</t>
+          <t>Grant</t>
         </is>
       </c>
       <c r="C59" s="3" t="inlineStr">
         <is>
-          <t>Sea Point</t>
+          <t>Gordons Bay</t>
         </is>
       </c>
       <c r="D59" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E59" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="60" ht="25" customHeight="1">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>Kaiyamo</t>
+          <t>Kahn</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
         <is>
-          <t>Nico</t>
+          <t>Michelle</t>
         </is>
       </c>
       <c r="C60" s="3" t="inlineStr">
         <is>
-          <t>Tsumeb</t>
+          <t>Sea Point</t>
         </is>
       </c>
       <c r="D60" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E60" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="61" ht="25" customHeight="1">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>Karriem</t>
+          <t>Kaiyamo</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
         <is>
-          <t>Faezal</t>
+          <t>Nico</t>
         </is>
       </c>
       <c r="C61" s="3" t="inlineStr">
         <is>
-          <t>Worcester</t>
+          <t>Tsumeb</t>
         </is>
       </c>
       <c r="D61" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E61" s="3" t="inlineStr">
@@ -13010,49 +12983,49 @@
     <row r="62" ht="25" customHeight="1">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>Kemp</t>
+          <t>Karriem</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
         <is>
-          <t>Amanda</t>
+          <t>Faezal</t>
         </is>
       </c>
       <c r="C62" s="3" t="inlineStr">
         <is>
-          <t>Milnerton</t>
+          <t>Worcester</t>
         </is>
       </c>
       <c r="D62" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E62" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="63" ht="25" customHeight="1">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>Kennel</t>
+          <t>Kemp</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
         <is>
-          <t>Esmeralda Catherine</t>
+          <t>Amanda</t>
         </is>
       </c>
       <c r="C63" s="3" t="inlineStr">
         <is>
-          <t>Newlands</t>
+          <t>Milnerton</t>
         </is>
       </c>
       <c r="D63" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E63" s="3" t="inlineStr">
@@ -13064,17 +13037,17 @@
     <row r="64" ht="25" customHeight="1">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>Kern</t>
+          <t>Kennel</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
         <is>
-          <t>Jerome</t>
+          <t>Esmeralda Catherine</t>
         </is>
       </c>
       <c r="C64" s="3" t="inlineStr">
         <is>
-          <t>Groote Schuur</t>
+          <t>Newlands</t>
         </is>
       </c>
       <c r="D64" s="3" t="inlineStr">
@@ -13091,22 +13064,22 @@
     <row r="65" ht="25" customHeight="1">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>Khan</t>
+          <t>Kern</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
         <is>
-          <t>Hassan</t>
+          <t>Jerome</t>
         </is>
       </c>
       <c r="C65" s="3" t="inlineStr">
         <is>
-          <t>Kirstenbosch</t>
+          <t>Groote Schuur</t>
         </is>
       </c>
       <c r="D65" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E65" s="3" t="inlineStr">
@@ -13118,17 +13091,17 @@
     <row r="66" ht="25" customHeight="1">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>Koenze</t>
+          <t>Khan</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
         <is>
-          <t>Alton</t>
+          <t>Hassan</t>
         </is>
       </c>
       <c r="C66" s="3" t="inlineStr">
         <is>
-          <t>Worcester</t>
+          <t>Kirstenbosch</t>
         </is>
       </c>
       <c r="D66" s="3" t="inlineStr">
@@ -13145,17 +13118,17 @@
     <row r="67" ht="25" customHeight="1">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>Koloko</t>
+          <t>Koenze</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
         <is>
-          <t>Muya</t>
+          <t>Alton</t>
         </is>
       </c>
       <c r="C67" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>Worcester</t>
         </is>
       </c>
       <c r="D67" s="3" t="inlineStr">
@@ -13172,44 +13145,44 @@
     <row r="68" ht="25" customHeight="1">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>Kruger</t>
+          <t>Koloko</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
         <is>
-          <t>Zwaai</t>
+          <t>Muya</t>
         </is>
       </c>
       <c r="C68" s="3" t="inlineStr">
         <is>
-          <t>Sedgefield</t>
+          <t>Durbanville</t>
         </is>
       </c>
       <c r="D68" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E68" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="69" ht="25" customHeight="1">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>Lakay</t>
+          <t>Kruger</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
         <is>
-          <t>Bevil</t>
+          <t>Zwaai</t>
         </is>
       </c>
       <c r="C69" s="3" t="inlineStr">
         <is>
-          <t>Mitchells Plain</t>
+          <t>Sedgefield</t>
         </is>
       </c>
       <c r="D69" s="3" t="inlineStr">
@@ -13226,17 +13199,17 @@
     <row r="70" ht="25" customHeight="1">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>Lang</t>
+          <t>Lakay</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
         <is>
-          <t>Paula</t>
+          <t>Bevil</t>
         </is>
       </c>
       <c r="C70" s="3" t="inlineStr">
         <is>
-          <t>Gordons Bay</t>
+          <t>Mitchells Plain</t>
         </is>
       </c>
       <c r="D70" s="3" t="inlineStr">
@@ -13258,7 +13231,7 @@
       </c>
       <c r="B71" s="3" t="inlineStr">
         <is>
-          <t>Jimmy</t>
+          <t>Paula</t>
         </is>
       </c>
       <c r="C71" s="3" t="inlineStr">
@@ -13273,29 +13246,29 @@
       </c>
       <c r="E71" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="72" ht="25" customHeight="1">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>Langmaak</t>
+          <t>Lang</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
         <is>
-          <t>Elke</t>
+          <t>Jimmy</t>
         </is>
       </c>
       <c r="C72" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Gordons Bay</t>
         </is>
       </c>
       <c r="D72" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E72" s="3" t="inlineStr">
@@ -13312,7 +13285,7 @@
       </c>
       <c r="B73" s="3" t="inlineStr">
         <is>
-          <t>Kai</t>
+          <t>Elke</t>
         </is>
       </c>
       <c r="C73" s="3" t="inlineStr">
@@ -13334,22 +13307,22 @@
     <row r="74" ht="25" customHeight="1">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>Laubscher</t>
+          <t>Langmaak</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
         <is>
-          <t>Herman</t>
+          <t>Kai</t>
         </is>
       </c>
       <c r="C74" s="3" t="inlineStr">
         <is>
-          <t>Ceres</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D74" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E74" s="3" t="inlineStr">
@@ -13361,17 +13334,17 @@
     <row r="75" ht="25" customHeight="1">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>Lee</t>
+          <t>Laubscher</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
         <is>
-          <t>Heather</t>
+          <t>Herman</t>
         </is>
       </c>
       <c r="C75" s="3" t="inlineStr">
         <is>
-          <t>Cape Of Good Hope</t>
+          <t>Ceres</t>
         </is>
       </c>
       <c r="D75" s="3" t="inlineStr">
@@ -13381,24 +13354,24 @@
       </c>
       <c r="E75" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="76" ht="25" customHeight="1">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>Lucas</t>
+          <t>Lee</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
         <is>
-          <t>Rashmiya</t>
+          <t>Heather</t>
         </is>
       </c>
       <c r="C76" s="3" t="inlineStr">
         <is>
-          <t>Mitchells Plain</t>
+          <t>Cape Of Good Hope</t>
         </is>
       </c>
       <c r="D76" s="3" t="inlineStr">
@@ -13408,24 +13381,24 @@
       </c>
       <c r="E76" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="77" ht="25" customHeight="1">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>MAYTHAM</t>
+          <t>Lucas</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
         <is>
-          <t>LANCE</t>
+          <t>Rashmiya</t>
         </is>
       </c>
       <c r="C77" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Mitchells Plain</t>
         </is>
       </c>
       <c r="D77" s="3" t="inlineStr">
@@ -13447,7 +13420,7 @@
       </c>
       <c r="B78" s="3" t="inlineStr">
         <is>
-          <t>ROSEMARIE</t>
+          <t>LANCE</t>
         </is>
       </c>
       <c r="C78" s="3" t="inlineStr">
@@ -13469,17 +13442,17 @@
     <row r="79" ht="25" customHeight="1">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>MacRobert</t>
+          <t>MAYTHAM</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
         <is>
-          <t>Pam</t>
+          <t>ROSEMARIE</t>
         </is>
       </c>
       <c r="C79" s="3" t="inlineStr">
         <is>
-          <t>Groote Schuur</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D79" s="3" t="inlineStr">
@@ -13496,49 +13469,49 @@
     <row r="80" ht="25" customHeight="1">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>Mangwende</t>
+          <t>MacRobert</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
         <is>
-          <t>Sharon</t>
+          <t>Pam</t>
         </is>
       </c>
       <c r="C80" s="3" t="inlineStr">
         <is>
-          <t>Cape Town</t>
+          <t>Groote Schuur</t>
         </is>
       </c>
       <c r="D80" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E80" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="81" ht="25" customHeight="1">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>McPherson</t>
+          <t>Mangwende</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
         <is>
-          <t>Stuart</t>
+          <t>Sharon</t>
         </is>
       </c>
       <c r="C81" s="3" t="inlineStr">
         <is>
-          <t>Newlands</t>
+          <t>Cape Town</t>
         </is>
       </c>
       <c r="D81" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E81" s="3" t="inlineStr">
@@ -13550,17 +13523,17 @@
     <row r="82" ht="25" customHeight="1">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>Metz</t>
+          <t>McPherson</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
         <is>
-          <t>Elisa</t>
+          <t>Stuart</t>
         </is>
       </c>
       <c r="C82" s="3" t="inlineStr">
         <is>
-          <t>Milnerton</t>
+          <t>Newlands</t>
         </is>
       </c>
       <c r="D82" s="3" t="inlineStr">
@@ -13570,24 +13543,24 @@
       </c>
       <c r="E82" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="83" ht="25" customHeight="1">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>Mkhize</t>
+          <t>Metz</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
         <is>
-          <t>Virginia</t>
+          <t>Elisa</t>
         </is>
       </c>
       <c r="C83" s="3" t="inlineStr">
         <is>
-          <t>Cape Town</t>
+          <t>Milnerton</t>
         </is>
       </c>
       <c r="D83" s="3" t="inlineStr">
@@ -13604,22 +13577,22 @@
     <row r="84" ht="25" customHeight="1">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>Moeller</t>
+          <t>Mkhize</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
         <is>
-          <t>Frauke E.</t>
+          <t>Virginia</t>
         </is>
       </c>
       <c r="C84" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Cape Town</t>
         </is>
       </c>
       <c r="D84" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E84" s="3" t="inlineStr">
@@ -13631,22 +13604,22 @@
     <row r="85" ht="25" customHeight="1">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>Moses</t>
+          <t>Moeller</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
         <is>
-          <t>Bernadine</t>
+          <t>Frauke E.</t>
         </is>
       </c>
       <c r="C85" s="3" t="inlineStr">
         <is>
-          <t>Cape Town</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D85" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E85" s="3" t="inlineStr">
@@ -13658,17 +13631,17 @@
     <row r="86" ht="25" customHeight="1">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>Mosesd</t>
+          <t>Moses</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
         <is>
-          <t>Brian</t>
+          <t>Bernadine</t>
         </is>
       </c>
       <c r="C86" s="3" t="inlineStr">
         <is>
-          <t>Cape Of Good Hope</t>
+          <t>Cape Town</t>
         </is>
       </c>
       <c r="D86" s="3" t="inlineStr">
@@ -13678,29 +13651,29 @@
       </c>
       <c r="E86" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="87" ht="25" customHeight="1">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>Mostert</t>
+          <t>Mosesd</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
         <is>
-          <t>Jacques</t>
+          <t>Brian</t>
         </is>
       </c>
       <c r="C87" s="3" t="inlineStr">
         <is>
-          <t>Merriman</t>
+          <t>Cape Of Good Hope</t>
         </is>
       </c>
       <c r="D87" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E87" s="3" t="inlineStr">
@@ -13712,22 +13685,22 @@
     <row r="88" ht="25" customHeight="1">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>Mutschler</t>
+          <t>Mostert</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
         <is>
-          <t>Peter</t>
+          <t>Jacques</t>
         </is>
       </c>
       <c r="C88" s="3" t="inlineStr">
         <is>
-          <t>Grootfontein</t>
+          <t>Merriman</t>
         </is>
       </c>
       <c r="D88" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E88" s="3" t="inlineStr">
@@ -13739,17 +13712,17 @@
     <row r="89" ht="25" customHeight="1">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>Myburg</t>
+          <t>Mutschler</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
         <is>
-          <t>Pieter</t>
+          <t>Peter</t>
         </is>
       </c>
       <c r="C89" s="3" t="inlineStr">
         <is>
-          <t>Wellington</t>
+          <t>Grootfontein</t>
         </is>
       </c>
       <c r="D89" s="3" t="inlineStr">
@@ -13759,14 +13732,14 @@
       </c>
       <c r="E89" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="90" ht="25" customHeight="1">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>Nel</t>
+          <t>Myburg</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -13776,7 +13749,7 @@
       </c>
       <c r="C90" s="3" t="inlineStr">
         <is>
-          <t>George</t>
+          <t>Wellington</t>
         </is>
       </c>
       <c r="D90" s="3" t="inlineStr">
@@ -13786,7 +13759,7 @@
       </c>
       <c r="E90" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -13798,12 +13771,12 @@
       </c>
       <c r="B91" s="3" t="inlineStr">
         <is>
-          <t>Tillie</t>
+          <t>Pieter</t>
         </is>
       </c>
       <c r="C91" s="3" t="inlineStr">
         <is>
-          <t>Eden</t>
+          <t>George</t>
         </is>
       </c>
       <c r="D91" s="3" t="inlineStr">
@@ -13820,17 +13793,17 @@
     <row r="92" ht="25" customHeight="1">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>Niehaus</t>
+          <t>Nel</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
         <is>
-          <t>Angela</t>
+          <t>Tillie</t>
         </is>
       </c>
       <c r="C92" s="3" t="inlineStr">
         <is>
-          <t>Bergvliet</t>
+          <t>Eden</t>
         </is>
       </c>
       <c r="D92" s="3" t="inlineStr">
@@ -13847,17 +13820,17 @@
     <row r="93" ht="25" customHeight="1">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>Nortjie</t>
+          <t>Niehaus</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
         <is>
-          <t>Rachel</t>
+          <t>Angela</t>
         </is>
       </c>
       <c r="C93" s="3" t="inlineStr">
         <is>
-          <t>Mitchells Plain</t>
+          <t>Bergvliet</t>
         </is>
       </c>
       <c r="D93" s="3" t="inlineStr">
@@ -13867,24 +13840,24 @@
       </c>
       <c r="E93" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="94" ht="25" customHeight="1">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>Ocker</t>
+          <t>Nortjie</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
         <is>
-          <t>Chris</t>
+          <t>Rachel</t>
         </is>
       </c>
       <c r="C94" s="3" t="inlineStr">
         <is>
-          <t>Fish Hoek</t>
+          <t>Mitchells Plain</t>
         </is>
       </c>
       <c r="D94" s="3" t="inlineStr">
@@ -13906,7 +13879,7 @@
       </c>
       <c r="B95" s="3" t="inlineStr">
         <is>
-          <t>Jenny</t>
+          <t>Chris</t>
         </is>
       </c>
       <c r="C95" s="3" t="inlineStr">
@@ -13928,17 +13901,17 @@
     <row r="96" ht="25" customHeight="1">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>Olivier</t>
+          <t>Ocker</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
         <is>
-          <t>Debra</t>
+          <t>Jenny</t>
         </is>
       </c>
       <c r="C96" s="3" t="inlineStr">
         <is>
-          <t>Sedgefield</t>
+          <t>Fish Hoek</t>
         </is>
       </c>
       <c r="D96" s="3" t="inlineStr">
@@ -13955,22 +13928,22 @@
     <row r="97" ht="25" customHeight="1">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>Ormandy</t>
+          <t>Olivier</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
         <is>
-          <t>Isabella Stratton</t>
+          <t>Debra</t>
         </is>
       </c>
       <c r="C97" s="3" t="inlineStr">
         <is>
-          <t>Milnerton</t>
+          <t>Sedgefield</t>
         </is>
       </c>
       <c r="D97" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E97" s="3" t="inlineStr">
@@ -13982,44 +13955,44 @@
     <row r="98" ht="25" customHeight="1">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>Peters</t>
+          <t>Ormandy</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
         <is>
-          <t>Maureen</t>
+          <t>Isabella Stratton</t>
         </is>
       </c>
       <c r="C98" s="3" t="inlineStr">
         <is>
-          <t>Ceres</t>
+          <t>Milnerton</t>
         </is>
       </c>
       <c r="D98" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E98" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="99" ht="25" customHeight="1">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>Pillay</t>
+          <t>Peters</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>Maureen</t>
         </is>
       </c>
       <c r="C99" s="3" t="inlineStr">
         <is>
-          <t>Tygerberg Hills</t>
+          <t>Ceres</t>
         </is>
       </c>
       <c r="D99" s="3" t="inlineStr">
@@ -14036,44 +14009,44 @@
     <row r="100" ht="25" customHeight="1">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>Poyowe</t>
+          <t>Pillay</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
         <is>
-          <t>Yvonne  Maureen</t>
+          <t>Patrick</t>
         </is>
       </c>
       <c r="C100" s="3" t="inlineStr">
         <is>
-          <t>Cape Of Good Hope</t>
+          <t>Tygerberg Hills</t>
         </is>
       </c>
       <c r="D100" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E100" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="101" ht="25" customHeight="1">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>Pretorius</t>
+          <t>Poyowe</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
         <is>
-          <t>Sheldon Edmund</t>
+          <t>Yvonne  Maureen</t>
         </is>
       </c>
       <c r="C101" s="3" t="inlineStr">
         <is>
-          <t>Merriman</t>
+          <t>Cape Of Good Hope</t>
         </is>
       </c>
       <c r="D101" s="3" t="inlineStr">
@@ -14090,22 +14063,22 @@
     <row r="102" ht="25" customHeight="1">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>Ras</t>
+          <t>Pretorius</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
         <is>
-          <t>Mary-Anne</t>
+          <t>Sheldon Edmund</t>
         </is>
       </c>
       <c r="C102" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Merriman</t>
         </is>
       </c>
       <c r="D102" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E102" s="3" t="inlineStr">
@@ -14117,17 +14090,17 @@
     <row r="103" ht="25" customHeight="1">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>Rossouw</t>
+          <t>Ras</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Mary-Anne</t>
         </is>
       </c>
       <c r="C103" s="3" t="inlineStr">
         <is>
-          <t>Tokai</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D103" s="3" t="inlineStr">
@@ -14137,24 +14110,24 @@
       </c>
       <c r="E103" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="104" ht="25" customHeight="1">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>Rothner</t>
+          <t>Rossouw</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
         <is>
-          <t>Andrea</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C104" s="3" t="inlineStr">
         <is>
-          <t>Eden</t>
+          <t>Tokai</t>
         </is>
       </c>
       <c r="D104" s="3" t="inlineStr">
@@ -14164,24 +14137,24 @@
       </c>
       <c r="E104" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="105" ht="25" customHeight="1">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>Roux</t>
+          <t>Rothner</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
         <is>
-          <t>Anthonie Petrus</t>
+          <t>Andrea</t>
         </is>
       </c>
       <c r="C105" s="3" t="inlineStr">
         <is>
-          <t>Moorreesburg</t>
+          <t>Eden</t>
         </is>
       </c>
       <c r="D105" s="3" t="inlineStr">
@@ -14191,24 +14164,24 @@
       </c>
       <c r="E105" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="106" ht="25" customHeight="1">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>Russell</t>
+          <t>Roux</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
         <is>
-          <t>Ingrid</t>
+          <t>Anthonie Petrus</t>
         </is>
       </c>
       <c r="C106" s="3" t="inlineStr">
         <is>
-          <t>Fish Hoek</t>
+          <t>Moorreesburg</t>
         </is>
       </c>
       <c r="D106" s="3" t="inlineStr">
@@ -14225,71 +14198,71 @@
     <row r="107" ht="25" customHeight="1">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>SNYMAN</t>
+          <t>Russell</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
         <is>
-          <t>LYN</t>
+          <t>Ingrid</t>
         </is>
       </c>
       <c r="C107" s="3" t="inlineStr">
         <is>
-          <t>Deep South</t>
+          <t>Fish Hoek</t>
         </is>
       </c>
       <c r="D107" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E107" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="108" ht="25" customHeight="1">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>STEENBERG</t>
+          <t>SNYMAN</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
         <is>
-          <t>TIM</t>
+          <t>LYN</t>
         </is>
       </c>
       <c r="C108" s="3" t="inlineStr">
         <is>
-          <t>Wellington</t>
+          <t>Deep South</t>
         </is>
       </c>
       <c r="D108" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E108" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="109" ht="25" customHeight="1">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>Sampie</t>
+          <t>STEENBERG</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
         <is>
-          <t>Sharon</t>
+          <t>TIM</t>
         </is>
       </c>
       <c r="C109" s="3" t="inlineStr">
         <is>
-          <t>Bergvliet</t>
+          <t>Wellington</t>
         </is>
       </c>
       <c r="D109" s="3" t="inlineStr">
@@ -14306,17 +14279,17 @@
     <row r="110" ht="25" customHeight="1">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>Schatz</t>
+          <t>Sampie</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
         <is>
-          <t>Vera</t>
+          <t>Sharon</t>
         </is>
       </c>
       <c r="C110" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Bergvliet</t>
         </is>
       </c>
       <c r="D110" s="3" t="inlineStr">
@@ -14326,7 +14299,7 @@
       </c>
       <c r="E110" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -14338,7 +14311,7 @@
       </c>
       <c r="B111" s="3" t="inlineStr">
         <is>
-          <t>Frank</t>
+          <t>Vera</t>
         </is>
       </c>
       <c r="C111" s="3" t="inlineStr">
@@ -14353,19 +14326,19 @@
       </c>
       <c r="E111" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="112" ht="25" customHeight="1">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>Sell</t>
+          <t>Schatz</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
         <is>
-          <t>Ami</t>
+          <t>Frank</t>
         </is>
       </c>
       <c r="C112" s="3" t="inlineStr">
@@ -14380,24 +14353,24 @@
       </c>
       <c r="E112" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="113" ht="25" customHeight="1">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>Simpson</t>
+          <t>Sell</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
         <is>
-          <t>Beryl</t>
+          <t>Ami</t>
         </is>
       </c>
       <c r="C113" s="3" t="inlineStr">
         <is>
-          <t>Cape Town</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D113" s="3" t="inlineStr">
@@ -14414,17 +14387,17 @@
     <row r="114" ht="25" customHeight="1">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>Sircoulomb</t>
+          <t>Simpson</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
         <is>
-          <t>Kenlis</t>
+          <t>Beryl</t>
         </is>
       </c>
       <c r="C114" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Cape Town</t>
         </is>
       </c>
       <c r="D114" s="3" t="inlineStr">
@@ -14446,7 +14419,7 @@
       </c>
       <c r="B115" s="3" t="inlineStr">
         <is>
-          <t>Holger</t>
+          <t>Kenlis</t>
         </is>
       </c>
       <c r="C115" s="3" t="inlineStr">
@@ -14461,24 +14434,24 @@
       </c>
       <c r="E115" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="116" ht="25" customHeight="1">
       <c r="A116" s="3" t="inlineStr">
         <is>
-          <t>Smit</t>
+          <t>Sircoulomb</t>
         </is>
       </c>
       <c r="B116" s="3" t="inlineStr">
         <is>
-          <t>Herman</t>
+          <t>Holger</t>
         </is>
       </c>
       <c r="C116" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D116" s="3" t="inlineStr">
@@ -14488,24 +14461,24 @@
       </c>
       <c r="E116" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="117" ht="25" customHeight="1">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Smit</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
         <is>
-          <t>Bennie</t>
+          <t>Herman</t>
         </is>
       </c>
       <c r="C117" s="3" t="inlineStr">
         <is>
-          <t>Wellington</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D117" s="3" t="inlineStr">
@@ -14515,7 +14488,7 @@
       </c>
       <c r="E117" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -14527,12 +14500,12 @@
       </c>
       <c r="B118" s="3" t="inlineStr">
         <is>
-          <t>Carmen Dolores</t>
+          <t>Bennie</t>
         </is>
       </c>
       <c r="C118" s="3" t="inlineStr">
         <is>
-          <t>Tokai</t>
+          <t>Wellington</t>
         </is>
       </c>
       <c r="D118" s="3" t="inlineStr">
@@ -14542,7 +14515,7 @@
       </c>
       <c r="E118" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -14554,7 +14527,7 @@
       </c>
       <c r="B119" s="3" t="inlineStr">
         <is>
-          <t>David John</t>
+          <t>Carmen Dolores</t>
         </is>
       </c>
       <c r="C119" s="3" t="inlineStr">
@@ -14576,17 +14549,17 @@
     <row r="120" ht="25" customHeight="1">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>Sochen</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="B120" s="3" t="inlineStr">
         <is>
-          <t>Diana</t>
+          <t>David John</t>
         </is>
       </c>
       <c r="C120" s="3" t="inlineStr">
         <is>
-          <t>Sea Point</t>
+          <t>Tokai</t>
         </is>
       </c>
       <c r="D120" s="3" t="inlineStr">
@@ -14596,56 +14569,56 @@
       </c>
       <c r="E120" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="121" ht="25" customHeight="1">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>Strauss</t>
+          <t>Sochen</t>
         </is>
       </c>
       <c r="B121" s="3" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>Diana</t>
         </is>
       </c>
       <c r="C121" s="3" t="inlineStr">
         <is>
-          <t>Kuilsriver</t>
+          <t>Sea Point</t>
         </is>
       </c>
       <c r="D121" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E121" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="122" ht="25" customHeight="1">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>Tshikala</t>
+          <t>Strauss</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
         <is>
-          <t>David Alex</t>
+          <t>Patrick</t>
         </is>
       </c>
       <c r="C122" s="3" t="inlineStr">
         <is>
-          <t>Athlone</t>
+          <t>Kuilsriver</t>
         </is>
       </c>
       <c r="D122" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E122" s="3" t="inlineStr">
@@ -14657,17 +14630,17 @@
     <row r="123" ht="25" customHeight="1">
       <c r="A123" s="3" t="inlineStr">
         <is>
-          <t>VAN BREDA</t>
+          <t>Tshikala</t>
         </is>
       </c>
       <c r="B123" s="3" t="inlineStr">
         <is>
-          <t>HILARY LISE</t>
+          <t>David Alex</t>
         </is>
       </c>
       <c r="C123" s="3" t="inlineStr">
         <is>
-          <t>Cape Town</t>
+          <t>Athlone</t>
         </is>
       </c>
       <c r="D123" s="3" t="inlineStr">
@@ -14684,17 +14657,17 @@
     <row r="124" ht="25" customHeight="1">
       <c r="A124" s="3" t="inlineStr">
         <is>
-          <t>VAN DER MERWE</t>
+          <t>VAN BREDA</t>
         </is>
       </c>
       <c r="B124" s="3" t="inlineStr">
         <is>
-          <t>MARINA</t>
+          <t>HILARY LISE</t>
         </is>
       </c>
       <c r="C124" s="3" t="inlineStr">
         <is>
-          <t>Malmesbury</t>
+          <t>Cape Town</t>
         </is>
       </c>
       <c r="D124" s="3" t="inlineStr">
@@ -14704,24 +14677,24 @@
       </c>
       <c r="E124" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="125" ht="25" customHeight="1">
       <c r="A125" s="3" t="inlineStr">
         <is>
-          <t>Van Rensburg</t>
+          <t>VAN DER MERWE</t>
         </is>
       </c>
       <c r="B125" s="3" t="inlineStr">
         <is>
-          <t>Neville</t>
+          <t>MARINA</t>
         </is>
       </c>
       <c r="C125" s="3" t="inlineStr">
         <is>
-          <t>Moorreesburg</t>
+          <t>Malmesbury</t>
         </is>
       </c>
       <c r="D125" s="3" t="inlineStr">
@@ -14738,44 +14711,44 @@
     <row r="126" ht="25" customHeight="1">
       <c r="A126" s="3" t="inlineStr">
         <is>
-          <t>Van Romburgh</t>
+          <t>Van Rensburg</t>
         </is>
       </c>
       <c r="B126" s="3" t="inlineStr">
         <is>
-          <t>Lorna</t>
+          <t>Neville</t>
         </is>
       </c>
       <c r="C126" s="3" t="inlineStr">
         <is>
-          <t>Fish Hoek</t>
+          <t>Moorreesburg</t>
         </is>
       </c>
       <c r="D126" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E126" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="127" ht="25" customHeight="1">
       <c r="A127" s="3" t="inlineStr">
         <is>
-          <t>Van Wyk-Nelson</t>
+          <t>Van Romburgh</t>
         </is>
       </c>
       <c r="B127" s="3" t="inlineStr">
         <is>
-          <t>Edith</t>
+          <t>Lorna</t>
         </is>
       </c>
       <c r="C127" s="3" t="inlineStr">
         <is>
-          <t>Kuilsriver</t>
+          <t>Fish Hoek</t>
         </is>
       </c>
       <c r="D127" s="3" t="inlineStr">
@@ -14792,22 +14765,22 @@
     <row r="128" ht="25" customHeight="1">
       <c r="A128" s="3" t="inlineStr">
         <is>
-          <t>Van de Merwe</t>
+          <t>Van Wyk-Nelson</t>
         </is>
       </c>
       <c r="B128" s="3" t="inlineStr">
         <is>
-          <t>Marina</t>
+          <t>Edith</t>
         </is>
       </c>
       <c r="C128" s="3" t="inlineStr">
         <is>
-          <t>Malmesbury</t>
+          <t>Kuilsriver</t>
         </is>
       </c>
       <c r="D128" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E128" s="3" t="inlineStr">
@@ -14819,22 +14792,22 @@
     <row r="129" ht="25" customHeight="1">
       <c r="A129" s="3" t="inlineStr">
         <is>
-          <t>Von Mollendorf</t>
+          <t>Van de Merwe</t>
         </is>
       </c>
       <c r="B129" s="3" t="inlineStr">
         <is>
-          <t>Rinette</t>
+          <t>Marina</t>
         </is>
       </c>
       <c r="C129" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>Malmesbury</t>
         </is>
       </c>
       <c r="D129" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E129" s="3" t="inlineStr">
@@ -14846,22 +14819,22 @@
     <row r="130" ht="25" customHeight="1">
       <c r="A130" s="3" t="inlineStr">
         <is>
-          <t>Vorster</t>
+          <t>Von Mollendorf</t>
         </is>
       </c>
       <c r="B130" s="3" t="inlineStr">
         <is>
-          <t>Rochelle</t>
+          <t>Rinette</t>
         </is>
       </c>
       <c r="C130" s="3" t="inlineStr">
         <is>
-          <t>Sedgefield</t>
+          <t>Durbanville</t>
         </is>
       </c>
       <c r="D130" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E130" s="3" t="inlineStr">
@@ -14873,22 +14846,22 @@
     <row r="131" ht="25" customHeight="1">
       <c r="A131" s="3" t="inlineStr">
         <is>
-          <t>Watson</t>
+          <t>Vorster</t>
         </is>
       </c>
       <c r="B131" s="3" t="inlineStr">
         <is>
-          <t>Allan</t>
+          <t>Rochelle</t>
         </is>
       </c>
       <c r="C131" s="3" t="inlineStr">
         <is>
-          <t>Sea Point</t>
+          <t>Sedgefield</t>
         </is>
       </c>
       <c r="D131" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E131" s="3" t="inlineStr">
@@ -14905,71 +14878,71 @@
       </c>
       <c r="B132" s="3" t="inlineStr">
         <is>
-          <t>Alison</t>
+          <t>Allan</t>
         </is>
       </c>
       <c r="C132" s="3" t="inlineStr">
         <is>
-          <t>Sedgefield</t>
+          <t>Sea Point</t>
         </is>
       </c>
       <c r="D132" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E132" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="133" ht="25" customHeight="1">
       <c r="A133" s="3" t="inlineStr">
         <is>
-          <t>Williams</t>
+          <t>Watson</t>
         </is>
       </c>
       <c r="B133" s="3" t="inlineStr">
         <is>
-          <t>Johanna</t>
+          <t>Alison</t>
         </is>
       </c>
       <c r="C133" s="3" t="inlineStr">
         <is>
-          <t>Mitchells Plain</t>
+          <t>Sedgefield</t>
         </is>
       </c>
       <c r="D133" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E133" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="134" ht="25" customHeight="1">
       <c r="A134" s="3" t="inlineStr">
         <is>
-          <t>Wills</t>
+          <t>Williams</t>
         </is>
       </c>
       <c r="B134" s="3" t="inlineStr">
         <is>
-          <t>Geila</t>
+          <t>Johanna</t>
         </is>
       </c>
       <c r="C134" s="3" t="inlineStr">
         <is>
-          <t>Athlone</t>
+          <t>Mitchells Plain</t>
         </is>
       </c>
       <c r="D134" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E134" s="3" t="inlineStr">
@@ -14981,22 +14954,22 @@
     <row r="135" ht="25" customHeight="1">
       <c r="A135" s="3" t="inlineStr">
         <is>
-          <t>Woodman</t>
+          <t>Wills</t>
         </is>
       </c>
       <c r="B135" s="3" t="inlineStr">
         <is>
-          <t>Joan</t>
+          <t>Geila</t>
         </is>
       </c>
       <c r="C135" s="3" t="inlineStr">
         <is>
-          <t>Mitchells Plain</t>
+          <t>Athlone</t>
         </is>
       </c>
       <c r="D135" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E135" s="3" t="inlineStr">
@@ -15008,44 +14981,44 @@
     <row r="136" ht="25" customHeight="1">
       <c r="A136" s="3" t="inlineStr">
         <is>
-          <t>Wright</t>
+          <t>Woodman</t>
         </is>
       </c>
       <c r="B136" s="3" t="inlineStr">
         <is>
-          <t>Rocky</t>
+          <t>Joan</t>
         </is>
       </c>
       <c r="C136" s="3" t="inlineStr">
         <is>
-          <t>Table View</t>
+          <t>Mitchells Plain</t>
         </is>
       </c>
       <c r="D136" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E136" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="137" ht="25" customHeight="1">
       <c r="A137" s="3" t="inlineStr">
         <is>
-          <t>Young</t>
+          <t>Wright</t>
         </is>
       </c>
       <c r="B137" s="3" t="inlineStr">
         <is>
-          <t>Judy</t>
+          <t>Rocky</t>
         </is>
       </c>
       <c r="C137" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>Table View</t>
         </is>
       </c>
       <c r="D137" s="3" t="inlineStr">
@@ -15055,7 +15028,7 @@
       </c>
       <c r="E137" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -15067,17 +15040,17 @@
       </c>
       <c r="B138" s="3" t="inlineStr">
         <is>
-          <t>Gerry</t>
+          <t>Judy</t>
         </is>
       </c>
       <c r="C138" s="3" t="inlineStr">
         <is>
-          <t>Mitchells Plain</t>
+          <t>Durbanville</t>
         </is>
       </c>
       <c r="D138" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E138" s="3" t="inlineStr">
@@ -15089,22 +15062,22 @@
     <row r="139" ht="25" customHeight="1">
       <c r="A139" s="3" t="inlineStr">
         <is>
-          <t>Zucker</t>
+          <t>Young</t>
         </is>
       </c>
       <c r="B139" s="3" t="inlineStr">
         <is>
-          <t>Leonie</t>
+          <t>Gerry</t>
         </is>
       </c>
       <c r="C139" s="3" t="inlineStr">
         <is>
-          <t>Milnerton</t>
+          <t>Mitchells Plain</t>
         </is>
       </c>
       <c r="D139" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E139" s="3" t="inlineStr">
@@ -15116,17 +15089,17 @@
     <row r="140" ht="25" customHeight="1">
       <c r="A140" s="3" t="inlineStr">
         <is>
-          <t>de Kock</t>
+          <t>Zucker</t>
         </is>
       </c>
       <c r="B140" s="3" t="inlineStr">
         <is>
-          <t>Engela</t>
+          <t>Leonie</t>
         </is>
       </c>
       <c r="C140" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Milnerton</t>
         </is>
       </c>
       <c r="D140" s="3" t="inlineStr">
@@ -15136,7 +15109,7 @@
       </c>
       <c r="E140" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -15148,7 +15121,7 @@
       </c>
       <c r="B141" s="3" t="inlineStr">
         <is>
-          <t>Francois</t>
+          <t>Engela</t>
         </is>
       </c>
       <c r="C141" s="3" t="inlineStr">
@@ -15170,22 +15143,22 @@
     <row r="142" ht="25" customHeight="1">
       <c r="A142" s="3" t="inlineStr">
         <is>
-          <t>stier</t>
+          <t>de Kock</t>
         </is>
       </c>
       <c r="B142" s="3" t="inlineStr">
         <is>
-          <t>RORY</t>
+          <t>Francois</t>
         </is>
       </c>
       <c r="C142" s="3" t="inlineStr">
         <is>
-          <t>Deep South</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D142" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E142" s="3" t="inlineStr">
@@ -15197,44 +15170,44 @@
     <row r="143" ht="25" customHeight="1">
       <c r="A143" s="3" t="inlineStr">
         <is>
-          <t>van Blerk</t>
+          <t>stier</t>
         </is>
       </c>
       <c r="B143" s="3" t="inlineStr">
         <is>
-          <t>Carl</t>
+          <t>RORY</t>
         </is>
       </c>
       <c r="C143" s="3" t="inlineStr">
         <is>
-          <t>Eden</t>
+          <t>Deep South</t>
         </is>
       </c>
       <c r="D143" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E143" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="144" ht="25" customHeight="1">
       <c r="A144" s="3" t="inlineStr">
         <is>
-          <t>van Rensburg</t>
+          <t>van Blerk</t>
         </is>
       </c>
       <c r="B144" s="3" t="inlineStr">
         <is>
-          <t>Johan</t>
+          <t>Carl</t>
         </is>
       </c>
       <c r="C144" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Eden</t>
         </is>
       </c>
       <c r="D144" s="3" t="inlineStr">
@@ -15256,7 +15229,7 @@
       </c>
       <c r="B145" s="3" t="inlineStr">
         <is>
-          <t>Anne</t>
+          <t>Johan</t>
         </is>
       </c>
       <c r="C145" s="3" t="inlineStr">
@@ -15278,17 +15251,17 @@
     <row r="146" ht="25" customHeight="1">
       <c r="A146" s="3" t="inlineStr">
         <is>
-          <t>van Wulven</t>
+          <t>van Rensburg</t>
         </is>
       </c>
       <c r="B146" s="3" t="inlineStr">
         <is>
-          <t>Jeannie</t>
+          <t>Anne</t>
         </is>
       </c>
       <c r="C146" s="3" t="inlineStr">
         <is>
-          <t>Tygerberg Hills</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D146" s="3" t="inlineStr">
@@ -15310,7 +15283,7 @@
       </c>
       <c r="B147" s="3" t="inlineStr">
         <is>
-          <t>Alan</t>
+          <t>Jeannie</t>
         </is>
       </c>
       <c r="C147" s="3" t="inlineStr">
@@ -15337,7 +15310,7 @@
       </c>
       <c r="B148" s="3" t="inlineStr">
         <is>
-          <t>Deon</t>
+          <t>Alan</t>
         </is>
       </c>
       <c r="C148" s="3" t="inlineStr">
@@ -15359,41 +15332,68 @@
     <row r="149" ht="25" customHeight="1">
       <c r="A149" s="3" t="inlineStr">
         <is>
+          <t>van Wulven</t>
+        </is>
+      </c>
+      <c r="B149" s="3" t="inlineStr">
+        <is>
+          <t>Deon</t>
+        </is>
+      </c>
+      <c r="C149" s="3" t="inlineStr">
+        <is>
+          <t>Tygerberg Hills</t>
+        </is>
+      </c>
+      <c r="D149" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E149" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="150" ht="25" customHeight="1">
+      <c r="A150" s="3" t="inlineStr">
+        <is>
           <t>van der Westhuizen</t>
         </is>
       </c>
-      <c r="B149" s="3" t="inlineStr">
+      <c r="B150" s="3" t="inlineStr">
         <is>
           <t>Hennie</t>
         </is>
       </c>
-      <c r="C149" s="3" t="inlineStr">
+      <c r="C150" s="3" t="inlineStr">
         <is>
           <t>Helderberg</t>
         </is>
       </c>
-      <c r="D149" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E149" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-    </row>
-    <row r="150">
-      <c r="A150" s="1" t="inlineStr">
-        <is>
-          <t>Number of attendees: 147</t>
+      <c r="D150" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E150" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="inlineStr">
         <is>
-          <t>Number of voters: 54</t>
+          <t>Number of attendees: 148</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="1" t="inlineStr">
+        <is>
+          <t>Number of voters: 55</t>
         </is>
       </c>
     </row>
@@ -15409,7 +15409,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15424,7 +15424,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Voting details as of 20/04/2021 11:25</t>
+          <t>410E Voting details as of 20/04/2021 15:16</t>
         </is>
       </c>
     </row>
@@ -15583,17 +15583,17 @@
     <row r="17" ht="25" customHeight="1">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>Milnerton</t>
+          <t>Nelspruit</t>
         </is>
       </c>
       <c r="B17" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" ht="25" customHeight="1">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>Nelspruit</t>
+          <t>North Durban</t>
         </is>
       </c>
       <c r="B18" s="3" t="n">
@@ -15603,7 +15603,7 @@
     <row r="19" ht="25" customHeight="1">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>North Durban</t>
+          <t>Port Alfred</t>
         </is>
       </c>
       <c r="B19" s="3" t="n">
@@ -15613,47 +15613,47 @@
     <row r="20" ht="25" customHeight="1">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>Port Alfred</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="B20" s="3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" ht="25" customHeight="1">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="B21" s="3" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" ht="25" customHeight="1">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="B22" s="3" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" ht="25" customHeight="1">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Roodepoort Clearwater Cyber</t>
         </is>
       </c>
       <c r="B23" s="3" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" ht="25" customHeight="1">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>Roodepoort Clearwater Cyber</t>
+          <t>Rustenburg</t>
         </is>
       </c>
       <c r="B24" s="3" t="n">
@@ -15663,7 +15663,7 @@
     <row r="25" ht="25" customHeight="1">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>Rustenburg</t>
+          <t>Standerton</t>
         </is>
       </c>
       <c r="B25" s="3" t="n">
@@ -15673,17 +15673,17 @@
     <row r="26" ht="25" customHeight="1">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>Standerton</t>
+          <t>The Wilds</t>
         </is>
       </c>
       <c r="B26" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" ht="25" customHeight="1">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>The Wilds</t>
+          <t>Uitenhage</t>
         </is>
       </c>
       <c r="B27" s="3" t="n">
@@ -15693,44 +15693,34 @@
     <row r="28" ht="25" customHeight="1">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>Uitenhage</t>
+          <t>Vereeniging</t>
         </is>
       </c>
       <c r="B28" s="3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" ht="25" customHeight="1">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>Vereeniging</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="B29" s="3" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" ht="25" customHeight="1">
-      <c r="A30" s="3" t="inlineStr">
-        <is>
-          <t>Wilro Park</t>
-        </is>
-      </c>
-      <c r="B30" s="3" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>Number of clubs: 27</t>
+        </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>Number of clubs: 28</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="1" t="inlineStr">
-        <is>
-          <t>Number of voters: 61</t>
+          <t>Number of voters: 60</t>
         </is>
       </c>
     </row>
@@ -15761,7 +15751,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Voting details as of 20/04/2021 11:25</t>
+          <t>410W Voting details as of 20/04/2021 15:16</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Registree stats backup on Tue 20 Apr 2021 20:45:56 SAST
</commit_message>
<xml_diff>
--- a/static/docs/registrees_list.xlsx
+++ b/static/docs/registrees_list.xlsx
@@ -451,7 +451,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>MD410 Registrees as of 20/04/2021 19:04</t>
+          <t>MD410 Registrees as of 20/04/2021 20:45</t>
         </is>
       </c>
     </row>
@@ -7993,7 +7993,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E126"/>
+  <dimension ref="A1:E128"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8011,7 +8011,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Registrees as of 20/04/2021 19:04</t>
+          <t>410E Registrees as of 20/04/2021 20:45</t>
         </is>
       </c>
     </row>
@@ -8072,17 +8072,17 @@
     <row r="4" ht="25" customHeight="1">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>Boswell</t>
+          <t>Blakeman</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>Mel</t>
+          <t>Belinda</t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>Nelspruit</t>
+          <t>North Durban</t>
         </is>
       </c>
       <c r="D4" s="3" t="inlineStr">
@@ -8099,17 +8099,17 @@
     <row r="5" ht="25" customHeight="1">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>Botha</t>
+          <t>Blakeman</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>Lyn(ette)</t>
+          <t>Belinda</t>
         </is>
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>Cowies Hill</t>
+          <t>North Durban</t>
         </is>
       </c>
       <c r="D5" s="3" t="inlineStr">
@@ -8119,24 +8119,24 @@
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="6" ht="25" customHeight="1">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>Brauteseth</t>
+          <t>Boswell</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Mel</t>
         </is>
       </c>
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Nelspruit</t>
         </is>
       </c>
       <c r="D6" s="3" t="inlineStr">
@@ -8146,24 +8146,24 @@
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="7" ht="25" customHeight="1">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>Brooker</t>
+          <t>Botha</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>Byron</t>
+          <t>Lyn(ette)</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Cowies Hill</t>
         </is>
       </c>
       <c r="D7" s="3" t="inlineStr">
@@ -8180,17 +8180,17 @@
     <row r="8" ht="25" customHeight="1">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>Bull</t>
+          <t>Brauteseth</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>Christopher</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>The Wilds</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D8" s="3" t="inlineStr">
@@ -8200,24 +8200,24 @@
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="9" ht="25" customHeight="1">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>Byars</t>
+          <t>Brooker</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>Karin</t>
+          <t>Byron</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
         <is>
-          <t>Manzini</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D9" s="3" t="inlineStr">
@@ -8227,24 +8227,24 @@
       </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="10" ht="25" customHeight="1">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>Chazen</t>
+          <t>Bull</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>Lionel</t>
+          <t>Christopher</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr">
         <is>
-          <t>Edenvale</t>
+          <t>The Wilds</t>
         </is>
       </c>
       <c r="D10" s="3" t="inlineStr">
@@ -8261,17 +8261,17 @@
     <row r="11" ht="25" customHeight="1">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>Chetty</t>
+          <t>Byars</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>Perry</t>
+          <t>Karin</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
-          <t>East Coast</t>
+          <t>Manzini</t>
         </is>
       </c>
       <c r="D11" s="3" t="inlineStr">
@@ -8288,22 +8288,22 @@
     <row r="12" ht="25" customHeight="1">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>Coppen</t>
+          <t>Chazen</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
         <is>
-          <t>Kate</t>
+          <t>Lionel</t>
         </is>
       </c>
       <c r="C12" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Edenvale</t>
         </is>
       </c>
       <c r="D12" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E12" s="3" t="inlineStr">
@@ -8315,22 +8315,22 @@
     <row r="13" ht="25" customHeight="1">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>Davids</t>
+          <t>Chetty</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>Melanie</t>
+          <t>Perry</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>East Coast</t>
         </is>
       </c>
       <c r="D13" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E13" s="3" t="inlineStr">
@@ -8342,22 +8342,22 @@
     <row r="14" ht="25" customHeight="1">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>De Wet</t>
+          <t>Coppen</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>Lara</t>
+          <t>Kate</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr">
         <is>
-          <t>Edenvale</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D14" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E14" s="3" t="inlineStr">
@@ -8369,44 +8369,44 @@
     <row r="15" ht="25" customHeight="1">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>Du Plooy</t>
+          <t>Davids</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>Peggy</t>
+          <t>Melanie</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
         <is>
-          <t>Krugersdorp</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D15" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E15" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="16" ht="25" customHeight="1">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>Du Plooy</t>
+          <t>De Wet</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>Ivan</t>
+          <t>Lara</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
         <is>
-          <t>Krugersdorp</t>
+          <t>Edenvale</t>
         </is>
       </c>
       <c r="D16" s="3" t="inlineStr">
@@ -8416,24 +8416,24 @@
       </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="17" ht="25" customHeight="1">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>Easton</t>
+          <t>Du Plooy</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>Glynn</t>
+          <t>Peggy</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
         <is>
-          <t>Helderkruin</t>
+          <t>Krugersdorp</t>
         </is>
       </c>
       <c r="D17" s="3" t="inlineStr">
@@ -8450,17 +8450,17 @@
     <row r="18" ht="25" customHeight="1">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>Easton</t>
+          <t>Du Plooy</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>Denise</t>
+          <t>Ivan</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
         <is>
-          <t>Helderkruin</t>
+          <t>Krugersdorp</t>
         </is>
       </c>
       <c r="D18" s="3" t="inlineStr">
@@ -8477,44 +8477,44 @@
     <row r="19" ht="25" customHeight="1">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>Els</t>
+          <t>Easton</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
-          <t>Johan</t>
+          <t>Glynn</t>
         </is>
       </c>
       <c r="C19" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Helderkruin</t>
         </is>
       </c>
       <c r="D19" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E19" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="20" ht="25" customHeight="1">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>Erasmus</t>
+          <t>Easton</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>Freddie</t>
+          <t>Denise</t>
         </is>
       </c>
       <c r="C20" s="3" t="inlineStr">
         <is>
-          <t>Uitenhage</t>
+          <t>Helderkruin</t>
         </is>
       </c>
       <c r="D20" s="3" t="inlineStr">
@@ -8531,44 +8531,44 @@
     <row r="21" ht="25" customHeight="1">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>Fourie</t>
+          <t>Els</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>Lucille</t>
+          <t>Johan</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D21" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E21" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="22" ht="25" customHeight="1">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>Foxcroft</t>
+          <t>Erasmus</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
         <is>
-          <t>Kelvin</t>
+          <t>Freddie</t>
         </is>
       </c>
       <c r="C22" s="3" t="inlineStr">
         <is>
-          <t>Helderkruin</t>
+          <t>Uitenhage</t>
         </is>
       </c>
       <c r="D22" s="3" t="inlineStr">
@@ -8585,17 +8585,17 @@
     <row r="23" ht="25" customHeight="1">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>Foxcroft</t>
+          <t>Fourie</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
         <is>
-          <t>Jenny</t>
+          <t>Lucille</t>
         </is>
       </c>
       <c r="C23" s="3" t="inlineStr">
         <is>
-          <t>Helderkruin</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D23" s="3" t="inlineStr">
@@ -8617,7 +8617,7 @@
       </c>
       <c r="B24" s="3" t="inlineStr">
         <is>
-          <t>Katherine</t>
+          <t>Kelvin</t>
         </is>
       </c>
       <c r="C24" s="3" t="inlineStr">
@@ -8639,17 +8639,17 @@
     <row r="25" ht="25" customHeight="1">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>Froise</t>
+          <t>Foxcroft</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
         <is>
-          <t>Martin</t>
+          <t>Jenny</t>
         </is>
       </c>
       <c r="C25" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Helderkruin</t>
         </is>
       </c>
       <c r="D25" s="3" t="inlineStr">
@@ -8666,17 +8666,17 @@
     <row r="26" ht="25" customHeight="1">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>Gerhard</t>
+          <t>Foxcroft</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
         <is>
-          <t>Bernd</t>
+          <t>Katherine</t>
         </is>
       </c>
       <c r="C26" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Helderkruin</t>
         </is>
       </c>
       <c r="D26" s="3" t="inlineStr">
@@ -8693,17 +8693,17 @@
     <row r="27" ht="25" customHeight="1">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>Gerhard</t>
+          <t>Froise</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
         <is>
-          <t>Shirley</t>
+          <t>Martin</t>
         </is>
       </c>
       <c r="C27" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D27" s="3" t="inlineStr">
@@ -8713,24 +8713,24 @@
       </c>
       <c r="E27" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="28" ht="25" customHeight="1">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>Graham</t>
+          <t>Gerhard</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
         <is>
-          <t>Valerie</t>
+          <t>Bernd</t>
         </is>
       </c>
       <c r="C28" s="3" t="inlineStr">
         <is>
-          <t>Nelspruit</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D28" s="3" t="inlineStr">
@@ -8747,17 +8747,17 @@
     <row r="29" ht="25" customHeight="1">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>Graham</t>
+          <t>Gerhard</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
         <is>
-          <t>Mike</t>
+          <t>Shirley</t>
         </is>
       </c>
       <c r="C29" s="3" t="inlineStr">
         <is>
-          <t>Nelspruit</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D29" s="3" t="inlineStr">
@@ -8774,22 +8774,22 @@
     <row r="30" ht="25" customHeight="1">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>Griffith</t>
+          <t>Graham</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
         <is>
-          <t>David</t>
+          <t>Valerie</t>
         </is>
       </c>
       <c r="C30" s="3" t="inlineStr">
         <is>
-          <t>The Wilds</t>
+          <t>Nelspruit</t>
         </is>
       </c>
       <c r="D30" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E30" s="3" t="inlineStr">
@@ -8801,17 +8801,17 @@
     <row r="31" ht="25" customHeight="1">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>Guthrie</t>
+          <t>Graham</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
         <is>
-          <t>Clint</t>
+          <t>Mike</t>
         </is>
       </c>
       <c r="C31" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Nelspruit</t>
         </is>
       </c>
       <c r="D31" s="3" t="inlineStr">
@@ -8828,17 +8828,17 @@
     <row r="32" ht="25" customHeight="1">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>HERMANUS</t>
+          <t>Griffith</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
         <is>
-          <t>MBULELO</t>
+          <t>David</t>
         </is>
       </c>
       <c r="C32" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>The Wilds</t>
         </is>
       </c>
       <c r="D32" s="3" t="inlineStr">
@@ -8855,17 +8855,17 @@
     <row r="33" ht="25" customHeight="1">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>HOLLIMAN</t>
+          <t>Guthrie</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
         <is>
-          <t>KEITH ALEXANDER</t>
+          <t>Clint</t>
         </is>
       </c>
       <c r="C33" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D33" s="3" t="inlineStr">
@@ -8882,22 +8882,22 @@
     <row r="34" ht="25" customHeight="1">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>Heathcote</t>
+          <t>HERMANUS</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
         <is>
-          <t>Mike</t>
+          <t>MBULELO</t>
         </is>
       </c>
       <c r="C34" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D34" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E34" s="3" t="inlineStr">
@@ -8909,17 +8909,17 @@
     <row r="35" ht="25" customHeight="1">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>Herzfeld</t>
+          <t>HOLLIMAN</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
         <is>
-          <t>Evelyn</t>
+          <t>KEITH ALEXANDER</t>
         </is>
       </c>
       <c r="C35" s="3" t="inlineStr">
         <is>
-          <t>Edenvale</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D35" s="3" t="inlineStr">
@@ -8936,17 +8936,17 @@
     <row r="36" ht="25" customHeight="1">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>Higgins</t>
+          <t>Heathcote</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
         <is>
-          <t>Wendy</t>
+          <t>Mike</t>
         </is>
       </c>
       <c r="C36" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D36" s="3" t="inlineStr">
@@ -8956,24 +8956,24 @@
       </c>
       <c r="E36" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="37" ht="25" customHeight="1">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>Hobbs</t>
+          <t>Herzfeld</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
         <is>
-          <t>Avril</t>
+          <t>Evelyn</t>
         </is>
       </c>
       <c r="C37" s="3" t="inlineStr">
         <is>
-          <t>North Durban</t>
+          <t>Edenvale</t>
         </is>
       </c>
       <c r="D37" s="3" t="inlineStr">
@@ -8983,24 +8983,24 @@
       </c>
       <c r="E37" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="38" ht="25" customHeight="1">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>Hobbs</t>
+          <t>Higgins</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
         <is>
-          <t>Trevor</t>
+          <t>Wendy</t>
         </is>
       </c>
       <c r="C38" s="3" t="inlineStr">
         <is>
-          <t>North Durban</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D38" s="3" t="inlineStr">
@@ -9010,24 +9010,24 @@
       </c>
       <c r="E38" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="39" ht="25" customHeight="1">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>Hocking</t>
+          <t>Hobbs</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
         <is>
-          <t>Jacqui</t>
+          <t>Avril</t>
         </is>
       </c>
       <c r="C39" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>North Durban</t>
         </is>
       </c>
       <c r="D39" s="3" t="inlineStr">
@@ -9044,17 +9044,17 @@
     <row r="40" ht="25" customHeight="1">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>Hocking</t>
+          <t>Hobbs</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
         <is>
-          <t>Cliff</t>
+          <t>Trevor</t>
         </is>
       </c>
       <c r="C40" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>North Durban</t>
         </is>
       </c>
       <c r="D40" s="3" t="inlineStr">
@@ -9064,24 +9064,24 @@
       </c>
       <c r="E40" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="41" ht="25" customHeight="1">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>JOHNSTON</t>
+          <t>Hocking</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
         <is>
-          <t>MALCOLM</t>
+          <t>Jacqui</t>
         </is>
       </c>
       <c r="C41" s="3" t="inlineStr">
         <is>
-          <t>Standerton</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D41" s="3" t="inlineStr">
@@ -9098,17 +9098,17 @@
     <row r="42" ht="25" customHeight="1">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>Jackson</t>
+          <t>Hocking</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
         <is>
-          <t>Alna</t>
+          <t>Cliff</t>
         </is>
       </c>
       <c r="C42" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D42" s="3" t="inlineStr">
@@ -9118,24 +9118,24 @@
       </c>
       <c r="E42" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="43" ht="25" customHeight="1">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>Kienast</t>
+          <t>JOHNSTON</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
         <is>
-          <t>Margie</t>
+          <t>MALCOLM</t>
         </is>
       </c>
       <c r="C43" s="3" t="inlineStr">
         <is>
-          <t>Edenvale</t>
+          <t>Standerton</t>
         </is>
       </c>
       <c r="D43" s="3" t="inlineStr">
@@ -9145,24 +9145,24 @@
       </c>
       <c r="E43" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="44" ht="25" customHeight="1">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>Kimari</t>
+          <t>Jackson</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
         <is>
-          <t>Joyce</t>
+          <t>Alna</t>
         </is>
       </c>
       <c r="C44" s="3" t="inlineStr">
         <is>
-          <t>Eden</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D44" s="3" t="inlineStr">
@@ -9172,24 +9172,24 @@
       </c>
       <c r="E44" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="45" ht="25" customHeight="1">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>King</t>
+          <t>Kienast</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
         <is>
-          <t>Ian</t>
+          <t>Margie</t>
         </is>
       </c>
       <c r="C45" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Edenvale</t>
         </is>
       </c>
       <c r="D45" s="3" t="inlineStr">
@@ -9199,24 +9199,24 @@
       </c>
       <c r="E45" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="46" ht="25" customHeight="1">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>King</t>
+          <t>Kimari</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
         <is>
-          <t>Sandy</t>
+          <t>Joyce</t>
         </is>
       </c>
       <c r="C46" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Eden</t>
         </is>
       </c>
       <c r="D46" s="3" t="inlineStr">
@@ -9226,24 +9226,24 @@
       </c>
       <c r="E46" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="47" ht="25" customHeight="1">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>Koekemoer</t>
+          <t>King</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
         <is>
-          <t>Christa</t>
+          <t>Ian</t>
         </is>
       </c>
       <c r="C47" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D47" s="3" t="inlineStr">
@@ -9253,56 +9253,56 @@
       </c>
       <c r="E47" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="48" ht="25" customHeight="1">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>Kruger</t>
+          <t>King</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
         <is>
-          <t>Pieter</t>
+          <t>Sandy</t>
         </is>
       </c>
       <c r="C48" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D48" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E48" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="49" ht="25" customHeight="1">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>Kruger</t>
+          <t>Koekemoer</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
         <is>
-          <t>Niqula</t>
+          <t>Christa</t>
         </is>
       </c>
       <c r="C49" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D49" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E49" s="3" t="inlineStr">
@@ -9314,22 +9314,22 @@
     <row r="50" ht="25" customHeight="1">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>Laas</t>
+          <t>Kruger</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
         <is>
-          <t>Natalie</t>
+          <t>Pieter</t>
         </is>
       </c>
       <c r="C50" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D50" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E50" s="3" t="inlineStr">
@@ -9341,12 +9341,12 @@
     <row r="51" ht="25" customHeight="1">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>Labuschagne</t>
+          <t>Kruger</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
         <is>
-          <t>Susan</t>
+          <t>Niqula</t>
         </is>
       </c>
       <c r="C51" s="3" t="inlineStr">
@@ -9356,7 +9356,7 @@
       </c>
       <c r="D51" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E51" s="3" t="inlineStr">
@@ -9368,12 +9368,12 @@
     <row r="52" ht="25" customHeight="1">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>Langton</t>
+          <t>Laas</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
         <is>
-          <t>Evelyn May</t>
+          <t>Natalie</t>
         </is>
       </c>
       <c r="C52" s="3" t="inlineStr">
@@ -9383,7 +9383,7 @@
       </c>
       <c r="D52" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E52" s="3" t="inlineStr">
@@ -9395,17 +9395,17 @@
     <row r="53" ht="25" customHeight="1">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>Lautenbach</t>
+          <t>Labuschagne</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
         <is>
-          <t>Steven</t>
+          <t>Susan</t>
         </is>
       </c>
       <c r="C53" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D53" s="3" t="inlineStr">
@@ -9415,29 +9415,29 @@
       </c>
       <c r="E53" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="54" ht="25" customHeight="1">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>Logan</t>
+          <t>Langton</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
         <is>
-          <t>Graeme</t>
+          <t>Evelyn May</t>
         </is>
       </c>
       <c r="C54" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D54" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E54" s="3" t="inlineStr">
@@ -9449,17 +9449,17 @@
     <row r="55" ht="25" customHeight="1">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>Love</t>
+          <t>Lautenbach</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
         <is>
-          <t>Dee</t>
+          <t>Steven</t>
         </is>
       </c>
       <c r="C55" s="3" t="inlineStr">
         <is>
-          <t>Cowies Hill</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D55" s="3" t="inlineStr">
@@ -9469,24 +9469,24 @@
       </c>
       <c r="E55" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="56" ht="25" customHeight="1">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>MILLS</t>
+          <t>Logan</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
         <is>
-          <t>BERNICE</t>
+          <t>Graeme</t>
         </is>
       </c>
       <c r="C56" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D56" s="3" t="inlineStr">
@@ -9496,24 +9496,24 @@
       </c>
       <c r="E56" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="57" ht="25" customHeight="1">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>Mare</t>
+          <t>Love</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
         <is>
-          <t>Beaulieu</t>
+          <t>Dee</t>
         </is>
       </c>
       <c r="C57" s="3" t="inlineStr">
         <is>
-          <t>Benoni Lakes</t>
+          <t>Cowies Hill</t>
         </is>
       </c>
       <c r="D57" s="3" t="inlineStr">
@@ -9523,24 +9523,24 @@
       </c>
       <c r="E57" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="58" ht="25" customHeight="1">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>Maré</t>
+          <t>MILLS</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
         <is>
-          <t>Nick</t>
+          <t>BERNICE</t>
         </is>
       </c>
       <c r="C58" s="3" t="inlineStr">
         <is>
-          <t>Benoni Lakes</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D58" s="3" t="inlineStr">
@@ -9550,24 +9550,24 @@
       </c>
       <c r="E58" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="59" ht="25" customHeight="1">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>Masson</t>
+          <t>Mare</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
         <is>
-          <t>Jean</t>
+          <t>Beaulieu</t>
         </is>
       </c>
       <c r="C59" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Benoni Lakes</t>
         </is>
       </c>
       <c r="D59" s="3" t="inlineStr">
@@ -9577,24 +9577,24 @@
       </c>
       <c r="E59" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="60" ht="25" customHeight="1">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>McDonald</t>
+          <t>Maré</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
         <is>
-          <t>Rochelle</t>
+          <t>Nick</t>
         </is>
       </c>
       <c r="C60" s="3" t="inlineStr">
         <is>
-          <t>Vereeniging</t>
+          <t>Benoni Lakes</t>
         </is>
       </c>
       <c r="D60" s="3" t="inlineStr">
@@ -9604,24 +9604,24 @@
       </c>
       <c r="E60" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="61" ht="25" customHeight="1">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>McKerrow</t>
+          <t>Masson</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
         <is>
-          <t>Alec</t>
+          <t>Jean</t>
         </is>
       </c>
       <c r="C61" s="3" t="inlineStr">
         <is>
-          <t>Port Alfred</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D61" s="3" t="inlineStr">
@@ -9638,17 +9638,17 @@
     <row r="62" ht="25" customHeight="1">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>Mccullough</t>
+          <t>McDonald</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
         <is>
-          <t>David</t>
+          <t>Rochelle</t>
         </is>
       </c>
       <c r="C62" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Vereeniging</t>
         </is>
       </c>
       <c r="D62" s="3" t="inlineStr">
@@ -9658,24 +9658,24 @@
       </c>
       <c r="E62" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="63" ht="25" customHeight="1">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>Meltzer</t>
+          <t>McKerrow</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Alec</t>
         </is>
       </c>
       <c r="C63" s="3" t="inlineStr">
         <is>
-          <t>The Wilds</t>
+          <t>Port Alfred</t>
         </is>
       </c>
       <c r="D63" s="3" t="inlineStr">
@@ -9685,24 +9685,24 @@
       </c>
       <c r="E63" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="64" ht="25" customHeight="1">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>Meyer</t>
+          <t>Mccullough</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
         <is>
-          <t>Denis</t>
+          <t>David</t>
         </is>
       </c>
       <c r="C64" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D64" s="3" t="inlineStr">
@@ -9712,24 +9712,24 @@
       </c>
       <c r="E64" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="65" ht="25" customHeight="1">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>Michas</t>
+          <t>Meltzer</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
         <is>
-          <t>Roy</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C65" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>The Wilds</t>
         </is>
       </c>
       <c r="D65" s="3" t="inlineStr">
@@ -9746,17 +9746,17 @@
     <row r="66" ht="25" customHeight="1">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>Michas</t>
+          <t>Meyer</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
         <is>
-          <t>Dawn</t>
+          <t>Denis</t>
         </is>
       </c>
       <c r="C66" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D66" s="3" t="inlineStr">
@@ -9766,24 +9766,24 @@
       </c>
       <c r="E66" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="67" ht="25" customHeight="1">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>Mills</t>
+          <t>Michas</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>Roy</t>
         </is>
       </c>
       <c r="C67" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D67" s="3" t="inlineStr">
@@ -9800,17 +9800,17 @@
     <row r="68" ht="25" customHeight="1">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>Mitchell</t>
+          <t>Michas</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
         <is>
-          <t>Alana</t>
+          <t>Dawn</t>
         </is>
       </c>
       <c r="C68" s="3" t="inlineStr">
         <is>
-          <t>Rustenburg</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D68" s="3" t="inlineStr">
@@ -9827,17 +9827,17 @@
     <row r="69" ht="25" customHeight="1">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>Mitchell</t>
+          <t>Mills</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
         <is>
-          <t>Juan</t>
+          <t>Patrick</t>
         </is>
       </c>
       <c r="C69" s="3" t="inlineStr">
         <is>
-          <t>Rustenburg</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D69" s="3" t="inlineStr">
@@ -9854,17 +9854,17 @@
     <row r="70" ht="25" customHeight="1">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>Murray</t>
+          <t>Mitchell</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
         <is>
-          <t>Suzanne</t>
+          <t>Alana</t>
         </is>
       </c>
       <c r="C70" s="3" t="inlineStr">
         <is>
-          <t>Vereeniging</t>
+          <t>Rustenburg</t>
         </is>
       </c>
       <c r="D70" s="3" t="inlineStr">
@@ -9874,24 +9874,24 @@
       </c>
       <c r="E70" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="71" ht="25" customHeight="1">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>Murray</t>
+          <t>Mitchell</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
         <is>
-          <t>Gary</t>
+          <t>Juan</t>
         </is>
       </c>
       <c r="C71" s="3" t="inlineStr">
         <is>
-          <t>Vereeniging</t>
+          <t>Rustenburg</t>
         </is>
       </c>
       <c r="D71" s="3" t="inlineStr">
@@ -9908,17 +9908,17 @@
     <row r="72" ht="25" customHeight="1">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>Nel</t>
+          <t>Murray</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
         <is>
-          <t>Theo</t>
+          <t>Suzanne</t>
         </is>
       </c>
       <c r="C72" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Vereeniging</t>
         </is>
       </c>
       <c r="D72" s="3" t="inlineStr">
@@ -9935,17 +9935,17 @@
     <row r="73" ht="25" customHeight="1">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>Newlands</t>
+          <t>Murray</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
         <is>
-          <t>Mike</t>
+          <t>Gary</t>
         </is>
       </c>
       <c r="C73" s="3" t="inlineStr">
         <is>
-          <t>Port Alfred</t>
+          <t>Vereeniging</t>
         </is>
       </c>
       <c r="D73" s="3" t="inlineStr">
@@ -9962,17 +9962,17 @@
     <row r="74" ht="25" customHeight="1">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>Ngobozana</t>
+          <t>Nel</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
         <is>
-          <t>Sphiwe</t>
+          <t>Theo</t>
         </is>
       </c>
       <c r="C74" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D74" s="3" t="inlineStr">
@@ -9982,24 +9982,24 @@
       </c>
       <c r="E74" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="75" ht="25" customHeight="1">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>Oberholzer</t>
+          <t>Newlands</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
         <is>
-          <t>PDG Bokkie</t>
+          <t>Mike</t>
         </is>
       </c>
       <c r="C75" s="3" t="inlineStr">
         <is>
-          <t>Uitenhage</t>
+          <t>Port Alfred</t>
         </is>
       </c>
       <c r="D75" s="3" t="inlineStr">
@@ -10016,17 +10016,17 @@
     <row r="76" ht="25" customHeight="1">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>PORTEOUS</t>
+          <t>Ngobozana</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
         <is>
-          <t>BRIAN</t>
+          <t>Sphiwe</t>
         </is>
       </c>
       <c r="C76" s="3" t="inlineStr">
         <is>
-          <t>Hibberdene</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D76" s="3" t="inlineStr">
@@ -10036,24 +10036,24 @@
       </c>
       <c r="E76" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="77" ht="25" customHeight="1">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>Paijmans</t>
+          <t>Oberholzer</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
         <is>
-          <t>Bronwyn Anne</t>
+          <t>PDG Bokkie</t>
         </is>
       </c>
       <c r="C77" s="3" t="inlineStr">
         <is>
-          <t>Cowies Hill</t>
+          <t>Uitenhage</t>
         </is>
       </c>
       <c r="D77" s="3" t="inlineStr">
@@ -10063,24 +10063,24 @@
       </c>
       <c r="E77" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="78" ht="25" customHeight="1">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>Pantoleon</t>
+          <t>PORTEOUS</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
         <is>
-          <t>Teresa</t>
+          <t>BRIAN</t>
         </is>
       </c>
       <c r="C78" s="3" t="inlineStr">
         <is>
-          <t>Vereeniging</t>
+          <t>Hibberdene</t>
         </is>
       </c>
       <c r="D78" s="3" t="inlineStr">
@@ -10097,17 +10097,17 @@
     <row r="79" ht="25" customHeight="1">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>Polkinghorne</t>
+          <t>Paijmans</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
         <is>
-          <t>Tracey</t>
+          <t>Bronwyn Anne</t>
         </is>
       </c>
       <c r="C79" s="3" t="inlineStr">
         <is>
-          <t>Kensington</t>
+          <t>Cowies Hill</t>
         </is>
       </c>
       <c r="D79" s="3" t="inlineStr">
@@ -10117,24 +10117,24 @@
       </c>
       <c r="E79" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="80" ht="25" customHeight="1">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>Polkinghorne</t>
+          <t>Pantoleon</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
         <is>
-          <t>Gavin</t>
+          <t>Teresa</t>
         </is>
       </c>
       <c r="C80" s="3" t="inlineStr">
         <is>
-          <t>Kensington</t>
+          <t>Vereeniging</t>
         </is>
       </c>
       <c r="D80" s="3" t="inlineStr">
@@ -10144,24 +10144,24 @@
       </c>
       <c r="E80" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="81" ht="25" customHeight="1">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>Ras</t>
+          <t>Polkinghorne</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
         <is>
-          <t>Leon Jacobus</t>
+          <t>Tracey</t>
         </is>
       </c>
       <c r="C81" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Kensington</t>
         </is>
       </c>
       <c r="D81" s="3" t="inlineStr">
@@ -10171,24 +10171,24 @@
       </c>
       <c r="E81" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="82" ht="25" customHeight="1">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>Reniers</t>
+          <t>Polkinghorne</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
         <is>
-          <t>Hugo</t>
+          <t>Gavin</t>
         </is>
       </c>
       <c r="C82" s="3" t="inlineStr">
         <is>
-          <t>Nelspruit</t>
+          <t>Kensington</t>
         </is>
       </c>
       <c r="D82" s="3" t="inlineStr">
@@ -10198,24 +10198,24 @@
       </c>
       <c r="E82" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="83" ht="25" customHeight="1">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>Sabatier</t>
+          <t>Ras</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
         <is>
-          <t>Rodney</t>
+          <t>Leon Jacobus</t>
         </is>
       </c>
       <c r="C83" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D83" s="3" t="inlineStr">
@@ -10225,24 +10225,24 @@
       </c>
       <c r="E83" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="84" ht="25" customHeight="1">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>Searle</t>
+          <t>Reniers</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
         <is>
-          <t>Francis</t>
+          <t>Hugo</t>
         </is>
       </c>
       <c r="C84" s="3" t="inlineStr">
         <is>
-          <t>Kouga</t>
+          <t>Nelspruit</t>
         </is>
       </c>
       <c r="D84" s="3" t="inlineStr">
@@ -10259,17 +10259,17 @@
     <row r="85" ht="25" customHeight="1">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>Searle</t>
+          <t>Sabatier</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
         <is>
-          <t>Gloria</t>
+          <t>Rodney</t>
         </is>
       </c>
       <c r="C85" s="3" t="inlineStr">
         <is>
-          <t>Kouga</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D85" s="3" t="inlineStr">
@@ -10279,24 +10279,24 @@
       </c>
       <c r="E85" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="86" ht="25" customHeight="1">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>Smit</t>
+          <t>Searle</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
         <is>
-          <t>Sue</t>
+          <t>Francis</t>
         </is>
       </c>
       <c r="C86" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Kouga</t>
         </is>
       </c>
       <c r="D86" s="3" t="inlineStr">
@@ -10313,17 +10313,17 @@
     <row r="87" ht="25" customHeight="1">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Searle</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
         <is>
-          <t>Jeff</t>
+          <t>Gloria</t>
         </is>
       </c>
       <c r="C87" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Kouga</t>
         </is>
       </c>
       <c r="D87" s="3" t="inlineStr">
@@ -10340,17 +10340,17 @@
     <row r="88" ht="25" customHeight="1">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>Stander</t>
+          <t>Smit</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
         <is>
-          <t>Max</t>
+          <t>Sue</t>
         </is>
       </c>
       <c r="C88" s="3" t="inlineStr">
         <is>
-          <t>Port Alfred</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D88" s="3" t="inlineStr">
@@ -10367,17 +10367,17 @@
     <row r="89" ht="25" customHeight="1">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>Stander</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
         <is>
-          <t>Ashley</t>
+          <t>Jeff</t>
         </is>
       </c>
       <c r="C89" s="3" t="inlineStr">
         <is>
-          <t>Krugersdorp</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D89" s="3" t="inlineStr">
@@ -10387,7 +10387,7 @@
       </c>
       <c r="E89" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -10399,12 +10399,12 @@
       </c>
       <c r="B90" s="3" t="inlineStr">
         <is>
-          <t>Brett Jason</t>
+          <t>Max</t>
         </is>
       </c>
       <c r="C90" s="3" t="inlineStr">
         <is>
-          <t>Krugersdorp</t>
+          <t>Port Alfred</t>
         </is>
       </c>
       <c r="D90" s="3" t="inlineStr">
@@ -10414,51 +10414,51 @@
       </c>
       <c r="E90" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="91" ht="25" customHeight="1">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>Steyn</t>
+          <t>Stander</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
         <is>
-          <t>Elna</t>
+          <t>Ashley</t>
         </is>
       </c>
       <c r="C91" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Krugersdorp</t>
         </is>
       </c>
       <c r="D91" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E91" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="92" ht="25" customHeight="1">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>Sturges</t>
+          <t>Stander</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
         <is>
-          <t>Trevor</t>
+          <t>Brett Jason</t>
         </is>
       </c>
       <c r="C92" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Krugersdorp</t>
         </is>
       </c>
       <c r="D92" s="3" t="inlineStr">
@@ -10475,22 +10475,22 @@
     <row r="93" ht="25" customHeight="1">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>Talbot</t>
+          <t>Steyn</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
         <is>
-          <t>Lauryn</t>
+          <t>Elna</t>
         </is>
       </c>
       <c r="C93" s="3" t="inlineStr">
         <is>
-          <t>Benoni Lakes</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D93" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E93" s="3" t="inlineStr">
@@ -10502,12 +10502,12 @@
     <row r="94" ht="25" customHeight="1">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>Theron</t>
+          <t>Sturges</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
         <is>
-          <t>Pierre</t>
+          <t>Trevor</t>
         </is>
       </c>
       <c r="C94" s="3" t="inlineStr">
@@ -10529,17 +10529,17 @@
     <row r="95" ht="25" customHeight="1">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>Theron</t>
+          <t>Talbot</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
         <is>
-          <t>Moira</t>
+          <t>Lauryn</t>
         </is>
       </c>
       <c r="C95" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Benoni Lakes</t>
         </is>
       </c>
       <c r="D95" s="3" t="inlineStr">
@@ -10556,17 +10556,17 @@
     <row r="96" ht="25" customHeight="1">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>Townsend</t>
+          <t>Theron</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
         <is>
-          <t>Diane</t>
+          <t>Pierre</t>
         </is>
       </c>
       <c r="C96" s="3" t="inlineStr">
         <is>
-          <t>Benoni Lakes</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D96" s="3" t="inlineStr">
@@ -10583,22 +10583,22 @@
     <row r="97" ht="25" customHeight="1">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>Toye</t>
+          <t>Theron</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
         <is>
-          <t>Omolayo</t>
+          <t>Moira</t>
         </is>
       </c>
       <c r="C97" s="3" t="inlineStr">
         <is>
-          <t>The Wilds</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D97" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E97" s="3" t="inlineStr">
@@ -10610,17 +10610,17 @@
     <row r="98" ht="25" customHeight="1">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>Tuckett</t>
+          <t>Townsend</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
         <is>
-          <t>Alistair</t>
+          <t>Diane</t>
         </is>
       </c>
       <c r="C98" s="3" t="inlineStr">
         <is>
-          <t>Roodepoort Clearwater Cyber</t>
+          <t>Benoni Lakes</t>
         </is>
       </c>
       <c r="D98" s="3" t="inlineStr">
@@ -10637,27 +10637,27 @@
     <row r="99" ht="25" customHeight="1">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>Tuckett</t>
+          <t>Toye</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
         <is>
-          <t>Rowan</t>
+          <t>Omolayo</t>
         </is>
       </c>
       <c r="C99" s="3" t="inlineStr">
         <is>
-          <t>Roodepoort Clearwater Cyber</t>
+          <t>The Wilds</t>
         </is>
       </c>
       <c r="D99" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E99" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -10669,7 +10669,7 @@
       </c>
       <c r="B100" s="3" t="inlineStr">
         <is>
-          <t>Gail</t>
+          <t>Alistair</t>
         </is>
       </c>
       <c r="C100" s="3" t="inlineStr">
@@ -10691,71 +10691,71 @@
     <row r="101" ht="25" customHeight="1">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>Uchytil</t>
+          <t>Tuckett</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
         <is>
-          <t>Jiri</t>
+          <t>Rowan</t>
         </is>
       </c>
       <c r="C101" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Roodepoort Clearwater Cyber</t>
         </is>
       </c>
       <c r="D101" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E101" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="102" ht="25" customHeight="1">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>VAN DER MERWE</t>
+          <t>Tuckett</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
         <is>
-          <t>PATRICIA</t>
+          <t>Gail</t>
         </is>
       </c>
       <c r="C102" s="3" t="inlineStr">
         <is>
-          <t>East London Port Rex</t>
+          <t>Roodepoort Clearwater Cyber</t>
         </is>
       </c>
       <c r="D102" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E102" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="103" ht="25" customHeight="1">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>Van Niekerk</t>
+          <t>Uchytil</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
         <is>
-          <t>Riaan</t>
+          <t>Jiri</t>
         </is>
       </c>
       <c r="C103" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D103" s="3" t="inlineStr">
@@ -10772,44 +10772,44 @@
     <row r="104" ht="25" customHeight="1">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>Van Nieuwenhuyzen</t>
+          <t>VAN DER MERWE</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
         <is>
-          <t>Hilgardt</t>
+          <t>PATRICIA</t>
         </is>
       </c>
       <c r="C104" s="3" t="inlineStr">
         <is>
-          <t>Worcester</t>
+          <t>East London Port Rex</t>
         </is>
       </c>
       <c r="D104" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E104" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="105" ht="25" customHeight="1">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>Venter</t>
+          <t>Van Niekerk</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
         <is>
-          <t>Louis</t>
+          <t>Riaan</t>
         </is>
       </c>
       <c r="C105" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D105" s="3" t="inlineStr">
@@ -10819,24 +10819,24 @@
       </c>
       <c r="E105" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="106" ht="25" customHeight="1">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>Volker</t>
+          <t>Van Nieuwenhuyzen</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
         <is>
-          <t>Russell</t>
+          <t>Hilgardt</t>
         </is>
       </c>
       <c r="C106" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Worcester</t>
         </is>
       </c>
       <c r="D106" s="3" t="inlineStr">
@@ -10846,29 +10846,29 @@
       </c>
       <c r="E106" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="107" ht="25" customHeight="1">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>Warman</t>
+          <t>Venter</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
         <is>
-          <t>Alastair</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="C107" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D107" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E107" s="3" t="inlineStr">
@@ -10880,17 +10880,17 @@
     <row r="108" ht="25" customHeight="1">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>Williamson</t>
+          <t>Volker</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
         <is>
-          <t>Neville</t>
+          <t>Russell</t>
         </is>
       </c>
       <c r="C108" s="3" t="inlineStr">
         <is>
-          <t>Port Alfred</t>
+          <t>King William's Town</t>
         </is>
       </c>
       <c r="D108" s="3" t="inlineStr">
@@ -10900,24 +10900,24 @@
       </c>
       <c r="E108" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="109" ht="25" customHeight="1">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>Wilter-Sturges</t>
+          <t>Warman</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
         <is>
-          <t>Meredith</t>
+          <t>Alastair</t>
         </is>
       </c>
       <c r="C109" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D109" s="3" t="inlineStr">
@@ -10927,29 +10927,29 @@
       </c>
       <c r="E109" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="110" ht="25" customHeight="1">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>de Silva</t>
+          <t>Williamson</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Neville</t>
         </is>
       </c>
       <c r="C110" s="3" t="inlineStr">
         <is>
-          <t>Edenvale</t>
+          <t>Port Alfred</t>
         </is>
       </c>
       <c r="D110" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E110" s="3" t="inlineStr">
@@ -10961,17 +10961,17 @@
     <row r="111" ht="25" customHeight="1">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>du Plooy</t>
+          <t>Wilter-Sturges</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
         <is>
-          <t>Tammy</t>
+          <t>Meredith</t>
         </is>
       </c>
       <c r="C111" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D111" s="3" t="inlineStr">
@@ -10981,51 +10981,51 @@
       </c>
       <c r="E111" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="112" ht="25" customHeight="1">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>du Plooy</t>
+          <t>de Silva</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
         <is>
-          <t>Marc</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="C112" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Edenvale</t>
         </is>
       </c>
       <c r="D112" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E112" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="113" ht="25" customHeight="1">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>du Toit</t>
+          <t>du Plooy</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
         <is>
-          <t>Desiree</t>
+          <t>Tammy</t>
         </is>
       </c>
       <c r="C113" s="3" t="inlineStr">
         <is>
-          <t>Ramsgate</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D113" s="3" t="inlineStr">
@@ -11035,24 +11035,24 @@
       </c>
       <c r="E113" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="114" ht="25" customHeight="1">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>le Roux</t>
+          <t>du Plooy</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
         <is>
-          <t>Jeanette</t>
+          <t>Marc</t>
         </is>
       </c>
       <c r="C114" s="3" t="inlineStr">
         <is>
-          <t>Gonubie</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D114" s="3" t="inlineStr">
@@ -11062,24 +11062,24 @@
       </c>
       <c r="E114" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="115" ht="25" customHeight="1">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>van Heerden</t>
+          <t>du Toit</t>
         </is>
       </c>
       <c r="B115" s="3" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Desiree</t>
         </is>
       </c>
       <c r="C115" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Ramsgate</t>
         </is>
       </c>
       <c r="D115" s="3" t="inlineStr">
@@ -11096,17 +11096,17 @@
     <row r="116" ht="25" customHeight="1">
       <c r="A116" s="3" t="inlineStr">
         <is>
-          <t>van Heerden</t>
+          <t>le Roux</t>
         </is>
       </c>
       <c r="B116" s="3" t="inlineStr">
         <is>
-          <t>Sandy</t>
+          <t>Jeanette</t>
         </is>
       </c>
       <c r="C116" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Gonubie</t>
         </is>
       </c>
       <c r="D116" s="3" t="inlineStr">
@@ -11116,7 +11116,7 @@
       </c>
       <c r="E116" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -11128,12 +11128,12 @@
       </c>
       <c r="B117" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Sydney</t>
         </is>
       </c>
       <c r="C117" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D117" s="3" t="inlineStr">
@@ -11143,24 +11143,24 @@
       </c>
       <c r="E117" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="118" ht="25" customHeight="1">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>van Wyk</t>
+          <t>van Heerden</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>Sandy</t>
         </is>
       </c>
       <c r="C118" s="3" t="inlineStr">
         <is>
-          <t>North Durban</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D118" s="3" t="inlineStr">
@@ -11170,24 +11170,24 @@
       </c>
       <c r="E118" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="119" ht="25" customHeight="1">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>van Wyk</t>
+          <t>van Heerden</t>
         </is>
       </c>
       <c r="B119" s="3" t="inlineStr">
         <is>
-          <t>Lindie</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C119" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D119" s="3" t="inlineStr">
@@ -11197,7 +11197,7 @@
       </c>
       <c r="E119" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -11209,12 +11209,12 @@
       </c>
       <c r="B120" s="3" t="inlineStr">
         <is>
-          <t>Willem</t>
+          <t>Kim</t>
         </is>
       </c>
       <c r="C120" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>North Durban</t>
         </is>
       </c>
       <c r="D120" s="3" t="inlineStr">
@@ -11236,7 +11236,7 @@
       </c>
       <c r="B121" s="3" t="inlineStr">
         <is>
-          <t>Patricia</t>
+          <t>Lindie</t>
         </is>
       </c>
       <c r="C121" s="3" t="inlineStr">
@@ -11258,44 +11258,44 @@
     <row r="122" ht="25" customHeight="1">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>van der Merwe</t>
+          <t>van Wyk</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
         <is>
-          <t>Ingrid</t>
+          <t>Willem</t>
         </is>
       </c>
       <c r="C122" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D122" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E122" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="123" ht="25" customHeight="1">
       <c r="A123" s="3" t="inlineStr">
         <is>
-          <t>von der Decken</t>
+          <t>van Wyk</t>
         </is>
       </c>
       <c r="B123" s="3" t="inlineStr">
         <is>
-          <t>Brian</t>
+          <t>Patricia</t>
         </is>
       </c>
       <c r="C123" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D123" s="3" t="inlineStr">
@@ -11305,46 +11305,100 @@
       </c>
       <c r="E123" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="124" ht="25" customHeight="1">
       <c r="A124" s="3" t="inlineStr">
         <is>
+          <t>van der Merwe</t>
+        </is>
+      </c>
+      <c r="B124" s="3" t="inlineStr">
+        <is>
+          <t>Ingrid</t>
+        </is>
+      </c>
+      <c r="C124" s="3" t="inlineStr">
+        <is>
+          <t>Letaba Tzaneen</t>
+        </is>
+      </c>
+      <c r="D124" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="E124" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="125" ht="25" customHeight="1">
+      <c r="A125" s="3" t="inlineStr">
+        <is>
+          <t>von der Decken</t>
+        </is>
+      </c>
+      <c r="B125" s="3" t="inlineStr">
+        <is>
+          <t>Brian</t>
+        </is>
+      </c>
+      <c r="C125" s="3" t="inlineStr">
+        <is>
+          <t>King William's Town</t>
+        </is>
+      </c>
+      <c r="D125" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E125" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="126" ht="25" customHeight="1">
+      <c r="A126" s="3" t="inlineStr">
+        <is>
           <t>‘t Hart</t>
         </is>
       </c>
-      <c r="B124" s="3" t="inlineStr">
+      <c r="B126" s="3" t="inlineStr">
         <is>
           <t>Michelle</t>
         </is>
       </c>
-      <c r="C124" s="3" t="inlineStr">
+      <c r="C126" s="3" t="inlineStr">
         <is>
           <t>Benoni Lakes</t>
         </is>
       </c>
-      <c r="D124" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E124" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" s="1" t="inlineStr">
-        <is>
-          <t>Number of attendees: 122</t>
-        </is>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" s="1" t="inlineStr">
+      <c r="D126" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E126" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="inlineStr">
+        <is>
+          <t>Number of attendees: 124</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="1" t="inlineStr">
         <is>
           <t>Number of voters: 59</t>
         </is>
@@ -11380,7 +11434,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Registrees as of 20/04/2021 19:04</t>
+          <t>410W Registrees as of 20/04/2021 20:45</t>
         </is>
       </c>
     </row>
@@ -15448,7 +15502,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Voting details as of 20/04/2021 19:04</t>
+          <t>410E Voting details as of 20/04/2021 20:45</t>
         </is>
       </c>
     </row>
@@ -15775,7 +15829,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Voting details as of 20/04/2021 19:04</t>
+          <t>410W Voting details as of 20/04/2021 20:45</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Registree stats backup on Wed 21 Apr 2021 09:02:06 SAST
</commit_message>
<xml_diff>
--- a/static/docs/registrees_list.xlsx
+++ b/static/docs/registrees_list.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F238"/>
+  <dimension ref="A1:F239"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,7 +451,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>MD410 Registrees as of 20/04/2021 20:45</t>
+          <t>MD410 Registrees as of 21/04/2021 09:02</t>
         </is>
       </c>
     </row>
@@ -1174,7 +1174,7 @@
       </c>
       <c r="E24" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F24" s="3" t="inlineStr">
@@ -5378,27 +5378,27 @@
     <row r="156" ht="25" customHeight="1">
       <c r="A156" s="3" t="inlineStr">
         <is>
-          <t>Reniers</t>
+          <t>Rashirai</t>
         </is>
       </c>
       <c r="B156" s="3" t="inlineStr">
         <is>
-          <t>Hugo</t>
+          <t>Tabeth</t>
         </is>
       </c>
       <c r="C156" s="3" t="inlineStr">
         <is>
-          <t>Nelspruit</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D156" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E156" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F156" s="3" t="inlineStr">
@@ -5410,17 +5410,17 @@
     <row r="157" ht="25" customHeight="1">
       <c r="A157" s="3" t="inlineStr">
         <is>
-          <t>Roman</t>
+          <t>Reniers</t>
         </is>
       </c>
       <c r="B157" s="3" t="inlineStr">
         <is>
-          <t>Sandy</t>
+          <t>Hugo</t>
         </is>
       </c>
       <c r="C157" s="3" t="inlineStr">
         <is>
-          <t>Bergvliet</t>
+          <t>Nelspruit</t>
         </is>
       </c>
       <c r="D157" s="3" t="inlineStr">
@@ -5430,29 +5430,29 @@
       </c>
       <c r="E157" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F157" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="158" ht="25" customHeight="1">
       <c r="A158" s="3" t="inlineStr">
         <is>
-          <t>Rossouw</t>
+          <t>Roman</t>
         </is>
       </c>
       <c r="B158" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Sandy</t>
         </is>
       </c>
       <c r="C158" s="3" t="inlineStr">
         <is>
-          <t>Tokai</t>
+          <t>Bergvliet</t>
         </is>
       </c>
       <c r="D158" s="3" t="inlineStr">
@@ -5462,7 +5462,7 @@
       </c>
       <c r="E158" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F158" s="3" t="inlineStr">
@@ -5474,17 +5474,17 @@
     <row r="159" ht="25" customHeight="1">
       <c r="A159" s="3" t="inlineStr">
         <is>
-          <t>Rothner</t>
+          <t>Rossouw</t>
         </is>
       </c>
       <c r="B159" s="3" t="inlineStr">
         <is>
-          <t>Andrea</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C159" s="3" t="inlineStr">
         <is>
-          <t>Eden</t>
+          <t>Tokai</t>
         </is>
       </c>
       <c r="D159" s="3" t="inlineStr">
@@ -5494,7 +5494,7 @@
       </c>
       <c r="E159" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F159" s="3" t="inlineStr">
@@ -5506,17 +5506,17 @@
     <row r="160" ht="25" customHeight="1">
       <c r="A160" s="3" t="inlineStr">
         <is>
-          <t>Roux</t>
+          <t>Rothner</t>
         </is>
       </c>
       <c r="B160" s="3" t="inlineStr">
         <is>
-          <t>Anthonie Petrus</t>
+          <t>Andrea</t>
         </is>
       </c>
       <c r="C160" s="3" t="inlineStr">
         <is>
-          <t>Moorreesburg</t>
+          <t>Eden</t>
         </is>
       </c>
       <c r="D160" s="3" t="inlineStr">
@@ -5526,7 +5526,7 @@
       </c>
       <c r="E160" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F160" s="3" t="inlineStr">
@@ -5538,17 +5538,17 @@
     <row r="161" ht="25" customHeight="1">
       <c r="A161" s="3" t="inlineStr">
         <is>
-          <t>Russell</t>
+          <t>Roux</t>
         </is>
       </c>
       <c r="B161" s="3" t="inlineStr">
         <is>
-          <t>Ingrid</t>
+          <t>Anthonie Petrus</t>
         </is>
       </c>
       <c r="C161" s="3" t="inlineStr">
         <is>
-          <t>Fish Hoek</t>
+          <t>Moorreesburg</t>
         </is>
       </c>
       <c r="D161" s="3" t="inlineStr">
@@ -5570,27 +5570,27 @@
     <row r="162" ht="25" customHeight="1">
       <c r="A162" s="3" t="inlineStr">
         <is>
-          <t>SNYMAN</t>
+          <t>Russell</t>
         </is>
       </c>
       <c r="B162" s="3" t="inlineStr">
         <is>
-          <t>LYN</t>
+          <t>Ingrid</t>
         </is>
       </c>
       <c r="C162" s="3" t="inlineStr">
         <is>
-          <t>Deep South</t>
+          <t>Fish Hoek</t>
         </is>
       </c>
       <c r="D162" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E162" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F162" s="3" t="inlineStr">
@@ -5602,27 +5602,27 @@
     <row r="163" ht="25" customHeight="1">
       <c r="A163" s="3" t="inlineStr">
         <is>
-          <t>STEENBERG</t>
+          <t>SNYMAN</t>
         </is>
       </c>
       <c r="B163" s="3" t="inlineStr">
         <is>
-          <t>TIM</t>
+          <t>LYN</t>
         </is>
       </c>
       <c r="C163" s="3" t="inlineStr">
         <is>
-          <t>Wellington</t>
+          <t>Deep South</t>
         </is>
       </c>
       <c r="D163" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E163" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F163" s="3" t="inlineStr">
@@ -5634,17 +5634,17 @@
     <row r="164" ht="25" customHeight="1">
       <c r="A164" s="3" t="inlineStr">
         <is>
-          <t>Sabatier</t>
+          <t>STEENBERG</t>
         </is>
       </c>
       <c r="B164" s="3" t="inlineStr">
         <is>
-          <t>Rodney</t>
+          <t>TIM</t>
         </is>
       </c>
       <c r="C164" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Wellington</t>
         </is>
       </c>
       <c r="D164" s="3" t="inlineStr">
@@ -5659,24 +5659,24 @@
       </c>
       <c r="F164" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="165" ht="25" customHeight="1">
       <c r="A165" s="3" t="inlineStr">
         <is>
-          <t>Sampie</t>
+          <t>Sabatier</t>
         </is>
       </c>
       <c r="B165" s="3" t="inlineStr">
         <is>
-          <t>Sharon</t>
+          <t>Rodney</t>
         </is>
       </c>
       <c r="C165" s="3" t="inlineStr">
         <is>
-          <t>Bergvliet</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D165" s="3" t="inlineStr">
@@ -5691,24 +5691,24 @@
       </c>
       <c r="F165" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="166" ht="25" customHeight="1">
       <c r="A166" s="3" t="inlineStr">
         <is>
-          <t>Schatz</t>
+          <t>Sampie</t>
         </is>
       </c>
       <c r="B166" s="3" t="inlineStr">
         <is>
-          <t>Vera</t>
+          <t>Sharon</t>
         </is>
       </c>
       <c r="C166" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Bergvliet</t>
         </is>
       </c>
       <c r="D166" s="3" t="inlineStr">
@@ -5718,7 +5718,7 @@
       </c>
       <c r="E166" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F166" s="3" t="inlineStr">
@@ -5735,7 +5735,7 @@
       </c>
       <c r="B167" s="3" t="inlineStr">
         <is>
-          <t>Frank</t>
+          <t>Vera</t>
         </is>
       </c>
       <c r="C167" s="3" t="inlineStr">
@@ -5750,7 +5750,7 @@
       </c>
       <c r="E167" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F167" s="3" t="inlineStr">
@@ -5762,17 +5762,17 @@
     <row r="168" ht="25" customHeight="1">
       <c r="A168" s="3" t="inlineStr">
         <is>
-          <t>Searle</t>
+          <t>Schatz</t>
         </is>
       </c>
       <c r="B168" s="3" t="inlineStr">
         <is>
-          <t>Francis</t>
+          <t>Frank</t>
         </is>
       </c>
       <c r="C168" s="3" t="inlineStr">
         <is>
-          <t>Kouga</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D168" s="3" t="inlineStr">
@@ -5787,7 +5787,7 @@
       </c>
       <c r="F168" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -5799,7 +5799,7 @@
       </c>
       <c r="B169" s="3" t="inlineStr">
         <is>
-          <t>Gloria</t>
+          <t>Francis</t>
         </is>
       </c>
       <c r="C169" s="3" t="inlineStr">
@@ -5814,7 +5814,7 @@
       </c>
       <c r="E169" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F169" s="3" t="inlineStr">
@@ -5826,17 +5826,17 @@
     <row r="170" ht="25" customHeight="1">
       <c r="A170" s="3" t="inlineStr">
         <is>
-          <t>Sell</t>
+          <t>Searle</t>
         </is>
       </c>
       <c r="B170" s="3" t="inlineStr">
         <is>
-          <t>Ami</t>
+          <t>Gloria</t>
         </is>
       </c>
       <c r="C170" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Kouga</t>
         </is>
       </c>
       <c r="D170" s="3" t="inlineStr">
@@ -5851,24 +5851,24 @@
       </c>
       <c r="F170" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="171" ht="25" customHeight="1">
       <c r="A171" s="3" t="inlineStr">
         <is>
-          <t>Simpson</t>
+          <t>Sell</t>
         </is>
       </c>
       <c r="B171" s="3" t="inlineStr">
         <is>
-          <t>Beryl</t>
+          <t>Ami</t>
         </is>
       </c>
       <c r="C171" s="3" t="inlineStr">
         <is>
-          <t>Cape Town</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D171" s="3" t="inlineStr">
@@ -5890,17 +5890,17 @@
     <row r="172" ht="25" customHeight="1">
       <c r="A172" s="3" t="inlineStr">
         <is>
-          <t>Sircoulomb</t>
+          <t>Simpson</t>
         </is>
       </c>
       <c r="B172" s="3" t="inlineStr">
         <is>
-          <t>Kenlis</t>
+          <t>Beryl</t>
         </is>
       </c>
       <c r="C172" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Cape Town</t>
         </is>
       </c>
       <c r="D172" s="3" t="inlineStr">
@@ -5927,7 +5927,7 @@
       </c>
       <c r="B173" s="3" t="inlineStr">
         <is>
-          <t>Holger</t>
+          <t>Kenlis</t>
         </is>
       </c>
       <c r="C173" s="3" t="inlineStr">
@@ -5942,7 +5942,7 @@
       </c>
       <c r="E173" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F173" s="3" t="inlineStr">
@@ -5954,12 +5954,12 @@
     <row r="174" ht="25" customHeight="1">
       <c r="A174" s="3" t="inlineStr">
         <is>
-          <t>Smeer</t>
+          <t>Sircoulomb</t>
         </is>
       </c>
       <c r="B174" s="3" t="inlineStr">
         <is>
-          <t>Hennie</t>
+          <t>Holger</t>
         </is>
       </c>
       <c r="C174" s="3" t="inlineStr">
@@ -5969,12 +5969,12 @@
       </c>
       <c r="D174" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E174" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F174" s="3" t="inlineStr">
@@ -5986,32 +5986,32 @@
     <row r="175" ht="25" customHeight="1">
       <c r="A175" s="3" t="inlineStr">
         <is>
-          <t>Smit</t>
+          <t>Smeer</t>
         </is>
       </c>
       <c r="B175" s="3" t="inlineStr">
         <is>
-          <t>Sue</t>
+          <t>Hennie</t>
         </is>
       </c>
       <c r="C175" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D175" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E175" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F175" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -6023,12 +6023,12 @@
       </c>
       <c r="B176" s="3" t="inlineStr">
         <is>
-          <t>Herman</t>
+          <t>Sue</t>
         </is>
       </c>
       <c r="C176" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D176" s="3" t="inlineStr">
@@ -6038,29 +6038,29 @@
       </c>
       <c r="E176" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F176" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="177" ht="25" customHeight="1">
       <c r="A177" s="3" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Smit</t>
         </is>
       </c>
       <c r="B177" s="3" t="inlineStr">
         <is>
-          <t>Jeff</t>
+          <t>Herman</t>
         </is>
       </c>
       <c r="C177" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D177" s="3" t="inlineStr">
@@ -6075,7 +6075,7 @@
       </c>
       <c r="F177" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -6087,12 +6087,12 @@
       </c>
       <c r="B178" s="3" t="inlineStr">
         <is>
-          <t>Bennie</t>
+          <t>Jeff</t>
         </is>
       </c>
       <c r="C178" s="3" t="inlineStr">
         <is>
-          <t>Wellington</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D178" s="3" t="inlineStr">
@@ -6102,12 +6102,12 @@
       </c>
       <c r="E178" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F178" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -6119,12 +6119,12 @@
       </c>
       <c r="B179" s="3" t="inlineStr">
         <is>
-          <t>Carmen Dolores</t>
+          <t>Bennie</t>
         </is>
       </c>
       <c r="C179" s="3" t="inlineStr">
         <is>
-          <t>Tokai</t>
+          <t>Wellington</t>
         </is>
       </c>
       <c r="D179" s="3" t="inlineStr">
@@ -6134,7 +6134,7 @@
       </c>
       <c r="E179" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F179" s="3" t="inlineStr">
@@ -6151,7 +6151,7 @@
       </c>
       <c r="B180" s="3" t="inlineStr">
         <is>
-          <t>David John</t>
+          <t>Carmen Dolores</t>
         </is>
       </c>
       <c r="C180" s="3" t="inlineStr">
@@ -6178,17 +6178,17 @@
     <row r="181" ht="25" customHeight="1">
       <c r="A181" s="3" t="inlineStr">
         <is>
-          <t>Sochen</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="B181" s="3" t="inlineStr">
         <is>
-          <t>Diana</t>
+          <t>David John</t>
         </is>
       </c>
       <c r="C181" s="3" t="inlineStr">
         <is>
-          <t>Sea Point</t>
+          <t>Tokai</t>
         </is>
       </c>
       <c r="D181" s="3" t="inlineStr">
@@ -6198,7 +6198,7 @@
       </c>
       <c r="E181" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F181" s="3" t="inlineStr">
@@ -6210,49 +6210,49 @@
     <row r="182" ht="25" customHeight="1">
       <c r="A182" s="3" t="inlineStr">
         <is>
-          <t>Steyn</t>
+          <t>Sochen</t>
         </is>
       </c>
       <c r="B182" s="3" t="inlineStr">
         <is>
-          <t>Elna</t>
+          <t>Diana</t>
         </is>
       </c>
       <c r="C182" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Sea Point</t>
         </is>
       </c>
       <c r="D182" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E182" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F182" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="183" ht="25" customHeight="1">
       <c r="A183" s="3" t="inlineStr">
         <is>
-          <t>Strauss</t>
+          <t>Steyn</t>
         </is>
       </c>
       <c r="B183" s="3" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>Elna</t>
         </is>
       </c>
       <c r="C183" s="3" t="inlineStr">
         <is>
-          <t>Kuilsriver</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D183" s="3" t="inlineStr">
@@ -6267,29 +6267,29 @@
       </c>
       <c r="F183" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="184" ht="25" customHeight="1">
       <c r="A184" s="3" t="inlineStr">
         <is>
-          <t>Strydom</t>
+          <t>Strauss</t>
         </is>
       </c>
       <c r="B184" s="3" t="inlineStr">
         <is>
-          <t>Melinda Lee</t>
+          <t>Patrick</t>
         </is>
       </c>
       <c r="C184" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Kuilsriver</t>
         </is>
       </c>
       <c r="D184" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E184" s="3" t="inlineStr">
@@ -6299,24 +6299,24 @@
       </c>
       <c r="F184" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="185" ht="25" customHeight="1">
       <c r="A185" s="3" t="inlineStr">
         <is>
-          <t>Sturges</t>
+          <t>Strydom</t>
         </is>
       </c>
       <c r="B185" s="3" t="inlineStr">
         <is>
-          <t>Trevor</t>
+          <t>Melinda Lee</t>
         </is>
       </c>
       <c r="C185" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D185" s="3" t="inlineStr">
@@ -6338,17 +6338,17 @@
     <row r="186" ht="25" customHeight="1">
       <c r="A186" s="3" t="inlineStr">
         <is>
-          <t>Talbot</t>
+          <t>Sturges</t>
         </is>
       </c>
       <c r="B186" s="3" t="inlineStr">
         <is>
-          <t>Lauryn</t>
+          <t>Trevor</t>
         </is>
       </c>
       <c r="C186" s="3" t="inlineStr">
         <is>
-          <t>Benoni Lakes</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D186" s="3" t="inlineStr">
@@ -6370,17 +6370,17 @@
     <row r="187" ht="25" customHeight="1">
       <c r="A187" s="3" t="inlineStr">
         <is>
-          <t>Theron</t>
+          <t>Talbot</t>
         </is>
       </c>
       <c r="B187" s="3" t="inlineStr">
         <is>
-          <t>Pierre</t>
+          <t>Lauryn</t>
         </is>
       </c>
       <c r="C187" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Benoni Lakes</t>
         </is>
       </c>
       <c r="D187" s="3" t="inlineStr">
@@ -6407,7 +6407,7 @@
       </c>
       <c r="B188" s="3" t="inlineStr">
         <is>
-          <t>Moira</t>
+          <t>Pierre</t>
         </is>
       </c>
       <c r="C188" s="3" t="inlineStr">
@@ -6434,22 +6434,22 @@
     <row r="189" ht="25" customHeight="1">
       <c r="A189" s="3" t="inlineStr">
         <is>
-          <t>Toye</t>
+          <t>Theron</t>
         </is>
       </c>
       <c r="B189" s="3" t="inlineStr">
         <is>
-          <t>Omolayo</t>
+          <t>Moira</t>
         </is>
       </c>
       <c r="C189" s="3" t="inlineStr">
         <is>
-          <t>The Wilds</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D189" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E189" s="3" t="inlineStr">
@@ -6466,22 +6466,22 @@
     <row r="190" ht="25" customHeight="1">
       <c r="A190" s="3" t="inlineStr">
         <is>
-          <t>Tshikala</t>
+          <t>Toye</t>
         </is>
       </c>
       <c r="B190" s="3" t="inlineStr">
         <is>
-          <t>David Alex</t>
+          <t>Omolayo</t>
         </is>
       </c>
       <c r="C190" s="3" t="inlineStr">
         <is>
-          <t>Athlone</t>
+          <t>The Wilds</t>
         </is>
       </c>
       <c r="D190" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E190" s="3" t="inlineStr">
@@ -6491,24 +6491,24 @@
       </c>
       <c r="F190" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="191" ht="25" customHeight="1">
       <c r="A191" s="3" t="inlineStr">
         <is>
-          <t>Tuckett</t>
+          <t>Tshikala</t>
         </is>
       </c>
       <c r="B191" s="3" t="inlineStr">
         <is>
-          <t>Alistair</t>
+          <t>David Alex</t>
         </is>
       </c>
       <c r="C191" s="3" t="inlineStr">
         <is>
-          <t>Roodepoort Clearwater Cyber</t>
+          <t>Athlone</t>
         </is>
       </c>
       <c r="D191" s="3" t="inlineStr">
@@ -6523,7 +6523,7 @@
       </c>
       <c r="F191" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -6535,7 +6535,7 @@
       </c>
       <c r="B192" s="3" t="inlineStr">
         <is>
-          <t>Rowan</t>
+          <t>Alistair</t>
         </is>
       </c>
       <c r="C192" s="3" t="inlineStr">
@@ -6550,7 +6550,7 @@
       </c>
       <c r="E192" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F192" s="3" t="inlineStr">
@@ -6567,7 +6567,7 @@
       </c>
       <c r="B193" s="3" t="inlineStr">
         <is>
-          <t>Gail</t>
+          <t>Rowan</t>
         </is>
       </c>
       <c r="C193" s="3" t="inlineStr">
@@ -6582,7 +6582,7 @@
       </c>
       <c r="E193" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F193" s="3" t="inlineStr">
@@ -6594,17 +6594,17 @@
     <row r="194" ht="25" customHeight="1">
       <c r="A194" s="3" t="inlineStr">
         <is>
-          <t>VAN BREDA</t>
+          <t>Tuckett</t>
         </is>
       </c>
       <c r="B194" s="3" t="inlineStr">
         <is>
-          <t>HILARY LISE</t>
+          <t>Gail</t>
         </is>
       </c>
       <c r="C194" s="3" t="inlineStr">
         <is>
-          <t>Cape Town</t>
+          <t>Roodepoort Clearwater Cyber</t>
         </is>
       </c>
       <c r="D194" s="3" t="inlineStr">
@@ -6619,39 +6619,39 @@
       </c>
       <c r="F194" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="195" ht="25" customHeight="1">
       <c r="A195" s="3" t="inlineStr">
         <is>
-          <t>VAN DER MERWE</t>
+          <t>VAN BREDA</t>
         </is>
       </c>
       <c r="B195" s="3" t="inlineStr">
         <is>
-          <t>PATRICIA</t>
+          <t>HILARY LISE</t>
         </is>
       </c>
       <c r="C195" s="3" t="inlineStr">
         <is>
-          <t>East London Port Rex</t>
+          <t>Cape Town</t>
         </is>
       </c>
       <c r="D195" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E195" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F195" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -6663,17 +6663,17 @@
       </c>
       <c r="B196" s="3" t="inlineStr">
         <is>
-          <t>MARINA</t>
+          <t>PATRICIA</t>
         </is>
       </c>
       <c r="C196" s="3" t="inlineStr">
         <is>
-          <t>Malmesbury</t>
+          <t>East London Port Rex</t>
         </is>
       </c>
       <c r="D196" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E196" s="3" t="inlineStr">
@@ -6683,56 +6683,56 @@
       </c>
       <c r="F196" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="197" ht="25" customHeight="1">
       <c r="A197" s="3" t="inlineStr">
         <is>
-          <t>Valadao</t>
+          <t>VAN DER MERWE</t>
         </is>
       </c>
       <c r="B197" s="3" t="inlineStr">
         <is>
-          <t>Tracy</t>
+          <t>MARINA</t>
         </is>
       </c>
       <c r="C197" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Malmesbury</t>
         </is>
       </c>
       <c r="D197" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E197" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F197" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="198" ht="25" customHeight="1">
       <c r="A198" s="3" t="inlineStr">
         <is>
-          <t>Van Niekerk</t>
+          <t>Valadao</t>
         </is>
       </c>
       <c r="B198" s="3" t="inlineStr">
         <is>
-          <t>Riaan</t>
+          <t>Tracy</t>
         </is>
       </c>
       <c r="C198" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D198" s="3" t="inlineStr">
@@ -6754,22 +6754,22 @@
     <row r="199" ht="25" customHeight="1">
       <c r="A199" s="3" t="inlineStr">
         <is>
-          <t>Van Nieuwenhuyzen</t>
+          <t>Van Niekerk</t>
         </is>
       </c>
       <c r="B199" s="3" t="inlineStr">
         <is>
-          <t>Hilgardt</t>
+          <t>Riaan</t>
         </is>
       </c>
       <c r="C199" s="3" t="inlineStr">
         <is>
-          <t>Worcester</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D199" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E199" s="3" t="inlineStr">
@@ -6786,17 +6786,17 @@
     <row r="200" ht="25" customHeight="1">
       <c r="A200" s="3" t="inlineStr">
         <is>
-          <t>Van Rensburg</t>
+          <t>Van Nieuwenhuyzen</t>
         </is>
       </c>
       <c r="B200" s="3" t="inlineStr">
         <is>
-          <t>Neville</t>
+          <t>Hilgardt</t>
         </is>
       </c>
       <c r="C200" s="3" t="inlineStr">
         <is>
-          <t>Moorreesburg</t>
+          <t>Worcester</t>
         </is>
       </c>
       <c r="D200" s="3" t="inlineStr">
@@ -6806,39 +6806,39 @@
       </c>
       <c r="E200" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F200" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="201" ht="25" customHeight="1">
       <c r="A201" s="3" t="inlineStr">
         <is>
-          <t>Van Romburgh</t>
+          <t>Van Rensburg</t>
         </is>
       </c>
       <c r="B201" s="3" t="inlineStr">
         <is>
-          <t>Lorna</t>
+          <t>Neville</t>
         </is>
       </c>
       <c r="C201" s="3" t="inlineStr">
         <is>
-          <t>Fish Hoek</t>
+          <t>Moorreesburg</t>
         </is>
       </c>
       <c r="D201" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E201" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F201" s="3" t="inlineStr">
@@ -6850,17 +6850,17 @@
     <row r="202" ht="25" customHeight="1">
       <c r="A202" s="3" t="inlineStr">
         <is>
-          <t>Van Wyk-Nelson</t>
+          <t>Van Romburgh</t>
         </is>
       </c>
       <c r="B202" s="3" t="inlineStr">
         <is>
-          <t>Edith</t>
+          <t>Lorna</t>
         </is>
       </c>
       <c r="C202" s="3" t="inlineStr">
         <is>
-          <t>Kuilsriver</t>
+          <t>Fish Hoek</t>
         </is>
       </c>
       <c r="D202" s="3" t="inlineStr">
@@ -6882,22 +6882,22 @@
     <row r="203" ht="25" customHeight="1">
       <c r="A203" s="3" t="inlineStr">
         <is>
-          <t>Van de Merwe</t>
+          <t>Van Wyk-Nelson</t>
         </is>
       </c>
       <c r="B203" s="3" t="inlineStr">
         <is>
-          <t>Marina</t>
+          <t>Edith</t>
         </is>
       </c>
       <c r="C203" s="3" t="inlineStr">
         <is>
-          <t>Malmesbury</t>
+          <t>Kuilsriver</t>
         </is>
       </c>
       <c r="D203" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E203" s="3" t="inlineStr">
@@ -6914,59 +6914,59 @@
     <row r="204" ht="25" customHeight="1">
       <c r="A204" s="3" t="inlineStr">
         <is>
-          <t>Venter</t>
+          <t>Van de Merwe</t>
         </is>
       </c>
       <c r="B204" s="3" t="inlineStr">
         <is>
-          <t>Louis</t>
+          <t>Marina</t>
         </is>
       </c>
       <c r="C204" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Malmesbury</t>
         </is>
       </c>
       <c r="D204" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E204" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F204" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="205" ht="25" customHeight="1">
       <c r="A205" s="3" t="inlineStr">
         <is>
-          <t>Volker</t>
+          <t>Venter</t>
         </is>
       </c>
       <c r="B205" s="3" t="inlineStr">
         <is>
-          <t>Russell</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="C205" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D205" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E205" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F205" s="3" t="inlineStr">
@@ -6978,96 +6978,96 @@
     <row r="206" ht="25" customHeight="1">
       <c r="A206" s="3" t="inlineStr">
         <is>
-          <t>Von Mollendorf</t>
+          <t>Volker</t>
         </is>
       </c>
       <c r="B206" s="3" t="inlineStr">
         <is>
-          <t>Rinette</t>
+          <t>Russell</t>
         </is>
       </c>
       <c r="C206" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>King William's Town</t>
         </is>
       </c>
       <c r="D206" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E206" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F206" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="207" ht="25" customHeight="1">
       <c r="A207" s="3" t="inlineStr">
         <is>
-          <t>Warman</t>
+          <t>Von Mollendorf</t>
         </is>
       </c>
       <c r="B207" s="3" t="inlineStr">
         <is>
-          <t>Alastair</t>
+          <t>Rinette</t>
         </is>
       </c>
       <c r="C207" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Durbanville</t>
         </is>
       </c>
       <c r="D207" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E207" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F207" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="208" ht="25" customHeight="1">
       <c r="A208" s="3" t="inlineStr">
         <is>
-          <t>Watson</t>
+          <t>Warman</t>
         </is>
       </c>
       <c r="B208" s="3" t="inlineStr">
         <is>
-          <t>Allan</t>
+          <t>Alastair</t>
         </is>
       </c>
       <c r="C208" s="3" t="inlineStr">
         <is>
-          <t>Sea Point</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D208" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E208" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F208" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -7079,22 +7079,22 @@
       </c>
       <c r="B209" s="3" t="inlineStr">
         <is>
-          <t>Alison</t>
+          <t>Allan</t>
         </is>
       </c>
       <c r="C209" s="3" t="inlineStr">
         <is>
-          <t>Sedgefield</t>
+          <t>Sea Point</t>
         </is>
       </c>
       <c r="D209" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E209" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F209" s="3" t="inlineStr">
@@ -7106,27 +7106,27 @@
     <row r="210" ht="25" customHeight="1">
       <c r="A210" s="3" t="inlineStr">
         <is>
-          <t>Williams</t>
+          <t>Watson</t>
         </is>
       </c>
       <c r="B210" s="3" t="inlineStr">
         <is>
-          <t>Johanna</t>
+          <t>Alison</t>
         </is>
       </c>
       <c r="C210" s="3" t="inlineStr">
         <is>
-          <t>Mitchells Plain</t>
+          <t>Sedgefield</t>
         </is>
       </c>
       <c r="D210" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E210" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F210" s="3" t="inlineStr">
@@ -7138,22 +7138,22 @@
     <row r="211" ht="25" customHeight="1">
       <c r="A211" s="3" t="inlineStr">
         <is>
-          <t>Wills</t>
+          <t>Williams</t>
         </is>
       </c>
       <c r="B211" s="3" t="inlineStr">
         <is>
-          <t>Geila</t>
+          <t>Johanna</t>
         </is>
       </c>
       <c r="C211" s="3" t="inlineStr">
         <is>
-          <t>Athlone</t>
+          <t>Mitchells Plain</t>
         </is>
       </c>
       <c r="D211" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E211" s="3" t="inlineStr">
@@ -7170,17 +7170,17 @@
     <row r="212" ht="25" customHeight="1">
       <c r="A212" s="3" t="inlineStr">
         <is>
-          <t>Wilter-Sturges</t>
+          <t>Wills</t>
         </is>
       </c>
       <c r="B212" s="3" t="inlineStr">
         <is>
-          <t>Meredith</t>
+          <t>Geila</t>
         </is>
       </c>
       <c r="C212" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Athlone</t>
         </is>
       </c>
       <c r="D212" s="3" t="inlineStr">
@@ -7195,24 +7195,24 @@
       </c>
       <c r="F212" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="213" ht="25" customHeight="1">
       <c r="A213" s="3" t="inlineStr">
         <is>
-          <t>Wright</t>
+          <t>Wilter-Sturges</t>
         </is>
       </c>
       <c r="B213" s="3" t="inlineStr">
         <is>
-          <t>Rocky</t>
+          <t>Meredith</t>
         </is>
       </c>
       <c r="C213" s="3" t="inlineStr">
         <is>
-          <t>Table View</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D213" s="3" t="inlineStr">
@@ -7222,29 +7222,29 @@
       </c>
       <c r="E213" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F213" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="214" ht="25" customHeight="1">
       <c r="A214" s="3" t="inlineStr">
         <is>
-          <t>Young</t>
+          <t>Wright</t>
         </is>
       </c>
       <c r="B214" s="3" t="inlineStr">
         <is>
-          <t>Judy</t>
+          <t>Rocky</t>
         </is>
       </c>
       <c r="C214" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>Table View</t>
         </is>
       </c>
       <c r="D214" s="3" t="inlineStr">
@@ -7254,7 +7254,7 @@
       </c>
       <c r="E214" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F214" s="3" t="inlineStr">
@@ -7266,17 +7266,17 @@
     <row r="215" ht="25" customHeight="1">
       <c r="A215" s="3" t="inlineStr">
         <is>
-          <t>de Kock</t>
+          <t>Young</t>
         </is>
       </c>
       <c r="B215" s="3" t="inlineStr">
         <is>
-          <t>Engela</t>
+          <t>Judy</t>
         </is>
       </c>
       <c r="C215" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Durbanville</t>
         </is>
       </c>
       <c r="D215" s="3" t="inlineStr">
@@ -7286,7 +7286,7 @@
       </c>
       <c r="E215" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F215" s="3" t="inlineStr">
@@ -7303,7 +7303,7 @@
       </c>
       <c r="B216" s="3" t="inlineStr">
         <is>
-          <t>Francois</t>
+          <t>Engela</t>
         </is>
       </c>
       <c r="C216" s="3" t="inlineStr">
@@ -7330,54 +7330,54 @@
     <row r="217" ht="25" customHeight="1">
       <c r="A217" s="3" t="inlineStr">
         <is>
-          <t>de Silva</t>
+          <t>de Kock</t>
         </is>
       </c>
       <c r="B217" s="3" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Francois</t>
         </is>
       </c>
       <c r="C217" s="3" t="inlineStr">
         <is>
-          <t>Edenvale</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D217" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E217" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F217" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="218" ht="25" customHeight="1">
       <c r="A218" s="3" t="inlineStr">
         <is>
-          <t>du Toit</t>
+          <t>de Silva</t>
         </is>
       </c>
       <c r="B218" s="3" t="inlineStr">
         <is>
-          <t>Desiree</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="C218" s="3" t="inlineStr">
         <is>
-          <t>Ramsgate</t>
+          <t>Edenvale</t>
         </is>
       </c>
       <c r="D218" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E218" s="3" t="inlineStr">
@@ -7394,22 +7394,22 @@
     <row r="219" ht="25" customHeight="1">
       <c r="A219" s="3" t="inlineStr">
         <is>
-          <t>stier</t>
+          <t>du Toit</t>
         </is>
       </c>
       <c r="B219" s="3" t="inlineStr">
         <is>
-          <t>RORY</t>
+          <t>Desiree</t>
         </is>
       </c>
       <c r="C219" s="3" t="inlineStr">
         <is>
-          <t>Deep South</t>
+          <t>Ramsgate</t>
         </is>
       </c>
       <c r="D219" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E219" s="3" t="inlineStr">
@@ -7419,34 +7419,34 @@
       </c>
       <c r="F219" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="220" ht="25" customHeight="1">
       <c r="A220" s="3" t="inlineStr">
         <is>
-          <t>van Blerk</t>
+          <t>stier</t>
         </is>
       </c>
       <c r="B220" s="3" t="inlineStr">
         <is>
-          <t>Carl</t>
+          <t>RORY</t>
         </is>
       </c>
       <c r="C220" s="3" t="inlineStr">
         <is>
-          <t>Eden</t>
+          <t>Deep South</t>
         </is>
       </c>
       <c r="D220" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E220" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F220" s="3" t="inlineStr">
@@ -7458,17 +7458,17 @@
     <row r="221" ht="25" customHeight="1">
       <c r="A221" s="3" t="inlineStr">
         <is>
-          <t>van Heerden</t>
+          <t>van Blerk</t>
         </is>
       </c>
       <c r="B221" s="3" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Carl</t>
         </is>
       </c>
       <c r="C221" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Eden</t>
         </is>
       </c>
       <c r="D221" s="3" t="inlineStr">
@@ -7483,7 +7483,7 @@
       </c>
       <c r="F221" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -7495,7 +7495,7 @@
       </c>
       <c r="B222" s="3" t="inlineStr">
         <is>
-          <t>Sandy</t>
+          <t>Sydney</t>
         </is>
       </c>
       <c r="C222" s="3" t="inlineStr">
@@ -7510,7 +7510,7 @@
       </c>
       <c r="E222" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F222" s="3" t="inlineStr">
@@ -7527,12 +7527,12 @@
       </c>
       <c r="B223" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Sandy</t>
         </is>
       </c>
       <c r="C223" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D223" s="3" t="inlineStr">
@@ -7554,17 +7554,17 @@
     <row r="224" ht="25" customHeight="1">
       <c r="A224" s="3" t="inlineStr">
         <is>
-          <t>van Rensburg</t>
+          <t>van Heerden</t>
         </is>
       </c>
       <c r="B224" s="3" t="inlineStr">
         <is>
-          <t>Johan</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C224" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D224" s="3" t="inlineStr">
@@ -7574,12 +7574,12 @@
       </c>
       <c r="E224" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F224" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -7591,7 +7591,7 @@
       </c>
       <c r="B225" s="3" t="inlineStr">
         <is>
-          <t>Anne</t>
+          <t>Johan</t>
         </is>
       </c>
       <c r="C225" s="3" t="inlineStr">
@@ -7618,17 +7618,17 @@
     <row r="226" ht="25" customHeight="1">
       <c r="A226" s="3" t="inlineStr">
         <is>
-          <t>van Wulven</t>
+          <t>van Rensburg</t>
         </is>
       </c>
       <c r="B226" s="3" t="inlineStr">
         <is>
-          <t>Jeannie</t>
+          <t>Anne</t>
         </is>
       </c>
       <c r="C226" s="3" t="inlineStr">
         <is>
-          <t>Tygerberg Hills</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D226" s="3" t="inlineStr">
@@ -7655,7 +7655,7 @@
       </c>
       <c r="B227" s="3" t="inlineStr">
         <is>
-          <t>Alan</t>
+          <t>Jeannie</t>
         </is>
       </c>
       <c r="C227" s="3" t="inlineStr">
@@ -7687,7 +7687,7 @@
       </c>
       <c r="B228" s="3" t="inlineStr">
         <is>
-          <t>Deon</t>
+          <t>Alan</t>
         </is>
       </c>
       <c r="C228" s="3" t="inlineStr">
@@ -7714,17 +7714,17 @@
     <row r="229" ht="25" customHeight="1">
       <c r="A229" s="3" t="inlineStr">
         <is>
-          <t>van Wyk</t>
+          <t>van Wulven</t>
         </is>
       </c>
       <c r="B229" s="3" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>Deon</t>
         </is>
       </c>
       <c r="C229" s="3" t="inlineStr">
         <is>
-          <t>North Durban</t>
+          <t>Tygerberg Hills</t>
         </is>
       </c>
       <c r="D229" s="3" t="inlineStr">
@@ -7739,7 +7739,7 @@
       </c>
       <c r="F229" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -7751,12 +7751,12 @@
       </c>
       <c r="B230" s="3" t="inlineStr">
         <is>
-          <t>Lindie</t>
+          <t>Kim</t>
         </is>
       </c>
       <c r="C230" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>North Durban</t>
         </is>
       </c>
       <c r="D230" s="3" t="inlineStr">
@@ -7783,12 +7783,12 @@
       </c>
       <c r="B231" s="3" t="inlineStr">
         <is>
-          <t>Willem</t>
+          <t>Lindie</t>
         </is>
       </c>
       <c r="C231" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D231" s="3" t="inlineStr">
@@ -7815,12 +7815,12 @@
       </c>
       <c r="B232" s="3" t="inlineStr">
         <is>
-          <t>Patricia</t>
+          <t>Willem</t>
         </is>
       </c>
       <c r="C232" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D232" s="3" t="inlineStr">
@@ -7842,27 +7842,27 @@
     <row r="233" ht="25" customHeight="1">
       <c r="A233" s="3" t="inlineStr">
         <is>
-          <t>van der Merwe</t>
+          <t>van Wyk</t>
         </is>
       </c>
       <c r="B233" s="3" t="inlineStr">
         <is>
-          <t>Ingrid</t>
+          <t>Patricia</t>
         </is>
       </c>
       <c r="C233" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D233" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E233" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F233" s="3" t="inlineStr">
@@ -7874,49 +7874,49 @@
     <row r="234" ht="25" customHeight="1">
       <c r="A234" s="3" t="inlineStr">
         <is>
-          <t>van der Westhuizen</t>
+          <t>van der Merwe</t>
         </is>
       </c>
       <c r="B234" s="3" t="inlineStr">
         <is>
-          <t>Hennie</t>
+          <t>Ingrid</t>
         </is>
       </c>
       <c r="C234" s="3" t="inlineStr">
         <is>
-          <t>Helderberg</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D234" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E234" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F234" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="235" ht="25" customHeight="1">
       <c r="A235" s="3" t="inlineStr">
         <is>
-          <t>von der Decken</t>
+          <t>van der Westhuizen</t>
         </is>
       </c>
       <c r="B235" s="3" t="inlineStr">
         <is>
-          <t>Brian</t>
+          <t>Hennie</t>
         </is>
       </c>
       <c r="C235" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Helderberg</t>
         </is>
       </c>
       <c r="D235" s="3" t="inlineStr">
@@ -7931,51 +7931,83 @@
       </c>
       <c r="F235" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="236" ht="25" customHeight="1">
       <c r="A236" s="3" t="inlineStr">
         <is>
+          <t>von der Decken</t>
+        </is>
+      </c>
+      <c r="B236" s="3" t="inlineStr">
+        <is>
+          <t>Brian</t>
+        </is>
+      </c>
+      <c r="C236" s="3" t="inlineStr">
+        <is>
+          <t>King William's Town</t>
+        </is>
+      </c>
+      <c r="D236" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E236" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F236" s="3" t="inlineStr">
+        <is>
+          <t>410E</t>
+        </is>
+      </c>
+    </row>
+    <row r="237" ht="25" customHeight="1">
+      <c r="A237" s="3" t="inlineStr">
+        <is>
           <t>‘t Hart</t>
         </is>
       </c>
-      <c r="B236" s="3" t="inlineStr">
+      <c r="B237" s="3" t="inlineStr">
         <is>
           <t>Michelle</t>
         </is>
       </c>
-      <c r="C236" s="3" t="inlineStr">
+      <c r="C237" s="3" t="inlineStr">
         <is>
           <t>Benoni Lakes</t>
         </is>
       </c>
-      <c r="D236" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E236" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F236" s="3" t="inlineStr">
+      <c r="D237" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E237" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F237" s="3" t="inlineStr">
         <is>
           <t>410E</t>
-        </is>
-      </c>
-    </row>
-    <row r="237">
-      <c r="A237" s="1" t="inlineStr">
-        <is>
-          <t>Number of attendees: 234</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="inlineStr">
+        <is>
+          <t>Number of attendees: 235</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" s="1" t="inlineStr">
         <is>
           <t>Number of voters: 102</t>
         </is>
@@ -7993,7 +8025,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E128"/>
+  <dimension ref="A1:E129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8011,7 +8043,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Registrees as of 20/04/2021 20:45</t>
+          <t>410E Registrees as of 21/04/2021 09:02</t>
         </is>
       </c>
     </row>
@@ -8308,7 +8340,7 @@
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -10232,44 +10264,44 @@
     <row r="84" ht="25" customHeight="1">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>Reniers</t>
+          <t>Rashirai</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
         <is>
-          <t>Hugo</t>
+          <t>Tabeth</t>
         </is>
       </c>
       <c r="C84" s="3" t="inlineStr">
         <is>
-          <t>Nelspruit</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D84" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E84" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="85" ht="25" customHeight="1">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>Sabatier</t>
+          <t>Reniers</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
         <is>
-          <t>Rodney</t>
+          <t>Hugo</t>
         </is>
       </c>
       <c r="C85" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Nelspruit</t>
         </is>
       </c>
       <c r="D85" s="3" t="inlineStr">
@@ -10286,17 +10318,17 @@
     <row r="86" ht="25" customHeight="1">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>Searle</t>
+          <t>Sabatier</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
         <is>
-          <t>Francis</t>
+          <t>Rodney</t>
         </is>
       </c>
       <c r="C86" s="3" t="inlineStr">
         <is>
-          <t>Kouga</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D86" s="3" t="inlineStr">
@@ -10318,7 +10350,7 @@
       </c>
       <c r="B87" s="3" t="inlineStr">
         <is>
-          <t>Gloria</t>
+          <t>Francis</t>
         </is>
       </c>
       <c r="C87" s="3" t="inlineStr">
@@ -10333,24 +10365,24 @@
       </c>
       <c r="E87" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="88" ht="25" customHeight="1">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>Smit</t>
+          <t>Searle</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
         <is>
-          <t>Sue</t>
+          <t>Gloria</t>
         </is>
       </c>
       <c r="C88" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Kouga</t>
         </is>
       </c>
       <c r="D88" s="3" t="inlineStr">
@@ -10360,24 +10392,24 @@
       </c>
       <c r="E88" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="89" ht="25" customHeight="1">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Smit</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
         <is>
-          <t>Jeff</t>
+          <t>Sue</t>
         </is>
       </c>
       <c r="C89" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D89" s="3" t="inlineStr">
@@ -10387,24 +10419,24 @@
       </c>
       <c r="E89" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="90" ht="25" customHeight="1">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>Stander</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
         <is>
-          <t>Max</t>
+          <t>Jeff</t>
         </is>
       </c>
       <c r="C90" s="3" t="inlineStr">
         <is>
-          <t>Port Alfred</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D90" s="3" t="inlineStr">
@@ -10414,7 +10446,7 @@
       </c>
       <c r="E90" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -10426,12 +10458,12 @@
       </c>
       <c r="B91" s="3" t="inlineStr">
         <is>
-          <t>Ashley</t>
+          <t>Max</t>
         </is>
       </c>
       <c r="C91" s="3" t="inlineStr">
         <is>
-          <t>Krugersdorp</t>
+          <t>Port Alfred</t>
         </is>
       </c>
       <c r="D91" s="3" t="inlineStr">
@@ -10453,7 +10485,7 @@
       </c>
       <c r="B92" s="3" t="inlineStr">
         <is>
-          <t>Brett Jason</t>
+          <t>Ashley</t>
         </is>
       </c>
       <c r="C92" s="3" t="inlineStr">
@@ -10468,29 +10500,29 @@
       </c>
       <c r="E92" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="93" ht="25" customHeight="1">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>Steyn</t>
+          <t>Stander</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
         <is>
-          <t>Elna</t>
+          <t>Brett Jason</t>
         </is>
       </c>
       <c r="C93" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Krugersdorp</t>
         </is>
       </c>
       <c r="D93" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E93" s="3" t="inlineStr">
@@ -10502,22 +10534,22 @@
     <row r="94" ht="25" customHeight="1">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>Sturges</t>
+          <t>Steyn</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
         <is>
-          <t>Trevor</t>
+          <t>Elna</t>
         </is>
       </c>
       <c r="C94" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D94" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E94" s="3" t="inlineStr">
@@ -10529,17 +10561,17 @@
     <row r="95" ht="25" customHeight="1">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>Talbot</t>
+          <t>Sturges</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
         <is>
-          <t>Lauryn</t>
+          <t>Trevor</t>
         </is>
       </c>
       <c r="C95" s="3" t="inlineStr">
         <is>
-          <t>Benoni Lakes</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D95" s="3" t="inlineStr">
@@ -10556,17 +10588,17 @@
     <row r="96" ht="25" customHeight="1">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>Theron</t>
+          <t>Talbot</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
         <is>
-          <t>Pierre</t>
+          <t>Lauryn</t>
         </is>
       </c>
       <c r="C96" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Benoni Lakes</t>
         </is>
       </c>
       <c r="D96" s="3" t="inlineStr">
@@ -10588,7 +10620,7 @@
       </c>
       <c r="B97" s="3" t="inlineStr">
         <is>
-          <t>Moira</t>
+          <t>Pierre</t>
         </is>
       </c>
       <c r="C97" s="3" t="inlineStr">
@@ -10610,17 +10642,17 @@
     <row r="98" ht="25" customHeight="1">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>Townsend</t>
+          <t>Theron</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
         <is>
-          <t>Diane</t>
+          <t>Moira</t>
         </is>
       </c>
       <c r="C98" s="3" t="inlineStr">
         <is>
-          <t>Benoni Lakes</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D98" s="3" t="inlineStr">
@@ -10637,22 +10669,22 @@
     <row r="99" ht="25" customHeight="1">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>Toye</t>
+          <t>Townsend</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
         <is>
-          <t>Omolayo</t>
+          <t>Diane</t>
         </is>
       </c>
       <c r="C99" s="3" t="inlineStr">
         <is>
-          <t>The Wilds</t>
+          <t>Benoni Lakes</t>
         </is>
       </c>
       <c r="D99" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E99" s="3" t="inlineStr">
@@ -10664,22 +10696,22 @@
     <row r="100" ht="25" customHeight="1">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>Tuckett</t>
+          <t>Toye</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
         <is>
-          <t>Alistair</t>
+          <t>Omolayo</t>
         </is>
       </c>
       <c r="C100" s="3" t="inlineStr">
         <is>
-          <t>Roodepoort Clearwater Cyber</t>
+          <t>The Wilds</t>
         </is>
       </c>
       <c r="D100" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E100" s="3" t="inlineStr">
@@ -10696,7 +10728,7 @@
       </c>
       <c r="B101" s="3" t="inlineStr">
         <is>
-          <t>Rowan</t>
+          <t>Alistair</t>
         </is>
       </c>
       <c r="C101" s="3" t="inlineStr">
@@ -10711,7 +10743,7 @@
       </c>
       <c r="E101" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -10723,7 +10755,7 @@
       </c>
       <c r="B102" s="3" t="inlineStr">
         <is>
-          <t>Gail</t>
+          <t>Rowan</t>
         </is>
       </c>
       <c r="C102" s="3" t="inlineStr">
@@ -10738,29 +10770,29 @@
       </c>
       <c r="E102" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="103" ht="25" customHeight="1">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>Uchytil</t>
+          <t>Tuckett</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
         <is>
-          <t>Jiri</t>
+          <t>Gail</t>
         </is>
       </c>
       <c r="C103" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Roodepoort Clearwater Cyber</t>
         </is>
       </c>
       <c r="D103" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E103" s="3" t="inlineStr">
@@ -10772,17 +10804,17 @@
     <row r="104" ht="25" customHeight="1">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>VAN DER MERWE</t>
+          <t>Uchytil</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
         <is>
-          <t>PATRICIA</t>
+          <t>Jiri</t>
         </is>
       </c>
       <c r="C104" s="3" t="inlineStr">
         <is>
-          <t>East London Port Rex</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D104" s="3" t="inlineStr">
@@ -10792,24 +10824,24 @@
       </c>
       <c r="E104" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="105" ht="25" customHeight="1">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>Van Niekerk</t>
+          <t>VAN DER MERWE</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
         <is>
-          <t>Riaan</t>
+          <t>PATRICIA</t>
         </is>
       </c>
       <c r="C105" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>East London Port Rex</t>
         </is>
       </c>
       <c r="D105" s="3" t="inlineStr">
@@ -10819,29 +10851,29 @@
       </c>
       <c r="E105" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="106" ht="25" customHeight="1">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>Van Nieuwenhuyzen</t>
+          <t>Van Niekerk</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
         <is>
-          <t>Hilgardt</t>
+          <t>Riaan</t>
         </is>
       </c>
       <c r="C106" s="3" t="inlineStr">
         <is>
-          <t>Worcester</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D106" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E106" s="3" t="inlineStr">
@@ -10853,71 +10885,71 @@
     <row r="107" ht="25" customHeight="1">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>Venter</t>
+          <t>Van Nieuwenhuyzen</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
         <is>
-          <t>Louis</t>
+          <t>Hilgardt</t>
         </is>
       </c>
       <c r="C107" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Worcester</t>
         </is>
       </c>
       <c r="D107" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E107" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="108" ht="25" customHeight="1">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>Volker</t>
+          <t>Venter</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
         <is>
-          <t>Russell</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="C108" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D108" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E108" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="109" ht="25" customHeight="1">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>Warman</t>
+          <t>Volker</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
         <is>
-          <t>Alastair</t>
+          <t>Russell</t>
         </is>
       </c>
       <c r="C109" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>King William's Town</t>
         </is>
       </c>
       <c r="D109" s="3" t="inlineStr">
@@ -10934,17 +10966,17 @@
     <row r="110" ht="25" customHeight="1">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>Williamson</t>
+          <t>Warman</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
         <is>
-          <t>Neville</t>
+          <t>Alastair</t>
         </is>
       </c>
       <c r="C110" s="3" t="inlineStr">
         <is>
-          <t>Port Alfred</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D110" s="3" t="inlineStr">
@@ -10954,24 +10986,24 @@
       </c>
       <c r="E110" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="111" ht="25" customHeight="1">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>Wilter-Sturges</t>
+          <t>Williamson</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
         <is>
-          <t>Meredith</t>
+          <t>Neville</t>
         </is>
       </c>
       <c r="C111" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Port Alfred</t>
         </is>
       </c>
       <c r="D111" s="3" t="inlineStr">
@@ -10988,22 +11020,22 @@
     <row r="112" ht="25" customHeight="1">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>de Silva</t>
+          <t>Wilter-Sturges</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Meredith</t>
         </is>
       </c>
       <c r="C112" s="3" t="inlineStr">
         <is>
-          <t>Edenvale</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D112" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E112" s="3" t="inlineStr">
@@ -11015,27 +11047,27 @@
     <row r="113" ht="25" customHeight="1">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>du Plooy</t>
+          <t>de Silva</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
         <is>
-          <t>Tammy</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="C113" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Edenvale</t>
         </is>
       </c>
       <c r="D113" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E113" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -11047,7 +11079,7 @@
       </c>
       <c r="B114" s="3" t="inlineStr">
         <is>
-          <t>Marc</t>
+          <t>Tammy</t>
         </is>
       </c>
       <c r="C114" s="3" t="inlineStr">
@@ -11069,17 +11101,17 @@
     <row r="115" ht="25" customHeight="1">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>du Toit</t>
+          <t>du Plooy</t>
         </is>
       </c>
       <c r="B115" s="3" t="inlineStr">
         <is>
-          <t>Desiree</t>
+          <t>Marc</t>
         </is>
       </c>
       <c r="C115" s="3" t="inlineStr">
         <is>
-          <t>Ramsgate</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D115" s="3" t="inlineStr">
@@ -11089,24 +11121,24 @@
       </c>
       <c r="E115" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="116" ht="25" customHeight="1">
       <c r="A116" s="3" t="inlineStr">
         <is>
-          <t>le Roux</t>
+          <t>du Toit</t>
         </is>
       </c>
       <c r="B116" s="3" t="inlineStr">
         <is>
-          <t>Jeanette</t>
+          <t>Desiree</t>
         </is>
       </c>
       <c r="C116" s="3" t="inlineStr">
         <is>
-          <t>Gonubie</t>
+          <t>Ramsgate</t>
         </is>
       </c>
       <c r="D116" s="3" t="inlineStr">
@@ -11116,24 +11148,24 @@
       </c>
       <c r="E116" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="117" ht="25" customHeight="1">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>van Heerden</t>
+          <t>le Roux</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Jeanette</t>
         </is>
       </c>
       <c r="C117" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Gonubie</t>
         </is>
       </c>
       <c r="D117" s="3" t="inlineStr">
@@ -11155,7 +11187,7 @@
       </c>
       <c r="B118" s="3" t="inlineStr">
         <is>
-          <t>Sandy</t>
+          <t>Sydney</t>
         </is>
       </c>
       <c r="C118" s="3" t="inlineStr">
@@ -11170,7 +11202,7 @@
       </c>
       <c r="E118" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -11182,12 +11214,12 @@
       </c>
       <c r="B119" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Sandy</t>
         </is>
       </c>
       <c r="C119" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D119" s="3" t="inlineStr">
@@ -11204,17 +11236,17 @@
     <row r="120" ht="25" customHeight="1">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>van Wyk</t>
+          <t>van Heerden</t>
         </is>
       </c>
       <c r="B120" s="3" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C120" s="3" t="inlineStr">
         <is>
-          <t>North Durban</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D120" s="3" t="inlineStr">
@@ -11224,7 +11256,7 @@
       </c>
       <c r="E120" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -11236,12 +11268,12 @@
       </c>
       <c r="B121" s="3" t="inlineStr">
         <is>
-          <t>Lindie</t>
+          <t>Kim</t>
         </is>
       </c>
       <c r="C121" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>North Durban</t>
         </is>
       </c>
       <c r="D121" s="3" t="inlineStr">
@@ -11263,12 +11295,12 @@
       </c>
       <c r="B122" s="3" t="inlineStr">
         <is>
-          <t>Willem</t>
+          <t>Lindie</t>
         </is>
       </c>
       <c r="C122" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D122" s="3" t="inlineStr">
@@ -11290,12 +11322,12 @@
       </c>
       <c r="B123" s="3" t="inlineStr">
         <is>
-          <t>Patricia</t>
+          <t>Willem</t>
         </is>
       </c>
       <c r="C123" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D123" s="3" t="inlineStr">
@@ -11312,93 +11344,120 @@
     <row r="124" ht="25" customHeight="1">
       <c r="A124" s="3" t="inlineStr">
         <is>
-          <t>van der Merwe</t>
+          <t>van Wyk</t>
         </is>
       </c>
       <c r="B124" s="3" t="inlineStr">
         <is>
-          <t>Ingrid</t>
+          <t>Patricia</t>
         </is>
       </c>
       <c r="C124" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D124" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E124" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="125" ht="25" customHeight="1">
       <c r="A125" s="3" t="inlineStr">
         <is>
-          <t>von der Decken</t>
+          <t>van der Merwe</t>
         </is>
       </c>
       <c r="B125" s="3" t="inlineStr">
         <is>
-          <t>Brian</t>
+          <t>Ingrid</t>
         </is>
       </c>
       <c r="C125" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D125" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E125" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="126" ht="25" customHeight="1">
       <c r="A126" s="3" t="inlineStr">
         <is>
+          <t>von der Decken</t>
+        </is>
+      </c>
+      <c r="B126" s="3" t="inlineStr">
+        <is>
+          <t>Brian</t>
+        </is>
+      </c>
+      <c r="C126" s="3" t="inlineStr">
+        <is>
+          <t>King William's Town</t>
+        </is>
+      </c>
+      <c r="D126" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E126" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="127" ht="25" customHeight="1">
+      <c r="A127" s="3" t="inlineStr">
+        <is>
           <t>‘t Hart</t>
         </is>
       </c>
-      <c r="B126" s="3" t="inlineStr">
+      <c r="B127" s="3" t="inlineStr">
         <is>
           <t>Michelle</t>
         </is>
       </c>
-      <c r="C126" s="3" t="inlineStr">
+      <c r="C127" s="3" t="inlineStr">
         <is>
           <t>Benoni Lakes</t>
         </is>
       </c>
-      <c r="D126" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E126" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" s="1" t="inlineStr">
-        <is>
-          <t>Number of attendees: 124</t>
+      <c r="D127" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E127" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="inlineStr">
+        <is>
+          <t>Number of attendees: 125</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="inlineStr">
         <is>
           <t>Number of voters: 59</t>
         </is>
@@ -11434,7 +11493,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Registrees as of 20/04/2021 20:45</t>
+          <t>410W Registrees as of 21/04/2021 09:02</t>
         </is>
       </c>
     </row>
@@ -15487,7 +15546,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15502,7 +15561,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Voting details as of 20/04/2021 20:45</t>
+          <t>410E Voting details as of 21/04/2021 09:02</t>
         </is>
       </c>
     </row>
@@ -15581,27 +15640,27 @@
     <row r="9" ht="25" customHeight="1">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>Helderkruin</t>
+          <t>Edenvale</t>
         </is>
       </c>
       <c r="B9" s="3" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" ht="25" customHeight="1">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>Hibberdene</t>
+          <t>Helderkruin</t>
         </is>
       </c>
       <c r="B10" s="3" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" ht="25" customHeight="1">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>Kensington</t>
+          <t>Hibberdene</t>
         </is>
       </c>
       <c r="B11" s="3" t="n">
@@ -15611,47 +15670,47 @@
     <row r="12" ht="25" customHeight="1">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Kensington</t>
         </is>
       </c>
       <c r="B12" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" ht="25" customHeight="1">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>Kouga</t>
+          <t>King William's Town</t>
         </is>
       </c>
       <c r="B13" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" ht="25" customHeight="1">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>Krugersdorp</t>
+          <t>Kouga</t>
         </is>
       </c>
       <c r="B14" s="3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" ht="25" customHeight="1">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Krugersdorp</t>
         </is>
       </c>
       <c r="B15" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" ht="25" customHeight="1">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="B16" s="3" t="n">
@@ -15661,7 +15720,7 @@
     <row r="17" ht="25" customHeight="1">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>Nelspruit</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="B17" s="3" t="n">
@@ -15671,7 +15730,7 @@
     <row r="18" ht="25" customHeight="1">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>North Durban</t>
+          <t>Nelspruit</t>
         </is>
       </c>
       <c r="B18" s="3" t="n">
@@ -15681,7 +15740,7 @@
     <row r="19" ht="25" customHeight="1">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>Port Alfred</t>
+          <t>North Durban</t>
         </is>
       </c>
       <c r="B19" s="3" t="n">
@@ -15691,47 +15750,47 @@
     <row r="20" ht="25" customHeight="1">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Port Alfred</t>
         </is>
       </c>
       <c r="B20" s="3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" ht="25" customHeight="1">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="B21" s="3" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" ht="25" customHeight="1">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="B22" s="3" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" ht="25" customHeight="1">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>Roodepoort Clearwater Cyber</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="B23" s="3" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" ht="25" customHeight="1">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>Rustenburg</t>
+          <t>Ramsgate</t>
         </is>
       </c>
       <c r="B24" s="3" t="n">
@@ -15741,7 +15800,7 @@
     <row r="25" ht="25" customHeight="1">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>Standerton</t>
+          <t>Roodepoort Clearwater Cyber</t>
         </is>
       </c>
       <c r="B25" s="3" t="n">
@@ -15751,52 +15810,72 @@
     <row r="26" ht="25" customHeight="1">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>The Wilds</t>
+          <t>Rustenburg</t>
         </is>
       </c>
       <c r="B26" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" ht="25" customHeight="1">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>Uitenhage</t>
+          <t>Standerton</t>
         </is>
       </c>
       <c r="B27" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" ht="25" customHeight="1">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>Vereeniging</t>
+          <t>The Wilds</t>
         </is>
       </c>
       <c r="B28" s="3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" ht="25" customHeight="1">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Uitenhage</t>
         </is>
       </c>
       <c r="B29" s="3" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" s="1" t="inlineStr">
-        <is>
-          <t>Number of clubs: 27</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="1" t="inlineStr">
+    <row r="30" ht="25" customHeight="1">
+      <c r="A30" s="3" t="inlineStr">
+        <is>
+          <t>Vereeniging</t>
+        </is>
+      </c>
+      <c r="B30" s="3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" ht="25" customHeight="1">
+      <c r="A31" s="3" t="inlineStr">
+        <is>
+          <t>Wilro Park</t>
+        </is>
+      </c>
+      <c r="B31" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>Number of clubs: 29</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
         <is>
           <t>Number of voters: 60</t>
         </is>
@@ -15829,7 +15908,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Voting details as of 20/04/2021 20:45</t>
+          <t>410W Voting details as of 21/04/2021 09:02</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Registree stats backup on Wed 21 Apr 2021 09:29:43 SAST
</commit_message>
<xml_diff>
--- a/static/docs/registrees_list.xlsx
+++ b/static/docs/registrees_list.xlsx
@@ -451,7 +451,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>MD410 Registrees as of 21/04/2021 09:27</t>
+          <t>MD410 Registrees as of 21/04/2021 09:29</t>
         </is>
       </c>
     </row>
@@ -3006,7 +3006,7 @@
       </c>
       <c r="E81" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F81" s="3" t="inlineStr">
@@ -8017,7 +8017,7 @@
     <row r="239">
       <c r="A239" s="1" t="inlineStr">
         <is>
-          <t>Number of voters: 100</t>
+          <t>Number of voters: 99</t>
         </is>
       </c>
     </row>
@@ -8051,7 +8051,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Registrees as of 21/04/2021 09:27</t>
+          <t>410E Registrees as of 21/04/2021 09:29</t>
         </is>
       </c>
     </row>
@@ -11501,7 +11501,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Registrees as of 21/04/2021 09:27</t>
+          <t>410W Registrees as of 21/04/2021 09:29</t>
         </is>
       </c>
     </row>
@@ -11825,7 +11825,7 @@
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -12959,7 +12959,7 @@
       </c>
       <c r="E55" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -14201,7 +14201,7 @@
       </c>
       <c r="E101" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -15538,7 +15538,7 @@
     <row r="152">
       <c r="A152" s="1" t="inlineStr">
         <is>
-          <t>Number of voters: 55</t>
+          <t>Number of voters: 56</t>
         </is>
       </c>
     </row>
@@ -15569,7 +15569,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Voting details as of 21/04/2021 09:27</t>
+          <t>410E Voting details as of 21/04/2021 09:29</t>
         </is>
       </c>
     </row>
@@ -15901,7 +15901,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15916,7 +15916,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Voting details as of 21/04/2021 09:27</t>
+          <t>410W Voting details as of 21/04/2021 09:29</t>
         </is>
       </c>
     </row>
@@ -15959,7 +15959,7 @@
         </is>
       </c>
       <c r="B5" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" ht="25" customHeight="1">
@@ -15995,27 +15995,27 @@
     <row r="9" ht="25" customHeight="1">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>Eden</t>
         </is>
       </c>
       <c r="B9" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" ht="25" customHeight="1">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>Eden</t>
+          <t>Fish Hoek</t>
         </is>
       </c>
       <c r="B10" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" ht="25" customHeight="1">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>Fish Hoek</t>
+          <t>George</t>
         </is>
       </c>
       <c r="B11" s="3" t="n">
@@ -16025,27 +16025,27 @@
     <row r="12" ht="25" customHeight="1">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>George</t>
+          <t>Gordons Bay</t>
         </is>
       </c>
       <c r="B12" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" ht="25" customHeight="1">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>Gordons Bay</t>
+          <t>Groote Schuur</t>
         </is>
       </c>
       <c r="B13" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" ht="25" customHeight="1">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>Groote Schuur</t>
+          <t>Grootfontein</t>
         </is>
       </c>
       <c r="B14" s="3" t="n">
@@ -16055,27 +16055,27 @@
     <row r="15" ht="25" customHeight="1">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>Grootfontein</t>
+          <t>Helderberg</t>
         </is>
       </c>
       <c r="B15" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" ht="25" customHeight="1">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>Helderberg</t>
+          <t>Henties Bay</t>
         </is>
       </c>
       <c r="B16" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" ht="25" customHeight="1">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>Henties Bay</t>
+          <t>Malgas</t>
         </is>
       </c>
       <c r="B17" s="3" t="n">
@@ -16085,7 +16085,7 @@
     <row r="18" ht="25" customHeight="1">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>Malgas</t>
+          <t>Malmesbury</t>
         </is>
       </c>
       <c r="B18" s="3" t="n">
@@ -16095,37 +16095,37 @@
     <row r="19" ht="25" customHeight="1">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>Malmesbury</t>
+          <t>Merriman</t>
         </is>
       </c>
       <c r="B19" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" ht="25" customHeight="1">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>Merriman</t>
+          <t>Milnerton</t>
         </is>
       </c>
       <c r="B20" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" ht="25" customHeight="1">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>Milnerton</t>
+          <t>Mitchells Plain</t>
         </is>
       </c>
       <c r="B21" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" ht="25" customHeight="1">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>Mitchells Plain</t>
+          <t>Moorreesburg</t>
         </is>
       </c>
       <c r="B22" s="3" t="n">
@@ -16135,7 +16135,7 @@
     <row r="23" ht="25" customHeight="1">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>Moorreesburg</t>
+          <t>Newlands</t>
         </is>
       </c>
       <c r="B23" s="3" t="n">
@@ -16145,57 +16145,57 @@
     <row r="24" ht="25" customHeight="1">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>Newlands</t>
+          <t>Rehoboth</t>
         </is>
       </c>
       <c r="B24" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" ht="25" customHeight="1">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>Rehoboth</t>
+          <t>Sea Point</t>
         </is>
       </c>
       <c r="B25" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" ht="25" customHeight="1">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>Sea Point</t>
+          <t>Sedgefield</t>
         </is>
       </c>
       <c r="B26" s="3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" ht="25" customHeight="1">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>Sedgefield</t>
+          <t>Stellenbosch</t>
         </is>
       </c>
       <c r="B27" s="3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" ht="25" customHeight="1">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>Stellenbosch</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="B28" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" ht="25" customHeight="1">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Table View</t>
         </is>
       </c>
       <c r="B29" s="3" t="n">
@@ -16205,7 +16205,7 @@
     <row r="30" ht="25" customHeight="1">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>Table View</t>
+          <t>Tokai</t>
         </is>
       </c>
       <c r="B30" s="3" t="n">
@@ -16215,17 +16215,17 @@
     <row r="31" ht="25" customHeight="1">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>Tokai</t>
+          <t>Tsumeb</t>
         </is>
       </c>
       <c r="B31" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" ht="25" customHeight="1">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>Tsumeb</t>
+          <t>Tygerberg Hills</t>
         </is>
       </c>
       <c r="B32" s="3" t="n">
@@ -16235,54 +16235,44 @@
     <row r="33" ht="25" customHeight="1">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>Tygerberg Hills</t>
+          <t>Wellington</t>
         </is>
       </c>
       <c r="B33" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" ht="25" customHeight="1">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>Wellington</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="B34" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" ht="25" customHeight="1">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Worcester</t>
         </is>
       </c>
       <c r="B35" s="3" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="36" ht="25" customHeight="1">
-      <c r="A36" s="3" t="inlineStr">
-        <is>
-          <t>Worcester</t>
-        </is>
-      </c>
-      <c r="B36" s="3" t="n">
-        <v>3</v>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>Number of clubs: 33</t>
+        </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>Number of clubs: 34</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="1" t="inlineStr">
-        <is>
-          <t>Number of voters: 55</t>
+          <t>Number of voters: 56</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Registree stats backup on Wed 21 Apr 2021 10:14:02 SAST
</commit_message>
<xml_diff>
--- a/static/docs/registrees_list.xlsx
+++ b/static/docs/registrees_list.xlsx
@@ -451,7 +451,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>MD410 Registrees as of 21/04/2021 09:29</t>
+          <t>MD410 Registrees as of 21/04/2021 10:14</t>
         </is>
       </c>
     </row>
@@ -1940,7 +1940,7 @@
       </c>
       <c r="C48" s="3" t="inlineStr">
         <is>
-          <t>Not Specified</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D48" s="3" t="inlineStr">
@@ -4990,7 +4990,7 @@
       </c>
       <c r="E143" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F143" s="3" t="inlineStr">
@@ -8017,7 +8017,7 @@
     <row r="239">
       <c r="A239" s="1" t="inlineStr">
         <is>
-          <t>Number of voters: 99</t>
+          <t>Number of voters: 98</t>
         </is>
       </c>
     </row>
@@ -8051,7 +8051,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Registrees as of 21/04/2021 09:29</t>
+          <t>410E Registrees as of 21/04/2021 10:14</t>
         </is>
       </c>
     </row>
@@ -8635,7 +8635,7 @@
       </c>
       <c r="C23" s="3" t="inlineStr">
         <is>
-          <t>Not Specified</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D23" s="3" t="inlineStr">
@@ -8932,7 +8932,7 @@
       </c>
       <c r="C34" s="3" t="inlineStr">
         <is>
-          <t>Not Specified</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D34" s="3" t="inlineStr">
@@ -10103,7 +10103,7 @@
       </c>
       <c r="E77" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -11467,7 +11467,7 @@
     <row r="129">
       <c r="A129" s="1" t="inlineStr">
         <is>
-          <t>Number of voters: 56</t>
+          <t>Number of voters: 55</t>
         </is>
       </c>
     </row>
@@ -11501,7 +11501,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Registrees as of 21/04/2021 09:29</t>
+          <t>410W Registrees as of 21/04/2021 10:14</t>
         </is>
       </c>
     </row>
@@ -13803,7 +13803,7 @@
     <row r="87" ht="25" customHeight="1">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>Mosesd</t>
+          <t>Moses</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -15569,7 +15569,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Voting details as of 21/04/2021 09:29</t>
+          <t>410E Voting details as of 21/04/2021 10:14</t>
         </is>
       </c>
     </row>
@@ -15852,7 +15852,7 @@
         </is>
       </c>
       <c r="B29" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" ht="25" customHeight="1">
@@ -15885,7 +15885,7 @@
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>Number of voters: 57</t>
+          <t>Number of voters: 56</t>
         </is>
       </c>
     </row>
@@ -15916,7 +15916,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Voting details as of 21/04/2021 09:29</t>
+          <t>410W Voting details as of 21/04/2021 10:14</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Registree stats backup on Wed 21 Apr 2021 10:21:32 SAST
</commit_message>
<xml_diff>
--- a/static/docs/registrees_list.xlsx
+++ b/static/docs/registrees_list.xlsx
@@ -451,7 +451,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>MD410 Registrees as of 21/04/2021 10:14</t>
+          <t>MD410 Registrees as of 21/04/2021 10:21</t>
         </is>
       </c>
     </row>
@@ -2014,7 +2014,7 @@
       </c>
       <c r="E50" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F50" s="3" t="inlineStr">
@@ -2046,7 +2046,7 @@
       </c>
       <c r="E51" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F51" s="3" t="inlineStr">
@@ -2078,7 +2078,7 @@
       </c>
       <c r="E52" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F52" s="3" t="inlineStr">
@@ -8017,7 +8017,7 @@
     <row r="239">
       <c r="A239" s="1" t="inlineStr">
         <is>
-          <t>Number of voters: 98</t>
+          <t>Number of voters: 95</t>
         </is>
       </c>
     </row>
@@ -8051,7 +8051,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Registrees as of 21/04/2021 10:14</t>
+          <t>410E Registrees as of 21/04/2021 10:21</t>
         </is>
       </c>
     </row>
@@ -8672,7 +8672,7 @@
       </c>
       <c r="E24" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -8699,7 +8699,7 @@
       </c>
       <c r="E25" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -8726,7 +8726,7 @@
       </c>
       <c r="E26" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -11467,7 +11467,7 @@
     <row r="129">
       <c r="A129" s="1" t="inlineStr">
         <is>
-          <t>Number of voters: 55</t>
+          <t>Number of voters: 52</t>
         </is>
       </c>
     </row>
@@ -11501,7 +11501,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Registrees as of 21/04/2021 10:14</t>
+          <t>410W Registrees as of 21/04/2021 10:21</t>
         </is>
       </c>
     </row>
@@ -15569,7 +15569,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Voting details as of 21/04/2021 10:14</t>
+          <t>410E Voting details as of 21/04/2021 10:21</t>
         </is>
       </c>
     </row>
@@ -15662,7 +15662,7 @@
         </is>
       </c>
       <c r="B10" s="3" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" ht="25" customHeight="1">
@@ -15885,7 +15885,7 @@
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>Number of voters: 56</t>
+          <t>Number of voters: 53</t>
         </is>
       </c>
     </row>
@@ -15916,7 +15916,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Voting details as of 21/04/2021 10:14</t>
+          <t>410W Voting details as of 21/04/2021 10:21</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Registree stats backup on Wed 21 Apr 2021 11:10:49 SAST
</commit_message>
<xml_diff>
--- a/static/docs/registrees_list.xlsx
+++ b/static/docs/registrees_list.xlsx
@@ -451,7 +451,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>MD410 Registrees as of 21/04/2021 10:21</t>
+          <t>MD410 Registrees as of 21/04/2021 11:10</t>
         </is>
       </c>
     </row>
@@ -5726,7 +5726,7 @@
       </c>
       <c r="E166" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F166" s="3" t="inlineStr">
@@ -5758,7 +5758,7 @@
       </c>
       <c r="E167" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F167" s="3" t="inlineStr">
@@ -8051,7 +8051,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Registrees as of 21/04/2021 10:21</t>
+          <t>410E Registrees as of 21/04/2021 11:10</t>
         </is>
       </c>
     </row>
@@ -11501,7 +11501,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Registrees as of 21/04/2021 10:21</t>
+          <t>410W Registrees as of 21/04/2021 11:10</t>
         </is>
       </c>
     </row>
@@ -14471,7 +14471,7 @@
       </c>
       <c r="E111" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -14498,7 +14498,7 @@
       </c>
       <c r="E112" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -15569,7 +15569,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Voting details as of 21/04/2021 10:21</t>
+          <t>410E Voting details as of 21/04/2021 11:10</t>
         </is>
       </c>
     </row>
@@ -15916,7 +15916,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Voting details as of 21/04/2021 10:21</t>
+          <t>410W Voting details as of 21/04/2021 11:10</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Registree stats backup on Wed 21 Apr 2021 11:44:54 SAST
</commit_message>
<xml_diff>
--- a/static/docs/registrees_list.xlsx
+++ b/static/docs/registrees_list.xlsx
@@ -451,7 +451,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>MD410 Registrees as of 21/04/2021 11:10</t>
+          <t>MD410 Registrees as of 21/04/2021 11:44</t>
         </is>
       </c>
     </row>
@@ -4286,7 +4286,7 @@
       </c>
       <c r="E121" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F121" s="3" t="inlineStr">
@@ -8017,7 +8017,7 @@
     <row r="239">
       <c r="A239" s="1" t="inlineStr">
         <is>
-          <t>Number of voters: 95</t>
+          <t>Number of voters: 94</t>
         </is>
       </c>
     </row>
@@ -8051,7 +8051,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Registrees as of 21/04/2021 11:10</t>
+          <t>410E Registrees as of 21/04/2021 11:44</t>
         </is>
       </c>
     </row>
@@ -9698,7 +9698,7 @@
       </c>
       <c r="E62" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -11467,7 +11467,7 @@
     <row r="129">
       <c r="A129" s="1" t="inlineStr">
         <is>
-          <t>Number of voters: 52</t>
+          <t>Number of voters: 51</t>
         </is>
       </c>
     </row>
@@ -11501,7 +11501,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Registrees as of 21/04/2021 11:10</t>
+          <t>410W Registrees as of 21/04/2021 11:44</t>
         </is>
       </c>
     </row>
@@ -15569,7 +15569,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Voting details as of 21/04/2021 11:10</t>
+          <t>410E Voting details as of 21/04/2021 11:44</t>
         </is>
       </c>
     </row>
@@ -15862,7 +15862,7 @@
         </is>
       </c>
       <c r="B30" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" ht="25" customHeight="1">
@@ -15885,7 +15885,7 @@
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>Number of voters: 53</t>
+          <t>Number of voters: 52</t>
         </is>
       </c>
     </row>
@@ -15916,7 +15916,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Voting details as of 21/04/2021 11:10</t>
+          <t>410W Voting details as of 21/04/2021 11:44</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Registree stats backup on Wed 21 Apr 2021 12:20:46 SAST
</commit_message>
<xml_diff>
--- a/static/docs/registrees_list.xlsx
+++ b/static/docs/registrees_list.xlsx
@@ -451,7 +451,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>MD410 Registrees as of 21/04/2021 11:44</t>
+          <t>MD410 Registrees as of 21/04/2021 12:20</t>
         </is>
       </c>
     </row>
@@ -894,7 +894,7 @@
       </c>
       <c r="E15" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F15" s="3" t="inlineStr">
@@ -1182,7 +1182,7 @@
       </c>
       <c r="E24" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F24" s="3" t="inlineStr">
@@ -8051,7 +8051,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Registrees as of 21/04/2021 11:44</t>
+          <t>410E Registrees as of 21/04/2021 12:20</t>
         </is>
       </c>
     </row>
@@ -8240,7 +8240,7 @@
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -8267,7 +8267,7 @@
       </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -8375,7 +8375,7 @@
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -10481,7 +10481,7 @@
       </c>
       <c r="E91" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -10697,7 +10697,7 @@
       </c>
       <c r="E99" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -11183,7 +11183,7 @@
       </c>
       <c r="E117" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -11501,7 +11501,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Registrees as of 21/04/2021 11:44</t>
+          <t>410W Registrees as of 21/04/2021 12:20</t>
         </is>
       </c>
     </row>
@@ -15554,7 +15554,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15569,7 +15569,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Voting details as of 21/04/2021 11:44</t>
+          <t>410E Voting details as of 21/04/2021 12:20</t>
         </is>
       </c>
     </row>
@@ -15602,7 +15602,7 @@
         </is>
       </c>
       <c r="B4" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" ht="25" customHeight="1">
@@ -15628,7 +15628,7 @@
     <row r="7" ht="25" customHeight="1">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>East London Beacon Bay</t>
+          <t>East Coast</t>
         </is>
       </c>
       <c r="B7" s="3" t="n">
@@ -15638,7 +15638,7 @@
     <row r="8" ht="25" customHeight="1">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>East London Port Rex</t>
+          <t>East London Beacon Bay</t>
         </is>
       </c>
       <c r="B8" s="3" t="n">
@@ -15648,7 +15648,7 @@
     <row r="9" ht="25" customHeight="1">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>Edenvale</t>
+          <t>East London Port Rex</t>
         </is>
       </c>
       <c r="B9" s="3" t="n">
@@ -15658,17 +15658,17 @@
     <row r="10" ht="25" customHeight="1">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>Helderkruin</t>
+          <t>Edenvale</t>
         </is>
       </c>
       <c r="B10" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" ht="25" customHeight="1">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>Hibberdene</t>
+          <t>Gonubie</t>
         </is>
       </c>
       <c r="B11" s="3" t="n">
@@ -15678,27 +15678,27 @@
     <row r="12" ht="25" customHeight="1">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>Kensington</t>
+          <t>Helderkruin</t>
         </is>
       </c>
       <c r="B12" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" ht="25" customHeight="1">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Hibberdene</t>
         </is>
       </c>
       <c r="B13" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" ht="25" customHeight="1">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>Kouga</t>
+          <t>Kensington</t>
         </is>
       </c>
       <c r="B14" s="3" t="n">
@@ -15708,37 +15708,37 @@
     <row r="15" ht="25" customHeight="1">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>Krugersdorp</t>
+          <t>King William's Town</t>
         </is>
       </c>
       <c r="B15" s="3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" ht="25" customHeight="1">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Kouga</t>
         </is>
       </c>
       <c r="B16" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" ht="25" customHeight="1">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Krugersdorp</t>
         </is>
       </c>
       <c r="B17" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" ht="25" customHeight="1">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>Nelspruit</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="B18" s="3" t="n">
@@ -15748,7 +15748,7 @@
     <row r="19" ht="25" customHeight="1">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>North Durban</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="B19" s="3" t="n">
@@ -15758,7 +15758,7 @@
     <row r="20" ht="25" customHeight="1">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>Port Alfred</t>
+          <t>Nelspruit</t>
         </is>
       </c>
       <c r="B20" s="3" t="n">
@@ -15768,17 +15768,17 @@
     <row r="21" ht="25" customHeight="1">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>North Durban</t>
         </is>
       </c>
       <c r="B21" s="3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" ht="25" customHeight="1">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Port Alfred</t>
         </is>
       </c>
       <c r="B22" s="3" t="n">
@@ -15788,17 +15788,17 @@
     <row r="23" ht="25" customHeight="1">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="B23" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" ht="25" customHeight="1">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>Ramsgate</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="B24" s="3" t="n">
@@ -15808,17 +15808,17 @@
     <row r="25" ht="25" customHeight="1">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>Roodepoort Clearwater Cyber</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="B25" s="3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" ht="25" customHeight="1">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>Rustenburg</t>
+          <t>Ramsgate</t>
         </is>
       </c>
       <c r="B26" s="3" t="n">
@@ -15828,7 +15828,7 @@
     <row r="27" ht="25" customHeight="1">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>Standerton</t>
+          <t>Roodepoort Clearwater Cyber</t>
         </is>
       </c>
       <c r="B27" s="3" t="n">
@@ -15838,17 +15838,17 @@
     <row r="28" ht="25" customHeight="1">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>The Wilds</t>
+          <t>Rustenburg</t>
         </is>
       </c>
       <c r="B28" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" ht="25" customHeight="1">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>Uitenhage</t>
+          <t>Standerton</t>
         </is>
       </c>
       <c r="B29" s="3" t="n">
@@ -15858,32 +15858,52 @@
     <row r="30" ht="25" customHeight="1">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>Vereeniging</t>
+          <t>The Wilds</t>
         </is>
       </c>
       <c r="B30" s="3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" ht="25" customHeight="1">
       <c r="A31" s="3" t="inlineStr">
         <is>
+          <t>Uitenhage</t>
+        </is>
+      </c>
+      <c r="B31" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" ht="25" customHeight="1">
+      <c r="A32" s="3" t="inlineStr">
+        <is>
+          <t>Vereeniging</t>
+        </is>
+      </c>
+      <c r="B32" s="3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" ht="25" customHeight="1">
+      <c r="A33" s="3" t="inlineStr">
+        <is>
           <t>Wilro Park</t>
         </is>
       </c>
-      <c r="B31" s="3" t="n">
+      <c r="B33" s="3" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" s="1" t="inlineStr">
-        <is>
-          <t>Number of clubs: 29</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="1" t="inlineStr">
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>Number of clubs: 31</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
         <is>
           <t>Number of voters: 52</t>
         </is>
@@ -15916,7 +15936,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Voting details as of 21/04/2021 11:44</t>
+          <t>410W Voting details as of 21/04/2021 12:20</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Registree stats backup on Wed 21 Apr 2021 13:45:21 SAST
</commit_message>
<xml_diff>
--- a/static/docs/registrees_list.xlsx
+++ b/static/docs/registrees_list.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F240"/>
+  <dimension ref="A1:F241"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,7 +451,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>MD410 Registrees as of 21/04/2021 12:57</t>
+          <t>MD410 Registrees as of 21/04/2021 13:45</t>
         </is>
       </c>
     </row>
@@ -7599,17 +7599,17 @@
       </c>
       <c r="B225" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Craig</t>
         </is>
       </c>
       <c r="C225" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>East London Beacon Bay</t>
         </is>
       </c>
       <c r="D225" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E225" s="3" t="inlineStr">
@@ -7626,17 +7626,17 @@
     <row r="226" ht="25" customHeight="1">
       <c r="A226" s="3" t="inlineStr">
         <is>
-          <t>van Rensburg</t>
+          <t>van Heerden</t>
         </is>
       </c>
       <c r="B226" s="3" t="inlineStr">
         <is>
-          <t>Johan</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C226" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D226" s="3" t="inlineStr">
@@ -7646,12 +7646,12 @@
       </c>
       <c r="E226" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F226" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -7663,7 +7663,7 @@
       </c>
       <c r="B227" s="3" t="inlineStr">
         <is>
-          <t>Anne</t>
+          <t>Johan</t>
         </is>
       </c>
       <c r="C227" s="3" t="inlineStr">
@@ -7690,17 +7690,17 @@
     <row r="228" ht="25" customHeight="1">
       <c r="A228" s="3" t="inlineStr">
         <is>
-          <t>van Wulven</t>
+          <t>van Rensburg</t>
         </is>
       </c>
       <c r="B228" s="3" t="inlineStr">
         <is>
-          <t>Jeannie</t>
+          <t>Anne</t>
         </is>
       </c>
       <c r="C228" s="3" t="inlineStr">
         <is>
-          <t>Tygerberg Hills</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D228" s="3" t="inlineStr">
@@ -7727,7 +7727,7 @@
       </c>
       <c r="B229" s="3" t="inlineStr">
         <is>
-          <t>Alan</t>
+          <t>Jeannie</t>
         </is>
       </c>
       <c r="C229" s="3" t="inlineStr">
@@ -7759,7 +7759,7 @@
       </c>
       <c r="B230" s="3" t="inlineStr">
         <is>
-          <t>Deon</t>
+          <t>Alan</t>
         </is>
       </c>
       <c r="C230" s="3" t="inlineStr">
@@ -7786,17 +7786,17 @@
     <row r="231" ht="25" customHeight="1">
       <c r="A231" s="3" t="inlineStr">
         <is>
-          <t>van Wyk</t>
+          <t>van Wulven</t>
         </is>
       </c>
       <c r="B231" s="3" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>Deon</t>
         </is>
       </c>
       <c r="C231" s="3" t="inlineStr">
         <is>
-          <t>North Durban</t>
+          <t>Tygerberg Hills</t>
         </is>
       </c>
       <c r="D231" s="3" t="inlineStr">
@@ -7811,7 +7811,7 @@
       </c>
       <c r="F231" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -7823,12 +7823,12 @@
       </c>
       <c r="B232" s="3" t="inlineStr">
         <is>
-          <t>Lindie</t>
+          <t>Kim</t>
         </is>
       </c>
       <c r="C232" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>North Durban</t>
         </is>
       </c>
       <c r="D232" s="3" t="inlineStr">
@@ -7855,12 +7855,12 @@
       </c>
       <c r="B233" s="3" t="inlineStr">
         <is>
-          <t>Willem</t>
+          <t>Lindie</t>
         </is>
       </c>
       <c r="C233" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D233" s="3" t="inlineStr">
@@ -7887,12 +7887,12 @@
       </c>
       <c r="B234" s="3" t="inlineStr">
         <is>
-          <t>Patricia</t>
+          <t>Willem</t>
         </is>
       </c>
       <c r="C234" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D234" s="3" t="inlineStr">
@@ -7914,22 +7914,22 @@
     <row r="235" ht="25" customHeight="1">
       <c r="A235" s="3" t="inlineStr">
         <is>
-          <t>van der Merwe</t>
+          <t>van Wyk</t>
         </is>
       </c>
       <c r="B235" s="3" t="inlineStr">
         <is>
-          <t>Ingrid</t>
+          <t>Patricia</t>
         </is>
       </c>
       <c r="C235" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D235" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E235" s="3" t="inlineStr">
@@ -7946,49 +7946,49 @@
     <row r="236" ht="25" customHeight="1">
       <c r="A236" s="3" t="inlineStr">
         <is>
-          <t>van der Westhuizen</t>
+          <t>van der Merwe</t>
         </is>
       </c>
       <c r="B236" s="3" t="inlineStr">
         <is>
-          <t>Hennie</t>
+          <t>Ingrid</t>
         </is>
       </c>
       <c r="C236" s="3" t="inlineStr">
         <is>
-          <t>Helderberg</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D236" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E236" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F236" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="237" ht="25" customHeight="1">
       <c r="A237" s="3" t="inlineStr">
         <is>
-          <t>von der Decken</t>
+          <t>van der Westhuizen</t>
         </is>
       </c>
       <c r="B237" s="3" t="inlineStr">
         <is>
-          <t>Brian</t>
+          <t>Hennie</t>
         </is>
       </c>
       <c r="C237" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Helderberg</t>
         </is>
       </c>
       <c r="D237" s="3" t="inlineStr">
@@ -8003,53 +8003,85 @@
       </c>
       <c r="F237" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="238" ht="25" customHeight="1">
       <c r="A238" s="3" t="inlineStr">
         <is>
+          <t>von der Decken</t>
+        </is>
+      </c>
+      <c r="B238" s="3" t="inlineStr">
+        <is>
+          <t>Brian</t>
+        </is>
+      </c>
+      <c r="C238" s="3" t="inlineStr">
+        <is>
+          <t>King William's Town</t>
+        </is>
+      </c>
+      <c r="D238" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E238" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F238" s="3" t="inlineStr">
+        <is>
+          <t>410E</t>
+        </is>
+      </c>
+    </row>
+    <row r="239" ht="25" customHeight="1">
+      <c r="A239" s="3" t="inlineStr">
+        <is>
           <t>‘t Hart</t>
         </is>
       </c>
-      <c r="B238" s="3" t="inlineStr">
+      <c r="B239" s="3" t="inlineStr">
         <is>
           <t>Michelle</t>
         </is>
       </c>
-      <c r="C238" s="3" t="inlineStr">
+      <c r="C239" s="3" t="inlineStr">
         <is>
           <t>Benoni Lakes</t>
         </is>
       </c>
-      <c r="D238" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E238" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F238" s="3" t="inlineStr">
+      <c r="D239" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E239" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F239" s="3" t="inlineStr">
         <is>
           <t>410E</t>
-        </is>
-      </c>
-    </row>
-    <row r="239">
-      <c r="A239" s="1" t="inlineStr">
-        <is>
-          <t>Number of attendees: 236</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="inlineStr">
         <is>
-          <t>Number of voters: 94</t>
+          <t>Number of attendees: 237</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" s="1" t="inlineStr">
+        <is>
+          <t>Number of voters: 95</t>
         </is>
       </c>
     </row>
@@ -8065,7 +8097,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E131"/>
+  <dimension ref="A1:E133"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8083,7 +8115,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Registrees as of 21/04/2021 12:57</t>
+          <t>410E Registrees as of 21/04/2021 13:45</t>
         </is>
       </c>
     </row>
@@ -8144,17 +8176,17 @@
     <row r="4" ht="25" customHeight="1">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>Blakeman</t>
+          <t>Blake</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>Belinda</t>
+          <t>Suzette</t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>North Durban</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D4" s="3" t="inlineStr">
@@ -8198,17 +8230,17 @@
     <row r="6" ht="25" customHeight="1">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>Boswell</t>
+          <t>Blakeman</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>Mel</t>
+          <t>Belinda</t>
         </is>
       </c>
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t>Nelspruit</t>
+          <t>North Durban</t>
         </is>
       </c>
       <c r="D6" s="3" t="inlineStr">
@@ -8225,17 +8257,17 @@
     <row r="7" ht="25" customHeight="1">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>Botha</t>
+          <t>Boswell</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>Lyn(ette)</t>
+          <t>Mel</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>Cowies Hill</t>
+          <t>Nelspruit</t>
         </is>
       </c>
       <c r="D7" s="3" t="inlineStr">
@@ -8245,24 +8277,24 @@
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="8" ht="25" customHeight="1">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>Brauteseth</t>
+          <t>Botha</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Lyn(ette)</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Cowies Hill</t>
         </is>
       </c>
       <c r="D8" s="3" t="inlineStr">
@@ -8272,24 +8304,24 @@
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="9" ht="25" customHeight="1">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>Brooker</t>
+          <t>Brauteseth</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>Byron</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D9" s="3" t="inlineStr">
@@ -8306,17 +8338,17 @@
     <row r="10" ht="25" customHeight="1">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>Bull</t>
+          <t>Brooker</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>Christopher</t>
+          <t>Byron</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr">
         <is>
-          <t>The Wilds</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D10" s="3" t="inlineStr">
@@ -8333,17 +8365,17 @@
     <row r="11" ht="25" customHeight="1">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>Byars</t>
+          <t>Bull</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>Karin</t>
+          <t>Christopher</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
-          <t>Manzini</t>
+          <t>The Wilds</t>
         </is>
       </c>
       <c r="D11" s="3" t="inlineStr">
@@ -8360,17 +8392,17 @@
     <row r="12" ht="25" customHeight="1">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>Chazen</t>
+          <t>Byars</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
         <is>
-          <t>Lionel</t>
+          <t>Karin</t>
         </is>
       </c>
       <c r="C12" s="3" t="inlineStr">
         <is>
-          <t>Edenvale</t>
+          <t>Manzini</t>
         </is>
       </c>
       <c r="D12" s="3" t="inlineStr">
@@ -8380,24 +8412,24 @@
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="13" ht="25" customHeight="1">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>Chetty</t>
+          <t>Chazen</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>Perry</t>
+          <t>Lionel</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
         <is>
-          <t>East Coast</t>
+          <t>Edenvale</t>
         </is>
       </c>
       <c r="D13" s="3" t="inlineStr">
@@ -8414,44 +8446,44 @@
     <row r="14" ht="25" customHeight="1">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>Coppen</t>
+          <t>Chetty</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>Kate</t>
+          <t>Perry</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>East Coast</t>
         </is>
       </c>
       <c r="D14" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="15" ht="25" customHeight="1">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>Davids</t>
+          <t>Coppen</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>Melanie</t>
+          <t>Kate</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D15" s="3" t="inlineStr">
@@ -8468,22 +8500,22 @@
     <row r="16" ht="25" customHeight="1">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>De Wet</t>
+          <t>Davids</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>Lara</t>
+          <t>Melanie</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
         <is>
-          <t>Edenvale</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D16" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E16" s="3" t="inlineStr">
@@ -8495,17 +8527,17 @@
     <row r="17" ht="25" customHeight="1">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>Du Plooy</t>
+          <t>De Wet</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>Peggy</t>
+          <t>Lara</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
         <is>
-          <t>Krugersdorp</t>
+          <t>Edenvale</t>
         </is>
       </c>
       <c r="D17" s="3" t="inlineStr">
@@ -8515,7 +8547,7 @@
       </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -8527,7 +8559,7 @@
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>Ivan</t>
+          <t>Peggy</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
@@ -8549,17 +8581,17 @@
     <row r="19" ht="25" customHeight="1">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>Easton</t>
+          <t>Du Plooy</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
-          <t>Glynn</t>
+          <t>Ivan</t>
         </is>
       </c>
       <c r="C19" s="3" t="inlineStr">
         <is>
-          <t>Helderkruin</t>
+          <t>Krugersdorp</t>
         </is>
       </c>
       <c r="D19" s="3" t="inlineStr">
@@ -8581,7 +8613,7 @@
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>Denise</t>
+          <t>Glynn</t>
         </is>
       </c>
       <c r="C20" s="3" t="inlineStr">
@@ -8603,71 +8635,71 @@
     <row r="21" ht="25" customHeight="1">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>Els</t>
+          <t>Easton</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>Johan</t>
+          <t>Denise</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Helderkruin</t>
         </is>
       </c>
       <c r="D21" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E21" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="22" ht="25" customHeight="1">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>Erasmus</t>
+          <t>Els</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
         <is>
-          <t>Freddie</t>
+          <t>Johan</t>
         </is>
       </c>
       <c r="C22" s="3" t="inlineStr">
         <is>
-          <t>Uitenhage</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D22" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E22" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="23" ht="25" customHeight="1">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>Fourie</t>
+          <t>Erasmus</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
         <is>
-          <t>Lucille</t>
+          <t>Freddie</t>
         </is>
       </c>
       <c r="C23" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Uitenhage</t>
         </is>
       </c>
       <c r="D23" s="3" t="inlineStr">
@@ -8677,24 +8709,24 @@
       </c>
       <c r="E23" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="24" ht="25" customHeight="1">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>Foxcroft</t>
+          <t>Fourie</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
         <is>
-          <t>Kelvin</t>
+          <t>Lucille</t>
         </is>
       </c>
       <c r="C24" s="3" t="inlineStr">
         <is>
-          <t>Helderkruin</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D24" s="3" t="inlineStr">
@@ -8716,7 +8748,7 @@
       </c>
       <c r="B25" s="3" t="inlineStr">
         <is>
-          <t>Jenny</t>
+          <t>Kelvin</t>
         </is>
       </c>
       <c r="C25" s="3" t="inlineStr">
@@ -8743,7 +8775,7 @@
       </c>
       <c r="B26" s="3" t="inlineStr">
         <is>
-          <t>Katherine</t>
+          <t>Jenny</t>
         </is>
       </c>
       <c r="C26" s="3" t="inlineStr">
@@ -8765,17 +8797,17 @@
     <row r="27" ht="25" customHeight="1">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>Froise</t>
+          <t>Foxcroft</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
         <is>
-          <t>Martin</t>
+          <t>Katherine</t>
         </is>
       </c>
       <c r="C27" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Helderkruin</t>
         </is>
       </c>
       <c r="D27" s="3" t="inlineStr">
@@ -8785,24 +8817,24 @@
       </c>
       <c r="E27" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="28" ht="25" customHeight="1">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>Gerhard</t>
+          <t>Froise</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
         <is>
-          <t>Bernd</t>
+          <t>Martin</t>
         </is>
       </c>
       <c r="C28" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D28" s="3" t="inlineStr">
@@ -8824,7 +8856,7 @@
       </c>
       <c r="B29" s="3" t="inlineStr">
         <is>
-          <t>Shirley</t>
+          <t>Bernd</t>
         </is>
       </c>
       <c r="C29" s="3" t="inlineStr">
@@ -8839,24 +8871,24 @@
       </c>
       <c r="E29" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="30" ht="25" customHeight="1">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>Graham</t>
+          <t>Gerhard</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
         <is>
-          <t>Valerie</t>
+          <t>Shirley</t>
         </is>
       </c>
       <c r="C30" s="3" t="inlineStr">
         <is>
-          <t>Nelspruit</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D30" s="3" t="inlineStr">
@@ -8866,7 +8898,7 @@
       </c>
       <c r="E30" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -8878,7 +8910,7 @@
       </c>
       <c r="B31" s="3" t="inlineStr">
         <is>
-          <t>Mike</t>
+          <t>Valerie</t>
         </is>
       </c>
       <c r="C31" s="3" t="inlineStr">
@@ -8893,29 +8925,29 @@
       </c>
       <c r="E31" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="32" ht="25" customHeight="1">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>Griffith</t>
+          <t>Graham</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
         <is>
-          <t>David</t>
+          <t>Mike</t>
         </is>
       </c>
       <c r="C32" s="3" t="inlineStr">
         <is>
-          <t>The Wilds</t>
+          <t>Nelspruit</t>
         </is>
       </c>
       <c r="D32" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E32" s="3" t="inlineStr">
@@ -8927,22 +8959,22 @@
     <row r="33" ht="25" customHeight="1">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>Guthrie</t>
+          <t>Griffith</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
         <is>
-          <t>Clint</t>
+          <t>David</t>
         </is>
       </c>
       <c r="C33" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>The Wilds</t>
         </is>
       </c>
       <c r="D33" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E33" s="3" t="inlineStr">
@@ -8954,12 +8986,12 @@
     <row r="34" ht="25" customHeight="1">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>HERMANUS</t>
+          <t>Guthrie</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
         <is>
-          <t>MBULELO</t>
+          <t>Clint</t>
         </is>
       </c>
       <c r="C34" s="3" t="inlineStr">
@@ -8969,7 +9001,7 @@
       </c>
       <c r="D34" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E34" s="3" t="inlineStr">
@@ -8981,22 +9013,22 @@
     <row r="35" ht="25" customHeight="1">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>HOLLIMAN</t>
+          <t>HERMANUS</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
         <is>
-          <t>KEITH ALEXANDER</t>
+          <t>MBULELO</t>
         </is>
       </c>
       <c r="C35" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D35" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E35" s="3" t="inlineStr">
@@ -9008,17 +9040,17 @@
     <row r="36" ht="25" customHeight="1">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>Heathcote</t>
+          <t>HOLLIMAN</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
         <is>
-          <t>Mike</t>
+          <t>KEITH ALEXANDER</t>
         </is>
       </c>
       <c r="C36" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D36" s="3" t="inlineStr">
@@ -9028,24 +9060,24 @@
       </c>
       <c r="E36" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="37" ht="25" customHeight="1">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>Herzfeld</t>
+          <t>Heathcote</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
         <is>
-          <t>Evelyn</t>
+          <t>Mike</t>
         </is>
       </c>
       <c r="C37" s="3" t="inlineStr">
         <is>
-          <t>Edenvale</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D37" s="3" t="inlineStr">
@@ -9055,24 +9087,24 @@
       </c>
       <c r="E37" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="38" ht="25" customHeight="1">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>Higgins</t>
+          <t>Herzfeld</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
         <is>
-          <t>Wendy</t>
+          <t>Evelyn</t>
         </is>
       </c>
       <c r="C38" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Edenvale</t>
         </is>
       </c>
       <c r="D38" s="3" t="inlineStr">
@@ -9089,17 +9121,17 @@
     <row r="39" ht="25" customHeight="1">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>Hobbs</t>
+          <t>Higgins</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
         <is>
-          <t>Avril</t>
+          <t>Wendy</t>
         </is>
       </c>
       <c r="C39" s="3" t="inlineStr">
         <is>
-          <t>North Durban</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D39" s="3" t="inlineStr">
@@ -9109,7 +9141,7 @@
       </c>
       <c r="E39" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -9121,7 +9153,7 @@
       </c>
       <c r="B40" s="3" t="inlineStr">
         <is>
-          <t>Trevor</t>
+          <t>Avril</t>
         </is>
       </c>
       <c r="C40" s="3" t="inlineStr">
@@ -9143,17 +9175,17 @@
     <row r="41" ht="25" customHeight="1">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>Hocking</t>
+          <t>Hobbs</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
         <is>
-          <t>Jacqui</t>
+          <t>Trevor</t>
         </is>
       </c>
       <c r="C41" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>North Durban</t>
         </is>
       </c>
       <c r="D41" s="3" t="inlineStr">
@@ -9175,7 +9207,7 @@
       </c>
       <c r="B42" s="3" t="inlineStr">
         <is>
-          <t>Cliff</t>
+          <t>Jacqui</t>
         </is>
       </c>
       <c r="C42" s="3" t="inlineStr">
@@ -9190,24 +9222,24 @@
       </c>
       <c r="E42" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="43" ht="25" customHeight="1">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>JOHNSTON</t>
+          <t>Hocking</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
         <is>
-          <t>MALCOLM</t>
+          <t>Cliff</t>
         </is>
       </c>
       <c r="C43" s="3" t="inlineStr">
         <is>
-          <t>Standerton</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D43" s="3" t="inlineStr">
@@ -9217,24 +9249,24 @@
       </c>
       <c r="E43" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="44" ht="25" customHeight="1">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>Jackman</t>
+          <t>JOHNSTON</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
         <is>
-          <t>Gail</t>
+          <t>MALCOLM</t>
         </is>
       </c>
       <c r="C44" s="3" t="inlineStr">
         <is>
-          <t>Nelspruit</t>
+          <t>Standerton</t>
         </is>
       </c>
       <c r="D44" s="3" t="inlineStr">
@@ -9244,24 +9276,24 @@
       </c>
       <c r="E44" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="45" ht="25" customHeight="1">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>Jackson</t>
+          <t>Jackman</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
         <is>
-          <t>Alna</t>
+          <t>Gail</t>
         </is>
       </c>
       <c r="C45" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Nelspruit</t>
         </is>
       </c>
       <c r="D45" s="3" t="inlineStr">
@@ -9271,24 +9303,24 @@
       </c>
       <c r="E45" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="46" ht="25" customHeight="1">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>Kienast</t>
+          <t>Jackson</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
         <is>
-          <t>Margie</t>
+          <t>Alna</t>
         </is>
       </c>
       <c r="C46" s="3" t="inlineStr">
         <is>
-          <t>Edenvale</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D46" s="3" t="inlineStr">
@@ -9298,24 +9330,24 @@
       </c>
       <c r="E46" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="47" ht="25" customHeight="1">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>Kimari</t>
+          <t>Kienast</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
         <is>
-          <t>Joyce</t>
+          <t>Margie</t>
         </is>
       </c>
       <c r="C47" s="3" t="inlineStr">
         <is>
-          <t>Eden</t>
+          <t>Edenvale</t>
         </is>
       </c>
       <c r="D47" s="3" t="inlineStr">
@@ -9332,17 +9364,17 @@
     <row r="48" ht="25" customHeight="1">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>King</t>
+          <t>Kimari</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
         <is>
-          <t>Ian</t>
+          <t>Joyce</t>
         </is>
       </c>
       <c r="C48" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Eden</t>
         </is>
       </c>
       <c r="D48" s="3" t="inlineStr">
@@ -9352,7 +9384,7 @@
       </c>
       <c r="E48" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -9364,7 +9396,7 @@
       </c>
       <c r="B49" s="3" t="inlineStr">
         <is>
-          <t>Sandy</t>
+          <t>Ian</t>
         </is>
       </c>
       <c r="C49" s="3" t="inlineStr">
@@ -9386,17 +9418,17 @@
     <row r="50" ht="25" customHeight="1">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>Koekemoer</t>
+          <t>King</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
         <is>
-          <t>Christa</t>
+          <t>Sandy</t>
         </is>
       </c>
       <c r="C50" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D50" s="3" t="inlineStr">
@@ -9406,29 +9438,29 @@
       </c>
       <c r="E50" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="51" ht="25" customHeight="1">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>Kruger</t>
+          <t>Koekemoer</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
         <is>
-          <t>Pieter</t>
+          <t>Christa</t>
         </is>
       </c>
       <c r="C51" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D51" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E51" s="3" t="inlineStr">
@@ -9445,7 +9477,7 @@
       </c>
       <c r="B52" s="3" t="inlineStr">
         <is>
-          <t>Niqula</t>
+          <t>Pieter</t>
         </is>
       </c>
       <c r="C52" s="3" t="inlineStr">
@@ -9467,22 +9499,22 @@
     <row r="53" ht="25" customHeight="1">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>Laas</t>
+          <t>Kruger</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
         <is>
-          <t>Natalie</t>
+          <t>Niqula</t>
         </is>
       </c>
       <c r="C53" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D53" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E53" s="3" t="inlineStr">
@@ -9494,17 +9526,17 @@
     <row r="54" ht="25" customHeight="1">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>Labuschagne</t>
+          <t>Laas</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
         <is>
-          <t>Susan</t>
+          <t>Natalie</t>
         </is>
       </c>
       <c r="C54" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D54" s="3" t="inlineStr">
@@ -9521,22 +9553,22 @@
     <row r="55" ht="25" customHeight="1">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>Langton</t>
+          <t>Labuschagne</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
         <is>
-          <t>Evelyn May</t>
+          <t>Susan</t>
         </is>
       </c>
       <c r="C55" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D55" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E55" s="3" t="inlineStr">
@@ -9548,39 +9580,39 @@
     <row r="56" ht="25" customHeight="1">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>Lautenbach</t>
+          <t>Langton</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
         <is>
-          <t>Steven</t>
+          <t>Evelyn May</t>
         </is>
       </c>
       <c r="C56" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D56" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E56" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="57" ht="25" customHeight="1">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>Logan</t>
+          <t>Lautenbach</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
         <is>
-          <t>Graeme</t>
+          <t>Steven</t>
         </is>
       </c>
       <c r="C57" s="3" t="inlineStr">
@@ -9595,24 +9627,24 @@
       </c>
       <c r="E57" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="58" ht="25" customHeight="1">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>Love</t>
+          <t>Logan</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
         <is>
-          <t>Dee</t>
+          <t>Graeme</t>
         </is>
       </c>
       <c r="C58" s="3" t="inlineStr">
         <is>
-          <t>Cowies Hill</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D58" s="3" t="inlineStr">
@@ -9629,17 +9661,17 @@
     <row r="59" ht="25" customHeight="1">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>Luck</t>
+          <t>Love</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
         <is>
-          <t>Zarina</t>
+          <t>Dee</t>
         </is>
       </c>
       <c r="C59" s="3" t="inlineStr">
         <is>
-          <t>Newcastle</t>
+          <t>Cowies Hill</t>
         </is>
       </c>
       <c r="D59" s="3" t="inlineStr">
@@ -9649,24 +9681,24 @@
       </c>
       <c r="E59" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="60" ht="25" customHeight="1">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>MILLS</t>
+          <t>Luck</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
         <is>
-          <t>BERNICE</t>
+          <t>Zarina</t>
         </is>
       </c>
       <c r="C60" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Newcastle</t>
         </is>
       </c>
       <c r="D60" s="3" t="inlineStr">
@@ -9683,17 +9715,17 @@
     <row r="61" ht="25" customHeight="1">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>Mare</t>
+          <t>MILLS</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
         <is>
-          <t>Beaulieu</t>
+          <t>BERNICE</t>
         </is>
       </c>
       <c r="C61" s="3" t="inlineStr">
         <is>
-          <t>Benoni Lakes</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D61" s="3" t="inlineStr">
@@ -9710,12 +9742,12 @@
     <row r="62" ht="25" customHeight="1">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>Maré</t>
+          <t>Mare</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
         <is>
-          <t>Nick</t>
+          <t>Beaulieu</t>
         </is>
       </c>
       <c r="C62" s="3" t="inlineStr">
@@ -9730,24 +9762,24 @@
       </c>
       <c r="E62" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="63" ht="25" customHeight="1">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>Masson</t>
+          <t>Maré</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
         <is>
-          <t>Jean</t>
+          <t>Nick</t>
         </is>
       </c>
       <c r="C63" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Benoni Lakes</t>
         </is>
       </c>
       <c r="D63" s="3" t="inlineStr">
@@ -9764,17 +9796,17 @@
     <row r="64" ht="25" customHeight="1">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>McDonald</t>
+          <t>Masson</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
         <is>
-          <t>Rochelle</t>
+          <t>Jean</t>
         </is>
       </c>
       <c r="C64" s="3" t="inlineStr">
         <is>
-          <t>Vereeniging</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D64" s="3" t="inlineStr">
@@ -9791,17 +9823,17 @@
     <row r="65" ht="25" customHeight="1">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>McKerrow</t>
+          <t>McDonald</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
         <is>
-          <t>Alec</t>
+          <t>Rochelle</t>
         </is>
       </c>
       <c r="C65" s="3" t="inlineStr">
         <is>
-          <t>Port Alfred</t>
+          <t>Vereeniging</t>
         </is>
       </c>
       <c r="D65" s="3" t="inlineStr">
@@ -9818,17 +9850,17 @@
     <row r="66" ht="25" customHeight="1">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>Mccullough</t>
+          <t>McKerrow</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
         <is>
-          <t>David</t>
+          <t>Alec</t>
         </is>
       </c>
       <c r="C66" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Port Alfred</t>
         </is>
       </c>
       <c r="D66" s="3" t="inlineStr">
@@ -9845,17 +9877,17 @@
     <row r="67" ht="25" customHeight="1">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>Meltzer</t>
+          <t>Mccullough</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>David</t>
         </is>
       </c>
       <c r="C67" s="3" t="inlineStr">
         <is>
-          <t>The Wilds</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D67" s="3" t="inlineStr">
@@ -9865,24 +9897,24 @@
       </c>
       <c r="E67" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="68" ht="25" customHeight="1">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>Meyer</t>
+          <t>Meltzer</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
         <is>
-          <t>Denis</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C68" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>The Wilds</t>
         </is>
       </c>
       <c r="D68" s="3" t="inlineStr">
@@ -9899,17 +9931,17 @@
     <row r="69" ht="25" customHeight="1">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>Michas</t>
+          <t>Meyer</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
         <is>
-          <t>Roy</t>
+          <t>Denis</t>
         </is>
       </c>
       <c r="C69" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D69" s="3" t="inlineStr">
@@ -9931,7 +9963,7 @@
       </c>
       <c r="B70" s="3" t="inlineStr">
         <is>
-          <t>Dawn</t>
+          <t>Roy</t>
         </is>
       </c>
       <c r="C70" s="3" t="inlineStr">
@@ -9946,24 +9978,24 @@
       </c>
       <c r="E70" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="71" ht="25" customHeight="1">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>Mills</t>
+          <t>Michas</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>Dawn</t>
         </is>
       </c>
       <c r="C71" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D71" s="3" t="inlineStr">
@@ -9973,24 +10005,24 @@
       </c>
       <c r="E71" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="72" ht="25" customHeight="1">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>Mitchell</t>
+          <t>Mills</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
         <is>
-          <t>Alana</t>
+          <t>Patrick</t>
         </is>
       </c>
       <c r="C72" s="3" t="inlineStr">
         <is>
-          <t>Rustenburg</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D72" s="3" t="inlineStr">
@@ -10000,7 +10032,7 @@
       </c>
       <c r="E72" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -10012,7 +10044,7 @@
       </c>
       <c r="B73" s="3" t="inlineStr">
         <is>
-          <t>Juan</t>
+          <t>Alana</t>
         </is>
       </c>
       <c r="C73" s="3" t="inlineStr">
@@ -10027,24 +10059,24 @@
       </c>
       <c r="E73" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="74" ht="25" customHeight="1">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>Murray</t>
+          <t>Mitchell</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
         <is>
-          <t>Suzanne</t>
+          <t>Juan</t>
         </is>
       </c>
       <c r="C74" s="3" t="inlineStr">
         <is>
-          <t>Vereeniging</t>
+          <t>Rustenburg</t>
         </is>
       </c>
       <c r="D74" s="3" t="inlineStr">
@@ -10066,7 +10098,7 @@
       </c>
       <c r="B75" s="3" t="inlineStr">
         <is>
-          <t>Gary</t>
+          <t>Suzanne</t>
         </is>
       </c>
       <c r="C75" s="3" t="inlineStr">
@@ -10088,17 +10120,17 @@
     <row r="76" ht="25" customHeight="1">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>Nel</t>
+          <t>Murray</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
         <is>
-          <t>Theo</t>
+          <t>Gary</t>
         </is>
       </c>
       <c r="C76" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Vereeniging</t>
         </is>
       </c>
       <c r="D76" s="3" t="inlineStr">
@@ -10115,17 +10147,17 @@
     <row r="77" ht="25" customHeight="1">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>Newlands</t>
+          <t>Nel</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
         <is>
-          <t>Mike</t>
+          <t>Theo</t>
         </is>
       </c>
       <c r="C77" s="3" t="inlineStr">
         <is>
-          <t>Port Alfred</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D77" s="3" t="inlineStr">
@@ -10142,17 +10174,17 @@
     <row r="78" ht="25" customHeight="1">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>Ngobozana</t>
+          <t>Newlands</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
         <is>
-          <t>Sphiwe</t>
+          <t>Mike</t>
         </is>
       </c>
       <c r="C78" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Port Alfred</t>
         </is>
       </c>
       <c r="D78" s="3" t="inlineStr">
@@ -10162,24 +10194,24 @@
       </c>
       <c r="E78" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="79" ht="25" customHeight="1">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>Oberholzer</t>
+          <t>Ngobozana</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
         <is>
-          <t>PDG Bokkie</t>
+          <t>Sphiwe</t>
         </is>
       </c>
       <c r="C79" s="3" t="inlineStr">
         <is>
-          <t>Uitenhage</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D79" s="3" t="inlineStr">
@@ -10196,17 +10228,17 @@
     <row r="80" ht="25" customHeight="1">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>PORTEOUS</t>
+          <t>Oberholzer</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
         <is>
-          <t>BRIAN</t>
+          <t>PDG Bokkie</t>
         </is>
       </c>
       <c r="C80" s="3" t="inlineStr">
         <is>
-          <t>Hibberdene</t>
+          <t>Uitenhage</t>
         </is>
       </c>
       <c r="D80" s="3" t="inlineStr">
@@ -10216,24 +10248,24 @@
       </c>
       <c r="E80" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="81" ht="25" customHeight="1">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>Paijmans</t>
+          <t>PORTEOUS</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
         <is>
-          <t>Bronwyn Anne</t>
+          <t>BRIAN</t>
         </is>
       </c>
       <c r="C81" s="3" t="inlineStr">
         <is>
-          <t>Cowies Hill</t>
+          <t>Hibberdene</t>
         </is>
       </c>
       <c r="D81" s="3" t="inlineStr">
@@ -10243,24 +10275,24 @@
       </c>
       <c r="E81" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="82" ht="25" customHeight="1">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>Pantoleon</t>
+          <t>Paijmans</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
         <is>
-          <t>Teresa</t>
+          <t>Bronwyn Anne</t>
         </is>
       </c>
       <c r="C82" s="3" t="inlineStr">
         <is>
-          <t>Vereeniging</t>
+          <t>Cowies Hill</t>
         </is>
       </c>
       <c r="D82" s="3" t="inlineStr">
@@ -10270,24 +10302,24 @@
       </c>
       <c r="E82" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="83" ht="25" customHeight="1">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>Polkinghorne</t>
+          <t>Pantoleon</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
         <is>
-          <t>Tracey</t>
+          <t>Teresa</t>
         </is>
       </c>
       <c r="C83" s="3" t="inlineStr">
         <is>
-          <t>Kensington</t>
+          <t>Vereeniging</t>
         </is>
       </c>
       <c r="D83" s="3" t="inlineStr">
@@ -10309,7 +10341,7 @@
       </c>
       <c r="B84" s="3" t="inlineStr">
         <is>
-          <t>Gavin</t>
+          <t>Tracey</t>
         </is>
       </c>
       <c r="C84" s="3" t="inlineStr">
@@ -10324,24 +10356,24 @@
       </c>
       <c r="E84" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="85" ht="25" customHeight="1">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>Ras</t>
+          <t>Polkinghorne</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
         <is>
-          <t>Leon Jacobus</t>
+          <t>Gavin</t>
         </is>
       </c>
       <c r="C85" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Kensington</t>
         </is>
       </c>
       <c r="D85" s="3" t="inlineStr">
@@ -10358,22 +10390,22 @@
     <row r="86" ht="25" customHeight="1">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>Rashirai</t>
+          <t>Ras</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
         <is>
-          <t>Tabeth</t>
+          <t>Leon Jacobus</t>
         </is>
       </c>
       <c r="C86" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D86" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E86" s="3" t="inlineStr">
@@ -10385,44 +10417,44 @@
     <row r="87" ht="25" customHeight="1">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>Reniers</t>
+          <t>Rashirai</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
         <is>
-          <t>Hugo</t>
+          <t>Tabeth</t>
         </is>
       </c>
       <c r="C87" s="3" t="inlineStr">
         <is>
-          <t>Nelspruit</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D87" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E87" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="88" ht="25" customHeight="1">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>Sabatier</t>
+          <t>Reniers</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
         <is>
-          <t>Rodney</t>
+          <t>Hugo</t>
         </is>
       </c>
       <c r="C88" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Nelspruit</t>
         </is>
       </c>
       <c r="D88" s="3" t="inlineStr">
@@ -10439,17 +10471,17 @@
     <row r="89" ht="25" customHeight="1">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>Searle</t>
+          <t>Sabatier</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
         <is>
-          <t>Francis</t>
+          <t>Rodney</t>
         </is>
       </c>
       <c r="C89" s="3" t="inlineStr">
         <is>
-          <t>Kouga</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D89" s="3" t="inlineStr">
@@ -10471,7 +10503,7 @@
       </c>
       <c r="B90" s="3" t="inlineStr">
         <is>
-          <t>Gloria</t>
+          <t>Francis</t>
         </is>
       </c>
       <c r="C90" s="3" t="inlineStr">
@@ -10486,24 +10518,24 @@
       </c>
       <c r="E90" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="91" ht="25" customHeight="1">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>Smit</t>
+          <t>Searle</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
         <is>
-          <t>Sue</t>
+          <t>Gloria</t>
         </is>
       </c>
       <c r="C91" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Kouga</t>
         </is>
       </c>
       <c r="D91" s="3" t="inlineStr">
@@ -10520,17 +10552,17 @@
     <row r="92" ht="25" customHeight="1">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Smit</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
         <is>
-          <t>Jeff</t>
+          <t>Sue</t>
         </is>
       </c>
       <c r="C92" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D92" s="3" t="inlineStr">
@@ -10547,17 +10579,17 @@
     <row r="93" ht="25" customHeight="1">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>Stander</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
         <is>
-          <t>Max</t>
+          <t>Jeff</t>
         </is>
       </c>
       <c r="C93" s="3" t="inlineStr">
         <is>
-          <t>Port Alfred</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D93" s="3" t="inlineStr">
@@ -10579,12 +10611,12 @@
       </c>
       <c r="B94" s="3" t="inlineStr">
         <is>
-          <t>Ashley</t>
+          <t>Max</t>
         </is>
       </c>
       <c r="C94" s="3" t="inlineStr">
         <is>
-          <t>Krugersdorp</t>
+          <t>Port Alfred</t>
         </is>
       </c>
       <c r="D94" s="3" t="inlineStr">
@@ -10594,7 +10626,7 @@
       </c>
       <c r="E94" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -10606,7 +10638,7 @@
       </c>
       <c r="B95" s="3" t="inlineStr">
         <is>
-          <t>Brett Jason</t>
+          <t>Ashley</t>
         </is>
       </c>
       <c r="C95" s="3" t="inlineStr">
@@ -10621,29 +10653,29 @@
       </c>
       <c r="E95" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="96" ht="25" customHeight="1">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>Steyn</t>
+          <t>Stander</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
         <is>
-          <t>Elna</t>
+          <t>Brett Jason</t>
         </is>
       </c>
       <c r="C96" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Krugersdorp</t>
         </is>
       </c>
       <c r="D96" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E96" s="3" t="inlineStr">
@@ -10655,22 +10687,22 @@
     <row r="97" ht="25" customHeight="1">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>Sturges</t>
+          <t>Steyn</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
         <is>
-          <t>Trevor</t>
+          <t>Elna</t>
         </is>
       </c>
       <c r="C97" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D97" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E97" s="3" t="inlineStr">
@@ -10682,17 +10714,17 @@
     <row r="98" ht="25" customHeight="1">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>Talbot</t>
+          <t>Sturges</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
         <is>
-          <t>Lauryn</t>
+          <t>Trevor</t>
         </is>
       </c>
       <c r="C98" s="3" t="inlineStr">
         <is>
-          <t>Benoni Lakes</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D98" s="3" t="inlineStr">
@@ -10709,17 +10741,17 @@
     <row r="99" ht="25" customHeight="1">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>Theron</t>
+          <t>Talbot</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
         <is>
-          <t>Pierre</t>
+          <t>Lauryn</t>
         </is>
       </c>
       <c r="C99" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Benoni Lakes</t>
         </is>
       </c>
       <c r="D99" s="3" t="inlineStr">
@@ -10741,7 +10773,7 @@
       </c>
       <c r="B100" s="3" t="inlineStr">
         <is>
-          <t>Moira</t>
+          <t>Pierre</t>
         </is>
       </c>
       <c r="C100" s="3" t="inlineStr">
@@ -10763,17 +10795,17 @@
     <row r="101" ht="25" customHeight="1">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>Townsend</t>
+          <t>Theron</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
         <is>
-          <t>Diane</t>
+          <t>Moira</t>
         </is>
       </c>
       <c r="C101" s="3" t="inlineStr">
         <is>
-          <t>Benoni Lakes</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D101" s="3" t="inlineStr">
@@ -10783,56 +10815,56 @@
       </c>
       <c r="E101" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="102" ht="25" customHeight="1">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>Toye</t>
+          <t>Townsend</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
         <is>
-          <t>Omolayo</t>
+          <t>Diane</t>
         </is>
       </c>
       <c r="C102" s="3" t="inlineStr">
         <is>
-          <t>The Wilds</t>
+          <t>Benoni Lakes</t>
         </is>
       </c>
       <c r="D102" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E102" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="103" ht="25" customHeight="1">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>Tuckett</t>
+          <t>Toye</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
         <is>
-          <t>Alistair</t>
+          <t>Omolayo</t>
         </is>
       </c>
       <c r="C103" s="3" t="inlineStr">
         <is>
-          <t>Roodepoort Clearwater Cyber</t>
+          <t>The Wilds</t>
         </is>
       </c>
       <c r="D103" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E103" s="3" t="inlineStr">
@@ -10849,7 +10881,7 @@
       </c>
       <c r="B104" s="3" t="inlineStr">
         <is>
-          <t>Rowan</t>
+          <t>Alistair</t>
         </is>
       </c>
       <c r="C104" s="3" t="inlineStr">
@@ -10864,7 +10896,7 @@
       </c>
       <c r="E104" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -10876,7 +10908,7 @@
       </c>
       <c r="B105" s="3" t="inlineStr">
         <is>
-          <t>Gail</t>
+          <t>Rowan</t>
         </is>
       </c>
       <c r="C105" s="3" t="inlineStr">
@@ -10891,29 +10923,29 @@
       </c>
       <c r="E105" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="106" ht="25" customHeight="1">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>Uchytil</t>
+          <t>Tuckett</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
         <is>
-          <t>Jiri</t>
+          <t>Gail</t>
         </is>
       </c>
       <c r="C106" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Roodepoort Clearwater Cyber</t>
         </is>
       </c>
       <c r="D106" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E106" s="3" t="inlineStr">
@@ -10925,17 +10957,17 @@
     <row r="107" ht="25" customHeight="1">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>VAN DER MERWE</t>
+          <t>Uchytil</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
         <is>
-          <t>PATRICIA</t>
+          <t>Jiri</t>
         </is>
       </c>
       <c r="C107" s="3" t="inlineStr">
         <is>
-          <t>East London Port Rex</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D107" s="3" t="inlineStr">
@@ -10945,24 +10977,24 @@
       </c>
       <c r="E107" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="108" ht="25" customHeight="1">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>Van Niekerk</t>
+          <t>VAN DER MERWE</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
         <is>
-          <t>Riaan</t>
+          <t>PATRICIA</t>
         </is>
       </c>
       <c r="C108" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>East London Port Rex</t>
         </is>
       </c>
       <c r="D108" s="3" t="inlineStr">
@@ -10972,29 +11004,29 @@
       </c>
       <c r="E108" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="109" ht="25" customHeight="1">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>Van Nieuwenhuyzen</t>
+          <t>Van Niekerk</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
         <is>
-          <t>Hilgardt</t>
+          <t>Riaan</t>
         </is>
       </c>
       <c r="C109" s="3" t="inlineStr">
         <is>
-          <t>Worcester</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D109" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E109" s="3" t="inlineStr">
@@ -11006,22 +11038,22 @@
     <row r="110" ht="25" customHeight="1">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>Venter</t>
+          <t>Van Nieuwenhuyzen</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
         <is>
-          <t>Louis</t>
+          <t>Hilgardt</t>
         </is>
       </c>
       <c r="C110" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Worcester</t>
         </is>
       </c>
       <c r="D110" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E110" s="3" t="inlineStr">
@@ -11033,44 +11065,44 @@
     <row r="111" ht="25" customHeight="1">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>Volker</t>
+          <t>Venter</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
         <is>
-          <t>Russell</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="C111" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D111" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E111" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="112" ht="25" customHeight="1">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>Warman</t>
+          <t>Volker</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
         <is>
-          <t>Alastair</t>
+          <t>Russell</t>
         </is>
       </c>
       <c r="C112" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>King William's Town</t>
         </is>
       </c>
       <c r="D112" s="3" t="inlineStr">
@@ -11087,17 +11119,17 @@
     <row r="113" ht="25" customHeight="1">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>Williamson</t>
+          <t>Warman</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
         <is>
-          <t>Neville</t>
+          <t>Alastair</t>
         </is>
       </c>
       <c r="C113" s="3" t="inlineStr">
         <is>
-          <t>Port Alfred</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D113" s="3" t="inlineStr">
@@ -11107,24 +11139,24 @@
       </c>
       <c r="E113" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="114" ht="25" customHeight="1">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>Wilter-Sturges</t>
+          <t>Williamson</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
         <is>
-          <t>Meredith</t>
+          <t>Neville</t>
         </is>
       </c>
       <c r="C114" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Port Alfred</t>
         </is>
       </c>
       <c r="D114" s="3" t="inlineStr">
@@ -11141,22 +11173,22 @@
     <row r="115" ht="25" customHeight="1">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>de Silva</t>
+          <t>Wilter-Sturges</t>
         </is>
       </c>
       <c r="B115" s="3" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Meredith</t>
         </is>
       </c>
       <c r="C115" s="3" t="inlineStr">
         <is>
-          <t>Edenvale</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D115" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E115" s="3" t="inlineStr">
@@ -11168,27 +11200,27 @@
     <row r="116" ht="25" customHeight="1">
       <c r="A116" s="3" t="inlineStr">
         <is>
-          <t>du Plooy</t>
+          <t>de Silva</t>
         </is>
       </c>
       <c r="B116" s="3" t="inlineStr">
         <is>
-          <t>Tammy</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="C116" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Edenvale</t>
         </is>
       </c>
       <c r="D116" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E116" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -11200,7 +11232,7 @@
       </c>
       <c r="B117" s="3" t="inlineStr">
         <is>
-          <t>Marc</t>
+          <t>Tammy</t>
         </is>
       </c>
       <c r="C117" s="3" t="inlineStr">
@@ -11222,17 +11254,17 @@
     <row r="118" ht="25" customHeight="1">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>du Toit</t>
+          <t>du Plooy</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
         <is>
-          <t>Desiree</t>
+          <t>Marc</t>
         </is>
       </c>
       <c r="C118" s="3" t="inlineStr">
         <is>
-          <t>Ramsgate</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D118" s="3" t="inlineStr">
@@ -11249,17 +11281,17 @@
     <row r="119" ht="25" customHeight="1">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>le Roux</t>
+          <t>du Toit</t>
         </is>
       </c>
       <c r="B119" s="3" t="inlineStr">
         <is>
-          <t>Jeanette</t>
+          <t>Desiree</t>
         </is>
       </c>
       <c r="C119" s="3" t="inlineStr">
         <is>
-          <t>Gonubie</t>
+          <t>Ramsgate</t>
         </is>
       </c>
       <c r="D119" s="3" t="inlineStr">
@@ -11276,17 +11308,17 @@
     <row r="120" ht="25" customHeight="1">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>van Heerden</t>
+          <t>le Roux</t>
         </is>
       </c>
       <c r="B120" s="3" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Jeanette</t>
         </is>
       </c>
       <c r="C120" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Gonubie</t>
         </is>
       </c>
       <c r="D120" s="3" t="inlineStr">
@@ -11296,7 +11328,7 @@
       </c>
       <c r="E120" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -11308,7 +11340,7 @@
       </c>
       <c r="B121" s="3" t="inlineStr">
         <is>
-          <t>Sandy</t>
+          <t>Sydney</t>
         </is>
       </c>
       <c r="C121" s="3" t="inlineStr">
@@ -11323,7 +11355,7 @@
       </c>
       <c r="E121" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -11335,12 +11367,12 @@
       </c>
       <c r="B122" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Sandy</t>
         </is>
       </c>
       <c r="C122" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D122" s="3" t="inlineStr">
@@ -11357,44 +11389,44 @@
     <row r="123" ht="25" customHeight="1">
       <c r="A123" s="3" t="inlineStr">
         <is>
-          <t>van Wyk</t>
+          <t>van Heerden</t>
         </is>
       </c>
       <c r="B123" s="3" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>Craig</t>
         </is>
       </c>
       <c r="C123" s="3" t="inlineStr">
         <is>
-          <t>North Durban</t>
+          <t>East London Beacon Bay</t>
         </is>
       </c>
       <c r="D123" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E123" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="124" ht="25" customHeight="1">
       <c r="A124" s="3" t="inlineStr">
         <is>
-          <t>van Wyk</t>
+          <t>van Heerden</t>
         </is>
       </c>
       <c r="B124" s="3" t="inlineStr">
         <is>
-          <t>Lindie</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C124" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D124" s="3" t="inlineStr">
@@ -11404,7 +11436,7 @@
       </c>
       <c r="E124" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -11416,12 +11448,12 @@
       </c>
       <c r="B125" s="3" t="inlineStr">
         <is>
-          <t>Willem</t>
+          <t>Kim</t>
         </is>
       </c>
       <c r="C125" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>North Durban</t>
         </is>
       </c>
       <c r="D125" s="3" t="inlineStr">
@@ -11443,7 +11475,7 @@
       </c>
       <c r="B126" s="3" t="inlineStr">
         <is>
-          <t>Patricia</t>
+          <t>Lindie</t>
         </is>
       </c>
       <c r="C126" s="3" t="inlineStr">
@@ -11465,22 +11497,22 @@
     <row r="127" ht="25" customHeight="1">
       <c r="A127" s="3" t="inlineStr">
         <is>
-          <t>van der Merwe</t>
+          <t>van Wyk</t>
         </is>
       </c>
       <c r="B127" s="3" t="inlineStr">
         <is>
-          <t>Ingrid</t>
+          <t>Willem</t>
         </is>
       </c>
       <c r="C127" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D127" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E127" s="3" t="inlineStr">
@@ -11492,17 +11524,17 @@
     <row r="128" ht="25" customHeight="1">
       <c r="A128" s="3" t="inlineStr">
         <is>
-          <t>von der Decken</t>
+          <t>van Wyk</t>
         </is>
       </c>
       <c r="B128" s="3" t="inlineStr">
         <is>
-          <t>Brian</t>
+          <t>Patricia</t>
         </is>
       </c>
       <c r="C128" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D128" s="3" t="inlineStr">
@@ -11512,48 +11544,102 @@
       </c>
       <c r="E128" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="129" ht="25" customHeight="1">
       <c r="A129" s="3" t="inlineStr">
         <is>
+          <t>van der Merwe</t>
+        </is>
+      </c>
+      <c r="B129" s="3" t="inlineStr">
+        <is>
+          <t>Ingrid</t>
+        </is>
+      </c>
+      <c r="C129" s="3" t="inlineStr">
+        <is>
+          <t>Letaba Tzaneen</t>
+        </is>
+      </c>
+      <c r="D129" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="E129" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="130" ht="25" customHeight="1">
+      <c r="A130" s="3" t="inlineStr">
+        <is>
+          <t>von der Decken</t>
+        </is>
+      </c>
+      <c r="B130" s="3" t="inlineStr">
+        <is>
+          <t>Brian</t>
+        </is>
+      </c>
+      <c r="C130" s="3" t="inlineStr">
+        <is>
+          <t>King William's Town</t>
+        </is>
+      </c>
+      <c r="D130" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E130" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="131" ht="25" customHeight="1">
+      <c r="A131" s="3" t="inlineStr">
+        <is>
           <t>‘t Hart</t>
         </is>
       </c>
-      <c r="B129" s="3" t="inlineStr">
+      <c r="B131" s="3" t="inlineStr">
         <is>
           <t>Michelle</t>
         </is>
       </c>
-      <c r="C129" s="3" t="inlineStr">
+      <c r="C131" s="3" t="inlineStr">
         <is>
           <t>Benoni Lakes</t>
         </is>
       </c>
-      <c r="D129" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E129" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" s="1" t="inlineStr">
-        <is>
-          <t>Number of attendees: 127</t>
-        </is>
-      </c>
-    </row>
-    <row r="131">
-      <c r="A131" s="1" t="inlineStr">
-        <is>
-          <t>Number of voters: 51</t>
+      <c r="D131" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E131" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="inlineStr">
+        <is>
+          <t>Number of attendees: 129</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="1" t="inlineStr">
+        <is>
+          <t>Number of voters: 52</t>
         </is>
       </c>
     </row>
@@ -11587,7 +11673,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Registrees as of 21/04/2021 12:57</t>
+          <t>410W Registrees as of 21/04/2021 13:45</t>
         </is>
       </c>
     </row>
@@ -15655,7 +15741,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Voting details as of 21/04/2021 12:57</t>
+          <t>410E Voting details as of 21/04/2021 13:45</t>
         </is>
       </c>
     </row>
@@ -16032,7 +16118,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Voting details as of 21/04/2021 12:57</t>
+          <t>410W Voting details as of 21/04/2021 13:45</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Registree stats backup on Wed 21 Apr 2021 13:58:24 SAST
</commit_message>
<xml_diff>
--- a/static/docs/registrees_list.xlsx
+++ b/static/docs/registrees_list.xlsx
@@ -451,7 +451,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>MD410 Registrees as of 21/04/2021 13:45</t>
+          <t>MD410 Registrees as of 21/04/2021 13:58</t>
         </is>
       </c>
     </row>
@@ -5379,7 +5379,7 @@
       </c>
       <c r="F155" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -6851,7 +6851,7 @@
       </c>
       <c r="F201" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -8097,7 +8097,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E133"/>
+  <dimension ref="A1:E130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8115,7 +8115,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Registrees as of 21/04/2021 13:45</t>
+          <t>410E Registrees as of 21/04/2021 13:58</t>
         </is>
       </c>
     </row>
@@ -8230,17 +8230,17 @@
     <row r="6" ht="25" customHeight="1">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>Blakeman</t>
+          <t>Boswell</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>Belinda</t>
+          <t>Mel</t>
         </is>
       </c>
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t>North Durban</t>
+          <t>Nelspruit</t>
         </is>
       </c>
       <c r="D6" s="3" t="inlineStr">
@@ -8257,17 +8257,17 @@
     <row r="7" ht="25" customHeight="1">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>Boswell</t>
+          <t>Botha</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>Mel</t>
+          <t>Lyn(ette)</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>Nelspruit</t>
+          <t>Cowies Hill</t>
         </is>
       </c>
       <c r="D7" s="3" t="inlineStr">
@@ -8277,24 +8277,24 @@
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="8" ht="25" customHeight="1">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>Botha</t>
+          <t>Brauteseth</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>Lyn(ette)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>Cowies Hill</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D8" s="3" t="inlineStr">
@@ -8304,24 +8304,24 @@
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="9" ht="25" customHeight="1">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>Brauteseth</t>
+          <t>Brooker</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Byron</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D9" s="3" t="inlineStr">
@@ -8338,17 +8338,17 @@
     <row r="10" ht="25" customHeight="1">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>Brooker</t>
+          <t>Bull</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>Byron</t>
+          <t>Christopher</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>The Wilds</t>
         </is>
       </c>
       <c r="D10" s="3" t="inlineStr">
@@ -8365,17 +8365,17 @@
     <row r="11" ht="25" customHeight="1">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>Bull</t>
+          <t>Byars</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>Christopher</t>
+          <t>Karin</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
-          <t>The Wilds</t>
+          <t>Manzini</t>
         </is>
       </c>
       <c r="D11" s="3" t="inlineStr">
@@ -8392,17 +8392,17 @@
     <row r="12" ht="25" customHeight="1">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>Byars</t>
+          <t>Chazen</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
         <is>
-          <t>Karin</t>
+          <t>Lionel</t>
         </is>
       </c>
       <c r="C12" s="3" t="inlineStr">
         <is>
-          <t>Manzini</t>
+          <t>Edenvale</t>
         </is>
       </c>
       <c r="D12" s="3" t="inlineStr">
@@ -8412,24 +8412,24 @@
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="13" ht="25" customHeight="1">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>Chazen</t>
+          <t>Chetty</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>Lionel</t>
+          <t>Perry</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
         <is>
-          <t>Edenvale</t>
+          <t>East Coast</t>
         </is>
       </c>
       <c r="D13" s="3" t="inlineStr">
@@ -8446,44 +8446,44 @@
     <row r="14" ht="25" customHeight="1">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>Chetty</t>
+          <t>Coppen</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>Perry</t>
+          <t>Kate</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr">
         <is>
-          <t>East Coast</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D14" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="15" ht="25" customHeight="1">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>Coppen</t>
+          <t>Davids</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>Kate</t>
+          <t>Melanie</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D15" s="3" t="inlineStr">
@@ -8500,22 +8500,22 @@
     <row r="16" ht="25" customHeight="1">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>Davids</t>
+          <t>De Wet</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>Melanie</t>
+          <t>Lara</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Edenvale</t>
         </is>
       </c>
       <c r="D16" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E16" s="3" t="inlineStr">
@@ -8527,17 +8527,17 @@
     <row r="17" ht="25" customHeight="1">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>De Wet</t>
+          <t>Du Plooy</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>Lara</t>
+          <t>Peggy</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
         <is>
-          <t>Edenvale</t>
+          <t>Krugersdorp</t>
         </is>
       </c>
       <c r="D17" s="3" t="inlineStr">
@@ -8547,7 +8547,7 @@
       </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -8559,7 +8559,7 @@
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>Peggy</t>
+          <t>Ivan</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
@@ -8581,17 +8581,17 @@
     <row r="19" ht="25" customHeight="1">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>Du Plooy</t>
+          <t>Easton</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
-          <t>Ivan</t>
+          <t>Glynn</t>
         </is>
       </c>
       <c r="C19" s="3" t="inlineStr">
         <is>
-          <t>Krugersdorp</t>
+          <t>Helderkruin</t>
         </is>
       </c>
       <c r="D19" s="3" t="inlineStr">
@@ -8613,7 +8613,7 @@
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>Glynn</t>
+          <t>Denise</t>
         </is>
       </c>
       <c r="C20" s="3" t="inlineStr">
@@ -8635,71 +8635,71 @@
     <row r="21" ht="25" customHeight="1">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>Easton</t>
+          <t>Els</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>Denise</t>
+          <t>Johan</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
         <is>
-          <t>Helderkruin</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D21" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E21" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="22" ht="25" customHeight="1">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>Els</t>
+          <t>Erasmus</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
         <is>
-          <t>Johan</t>
+          <t>Freddie</t>
         </is>
       </c>
       <c r="C22" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Uitenhage</t>
         </is>
       </c>
       <c r="D22" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E22" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="23" ht="25" customHeight="1">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>Erasmus</t>
+          <t>Fourie</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
         <is>
-          <t>Freddie</t>
+          <t>Lucille</t>
         </is>
       </c>
       <c r="C23" s="3" t="inlineStr">
         <is>
-          <t>Uitenhage</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D23" s="3" t="inlineStr">
@@ -8709,24 +8709,24 @@
       </c>
       <c r="E23" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="24" ht="25" customHeight="1">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>Fourie</t>
+          <t>Foxcroft</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
         <is>
-          <t>Lucille</t>
+          <t>Kelvin</t>
         </is>
       </c>
       <c r="C24" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Helderkruin</t>
         </is>
       </c>
       <c r="D24" s="3" t="inlineStr">
@@ -8748,7 +8748,7 @@
       </c>
       <c r="B25" s="3" t="inlineStr">
         <is>
-          <t>Kelvin</t>
+          <t>Jenny</t>
         </is>
       </c>
       <c r="C25" s="3" t="inlineStr">
@@ -8775,7 +8775,7 @@
       </c>
       <c r="B26" s="3" t="inlineStr">
         <is>
-          <t>Jenny</t>
+          <t>Katherine</t>
         </is>
       </c>
       <c r="C26" s="3" t="inlineStr">
@@ -8797,17 +8797,17 @@
     <row r="27" ht="25" customHeight="1">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>Foxcroft</t>
+          <t>Froise</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
         <is>
-          <t>Katherine</t>
+          <t>Martin</t>
         </is>
       </c>
       <c r="C27" s="3" t="inlineStr">
         <is>
-          <t>Helderkruin</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D27" s="3" t="inlineStr">
@@ -8817,24 +8817,24 @@
       </c>
       <c r="E27" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="28" ht="25" customHeight="1">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>Froise</t>
+          <t>Gerhard</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
         <is>
-          <t>Martin</t>
+          <t>Bernd</t>
         </is>
       </c>
       <c r="C28" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D28" s="3" t="inlineStr">
@@ -8856,7 +8856,7 @@
       </c>
       <c r="B29" s="3" t="inlineStr">
         <is>
-          <t>Bernd</t>
+          <t>Shirley</t>
         </is>
       </c>
       <c r="C29" s="3" t="inlineStr">
@@ -8871,24 +8871,24 @@
       </c>
       <c r="E29" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="30" ht="25" customHeight="1">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>Gerhard</t>
+          <t>Graham</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
         <is>
-          <t>Shirley</t>
+          <t>Valerie</t>
         </is>
       </c>
       <c r="C30" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Nelspruit</t>
         </is>
       </c>
       <c r="D30" s="3" t="inlineStr">
@@ -8898,7 +8898,7 @@
       </c>
       <c r="E30" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -8910,7 +8910,7 @@
       </c>
       <c r="B31" s="3" t="inlineStr">
         <is>
-          <t>Valerie</t>
+          <t>Mike</t>
         </is>
       </c>
       <c r="C31" s="3" t="inlineStr">
@@ -8925,29 +8925,29 @@
       </c>
       <c r="E31" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="32" ht="25" customHeight="1">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>Graham</t>
+          <t>Griffith</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
         <is>
-          <t>Mike</t>
+          <t>David</t>
         </is>
       </c>
       <c r="C32" s="3" t="inlineStr">
         <is>
-          <t>Nelspruit</t>
+          <t>The Wilds</t>
         </is>
       </c>
       <c r="D32" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E32" s="3" t="inlineStr">
@@ -8959,22 +8959,22 @@
     <row r="33" ht="25" customHeight="1">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>Griffith</t>
+          <t>Guthrie</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
         <is>
-          <t>David</t>
+          <t>Clint</t>
         </is>
       </c>
       <c r="C33" s="3" t="inlineStr">
         <is>
-          <t>The Wilds</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D33" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E33" s="3" t="inlineStr">
@@ -8986,12 +8986,12 @@
     <row r="34" ht="25" customHeight="1">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>Guthrie</t>
+          <t>HERMANUS</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
         <is>
-          <t>Clint</t>
+          <t>MBULELO</t>
         </is>
       </c>
       <c r="C34" s="3" t="inlineStr">
@@ -9001,7 +9001,7 @@
       </c>
       <c r="D34" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E34" s="3" t="inlineStr">
@@ -9013,22 +9013,22 @@
     <row r="35" ht="25" customHeight="1">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>HERMANUS</t>
+          <t>HOLLIMAN</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
         <is>
-          <t>MBULELO</t>
+          <t>KEITH ALEXANDER</t>
         </is>
       </c>
       <c r="C35" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D35" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E35" s="3" t="inlineStr">
@@ -9040,17 +9040,17 @@
     <row r="36" ht="25" customHeight="1">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>HOLLIMAN</t>
+          <t>Heathcote</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
         <is>
-          <t>KEITH ALEXANDER</t>
+          <t>Mike</t>
         </is>
       </c>
       <c r="C36" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D36" s="3" t="inlineStr">
@@ -9060,24 +9060,24 @@
       </c>
       <c r="E36" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="37" ht="25" customHeight="1">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>Heathcote</t>
+          <t>Herzfeld</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
         <is>
-          <t>Mike</t>
+          <t>Evelyn</t>
         </is>
       </c>
       <c r="C37" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Edenvale</t>
         </is>
       </c>
       <c r="D37" s="3" t="inlineStr">
@@ -9087,24 +9087,24 @@
       </c>
       <c r="E37" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="38" ht="25" customHeight="1">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>Herzfeld</t>
+          <t>Higgins</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
         <is>
-          <t>Evelyn</t>
+          <t>Wendy</t>
         </is>
       </c>
       <c r="C38" s="3" t="inlineStr">
         <is>
-          <t>Edenvale</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D38" s="3" t="inlineStr">
@@ -9121,17 +9121,17 @@
     <row r="39" ht="25" customHeight="1">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>Higgins</t>
+          <t>Hobbs</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
         <is>
-          <t>Wendy</t>
+          <t>Avril</t>
         </is>
       </c>
       <c r="C39" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>North Durban</t>
         </is>
       </c>
       <c r="D39" s="3" t="inlineStr">
@@ -9141,7 +9141,7 @@
       </c>
       <c r="E39" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -9153,7 +9153,7 @@
       </c>
       <c r="B40" s="3" t="inlineStr">
         <is>
-          <t>Avril</t>
+          <t>Trevor</t>
         </is>
       </c>
       <c r="C40" s="3" t="inlineStr">
@@ -9175,17 +9175,17 @@
     <row r="41" ht="25" customHeight="1">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>Hobbs</t>
+          <t>Hocking</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
         <is>
-          <t>Trevor</t>
+          <t>Jacqui</t>
         </is>
       </c>
       <c r="C41" s="3" t="inlineStr">
         <is>
-          <t>North Durban</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D41" s="3" t="inlineStr">
@@ -9207,7 +9207,7 @@
       </c>
       <c r="B42" s="3" t="inlineStr">
         <is>
-          <t>Jacqui</t>
+          <t>Cliff</t>
         </is>
       </c>
       <c r="C42" s="3" t="inlineStr">
@@ -9222,24 +9222,24 @@
       </c>
       <c r="E42" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="43" ht="25" customHeight="1">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>Hocking</t>
+          <t>JOHNSTON</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
         <is>
-          <t>Cliff</t>
+          <t>MALCOLM</t>
         </is>
       </c>
       <c r="C43" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Standerton</t>
         </is>
       </c>
       <c r="D43" s="3" t="inlineStr">
@@ -9249,24 +9249,24 @@
       </c>
       <c r="E43" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="44" ht="25" customHeight="1">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>JOHNSTON</t>
+          <t>Jackman</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
         <is>
-          <t>MALCOLM</t>
+          <t>Gail</t>
         </is>
       </c>
       <c r="C44" s="3" t="inlineStr">
         <is>
-          <t>Standerton</t>
+          <t>Nelspruit</t>
         </is>
       </c>
       <c r="D44" s="3" t="inlineStr">
@@ -9276,24 +9276,24 @@
       </c>
       <c r="E44" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="45" ht="25" customHeight="1">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>Jackman</t>
+          <t>Jackson</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
         <is>
-          <t>Gail</t>
+          <t>Alna</t>
         </is>
       </c>
       <c r="C45" s="3" t="inlineStr">
         <is>
-          <t>Nelspruit</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D45" s="3" t="inlineStr">
@@ -9303,24 +9303,24 @@
       </c>
       <c r="E45" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="46" ht="25" customHeight="1">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>Jackson</t>
+          <t>Kienast</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
         <is>
-          <t>Alna</t>
+          <t>Margie</t>
         </is>
       </c>
       <c r="C46" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Edenvale</t>
         </is>
       </c>
       <c r="D46" s="3" t="inlineStr">
@@ -9330,24 +9330,24 @@
       </c>
       <c r="E46" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="47" ht="25" customHeight="1">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>Kienast</t>
+          <t>Kimari</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
         <is>
-          <t>Margie</t>
+          <t>Joyce</t>
         </is>
       </c>
       <c r="C47" s="3" t="inlineStr">
         <is>
-          <t>Edenvale</t>
+          <t>Eden</t>
         </is>
       </c>
       <c r="D47" s="3" t="inlineStr">
@@ -9364,17 +9364,17 @@
     <row r="48" ht="25" customHeight="1">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>Kimari</t>
+          <t>King</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
         <is>
-          <t>Joyce</t>
+          <t>Ian</t>
         </is>
       </c>
       <c r="C48" s="3" t="inlineStr">
         <is>
-          <t>Eden</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D48" s="3" t="inlineStr">
@@ -9384,7 +9384,7 @@
       </c>
       <c r="E48" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -9396,7 +9396,7 @@
       </c>
       <c r="B49" s="3" t="inlineStr">
         <is>
-          <t>Ian</t>
+          <t>Sandy</t>
         </is>
       </c>
       <c r="C49" s="3" t="inlineStr">
@@ -9418,17 +9418,17 @@
     <row r="50" ht="25" customHeight="1">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>King</t>
+          <t>Koekemoer</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
         <is>
-          <t>Sandy</t>
+          <t>Christa</t>
         </is>
       </c>
       <c r="C50" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D50" s="3" t="inlineStr">
@@ -9438,29 +9438,29 @@
       </c>
       <c r="E50" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="51" ht="25" customHeight="1">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>Koekemoer</t>
+          <t>Kruger</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
         <is>
-          <t>Christa</t>
+          <t>Pieter</t>
         </is>
       </c>
       <c r="C51" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D51" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E51" s="3" t="inlineStr">
@@ -9477,7 +9477,7 @@
       </c>
       <c r="B52" s="3" t="inlineStr">
         <is>
-          <t>Pieter</t>
+          <t>Niqula</t>
         </is>
       </c>
       <c r="C52" s="3" t="inlineStr">
@@ -9499,22 +9499,22 @@
     <row r="53" ht="25" customHeight="1">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>Kruger</t>
+          <t>Laas</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
         <is>
-          <t>Niqula</t>
+          <t>Natalie</t>
         </is>
       </c>
       <c r="C53" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D53" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E53" s="3" t="inlineStr">
@@ -9526,17 +9526,17 @@
     <row r="54" ht="25" customHeight="1">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>Laas</t>
+          <t>Labuschagne</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
         <is>
-          <t>Natalie</t>
+          <t>Susan</t>
         </is>
       </c>
       <c r="C54" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D54" s="3" t="inlineStr">
@@ -9553,22 +9553,22 @@
     <row r="55" ht="25" customHeight="1">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>Labuschagne</t>
+          <t>Langton</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
         <is>
-          <t>Susan</t>
+          <t>Evelyn May</t>
         </is>
       </c>
       <c r="C55" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D55" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E55" s="3" t="inlineStr">
@@ -9580,39 +9580,39 @@
     <row r="56" ht="25" customHeight="1">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>Langton</t>
+          <t>Lautenbach</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
         <is>
-          <t>Evelyn May</t>
+          <t>Steven</t>
         </is>
       </c>
       <c r="C56" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D56" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E56" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="57" ht="25" customHeight="1">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>Lautenbach</t>
+          <t>Logan</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
         <is>
-          <t>Steven</t>
+          <t>Graeme</t>
         </is>
       </c>
       <c r="C57" s="3" t="inlineStr">
@@ -9627,24 +9627,24 @@
       </c>
       <c r="E57" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="58" ht="25" customHeight="1">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>Logan</t>
+          <t>Love</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
         <is>
-          <t>Graeme</t>
+          <t>Dee</t>
         </is>
       </c>
       <c r="C58" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Cowies Hill</t>
         </is>
       </c>
       <c r="D58" s="3" t="inlineStr">
@@ -9661,17 +9661,17 @@
     <row r="59" ht="25" customHeight="1">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>Love</t>
+          <t>Luck</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
         <is>
-          <t>Dee</t>
+          <t>Zarina</t>
         </is>
       </c>
       <c r="C59" s="3" t="inlineStr">
         <is>
-          <t>Cowies Hill</t>
+          <t>Newcastle</t>
         </is>
       </c>
       <c r="D59" s="3" t="inlineStr">
@@ -9681,24 +9681,24 @@
       </c>
       <c r="E59" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="60" ht="25" customHeight="1">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>Luck</t>
+          <t>MILLS</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
         <is>
-          <t>Zarina</t>
+          <t>BERNICE</t>
         </is>
       </c>
       <c r="C60" s="3" t="inlineStr">
         <is>
-          <t>Newcastle</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D60" s="3" t="inlineStr">
@@ -9715,17 +9715,17 @@
     <row r="61" ht="25" customHeight="1">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>MILLS</t>
+          <t>Mare</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
         <is>
-          <t>BERNICE</t>
+          <t>Beaulieu</t>
         </is>
       </c>
       <c r="C61" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Benoni Lakes</t>
         </is>
       </c>
       <c r="D61" s="3" t="inlineStr">
@@ -9742,12 +9742,12 @@
     <row r="62" ht="25" customHeight="1">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>Mare</t>
+          <t>Maré</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
         <is>
-          <t>Beaulieu</t>
+          <t>Nick</t>
         </is>
       </c>
       <c r="C62" s="3" t="inlineStr">
@@ -9762,24 +9762,24 @@
       </c>
       <c r="E62" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="63" ht="25" customHeight="1">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>Maré</t>
+          <t>Masson</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
         <is>
-          <t>Nick</t>
+          <t>Jean</t>
         </is>
       </c>
       <c r="C63" s="3" t="inlineStr">
         <is>
-          <t>Benoni Lakes</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D63" s="3" t="inlineStr">
@@ -9796,17 +9796,17 @@
     <row r="64" ht="25" customHeight="1">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>Masson</t>
+          <t>McDonald</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
         <is>
-          <t>Jean</t>
+          <t>Rochelle</t>
         </is>
       </c>
       <c r="C64" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Vereeniging</t>
         </is>
       </c>
       <c r="D64" s="3" t="inlineStr">
@@ -9823,17 +9823,17 @@
     <row r="65" ht="25" customHeight="1">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>McDonald</t>
+          <t>McKerrow</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
         <is>
-          <t>Rochelle</t>
+          <t>Alec</t>
         </is>
       </c>
       <c r="C65" s="3" t="inlineStr">
         <is>
-          <t>Vereeniging</t>
+          <t>Port Alfred</t>
         </is>
       </c>
       <c r="D65" s="3" t="inlineStr">
@@ -9850,17 +9850,17 @@
     <row r="66" ht="25" customHeight="1">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>McKerrow</t>
+          <t>Mccullough</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
         <is>
-          <t>Alec</t>
+          <t>David</t>
         </is>
       </c>
       <c r="C66" s="3" t="inlineStr">
         <is>
-          <t>Port Alfred</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D66" s="3" t="inlineStr">
@@ -9877,17 +9877,17 @@
     <row r="67" ht="25" customHeight="1">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>Mccullough</t>
+          <t>Meltzer</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
         <is>
-          <t>David</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C67" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>The Wilds</t>
         </is>
       </c>
       <c r="D67" s="3" t="inlineStr">
@@ -9897,24 +9897,24 @@
       </c>
       <c r="E67" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="68" ht="25" customHeight="1">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>Meltzer</t>
+          <t>Meyer</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Denis</t>
         </is>
       </c>
       <c r="C68" s="3" t="inlineStr">
         <is>
-          <t>The Wilds</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D68" s="3" t="inlineStr">
@@ -9931,17 +9931,17 @@
     <row r="69" ht="25" customHeight="1">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>Meyer</t>
+          <t>Michas</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
         <is>
-          <t>Denis</t>
+          <t>Roy</t>
         </is>
       </c>
       <c r="C69" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D69" s="3" t="inlineStr">
@@ -9963,7 +9963,7 @@
       </c>
       <c r="B70" s="3" t="inlineStr">
         <is>
-          <t>Roy</t>
+          <t>Dawn</t>
         </is>
       </c>
       <c r="C70" s="3" t="inlineStr">
@@ -9978,24 +9978,24 @@
       </c>
       <c r="E70" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="71" ht="25" customHeight="1">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>Michas</t>
+          <t>Mills</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
         <is>
-          <t>Dawn</t>
+          <t>Patrick</t>
         </is>
       </c>
       <c r="C71" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D71" s="3" t="inlineStr">
@@ -10005,24 +10005,24 @@
       </c>
       <c r="E71" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="72" ht="25" customHeight="1">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>Mills</t>
+          <t>Mitchell</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>Alana</t>
         </is>
       </c>
       <c r="C72" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Rustenburg</t>
         </is>
       </c>
       <c r="D72" s="3" t="inlineStr">
@@ -10032,7 +10032,7 @@
       </c>
       <c r="E72" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -10044,7 +10044,7 @@
       </c>
       <c r="B73" s="3" t="inlineStr">
         <is>
-          <t>Alana</t>
+          <t>Juan</t>
         </is>
       </c>
       <c r="C73" s="3" t="inlineStr">
@@ -10059,24 +10059,24 @@
       </c>
       <c r="E73" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="74" ht="25" customHeight="1">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>Mitchell</t>
+          <t>Murray</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
         <is>
-          <t>Juan</t>
+          <t>Suzanne</t>
         </is>
       </c>
       <c r="C74" s="3" t="inlineStr">
         <is>
-          <t>Rustenburg</t>
+          <t>Vereeniging</t>
         </is>
       </c>
       <c r="D74" s="3" t="inlineStr">
@@ -10098,7 +10098,7 @@
       </c>
       <c r="B75" s="3" t="inlineStr">
         <is>
-          <t>Suzanne</t>
+          <t>Gary</t>
         </is>
       </c>
       <c r="C75" s="3" t="inlineStr">
@@ -10120,17 +10120,17 @@
     <row r="76" ht="25" customHeight="1">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>Murray</t>
+          <t>Nel</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
         <is>
-          <t>Gary</t>
+          <t>Theo</t>
         </is>
       </c>
       <c r="C76" s="3" t="inlineStr">
         <is>
-          <t>Vereeniging</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D76" s="3" t="inlineStr">
@@ -10147,17 +10147,17 @@
     <row r="77" ht="25" customHeight="1">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>Nel</t>
+          <t>Newlands</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
         <is>
-          <t>Theo</t>
+          <t>Mike</t>
         </is>
       </c>
       <c r="C77" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Port Alfred</t>
         </is>
       </c>
       <c r="D77" s="3" t="inlineStr">
@@ -10174,17 +10174,17 @@
     <row r="78" ht="25" customHeight="1">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>Newlands</t>
+          <t>Ngobozana</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
         <is>
-          <t>Mike</t>
+          <t>Sphiwe</t>
         </is>
       </c>
       <c r="C78" s="3" t="inlineStr">
         <is>
-          <t>Port Alfred</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D78" s="3" t="inlineStr">
@@ -10194,24 +10194,24 @@
       </c>
       <c r="E78" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="79" ht="25" customHeight="1">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>Ngobozana</t>
+          <t>Oberholzer</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
         <is>
-          <t>Sphiwe</t>
+          <t>PDG Bokkie</t>
         </is>
       </c>
       <c r="C79" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Uitenhage</t>
         </is>
       </c>
       <c r="D79" s="3" t="inlineStr">
@@ -10228,17 +10228,17 @@
     <row r="80" ht="25" customHeight="1">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>Oberholzer</t>
+          <t>PORTEOUS</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
         <is>
-          <t>PDG Bokkie</t>
+          <t>BRIAN</t>
         </is>
       </c>
       <c r="C80" s="3" t="inlineStr">
         <is>
-          <t>Uitenhage</t>
+          <t>Hibberdene</t>
         </is>
       </c>
       <c r="D80" s="3" t="inlineStr">
@@ -10248,24 +10248,24 @@
       </c>
       <c r="E80" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="81" ht="25" customHeight="1">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>PORTEOUS</t>
+          <t>Paijmans</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
         <is>
-          <t>BRIAN</t>
+          <t>Bronwyn Anne</t>
         </is>
       </c>
       <c r="C81" s="3" t="inlineStr">
         <is>
-          <t>Hibberdene</t>
+          <t>Cowies Hill</t>
         </is>
       </c>
       <c r="D81" s="3" t="inlineStr">
@@ -10275,24 +10275,24 @@
       </c>
       <c r="E81" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="82" ht="25" customHeight="1">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>Paijmans</t>
+          <t>Pantoleon</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
         <is>
-          <t>Bronwyn Anne</t>
+          <t>Teresa</t>
         </is>
       </c>
       <c r="C82" s="3" t="inlineStr">
         <is>
-          <t>Cowies Hill</t>
+          <t>Vereeniging</t>
         </is>
       </c>
       <c r="D82" s="3" t="inlineStr">
@@ -10302,24 +10302,24 @@
       </c>
       <c r="E82" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="83" ht="25" customHeight="1">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>Pantoleon</t>
+          <t>Polkinghorne</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
         <is>
-          <t>Teresa</t>
+          <t>Tracey</t>
         </is>
       </c>
       <c r="C83" s="3" t="inlineStr">
         <is>
-          <t>Vereeniging</t>
+          <t>Kensington</t>
         </is>
       </c>
       <c r="D83" s="3" t="inlineStr">
@@ -10341,7 +10341,7 @@
       </c>
       <c r="B84" s="3" t="inlineStr">
         <is>
-          <t>Tracey</t>
+          <t>Gavin</t>
         </is>
       </c>
       <c r="C84" s="3" t="inlineStr">
@@ -10356,29 +10356,29 @@
       </c>
       <c r="E84" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="85" ht="25" customHeight="1">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>Polkinghorne</t>
+          <t>Rashirai</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
         <is>
-          <t>Gavin</t>
+          <t>Tabeth</t>
         </is>
       </c>
       <c r="C85" s="3" t="inlineStr">
         <is>
-          <t>Kensington</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D85" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E85" s="3" t="inlineStr">
@@ -10390,17 +10390,17 @@
     <row r="86" ht="25" customHeight="1">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>Ras</t>
+          <t>Reniers</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
         <is>
-          <t>Leon Jacobus</t>
+          <t>Hugo</t>
         </is>
       </c>
       <c r="C86" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Nelspruit</t>
         </is>
       </c>
       <c r="D86" s="3" t="inlineStr">
@@ -10410,51 +10410,51 @@
       </c>
       <c r="E86" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="87" ht="25" customHeight="1">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>Rashirai</t>
+          <t>Sabatier</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
         <is>
-          <t>Tabeth</t>
+          <t>Rodney</t>
         </is>
       </c>
       <c r="C87" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D87" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E87" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="88" ht="25" customHeight="1">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>Reniers</t>
+          <t>Searle</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
         <is>
-          <t>Hugo</t>
+          <t>Francis</t>
         </is>
       </c>
       <c r="C88" s="3" t="inlineStr">
         <is>
-          <t>Nelspruit</t>
+          <t>Kouga</t>
         </is>
       </c>
       <c r="D88" s="3" t="inlineStr">
@@ -10471,17 +10471,17 @@
     <row r="89" ht="25" customHeight="1">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>Sabatier</t>
+          <t>Searle</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
         <is>
-          <t>Rodney</t>
+          <t>Gloria</t>
         </is>
       </c>
       <c r="C89" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Kouga</t>
         </is>
       </c>
       <c r="D89" s="3" t="inlineStr">
@@ -10491,24 +10491,24 @@
       </c>
       <c r="E89" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="90" ht="25" customHeight="1">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>Searle</t>
+          <t>Smit</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
         <is>
-          <t>Francis</t>
+          <t>Sue</t>
         </is>
       </c>
       <c r="C90" s="3" t="inlineStr">
         <is>
-          <t>Kouga</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D90" s="3" t="inlineStr">
@@ -10518,24 +10518,24 @@
       </c>
       <c r="E90" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="91" ht="25" customHeight="1">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>Searle</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
         <is>
-          <t>Gloria</t>
+          <t>Jeff</t>
         </is>
       </c>
       <c r="C91" s="3" t="inlineStr">
         <is>
-          <t>Kouga</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D91" s="3" t="inlineStr">
@@ -10552,17 +10552,17 @@
     <row r="92" ht="25" customHeight="1">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>Smit</t>
+          <t>Stander</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
         <is>
-          <t>Sue</t>
+          <t>Max</t>
         </is>
       </c>
       <c r="C92" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Port Alfred</t>
         </is>
       </c>
       <c r="D92" s="3" t="inlineStr">
@@ -10579,17 +10579,17 @@
     <row r="93" ht="25" customHeight="1">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Stander</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
         <is>
-          <t>Jeff</t>
+          <t>Ashley</t>
         </is>
       </c>
       <c r="C93" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Krugersdorp</t>
         </is>
       </c>
       <c r="D93" s="3" t="inlineStr">
@@ -10599,7 +10599,7 @@
       </c>
       <c r="E93" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -10611,12 +10611,12 @@
       </c>
       <c r="B94" s="3" t="inlineStr">
         <is>
-          <t>Max</t>
+          <t>Brett Jason</t>
         </is>
       </c>
       <c r="C94" s="3" t="inlineStr">
         <is>
-          <t>Port Alfred</t>
+          <t>Krugersdorp</t>
         </is>
       </c>
       <c r="D94" s="3" t="inlineStr">
@@ -10633,44 +10633,44 @@
     <row r="95" ht="25" customHeight="1">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>Stander</t>
+          <t>Steyn</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
         <is>
-          <t>Ashley</t>
+          <t>Elna</t>
         </is>
       </c>
       <c r="C95" s="3" t="inlineStr">
         <is>
-          <t>Krugersdorp</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D95" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E95" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="96" ht="25" customHeight="1">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>Stander</t>
+          <t>Sturges</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
         <is>
-          <t>Brett Jason</t>
+          <t>Trevor</t>
         </is>
       </c>
       <c r="C96" s="3" t="inlineStr">
         <is>
-          <t>Krugersdorp</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D96" s="3" t="inlineStr">
@@ -10687,22 +10687,22 @@
     <row r="97" ht="25" customHeight="1">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>Steyn</t>
+          <t>Talbot</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
         <is>
-          <t>Elna</t>
+          <t>Lauryn</t>
         </is>
       </c>
       <c r="C97" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Benoni Lakes</t>
         </is>
       </c>
       <c r="D97" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E97" s="3" t="inlineStr">
@@ -10714,12 +10714,12 @@
     <row r="98" ht="25" customHeight="1">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>Sturges</t>
+          <t>Theron</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
         <is>
-          <t>Trevor</t>
+          <t>Pierre</t>
         </is>
       </c>
       <c r="C98" s="3" t="inlineStr">
@@ -10741,17 +10741,17 @@
     <row r="99" ht="25" customHeight="1">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>Talbot</t>
+          <t>Theron</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
         <is>
-          <t>Lauryn</t>
+          <t>Moira</t>
         </is>
       </c>
       <c r="C99" s="3" t="inlineStr">
         <is>
-          <t>Benoni Lakes</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D99" s="3" t="inlineStr">
@@ -10768,17 +10768,17 @@
     <row r="100" ht="25" customHeight="1">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>Theron</t>
+          <t>Townsend</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
         <is>
-          <t>Pierre</t>
+          <t>Diane</t>
         </is>
       </c>
       <c r="C100" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Benoni Lakes</t>
         </is>
       </c>
       <c r="D100" s="3" t="inlineStr">
@@ -10788,29 +10788,29 @@
       </c>
       <c r="E100" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="101" ht="25" customHeight="1">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>Theron</t>
+          <t>Toye</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
         <is>
-          <t>Moira</t>
+          <t>Omolayo</t>
         </is>
       </c>
       <c r="C101" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>The Wilds</t>
         </is>
       </c>
       <c r="D101" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E101" s="3" t="inlineStr">
@@ -10822,17 +10822,17 @@
     <row r="102" ht="25" customHeight="1">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>Townsend</t>
+          <t>Tuckett</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
         <is>
-          <t>Diane</t>
+          <t>Alistair</t>
         </is>
       </c>
       <c r="C102" s="3" t="inlineStr">
         <is>
-          <t>Benoni Lakes</t>
+          <t>Roodepoort Clearwater Cyber</t>
         </is>
       </c>
       <c r="D102" s="3" t="inlineStr">
@@ -10842,34 +10842,34 @@
       </c>
       <c r="E102" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="103" ht="25" customHeight="1">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>Toye</t>
+          <t>Tuckett</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
         <is>
-          <t>Omolayo</t>
+          <t>Rowan</t>
         </is>
       </c>
       <c r="C103" s="3" t="inlineStr">
         <is>
-          <t>The Wilds</t>
+          <t>Roodepoort Clearwater Cyber</t>
         </is>
       </c>
       <c r="D103" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E103" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -10881,7 +10881,7 @@
       </c>
       <c r="B104" s="3" t="inlineStr">
         <is>
-          <t>Alistair</t>
+          <t>Gail</t>
         </is>
       </c>
       <c r="C104" s="3" t="inlineStr">
@@ -10903,71 +10903,71 @@
     <row r="105" ht="25" customHeight="1">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>Tuckett</t>
+          <t>Uchytil</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
         <is>
-          <t>Rowan</t>
+          <t>Jiri</t>
         </is>
       </c>
       <c r="C105" s="3" t="inlineStr">
         <is>
-          <t>Roodepoort Clearwater Cyber</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D105" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E105" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="106" ht="25" customHeight="1">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>Tuckett</t>
+          <t>VAN DER MERWE</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
         <is>
-          <t>Gail</t>
+          <t>PATRICIA</t>
         </is>
       </c>
       <c r="C106" s="3" t="inlineStr">
         <is>
-          <t>Roodepoort Clearwater Cyber</t>
+          <t>East London Port Rex</t>
         </is>
       </c>
       <c r="D106" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E106" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="107" ht="25" customHeight="1">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>Uchytil</t>
+          <t>Van Niekerk</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
         <is>
-          <t>Jiri</t>
+          <t>Riaan</t>
         </is>
       </c>
       <c r="C107" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D107" s="3" t="inlineStr">
@@ -10984,17 +10984,17 @@
     <row r="108" ht="25" customHeight="1">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>VAN DER MERWE</t>
+          <t>Venter</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
         <is>
-          <t>PATRICIA</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="C108" s="3" t="inlineStr">
         <is>
-          <t>East London Port Rex</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D108" s="3" t="inlineStr">
@@ -11004,51 +11004,51 @@
       </c>
       <c r="E108" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="109" ht="25" customHeight="1">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>Van Niekerk</t>
+          <t>Volker</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
         <is>
-          <t>Riaan</t>
+          <t>Russell</t>
         </is>
       </c>
       <c r="C109" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>King William's Town</t>
         </is>
       </c>
       <c r="D109" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E109" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="110" ht="25" customHeight="1">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>Van Nieuwenhuyzen</t>
+          <t>Warman</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
         <is>
-          <t>Hilgardt</t>
+          <t>Alastair</t>
         </is>
       </c>
       <c r="C110" s="3" t="inlineStr">
         <is>
-          <t>Worcester</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D110" s="3" t="inlineStr">
@@ -11058,29 +11058,29 @@
       </c>
       <c r="E110" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="111" ht="25" customHeight="1">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>Venter</t>
+          <t>Williamson</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
         <is>
-          <t>Louis</t>
+          <t>Neville</t>
         </is>
       </c>
       <c r="C111" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Port Alfred</t>
         </is>
       </c>
       <c r="D111" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E111" s="3" t="inlineStr">
@@ -11092,17 +11092,17 @@
     <row r="112" ht="25" customHeight="1">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>Volker</t>
+          <t>Wilter-Sturges</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
         <is>
-          <t>Russell</t>
+          <t>Meredith</t>
         </is>
       </c>
       <c r="C112" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D112" s="3" t="inlineStr">
@@ -11112,51 +11112,51 @@
       </c>
       <c r="E112" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="113" ht="25" customHeight="1">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>Warman</t>
+          <t>de Silva</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
         <is>
-          <t>Alastair</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="C113" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Edenvale</t>
         </is>
       </c>
       <c r="D113" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E113" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="114" ht="25" customHeight="1">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>Williamson</t>
+          <t>du Plooy</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
         <is>
-          <t>Neville</t>
+          <t>Tammy</t>
         </is>
       </c>
       <c r="C114" s="3" t="inlineStr">
         <is>
-          <t>Port Alfred</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D114" s="3" t="inlineStr">
@@ -11166,24 +11166,24 @@
       </c>
       <c r="E114" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="115" ht="25" customHeight="1">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>Wilter-Sturges</t>
+          <t>du Plooy</t>
         </is>
       </c>
       <c r="B115" s="3" t="inlineStr">
         <is>
-          <t>Meredith</t>
+          <t>Marc</t>
         </is>
       </c>
       <c r="C115" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D115" s="3" t="inlineStr">
@@ -11193,51 +11193,51 @@
       </c>
       <c r="E115" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="116" ht="25" customHeight="1">
       <c r="A116" s="3" t="inlineStr">
         <is>
-          <t>de Silva</t>
+          <t>du Toit</t>
         </is>
       </c>
       <c r="B116" s="3" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Desiree</t>
         </is>
       </c>
       <c r="C116" s="3" t="inlineStr">
         <is>
-          <t>Edenvale</t>
+          <t>Ramsgate</t>
         </is>
       </c>
       <c r="D116" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E116" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="117" ht="25" customHeight="1">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>du Plooy</t>
+          <t>le Roux</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
         <is>
-          <t>Tammy</t>
+          <t>Jeanette</t>
         </is>
       </c>
       <c r="C117" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Gonubie</t>
         </is>
       </c>
       <c r="D117" s="3" t="inlineStr">
@@ -11254,17 +11254,17 @@
     <row r="118" ht="25" customHeight="1">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>du Plooy</t>
+          <t>van Heerden</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
         <is>
-          <t>Marc</t>
+          <t>Sydney</t>
         </is>
       </c>
       <c r="C118" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D118" s="3" t="inlineStr">
@@ -11274,24 +11274,24 @@
       </c>
       <c r="E118" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="119" ht="25" customHeight="1">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>du Toit</t>
+          <t>van Heerden</t>
         </is>
       </c>
       <c r="B119" s="3" t="inlineStr">
         <is>
-          <t>Desiree</t>
+          <t>Sandy</t>
         </is>
       </c>
       <c r="C119" s="3" t="inlineStr">
         <is>
-          <t>Ramsgate</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D119" s="3" t="inlineStr">
@@ -11308,22 +11308,22 @@
     <row r="120" ht="25" customHeight="1">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>le Roux</t>
+          <t>van Heerden</t>
         </is>
       </c>
       <c r="B120" s="3" t="inlineStr">
         <is>
-          <t>Jeanette</t>
+          <t>Craig</t>
         </is>
       </c>
       <c r="C120" s="3" t="inlineStr">
         <is>
-          <t>Gonubie</t>
+          <t>East London Beacon Bay</t>
         </is>
       </c>
       <c r="D120" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E120" s="3" t="inlineStr">
@@ -11340,12 +11340,12 @@
       </c>
       <c r="B121" s="3" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C121" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D121" s="3" t="inlineStr">
@@ -11355,24 +11355,24 @@
       </c>
       <c r="E121" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="122" ht="25" customHeight="1">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>van Heerden</t>
+          <t>van Wyk</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
         <is>
-          <t>Sandy</t>
+          <t>Kim</t>
         </is>
       </c>
       <c r="C122" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>North Durban</t>
         </is>
       </c>
       <c r="D122" s="3" t="inlineStr">
@@ -11382,51 +11382,51 @@
       </c>
       <c r="E122" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="123" ht="25" customHeight="1">
       <c r="A123" s="3" t="inlineStr">
         <is>
-          <t>van Heerden</t>
+          <t>van Wyk</t>
         </is>
       </c>
       <c r="B123" s="3" t="inlineStr">
         <is>
-          <t>Craig</t>
+          <t>Lindie</t>
         </is>
       </c>
       <c r="C123" s="3" t="inlineStr">
         <is>
-          <t>East London Beacon Bay</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D123" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E123" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="124" ht="25" customHeight="1">
       <c r="A124" s="3" t="inlineStr">
         <is>
-          <t>van Heerden</t>
+          <t>van Wyk</t>
         </is>
       </c>
       <c r="B124" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Willem</t>
         </is>
       </c>
       <c r="C124" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D124" s="3" t="inlineStr">
@@ -11436,7 +11436,7 @@
       </c>
       <c r="E124" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -11448,12 +11448,12 @@
       </c>
       <c r="B125" s="3" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>Patricia</t>
         </is>
       </c>
       <c r="C125" s="3" t="inlineStr">
         <is>
-          <t>North Durban</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D125" s="3" t="inlineStr">
@@ -11470,22 +11470,22 @@
     <row r="126" ht="25" customHeight="1">
       <c r="A126" s="3" t="inlineStr">
         <is>
-          <t>van Wyk</t>
+          <t>van der Merwe</t>
         </is>
       </c>
       <c r="B126" s="3" t="inlineStr">
         <is>
-          <t>Lindie</t>
+          <t>Ingrid</t>
         </is>
       </c>
       <c r="C126" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D126" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E126" s="3" t="inlineStr">
@@ -11497,17 +11497,17 @@
     <row r="127" ht="25" customHeight="1">
       <c r="A127" s="3" t="inlineStr">
         <is>
-          <t>van Wyk</t>
+          <t>von der Decken</t>
         </is>
       </c>
       <c r="B127" s="3" t="inlineStr">
         <is>
-          <t>Willem</t>
+          <t>Brian</t>
         </is>
       </c>
       <c r="C127" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>King William's Town</t>
         </is>
       </c>
       <c r="D127" s="3" t="inlineStr">
@@ -11517,24 +11517,24 @@
       </c>
       <c r="E127" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="128" ht="25" customHeight="1">
       <c r="A128" s="3" t="inlineStr">
         <is>
-          <t>van Wyk</t>
+          <t>‘t Hart</t>
         </is>
       </c>
       <c r="B128" s="3" t="inlineStr">
         <is>
-          <t>Patricia</t>
+          <t>Michelle</t>
         </is>
       </c>
       <c r="C128" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Benoni Lakes</t>
         </is>
       </c>
       <c r="D128" s="3" t="inlineStr">
@@ -11548,96 +11548,15 @@
         </is>
       </c>
     </row>
-    <row r="129" ht="25" customHeight="1">
-      <c r="A129" s="3" t="inlineStr">
-        <is>
-          <t>van der Merwe</t>
-        </is>
-      </c>
-      <c r="B129" s="3" t="inlineStr">
-        <is>
-          <t>Ingrid</t>
-        </is>
-      </c>
-      <c r="C129" s="3" t="inlineStr">
-        <is>
-          <t>Letaba Tzaneen</t>
-        </is>
-      </c>
-      <c r="D129" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="E129" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="130" ht="25" customHeight="1">
-      <c r="A130" s="3" t="inlineStr">
-        <is>
-          <t>von der Decken</t>
-        </is>
-      </c>
-      <c r="B130" s="3" t="inlineStr">
-        <is>
-          <t>Brian</t>
-        </is>
-      </c>
-      <c r="C130" s="3" t="inlineStr">
-        <is>
-          <t>King William's Town</t>
-        </is>
-      </c>
-      <c r="D130" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E130" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-    </row>
-    <row r="131" ht="25" customHeight="1">
-      <c r="A131" s="3" t="inlineStr">
-        <is>
-          <t>‘t Hart</t>
-        </is>
-      </c>
-      <c r="B131" s="3" t="inlineStr">
-        <is>
-          <t>Michelle</t>
-        </is>
-      </c>
-      <c r="C131" s="3" t="inlineStr">
-        <is>
-          <t>Benoni Lakes</t>
-        </is>
-      </c>
-      <c r="D131" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E131" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="132">
-      <c r="A132" s="1" t="inlineStr">
-        <is>
-          <t>Number of attendees: 129</t>
-        </is>
-      </c>
-    </row>
-    <row r="133">
-      <c r="A133" s="1" t="inlineStr">
+    <row r="129">
+      <c r="A129" s="1" t="inlineStr">
+        <is>
+          <t>Number of attendees: 126</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="inlineStr">
         <is>
           <t>Number of voters: 52</t>
         </is>
@@ -11655,7 +11574,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E152"/>
+  <dimension ref="A1:E154"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11673,7 +11592,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Registrees as of 21/04/2021 13:45</t>
+          <t>410W Registrees as of 21/04/2021 13:58</t>
         </is>
       </c>
     </row>
@@ -14434,17 +14353,17 @@
     <row r="104" ht="25" customHeight="1">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>Rossouw</t>
+          <t>Ras</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Leon Jacobus</t>
         </is>
       </c>
       <c r="C104" s="3" t="inlineStr">
         <is>
-          <t>Tokai</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D104" s="3" t="inlineStr">
@@ -14454,24 +14373,24 @@
       </c>
       <c r="E104" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="105" ht="25" customHeight="1">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>Rothner</t>
+          <t>Rossouw</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
         <is>
-          <t>Andrea</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C105" s="3" t="inlineStr">
         <is>
-          <t>Eden</t>
+          <t>Tokai</t>
         </is>
       </c>
       <c r="D105" s="3" t="inlineStr">
@@ -14481,24 +14400,24 @@
       </c>
       <c r="E105" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="106" ht="25" customHeight="1">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>Roux</t>
+          <t>Rothner</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
         <is>
-          <t>Anthonie Petrus</t>
+          <t>Andrea</t>
         </is>
       </c>
       <c r="C106" s="3" t="inlineStr">
         <is>
-          <t>Moorreesburg</t>
+          <t>Eden</t>
         </is>
       </c>
       <c r="D106" s="3" t="inlineStr">
@@ -14508,24 +14427,24 @@
       </c>
       <c r="E106" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="107" ht="25" customHeight="1">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>Russell</t>
+          <t>Roux</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
         <is>
-          <t>Ingrid</t>
+          <t>Anthonie Petrus</t>
         </is>
       </c>
       <c r="C107" s="3" t="inlineStr">
         <is>
-          <t>Fish Hoek</t>
+          <t>Moorreesburg</t>
         </is>
       </c>
       <c r="D107" s="3" t="inlineStr">
@@ -14542,71 +14461,71 @@
     <row r="108" ht="25" customHeight="1">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>SNYMAN</t>
+          <t>Russell</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
         <is>
-          <t>LYN</t>
+          <t>Ingrid</t>
         </is>
       </c>
       <c r="C108" s="3" t="inlineStr">
         <is>
-          <t>Deep South</t>
+          <t>Fish Hoek</t>
         </is>
       </c>
       <c r="D108" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E108" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="109" ht="25" customHeight="1">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>STEENBERG</t>
+          <t>SNYMAN</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
         <is>
-          <t>TIM</t>
+          <t>LYN</t>
         </is>
       </c>
       <c r="C109" s="3" t="inlineStr">
         <is>
-          <t>Wellington</t>
+          <t>Deep South</t>
         </is>
       </c>
       <c r="D109" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E109" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="110" ht="25" customHeight="1">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>Sampie</t>
+          <t>STEENBERG</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
         <is>
-          <t>Sharon</t>
+          <t>TIM</t>
         </is>
       </c>
       <c r="C110" s="3" t="inlineStr">
         <is>
-          <t>Bergvliet</t>
+          <t>Wellington</t>
         </is>
       </c>
       <c r="D110" s="3" t="inlineStr">
@@ -14623,17 +14542,17 @@
     <row r="111" ht="25" customHeight="1">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>Schatz</t>
+          <t>Sampie</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
         <is>
-          <t>Vera</t>
+          <t>Sharon</t>
         </is>
       </c>
       <c r="C111" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Bergvliet</t>
         </is>
       </c>
       <c r="D111" s="3" t="inlineStr">
@@ -14655,7 +14574,7 @@
       </c>
       <c r="B112" s="3" t="inlineStr">
         <is>
-          <t>Frank</t>
+          <t>Vera</t>
         </is>
       </c>
       <c r="C112" s="3" t="inlineStr">
@@ -14670,19 +14589,19 @@
       </c>
       <c r="E112" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="113" ht="25" customHeight="1">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>Sell</t>
+          <t>Schatz</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
         <is>
-          <t>Ami</t>
+          <t>Frank</t>
         </is>
       </c>
       <c r="C113" s="3" t="inlineStr">
@@ -14704,17 +14623,17 @@
     <row r="114" ht="25" customHeight="1">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>Simpson</t>
+          <t>Sell</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
         <is>
-          <t>Beryl</t>
+          <t>Ami</t>
         </is>
       </c>
       <c r="C114" s="3" t="inlineStr">
         <is>
-          <t>Cape Town</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D114" s="3" t="inlineStr">
@@ -14731,17 +14650,17 @@
     <row r="115" ht="25" customHeight="1">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>Sircoulomb</t>
+          <t>Simpson</t>
         </is>
       </c>
       <c r="B115" s="3" t="inlineStr">
         <is>
-          <t>Kenlis</t>
+          <t>Beryl</t>
         </is>
       </c>
       <c r="C115" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Cape Town</t>
         </is>
       </c>
       <c r="D115" s="3" t="inlineStr">
@@ -14763,7 +14682,7 @@
       </c>
       <c r="B116" s="3" t="inlineStr">
         <is>
-          <t>Holger</t>
+          <t>Kenlis</t>
         </is>
       </c>
       <c r="C116" s="3" t="inlineStr">
@@ -14778,24 +14697,24 @@
       </c>
       <c r="E116" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="117" ht="25" customHeight="1">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>Smit</t>
+          <t>Sircoulomb</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
         <is>
-          <t>Herman</t>
+          <t>Holger</t>
         </is>
       </c>
       <c r="C117" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D117" s="3" t="inlineStr">
@@ -14805,24 +14724,24 @@
       </c>
       <c r="E117" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="118" ht="25" customHeight="1">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Smit</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
         <is>
-          <t>Bennie</t>
+          <t>Herman</t>
         </is>
       </c>
       <c r="C118" s="3" t="inlineStr">
         <is>
-          <t>Wellington</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D118" s="3" t="inlineStr">
@@ -14832,7 +14751,7 @@
       </c>
       <c r="E118" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -14844,12 +14763,12 @@
       </c>
       <c r="B119" s="3" t="inlineStr">
         <is>
-          <t>Carmen Dolores</t>
+          <t>Bennie</t>
         </is>
       </c>
       <c r="C119" s="3" t="inlineStr">
         <is>
-          <t>Tokai</t>
+          <t>Wellington</t>
         </is>
       </c>
       <c r="D119" s="3" t="inlineStr">
@@ -14859,7 +14778,7 @@
       </c>
       <c r="E119" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -14871,7 +14790,7 @@
       </c>
       <c r="B120" s="3" t="inlineStr">
         <is>
-          <t>David John</t>
+          <t>Carmen Dolores</t>
         </is>
       </c>
       <c r="C120" s="3" t="inlineStr">
@@ -14893,17 +14812,17 @@
     <row r="121" ht="25" customHeight="1">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>Sochen</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="B121" s="3" t="inlineStr">
         <is>
-          <t>Diana</t>
+          <t>David John</t>
         </is>
       </c>
       <c r="C121" s="3" t="inlineStr">
         <is>
-          <t>Sea Point</t>
+          <t>Tokai</t>
         </is>
       </c>
       <c r="D121" s="3" t="inlineStr">
@@ -14913,56 +14832,56 @@
       </c>
       <c r="E121" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="122" ht="25" customHeight="1">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>Strauss</t>
+          <t>Sochen</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>Diana</t>
         </is>
       </c>
       <c r="C122" s="3" t="inlineStr">
         <is>
-          <t>Kuilsriver</t>
+          <t>Sea Point</t>
         </is>
       </c>
       <c r="D122" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E122" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="123" ht="25" customHeight="1">
       <c r="A123" s="3" t="inlineStr">
         <is>
-          <t>Tshikala</t>
+          <t>Strauss</t>
         </is>
       </c>
       <c r="B123" s="3" t="inlineStr">
         <is>
-          <t>David Alex</t>
+          <t>Patrick</t>
         </is>
       </c>
       <c r="C123" s="3" t="inlineStr">
         <is>
-          <t>Athlone</t>
+          <t>Kuilsriver</t>
         </is>
       </c>
       <c r="D123" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E123" s="3" t="inlineStr">
@@ -14974,17 +14893,17 @@
     <row r="124" ht="25" customHeight="1">
       <c r="A124" s="3" t="inlineStr">
         <is>
-          <t>VAN BREDA</t>
+          <t>Tshikala</t>
         </is>
       </c>
       <c r="B124" s="3" t="inlineStr">
         <is>
-          <t>HILARY LISE</t>
+          <t>David Alex</t>
         </is>
       </c>
       <c r="C124" s="3" t="inlineStr">
         <is>
-          <t>Cape Town</t>
+          <t>Athlone</t>
         </is>
       </c>
       <c r="D124" s="3" t="inlineStr">
@@ -15001,17 +14920,17 @@
     <row r="125" ht="25" customHeight="1">
       <c r="A125" s="3" t="inlineStr">
         <is>
-          <t>VAN DER MERWE</t>
+          <t>VAN BREDA</t>
         </is>
       </c>
       <c r="B125" s="3" t="inlineStr">
         <is>
-          <t>MARINA</t>
+          <t>HILARY LISE</t>
         </is>
       </c>
       <c r="C125" s="3" t="inlineStr">
         <is>
-          <t>Malmesbury</t>
+          <t>Cape Town</t>
         </is>
       </c>
       <c r="D125" s="3" t="inlineStr">
@@ -15021,24 +14940,24 @@
       </c>
       <c r="E125" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="126" ht="25" customHeight="1">
       <c r="A126" s="3" t="inlineStr">
         <is>
-          <t>Van Rensburg</t>
+          <t>VAN DER MERWE</t>
         </is>
       </c>
       <c r="B126" s="3" t="inlineStr">
         <is>
-          <t>Neville</t>
+          <t>MARINA</t>
         </is>
       </c>
       <c r="C126" s="3" t="inlineStr">
         <is>
-          <t>Moorreesburg</t>
+          <t>Malmesbury</t>
         </is>
       </c>
       <c r="D126" s="3" t="inlineStr">
@@ -15055,22 +14974,22 @@
     <row r="127" ht="25" customHeight="1">
       <c r="A127" s="3" t="inlineStr">
         <is>
-          <t>Van Romburgh</t>
+          <t>Van Nieuwenhuyzen</t>
         </is>
       </c>
       <c r="B127" s="3" t="inlineStr">
         <is>
-          <t>Lorna</t>
+          <t>Hilgardt</t>
         </is>
       </c>
       <c r="C127" s="3" t="inlineStr">
         <is>
-          <t>Fish Hoek</t>
+          <t>Worcester</t>
         </is>
       </c>
       <c r="D127" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E127" s="3" t="inlineStr">
@@ -15082,49 +15001,49 @@
     <row r="128" ht="25" customHeight="1">
       <c r="A128" s="3" t="inlineStr">
         <is>
-          <t>Van Wyk-Nelson</t>
+          <t>Van Rensburg</t>
         </is>
       </c>
       <c r="B128" s="3" t="inlineStr">
         <is>
-          <t>Edith</t>
+          <t>Neville</t>
         </is>
       </c>
       <c r="C128" s="3" t="inlineStr">
         <is>
-          <t>Kuilsriver</t>
+          <t>Moorreesburg</t>
         </is>
       </c>
       <c r="D128" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E128" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="129" ht="25" customHeight="1">
       <c r="A129" s="3" t="inlineStr">
         <is>
-          <t>Van de Merwe</t>
+          <t>Van Romburgh</t>
         </is>
       </c>
       <c r="B129" s="3" t="inlineStr">
         <is>
-          <t>Marina</t>
+          <t>Lorna</t>
         </is>
       </c>
       <c r="C129" s="3" t="inlineStr">
         <is>
-          <t>Malmesbury</t>
+          <t>Fish Hoek</t>
         </is>
       </c>
       <c r="D129" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E129" s="3" t="inlineStr">
@@ -15136,17 +15055,17 @@
     <row r="130" ht="25" customHeight="1">
       <c r="A130" s="3" t="inlineStr">
         <is>
-          <t>Von Mollendorf</t>
+          <t>Van Wyk-Nelson</t>
         </is>
       </c>
       <c r="B130" s="3" t="inlineStr">
         <is>
-          <t>Rinette</t>
+          <t>Edith</t>
         </is>
       </c>
       <c r="C130" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>Kuilsriver</t>
         </is>
       </c>
       <c r="D130" s="3" t="inlineStr">
@@ -15163,17 +15082,17 @@
     <row r="131" ht="25" customHeight="1">
       <c r="A131" s="3" t="inlineStr">
         <is>
-          <t>Vorster</t>
+          <t>Van de Merwe</t>
         </is>
       </c>
       <c r="B131" s="3" t="inlineStr">
         <is>
-          <t>Rochelle</t>
+          <t>Marina</t>
         </is>
       </c>
       <c r="C131" s="3" t="inlineStr">
         <is>
-          <t>Sedgefield</t>
+          <t>Malmesbury</t>
         </is>
       </c>
       <c r="D131" s="3" t="inlineStr">
@@ -15190,17 +15109,17 @@
     <row r="132" ht="25" customHeight="1">
       <c r="A132" s="3" t="inlineStr">
         <is>
-          <t>Watson</t>
+          <t>Von Mollendorf</t>
         </is>
       </c>
       <c r="B132" s="3" t="inlineStr">
         <is>
-          <t>Allan</t>
+          <t>Rinette</t>
         </is>
       </c>
       <c r="C132" s="3" t="inlineStr">
         <is>
-          <t>Sea Point</t>
+          <t>Durbanville</t>
         </is>
       </c>
       <c r="D132" s="3" t="inlineStr">
@@ -15217,12 +15136,12 @@
     <row r="133" ht="25" customHeight="1">
       <c r="A133" s="3" t="inlineStr">
         <is>
-          <t>Watson</t>
+          <t>Vorster</t>
         </is>
       </c>
       <c r="B133" s="3" t="inlineStr">
         <is>
-          <t>Alison</t>
+          <t>Rochelle</t>
         </is>
       </c>
       <c r="C133" s="3" t="inlineStr">
@@ -15237,24 +15156,24 @@
       </c>
       <c r="E133" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="134" ht="25" customHeight="1">
       <c r="A134" s="3" t="inlineStr">
         <is>
-          <t>Williams</t>
+          <t>Watson</t>
         </is>
       </c>
       <c r="B134" s="3" t="inlineStr">
         <is>
-          <t>Johanna</t>
+          <t>Allan</t>
         </is>
       </c>
       <c r="C134" s="3" t="inlineStr">
         <is>
-          <t>Mitchells Plain</t>
+          <t>Sea Point</t>
         </is>
       </c>
       <c r="D134" s="3" t="inlineStr">
@@ -15271,17 +15190,17 @@
     <row r="135" ht="25" customHeight="1">
       <c r="A135" s="3" t="inlineStr">
         <is>
-          <t>Wills</t>
+          <t>Watson</t>
         </is>
       </c>
       <c r="B135" s="3" t="inlineStr">
         <is>
-          <t>Geila</t>
+          <t>Alison</t>
         </is>
       </c>
       <c r="C135" s="3" t="inlineStr">
         <is>
-          <t>Athlone</t>
+          <t>Sedgefield</t>
         </is>
       </c>
       <c r="D135" s="3" t="inlineStr">
@@ -15291,19 +15210,19 @@
       </c>
       <c r="E135" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="136" ht="25" customHeight="1">
       <c r="A136" s="3" t="inlineStr">
         <is>
-          <t>Woodman</t>
+          <t>Williams</t>
         </is>
       </c>
       <c r="B136" s="3" t="inlineStr">
         <is>
-          <t>Joan</t>
+          <t>Johanna</t>
         </is>
       </c>
       <c r="C136" s="3" t="inlineStr">
@@ -15325,17 +15244,17 @@
     <row r="137" ht="25" customHeight="1">
       <c r="A137" s="3" t="inlineStr">
         <is>
-          <t>Wright</t>
+          <t>Wills</t>
         </is>
       </c>
       <c r="B137" s="3" t="inlineStr">
         <is>
-          <t>Rocky</t>
+          <t>Geila</t>
         </is>
       </c>
       <c r="C137" s="3" t="inlineStr">
         <is>
-          <t>Table View</t>
+          <t>Athlone</t>
         </is>
       </c>
       <c r="D137" s="3" t="inlineStr">
@@ -15345,29 +15264,29 @@
       </c>
       <c r="E137" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="138" ht="25" customHeight="1">
       <c r="A138" s="3" t="inlineStr">
         <is>
-          <t>Young</t>
+          <t>Woodman</t>
         </is>
       </c>
       <c r="B138" s="3" t="inlineStr">
         <is>
-          <t>Judy</t>
+          <t>Joan</t>
         </is>
       </c>
       <c r="C138" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>Mitchells Plain</t>
         </is>
       </c>
       <c r="D138" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E138" s="3" t="inlineStr">
@@ -15379,44 +15298,44 @@
     <row r="139" ht="25" customHeight="1">
       <c r="A139" s="3" t="inlineStr">
         <is>
-          <t>Young</t>
+          <t>Wright</t>
         </is>
       </c>
       <c r="B139" s="3" t="inlineStr">
         <is>
-          <t>Gerry</t>
+          <t>Rocky</t>
         </is>
       </c>
       <c r="C139" s="3" t="inlineStr">
         <is>
-          <t>Mitchells Plain</t>
+          <t>Table View</t>
         </is>
       </c>
       <c r="D139" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E139" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="140" ht="25" customHeight="1">
       <c r="A140" s="3" t="inlineStr">
         <is>
-          <t>Zucker</t>
+          <t>Young</t>
         </is>
       </c>
       <c r="B140" s="3" t="inlineStr">
         <is>
-          <t>Leonie</t>
+          <t>Judy</t>
         </is>
       </c>
       <c r="C140" s="3" t="inlineStr">
         <is>
-          <t>Milnerton</t>
+          <t>Durbanville</t>
         </is>
       </c>
       <c r="D140" s="3" t="inlineStr">
@@ -15433,44 +15352,44 @@
     <row r="141" ht="25" customHeight="1">
       <c r="A141" s="3" t="inlineStr">
         <is>
-          <t>de Kock</t>
+          <t>Young</t>
         </is>
       </c>
       <c r="B141" s="3" t="inlineStr">
         <is>
-          <t>Engela</t>
+          <t>Gerry</t>
         </is>
       </c>
       <c r="C141" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Mitchells Plain</t>
         </is>
       </c>
       <c r="D141" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E141" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="142" ht="25" customHeight="1">
       <c r="A142" s="3" t="inlineStr">
         <is>
-          <t>de Kock</t>
+          <t>Zucker</t>
         </is>
       </c>
       <c r="B142" s="3" t="inlineStr">
         <is>
-          <t>Francois</t>
+          <t>Leonie</t>
         </is>
       </c>
       <c r="C142" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Milnerton</t>
         </is>
       </c>
       <c r="D142" s="3" t="inlineStr">
@@ -15480,29 +15399,29 @@
       </c>
       <c r="E142" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="143" ht="25" customHeight="1">
       <c r="A143" s="3" t="inlineStr">
         <is>
-          <t>stier</t>
+          <t>de Kock</t>
         </is>
       </c>
       <c r="B143" s="3" t="inlineStr">
         <is>
-          <t>RORY</t>
+          <t>Engela</t>
         </is>
       </c>
       <c r="C143" s="3" t="inlineStr">
         <is>
-          <t>Deep South</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D143" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E143" s="3" t="inlineStr">
@@ -15514,17 +15433,17 @@
     <row r="144" ht="25" customHeight="1">
       <c r="A144" s="3" t="inlineStr">
         <is>
-          <t>van Blerk</t>
+          <t>de Kock</t>
         </is>
       </c>
       <c r="B144" s="3" t="inlineStr">
         <is>
-          <t>Carl</t>
+          <t>Francois</t>
         </is>
       </c>
       <c r="C144" s="3" t="inlineStr">
         <is>
-          <t>Eden</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D144" s="3" t="inlineStr">
@@ -15534,51 +15453,51 @@
       </c>
       <c r="E144" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="145" ht="25" customHeight="1">
       <c r="A145" s="3" t="inlineStr">
         <is>
-          <t>van Rensburg</t>
+          <t>stier</t>
         </is>
       </c>
       <c r="B145" s="3" t="inlineStr">
         <is>
-          <t>Johan</t>
+          <t>RORY</t>
         </is>
       </c>
       <c r="C145" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Deep South</t>
         </is>
       </c>
       <c r="D145" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E145" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="146" ht="25" customHeight="1">
       <c r="A146" s="3" t="inlineStr">
         <is>
-          <t>van Rensburg</t>
+          <t>van Blerk</t>
         </is>
       </c>
       <c r="B146" s="3" t="inlineStr">
         <is>
-          <t>Anne</t>
+          <t>Carl</t>
         </is>
       </c>
       <c r="C146" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Eden</t>
         </is>
       </c>
       <c r="D146" s="3" t="inlineStr">
@@ -15595,17 +15514,17 @@
     <row r="147" ht="25" customHeight="1">
       <c r="A147" s="3" t="inlineStr">
         <is>
-          <t>van Wulven</t>
+          <t>van Rensburg</t>
         </is>
       </c>
       <c r="B147" s="3" t="inlineStr">
         <is>
-          <t>Jeannie</t>
+          <t>Johan</t>
         </is>
       </c>
       <c r="C147" s="3" t="inlineStr">
         <is>
-          <t>Tygerberg Hills</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D147" s="3" t="inlineStr">
@@ -15622,17 +15541,17 @@
     <row r="148" ht="25" customHeight="1">
       <c r="A148" s="3" t="inlineStr">
         <is>
-          <t>van Wulven</t>
+          <t>van Rensburg</t>
         </is>
       </c>
       <c r="B148" s="3" t="inlineStr">
         <is>
-          <t>Alan</t>
+          <t>Anne</t>
         </is>
       </c>
       <c r="C148" s="3" t="inlineStr">
         <is>
-          <t>Tygerberg Hills</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D148" s="3" t="inlineStr">
@@ -15654,7 +15573,7 @@
       </c>
       <c r="B149" s="3" t="inlineStr">
         <is>
-          <t>Deon</t>
+          <t>Jeannie</t>
         </is>
       </c>
       <c r="C149" s="3" t="inlineStr">
@@ -15676,39 +15595,93 @@
     <row r="150" ht="25" customHeight="1">
       <c r="A150" s="3" t="inlineStr">
         <is>
+          <t>van Wulven</t>
+        </is>
+      </c>
+      <c r="B150" s="3" t="inlineStr">
+        <is>
+          <t>Alan</t>
+        </is>
+      </c>
+      <c r="C150" s="3" t="inlineStr">
+        <is>
+          <t>Tygerberg Hills</t>
+        </is>
+      </c>
+      <c r="D150" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E150" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="151" ht="25" customHeight="1">
+      <c r="A151" s="3" t="inlineStr">
+        <is>
+          <t>van Wulven</t>
+        </is>
+      </c>
+      <c r="B151" s="3" t="inlineStr">
+        <is>
+          <t>Deon</t>
+        </is>
+      </c>
+      <c r="C151" s="3" t="inlineStr">
+        <is>
+          <t>Tygerberg Hills</t>
+        </is>
+      </c>
+      <c r="D151" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E151" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="152" ht="25" customHeight="1">
+      <c r="A152" s="3" t="inlineStr">
+        <is>
           <t>van der Westhuizen</t>
         </is>
       </c>
-      <c r="B150" s="3" t="inlineStr">
+      <c r="B152" s="3" t="inlineStr">
         <is>
           <t>Hennie</t>
         </is>
       </c>
-      <c r="C150" s="3" t="inlineStr">
+      <c r="C152" s="3" t="inlineStr">
         <is>
           <t>Helderberg</t>
         </is>
       </c>
-      <c r="D150" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E150" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-    </row>
-    <row r="151">
-      <c r="A151" s="1" t="inlineStr">
-        <is>
-          <t>Number of attendees: 148</t>
-        </is>
-      </c>
-    </row>
-    <row r="152">
-      <c r="A152" s="1" t="inlineStr">
+      <c r="D152" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E152" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="1" t="inlineStr">
+        <is>
+          <t>Number of attendees: 150</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="1" t="inlineStr">
         <is>
           <t>Number of voters: 56</t>
         </is>
@@ -15741,7 +15714,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Voting details as of 21/04/2021 13:45</t>
+          <t>410E Voting details as of 21/04/2021 13:58</t>
         </is>
       </c>
     </row>
@@ -16118,7 +16091,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Voting details as of 21/04/2021 13:45</t>
+          <t>410W Voting details as of 21/04/2021 13:58</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Registree stats backup on Thu 22 Apr 2021 08:27:20 SAST
</commit_message>
<xml_diff>
--- a/static/docs/registrees_list.xlsx
+++ b/static/docs/registrees_list.xlsx
@@ -451,7 +451,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>MD410 Registrees as of 21/04/2021 13:58</t>
+          <t>MD410 Registrees as of 22/04/2021 08:27</t>
         </is>
       </c>
     </row>
@@ -8115,7 +8115,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Registrees as of 21/04/2021 13:58</t>
+          <t>410E Registrees as of 22/04/2021 08:27</t>
         </is>
       </c>
     </row>
@@ -11592,7 +11592,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Registrees as of 21/04/2021 13:58</t>
+          <t>410W Registrees as of 22/04/2021 08:27</t>
         </is>
       </c>
     </row>
@@ -15714,7 +15714,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Voting details as of 21/04/2021 13:58</t>
+          <t>410E Voting details as of 22/04/2021 08:27</t>
         </is>
       </c>
     </row>
@@ -16091,7 +16091,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Voting details as of 21/04/2021 13:58</t>
+          <t>410W Voting details as of 22/04/2021 08:27</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Registree stats backup on Thu 22 Apr 2021 13:11:51 SAST
</commit_message>
<xml_diff>
--- a/static/docs/registrees_list.xlsx
+++ b/static/docs/registrees_list.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F241"/>
+  <dimension ref="A1:F242"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,7 +451,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>MD410 Registrees as of 22/04/2021 08:27</t>
+          <t>MD410 Registrees as of 22/04/2021 13:11</t>
         </is>
       </c>
     </row>
@@ -7498,17 +7498,17 @@
     <row r="222" ht="25" customHeight="1">
       <c r="A222" s="3" t="inlineStr">
         <is>
-          <t>van Blerk</t>
+          <t>tyler</t>
         </is>
       </c>
       <c r="B222" s="3" t="inlineStr">
         <is>
-          <t>Carl</t>
+          <t>natascha</t>
         </is>
       </c>
       <c r="C222" s="3" t="inlineStr">
         <is>
-          <t>Eden</t>
+          <t>Kensington</t>
         </is>
       </c>
       <c r="D222" s="3" t="inlineStr">
@@ -7523,24 +7523,24 @@
       </c>
       <c r="F222" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="223" ht="25" customHeight="1">
       <c r="A223" s="3" t="inlineStr">
         <is>
-          <t>van Heerden</t>
+          <t>van Blerk</t>
         </is>
       </c>
       <c r="B223" s="3" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Carl</t>
         </is>
       </c>
       <c r="C223" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Eden</t>
         </is>
       </c>
       <c r="D223" s="3" t="inlineStr">
@@ -7555,7 +7555,7 @@
       </c>
       <c r="F223" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -7567,7 +7567,7 @@
       </c>
       <c r="B224" s="3" t="inlineStr">
         <is>
-          <t>Sandy</t>
+          <t>Sydney</t>
         </is>
       </c>
       <c r="C224" s="3" t="inlineStr">
@@ -7582,7 +7582,7 @@
       </c>
       <c r="E224" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F224" s="3" t="inlineStr">
@@ -7599,17 +7599,17 @@
       </c>
       <c r="B225" s="3" t="inlineStr">
         <is>
-          <t>Craig</t>
+          <t>Sandy</t>
         </is>
       </c>
       <c r="C225" s="3" t="inlineStr">
         <is>
-          <t>East London Beacon Bay</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D225" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E225" s="3" t="inlineStr">
@@ -7631,17 +7631,17 @@
       </c>
       <c r="B226" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Craig</t>
         </is>
       </c>
       <c r="C226" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>East London Beacon Bay</t>
         </is>
       </c>
       <c r="D226" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E226" s="3" t="inlineStr">
@@ -7658,17 +7658,17 @@
     <row r="227" ht="25" customHeight="1">
       <c r="A227" s="3" t="inlineStr">
         <is>
-          <t>van Rensburg</t>
+          <t>van Heerden</t>
         </is>
       </c>
       <c r="B227" s="3" t="inlineStr">
         <is>
-          <t>Johan</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C227" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D227" s="3" t="inlineStr">
@@ -7678,12 +7678,12 @@
       </c>
       <c r="E227" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F227" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -7695,7 +7695,7 @@
       </c>
       <c r="B228" s="3" t="inlineStr">
         <is>
-          <t>Anne</t>
+          <t>Johan</t>
         </is>
       </c>
       <c r="C228" s="3" t="inlineStr">
@@ -7722,17 +7722,17 @@
     <row r="229" ht="25" customHeight="1">
       <c r="A229" s="3" t="inlineStr">
         <is>
-          <t>van Wulven</t>
+          <t>van Rensburg</t>
         </is>
       </c>
       <c r="B229" s="3" t="inlineStr">
         <is>
-          <t>Jeannie</t>
+          <t>Anne</t>
         </is>
       </c>
       <c r="C229" s="3" t="inlineStr">
         <is>
-          <t>Tygerberg Hills</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D229" s="3" t="inlineStr">
@@ -7759,7 +7759,7 @@
       </c>
       <c r="B230" s="3" t="inlineStr">
         <is>
-          <t>Alan</t>
+          <t>Jeannie</t>
         </is>
       </c>
       <c r="C230" s="3" t="inlineStr">
@@ -7791,7 +7791,7 @@
       </c>
       <c r="B231" s="3" t="inlineStr">
         <is>
-          <t>Deon</t>
+          <t>Alan</t>
         </is>
       </c>
       <c r="C231" s="3" t="inlineStr">
@@ -7818,17 +7818,17 @@
     <row r="232" ht="25" customHeight="1">
       <c r="A232" s="3" t="inlineStr">
         <is>
-          <t>van Wyk</t>
+          <t>van Wulven</t>
         </is>
       </c>
       <c r="B232" s="3" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>Deon</t>
         </is>
       </c>
       <c r="C232" s="3" t="inlineStr">
         <is>
-          <t>North Durban</t>
+          <t>Tygerberg Hills</t>
         </is>
       </c>
       <c r="D232" s="3" t="inlineStr">
@@ -7843,7 +7843,7 @@
       </c>
       <c r="F232" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -7855,12 +7855,12 @@
       </c>
       <c r="B233" s="3" t="inlineStr">
         <is>
-          <t>Lindie</t>
+          <t>Kim</t>
         </is>
       </c>
       <c r="C233" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>North Durban</t>
         </is>
       </c>
       <c r="D233" s="3" t="inlineStr">
@@ -7887,12 +7887,12 @@
       </c>
       <c r="B234" s="3" t="inlineStr">
         <is>
-          <t>Willem</t>
+          <t>Lindie</t>
         </is>
       </c>
       <c r="C234" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D234" s="3" t="inlineStr">
@@ -7919,12 +7919,12 @@
       </c>
       <c r="B235" s="3" t="inlineStr">
         <is>
-          <t>Patricia</t>
+          <t>Willem</t>
         </is>
       </c>
       <c r="C235" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D235" s="3" t="inlineStr">
@@ -7946,22 +7946,22 @@
     <row r="236" ht="25" customHeight="1">
       <c r="A236" s="3" t="inlineStr">
         <is>
-          <t>van der Merwe</t>
+          <t>van Wyk</t>
         </is>
       </c>
       <c r="B236" s="3" t="inlineStr">
         <is>
-          <t>Ingrid</t>
+          <t>Patricia</t>
         </is>
       </c>
       <c r="C236" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D236" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E236" s="3" t="inlineStr">
@@ -7978,49 +7978,49 @@
     <row r="237" ht="25" customHeight="1">
       <c r="A237" s="3" t="inlineStr">
         <is>
-          <t>van der Westhuizen</t>
+          <t>van der Merwe</t>
         </is>
       </c>
       <c r="B237" s="3" t="inlineStr">
         <is>
-          <t>Hennie</t>
+          <t>Ingrid</t>
         </is>
       </c>
       <c r="C237" s="3" t="inlineStr">
         <is>
-          <t>Helderberg</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D237" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E237" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F237" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="238" ht="25" customHeight="1">
       <c r="A238" s="3" t="inlineStr">
         <is>
-          <t>von der Decken</t>
+          <t>van der Westhuizen</t>
         </is>
       </c>
       <c r="B238" s="3" t="inlineStr">
         <is>
-          <t>Brian</t>
+          <t>Hennie</t>
         </is>
       </c>
       <c r="C238" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Helderberg</t>
         </is>
       </c>
       <c r="D238" s="3" t="inlineStr">
@@ -8035,51 +8035,83 @@
       </c>
       <c r="F238" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="239" ht="25" customHeight="1">
       <c r="A239" s="3" t="inlineStr">
         <is>
+          <t>von der Decken</t>
+        </is>
+      </c>
+      <c r="B239" s="3" t="inlineStr">
+        <is>
+          <t>Brian</t>
+        </is>
+      </c>
+      <c r="C239" s="3" t="inlineStr">
+        <is>
+          <t>King William's Town</t>
+        </is>
+      </c>
+      <c r="D239" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E239" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F239" s="3" t="inlineStr">
+        <is>
+          <t>410E</t>
+        </is>
+      </c>
+    </row>
+    <row r="240" ht="25" customHeight="1">
+      <c r="A240" s="3" t="inlineStr">
+        <is>
           <t>‘t Hart</t>
         </is>
       </c>
-      <c r="B239" s="3" t="inlineStr">
+      <c r="B240" s="3" t="inlineStr">
         <is>
           <t>Michelle</t>
         </is>
       </c>
-      <c r="C239" s="3" t="inlineStr">
+      <c r="C240" s="3" t="inlineStr">
         <is>
           <t>Benoni Lakes</t>
         </is>
       </c>
-      <c r="D239" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E239" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F239" s="3" t="inlineStr">
+      <c r="D240" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E240" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F240" s="3" t="inlineStr">
         <is>
           <t>410E</t>
-        </is>
-      </c>
-    </row>
-    <row r="240">
-      <c r="A240" s="1" t="inlineStr">
-        <is>
-          <t>Number of attendees: 237</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="inlineStr">
+        <is>
+          <t>Number of attendees: 238</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" s="1" t="inlineStr">
         <is>
           <t>Number of voters: 95</t>
         </is>
@@ -8097,7 +8129,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E130"/>
+  <dimension ref="A1:E131"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8115,7 +8147,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Registrees as of 22/04/2021 08:27</t>
+          <t>410E Registrees as of 22/04/2021 13:11</t>
         </is>
       </c>
     </row>
@@ -11254,17 +11286,17 @@
     <row r="118" ht="25" customHeight="1">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>van Heerden</t>
+          <t>tyler</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>natascha</t>
         </is>
       </c>
       <c r="C118" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Kensington</t>
         </is>
       </c>
       <c r="D118" s="3" t="inlineStr">
@@ -11286,7 +11318,7 @@
       </c>
       <c r="B119" s="3" t="inlineStr">
         <is>
-          <t>Sandy</t>
+          <t>Sydney</t>
         </is>
       </c>
       <c r="C119" s="3" t="inlineStr">
@@ -11301,7 +11333,7 @@
       </c>
       <c r="E119" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -11313,17 +11345,17 @@
       </c>
       <c r="B120" s="3" t="inlineStr">
         <is>
-          <t>Craig</t>
+          <t>Sandy</t>
         </is>
       </c>
       <c r="C120" s="3" t="inlineStr">
         <is>
-          <t>East London Beacon Bay</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D120" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E120" s="3" t="inlineStr">
@@ -11340,17 +11372,17 @@
       </c>
       <c r="B121" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Craig</t>
         </is>
       </c>
       <c r="C121" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>East London Beacon Bay</t>
         </is>
       </c>
       <c r="D121" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E121" s="3" t="inlineStr">
@@ -11362,17 +11394,17 @@
     <row r="122" ht="25" customHeight="1">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>van Wyk</t>
+          <t>van Heerden</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C122" s="3" t="inlineStr">
         <is>
-          <t>North Durban</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D122" s="3" t="inlineStr">
@@ -11382,7 +11414,7 @@
       </c>
       <c r="E122" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -11394,12 +11426,12 @@
       </c>
       <c r="B123" s="3" t="inlineStr">
         <is>
-          <t>Lindie</t>
+          <t>Kim</t>
         </is>
       </c>
       <c r="C123" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>North Durban</t>
         </is>
       </c>
       <c r="D123" s="3" t="inlineStr">
@@ -11421,12 +11453,12 @@
       </c>
       <c r="B124" s="3" t="inlineStr">
         <is>
-          <t>Willem</t>
+          <t>Lindie</t>
         </is>
       </c>
       <c r="C124" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D124" s="3" t="inlineStr">
@@ -11448,12 +11480,12 @@
       </c>
       <c r="B125" s="3" t="inlineStr">
         <is>
-          <t>Patricia</t>
+          <t>Willem</t>
         </is>
       </c>
       <c r="C125" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D125" s="3" t="inlineStr">
@@ -11470,22 +11502,22 @@
     <row r="126" ht="25" customHeight="1">
       <c r="A126" s="3" t="inlineStr">
         <is>
-          <t>van der Merwe</t>
+          <t>van Wyk</t>
         </is>
       </c>
       <c r="B126" s="3" t="inlineStr">
         <is>
-          <t>Ingrid</t>
+          <t>Patricia</t>
         </is>
       </c>
       <c r="C126" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D126" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E126" s="3" t="inlineStr">
@@ -11497,66 +11529,93 @@
     <row r="127" ht="25" customHeight="1">
       <c r="A127" s="3" t="inlineStr">
         <is>
-          <t>von der Decken</t>
+          <t>van der Merwe</t>
         </is>
       </c>
       <c r="B127" s="3" t="inlineStr">
         <is>
-          <t>Brian</t>
+          <t>Ingrid</t>
         </is>
       </c>
       <c r="C127" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D127" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E127" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="128" ht="25" customHeight="1">
       <c r="A128" s="3" t="inlineStr">
         <is>
+          <t>von der Decken</t>
+        </is>
+      </c>
+      <c r="B128" s="3" t="inlineStr">
+        <is>
+          <t>Brian</t>
+        </is>
+      </c>
+      <c r="C128" s="3" t="inlineStr">
+        <is>
+          <t>King William's Town</t>
+        </is>
+      </c>
+      <c r="D128" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E128" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="129" ht="25" customHeight="1">
+      <c r="A129" s="3" t="inlineStr">
+        <is>
           <t>‘t Hart</t>
         </is>
       </c>
-      <c r="B128" s="3" t="inlineStr">
+      <c r="B129" s="3" t="inlineStr">
         <is>
           <t>Michelle</t>
         </is>
       </c>
-      <c r="C128" s="3" t="inlineStr">
+      <c r="C129" s="3" t="inlineStr">
         <is>
           <t>Benoni Lakes</t>
         </is>
       </c>
-      <c r="D128" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E128" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129" s="1" t="inlineStr">
-        <is>
-          <t>Number of attendees: 126</t>
+      <c r="D129" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E129" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="inlineStr">
+        <is>
+          <t>Number of attendees: 127</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="1" t="inlineStr">
         <is>
           <t>Number of voters: 52</t>
         </is>
@@ -11592,7 +11651,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Registrees as of 22/04/2021 08:27</t>
+          <t>410W Registrees as of 22/04/2021 13:11</t>
         </is>
       </c>
     </row>
@@ -15714,7 +15773,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Voting details as of 22/04/2021 08:27</t>
+          <t>410E Voting details as of 22/04/2021 13:11</t>
         </is>
       </c>
     </row>
@@ -16091,7 +16150,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Voting details as of 22/04/2021 08:27</t>
+          <t>410W Voting details as of 22/04/2021 13:11</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Registree stats backup on Thu 22 Apr 2021 15:29:16 SAST
</commit_message>
<xml_diff>
--- a/static/docs/registrees_list.xlsx
+++ b/static/docs/registrees_list.xlsx
@@ -451,7 +451,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>MD410 Registrees as of 22/04/2021 13:11</t>
+          <t>MD410 Registrees as of 22/04/2021 15:29</t>
         </is>
       </c>
     </row>
@@ -8129,7 +8129,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E131"/>
+  <dimension ref="A1:E132"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8147,7 +8147,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Registrees as of 22/04/2021 13:11</t>
+          <t>410E Registrees as of 22/04/2021 15:29</t>
         </is>
       </c>
     </row>
@@ -8613,27 +8613,27 @@
     <row r="19" ht="25" customHeight="1">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>Easton</t>
+          <t>Du Preez</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
-          <t>Glynn</t>
+          <t>Marihana</t>
         </is>
       </c>
       <c r="C19" s="3" t="inlineStr">
         <is>
-          <t>Helderkruin</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D19" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E19" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -8645,7 +8645,7 @@
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>Denise</t>
+          <t>Glynn</t>
         </is>
       </c>
       <c r="C20" s="3" t="inlineStr">
@@ -8667,71 +8667,71 @@
     <row r="21" ht="25" customHeight="1">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>Els</t>
+          <t>Easton</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>Johan</t>
+          <t>Denise</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Helderkruin</t>
         </is>
       </c>
       <c r="D21" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E21" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="22" ht="25" customHeight="1">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>Erasmus</t>
+          <t>Els</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
         <is>
-          <t>Freddie</t>
+          <t>Johan</t>
         </is>
       </c>
       <c r="C22" s="3" t="inlineStr">
         <is>
-          <t>Uitenhage</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D22" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E22" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="23" ht="25" customHeight="1">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>Fourie</t>
+          <t>Erasmus</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
         <is>
-          <t>Lucille</t>
+          <t>Freddie</t>
         </is>
       </c>
       <c r="C23" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Uitenhage</t>
         </is>
       </c>
       <c r="D23" s="3" t="inlineStr">
@@ -8741,24 +8741,24 @@
       </c>
       <c r="E23" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="24" ht="25" customHeight="1">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>Foxcroft</t>
+          <t>Fourie</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
         <is>
-          <t>Kelvin</t>
+          <t>Lucille</t>
         </is>
       </c>
       <c r="C24" s="3" t="inlineStr">
         <is>
-          <t>Helderkruin</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D24" s="3" t="inlineStr">
@@ -8780,7 +8780,7 @@
       </c>
       <c r="B25" s="3" t="inlineStr">
         <is>
-          <t>Jenny</t>
+          <t>Kelvin</t>
         </is>
       </c>
       <c r="C25" s="3" t="inlineStr">
@@ -8807,7 +8807,7 @@
       </c>
       <c r="B26" s="3" t="inlineStr">
         <is>
-          <t>Katherine</t>
+          <t>Jenny</t>
         </is>
       </c>
       <c r="C26" s="3" t="inlineStr">
@@ -8829,17 +8829,17 @@
     <row r="27" ht="25" customHeight="1">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>Froise</t>
+          <t>Foxcroft</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
         <is>
-          <t>Martin</t>
+          <t>Katherine</t>
         </is>
       </c>
       <c r="C27" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Helderkruin</t>
         </is>
       </c>
       <c r="D27" s="3" t="inlineStr">
@@ -8849,24 +8849,24 @@
       </c>
       <c r="E27" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="28" ht="25" customHeight="1">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>Gerhard</t>
+          <t>Froise</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
         <is>
-          <t>Bernd</t>
+          <t>Martin</t>
         </is>
       </c>
       <c r="C28" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D28" s="3" t="inlineStr">
@@ -8888,7 +8888,7 @@
       </c>
       <c r="B29" s="3" t="inlineStr">
         <is>
-          <t>Shirley</t>
+          <t>Bernd</t>
         </is>
       </c>
       <c r="C29" s="3" t="inlineStr">
@@ -8903,24 +8903,24 @@
       </c>
       <c r="E29" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="30" ht="25" customHeight="1">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>Graham</t>
+          <t>Gerhard</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
         <is>
-          <t>Valerie</t>
+          <t>Shirley</t>
         </is>
       </c>
       <c r="C30" s="3" t="inlineStr">
         <is>
-          <t>Nelspruit</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D30" s="3" t="inlineStr">
@@ -8930,7 +8930,7 @@
       </c>
       <c r="E30" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -8942,7 +8942,7 @@
       </c>
       <c r="B31" s="3" t="inlineStr">
         <is>
-          <t>Mike</t>
+          <t>Valerie</t>
         </is>
       </c>
       <c r="C31" s="3" t="inlineStr">
@@ -8957,29 +8957,29 @@
       </c>
       <c r="E31" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="32" ht="25" customHeight="1">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>Griffith</t>
+          <t>Graham</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
         <is>
-          <t>David</t>
+          <t>Mike</t>
         </is>
       </c>
       <c r="C32" s="3" t="inlineStr">
         <is>
-          <t>The Wilds</t>
+          <t>Nelspruit</t>
         </is>
       </c>
       <c r="D32" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E32" s="3" t="inlineStr">
@@ -8991,22 +8991,22 @@
     <row r="33" ht="25" customHeight="1">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>Guthrie</t>
+          <t>Griffith</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
         <is>
-          <t>Clint</t>
+          <t>David</t>
         </is>
       </c>
       <c r="C33" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>The Wilds</t>
         </is>
       </c>
       <c r="D33" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E33" s="3" t="inlineStr">
@@ -9018,12 +9018,12 @@
     <row r="34" ht="25" customHeight="1">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>HERMANUS</t>
+          <t>Guthrie</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
         <is>
-          <t>MBULELO</t>
+          <t>Clint</t>
         </is>
       </c>
       <c r="C34" s="3" t="inlineStr">
@@ -9033,7 +9033,7 @@
       </c>
       <c r="D34" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E34" s="3" t="inlineStr">
@@ -9045,22 +9045,22 @@
     <row r="35" ht="25" customHeight="1">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>HOLLIMAN</t>
+          <t>HERMANUS</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
         <is>
-          <t>KEITH ALEXANDER</t>
+          <t>MBULELO</t>
         </is>
       </c>
       <c r="C35" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D35" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E35" s="3" t="inlineStr">
@@ -9072,17 +9072,17 @@
     <row r="36" ht="25" customHeight="1">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>Heathcote</t>
+          <t>HOLLIMAN</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
         <is>
-          <t>Mike</t>
+          <t>KEITH ALEXANDER</t>
         </is>
       </c>
       <c r="C36" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D36" s="3" t="inlineStr">
@@ -9092,24 +9092,24 @@
       </c>
       <c r="E36" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="37" ht="25" customHeight="1">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>Herzfeld</t>
+          <t>Heathcote</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
         <is>
-          <t>Evelyn</t>
+          <t>Mike</t>
         </is>
       </c>
       <c r="C37" s="3" t="inlineStr">
         <is>
-          <t>Edenvale</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D37" s="3" t="inlineStr">
@@ -9119,24 +9119,24 @@
       </c>
       <c r="E37" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="38" ht="25" customHeight="1">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>Higgins</t>
+          <t>Herzfeld</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
         <is>
-          <t>Wendy</t>
+          <t>Evelyn</t>
         </is>
       </c>
       <c r="C38" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Edenvale</t>
         </is>
       </c>
       <c r="D38" s="3" t="inlineStr">
@@ -9153,17 +9153,17 @@
     <row r="39" ht="25" customHeight="1">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>Hobbs</t>
+          <t>Higgins</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
         <is>
-          <t>Avril</t>
+          <t>Wendy</t>
         </is>
       </c>
       <c r="C39" s="3" t="inlineStr">
         <is>
-          <t>North Durban</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D39" s="3" t="inlineStr">
@@ -9173,7 +9173,7 @@
       </c>
       <c r="E39" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -9185,7 +9185,7 @@
       </c>
       <c r="B40" s="3" t="inlineStr">
         <is>
-          <t>Trevor</t>
+          <t>Avril</t>
         </is>
       </c>
       <c r="C40" s="3" t="inlineStr">
@@ -9207,17 +9207,17 @@
     <row r="41" ht="25" customHeight="1">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>Hocking</t>
+          <t>Hobbs</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
         <is>
-          <t>Jacqui</t>
+          <t>Trevor</t>
         </is>
       </c>
       <c r="C41" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>North Durban</t>
         </is>
       </c>
       <c r="D41" s="3" t="inlineStr">
@@ -9239,7 +9239,7 @@
       </c>
       <c r="B42" s="3" t="inlineStr">
         <is>
-          <t>Cliff</t>
+          <t>Jacqui</t>
         </is>
       </c>
       <c r="C42" s="3" t="inlineStr">
@@ -9254,24 +9254,24 @@
       </c>
       <c r="E42" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="43" ht="25" customHeight="1">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>JOHNSTON</t>
+          <t>Hocking</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
         <is>
-          <t>MALCOLM</t>
+          <t>Cliff</t>
         </is>
       </c>
       <c r="C43" s="3" t="inlineStr">
         <is>
-          <t>Standerton</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D43" s="3" t="inlineStr">
@@ -9281,24 +9281,24 @@
       </c>
       <c r="E43" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="44" ht="25" customHeight="1">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>Jackman</t>
+          <t>JOHNSTON</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
         <is>
-          <t>Gail</t>
+          <t>MALCOLM</t>
         </is>
       </c>
       <c r="C44" s="3" t="inlineStr">
         <is>
-          <t>Nelspruit</t>
+          <t>Standerton</t>
         </is>
       </c>
       <c r="D44" s="3" t="inlineStr">
@@ -9308,24 +9308,24 @@
       </c>
       <c r="E44" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="45" ht="25" customHeight="1">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>Jackson</t>
+          <t>Jackman</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
         <is>
-          <t>Alna</t>
+          <t>Gail</t>
         </is>
       </c>
       <c r="C45" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Nelspruit</t>
         </is>
       </c>
       <c r="D45" s="3" t="inlineStr">
@@ -9335,24 +9335,24 @@
       </c>
       <c r="E45" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="46" ht="25" customHeight="1">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>Kienast</t>
+          <t>Jackson</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
         <is>
-          <t>Margie</t>
+          <t>Alna</t>
         </is>
       </c>
       <c r="C46" s="3" t="inlineStr">
         <is>
-          <t>Edenvale</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D46" s="3" t="inlineStr">
@@ -9362,24 +9362,24 @@
       </c>
       <c r="E46" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="47" ht="25" customHeight="1">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>Kimari</t>
+          <t>Kienast</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
         <is>
-          <t>Joyce</t>
+          <t>Margie</t>
         </is>
       </c>
       <c r="C47" s="3" t="inlineStr">
         <is>
-          <t>Eden</t>
+          <t>Edenvale</t>
         </is>
       </c>
       <c r="D47" s="3" t="inlineStr">
@@ -9396,17 +9396,17 @@
     <row r="48" ht="25" customHeight="1">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>King</t>
+          <t>Kimari</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
         <is>
-          <t>Ian</t>
+          <t>Joyce</t>
         </is>
       </c>
       <c r="C48" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Eden</t>
         </is>
       </c>
       <c r="D48" s="3" t="inlineStr">
@@ -9416,7 +9416,7 @@
       </c>
       <c r="E48" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -9428,7 +9428,7 @@
       </c>
       <c r="B49" s="3" t="inlineStr">
         <is>
-          <t>Sandy</t>
+          <t>Ian</t>
         </is>
       </c>
       <c r="C49" s="3" t="inlineStr">
@@ -9450,17 +9450,17 @@
     <row r="50" ht="25" customHeight="1">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>Koekemoer</t>
+          <t>King</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
         <is>
-          <t>Christa</t>
+          <t>Sandy</t>
         </is>
       </c>
       <c r="C50" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D50" s="3" t="inlineStr">
@@ -9470,29 +9470,29 @@
       </c>
       <c r="E50" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="51" ht="25" customHeight="1">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>Kruger</t>
+          <t>Koekemoer</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
         <is>
-          <t>Pieter</t>
+          <t>Christa</t>
         </is>
       </c>
       <c r="C51" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D51" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E51" s="3" t="inlineStr">
@@ -9509,7 +9509,7 @@
       </c>
       <c r="B52" s="3" t="inlineStr">
         <is>
-          <t>Niqula</t>
+          <t>Pieter</t>
         </is>
       </c>
       <c r="C52" s="3" t="inlineStr">
@@ -9531,22 +9531,22 @@
     <row r="53" ht="25" customHeight="1">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>Laas</t>
+          <t>Kruger</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
         <is>
-          <t>Natalie</t>
+          <t>Niqula</t>
         </is>
       </c>
       <c r="C53" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D53" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E53" s="3" t="inlineStr">
@@ -9558,17 +9558,17 @@
     <row r="54" ht="25" customHeight="1">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>Labuschagne</t>
+          <t>Laas</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
         <is>
-          <t>Susan</t>
+          <t>Natalie</t>
         </is>
       </c>
       <c r="C54" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D54" s="3" t="inlineStr">
@@ -9585,22 +9585,22 @@
     <row r="55" ht="25" customHeight="1">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>Langton</t>
+          <t>Labuschagne</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
         <is>
-          <t>Evelyn May</t>
+          <t>Susan</t>
         </is>
       </c>
       <c r="C55" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D55" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E55" s="3" t="inlineStr">
@@ -9612,39 +9612,39 @@
     <row r="56" ht="25" customHeight="1">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>Lautenbach</t>
+          <t>Langton</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
         <is>
-          <t>Steven</t>
+          <t>Evelyn May</t>
         </is>
       </c>
       <c r="C56" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D56" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E56" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="57" ht="25" customHeight="1">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>Logan</t>
+          <t>Lautenbach</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
         <is>
-          <t>Graeme</t>
+          <t>Steven</t>
         </is>
       </c>
       <c r="C57" s="3" t="inlineStr">
@@ -9659,24 +9659,24 @@
       </c>
       <c r="E57" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="58" ht="25" customHeight="1">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>Love</t>
+          <t>Logan</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
         <is>
-          <t>Dee</t>
+          <t>Graeme</t>
         </is>
       </c>
       <c r="C58" s="3" t="inlineStr">
         <is>
-          <t>Cowies Hill</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D58" s="3" t="inlineStr">
@@ -9693,17 +9693,17 @@
     <row r="59" ht="25" customHeight="1">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>Luck</t>
+          <t>Love</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
         <is>
-          <t>Zarina</t>
+          <t>Dee</t>
         </is>
       </c>
       <c r="C59" s="3" t="inlineStr">
         <is>
-          <t>Newcastle</t>
+          <t>Cowies Hill</t>
         </is>
       </c>
       <c r="D59" s="3" t="inlineStr">
@@ -9713,24 +9713,24 @@
       </c>
       <c r="E59" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="60" ht="25" customHeight="1">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>MILLS</t>
+          <t>Luck</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
         <is>
-          <t>BERNICE</t>
+          <t>Zarina</t>
         </is>
       </c>
       <c r="C60" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Newcastle</t>
         </is>
       </c>
       <c r="D60" s="3" t="inlineStr">
@@ -9747,17 +9747,17 @@
     <row r="61" ht="25" customHeight="1">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>Mare</t>
+          <t>MILLS</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
         <is>
-          <t>Beaulieu</t>
+          <t>BERNICE</t>
         </is>
       </c>
       <c r="C61" s="3" t="inlineStr">
         <is>
-          <t>Benoni Lakes</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D61" s="3" t="inlineStr">
@@ -9774,12 +9774,12 @@
     <row r="62" ht="25" customHeight="1">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>Maré</t>
+          <t>Mare</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
         <is>
-          <t>Nick</t>
+          <t>Beaulieu</t>
         </is>
       </c>
       <c r="C62" s="3" t="inlineStr">
@@ -9794,24 +9794,24 @@
       </c>
       <c r="E62" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="63" ht="25" customHeight="1">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>Masson</t>
+          <t>Maré</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
         <is>
-          <t>Jean</t>
+          <t>Nick</t>
         </is>
       </c>
       <c r="C63" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Benoni Lakes</t>
         </is>
       </c>
       <c r="D63" s="3" t="inlineStr">
@@ -9828,17 +9828,17 @@
     <row r="64" ht="25" customHeight="1">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>McDonald</t>
+          <t>Masson</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
         <is>
-          <t>Rochelle</t>
+          <t>Jean</t>
         </is>
       </c>
       <c r="C64" s="3" t="inlineStr">
         <is>
-          <t>Vereeniging</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D64" s="3" t="inlineStr">
@@ -9855,17 +9855,17 @@
     <row r="65" ht="25" customHeight="1">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>McKerrow</t>
+          <t>McDonald</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
         <is>
-          <t>Alec</t>
+          <t>Rochelle</t>
         </is>
       </c>
       <c r="C65" s="3" t="inlineStr">
         <is>
-          <t>Port Alfred</t>
+          <t>Vereeniging</t>
         </is>
       </c>
       <c r="D65" s="3" t="inlineStr">
@@ -9882,17 +9882,17 @@
     <row r="66" ht="25" customHeight="1">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>Mccullough</t>
+          <t>McKerrow</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
         <is>
-          <t>David</t>
+          <t>Alec</t>
         </is>
       </c>
       <c r="C66" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Port Alfred</t>
         </is>
       </c>
       <c r="D66" s="3" t="inlineStr">
@@ -9909,17 +9909,17 @@
     <row r="67" ht="25" customHeight="1">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>Meltzer</t>
+          <t>Mccullough</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>David</t>
         </is>
       </c>
       <c r="C67" s="3" t="inlineStr">
         <is>
-          <t>The Wilds</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D67" s="3" t="inlineStr">
@@ -9929,24 +9929,24 @@
       </c>
       <c r="E67" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="68" ht="25" customHeight="1">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>Meyer</t>
+          <t>Meltzer</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
         <is>
-          <t>Denis</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C68" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>The Wilds</t>
         </is>
       </c>
       <c r="D68" s="3" t="inlineStr">
@@ -9963,17 +9963,17 @@
     <row r="69" ht="25" customHeight="1">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>Michas</t>
+          <t>Meyer</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
         <is>
-          <t>Roy</t>
+          <t>Denis</t>
         </is>
       </c>
       <c r="C69" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D69" s="3" t="inlineStr">
@@ -9995,7 +9995,7 @@
       </c>
       <c r="B70" s="3" t="inlineStr">
         <is>
-          <t>Dawn</t>
+          <t>Roy</t>
         </is>
       </c>
       <c r="C70" s="3" t="inlineStr">
@@ -10010,24 +10010,24 @@
       </c>
       <c r="E70" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="71" ht="25" customHeight="1">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>Mills</t>
+          <t>Michas</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>Dawn</t>
         </is>
       </c>
       <c r="C71" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D71" s="3" t="inlineStr">
@@ -10037,24 +10037,24 @@
       </c>
       <c r="E71" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="72" ht="25" customHeight="1">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>Mitchell</t>
+          <t>Mills</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
         <is>
-          <t>Alana</t>
+          <t>Patrick</t>
         </is>
       </c>
       <c r="C72" s="3" t="inlineStr">
         <is>
-          <t>Rustenburg</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D72" s="3" t="inlineStr">
@@ -10064,7 +10064,7 @@
       </c>
       <c r="E72" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -10076,7 +10076,7 @@
       </c>
       <c r="B73" s="3" t="inlineStr">
         <is>
-          <t>Juan</t>
+          <t>Alana</t>
         </is>
       </c>
       <c r="C73" s="3" t="inlineStr">
@@ -10091,24 +10091,24 @@
       </c>
       <c r="E73" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="74" ht="25" customHeight="1">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>Murray</t>
+          <t>Mitchell</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
         <is>
-          <t>Suzanne</t>
+          <t>Juan</t>
         </is>
       </c>
       <c r="C74" s="3" t="inlineStr">
         <is>
-          <t>Vereeniging</t>
+          <t>Rustenburg</t>
         </is>
       </c>
       <c r="D74" s="3" t="inlineStr">
@@ -10130,7 +10130,7 @@
       </c>
       <c r="B75" s="3" t="inlineStr">
         <is>
-          <t>Gary</t>
+          <t>Suzanne</t>
         </is>
       </c>
       <c r="C75" s="3" t="inlineStr">
@@ -10152,17 +10152,17 @@
     <row r="76" ht="25" customHeight="1">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>Nel</t>
+          <t>Murray</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
         <is>
-          <t>Theo</t>
+          <t>Gary</t>
         </is>
       </c>
       <c r="C76" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Vereeniging</t>
         </is>
       </c>
       <c r="D76" s="3" t="inlineStr">
@@ -10179,17 +10179,17 @@
     <row r="77" ht="25" customHeight="1">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>Newlands</t>
+          <t>Nel</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
         <is>
-          <t>Mike</t>
+          <t>Theo</t>
         </is>
       </c>
       <c r="C77" s="3" t="inlineStr">
         <is>
-          <t>Port Alfred</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D77" s="3" t="inlineStr">
@@ -10206,17 +10206,17 @@
     <row r="78" ht="25" customHeight="1">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>Ngobozana</t>
+          <t>Newlands</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
         <is>
-          <t>Sphiwe</t>
+          <t>Mike</t>
         </is>
       </c>
       <c r="C78" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Port Alfred</t>
         </is>
       </c>
       <c r="D78" s="3" t="inlineStr">
@@ -10226,24 +10226,24 @@
       </c>
       <c r="E78" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="79" ht="25" customHeight="1">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>Oberholzer</t>
+          <t>Ngobozana</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
         <is>
-          <t>PDG Bokkie</t>
+          <t>Sphiwe</t>
         </is>
       </c>
       <c r="C79" s="3" t="inlineStr">
         <is>
-          <t>Uitenhage</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D79" s="3" t="inlineStr">
@@ -10260,17 +10260,17 @@
     <row r="80" ht="25" customHeight="1">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>PORTEOUS</t>
+          <t>Oberholzer</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
         <is>
-          <t>BRIAN</t>
+          <t>PDG Bokkie</t>
         </is>
       </c>
       <c r="C80" s="3" t="inlineStr">
         <is>
-          <t>Hibberdene</t>
+          <t>Uitenhage</t>
         </is>
       </c>
       <c r="D80" s="3" t="inlineStr">
@@ -10280,24 +10280,24 @@
       </c>
       <c r="E80" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="81" ht="25" customHeight="1">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>Paijmans</t>
+          <t>PORTEOUS</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
         <is>
-          <t>Bronwyn Anne</t>
+          <t>BRIAN</t>
         </is>
       </c>
       <c r="C81" s="3" t="inlineStr">
         <is>
-          <t>Cowies Hill</t>
+          <t>Hibberdene</t>
         </is>
       </c>
       <c r="D81" s="3" t="inlineStr">
@@ -10307,24 +10307,24 @@
       </c>
       <c r="E81" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="82" ht="25" customHeight="1">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>Pantoleon</t>
+          <t>Paijmans</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
         <is>
-          <t>Teresa</t>
+          <t>Bronwyn Anne</t>
         </is>
       </c>
       <c r="C82" s="3" t="inlineStr">
         <is>
-          <t>Vereeniging</t>
+          <t>Cowies Hill</t>
         </is>
       </c>
       <c r="D82" s="3" t="inlineStr">
@@ -10334,24 +10334,24 @@
       </c>
       <c r="E82" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="83" ht="25" customHeight="1">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>Polkinghorne</t>
+          <t>Pantoleon</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
         <is>
-          <t>Tracey</t>
+          <t>Teresa</t>
         </is>
       </c>
       <c r="C83" s="3" t="inlineStr">
         <is>
-          <t>Kensington</t>
+          <t>Vereeniging</t>
         </is>
       </c>
       <c r="D83" s="3" t="inlineStr">
@@ -10373,7 +10373,7 @@
       </c>
       <c r="B84" s="3" t="inlineStr">
         <is>
-          <t>Gavin</t>
+          <t>Tracey</t>
         </is>
       </c>
       <c r="C84" s="3" t="inlineStr">
@@ -10388,29 +10388,29 @@
       </c>
       <c r="E84" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="85" ht="25" customHeight="1">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>Rashirai</t>
+          <t>Polkinghorne</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
         <is>
-          <t>Tabeth</t>
+          <t>Gavin</t>
         </is>
       </c>
       <c r="C85" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Kensington</t>
         </is>
       </c>
       <c r="D85" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E85" s="3" t="inlineStr">
@@ -10422,44 +10422,44 @@
     <row r="86" ht="25" customHeight="1">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>Reniers</t>
+          <t>Rashirai</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
         <is>
-          <t>Hugo</t>
+          <t>Tabeth</t>
         </is>
       </c>
       <c r="C86" s="3" t="inlineStr">
         <is>
-          <t>Nelspruit</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D86" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E86" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="87" ht="25" customHeight="1">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>Sabatier</t>
+          <t>Reniers</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
         <is>
-          <t>Rodney</t>
+          <t>Hugo</t>
         </is>
       </c>
       <c r="C87" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Nelspruit</t>
         </is>
       </c>
       <c r="D87" s="3" t="inlineStr">
@@ -10476,17 +10476,17 @@
     <row r="88" ht="25" customHeight="1">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>Searle</t>
+          <t>Sabatier</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
         <is>
-          <t>Francis</t>
+          <t>Rodney</t>
         </is>
       </c>
       <c r="C88" s="3" t="inlineStr">
         <is>
-          <t>Kouga</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D88" s="3" t="inlineStr">
@@ -10508,7 +10508,7 @@
       </c>
       <c r="B89" s="3" t="inlineStr">
         <is>
-          <t>Gloria</t>
+          <t>Francis</t>
         </is>
       </c>
       <c r="C89" s="3" t="inlineStr">
@@ -10523,24 +10523,24 @@
       </c>
       <c r="E89" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="90" ht="25" customHeight="1">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>Smit</t>
+          <t>Searle</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
         <is>
-          <t>Sue</t>
+          <t>Gloria</t>
         </is>
       </c>
       <c r="C90" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Kouga</t>
         </is>
       </c>
       <c r="D90" s="3" t="inlineStr">
@@ -10557,17 +10557,17 @@
     <row r="91" ht="25" customHeight="1">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Smit</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
         <is>
-          <t>Jeff</t>
+          <t>Sue</t>
         </is>
       </c>
       <c r="C91" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D91" s="3" t="inlineStr">
@@ -10584,17 +10584,17 @@
     <row r="92" ht="25" customHeight="1">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>Stander</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
         <is>
-          <t>Max</t>
+          <t>Jeff</t>
         </is>
       </c>
       <c r="C92" s="3" t="inlineStr">
         <is>
-          <t>Port Alfred</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D92" s="3" t="inlineStr">
@@ -10616,12 +10616,12 @@
       </c>
       <c r="B93" s="3" t="inlineStr">
         <is>
-          <t>Ashley</t>
+          <t>Max</t>
         </is>
       </c>
       <c r="C93" s="3" t="inlineStr">
         <is>
-          <t>Krugersdorp</t>
+          <t>Port Alfred</t>
         </is>
       </c>
       <c r="D93" s="3" t="inlineStr">
@@ -10631,7 +10631,7 @@
       </c>
       <c r="E93" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -10643,7 +10643,7 @@
       </c>
       <c r="B94" s="3" t="inlineStr">
         <is>
-          <t>Brett Jason</t>
+          <t>Ashley</t>
         </is>
       </c>
       <c r="C94" s="3" t="inlineStr">
@@ -10658,29 +10658,29 @@
       </c>
       <c r="E94" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="95" ht="25" customHeight="1">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>Steyn</t>
+          <t>Stander</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
         <is>
-          <t>Elna</t>
+          <t>Brett Jason</t>
         </is>
       </c>
       <c r="C95" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Krugersdorp</t>
         </is>
       </c>
       <c r="D95" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E95" s="3" t="inlineStr">
@@ -10692,22 +10692,22 @@
     <row r="96" ht="25" customHeight="1">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>Sturges</t>
+          <t>Steyn</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
         <is>
-          <t>Trevor</t>
+          <t>Elna</t>
         </is>
       </c>
       <c r="C96" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D96" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E96" s="3" t="inlineStr">
@@ -10719,17 +10719,17 @@
     <row r="97" ht="25" customHeight="1">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>Talbot</t>
+          <t>Sturges</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
         <is>
-          <t>Lauryn</t>
+          <t>Trevor</t>
         </is>
       </c>
       <c r="C97" s="3" t="inlineStr">
         <is>
-          <t>Benoni Lakes</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D97" s="3" t="inlineStr">
@@ -10746,17 +10746,17 @@
     <row r="98" ht="25" customHeight="1">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>Theron</t>
+          <t>Talbot</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
         <is>
-          <t>Pierre</t>
+          <t>Lauryn</t>
         </is>
       </c>
       <c r="C98" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Benoni Lakes</t>
         </is>
       </c>
       <c r="D98" s="3" t="inlineStr">
@@ -10778,7 +10778,7 @@
       </c>
       <c r="B99" s="3" t="inlineStr">
         <is>
-          <t>Moira</t>
+          <t>Pierre</t>
         </is>
       </c>
       <c r="C99" s="3" t="inlineStr">
@@ -10800,17 +10800,17 @@
     <row r="100" ht="25" customHeight="1">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>Townsend</t>
+          <t>Theron</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
         <is>
-          <t>Diane</t>
+          <t>Moira</t>
         </is>
       </c>
       <c r="C100" s="3" t="inlineStr">
         <is>
-          <t>Benoni Lakes</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D100" s="3" t="inlineStr">
@@ -10820,56 +10820,56 @@
       </c>
       <c r="E100" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="101" ht="25" customHeight="1">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>Toye</t>
+          <t>Townsend</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
         <is>
-          <t>Omolayo</t>
+          <t>Diane</t>
         </is>
       </c>
       <c r="C101" s="3" t="inlineStr">
         <is>
-          <t>The Wilds</t>
+          <t>Benoni Lakes</t>
         </is>
       </c>
       <c r="D101" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E101" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="102" ht="25" customHeight="1">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>Tuckett</t>
+          <t>Toye</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
         <is>
-          <t>Alistair</t>
+          <t>Omolayo</t>
         </is>
       </c>
       <c r="C102" s="3" t="inlineStr">
         <is>
-          <t>Roodepoort Clearwater Cyber</t>
+          <t>The Wilds</t>
         </is>
       </c>
       <c r="D102" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E102" s="3" t="inlineStr">
@@ -10886,7 +10886,7 @@
       </c>
       <c r="B103" s="3" t="inlineStr">
         <is>
-          <t>Rowan</t>
+          <t>Alistair</t>
         </is>
       </c>
       <c r="C103" s="3" t="inlineStr">
@@ -10901,7 +10901,7 @@
       </c>
       <c r="E103" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -10913,7 +10913,7 @@
       </c>
       <c r="B104" s="3" t="inlineStr">
         <is>
-          <t>Gail</t>
+          <t>Rowan</t>
         </is>
       </c>
       <c r="C104" s="3" t="inlineStr">
@@ -10928,29 +10928,29 @@
       </c>
       <c r="E104" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="105" ht="25" customHeight="1">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>Uchytil</t>
+          <t>Tuckett</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
         <is>
-          <t>Jiri</t>
+          <t>Gail</t>
         </is>
       </c>
       <c r="C105" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Roodepoort Clearwater Cyber</t>
         </is>
       </c>
       <c r="D105" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E105" s="3" t="inlineStr">
@@ -10962,17 +10962,17 @@
     <row r="106" ht="25" customHeight="1">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>VAN DER MERWE</t>
+          <t>Uchytil</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
         <is>
-          <t>PATRICIA</t>
+          <t>Jiri</t>
         </is>
       </c>
       <c r="C106" s="3" t="inlineStr">
         <is>
-          <t>East London Port Rex</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D106" s="3" t="inlineStr">
@@ -10982,24 +10982,24 @@
       </c>
       <c r="E106" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="107" ht="25" customHeight="1">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>Van Niekerk</t>
+          <t>VAN DER MERWE</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
         <is>
-          <t>Riaan</t>
+          <t>PATRICIA</t>
         </is>
       </c>
       <c r="C107" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>East London Port Rex</t>
         </is>
       </c>
       <c r="D107" s="3" t="inlineStr">
@@ -11009,24 +11009,24 @@
       </c>
       <c r="E107" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="108" ht="25" customHeight="1">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>Venter</t>
+          <t>Van Niekerk</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
         <is>
-          <t>Louis</t>
+          <t>Riaan</t>
         </is>
       </c>
       <c r="C108" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D108" s="3" t="inlineStr">
@@ -11043,44 +11043,44 @@
     <row r="109" ht="25" customHeight="1">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>Volker</t>
+          <t>Venter</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
         <is>
-          <t>Russell</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="C109" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D109" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E109" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="110" ht="25" customHeight="1">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>Warman</t>
+          <t>Volker</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
         <is>
-          <t>Alastair</t>
+          <t>Russell</t>
         </is>
       </c>
       <c r="C110" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>King William's Town</t>
         </is>
       </c>
       <c r="D110" s="3" t="inlineStr">
@@ -11097,17 +11097,17 @@
     <row r="111" ht="25" customHeight="1">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>Williamson</t>
+          <t>Warman</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
         <is>
-          <t>Neville</t>
+          <t>Alastair</t>
         </is>
       </c>
       <c r="C111" s="3" t="inlineStr">
         <is>
-          <t>Port Alfred</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D111" s="3" t="inlineStr">
@@ -11117,24 +11117,24 @@
       </c>
       <c r="E111" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="112" ht="25" customHeight="1">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>Wilter-Sturges</t>
+          <t>Williamson</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
         <is>
-          <t>Meredith</t>
+          <t>Neville</t>
         </is>
       </c>
       <c r="C112" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Port Alfred</t>
         </is>
       </c>
       <c r="D112" s="3" t="inlineStr">
@@ -11151,22 +11151,22 @@
     <row r="113" ht="25" customHeight="1">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>de Silva</t>
+          <t>Wilter-Sturges</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Meredith</t>
         </is>
       </c>
       <c r="C113" s="3" t="inlineStr">
         <is>
-          <t>Edenvale</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D113" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E113" s="3" t="inlineStr">
@@ -11178,27 +11178,27 @@
     <row r="114" ht="25" customHeight="1">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>du Plooy</t>
+          <t>de Silva</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
         <is>
-          <t>Tammy</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="C114" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Edenvale</t>
         </is>
       </c>
       <c r="D114" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E114" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -11210,7 +11210,7 @@
       </c>
       <c r="B115" s="3" t="inlineStr">
         <is>
-          <t>Marc</t>
+          <t>Tammy</t>
         </is>
       </c>
       <c r="C115" s="3" t="inlineStr">
@@ -11232,17 +11232,17 @@
     <row r="116" ht="25" customHeight="1">
       <c r="A116" s="3" t="inlineStr">
         <is>
-          <t>du Toit</t>
+          <t>du Plooy</t>
         </is>
       </c>
       <c r="B116" s="3" t="inlineStr">
         <is>
-          <t>Desiree</t>
+          <t>Marc</t>
         </is>
       </c>
       <c r="C116" s="3" t="inlineStr">
         <is>
-          <t>Ramsgate</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D116" s="3" t="inlineStr">
@@ -11259,17 +11259,17 @@
     <row r="117" ht="25" customHeight="1">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>le Roux</t>
+          <t>du Toit</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
         <is>
-          <t>Jeanette</t>
+          <t>Desiree</t>
         </is>
       </c>
       <c r="C117" s="3" t="inlineStr">
         <is>
-          <t>Gonubie</t>
+          <t>Ramsgate</t>
         </is>
       </c>
       <c r="D117" s="3" t="inlineStr">
@@ -11286,17 +11286,17 @@
     <row r="118" ht="25" customHeight="1">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>tyler</t>
+          <t>le Roux</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
         <is>
-          <t>natascha</t>
+          <t>Jeanette</t>
         </is>
       </c>
       <c r="C118" s="3" t="inlineStr">
         <is>
-          <t>Kensington</t>
+          <t>Gonubie</t>
         </is>
       </c>
       <c r="D118" s="3" t="inlineStr">
@@ -11306,24 +11306,24 @@
       </c>
       <c r="E118" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="119" ht="25" customHeight="1">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>van Heerden</t>
+          <t>tyler</t>
         </is>
       </c>
       <c r="B119" s="3" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>natascha</t>
         </is>
       </c>
       <c r="C119" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Kensington</t>
         </is>
       </c>
       <c r="D119" s="3" t="inlineStr">
@@ -11345,7 +11345,7 @@
       </c>
       <c r="B120" s="3" t="inlineStr">
         <is>
-          <t>Sandy</t>
+          <t>Sydney</t>
         </is>
       </c>
       <c r="C120" s="3" t="inlineStr">
@@ -11360,7 +11360,7 @@
       </c>
       <c r="E120" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -11372,17 +11372,17 @@
       </c>
       <c r="B121" s="3" t="inlineStr">
         <is>
-          <t>Craig</t>
+          <t>Sandy</t>
         </is>
       </c>
       <c r="C121" s="3" t="inlineStr">
         <is>
-          <t>East London Beacon Bay</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D121" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E121" s="3" t="inlineStr">
@@ -11399,17 +11399,17 @@
       </c>
       <c r="B122" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Craig</t>
         </is>
       </c>
       <c r="C122" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>East London Beacon Bay</t>
         </is>
       </c>
       <c r="D122" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E122" s="3" t="inlineStr">
@@ -11421,17 +11421,17 @@
     <row r="123" ht="25" customHeight="1">
       <c r="A123" s="3" t="inlineStr">
         <is>
-          <t>van Wyk</t>
+          <t>van Heerden</t>
         </is>
       </c>
       <c r="B123" s="3" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C123" s="3" t="inlineStr">
         <is>
-          <t>North Durban</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D123" s="3" t="inlineStr">
@@ -11441,7 +11441,7 @@
       </c>
       <c r="E123" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -11453,12 +11453,12 @@
       </c>
       <c r="B124" s="3" t="inlineStr">
         <is>
-          <t>Lindie</t>
+          <t>Kim</t>
         </is>
       </c>
       <c r="C124" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>North Durban</t>
         </is>
       </c>
       <c r="D124" s="3" t="inlineStr">
@@ -11480,12 +11480,12 @@
       </c>
       <c r="B125" s="3" t="inlineStr">
         <is>
-          <t>Willem</t>
+          <t>Lindie</t>
         </is>
       </c>
       <c r="C125" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D125" s="3" t="inlineStr">
@@ -11507,12 +11507,12 @@
       </c>
       <c r="B126" s="3" t="inlineStr">
         <is>
-          <t>Patricia</t>
+          <t>Willem</t>
         </is>
       </c>
       <c r="C126" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D126" s="3" t="inlineStr">
@@ -11529,22 +11529,22 @@
     <row r="127" ht="25" customHeight="1">
       <c r="A127" s="3" t="inlineStr">
         <is>
-          <t>van der Merwe</t>
+          <t>van Wyk</t>
         </is>
       </c>
       <c r="B127" s="3" t="inlineStr">
         <is>
-          <t>Ingrid</t>
+          <t>Patricia</t>
         </is>
       </c>
       <c r="C127" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D127" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E127" s="3" t="inlineStr">
@@ -11556,66 +11556,93 @@
     <row r="128" ht="25" customHeight="1">
       <c r="A128" s="3" t="inlineStr">
         <is>
-          <t>von der Decken</t>
+          <t>van der Merwe</t>
         </is>
       </c>
       <c r="B128" s="3" t="inlineStr">
         <is>
-          <t>Brian</t>
+          <t>Ingrid</t>
         </is>
       </c>
       <c r="C128" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D128" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E128" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="129" ht="25" customHeight="1">
       <c r="A129" s="3" t="inlineStr">
         <is>
+          <t>von der Decken</t>
+        </is>
+      </c>
+      <c r="B129" s="3" t="inlineStr">
+        <is>
+          <t>Brian</t>
+        </is>
+      </c>
+      <c r="C129" s="3" t="inlineStr">
+        <is>
+          <t>King William's Town</t>
+        </is>
+      </c>
+      <c r="D129" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E129" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="130" ht="25" customHeight="1">
+      <c r="A130" s="3" t="inlineStr">
+        <is>
           <t>‘t Hart</t>
         </is>
       </c>
-      <c r="B129" s="3" t="inlineStr">
+      <c r="B130" s="3" t="inlineStr">
         <is>
           <t>Michelle</t>
         </is>
       </c>
-      <c r="C129" s="3" t="inlineStr">
+      <c r="C130" s="3" t="inlineStr">
         <is>
           <t>Benoni Lakes</t>
         </is>
       </c>
-      <c r="D129" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E129" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" s="1" t="inlineStr">
-        <is>
-          <t>Number of attendees: 127</t>
+      <c r="D130" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E130" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="inlineStr">
+        <is>
+          <t>Number of attendees: 128</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="inlineStr">
         <is>
           <t>Number of voters: 52</t>
         </is>
@@ -11651,7 +11678,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Registrees as of 22/04/2021 13:11</t>
+          <t>410W Registrees as of 22/04/2021 15:29</t>
         </is>
       </c>
     </row>
@@ -15773,7 +15800,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Voting details as of 22/04/2021 13:11</t>
+          <t>410E Voting details as of 22/04/2021 15:29</t>
         </is>
       </c>
     </row>
@@ -16150,7 +16177,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Voting details as of 22/04/2021 13:11</t>
+          <t>410W Voting details as of 22/04/2021 15:29</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Registree stats backup on Fri 23 Apr 2021 09:24:54 SAST
</commit_message>
<xml_diff>
--- a/static/docs/registrees_list.xlsx
+++ b/static/docs/registrees_list.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F242"/>
+  <dimension ref="A1:F243"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,7 +451,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>MD410 Registrees as of 22/04/2021 15:29</t>
+          <t>MD410 Registrees as of 23/04/2021 09:24</t>
         </is>
       </c>
     </row>
@@ -6954,22 +6954,22 @@
     <row r="205" ht="25" customHeight="1">
       <c r="A205" s="3" t="inlineStr">
         <is>
-          <t>Van de Merwe</t>
+          <t>Van Zyl</t>
         </is>
       </c>
       <c r="B205" s="3" t="inlineStr">
         <is>
-          <t>Marina</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="C205" s="3" t="inlineStr">
         <is>
-          <t>Malmesbury</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D205" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E205" s="3" t="inlineStr">
@@ -6979,29 +6979,29 @@
       </c>
       <c r="F205" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="206" ht="25" customHeight="1">
       <c r="A206" s="3" t="inlineStr">
         <is>
-          <t>Venter</t>
+          <t>Van de Merwe</t>
         </is>
       </c>
       <c r="B206" s="3" t="inlineStr">
         <is>
-          <t>Louis</t>
+          <t>Marina</t>
         </is>
       </c>
       <c r="C206" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Malmesbury</t>
         </is>
       </c>
       <c r="D206" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E206" s="3" t="inlineStr">
@@ -7011,34 +7011,34 @@
       </c>
       <c r="F206" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="207" ht="25" customHeight="1">
       <c r="A207" s="3" t="inlineStr">
         <is>
-          <t>Volker</t>
+          <t>Venter</t>
         </is>
       </c>
       <c r="B207" s="3" t="inlineStr">
         <is>
-          <t>Russell</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="C207" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D207" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E207" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F207" s="3" t="inlineStr">
@@ -7050,96 +7050,96 @@
     <row r="208" ht="25" customHeight="1">
       <c r="A208" s="3" t="inlineStr">
         <is>
-          <t>Von Mollendorf</t>
+          <t>Volker</t>
         </is>
       </c>
       <c r="B208" s="3" t="inlineStr">
         <is>
-          <t>Rinette</t>
+          <t>Russell</t>
         </is>
       </c>
       <c r="C208" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>King William's Town</t>
         </is>
       </c>
       <c r="D208" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E208" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F208" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="209" ht="25" customHeight="1">
       <c r="A209" s="3" t="inlineStr">
         <is>
-          <t>Warman</t>
+          <t>Von Mollendorf</t>
         </is>
       </c>
       <c r="B209" s="3" t="inlineStr">
         <is>
-          <t>Alastair</t>
+          <t>Rinette</t>
         </is>
       </c>
       <c r="C209" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Durbanville</t>
         </is>
       </c>
       <c r="D209" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E209" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F209" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="210" ht="25" customHeight="1">
       <c r="A210" s="3" t="inlineStr">
         <is>
-          <t>Watson</t>
+          <t>Warman</t>
         </is>
       </c>
       <c r="B210" s="3" t="inlineStr">
         <is>
-          <t>Allan</t>
+          <t>Alastair</t>
         </is>
       </c>
       <c r="C210" s="3" t="inlineStr">
         <is>
-          <t>Sea Point</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D210" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E210" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F210" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -7151,22 +7151,22 @@
       </c>
       <c r="B211" s="3" t="inlineStr">
         <is>
-          <t>Alison</t>
+          <t>Allan</t>
         </is>
       </c>
       <c r="C211" s="3" t="inlineStr">
         <is>
-          <t>Sedgefield</t>
+          <t>Sea Point</t>
         </is>
       </c>
       <c r="D211" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E211" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F211" s="3" t="inlineStr">
@@ -7178,27 +7178,27 @@
     <row r="212" ht="25" customHeight="1">
       <c r="A212" s="3" t="inlineStr">
         <is>
-          <t>Williams</t>
+          <t>Watson</t>
         </is>
       </c>
       <c r="B212" s="3" t="inlineStr">
         <is>
-          <t>Johanna</t>
+          <t>Alison</t>
         </is>
       </c>
       <c r="C212" s="3" t="inlineStr">
         <is>
-          <t>Mitchells Plain</t>
+          <t>Sedgefield</t>
         </is>
       </c>
       <c r="D212" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E212" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F212" s="3" t="inlineStr">
@@ -7210,22 +7210,22 @@
     <row r="213" ht="25" customHeight="1">
       <c r="A213" s="3" t="inlineStr">
         <is>
-          <t>Wills</t>
+          <t>Williams</t>
         </is>
       </c>
       <c r="B213" s="3" t="inlineStr">
         <is>
-          <t>Geila</t>
+          <t>Johanna</t>
         </is>
       </c>
       <c r="C213" s="3" t="inlineStr">
         <is>
-          <t>Athlone</t>
+          <t>Mitchells Plain</t>
         </is>
       </c>
       <c r="D213" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E213" s="3" t="inlineStr">
@@ -7242,17 +7242,17 @@
     <row r="214" ht="25" customHeight="1">
       <c r="A214" s="3" t="inlineStr">
         <is>
-          <t>Wilter-Sturges</t>
+          <t>Wills</t>
         </is>
       </c>
       <c r="B214" s="3" t="inlineStr">
         <is>
-          <t>Meredith</t>
+          <t>Geila</t>
         </is>
       </c>
       <c r="C214" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Athlone</t>
         </is>
       </c>
       <c r="D214" s="3" t="inlineStr">
@@ -7267,24 +7267,24 @@
       </c>
       <c r="F214" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="215" ht="25" customHeight="1">
       <c r="A215" s="3" t="inlineStr">
         <is>
-          <t>Wright</t>
+          <t>Wilter-Sturges</t>
         </is>
       </c>
       <c r="B215" s="3" t="inlineStr">
         <is>
-          <t>Rocky</t>
+          <t>Meredith</t>
         </is>
       </c>
       <c r="C215" s="3" t="inlineStr">
         <is>
-          <t>Table View</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D215" s="3" t="inlineStr">
@@ -7294,29 +7294,29 @@
       </c>
       <c r="E215" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F215" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="216" ht="25" customHeight="1">
       <c r="A216" s="3" t="inlineStr">
         <is>
-          <t>Young</t>
+          <t>Wright</t>
         </is>
       </c>
       <c r="B216" s="3" t="inlineStr">
         <is>
-          <t>Judy</t>
+          <t>Rocky</t>
         </is>
       </c>
       <c r="C216" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>Table View</t>
         </is>
       </c>
       <c r="D216" s="3" t="inlineStr">
@@ -7326,7 +7326,7 @@
       </c>
       <c r="E216" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F216" s="3" t="inlineStr">
@@ -7338,17 +7338,17 @@
     <row r="217" ht="25" customHeight="1">
       <c r="A217" s="3" t="inlineStr">
         <is>
-          <t>de Kock</t>
+          <t>Young</t>
         </is>
       </c>
       <c r="B217" s="3" t="inlineStr">
         <is>
-          <t>Engela</t>
+          <t>Judy</t>
         </is>
       </c>
       <c r="C217" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Durbanville</t>
         </is>
       </c>
       <c r="D217" s="3" t="inlineStr">
@@ -7358,7 +7358,7 @@
       </c>
       <c r="E217" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F217" s="3" t="inlineStr">
@@ -7375,7 +7375,7 @@
       </c>
       <c r="B218" s="3" t="inlineStr">
         <is>
-          <t>Francois</t>
+          <t>Engela</t>
         </is>
       </c>
       <c r="C218" s="3" t="inlineStr">
@@ -7402,59 +7402,59 @@
     <row r="219" ht="25" customHeight="1">
       <c r="A219" s="3" t="inlineStr">
         <is>
-          <t>de Silva</t>
+          <t>de Kock</t>
         </is>
       </c>
       <c r="B219" s="3" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Francois</t>
         </is>
       </c>
       <c r="C219" s="3" t="inlineStr">
         <is>
-          <t>Edenvale</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D219" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E219" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F219" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="220" ht="25" customHeight="1">
       <c r="A220" s="3" t="inlineStr">
         <is>
-          <t>du Toit</t>
+          <t>de Silva</t>
         </is>
       </c>
       <c r="B220" s="3" t="inlineStr">
         <is>
-          <t>Desiree</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="C220" s="3" t="inlineStr">
         <is>
-          <t>Ramsgate</t>
+          <t>Edenvale</t>
         </is>
       </c>
       <c r="D220" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E220" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F220" s="3" t="inlineStr">
@@ -7466,22 +7466,22 @@
     <row r="221" ht="25" customHeight="1">
       <c r="A221" s="3" t="inlineStr">
         <is>
-          <t>stier</t>
+          <t>du Toit</t>
         </is>
       </c>
       <c r="B221" s="3" t="inlineStr">
         <is>
-          <t>RORY</t>
+          <t>Desiree</t>
         </is>
       </c>
       <c r="C221" s="3" t="inlineStr">
         <is>
-          <t>Deep South</t>
+          <t>Ramsgate</t>
         </is>
       </c>
       <c r="D221" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E221" s="3" t="inlineStr">
@@ -7491,56 +7491,56 @@
       </c>
       <c r="F221" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="222" ht="25" customHeight="1">
       <c r="A222" s="3" t="inlineStr">
         <is>
-          <t>tyler</t>
+          <t>stier</t>
         </is>
       </c>
       <c r="B222" s="3" t="inlineStr">
         <is>
-          <t>natascha</t>
+          <t>RORY</t>
         </is>
       </c>
       <c r="C222" s="3" t="inlineStr">
         <is>
-          <t>Kensington</t>
+          <t>Deep South</t>
         </is>
       </c>
       <c r="D222" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E222" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F222" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="223" ht="25" customHeight="1">
       <c r="A223" s="3" t="inlineStr">
         <is>
-          <t>van Blerk</t>
+          <t>tyler</t>
         </is>
       </c>
       <c r="B223" s="3" t="inlineStr">
         <is>
-          <t>Carl</t>
+          <t>natascha</t>
         </is>
       </c>
       <c r="C223" s="3" t="inlineStr">
         <is>
-          <t>Eden</t>
+          <t>Kensington</t>
         </is>
       </c>
       <c r="D223" s="3" t="inlineStr">
@@ -7555,24 +7555,24 @@
       </c>
       <c r="F223" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="224" ht="25" customHeight="1">
       <c r="A224" s="3" t="inlineStr">
         <is>
-          <t>van Heerden</t>
+          <t>van Blerk</t>
         </is>
       </c>
       <c r="B224" s="3" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Carl</t>
         </is>
       </c>
       <c r="C224" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Eden</t>
         </is>
       </c>
       <c r="D224" s="3" t="inlineStr">
@@ -7587,7 +7587,7 @@
       </c>
       <c r="F224" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -7599,7 +7599,7 @@
       </c>
       <c r="B225" s="3" t="inlineStr">
         <is>
-          <t>Sandy</t>
+          <t>Sydney</t>
         </is>
       </c>
       <c r="C225" s="3" t="inlineStr">
@@ -7614,7 +7614,7 @@
       </c>
       <c r="E225" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F225" s="3" t="inlineStr">
@@ -7631,17 +7631,17 @@
       </c>
       <c r="B226" s="3" t="inlineStr">
         <is>
-          <t>Craig</t>
+          <t>Sandy</t>
         </is>
       </c>
       <c r="C226" s="3" t="inlineStr">
         <is>
-          <t>East London Beacon Bay</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D226" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E226" s="3" t="inlineStr">
@@ -7663,17 +7663,17 @@
       </c>
       <c r="B227" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Craig</t>
         </is>
       </c>
       <c r="C227" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>East London Beacon Bay</t>
         </is>
       </c>
       <c r="D227" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E227" s="3" t="inlineStr">
@@ -7690,17 +7690,17 @@
     <row r="228" ht="25" customHeight="1">
       <c r="A228" s="3" t="inlineStr">
         <is>
-          <t>van Rensburg</t>
+          <t>van Heerden</t>
         </is>
       </c>
       <c r="B228" s="3" t="inlineStr">
         <is>
-          <t>Johan</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C228" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D228" s="3" t="inlineStr">
@@ -7710,12 +7710,12 @@
       </c>
       <c r="E228" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F228" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -7727,7 +7727,7 @@
       </c>
       <c r="B229" s="3" t="inlineStr">
         <is>
-          <t>Anne</t>
+          <t>Johan</t>
         </is>
       </c>
       <c r="C229" s="3" t="inlineStr">
@@ -7754,17 +7754,17 @@
     <row r="230" ht="25" customHeight="1">
       <c r="A230" s="3" t="inlineStr">
         <is>
-          <t>van Wulven</t>
+          <t>van Rensburg</t>
         </is>
       </c>
       <c r="B230" s="3" t="inlineStr">
         <is>
-          <t>Jeannie</t>
+          <t>Anne</t>
         </is>
       </c>
       <c r="C230" s="3" t="inlineStr">
         <is>
-          <t>Tygerberg Hills</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D230" s="3" t="inlineStr">
@@ -7791,7 +7791,7 @@
       </c>
       <c r="B231" s="3" t="inlineStr">
         <is>
-          <t>Alan</t>
+          <t>Jeannie</t>
         </is>
       </c>
       <c r="C231" s="3" t="inlineStr">
@@ -7823,7 +7823,7 @@
       </c>
       <c r="B232" s="3" t="inlineStr">
         <is>
-          <t>Deon</t>
+          <t>Alan</t>
         </is>
       </c>
       <c r="C232" s="3" t="inlineStr">
@@ -7850,17 +7850,17 @@
     <row r="233" ht="25" customHeight="1">
       <c r="A233" s="3" t="inlineStr">
         <is>
-          <t>van Wyk</t>
+          <t>van Wulven</t>
         </is>
       </c>
       <c r="B233" s="3" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>Deon</t>
         </is>
       </c>
       <c r="C233" s="3" t="inlineStr">
         <is>
-          <t>North Durban</t>
+          <t>Tygerberg Hills</t>
         </is>
       </c>
       <c r="D233" s="3" t="inlineStr">
@@ -7875,7 +7875,7 @@
       </c>
       <c r="F233" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -7887,12 +7887,12 @@
       </c>
       <c r="B234" s="3" t="inlineStr">
         <is>
-          <t>Lindie</t>
+          <t>Kim</t>
         </is>
       </c>
       <c r="C234" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>North Durban</t>
         </is>
       </c>
       <c r="D234" s="3" t="inlineStr">
@@ -7919,12 +7919,12 @@
       </c>
       <c r="B235" s="3" t="inlineStr">
         <is>
-          <t>Willem</t>
+          <t>Lindie</t>
         </is>
       </c>
       <c r="C235" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D235" s="3" t="inlineStr">
@@ -7951,12 +7951,12 @@
       </c>
       <c r="B236" s="3" t="inlineStr">
         <is>
-          <t>Patricia</t>
+          <t>Willem</t>
         </is>
       </c>
       <c r="C236" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D236" s="3" t="inlineStr">
@@ -7978,22 +7978,22 @@
     <row r="237" ht="25" customHeight="1">
       <c r="A237" s="3" t="inlineStr">
         <is>
-          <t>van der Merwe</t>
+          <t>van Wyk</t>
         </is>
       </c>
       <c r="B237" s="3" t="inlineStr">
         <is>
-          <t>Ingrid</t>
+          <t>Patricia</t>
         </is>
       </c>
       <c r="C237" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D237" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E237" s="3" t="inlineStr">
@@ -8010,49 +8010,49 @@
     <row r="238" ht="25" customHeight="1">
       <c r="A238" s="3" t="inlineStr">
         <is>
-          <t>van der Westhuizen</t>
+          <t>van der Merwe</t>
         </is>
       </c>
       <c r="B238" s="3" t="inlineStr">
         <is>
-          <t>Hennie</t>
+          <t>Ingrid</t>
         </is>
       </c>
       <c r="C238" s="3" t="inlineStr">
         <is>
-          <t>Helderberg</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D238" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E238" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F238" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="239" ht="25" customHeight="1">
       <c r="A239" s="3" t="inlineStr">
         <is>
-          <t>von der Decken</t>
+          <t>van der Westhuizen</t>
         </is>
       </c>
       <c r="B239" s="3" t="inlineStr">
         <is>
-          <t>Brian</t>
+          <t>Hennie</t>
         </is>
       </c>
       <c r="C239" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Helderberg</t>
         </is>
       </c>
       <c r="D239" s="3" t="inlineStr">
@@ -8067,51 +8067,83 @@
       </c>
       <c r="F239" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="240" ht="25" customHeight="1">
       <c r="A240" s="3" t="inlineStr">
         <is>
+          <t>von der Decken</t>
+        </is>
+      </c>
+      <c r="B240" s="3" t="inlineStr">
+        <is>
+          <t>Brian</t>
+        </is>
+      </c>
+      <c r="C240" s="3" t="inlineStr">
+        <is>
+          <t>King William's Town</t>
+        </is>
+      </c>
+      <c r="D240" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E240" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F240" s="3" t="inlineStr">
+        <is>
+          <t>410E</t>
+        </is>
+      </c>
+    </row>
+    <row r="241" ht="25" customHeight="1">
+      <c r="A241" s="3" t="inlineStr">
+        <is>
           <t>‘t Hart</t>
         </is>
       </c>
-      <c r="B240" s="3" t="inlineStr">
+      <c r="B241" s="3" t="inlineStr">
         <is>
           <t>Michelle</t>
         </is>
       </c>
-      <c r="C240" s="3" t="inlineStr">
+      <c r="C241" s="3" t="inlineStr">
         <is>
           <t>Benoni Lakes</t>
         </is>
       </c>
-      <c r="D240" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E240" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F240" s="3" t="inlineStr">
+      <c r="D241" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E241" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F241" s="3" t="inlineStr">
         <is>
           <t>410E</t>
-        </is>
-      </c>
-    </row>
-    <row r="241">
-      <c r="A241" s="1" t="inlineStr">
-        <is>
-          <t>Number of attendees: 238</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="inlineStr">
+        <is>
+          <t>Number of attendees: 239</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" s="1" t="inlineStr">
         <is>
           <t>Number of voters: 95</t>
         </is>
@@ -8129,7 +8161,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E132"/>
+  <dimension ref="A1:E133"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8147,7 +8179,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Registrees as of 22/04/2021 15:29</t>
+          <t>410E Registrees as of 23/04/2021 09:24</t>
         </is>
       </c>
     </row>
@@ -11043,7 +11075,7 @@
     <row r="109" ht="25" customHeight="1">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>Venter</t>
+          <t>Van Zyl</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
@@ -11053,7 +11085,7 @@
       </c>
       <c r="C109" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D109" s="3" t="inlineStr">
@@ -11070,44 +11102,44 @@
     <row r="110" ht="25" customHeight="1">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>Volker</t>
+          <t>Venter</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
         <is>
-          <t>Russell</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="C110" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D110" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E110" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="111" ht="25" customHeight="1">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>Warman</t>
+          <t>Volker</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
         <is>
-          <t>Alastair</t>
+          <t>Russell</t>
         </is>
       </c>
       <c r="C111" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>King William's Town</t>
         </is>
       </c>
       <c r="D111" s="3" t="inlineStr">
@@ -11124,17 +11156,17 @@
     <row r="112" ht="25" customHeight="1">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>Williamson</t>
+          <t>Warman</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
         <is>
-          <t>Neville</t>
+          <t>Alastair</t>
         </is>
       </c>
       <c r="C112" s="3" t="inlineStr">
         <is>
-          <t>Port Alfred</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D112" s="3" t="inlineStr">
@@ -11144,24 +11176,24 @@
       </c>
       <c r="E112" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="113" ht="25" customHeight="1">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>Wilter-Sturges</t>
+          <t>Williamson</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
         <is>
-          <t>Meredith</t>
+          <t>Neville</t>
         </is>
       </c>
       <c r="C113" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Port Alfred</t>
         </is>
       </c>
       <c r="D113" s="3" t="inlineStr">
@@ -11178,22 +11210,22 @@
     <row r="114" ht="25" customHeight="1">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>de Silva</t>
+          <t>Wilter-Sturges</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Meredith</t>
         </is>
       </c>
       <c r="C114" s="3" t="inlineStr">
         <is>
-          <t>Edenvale</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D114" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E114" s="3" t="inlineStr">
@@ -11205,27 +11237,27 @@
     <row r="115" ht="25" customHeight="1">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>du Plooy</t>
+          <t>de Silva</t>
         </is>
       </c>
       <c r="B115" s="3" t="inlineStr">
         <is>
-          <t>Tammy</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="C115" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Edenvale</t>
         </is>
       </c>
       <c r="D115" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E115" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -11237,7 +11269,7 @@
       </c>
       <c r="B116" s="3" t="inlineStr">
         <is>
-          <t>Marc</t>
+          <t>Tammy</t>
         </is>
       </c>
       <c r="C116" s="3" t="inlineStr">
@@ -11259,17 +11291,17 @@
     <row r="117" ht="25" customHeight="1">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>du Toit</t>
+          <t>du Plooy</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
         <is>
-          <t>Desiree</t>
+          <t>Marc</t>
         </is>
       </c>
       <c r="C117" s="3" t="inlineStr">
         <is>
-          <t>Ramsgate</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D117" s="3" t="inlineStr">
@@ -11286,17 +11318,17 @@
     <row r="118" ht="25" customHeight="1">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>le Roux</t>
+          <t>du Toit</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
         <is>
-          <t>Jeanette</t>
+          <t>Desiree</t>
         </is>
       </c>
       <c r="C118" s="3" t="inlineStr">
         <is>
-          <t>Gonubie</t>
+          <t>Ramsgate</t>
         </is>
       </c>
       <c r="D118" s="3" t="inlineStr">
@@ -11313,17 +11345,17 @@
     <row r="119" ht="25" customHeight="1">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>tyler</t>
+          <t>le Roux</t>
         </is>
       </c>
       <c r="B119" s="3" t="inlineStr">
         <is>
-          <t>natascha</t>
+          <t>Jeanette</t>
         </is>
       </c>
       <c r="C119" s="3" t="inlineStr">
         <is>
-          <t>Kensington</t>
+          <t>Gonubie</t>
         </is>
       </c>
       <c r="D119" s="3" t="inlineStr">
@@ -11333,24 +11365,24 @@
       </c>
       <c r="E119" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="120" ht="25" customHeight="1">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>van Heerden</t>
+          <t>tyler</t>
         </is>
       </c>
       <c r="B120" s="3" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>natascha</t>
         </is>
       </c>
       <c r="C120" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Kensington</t>
         </is>
       </c>
       <c r="D120" s="3" t="inlineStr">
@@ -11372,7 +11404,7 @@
       </c>
       <c r="B121" s="3" t="inlineStr">
         <is>
-          <t>Sandy</t>
+          <t>Sydney</t>
         </is>
       </c>
       <c r="C121" s="3" t="inlineStr">
@@ -11387,7 +11419,7 @@
       </c>
       <c r="E121" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -11399,17 +11431,17 @@
       </c>
       <c r="B122" s="3" t="inlineStr">
         <is>
-          <t>Craig</t>
+          <t>Sandy</t>
         </is>
       </c>
       <c r="C122" s="3" t="inlineStr">
         <is>
-          <t>East London Beacon Bay</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D122" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E122" s="3" t="inlineStr">
@@ -11426,17 +11458,17 @@
       </c>
       <c r="B123" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Craig</t>
         </is>
       </c>
       <c r="C123" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>East London Beacon Bay</t>
         </is>
       </c>
       <c r="D123" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E123" s="3" t="inlineStr">
@@ -11448,17 +11480,17 @@
     <row r="124" ht="25" customHeight="1">
       <c r="A124" s="3" t="inlineStr">
         <is>
-          <t>van Wyk</t>
+          <t>van Heerden</t>
         </is>
       </c>
       <c r="B124" s="3" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C124" s="3" t="inlineStr">
         <is>
-          <t>North Durban</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D124" s="3" t="inlineStr">
@@ -11468,7 +11500,7 @@
       </c>
       <c r="E124" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -11480,12 +11512,12 @@
       </c>
       <c r="B125" s="3" t="inlineStr">
         <is>
-          <t>Lindie</t>
+          <t>Kim</t>
         </is>
       </c>
       <c r="C125" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>North Durban</t>
         </is>
       </c>
       <c r="D125" s="3" t="inlineStr">
@@ -11507,12 +11539,12 @@
       </c>
       <c r="B126" s="3" t="inlineStr">
         <is>
-          <t>Willem</t>
+          <t>Lindie</t>
         </is>
       </c>
       <c r="C126" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D126" s="3" t="inlineStr">
@@ -11534,12 +11566,12 @@
       </c>
       <c r="B127" s="3" t="inlineStr">
         <is>
-          <t>Patricia</t>
+          <t>Willem</t>
         </is>
       </c>
       <c r="C127" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D127" s="3" t="inlineStr">
@@ -11556,22 +11588,22 @@
     <row r="128" ht="25" customHeight="1">
       <c r="A128" s="3" t="inlineStr">
         <is>
-          <t>van der Merwe</t>
+          <t>van Wyk</t>
         </is>
       </c>
       <c r="B128" s="3" t="inlineStr">
         <is>
-          <t>Ingrid</t>
+          <t>Patricia</t>
         </is>
       </c>
       <c r="C128" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D128" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E128" s="3" t="inlineStr">
@@ -11583,66 +11615,93 @@
     <row r="129" ht="25" customHeight="1">
       <c r="A129" s="3" t="inlineStr">
         <is>
-          <t>von der Decken</t>
+          <t>van der Merwe</t>
         </is>
       </c>
       <c r="B129" s="3" t="inlineStr">
         <is>
-          <t>Brian</t>
+          <t>Ingrid</t>
         </is>
       </c>
       <c r="C129" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D129" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E129" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="130" ht="25" customHeight="1">
       <c r="A130" s="3" t="inlineStr">
         <is>
+          <t>von der Decken</t>
+        </is>
+      </c>
+      <c r="B130" s="3" t="inlineStr">
+        <is>
+          <t>Brian</t>
+        </is>
+      </c>
+      <c r="C130" s="3" t="inlineStr">
+        <is>
+          <t>King William's Town</t>
+        </is>
+      </c>
+      <c r="D130" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E130" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="131" ht="25" customHeight="1">
+      <c r="A131" s="3" t="inlineStr">
+        <is>
           <t>‘t Hart</t>
         </is>
       </c>
-      <c r="B130" s="3" t="inlineStr">
+      <c r="B131" s="3" t="inlineStr">
         <is>
           <t>Michelle</t>
         </is>
       </c>
-      <c r="C130" s="3" t="inlineStr">
+      <c r="C131" s="3" t="inlineStr">
         <is>
           <t>Benoni Lakes</t>
         </is>
       </c>
-      <c r="D130" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E130" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="131">
-      <c r="A131" s="1" t="inlineStr">
-        <is>
-          <t>Number of attendees: 128</t>
+      <c r="D131" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E131" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="inlineStr">
+        <is>
+          <t>Number of attendees: 129</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="1" t="inlineStr">
         <is>
           <t>Number of voters: 52</t>
         </is>
@@ -11678,7 +11737,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Registrees as of 22/04/2021 15:29</t>
+          <t>410W Registrees as of 23/04/2021 09:24</t>
         </is>
       </c>
     </row>
@@ -15800,7 +15859,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Voting details as of 22/04/2021 15:29</t>
+          <t>410E Voting details as of 23/04/2021 09:24</t>
         </is>
       </c>
     </row>
@@ -16177,7 +16236,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Voting details as of 22/04/2021 15:29</t>
+          <t>410W Voting details as of 23/04/2021 09:24</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Registree stats backup on Fri 23 Apr 2021 11:02:40 SAST
</commit_message>
<xml_diff>
--- a/static/docs/registrees_list.xlsx
+++ b/static/docs/registrees_list.xlsx
@@ -451,7 +451,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>MD410 Registrees as of 23/04/2021 09:24</t>
+          <t>MD410 Registrees as of 23/04/2021 11:02</t>
         </is>
       </c>
     </row>
@@ -8161,7 +8161,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E133"/>
+  <dimension ref="A1:E134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8179,7 +8179,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Registrees as of 23/04/2021 09:24</t>
+          <t>410E Registrees as of 23/04/2021 11:02</t>
         </is>
       </c>
     </row>
@@ -8753,17 +8753,17 @@
     <row r="23" ht="25" customHeight="1">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>Erasmus</t>
+          <t>Elske</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
         <is>
-          <t>Freddie</t>
+          <t>Valerie</t>
         </is>
       </c>
       <c r="C23" s="3" t="inlineStr">
         <is>
-          <t>Uitenhage</t>
+          <t>Krugersdorp</t>
         </is>
       </c>
       <c r="D23" s="3" t="inlineStr">
@@ -8773,24 +8773,24 @@
       </c>
       <c r="E23" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="24" ht="25" customHeight="1">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>Fourie</t>
+          <t>Erasmus</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
         <is>
-          <t>Lucille</t>
+          <t>Freddie</t>
         </is>
       </c>
       <c r="C24" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Uitenhage</t>
         </is>
       </c>
       <c r="D24" s="3" t="inlineStr">
@@ -8800,24 +8800,24 @@
       </c>
       <c r="E24" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="25" ht="25" customHeight="1">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>Foxcroft</t>
+          <t>Fourie</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
         <is>
-          <t>Kelvin</t>
+          <t>Lucille</t>
         </is>
       </c>
       <c r="C25" s="3" t="inlineStr">
         <is>
-          <t>Helderkruin</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D25" s="3" t="inlineStr">
@@ -8839,7 +8839,7 @@
       </c>
       <c r="B26" s="3" t="inlineStr">
         <is>
-          <t>Jenny</t>
+          <t>Kelvin</t>
         </is>
       </c>
       <c r="C26" s="3" t="inlineStr">
@@ -8866,7 +8866,7 @@
       </c>
       <c r="B27" s="3" t="inlineStr">
         <is>
-          <t>Katherine</t>
+          <t>Jenny</t>
         </is>
       </c>
       <c r="C27" s="3" t="inlineStr">
@@ -8888,17 +8888,17 @@
     <row r="28" ht="25" customHeight="1">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>Froise</t>
+          <t>Foxcroft</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
         <is>
-          <t>Martin</t>
+          <t>Katherine</t>
         </is>
       </c>
       <c r="C28" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Helderkruin</t>
         </is>
       </c>
       <c r="D28" s="3" t="inlineStr">
@@ -8908,24 +8908,24 @@
       </c>
       <c r="E28" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="29" ht="25" customHeight="1">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>Gerhard</t>
+          <t>Froise</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
         <is>
-          <t>Bernd</t>
+          <t>Martin</t>
         </is>
       </c>
       <c r="C29" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D29" s="3" t="inlineStr">
@@ -8947,7 +8947,7 @@
       </c>
       <c r="B30" s="3" t="inlineStr">
         <is>
-          <t>Shirley</t>
+          <t>Bernd</t>
         </is>
       </c>
       <c r="C30" s="3" t="inlineStr">
@@ -8962,24 +8962,24 @@
       </c>
       <c r="E30" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="31" ht="25" customHeight="1">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>Graham</t>
+          <t>Gerhard</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
         <is>
-          <t>Valerie</t>
+          <t>Shirley</t>
         </is>
       </c>
       <c r="C31" s="3" t="inlineStr">
         <is>
-          <t>Nelspruit</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D31" s="3" t="inlineStr">
@@ -8989,7 +8989,7 @@
       </c>
       <c r="E31" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -9001,7 +9001,7 @@
       </c>
       <c r="B32" s="3" t="inlineStr">
         <is>
-          <t>Mike</t>
+          <t>Valerie</t>
         </is>
       </c>
       <c r="C32" s="3" t="inlineStr">
@@ -9016,29 +9016,29 @@
       </c>
       <c r="E32" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="33" ht="25" customHeight="1">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>Griffith</t>
+          <t>Graham</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
         <is>
-          <t>David</t>
+          <t>Mike</t>
         </is>
       </c>
       <c r="C33" s="3" t="inlineStr">
         <is>
-          <t>The Wilds</t>
+          <t>Nelspruit</t>
         </is>
       </c>
       <c r="D33" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E33" s="3" t="inlineStr">
@@ -9050,22 +9050,22 @@
     <row r="34" ht="25" customHeight="1">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>Guthrie</t>
+          <t>Griffith</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
         <is>
-          <t>Clint</t>
+          <t>David</t>
         </is>
       </c>
       <c r="C34" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>The Wilds</t>
         </is>
       </c>
       <c r="D34" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E34" s="3" t="inlineStr">
@@ -9077,12 +9077,12 @@
     <row r="35" ht="25" customHeight="1">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>HERMANUS</t>
+          <t>Guthrie</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
         <is>
-          <t>MBULELO</t>
+          <t>Clint</t>
         </is>
       </c>
       <c r="C35" s="3" t="inlineStr">
@@ -9092,7 +9092,7 @@
       </c>
       <c r="D35" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E35" s="3" t="inlineStr">
@@ -9104,22 +9104,22 @@
     <row r="36" ht="25" customHeight="1">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>HOLLIMAN</t>
+          <t>HERMANUS</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
         <is>
-          <t>KEITH ALEXANDER</t>
+          <t>MBULELO</t>
         </is>
       </c>
       <c r="C36" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D36" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E36" s="3" t="inlineStr">
@@ -9131,17 +9131,17 @@
     <row r="37" ht="25" customHeight="1">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>Heathcote</t>
+          <t>HOLLIMAN</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
         <is>
-          <t>Mike</t>
+          <t>KEITH ALEXANDER</t>
         </is>
       </c>
       <c r="C37" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D37" s="3" t="inlineStr">
@@ -9151,24 +9151,24 @@
       </c>
       <c r="E37" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="38" ht="25" customHeight="1">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>Herzfeld</t>
+          <t>Heathcote</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
         <is>
-          <t>Evelyn</t>
+          <t>Mike</t>
         </is>
       </c>
       <c r="C38" s="3" t="inlineStr">
         <is>
-          <t>Edenvale</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D38" s="3" t="inlineStr">
@@ -9178,24 +9178,24 @@
       </c>
       <c r="E38" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="39" ht="25" customHeight="1">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>Higgins</t>
+          <t>Herzfeld</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
         <is>
-          <t>Wendy</t>
+          <t>Evelyn</t>
         </is>
       </c>
       <c r="C39" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Edenvale</t>
         </is>
       </c>
       <c r="D39" s="3" t="inlineStr">
@@ -9212,17 +9212,17 @@
     <row r="40" ht="25" customHeight="1">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>Hobbs</t>
+          <t>Higgins</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
         <is>
-          <t>Avril</t>
+          <t>Wendy</t>
         </is>
       </c>
       <c r="C40" s="3" t="inlineStr">
         <is>
-          <t>North Durban</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D40" s="3" t="inlineStr">
@@ -9232,7 +9232,7 @@
       </c>
       <c r="E40" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -9244,7 +9244,7 @@
       </c>
       <c r="B41" s="3" t="inlineStr">
         <is>
-          <t>Trevor</t>
+          <t>Avril</t>
         </is>
       </c>
       <c r="C41" s="3" t="inlineStr">
@@ -9266,17 +9266,17 @@
     <row r="42" ht="25" customHeight="1">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>Hocking</t>
+          <t>Hobbs</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
         <is>
-          <t>Jacqui</t>
+          <t>Trevor</t>
         </is>
       </c>
       <c r="C42" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>North Durban</t>
         </is>
       </c>
       <c r="D42" s="3" t="inlineStr">
@@ -9298,7 +9298,7 @@
       </c>
       <c r="B43" s="3" t="inlineStr">
         <is>
-          <t>Cliff</t>
+          <t>Jacqui</t>
         </is>
       </c>
       <c r="C43" s="3" t="inlineStr">
@@ -9313,24 +9313,24 @@
       </c>
       <c r="E43" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="44" ht="25" customHeight="1">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>JOHNSTON</t>
+          <t>Hocking</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
         <is>
-          <t>MALCOLM</t>
+          <t>Cliff</t>
         </is>
       </c>
       <c r="C44" s="3" t="inlineStr">
         <is>
-          <t>Standerton</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D44" s="3" t="inlineStr">
@@ -9340,24 +9340,24 @@
       </c>
       <c r="E44" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="45" ht="25" customHeight="1">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>Jackman</t>
+          <t>JOHNSTON</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
         <is>
-          <t>Gail</t>
+          <t>MALCOLM</t>
         </is>
       </c>
       <c r="C45" s="3" t="inlineStr">
         <is>
-          <t>Nelspruit</t>
+          <t>Standerton</t>
         </is>
       </c>
       <c r="D45" s="3" t="inlineStr">
@@ -9367,24 +9367,24 @@
       </c>
       <c r="E45" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="46" ht="25" customHeight="1">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>Jackson</t>
+          <t>Jackman</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
         <is>
-          <t>Alna</t>
+          <t>Gail</t>
         </is>
       </c>
       <c r="C46" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Nelspruit</t>
         </is>
       </c>
       <c r="D46" s="3" t="inlineStr">
@@ -9394,24 +9394,24 @@
       </c>
       <c r="E46" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="47" ht="25" customHeight="1">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>Kienast</t>
+          <t>Jackson</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
         <is>
-          <t>Margie</t>
+          <t>Alna</t>
         </is>
       </c>
       <c r="C47" s="3" t="inlineStr">
         <is>
-          <t>Edenvale</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D47" s="3" t="inlineStr">
@@ -9421,24 +9421,24 @@
       </c>
       <c r="E47" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="48" ht="25" customHeight="1">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>Kimari</t>
+          <t>Kienast</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
         <is>
-          <t>Joyce</t>
+          <t>Margie</t>
         </is>
       </c>
       <c r="C48" s="3" t="inlineStr">
         <is>
-          <t>Eden</t>
+          <t>Edenvale</t>
         </is>
       </c>
       <c r="D48" s="3" t="inlineStr">
@@ -9455,17 +9455,17 @@
     <row r="49" ht="25" customHeight="1">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>King</t>
+          <t>Kimari</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
         <is>
-          <t>Ian</t>
+          <t>Joyce</t>
         </is>
       </c>
       <c r="C49" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Eden</t>
         </is>
       </c>
       <c r="D49" s="3" t="inlineStr">
@@ -9475,7 +9475,7 @@
       </c>
       <c r="E49" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -9487,7 +9487,7 @@
       </c>
       <c r="B50" s="3" t="inlineStr">
         <is>
-          <t>Sandy</t>
+          <t>Ian</t>
         </is>
       </c>
       <c r="C50" s="3" t="inlineStr">
@@ -9509,17 +9509,17 @@
     <row r="51" ht="25" customHeight="1">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>Koekemoer</t>
+          <t>King</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
         <is>
-          <t>Christa</t>
+          <t>Sandy</t>
         </is>
       </c>
       <c r="C51" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D51" s="3" t="inlineStr">
@@ -9529,29 +9529,29 @@
       </c>
       <c r="E51" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="52" ht="25" customHeight="1">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>Kruger</t>
+          <t>Koekemoer</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
         <is>
-          <t>Pieter</t>
+          <t>Christa</t>
         </is>
       </c>
       <c r="C52" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D52" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E52" s="3" t="inlineStr">
@@ -9568,7 +9568,7 @@
       </c>
       <c r="B53" s="3" t="inlineStr">
         <is>
-          <t>Niqula</t>
+          <t>Pieter</t>
         </is>
       </c>
       <c r="C53" s="3" t="inlineStr">
@@ -9590,22 +9590,22 @@
     <row r="54" ht="25" customHeight="1">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>Laas</t>
+          <t>Kruger</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
         <is>
-          <t>Natalie</t>
+          <t>Niqula</t>
         </is>
       </c>
       <c r="C54" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D54" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E54" s="3" t="inlineStr">
@@ -9617,17 +9617,17 @@
     <row r="55" ht="25" customHeight="1">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>Labuschagne</t>
+          <t>Laas</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
         <is>
-          <t>Susan</t>
+          <t>Natalie</t>
         </is>
       </c>
       <c r="C55" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D55" s="3" t="inlineStr">
@@ -9644,22 +9644,22 @@
     <row r="56" ht="25" customHeight="1">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>Langton</t>
+          <t>Labuschagne</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
         <is>
-          <t>Evelyn May</t>
+          <t>Susan</t>
         </is>
       </c>
       <c r="C56" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D56" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E56" s="3" t="inlineStr">
@@ -9671,39 +9671,39 @@
     <row r="57" ht="25" customHeight="1">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>Lautenbach</t>
+          <t>Langton</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
         <is>
-          <t>Steven</t>
+          <t>Evelyn May</t>
         </is>
       </c>
       <c r="C57" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D57" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E57" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="58" ht="25" customHeight="1">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>Logan</t>
+          <t>Lautenbach</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
         <is>
-          <t>Graeme</t>
+          <t>Steven</t>
         </is>
       </c>
       <c r="C58" s="3" t="inlineStr">
@@ -9718,24 +9718,24 @@
       </c>
       <c r="E58" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="59" ht="25" customHeight="1">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>Love</t>
+          <t>Logan</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
         <is>
-          <t>Dee</t>
+          <t>Graeme</t>
         </is>
       </c>
       <c r="C59" s="3" t="inlineStr">
         <is>
-          <t>Cowies Hill</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D59" s="3" t="inlineStr">
@@ -9752,17 +9752,17 @@
     <row r="60" ht="25" customHeight="1">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>Luck</t>
+          <t>Love</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
         <is>
-          <t>Zarina</t>
+          <t>Dee</t>
         </is>
       </c>
       <c r="C60" s="3" t="inlineStr">
         <is>
-          <t>Newcastle</t>
+          <t>Cowies Hill</t>
         </is>
       </c>
       <c r="D60" s="3" t="inlineStr">
@@ -9772,24 +9772,24 @@
       </c>
       <c r="E60" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="61" ht="25" customHeight="1">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>MILLS</t>
+          <t>Luck</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
         <is>
-          <t>BERNICE</t>
+          <t>Zarina</t>
         </is>
       </c>
       <c r="C61" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Newcastle</t>
         </is>
       </c>
       <c r="D61" s="3" t="inlineStr">
@@ -9806,17 +9806,17 @@
     <row r="62" ht="25" customHeight="1">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>Mare</t>
+          <t>MILLS</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
         <is>
-          <t>Beaulieu</t>
+          <t>BERNICE</t>
         </is>
       </c>
       <c r="C62" s="3" t="inlineStr">
         <is>
-          <t>Benoni Lakes</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D62" s="3" t="inlineStr">
@@ -9833,12 +9833,12 @@
     <row r="63" ht="25" customHeight="1">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>Maré</t>
+          <t>Mare</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
         <is>
-          <t>Nick</t>
+          <t>Beaulieu</t>
         </is>
       </c>
       <c r="C63" s="3" t="inlineStr">
@@ -9853,24 +9853,24 @@
       </c>
       <c r="E63" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="64" ht="25" customHeight="1">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>Masson</t>
+          <t>Maré</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
         <is>
-          <t>Jean</t>
+          <t>Nick</t>
         </is>
       </c>
       <c r="C64" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Benoni Lakes</t>
         </is>
       </c>
       <c r="D64" s="3" t="inlineStr">
@@ -9887,17 +9887,17 @@
     <row r="65" ht="25" customHeight="1">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>McDonald</t>
+          <t>Masson</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
         <is>
-          <t>Rochelle</t>
+          <t>Jean</t>
         </is>
       </c>
       <c r="C65" s="3" t="inlineStr">
         <is>
-          <t>Vereeniging</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D65" s="3" t="inlineStr">
@@ -9914,17 +9914,17 @@
     <row r="66" ht="25" customHeight="1">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>McKerrow</t>
+          <t>McDonald</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
         <is>
-          <t>Alec</t>
+          <t>Rochelle</t>
         </is>
       </c>
       <c r="C66" s="3" t="inlineStr">
         <is>
-          <t>Port Alfred</t>
+          <t>Vereeniging</t>
         </is>
       </c>
       <c r="D66" s="3" t="inlineStr">
@@ -9941,17 +9941,17 @@
     <row r="67" ht="25" customHeight="1">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>Mccullough</t>
+          <t>McKerrow</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
         <is>
-          <t>David</t>
+          <t>Alec</t>
         </is>
       </c>
       <c r="C67" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Port Alfred</t>
         </is>
       </c>
       <c r="D67" s="3" t="inlineStr">
@@ -9968,17 +9968,17 @@
     <row r="68" ht="25" customHeight="1">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>Meltzer</t>
+          <t>Mccullough</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>David</t>
         </is>
       </c>
       <c r="C68" s="3" t="inlineStr">
         <is>
-          <t>The Wilds</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D68" s="3" t="inlineStr">
@@ -9988,24 +9988,24 @@
       </c>
       <c r="E68" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="69" ht="25" customHeight="1">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>Meyer</t>
+          <t>Meltzer</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
         <is>
-          <t>Denis</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C69" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>The Wilds</t>
         </is>
       </c>
       <c r="D69" s="3" t="inlineStr">
@@ -10022,17 +10022,17 @@
     <row r="70" ht="25" customHeight="1">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>Michas</t>
+          <t>Meyer</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
         <is>
-          <t>Roy</t>
+          <t>Denis</t>
         </is>
       </c>
       <c r="C70" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D70" s="3" t="inlineStr">
@@ -10054,7 +10054,7 @@
       </c>
       <c r="B71" s="3" t="inlineStr">
         <is>
-          <t>Dawn</t>
+          <t>Roy</t>
         </is>
       </c>
       <c r="C71" s="3" t="inlineStr">
@@ -10069,24 +10069,24 @@
       </c>
       <c r="E71" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="72" ht="25" customHeight="1">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>Mills</t>
+          <t>Michas</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>Dawn</t>
         </is>
       </c>
       <c r="C72" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D72" s="3" t="inlineStr">
@@ -10096,24 +10096,24 @@
       </c>
       <c r="E72" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="73" ht="25" customHeight="1">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>Mitchell</t>
+          <t>Mills</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
         <is>
-          <t>Alana</t>
+          <t>Patrick</t>
         </is>
       </c>
       <c r="C73" s="3" t="inlineStr">
         <is>
-          <t>Rustenburg</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D73" s="3" t="inlineStr">
@@ -10123,7 +10123,7 @@
       </c>
       <c r="E73" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -10135,7 +10135,7 @@
       </c>
       <c r="B74" s="3" t="inlineStr">
         <is>
-          <t>Juan</t>
+          <t>Alana</t>
         </is>
       </c>
       <c r="C74" s="3" t="inlineStr">
@@ -10150,24 +10150,24 @@
       </c>
       <c r="E74" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="75" ht="25" customHeight="1">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>Murray</t>
+          <t>Mitchell</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
         <is>
-          <t>Suzanne</t>
+          <t>Juan</t>
         </is>
       </c>
       <c r="C75" s="3" t="inlineStr">
         <is>
-          <t>Vereeniging</t>
+          <t>Rustenburg</t>
         </is>
       </c>
       <c r="D75" s="3" t="inlineStr">
@@ -10189,7 +10189,7 @@
       </c>
       <c r="B76" s="3" t="inlineStr">
         <is>
-          <t>Gary</t>
+          <t>Suzanne</t>
         </is>
       </c>
       <c r="C76" s="3" t="inlineStr">
@@ -10211,17 +10211,17 @@
     <row r="77" ht="25" customHeight="1">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>Nel</t>
+          <t>Murray</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
         <is>
-          <t>Theo</t>
+          <t>Gary</t>
         </is>
       </c>
       <c r="C77" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Vereeniging</t>
         </is>
       </c>
       <c r="D77" s="3" t="inlineStr">
@@ -10238,17 +10238,17 @@
     <row r="78" ht="25" customHeight="1">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>Newlands</t>
+          <t>Nel</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
         <is>
-          <t>Mike</t>
+          <t>Theo</t>
         </is>
       </c>
       <c r="C78" s="3" t="inlineStr">
         <is>
-          <t>Port Alfred</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D78" s="3" t="inlineStr">
@@ -10265,17 +10265,17 @@
     <row r="79" ht="25" customHeight="1">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>Ngobozana</t>
+          <t>Newlands</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
         <is>
-          <t>Sphiwe</t>
+          <t>Mike</t>
         </is>
       </c>
       <c r="C79" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Port Alfred</t>
         </is>
       </c>
       <c r="D79" s="3" t="inlineStr">
@@ -10285,24 +10285,24 @@
       </c>
       <c r="E79" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="80" ht="25" customHeight="1">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>Oberholzer</t>
+          <t>Ngobozana</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
         <is>
-          <t>PDG Bokkie</t>
+          <t>Sphiwe</t>
         </is>
       </c>
       <c r="C80" s="3" t="inlineStr">
         <is>
-          <t>Uitenhage</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D80" s="3" t="inlineStr">
@@ -10319,17 +10319,17 @@
     <row r="81" ht="25" customHeight="1">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>PORTEOUS</t>
+          <t>Oberholzer</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
         <is>
-          <t>BRIAN</t>
+          <t>PDG Bokkie</t>
         </is>
       </c>
       <c r="C81" s="3" t="inlineStr">
         <is>
-          <t>Hibberdene</t>
+          <t>Uitenhage</t>
         </is>
       </c>
       <c r="D81" s="3" t="inlineStr">
@@ -10339,24 +10339,24 @@
       </c>
       <c r="E81" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="82" ht="25" customHeight="1">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>Paijmans</t>
+          <t>PORTEOUS</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
         <is>
-          <t>Bronwyn Anne</t>
+          <t>BRIAN</t>
         </is>
       </c>
       <c r="C82" s="3" t="inlineStr">
         <is>
-          <t>Cowies Hill</t>
+          <t>Hibberdene</t>
         </is>
       </c>
       <c r="D82" s="3" t="inlineStr">
@@ -10366,24 +10366,24 @@
       </c>
       <c r="E82" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="83" ht="25" customHeight="1">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>Pantoleon</t>
+          <t>Paijmans</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
         <is>
-          <t>Teresa</t>
+          <t>Bronwyn Anne</t>
         </is>
       </c>
       <c r="C83" s="3" t="inlineStr">
         <is>
-          <t>Vereeniging</t>
+          <t>Cowies Hill</t>
         </is>
       </c>
       <c r="D83" s="3" t="inlineStr">
@@ -10393,24 +10393,24 @@
       </c>
       <c r="E83" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="84" ht="25" customHeight="1">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>Polkinghorne</t>
+          <t>Pantoleon</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
         <is>
-          <t>Tracey</t>
+          <t>Teresa</t>
         </is>
       </c>
       <c r="C84" s="3" t="inlineStr">
         <is>
-          <t>Kensington</t>
+          <t>Vereeniging</t>
         </is>
       </c>
       <c r="D84" s="3" t="inlineStr">
@@ -10432,7 +10432,7 @@
       </c>
       <c r="B85" s="3" t="inlineStr">
         <is>
-          <t>Gavin</t>
+          <t>Tracey</t>
         </is>
       </c>
       <c r="C85" s="3" t="inlineStr">
@@ -10447,29 +10447,29 @@
       </c>
       <c r="E85" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="86" ht="25" customHeight="1">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>Rashirai</t>
+          <t>Polkinghorne</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
         <is>
-          <t>Tabeth</t>
+          <t>Gavin</t>
         </is>
       </c>
       <c r="C86" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Kensington</t>
         </is>
       </c>
       <c r="D86" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E86" s="3" t="inlineStr">
@@ -10481,44 +10481,44 @@
     <row r="87" ht="25" customHeight="1">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>Reniers</t>
+          <t>Rashirai</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
         <is>
-          <t>Hugo</t>
+          <t>Tabeth</t>
         </is>
       </c>
       <c r="C87" s="3" t="inlineStr">
         <is>
-          <t>Nelspruit</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D87" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E87" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="88" ht="25" customHeight="1">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>Sabatier</t>
+          <t>Reniers</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
         <is>
-          <t>Rodney</t>
+          <t>Hugo</t>
         </is>
       </c>
       <c r="C88" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Nelspruit</t>
         </is>
       </c>
       <c r="D88" s="3" t="inlineStr">
@@ -10535,17 +10535,17 @@
     <row r="89" ht="25" customHeight="1">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>Searle</t>
+          <t>Sabatier</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
         <is>
-          <t>Francis</t>
+          <t>Rodney</t>
         </is>
       </c>
       <c r="C89" s="3" t="inlineStr">
         <is>
-          <t>Kouga</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D89" s="3" t="inlineStr">
@@ -10567,7 +10567,7 @@
       </c>
       <c r="B90" s="3" t="inlineStr">
         <is>
-          <t>Gloria</t>
+          <t>Francis</t>
         </is>
       </c>
       <c r="C90" s="3" t="inlineStr">
@@ -10582,24 +10582,24 @@
       </c>
       <c r="E90" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="91" ht="25" customHeight="1">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>Smit</t>
+          <t>Searle</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
         <is>
-          <t>Sue</t>
+          <t>Gloria</t>
         </is>
       </c>
       <c r="C91" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Kouga</t>
         </is>
       </c>
       <c r="D91" s="3" t="inlineStr">
@@ -10616,17 +10616,17 @@
     <row r="92" ht="25" customHeight="1">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Smit</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
         <is>
-          <t>Jeff</t>
+          <t>Sue</t>
         </is>
       </c>
       <c r="C92" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D92" s="3" t="inlineStr">
@@ -10643,17 +10643,17 @@
     <row r="93" ht="25" customHeight="1">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>Stander</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
         <is>
-          <t>Max</t>
+          <t>Jeff</t>
         </is>
       </c>
       <c r="C93" s="3" t="inlineStr">
         <is>
-          <t>Port Alfred</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D93" s="3" t="inlineStr">
@@ -10675,12 +10675,12 @@
       </c>
       <c r="B94" s="3" t="inlineStr">
         <is>
-          <t>Ashley</t>
+          <t>Max</t>
         </is>
       </c>
       <c r="C94" s="3" t="inlineStr">
         <is>
-          <t>Krugersdorp</t>
+          <t>Port Alfred</t>
         </is>
       </c>
       <c r="D94" s="3" t="inlineStr">
@@ -10690,7 +10690,7 @@
       </c>
       <c r="E94" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -10702,7 +10702,7 @@
       </c>
       <c r="B95" s="3" t="inlineStr">
         <is>
-          <t>Brett Jason</t>
+          <t>Ashley</t>
         </is>
       </c>
       <c r="C95" s="3" t="inlineStr">
@@ -10717,29 +10717,29 @@
       </c>
       <c r="E95" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="96" ht="25" customHeight="1">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>Steyn</t>
+          <t>Stander</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
         <is>
-          <t>Elna</t>
+          <t>Brett Jason</t>
         </is>
       </c>
       <c r="C96" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Krugersdorp</t>
         </is>
       </c>
       <c r="D96" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E96" s="3" t="inlineStr">
@@ -10751,22 +10751,22 @@
     <row r="97" ht="25" customHeight="1">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>Sturges</t>
+          <t>Steyn</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
         <is>
-          <t>Trevor</t>
+          <t>Elna</t>
         </is>
       </c>
       <c r="C97" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D97" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E97" s="3" t="inlineStr">
@@ -10778,17 +10778,17 @@
     <row r="98" ht="25" customHeight="1">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>Talbot</t>
+          <t>Sturges</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
         <is>
-          <t>Lauryn</t>
+          <t>Trevor</t>
         </is>
       </c>
       <c r="C98" s="3" t="inlineStr">
         <is>
-          <t>Benoni Lakes</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D98" s="3" t="inlineStr">
@@ -10805,17 +10805,17 @@
     <row r="99" ht="25" customHeight="1">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>Theron</t>
+          <t>Talbot</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
         <is>
-          <t>Pierre</t>
+          <t>Lauryn</t>
         </is>
       </c>
       <c r="C99" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Benoni Lakes</t>
         </is>
       </c>
       <c r="D99" s="3" t="inlineStr">
@@ -10837,7 +10837,7 @@
       </c>
       <c r="B100" s="3" t="inlineStr">
         <is>
-          <t>Moira</t>
+          <t>Pierre</t>
         </is>
       </c>
       <c r="C100" s="3" t="inlineStr">
@@ -10859,17 +10859,17 @@
     <row r="101" ht="25" customHeight="1">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>Townsend</t>
+          <t>Theron</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
         <is>
-          <t>Diane</t>
+          <t>Moira</t>
         </is>
       </c>
       <c r="C101" s="3" t="inlineStr">
         <is>
-          <t>Benoni Lakes</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D101" s="3" t="inlineStr">
@@ -10879,56 +10879,56 @@
       </c>
       <c r="E101" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="102" ht="25" customHeight="1">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>Toye</t>
+          <t>Townsend</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
         <is>
-          <t>Omolayo</t>
+          <t>Diane</t>
         </is>
       </c>
       <c r="C102" s="3" t="inlineStr">
         <is>
-          <t>The Wilds</t>
+          <t>Benoni Lakes</t>
         </is>
       </c>
       <c r="D102" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E102" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="103" ht="25" customHeight="1">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>Tuckett</t>
+          <t>Toye</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
         <is>
-          <t>Alistair</t>
+          <t>Omolayo</t>
         </is>
       </c>
       <c r="C103" s="3" t="inlineStr">
         <is>
-          <t>Roodepoort Clearwater Cyber</t>
+          <t>The Wilds</t>
         </is>
       </c>
       <c r="D103" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E103" s="3" t="inlineStr">
@@ -10945,7 +10945,7 @@
       </c>
       <c r="B104" s="3" t="inlineStr">
         <is>
-          <t>Rowan</t>
+          <t>Alistair</t>
         </is>
       </c>
       <c r="C104" s="3" t="inlineStr">
@@ -10960,7 +10960,7 @@
       </c>
       <c r="E104" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -10972,7 +10972,7 @@
       </c>
       <c r="B105" s="3" t="inlineStr">
         <is>
-          <t>Gail</t>
+          <t>Rowan</t>
         </is>
       </c>
       <c r="C105" s="3" t="inlineStr">
@@ -10987,29 +10987,29 @@
       </c>
       <c r="E105" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="106" ht="25" customHeight="1">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>Uchytil</t>
+          <t>Tuckett</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
         <is>
-          <t>Jiri</t>
+          <t>Gail</t>
         </is>
       </c>
       <c r="C106" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Roodepoort Clearwater Cyber</t>
         </is>
       </c>
       <c r="D106" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E106" s="3" t="inlineStr">
@@ -11021,17 +11021,17 @@
     <row r="107" ht="25" customHeight="1">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>VAN DER MERWE</t>
+          <t>Uchytil</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
         <is>
-          <t>PATRICIA</t>
+          <t>Jiri</t>
         </is>
       </c>
       <c r="C107" s="3" t="inlineStr">
         <is>
-          <t>East London Port Rex</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D107" s="3" t="inlineStr">
@@ -11041,24 +11041,24 @@
       </c>
       <c r="E107" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="108" ht="25" customHeight="1">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>Van Niekerk</t>
+          <t>VAN DER MERWE</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
         <is>
-          <t>Riaan</t>
+          <t>PATRICIA</t>
         </is>
       </c>
       <c r="C108" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>East London Port Rex</t>
         </is>
       </c>
       <c r="D108" s="3" t="inlineStr">
@@ -11068,24 +11068,24 @@
       </c>
       <c r="E108" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="109" ht="25" customHeight="1">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>Van Zyl</t>
+          <t>Van Niekerk</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
         <is>
-          <t>Louis</t>
+          <t>Riaan</t>
         </is>
       </c>
       <c r="C109" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D109" s="3" t="inlineStr">
@@ -11102,7 +11102,7 @@
     <row r="110" ht="25" customHeight="1">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>Venter</t>
+          <t>Van Zyl</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -11112,7 +11112,7 @@
       </c>
       <c r="C110" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D110" s="3" t="inlineStr">
@@ -11129,44 +11129,44 @@
     <row r="111" ht="25" customHeight="1">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>Volker</t>
+          <t>Venter</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
         <is>
-          <t>Russell</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="C111" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D111" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E111" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="112" ht="25" customHeight="1">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>Warman</t>
+          <t>Volker</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
         <is>
-          <t>Alastair</t>
+          <t>Russell</t>
         </is>
       </c>
       <c r="C112" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>King William's Town</t>
         </is>
       </c>
       <c r="D112" s="3" t="inlineStr">
@@ -11183,17 +11183,17 @@
     <row r="113" ht="25" customHeight="1">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>Williamson</t>
+          <t>Warman</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
         <is>
-          <t>Neville</t>
+          <t>Alastair</t>
         </is>
       </c>
       <c r="C113" s="3" t="inlineStr">
         <is>
-          <t>Port Alfred</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D113" s="3" t="inlineStr">
@@ -11203,24 +11203,24 @@
       </c>
       <c r="E113" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="114" ht="25" customHeight="1">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>Wilter-Sturges</t>
+          <t>Williamson</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
         <is>
-          <t>Meredith</t>
+          <t>Neville</t>
         </is>
       </c>
       <c r="C114" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Port Alfred</t>
         </is>
       </c>
       <c r="D114" s="3" t="inlineStr">
@@ -11237,22 +11237,22 @@
     <row r="115" ht="25" customHeight="1">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>de Silva</t>
+          <t>Wilter-Sturges</t>
         </is>
       </c>
       <c r="B115" s="3" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Meredith</t>
         </is>
       </c>
       <c r="C115" s="3" t="inlineStr">
         <is>
-          <t>Edenvale</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D115" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E115" s="3" t="inlineStr">
@@ -11264,27 +11264,27 @@
     <row r="116" ht="25" customHeight="1">
       <c r="A116" s="3" t="inlineStr">
         <is>
-          <t>du Plooy</t>
+          <t>de Silva</t>
         </is>
       </c>
       <c r="B116" s="3" t="inlineStr">
         <is>
-          <t>Tammy</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="C116" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Edenvale</t>
         </is>
       </c>
       <c r="D116" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E116" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -11296,7 +11296,7 @@
       </c>
       <c r="B117" s="3" t="inlineStr">
         <is>
-          <t>Marc</t>
+          <t>Tammy</t>
         </is>
       </c>
       <c r="C117" s="3" t="inlineStr">
@@ -11318,17 +11318,17 @@
     <row r="118" ht="25" customHeight="1">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>du Toit</t>
+          <t>du Plooy</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
         <is>
-          <t>Desiree</t>
+          <t>Marc</t>
         </is>
       </c>
       <c r="C118" s="3" t="inlineStr">
         <is>
-          <t>Ramsgate</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D118" s="3" t="inlineStr">
@@ -11345,17 +11345,17 @@
     <row r="119" ht="25" customHeight="1">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>le Roux</t>
+          <t>du Toit</t>
         </is>
       </c>
       <c r="B119" s="3" t="inlineStr">
         <is>
-          <t>Jeanette</t>
+          <t>Desiree</t>
         </is>
       </c>
       <c r="C119" s="3" t="inlineStr">
         <is>
-          <t>Gonubie</t>
+          <t>Ramsgate</t>
         </is>
       </c>
       <c r="D119" s="3" t="inlineStr">
@@ -11372,17 +11372,17 @@
     <row r="120" ht="25" customHeight="1">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>tyler</t>
+          <t>le Roux</t>
         </is>
       </c>
       <c r="B120" s="3" t="inlineStr">
         <is>
-          <t>natascha</t>
+          <t>Jeanette</t>
         </is>
       </c>
       <c r="C120" s="3" t="inlineStr">
         <is>
-          <t>Kensington</t>
+          <t>Gonubie</t>
         </is>
       </c>
       <c r="D120" s="3" t="inlineStr">
@@ -11392,24 +11392,24 @@
       </c>
       <c r="E120" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="121" ht="25" customHeight="1">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>van Heerden</t>
+          <t>tyler</t>
         </is>
       </c>
       <c r="B121" s="3" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>natascha</t>
         </is>
       </c>
       <c r="C121" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Kensington</t>
         </is>
       </c>
       <c r="D121" s="3" t="inlineStr">
@@ -11431,7 +11431,7 @@
       </c>
       <c r="B122" s="3" t="inlineStr">
         <is>
-          <t>Sandy</t>
+          <t>Sydney</t>
         </is>
       </c>
       <c r="C122" s="3" t="inlineStr">
@@ -11446,7 +11446,7 @@
       </c>
       <c r="E122" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -11458,17 +11458,17 @@
       </c>
       <c r="B123" s="3" t="inlineStr">
         <is>
-          <t>Craig</t>
+          <t>Sandy</t>
         </is>
       </c>
       <c r="C123" s="3" t="inlineStr">
         <is>
-          <t>East London Beacon Bay</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D123" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E123" s="3" t="inlineStr">
@@ -11485,17 +11485,17 @@
       </c>
       <c r="B124" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Craig</t>
         </is>
       </c>
       <c r="C124" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>East London Beacon Bay</t>
         </is>
       </c>
       <c r="D124" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E124" s="3" t="inlineStr">
@@ -11507,17 +11507,17 @@
     <row r="125" ht="25" customHeight="1">
       <c r="A125" s="3" t="inlineStr">
         <is>
-          <t>van Wyk</t>
+          <t>van Heerden</t>
         </is>
       </c>
       <c r="B125" s="3" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C125" s="3" t="inlineStr">
         <is>
-          <t>North Durban</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D125" s="3" t="inlineStr">
@@ -11527,7 +11527,7 @@
       </c>
       <c r="E125" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -11539,12 +11539,12 @@
       </c>
       <c r="B126" s="3" t="inlineStr">
         <is>
-          <t>Lindie</t>
+          <t>Kim</t>
         </is>
       </c>
       <c r="C126" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>North Durban</t>
         </is>
       </c>
       <c r="D126" s="3" t="inlineStr">
@@ -11566,12 +11566,12 @@
       </c>
       <c r="B127" s="3" t="inlineStr">
         <is>
-          <t>Willem</t>
+          <t>Lindie</t>
         </is>
       </c>
       <c r="C127" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D127" s="3" t="inlineStr">
@@ -11593,12 +11593,12 @@
       </c>
       <c r="B128" s="3" t="inlineStr">
         <is>
-          <t>Patricia</t>
+          <t>Willem</t>
         </is>
       </c>
       <c r="C128" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D128" s="3" t="inlineStr">
@@ -11615,22 +11615,22 @@
     <row r="129" ht="25" customHeight="1">
       <c r="A129" s="3" t="inlineStr">
         <is>
-          <t>van der Merwe</t>
+          <t>van Wyk</t>
         </is>
       </c>
       <c r="B129" s="3" t="inlineStr">
         <is>
-          <t>Ingrid</t>
+          <t>Patricia</t>
         </is>
       </c>
       <c r="C129" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D129" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E129" s="3" t="inlineStr">
@@ -11642,66 +11642,93 @@
     <row r="130" ht="25" customHeight="1">
       <c r="A130" s="3" t="inlineStr">
         <is>
-          <t>von der Decken</t>
+          <t>van der Merwe</t>
         </is>
       </c>
       <c r="B130" s="3" t="inlineStr">
         <is>
-          <t>Brian</t>
+          <t>Ingrid</t>
         </is>
       </c>
       <c r="C130" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D130" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E130" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="131" ht="25" customHeight="1">
       <c r="A131" s="3" t="inlineStr">
         <is>
+          <t>von der Decken</t>
+        </is>
+      </c>
+      <c r="B131" s="3" t="inlineStr">
+        <is>
+          <t>Brian</t>
+        </is>
+      </c>
+      <c r="C131" s="3" t="inlineStr">
+        <is>
+          <t>King William's Town</t>
+        </is>
+      </c>
+      <c r="D131" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E131" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="132" ht="25" customHeight="1">
+      <c r="A132" s="3" t="inlineStr">
+        <is>
           <t>‘t Hart</t>
         </is>
       </c>
-      <c r="B131" s="3" t="inlineStr">
+      <c r="B132" s="3" t="inlineStr">
         <is>
           <t>Michelle</t>
         </is>
       </c>
-      <c r="C131" s="3" t="inlineStr">
+      <c r="C132" s="3" t="inlineStr">
         <is>
           <t>Benoni Lakes</t>
         </is>
       </c>
-      <c r="D131" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E131" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="132">
-      <c r="A132" s="1" t="inlineStr">
-        <is>
-          <t>Number of attendees: 129</t>
+      <c r="D132" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E132" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="inlineStr">
+        <is>
+          <t>Number of attendees: 130</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="inlineStr">
         <is>
           <t>Number of voters: 52</t>
         </is>
@@ -11737,7 +11764,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Registrees as of 23/04/2021 09:24</t>
+          <t>410W Registrees as of 23/04/2021 11:02</t>
         </is>
       </c>
     </row>
@@ -15859,7 +15886,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Voting details as of 23/04/2021 09:24</t>
+          <t>410E Voting details as of 23/04/2021 11:02</t>
         </is>
       </c>
     </row>
@@ -16236,7 +16263,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Voting details as of 23/04/2021 09:24</t>
+          <t>410W Voting details as of 23/04/2021 11:02</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Registree stats backup on Fri 23 Apr 2021 16:16:00 SAST
</commit_message>
<xml_diff>
--- a/static/docs/registrees_list.xlsx
+++ b/static/docs/registrees_list.xlsx
@@ -451,7 +451,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>MD410 Registrees as of 23/04/2021 11:02</t>
+          <t>MD410 Registrees as of 23/04/2021 16:15</t>
         </is>
       </c>
     </row>
@@ -8179,7 +8179,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Registrees as of 23/04/2021 11:02</t>
+          <t>410E Registrees as of 23/04/2021 16:15</t>
         </is>
       </c>
     </row>
@@ -11746,7 +11746,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E154"/>
+  <dimension ref="A1:E155"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11764,7 +11764,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Registrees as of 23/04/2021 11:02</t>
+          <t>410W Registrees as of 23/04/2021 16:15</t>
         </is>
       </c>
     </row>
@@ -13553,17 +13553,17 @@
     <row r="68" ht="25" customHeight="1">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>Koloko</t>
+          <t>Koenze</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
         <is>
-          <t>Muya</t>
+          <t>Alton</t>
         </is>
       </c>
       <c r="C68" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>Worcester</t>
         </is>
       </c>
       <c r="D68" s="3" t="inlineStr">
@@ -13580,44 +13580,44 @@
     <row r="69" ht="25" customHeight="1">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>Kruger</t>
+          <t>Koloko</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
         <is>
-          <t>Zwaai</t>
+          <t>Muya</t>
         </is>
       </c>
       <c r="C69" s="3" t="inlineStr">
         <is>
-          <t>Sedgefield</t>
+          <t>Durbanville</t>
         </is>
       </c>
       <c r="D69" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E69" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="70" ht="25" customHeight="1">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>Lakay</t>
+          <t>Kruger</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
         <is>
-          <t>Bevil</t>
+          <t>Zwaai</t>
         </is>
       </c>
       <c r="C70" s="3" t="inlineStr">
         <is>
-          <t>Mitchells Plain</t>
+          <t>Sedgefield</t>
         </is>
       </c>
       <c r="D70" s="3" t="inlineStr">
@@ -13634,17 +13634,17 @@
     <row r="71" ht="25" customHeight="1">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>Lang</t>
+          <t>Lakay</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
         <is>
-          <t>Paula</t>
+          <t>Bevil</t>
         </is>
       </c>
       <c r="C71" s="3" t="inlineStr">
         <is>
-          <t>Gordons Bay</t>
+          <t>Mitchells Plain</t>
         </is>
       </c>
       <c r="D71" s="3" t="inlineStr">
@@ -13666,7 +13666,7 @@
       </c>
       <c r="B72" s="3" t="inlineStr">
         <is>
-          <t>Jimmy</t>
+          <t>Paula</t>
         </is>
       </c>
       <c r="C72" s="3" t="inlineStr">
@@ -13681,29 +13681,29 @@
       </c>
       <c r="E72" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="73" ht="25" customHeight="1">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>Langmaak</t>
+          <t>Lang</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
         <is>
-          <t>Elke</t>
+          <t>Jimmy</t>
         </is>
       </c>
       <c r="C73" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Gordons Bay</t>
         </is>
       </c>
       <c r="D73" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E73" s="3" t="inlineStr">
@@ -13720,7 +13720,7 @@
       </c>
       <c r="B74" s="3" t="inlineStr">
         <is>
-          <t>Kai</t>
+          <t>Elke</t>
         </is>
       </c>
       <c r="C74" s="3" t="inlineStr">
@@ -13742,22 +13742,22 @@
     <row r="75" ht="25" customHeight="1">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>Laubscher</t>
+          <t>Langmaak</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
         <is>
-          <t>Herman</t>
+          <t>Kai</t>
         </is>
       </c>
       <c r="C75" s="3" t="inlineStr">
         <is>
-          <t>Ceres</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D75" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E75" s="3" t="inlineStr">
@@ -13769,17 +13769,17 @@
     <row r="76" ht="25" customHeight="1">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>Lee</t>
+          <t>Laubscher</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
         <is>
-          <t>Heather</t>
+          <t>Herman</t>
         </is>
       </c>
       <c r="C76" s="3" t="inlineStr">
         <is>
-          <t>Cape Of Good Hope</t>
+          <t>Ceres</t>
         </is>
       </c>
       <c r="D76" s="3" t="inlineStr">
@@ -13789,24 +13789,24 @@
       </c>
       <c r="E76" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="77" ht="25" customHeight="1">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>Lucas</t>
+          <t>Lee</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
         <is>
-          <t>Rashmiya</t>
+          <t>Heather</t>
         </is>
       </c>
       <c r="C77" s="3" t="inlineStr">
         <is>
-          <t>Mitchells Plain</t>
+          <t>Cape Of Good Hope</t>
         </is>
       </c>
       <c r="D77" s="3" t="inlineStr">
@@ -13816,24 +13816,24 @@
       </c>
       <c r="E77" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="78" ht="25" customHeight="1">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>MAYTHAM</t>
+          <t>Lucas</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
         <is>
-          <t>LANCE</t>
+          <t>Rashmiya</t>
         </is>
       </c>
       <c r="C78" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Mitchells Plain</t>
         </is>
       </c>
       <c r="D78" s="3" t="inlineStr">
@@ -13855,7 +13855,7 @@
       </c>
       <c r="B79" s="3" t="inlineStr">
         <is>
-          <t>ROSEMARIE</t>
+          <t>LANCE</t>
         </is>
       </c>
       <c r="C79" s="3" t="inlineStr">
@@ -13877,17 +13877,17 @@
     <row r="80" ht="25" customHeight="1">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>MacRobert</t>
+          <t>MAYTHAM</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
         <is>
-          <t>Pam</t>
+          <t>ROSEMARIE</t>
         </is>
       </c>
       <c r="C80" s="3" t="inlineStr">
         <is>
-          <t>Groote Schuur</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D80" s="3" t="inlineStr">
@@ -13904,49 +13904,49 @@
     <row r="81" ht="25" customHeight="1">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>Mangwende</t>
+          <t>MacRobert</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
         <is>
-          <t>Sharon</t>
+          <t>Pam</t>
         </is>
       </c>
       <c r="C81" s="3" t="inlineStr">
         <is>
-          <t>Cape Town</t>
+          <t>Groote Schuur</t>
         </is>
       </c>
       <c r="D81" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E81" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="82" ht="25" customHeight="1">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>McPherson</t>
+          <t>Mangwende</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
         <is>
-          <t>Stuart</t>
+          <t>Sharon</t>
         </is>
       </c>
       <c r="C82" s="3" t="inlineStr">
         <is>
-          <t>Newlands</t>
+          <t>Cape Town</t>
         </is>
       </c>
       <c r="D82" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E82" s="3" t="inlineStr">
@@ -13958,17 +13958,17 @@
     <row r="83" ht="25" customHeight="1">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>Metz</t>
+          <t>McPherson</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
         <is>
-          <t>Elisa</t>
+          <t>Stuart</t>
         </is>
       </c>
       <c r="C83" s="3" t="inlineStr">
         <is>
-          <t>Milnerton</t>
+          <t>Newlands</t>
         </is>
       </c>
       <c r="D83" s="3" t="inlineStr">
@@ -13978,24 +13978,24 @@
       </c>
       <c r="E83" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="84" ht="25" customHeight="1">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>Mkhize</t>
+          <t>Metz</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
         <is>
-          <t>Virginia</t>
+          <t>Elisa</t>
         </is>
       </c>
       <c r="C84" s="3" t="inlineStr">
         <is>
-          <t>Cape Town</t>
+          <t>Milnerton</t>
         </is>
       </c>
       <c r="D84" s="3" t="inlineStr">
@@ -14012,22 +14012,22 @@
     <row r="85" ht="25" customHeight="1">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>Moeller</t>
+          <t>Mkhize</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
         <is>
-          <t>Frauke E.</t>
+          <t>Virginia</t>
         </is>
       </c>
       <c r="C85" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Cape Town</t>
         </is>
       </c>
       <c r="D85" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E85" s="3" t="inlineStr">
@@ -14039,22 +14039,22 @@
     <row r="86" ht="25" customHeight="1">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>Moses</t>
+          <t>Moeller</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
         <is>
-          <t>Bernadine</t>
+          <t>Frauke E.</t>
         </is>
       </c>
       <c r="C86" s="3" t="inlineStr">
         <is>
-          <t>Cape Town</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D86" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E86" s="3" t="inlineStr">
@@ -14071,12 +14071,12 @@
       </c>
       <c r="B87" s="3" t="inlineStr">
         <is>
-          <t>Brian</t>
+          <t>Bernadine</t>
         </is>
       </c>
       <c r="C87" s="3" t="inlineStr">
         <is>
-          <t>Cape Of Good Hope</t>
+          <t>Cape Town</t>
         </is>
       </c>
       <c r="D87" s="3" t="inlineStr">
@@ -14086,29 +14086,29 @@
       </c>
       <c r="E87" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="88" ht="25" customHeight="1">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>Mostert</t>
+          <t>Moses</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
         <is>
-          <t>Jacques</t>
+          <t>Brian</t>
         </is>
       </c>
       <c r="C88" s="3" t="inlineStr">
         <is>
-          <t>Merriman</t>
+          <t>Cape Of Good Hope</t>
         </is>
       </c>
       <c r="D88" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E88" s="3" t="inlineStr">
@@ -14120,22 +14120,22 @@
     <row r="89" ht="25" customHeight="1">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>Mutschler</t>
+          <t>Mostert</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
         <is>
-          <t>Peter</t>
+          <t>Jacques</t>
         </is>
       </c>
       <c r="C89" s="3" t="inlineStr">
         <is>
-          <t>Grootfontein</t>
+          <t>Merriman</t>
         </is>
       </c>
       <c r="D89" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E89" s="3" t="inlineStr">
@@ -14147,17 +14147,17 @@
     <row r="90" ht="25" customHeight="1">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>Myburg</t>
+          <t>Mutschler</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
         <is>
-          <t>Pieter</t>
+          <t>Peter</t>
         </is>
       </c>
       <c r="C90" s="3" t="inlineStr">
         <is>
-          <t>Wellington</t>
+          <t>Grootfontein</t>
         </is>
       </c>
       <c r="D90" s="3" t="inlineStr">
@@ -14167,14 +14167,14 @@
       </c>
       <c r="E90" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="91" ht="25" customHeight="1">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>Nel</t>
+          <t>Myburg</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -14184,7 +14184,7 @@
       </c>
       <c r="C91" s="3" t="inlineStr">
         <is>
-          <t>George</t>
+          <t>Wellington</t>
         </is>
       </c>
       <c r="D91" s="3" t="inlineStr">
@@ -14194,7 +14194,7 @@
       </c>
       <c r="E91" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -14206,12 +14206,12 @@
       </c>
       <c r="B92" s="3" t="inlineStr">
         <is>
-          <t>Tillie</t>
+          <t>Pieter</t>
         </is>
       </c>
       <c r="C92" s="3" t="inlineStr">
         <is>
-          <t>Eden</t>
+          <t>George</t>
         </is>
       </c>
       <c r="D92" s="3" t="inlineStr">
@@ -14228,17 +14228,17 @@
     <row r="93" ht="25" customHeight="1">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>Niehaus</t>
+          <t>Nel</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
         <is>
-          <t>Angela</t>
+          <t>Tillie</t>
         </is>
       </c>
       <c r="C93" s="3" t="inlineStr">
         <is>
-          <t>Bergvliet</t>
+          <t>Eden</t>
         </is>
       </c>
       <c r="D93" s="3" t="inlineStr">
@@ -14255,17 +14255,17 @@
     <row r="94" ht="25" customHeight="1">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>Nortjie</t>
+          <t>Niehaus</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
         <is>
-          <t>Rachel</t>
+          <t>Angela</t>
         </is>
       </c>
       <c r="C94" s="3" t="inlineStr">
         <is>
-          <t>Mitchells Plain</t>
+          <t>Bergvliet</t>
         </is>
       </c>
       <c r="D94" s="3" t="inlineStr">
@@ -14275,24 +14275,24 @@
       </c>
       <c r="E94" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="95" ht="25" customHeight="1">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>Ocker</t>
+          <t>Nortjie</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
         <is>
-          <t>Chris</t>
+          <t>Rachel</t>
         </is>
       </c>
       <c r="C95" s="3" t="inlineStr">
         <is>
-          <t>Fish Hoek</t>
+          <t>Mitchells Plain</t>
         </is>
       </c>
       <c r="D95" s="3" t="inlineStr">
@@ -14314,7 +14314,7 @@
       </c>
       <c r="B96" s="3" t="inlineStr">
         <is>
-          <t>Jenny</t>
+          <t>Chris</t>
         </is>
       </c>
       <c r="C96" s="3" t="inlineStr">
@@ -14336,17 +14336,17 @@
     <row r="97" ht="25" customHeight="1">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>Olivier</t>
+          <t>Ocker</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
         <is>
-          <t>Debra</t>
+          <t>Jenny</t>
         </is>
       </c>
       <c r="C97" s="3" t="inlineStr">
         <is>
-          <t>Sedgefield</t>
+          <t>Fish Hoek</t>
         </is>
       </c>
       <c r="D97" s="3" t="inlineStr">
@@ -14363,22 +14363,22 @@
     <row r="98" ht="25" customHeight="1">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>Ormandy</t>
+          <t>Olivier</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
         <is>
-          <t>Isabella Stratton</t>
+          <t>Debra</t>
         </is>
       </c>
       <c r="C98" s="3" t="inlineStr">
         <is>
-          <t>Milnerton</t>
+          <t>Sedgefield</t>
         </is>
       </c>
       <c r="D98" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E98" s="3" t="inlineStr">
@@ -14390,44 +14390,44 @@
     <row r="99" ht="25" customHeight="1">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>Peters</t>
+          <t>Ormandy</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
         <is>
-          <t>Maureen</t>
+          <t>Isabella Stratton</t>
         </is>
       </c>
       <c r="C99" s="3" t="inlineStr">
         <is>
-          <t>Ceres</t>
+          <t>Milnerton</t>
         </is>
       </c>
       <c r="D99" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E99" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="100" ht="25" customHeight="1">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>Pillay</t>
+          <t>Peters</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>Maureen</t>
         </is>
       </c>
       <c r="C100" s="3" t="inlineStr">
         <is>
-          <t>Tygerberg Hills</t>
+          <t>Ceres</t>
         </is>
       </c>
       <c r="D100" s="3" t="inlineStr">
@@ -14444,22 +14444,22 @@
     <row r="101" ht="25" customHeight="1">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>Poyowe</t>
+          <t>Pillay</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
         <is>
-          <t>Yvonne  Maureen</t>
+          <t>Patrick</t>
         </is>
       </c>
       <c r="C101" s="3" t="inlineStr">
         <is>
-          <t>Cape Of Good Hope</t>
+          <t>Tygerberg Hills</t>
         </is>
       </c>
       <c r="D101" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E101" s="3" t="inlineStr">
@@ -14471,17 +14471,17 @@
     <row r="102" ht="25" customHeight="1">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>Pretorius</t>
+          <t>Poyowe</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
         <is>
-          <t>Sheldon Edmund</t>
+          <t>Yvonne  Maureen</t>
         </is>
       </c>
       <c r="C102" s="3" t="inlineStr">
         <is>
-          <t>Merriman</t>
+          <t>Cape Of Good Hope</t>
         </is>
       </c>
       <c r="D102" s="3" t="inlineStr">
@@ -14491,29 +14491,29 @@
       </c>
       <c r="E102" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="103" ht="25" customHeight="1">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>Ras</t>
+          <t>Pretorius</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
         <is>
-          <t>Mary-Anne</t>
+          <t>Sheldon Edmund</t>
         </is>
       </c>
       <c r="C103" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Merriman</t>
         </is>
       </c>
       <c r="D103" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E103" s="3" t="inlineStr">
@@ -14530,7 +14530,7 @@
       </c>
       <c r="B104" s="3" t="inlineStr">
         <is>
-          <t>Leon Jacobus</t>
+          <t>Mary-Anne</t>
         </is>
       </c>
       <c r="C104" s="3" t="inlineStr">
@@ -14552,17 +14552,17 @@
     <row r="105" ht="25" customHeight="1">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>Rossouw</t>
+          <t>Ras</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Leon Jacobus</t>
         </is>
       </c>
       <c r="C105" s="3" t="inlineStr">
         <is>
-          <t>Tokai</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D105" s="3" t="inlineStr">
@@ -14572,24 +14572,24 @@
       </c>
       <c r="E105" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="106" ht="25" customHeight="1">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>Rothner</t>
+          <t>Rossouw</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
         <is>
-          <t>Andrea</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C106" s="3" t="inlineStr">
         <is>
-          <t>Eden</t>
+          <t>Tokai</t>
         </is>
       </c>
       <c r="D106" s="3" t="inlineStr">
@@ -14599,24 +14599,24 @@
       </c>
       <c r="E106" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="107" ht="25" customHeight="1">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>Roux</t>
+          <t>Rothner</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
         <is>
-          <t>Anthonie Petrus</t>
+          <t>Andrea</t>
         </is>
       </c>
       <c r="C107" s="3" t="inlineStr">
         <is>
-          <t>Moorreesburg</t>
+          <t>Eden</t>
         </is>
       </c>
       <c r="D107" s="3" t="inlineStr">
@@ -14626,24 +14626,24 @@
       </c>
       <c r="E107" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="108" ht="25" customHeight="1">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>Russell</t>
+          <t>Roux</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
         <is>
-          <t>Ingrid</t>
+          <t>Anthonie Petrus</t>
         </is>
       </c>
       <c r="C108" s="3" t="inlineStr">
         <is>
-          <t>Fish Hoek</t>
+          <t>Moorreesburg</t>
         </is>
       </c>
       <c r="D108" s="3" t="inlineStr">
@@ -14660,71 +14660,71 @@
     <row r="109" ht="25" customHeight="1">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>SNYMAN</t>
+          <t>Russell</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
         <is>
-          <t>LYN</t>
+          <t>Ingrid</t>
         </is>
       </c>
       <c r="C109" s="3" t="inlineStr">
         <is>
-          <t>Deep South</t>
+          <t>Fish Hoek</t>
         </is>
       </c>
       <c r="D109" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E109" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="110" ht="25" customHeight="1">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>STEENBERG</t>
+          <t>SNYMAN</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
         <is>
-          <t>TIM</t>
+          <t>LYN</t>
         </is>
       </c>
       <c r="C110" s="3" t="inlineStr">
         <is>
-          <t>Wellington</t>
+          <t>Deep South</t>
         </is>
       </c>
       <c r="D110" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E110" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="111" ht="25" customHeight="1">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>Sampie</t>
+          <t>STEENBERG</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
         <is>
-          <t>Sharon</t>
+          <t>TIM</t>
         </is>
       </c>
       <c r="C111" s="3" t="inlineStr">
         <is>
-          <t>Bergvliet</t>
+          <t>Wellington</t>
         </is>
       </c>
       <c r="D111" s="3" t="inlineStr">
@@ -14741,17 +14741,17 @@
     <row r="112" ht="25" customHeight="1">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>Schatz</t>
+          <t>Sampie</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
         <is>
-          <t>Vera</t>
+          <t>Sharon</t>
         </is>
       </c>
       <c r="C112" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Bergvliet</t>
         </is>
       </c>
       <c r="D112" s="3" t="inlineStr">
@@ -14773,7 +14773,7 @@
       </c>
       <c r="B113" s="3" t="inlineStr">
         <is>
-          <t>Frank</t>
+          <t>Vera</t>
         </is>
       </c>
       <c r="C113" s="3" t="inlineStr">
@@ -14788,19 +14788,19 @@
       </c>
       <c r="E113" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="114" ht="25" customHeight="1">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>Sell</t>
+          <t>Schatz</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
         <is>
-          <t>Ami</t>
+          <t>Frank</t>
         </is>
       </c>
       <c r="C114" s="3" t="inlineStr">
@@ -14822,17 +14822,17 @@
     <row r="115" ht="25" customHeight="1">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>Simpson</t>
+          <t>Sell</t>
         </is>
       </c>
       <c r="B115" s="3" t="inlineStr">
         <is>
-          <t>Beryl</t>
+          <t>Ami</t>
         </is>
       </c>
       <c r="C115" s="3" t="inlineStr">
         <is>
-          <t>Cape Town</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D115" s="3" t="inlineStr">
@@ -14849,17 +14849,17 @@
     <row r="116" ht="25" customHeight="1">
       <c r="A116" s="3" t="inlineStr">
         <is>
-          <t>Sircoulomb</t>
+          <t>Simpson</t>
         </is>
       </c>
       <c r="B116" s="3" t="inlineStr">
         <is>
-          <t>Kenlis</t>
+          <t>Beryl</t>
         </is>
       </c>
       <c r="C116" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Cape Town</t>
         </is>
       </c>
       <c r="D116" s="3" t="inlineStr">
@@ -14881,7 +14881,7 @@
       </c>
       <c r="B117" s="3" t="inlineStr">
         <is>
-          <t>Holger</t>
+          <t>Kenlis</t>
         </is>
       </c>
       <c r="C117" s="3" t="inlineStr">
@@ -14896,24 +14896,24 @@
       </c>
       <c r="E117" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="118" ht="25" customHeight="1">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>Smit</t>
+          <t>Sircoulomb</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
         <is>
-          <t>Herman</t>
+          <t>Holger</t>
         </is>
       </c>
       <c r="C118" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D118" s="3" t="inlineStr">
@@ -14923,24 +14923,24 @@
       </c>
       <c r="E118" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="119" ht="25" customHeight="1">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Smit</t>
         </is>
       </c>
       <c r="B119" s="3" t="inlineStr">
         <is>
-          <t>Bennie</t>
+          <t>Herman</t>
         </is>
       </c>
       <c r="C119" s="3" t="inlineStr">
         <is>
-          <t>Wellington</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D119" s="3" t="inlineStr">
@@ -14950,7 +14950,7 @@
       </c>
       <c r="E119" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -14962,12 +14962,12 @@
       </c>
       <c r="B120" s="3" t="inlineStr">
         <is>
-          <t>Carmen Dolores</t>
+          <t>Bennie</t>
         </is>
       </c>
       <c r="C120" s="3" t="inlineStr">
         <is>
-          <t>Tokai</t>
+          <t>Wellington</t>
         </is>
       </c>
       <c r="D120" s="3" t="inlineStr">
@@ -14977,7 +14977,7 @@
       </c>
       <c r="E120" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -14989,7 +14989,7 @@
       </c>
       <c r="B121" s="3" t="inlineStr">
         <is>
-          <t>David John</t>
+          <t>Carmen Dolores</t>
         </is>
       </c>
       <c r="C121" s="3" t="inlineStr">
@@ -15011,17 +15011,17 @@
     <row r="122" ht="25" customHeight="1">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>Sochen</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
         <is>
-          <t>Diana</t>
+          <t>David John</t>
         </is>
       </c>
       <c r="C122" s="3" t="inlineStr">
         <is>
-          <t>Sea Point</t>
+          <t>Tokai</t>
         </is>
       </c>
       <c r="D122" s="3" t="inlineStr">
@@ -15031,56 +15031,56 @@
       </c>
       <c r="E122" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="123" ht="25" customHeight="1">
       <c r="A123" s="3" t="inlineStr">
         <is>
-          <t>Strauss</t>
+          <t>Sochen</t>
         </is>
       </c>
       <c r="B123" s="3" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>Diana</t>
         </is>
       </c>
       <c r="C123" s="3" t="inlineStr">
         <is>
-          <t>Kuilsriver</t>
+          <t>Sea Point</t>
         </is>
       </c>
       <c r="D123" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E123" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="124" ht="25" customHeight="1">
       <c r="A124" s="3" t="inlineStr">
         <is>
-          <t>Tshikala</t>
+          <t>Strauss</t>
         </is>
       </c>
       <c r="B124" s="3" t="inlineStr">
         <is>
-          <t>David Alex</t>
+          <t>Patrick</t>
         </is>
       </c>
       <c r="C124" s="3" t="inlineStr">
         <is>
-          <t>Athlone</t>
+          <t>Kuilsriver</t>
         </is>
       </c>
       <c r="D124" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E124" s="3" t="inlineStr">
@@ -15092,17 +15092,17 @@
     <row r="125" ht="25" customHeight="1">
       <c r="A125" s="3" t="inlineStr">
         <is>
-          <t>VAN BREDA</t>
+          <t>Tshikala</t>
         </is>
       </c>
       <c r="B125" s="3" t="inlineStr">
         <is>
-          <t>HILARY LISE</t>
+          <t>David Alex</t>
         </is>
       </c>
       <c r="C125" s="3" t="inlineStr">
         <is>
-          <t>Cape Town</t>
+          <t>Athlone</t>
         </is>
       </c>
       <c r="D125" s="3" t="inlineStr">
@@ -15119,17 +15119,17 @@
     <row r="126" ht="25" customHeight="1">
       <c r="A126" s="3" t="inlineStr">
         <is>
-          <t>VAN DER MERWE</t>
+          <t>VAN BREDA</t>
         </is>
       </c>
       <c r="B126" s="3" t="inlineStr">
         <is>
-          <t>MARINA</t>
+          <t>HILARY LISE</t>
         </is>
       </c>
       <c r="C126" s="3" t="inlineStr">
         <is>
-          <t>Malmesbury</t>
+          <t>Cape Town</t>
         </is>
       </c>
       <c r="D126" s="3" t="inlineStr">
@@ -15139,24 +15139,24 @@
       </c>
       <c r="E126" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="127" ht="25" customHeight="1">
       <c r="A127" s="3" t="inlineStr">
         <is>
-          <t>Van Nieuwenhuyzen</t>
+          <t>VAN DER MERWE</t>
         </is>
       </c>
       <c r="B127" s="3" t="inlineStr">
         <is>
-          <t>Hilgardt</t>
+          <t>MARINA</t>
         </is>
       </c>
       <c r="C127" s="3" t="inlineStr">
         <is>
-          <t>Worcester</t>
+          <t>Malmesbury</t>
         </is>
       </c>
       <c r="D127" s="3" t="inlineStr">
@@ -15166,24 +15166,24 @@
       </c>
       <c r="E127" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="128" ht="25" customHeight="1">
       <c r="A128" s="3" t="inlineStr">
         <is>
-          <t>Van Rensburg</t>
+          <t>Van Nieuwenhuyzen</t>
         </is>
       </c>
       <c r="B128" s="3" t="inlineStr">
         <is>
-          <t>Neville</t>
+          <t>Hilgardt</t>
         </is>
       </c>
       <c r="C128" s="3" t="inlineStr">
         <is>
-          <t>Moorreesburg</t>
+          <t>Worcester</t>
         </is>
       </c>
       <c r="D128" s="3" t="inlineStr">
@@ -15193,51 +15193,51 @@
       </c>
       <c r="E128" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="129" ht="25" customHeight="1">
       <c r="A129" s="3" t="inlineStr">
         <is>
-          <t>Van Romburgh</t>
+          <t>Van Rensburg</t>
         </is>
       </c>
       <c r="B129" s="3" t="inlineStr">
         <is>
-          <t>Lorna</t>
+          <t>Neville</t>
         </is>
       </c>
       <c r="C129" s="3" t="inlineStr">
         <is>
-          <t>Fish Hoek</t>
+          <t>Moorreesburg</t>
         </is>
       </c>
       <c r="D129" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E129" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="130" ht="25" customHeight="1">
       <c r="A130" s="3" t="inlineStr">
         <is>
-          <t>Van Wyk-Nelson</t>
+          <t>Van Romburgh</t>
         </is>
       </c>
       <c r="B130" s="3" t="inlineStr">
         <is>
-          <t>Edith</t>
+          <t>Lorna</t>
         </is>
       </c>
       <c r="C130" s="3" t="inlineStr">
         <is>
-          <t>Kuilsriver</t>
+          <t>Fish Hoek</t>
         </is>
       </c>
       <c r="D130" s="3" t="inlineStr">
@@ -15254,22 +15254,22 @@
     <row r="131" ht="25" customHeight="1">
       <c r="A131" s="3" t="inlineStr">
         <is>
-          <t>Van de Merwe</t>
+          <t>Van Wyk-Nelson</t>
         </is>
       </c>
       <c r="B131" s="3" t="inlineStr">
         <is>
-          <t>Marina</t>
+          <t>Edith</t>
         </is>
       </c>
       <c r="C131" s="3" t="inlineStr">
         <is>
-          <t>Malmesbury</t>
+          <t>Kuilsriver</t>
         </is>
       </c>
       <c r="D131" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E131" s="3" t="inlineStr">
@@ -15281,22 +15281,22 @@
     <row r="132" ht="25" customHeight="1">
       <c r="A132" s="3" t="inlineStr">
         <is>
-          <t>Von Mollendorf</t>
+          <t>Van de Merwe</t>
         </is>
       </c>
       <c r="B132" s="3" t="inlineStr">
         <is>
-          <t>Rinette</t>
+          <t>Marina</t>
         </is>
       </c>
       <c r="C132" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>Malmesbury</t>
         </is>
       </c>
       <c r="D132" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E132" s="3" t="inlineStr">
@@ -15308,22 +15308,22 @@
     <row r="133" ht="25" customHeight="1">
       <c r="A133" s="3" t="inlineStr">
         <is>
-          <t>Vorster</t>
+          <t>Von Mollendorf</t>
         </is>
       </c>
       <c r="B133" s="3" t="inlineStr">
         <is>
-          <t>Rochelle</t>
+          <t>Rinette</t>
         </is>
       </c>
       <c r="C133" s="3" t="inlineStr">
         <is>
-          <t>Sedgefield</t>
+          <t>Durbanville</t>
         </is>
       </c>
       <c r="D133" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E133" s="3" t="inlineStr">
@@ -15335,22 +15335,22 @@
     <row r="134" ht="25" customHeight="1">
       <c r="A134" s="3" t="inlineStr">
         <is>
-          <t>Watson</t>
+          <t>Vorster</t>
         </is>
       </c>
       <c r="B134" s="3" t="inlineStr">
         <is>
-          <t>Allan</t>
+          <t>Rochelle</t>
         </is>
       </c>
       <c r="C134" s="3" t="inlineStr">
         <is>
-          <t>Sea Point</t>
+          <t>Sedgefield</t>
         </is>
       </c>
       <c r="D134" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E134" s="3" t="inlineStr">
@@ -15367,71 +15367,71 @@
       </c>
       <c r="B135" s="3" t="inlineStr">
         <is>
-          <t>Alison</t>
+          <t>Allan</t>
         </is>
       </c>
       <c r="C135" s="3" t="inlineStr">
         <is>
-          <t>Sedgefield</t>
+          <t>Sea Point</t>
         </is>
       </c>
       <c r="D135" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E135" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="136" ht="25" customHeight="1">
       <c r="A136" s="3" t="inlineStr">
         <is>
-          <t>Williams</t>
+          <t>Watson</t>
         </is>
       </c>
       <c r="B136" s="3" t="inlineStr">
         <is>
-          <t>Johanna</t>
+          <t>Alison</t>
         </is>
       </c>
       <c r="C136" s="3" t="inlineStr">
         <is>
-          <t>Mitchells Plain</t>
+          <t>Sedgefield</t>
         </is>
       </c>
       <c r="D136" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E136" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="137" ht="25" customHeight="1">
       <c r="A137" s="3" t="inlineStr">
         <is>
-          <t>Wills</t>
+          <t>Williams</t>
         </is>
       </c>
       <c r="B137" s="3" t="inlineStr">
         <is>
-          <t>Geila</t>
+          <t>Johanna</t>
         </is>
       </c>
       <c r="C137" s="3" t="inlineStr">
         <is>
-          <t>Athlone</t>
+          <t>Mitchells Plain</t>
         </is>
       </c>
       <c r="D137" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E137" s="3" t="inlineStr">
@@ -15443,22 +15443,22 @@
     <row r="138" ht="25" customHeight="1">
       <c r="A138" s="3" t="inlineStr">
         <is>
-          <t>Woodman</t>
+          <t>Wills</t>
         </is>
       </c>
       <c r="B138" s="3" t="inlineStr">
         <is>
-          <t>Joan</t>
+          <t>Geila</t>
         </is>
       </c>
       <c r="C138" s="3" t="inlineStr">
         <is>
-          <t>Mitchells Plain</t>
+          <t>Athlone</t>
         </is>
       </c>
       <c r="D138" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E138" s="3" t="inlineStr">
@@ -15470,44 +15470,44 @@
     <row r="139" ht="25" customHeight="1">
       <c r="A139" s="3" t="inlineStr">
         <is>
-          <t>Wright</t>
+          <t>Woodman</t>
         </is>
       </c>
       <c r="B139" s="3" t="inlineStr">
         <is>
-          <t>Rocky</t>
+          <t>Joan</t>
         </is>
       </c>
       <c r="C139" s="3" t="inlineStr">
         <is>
-          <t>Table View</t>
+          <t>Mitchells Plain</t>
         </is>
       </c>
       <c r="D139" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E139" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="140" ht="25" customHeight="1">
       <c r="A140" s="3" t="inlineStr">
         <is>
-          <t>Young</t>
+          <t>Wright</t>
         </is>
       </c>
       <c r="B140" s="3" t="inlineStr">
         <is>
-          <t>Judy</t>
+          <t>Rocky</t>
         </is>
       </c>
       <c r="C140" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>Table View</t>
         </is>
       </c>
       <c r="D140" s="3" t="inlineStr">
@@ -15517,7 +15517,7 @@
       </c>
       <c r="E140" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -15529,17 +15529,17 @@
       </c>
       <c r="B141" s="3" t="inlineStr">
         <is>
-          <t>Gerry</t>
+          <t>Judy</t>
         </is>
       </c>
       <c r="C141" s="3" t="inlineStr">
         <is>
-          <t>Mitchells Plain</t>
+          <t>Durbanville</t>
         </is>
       </c>
       <c r="D141" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E141" s="3" t="inlineStr">
@@ -15551,22 +15551,22 @@
     <row r="142" ht="25" customHeight="1">
       <c r="A142" s="3" t="inlineStr">
         <is>
-          <t>Zucker</t>
+          <t>Young</t>
         </is>
       </c>
       <c r="B142" s="3" t="inlineStr">
         <is>
-          <t>Leonie</t>
+          <t>Gerry</t>
         </is>
       </c>
       <c r="C142" s="3" t="inlineStr">
         <is>
-          <t>Milnerton</t>
+          <t>Mitchells Plain</t>
         </is>
       </c>
       <c r="D142" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E142" s="3" t="inlineStr">
@@ -15578,17 +15578,17 @@
     <row r="143" ht="25" customHeight="1">
       <c r="A143" s="3" t="inlineStr">
         <is>
-          <t>de Kock</t>
+          <t>Zucker</t>
         </is>
       </c>
       <c r="B143" s="3" t="inlineStr">
         <is>
-          <t>Engela</t>
+          <t>Leonie</t>
         </is>
       </c>
       <c r="C143" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Milnerton</t>
         </is>
       </c>
       <c r="D143" s="3" t="inlineStr">
@@ -15598,7 +15598,7 @@
       </c>
       <c r="E143" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -15610,7 +15610,7 @@
       </c>
       <c r="B144" s="3" t="inlineStr">
         <is>
-          <t>Francois</t>
+          <t>Engela</t>
         </is>
       </c>
       <c r="C144" s="3" t="inlineStr">
@@ -15632,22 +15632,22 @@
     <row r="145" ht="25" customHeight="1">
       <c r="A145" s="3" t="inlineStr">
         <is>
-          <t>stier</t>
+          <t>de Kock</t>
         </is>
       </c>
       <c r="B145" s="3" t="inlineStr">
         <is>
-          <t>RORY</t>
+          <t>Francois</t>
         </is>
       </c>
       <c r="C145" s="3" t="inlineStr">
         <is>
-          <t>Deep South</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D145" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E145" s="3" t="inlineStr">
@@ -15659,44 +15659,44 @@
     <row r="146" ht="25" customHeight="1">
       <c r="A146" s="3" t="inlineStr">
         <is>
-          <t>van Blerk</t>
+          <t>stier</t>
         </is>
       </c>
       <c r="B146" s="3" t="inlineStr">
         <is>
-          <t>Carl</t>
+          <t>RORY</t>
         </is>
       </c>
       <c r="C146" s="3" t="inlineStr">
         <is>
-          <t>Eden</t>
+          <t>Deep South</t>
         </is>
       </c>
       <c r="D146" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E146" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="147" ht="25" customHeight="1">
       <c r="A147" s="3" t="inlineStr">
         <is>
-          <t>van Rensburg</t>
+          <t>van Blerk</t>
         </is>
       </c>
       <c r="B147" s="3" t="inlineStr">
         <is>
-          <t>Johan</t>
+          <t>Carl</t>
         </is>
       </c>
       <c r="C147" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Eden</t>
         </is>
       </c>
       <c r="D147" s="3" t="inlineStr">
@@ -15718,7 +15718,7 @@
       </c>
       <c r="B148" s="3" t="inlineStr">
         <is>
-          <t>Anne</t>
+          <t>Johan</t>
         </is>
       </c>
       <c r="C148" s="3" t="inlineStr">
@@ -15740,17 +15740,17 @@
     <row r="149" ht="25" customHeight="1">
       <c r="A149" s="3" t="inlineStr">
         <is>
-          <t>van Wulven</t>
+          <t>van Rensburg</t>
         </is>
       </c>
       <c r="B149" s="3" t="inlineStr">
         <is>
-          <t>Jeannie</t>
+          <t>Anne</t>
         </is>
       </c>
       <c r="C149" s="3" t="inlineStr">
         <is>
-          <t>Tygerberg Hills</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D149" s="3" t="inlineStr">
@@ -15772,7 +15772,7 @@
       </c>
       <c r="B150" s="3" t="inlineStr">
         <is>
-          <t>Alan</t>
+          <t>Jeannie</t>
         </is>
       </c>
       <c r="C150" s="3" t="inlineStr">
@@ -15799,7 +15799,7 @@
       </c>
       <c r="B151" s="3" t="inlineStr">
         <is>
-          <t>Deon</t>
+          <t>Alan</t>
         </is>
       </c>
       <c r="C151" s="3" t="inlineStr">
@@ -15821,39 +15821,66 @@
     <row r="152" ht="25" customHeight="1">
       <c r="A152" s="3" t="inlineStr">
         <is>
+          <t>van Wulven</t>
+        </is>
+      </c>
+      <c r="B152" s="3" t="inlineStr">
+        <is>
+          <t>Deon</t>
+        </is>
+      </c>
+      <c r="C152" s="3" t="inlineStr">
+        <is>
+          <t>Tygerberg Hills</t>
+        </is>
+      </c>
+      <c r="D152" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E152" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="153" ht="25" customHeight="1">
+      <c r="A153" s="3" t="inlineStr">
+        <is>
           <t>van der Westhuizen</t>
         </is>
       </c>
-      <c r="B152" s="3" t="inlineStr">
+      <c r="B153" s="3" t="inlineStr">
         <is>
           <t>Hennie</t>
         </is>
       </c>
-      <c r="C152" s="3" t="inlineStr">
+      <c r="C153" s="3" t="inlineStr">
         <is>
           <t>Helderberg</t>
         </is>
       </c>
-      <c r="D152" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E152" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-    </row>
-    <row r="153">
-      <c r="A153" s="1" t="inlineStr">
-        <is>
-          <t>Number of attendees: 150</t>
+      <c r="D153" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E153" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="inlineStr">
+        <is>
+          <t>Number of attendees: 151</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="1" t="inlineStr">
         <is>
           <t>Number of voters: 56</t>
         </is>
@@ -15886,7 +15913,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Voting details as of 23/04/2021 11:02</t>
+          <t>410E Voting details as of 23/04/2021 16:15</t>
         </is>
       </c>
     </row>
@@ -16263,7 +16290,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Voting details as of 23/04/2021 11:02</t>
+          <t>410W Voting details as of 23/04/2021 16:15</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Registree stats backup on Fri 23 Apr 2021 16:29:45 SAST
</commit_message>
<xml_diff>
--- a/static/docs/registrees_list.xlsx
+++ b/static/docs/registrees_list.xlsx
@@ -451,7 +451,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>MD410 Registrees as of 23/04/2021 16:15</t>
+          <t>MD410 Registrees as of 23/04/2021 16:29</t>
         </is>
       </c>
     </row>
@@ -8179,7 +8179,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Registrees as of 23/04/2021 16:15</t>
+          <t>410E Registrees as of 23/04/2021 16:29</t>
         </is>
       </c>
     </row>
@@ -11764,7 +11764,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Registrees as of 23/04/2021 16:15</t>
+          <t>410W Registrees as of 23/04/2021 16:29</t>
         </is>
       </c>
     </row>
@@ -15913,7 +15913,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Voting details as of 23/04/2021 16:15</t>
+          <t>410E Voting details as of 23/04/2021 16:29</t>
         </is>
       </c>
     </row>
@@ -16290,7 +16290,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Voting details as of 23/04/2021 16:15</t>
+          <t>410W Voting details as of 23/04/2021 16:29</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Registree stats backup on Mon 26 Apr 2021 18:29:12 SAST
</commit_message>
<xml_diff>
--- a/static/docs/registrees_list.xlsx
+++ b/static/docs/registrees_list.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F244"/>
+  <dimension ref="A1:F245"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,7 +451,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>MD410 Registrees as of 24/04/2021 14:19</t>
+          <t>MD410 Registrees as of 26/04/2021 18:29</t>
         </is>
       </c>
     </row>
@@ -6538,27 +6538,27 @@
     <row r="192" ht="25" customHeight="1">
       <c r="A192" s="3" t="inlineStr">
         <is>
-          <t>Toye</t>
+          <t>Townsend</t>
         </is>
       </c>
       <c r="B192" s="3" t="inlineStr">
         <is>
-          <t>Omolayo</t>
+          <t>Diane</t>
         </is>
       </c>
       <c r="C192" s="3" t="inlineStr">
         <is>
-          <t>The Wilds</t>
+          <t>Benoni Lakes</t>
         </is>
       </c>
       <c r="D192" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E192" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F192" s="3" t="inlineStr">
@@ -6570,22 +6570,22 @@
     <row r="193" ht="25" customHeight="1">
       <c r="A193" s="3" t="inlineStr">
         <is>
-          <t>Tshikala</t>
+          <t>Toye</t>
         </is>
       </c>
       <c r="B193" s="3" t="inlineStr">
         <is>
-          <t>David Alex</t>
+          <t>Omolayo</t>
         </is>
       </c>
       <c r="C193" s="3" t="inlineStr">
         <is>
-          <t>Athlone</t>
+          <t>The Wilds</t>
         </is>
       </c>
       <c r="D193" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E193" s="3" t="inlineStr">
@@ -6595,24 +6595,24 @@
       </c>
       <c r="F193" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="194" ht="25" customHeight="1">
       <c r="A194" s="3" t="inlineStr">
         <is>
-          <t>Tuckett</t>
+          <t>Tshikala</t>
         </is>
       </c>
       <c r="B194" s="3" t="inlineStr">
         <is>
-          <t>Alistair</t>
+          <t>David Alex</t>
         </is>
       </c>
       <c r="C194" s="3" t="inlineStr">
         <is>
-          <t>Roodepoort Clearwater Cyber</t>
+          <t>Athlone</t>
         </is>
       </c>
       <c r="D194" s="3" t="inlineStr">
@@ -6627,7 +6627,7 @@
       </c>
       <c r="F194" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -6639,7 +6639,7 @@
       </c>
       <c r="B195" s="3" t="inlineStr">
         <is>
-          <t>Rowan</t>
+          <t>Alistair</t>
         </is>
       </c>
       <c r="C195" s="3" t="inlineStr">
@@ -6654,7 +6654,7 @@
       </c>
       <c r="E195" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F195" s="3" t="inlineStr">
@@ -6671,7 +6671,7 @@
       </c>
       <c r="B196" s="3" t="inlineStr">
         <is>
-          <t>Gail</t>
+          <t>Rowan</t>
         </is>
       </c>
       <c r="C196" s="3" t="inlineStr">
@@ -6686,7 +6686,7 @@
       </c>
       <c r="E196" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F196" s="3" t="inlineStr">
@@ -6698,17 +6698,17 @@
     <row r="197" ht="25" customHeight="1">
       <c r="A197" s="3" t="inlineStr">
         <is>
-          <t>VAN BREDA</t>
+          <t>Tuckett</t>
         </is>
       </c>
       <c r="B197" s="3" t="inlineStr">
         <is>
-          <t>HILARY LISE</t>
+          <t>Gail</t>
         </is>
       </c>
       <c r="C197" s="3" t="inlineStr">
         <is>
-          <t>Cape Town</t>
+          <t>Roodepoort Clearwater Cyber</t>
         </is>
       </c>
       <c r="D197" s="3" t="inlineStr">
@@ -6723,39 +6723,39 @@
       </c>
       <c r="F197" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="198" ht="25" customHeight="1">
       <c r="A198" s="3" t="inlineStr">
         <is>
-          <t>VAN DER MERWE</t>
+          <t>VAN BREDA</t>
         </is>
       </c>
       <c r="B198" s="3" t="inlineStr">
         <is>
-          <t>PATRICIA</t>
+          <t>HILARY LISE</t>
         </is>
       </c>
       <c r="C198" s="3" t="inlineStr">
         <is>
-          <t>East London Port Rex</t>
+          <t>Cape Town</t>
         </is>
       </c>
       <c r="D198" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E198" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F198" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -6767,17 +6767,17 @@
       </c>
       <c r="B199" s="3" t="inlineStr">
         <is>
-          <t>MARINA</t>
+          <t>PATRICIA</t>
         </is>
       </c>
       <c r="C199" s="3" t="inlineStr">
         <is>
-          <t>Malmesbury</t>
+          <t>East London Port Rex</t>
         </is>
       </c>
       <c r="D199" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E199" s="3" t="inlineStr">
@@ -6787,56 +6787,56 @@
       </c>
       <c r="F199" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="200" ht="25" customHeight="1">
       <c r="A200" s="3" t="inlineStr">
         <is>
-          <t>Valadao</t>
+          <t>VAN DER MERWE</t>
         </is>
       </c>
       <c r="B200" s="3" t="inlineStr">
         <is>
-          <t>Tracy</t>
+          <t>MARINA</t>
         </is>
       </c>
       <c r="C200" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Malmesbury</t>
         </is>
       </c>
       <c r="D200" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E200" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F200" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="201" ht="25" customHeight="1">
       <c r="A201" s="3" t="inlineStr">
         <is>
-          <t>Van Niekerk</t>
+          <t>Valadao</t>
         </is>
       </c>
       <c r="B201" s="3" t="inlineStr">
         <is>
-          <t>Riaan</t>
+          <t>Tracy</t>
         </is>
       </c>
       <c r="C201" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D201" s="3" t="inlineStr">
@@ -6858,22 +6858,22 @@
     <row r="202" ht="25" customHeight="1">
       <c r="A202" s="3" t="inlineStr">
         <is>
-          <t>Van Nieuwenhuyzen</t>
+          <t>Van Niekerk</t>
         </is>
       </c>
       <c r="B202" s="3" t="inlineStr">
         <is>
-          <t>Hilgardt</t>
+          <t>Riaan</t>
         </is>
       </c>
       <c r="C202" s="3" t="inlineStr">
         <is>
-          <t>Worcester</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D202" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E202" s="3" t="inlineStr">
@@ -6883,24 +6883,24 @@
       </c>
       <c r="F202" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="203" ht="25" customHeight="1">
       <c r="A203" s="3" t="inlineStr">
         <is>
-          <t>Van Rensburg</t>
+          <t>Van Nieuwenhuyzen</t>
         </is>
       </c>
       <c r="B203" s="3" t="inlineStr">
         <is>
-          <t>Neville</t>
+          <t>Hilgardt</t>
         </is>
       </c>
       <c r="C203" s="3" t="inlineStr">
         <is>
-          <t>Moorreesburg</t>
+          <t>Worcester</t>
         </is>
       </c>
       <c r="D203" s="3" t="inlineStr">
@@ -6910,7 +6910,7 @@
       </c>
       <c r="E203" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F203" s="3" t="inlineStr">
@@ -6922,27 +6922,27 @@
     <row r="204" ht="25" customHeight="1">
       <c r="A204" s="3" t="inlineStr">
         <is>
-          <t>Van Romburgh</t>
+          <t>Van Rensburg</t>
         </is>
       </c>
       <c r="B204" s="3" t="inlineStr">
         <is>
-          <t>Lorna</t>
+          <t>Neville</t>
         </is>
       </c>
       <c r="C204" s="3" t="inlineStr">
         <is>
-          <t>Fish Hoek</t>
+          <t>Moorreesburg</t>
         </is>
       </c>
       <c r="D204" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E204" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F204" s="3" t="inlineStr">
@@ -6954,17 +6954,17 @@
     <row r="205" ht="25" customHeight="1">
       <c r="A205" s="3" t="inlineStr">
         <is>
-          <t>Van Wyk-Nelson</t>
+          <t>Van Romburgh</t>
         </is>
       </c>
       <c r="B205" s="3" t="inlineStr">
         <is>
-          <t>Edith</t>
+          <t>Lorna</t>
         </is>
       </c>
       <c r="C205" s="3" t="inlineStr">
         <is>
-          <t>Kuilsriver</t>
+          <t>Fish Hoek</t>
         </is>
       </c>
       <c r="D205" s="3" t="inlineStr">
@@ -6986,17 +6986,17 @@
     <row r="206" ht="25" customHeight="1">
       <c r="A206" s="3" t="inlineStr">
         <is>
-          <t>Van Zyl</t>
+          <t>Van Wyk-Nelson</t>
         </is>
       </c>
       <c r="B206" s="3" t="inlineStr">
         <is>
-          <t>Louis</t>
+          <t>Edith</t>
         </is>
       </c>
       <c r="C206" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Kuilsriver</t>
         </is>
       </c>
       <c r="D206" s="3" t="inlineStr">
@@ -7011,29 +7011,29 @@
       </c>
       <c r="F206" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="207" ht="25" customHeight="1">
       <c r="A207" s="3" t="inlineStr">
         <is>
-          <t>Van de Merwe</t>
+          <t>Van Zyl</t>
         </is>
       </c>
       <c r="B207" s="3" t="inlineStr">
         <is>
-          <t>Marina</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="C207" s="3" t="inlineStr">
         <is>
-          <t>Malmesbury</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D207" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E207" s="3" t="inlineStr">
@@ -7043,29 +7043,29 @@
       </c>
       <c r="F207" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="208" ht="25" customHeight="1">
       <c r="A208" s="3" t="inlineStr">
         <is>
-          <t>Venter</t>
+          <t>Van de Merwe</t>
         </is>
       </c>
       <c r="B208" s="3" t="inlineStr">
         <is>
-          <t>Louis</t>
+          <t>Marina</t>
         </is>
       </c>
       <c r="C208" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Malmesbury</t>
         </is>
       </c>
       <c r="D208" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E208" s="3" t="inlineStr">
@@ -7075,34 +7075,34 @@
       </c>
       <c r="F208" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="209" ht="25" customHeight="1">
       <c r="A209" s="3" t="inlineStr">
         <is>
-          <t>Volker</t>
+          <t>Venter</t>
         </is>
       </c>
       <c r="B209" s="3" t="inlineStr">
         <is>
-          <t>Russell</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="C209" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D209" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E209" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F209" s="3" t="inlineStr">
@@ -7114,96 +7114,96 @@
     <row r="210" ht="25" customHeight="1">
       <c r="A210" s="3" t="inlineStr">
         <is>
-          <t>Von Mollendorf</t>
+          <t>Volker</t>
         </is>
       </c>
       <c r="B210" s="3" t="inlineStr">
         <is>
-          <t>Rinette</t>
+          <t>Russell</t>
         </is>
       </c>
       <c r="C210" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>King William's Town</t>
         </is>
       </c>
       <c r="D210" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E210" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F210" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="211" ht="25" customHeight="1">
       <c r="A211" s="3" t="inlineStr">
         <is>
-          <t>Warman</t>
+          <t>Von Mollendorf</t>
         </is>
       </c>
       <c r="B211" s="3" t="inlineStr">
         <is>
-          <t>Alastair</t>
+          <t>Rinette</t>
         </is>
       </c>
       <c r="C211" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Durbanville</t>
         </is>
       </c>
       <c r="D211" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E211" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F211" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="212" ht="25" customHeight="1">
       <c r="A212" s="3" t="inlineStr">
         <is>
-          <t>Watson</t>
+          <t>Warman</t>
         </is>
       </c>
       <c r="B212" s="3" t="inlineStr">
         <is>
-          <t>Allan</t>
+          <t>Alastair</t>
         </is>
       </c>
       <c r="C212" s="3" t="inlineStr">
         <is>
-          <t>Sea Point</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D212" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E212" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F212" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -7215,22 +7215,22 @@
       </c>
       <c r="B213" s="3" t="inlineStr">
         <is>
-          <t>Alison</t>
+          <t>Allan</t>
         </is>
       </c>
       <c r="C213" s="3" t="inlineStr">
         <is>
-          <t>Sedgefield</t>
+          <t>Sea Point</t>
         </is>
       </c>
       <c r="D213" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E213" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F213" s="3" t="inlineStr">
@@ -7242,27 +7242,27 @@
     <row r="214" ht="25" customHeight="1">
       <c r="A214" s="3" t="inlineStr">
         <is>
-          <t>Williams</t>
+          <t>Watson</t>
         </is>
       </c>
       <c r="B214" s="3" t="inlineStr">
         <is>
-          <t>Johanna</t>
+          <t>Alison</t>
         </is>
       </c>
       <c r="C214" s="3" t="inlineStr">
         <is>
-          <t>Mitchells Plain</t>
+          <t>Sedgefield</t>
         </is>
       </c>
       <c r="D214" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E214" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F214" s="3" t="inlineStr">
@@ -7274,22 +7274,22 @@
     <row r="215" ht="25" customHeight="1">
       <c r="A215" s="3" t="inlineStr">
         <is>
-          <t>Wills</t>
+          <t>Williams</t>
         </is>
       </c>
       <c r="B215" s="3" t="inlineStr">
         <is>
-          <t>Geila</t>
+          <t>Johanna</t>
         </is>
       </c>
       <c r="C215" s="3" t="inlineStr">
         <is>
-          <t>Athlone</t>
+          <t>Mitchells Plain</t>
         </is>
       </c>
       <c r="D215" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E215" s="3" t="inlineStr">
@@ -7306,17 +7306,17 @@
     <row r="216" ht="25" customHeight="1">
       <c r="A216" s="3" t="inlineStr">
         <is>
-          <t>Wilter-Sturges</t>
+          <t>Wills</t>
         </is>
       </c>
       <c r="B216" s="3" t="inlineStr">
         <is>
-          <t>Meredith</t>
+          <t>Geila</t>
         </is>
       </c>
       <c r="C216" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Athlone</t>
         </is>
       </c>
       <c r="D216" s="3" t="inlineStr">
@@ -7331,24 +7331,24 @@
       </c>
       <c r="F216" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="217" ht="25" customHeight="1">
       <c r="A217" s="3" t="inlineStr">
         <is>
-          <t>Wright</t>
+          <t>Wilter-Sturges</t>
         </is>
       </c>
       <c r="B217" s="3" t="inlineStr">
         <is>
-          <t>Rocky</t>
+          <t>Meredith</t>
         </is>
       </c>
       <c r="C217" s="3" t="inlineStr">
         <is>
-          <t>Table View</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D217" s="3" t="inlineStr">
@@ -7358,29 +7358,29 @@
       </c>
       <c r="E217" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F217" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="218" ht="25" customHeight="1">
       <c r="A218" s="3" t="inlineStr">
         <is>
-          <t>Young</t>
+          <t>Wright</t>
         </is>
       </c>
       <c r="B218" s="3" t="inlineStr">
         <is>
-          <t>Judy</t>
+          <t>Rocky</t>
         </is>
       </c>
       <c r="C218" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>Table View</t>
         </is>
       </c>
       <c r="D218" s="3" t="inlineStr">
@@ -7390,7 +7390,7 @@
       </c>
       <c r="E218" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F218" s="3" t="inlineStr">
@@ -7402,17 +7402,17 @@
     <row r="219" ht="25" customHeight="1">
       <c r="A219" s="3" t="inlineStr">
         <is>
-          <t>de Kock</t>
+          <t>Young</t>
         </is>
       </c>
       <c r="B219" s="3" t="inlineStr">
         <is>
-          <t>Engela</t>
+          <t>Judy</t>
         </is>
       </c>
       <c r="C219" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Durbanville</t>
         </is>
       </c>
       <c r="D219" s="3" t="inlineStr">
@@ -7422,7 +7422,7 @@
       </c>
       <c r="E219" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F219" s="3" t="inlineStr">
@@ -7439,7 +7439,7 @@
       </c>
       <c r="B220" s="3" t="inlineStr">
         <is>
-          <t>Francois</t>
+          <t>Engela</t>
         </is>
       </c>
       <c r="C220" s="3" t="inlineStr">
@@ -7466,59 +7466,59 @@
     <row r="221" ht="25" customHeight="1">
       <c r="A221" s="3" t="inlineStr">
         <is>
-          <t>de Silva</t>
+          <t>de Kock</t>
         </is>
       </c>
       <c r="B221" s="3" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Francois</t>
         </is>
       </c>
       <c r="C221" s="3" t="inlineStr">
         <is>
-          <t>Edenvale</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D221" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E221" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F221" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="222" ht="25" customHeight="1">
       <c r="A222" s="3" t="inlineStr">
         <is>
-          <t>du Toit</t>
+          <t>de Silva</t>
         </is>
       </c>
       <c r="B222" s="3" t="inlineStr">
         <is>
-          <t>Desiree</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="C222" s="3" t="inlineStr">
         <is>
-          <t>Ramsgate</t>
+          <t>Edenvale</t>
         </is>
       </c>
       <c r="D222" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E222" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F222" s="3" t="inlineStr">
@@ -7530,22 +7530,22 @@
     <row r="223" ht="25" customHeight="1">
       <c r="A223" s="3" t="inlineStr">
         <is>
-          <t>stier</t>
+          <t>du Toit</t>
         </is>
       </c>
       <c r="B223" s="3" t="inlineStr">
         <is>
-          <t>RORY</t>
+          <t>Desiree</t>
         </is>
       </c>
       <c r="C223" s="3" t="inlineStr">
         <is>
-          <t>Deep South</t>
+          <t>Ramsgate</t>
         </is>
       </c>
       <c r="D223" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E223" s="3" t="inlineStr">
@@ -7555,56 +7555,56 @@
       </c>
       <c r="F223" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="224" ht="25" customHeight="1">
       <c r="A224" s="3" t="inlineStr">
         <is>
-          <t>tyler</t>
+          <t>stier</t>
         </is>
       </c>
       <c r="B224" s="3" t="inlineStr">
         <is>
-          <t>natascha</t>
+          <t>RORY</t>
         </is>
       </c>
       <c r="C224" s="3" t="inlineStr">
         <is>
-          <t>Kensington</t>
+          <t>Deep South</t>
         </is>
       </c>
       <c r="D224" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E224" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F224" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="225" ht="25" customHeight="1">
       <c r="A225" s="3" t="inlineStr">
         <is>
-          <t>van Blerk</t>
+          <t>tyler</t>
         </is>
       </c>
       <c r="B225" s="3" t="inlineStr">
         <is>
-          <t>Carl</t>
+          <t>natascha</t>
         </is>
       </c>
       <c r="C225" s="3" t="inlineStr">
         <is>
-          <t>Eden</t>
+          <t>Kensington</t>
         </is>
       </c>
       <c r="D225" s="3" t="inlineStr">
@@ -7619,24 +7619,24 @@
       </c>
       <c r="F225" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="226" ht="25" customHeight="1">
       <c r="A226" s="3" t="inlineStr">
         <is>
-          <t>van Heerden</t>
+          <t>van Blerk</t>
         </is>
       </c>
       <c r="B226" s="3" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Carl</t>
         </is>
       </c>
       <c r="C226" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Eden</t>
         </is>
       </c>
       <c r="D226" s="3" t="inlineStr">
@@ -7651,7 +7651,7 @@
       </c>
       <c r="F226" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -7663,7 +7663,7 @@
       </c>
       <c r="B227" s="3" t="inlineStr">
         <is>
-          <t>Sandy</t>
+          <t>Sydney</t>
         </is>
       </c>
       <c r="C227" s="3" t="inlineStr">
@@ -7678,7 +7678,7 @@
       </c>
       <c r="E227" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F227" s="3" t="inlineStr">
@@ -7695,17 +7695,17 @@
       </c>
       <c r="B228" s="3" t="inlineStr">
         <is>
-          <t>Craig</t>
+          <t>Sandy</t>
         </is>
       </c>
       <c r="C228" s="3" t="inlineStr">
         <is>
-          <t>East London Beacon Bay</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D228" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E228" s="3" t="inlineStr">
@@ -7727,17 +7727,17 @@
       </c>
       <c r="B229" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Craig</t>
         </is>
       </c>
       <c r="C229" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>East London Beacon Bay</t>
         </is>
       </c>
       <c r="D229" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E229" s="3" t="inlineStr">
@@ -7754,17 +7754,17 @@
     <row r="230" ht="25" customHeight="1">
       <c r="A230" s="3" t="inlineStr">
         <is>
-          <t>van Rensburg</t>
+          <t>van Heerden</t>
         </is>
       </c>
       <c r="B230" s="3" t="inlineStr">
         <is>
-          <t>Johan</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C230" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D230" s="3" t="inlineStr">
@@ -7774,12 +7774,12 @@
       </c>
       <c r="E230" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F230" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -7791,7 +7791,7 @@
       </c>
       <c r="B231" s="3" t="inlineStr">
         <is>
-          <t>Anne</t>
+          <t>Johan</t>
         </is>
       </c>
       <c r="C231" s="3" t="inlineStr">
@@ -7818,17 +7818,17 @@
     <row r="232" ht="25" customHeight="1">
       <c r="A232" s="3" t="inlineStr">
         <is>
-          <t>van Wulven</t>
+          <t>van Rensburg</t>
         </is>
       </c>
       <c r="B232" s="3" t="inlineStr">
         <is>
-          <t>Jeannie</t>
+          <t>Anne</t>
         </is>
       </c>
       <c r="C232" s="3" t="inlineStr">
         <is>
-          <t>Tygerberg Hills</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D232" s="3" t="inlineStr">
@@ -7855,7 +7855,7 @@
       </c>
       <c r="B233" s="3" t="inlineStr">
         <is>
-          <t>Alan</t>
+          <t>Jeannie</t>
         </is>
       </c>
       <c r="C233" s="3" t="inlineStr">
@@ -7887,7 +7887,7 @@
       </c>
       <c r="B234" s="3" t="inlineStr">
         <is>
-          <t>Deon</t>
+          <t>Alan</t>
         </is>
       </c>
       <c r="C234" s="3" t="inlineStr">
@@ -7914,17 +7914,17 @@
     <row r="235" ht="25" customHeight="1">
       <c r="A235" s="3" t="inlineStr">
         <is>
-          <t>van Wyk</t>
+          <t>van Wulven</t>
         </is>
       </c>
       <c r="B235" s="3" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>Deon</t>
         </is>
       </c>
       <c r="C235" s="3" t="inlineStr">
         <is>
-          <t>North Durban</t>
+          <t>Tygerberg Hills</t>
         </is>
       </c>
       <c r="D235" s="3" t="inlineStr">
@@ -7939,7 +7939,7 @@
       </c>
       <c r="F235" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -7951,12 +7951,12 @@
       </c>
       <c r="B236" s="3" t="inlineStr">
         <is>
-          <t>Lindie</t>
+          <t>Kim</t>
         </is>
       </c>
       <c r="C236" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>North Durban</t>
         </is>
       </c>
       <c r="D236" s="3" t="inlineStr">
@@ -7983,12 +7983,12 @@
       </c>
       <c r="B237" s="3" t="inlineStr">
         <is>
-          <t>Willem</t>
+          <t>Lindie</t>
         </is>
       </c>
       <c r="C237" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D237" s="3" t="inlineStr">
@@ -8015,12 +8015,12 @@
       </c>
       <c r="B238" s="3" t="inlineStr">
         <is>
-          <t>Patricia</t>
+          <t>Willem</t>
         </is>
       </c>
       <c r="C238" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D238" s="3" t="inlineStr">
@@ -8042,22 +8042,22 @@
     <row r="239" ht="25" customHeight="1">
       <c r="A239" s="3" t="inlineStr">
         <is>
-          <t>van der Merwe</t>
+          <t>van Wyk</t>
         </is>
       </c>
       <c r="B239" s="3" t="inlineStr">
         <is>
-          <t>Ingrid</t>
+          <t>Patricia</t>
         </is>
       </c>
       <c r="C239" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D239" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E239" s="3" t="inlineStr">
@@ -8074,49 +8074,49 @@
     <row r="240" ht="25" customHeight="1">
       <c r="A240" s="3" t="inlineStr">
         <is>
-          <t>van der Westhuizen</t>
+          <t>van der Merwe</t>
         </is>
       </c>
       <c r="B240" s="3" t="inlineStr">
         <is>
-          <t>Hennie</t>
+          <t>Ingrid</t>
         </is>
       </c>
       <c r="C240" s="3" t="inlineStr">
         <is>
-          <t>Helderberg</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D240" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E240" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F240" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="241" ht="25" customHeight="1">
       <c r="A241" s="3" t="inlineStr">
         <is>
-          <t>von der Decken</t>
+          <t>van der Westhuizen</t>
         </is>
       </c>
       <c r="B241" s="3" t="inlineStr">
         <is>
-          <t>Brian</t>
+          <t>Hennie</t>
         </is>
       </c>
       <c r="C241" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Helderberg</t>
         </is>
       </c>
       <c r="D241" s="3" t="inlineStr">
@@ -8131,53 +8131,85 @@
       </c>
       <c r="F241" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="242" ht="25" customHeight="1">
       <c r="A242" s="3" t="inlineStr">
         <is>
+          <t>von der Decken</t>
+        </is>
+      </c>
+      <c r="B242" s="3" t="inlineStr">
+        <is>
+          <t>Brian</t>
+        </is>
+      </c>
+      <c r="C242" s="3" t="inlineStr">
+        <is>
+          <t>King William's Town</t>
+        </is>
+      </c>
+      <c r="D242" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E242" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F242" s="3" t="inlineStr">
+        <is>
+          <t>410E</t>
+        </is>
+      </c>
+    </row>
+    <row r="243" ht="25" customHeight="1">
+      <c r="A243" s="3" t="inlineStr">
+        <is>
           <t>‘t Hart</t>
         </is>
       </c>
-      <c r="B242" s="3" t="inlineStr">
+      <c r="B243" s="3" t="inlineStr">
         <is>
           <t>Michelle</t>
         </is>
       </c>
-      <c r="C242" s="3" t="inlineStr">
+      <c r="C243" s="3" t="inlineStr">
         <is>
           <t>Benoni Lakes</t>
         </is>
       </c>
-      <c r="D242" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E242" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F242" s="3" t="inlineStr">
+      <c r="D243" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E243" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F243" s="3" t="inlineStr">
         <is>
           <t>410E</t>
-        </is>
-      </c>
-    </row>
-    <row r="243">
-      <c r="A243" s="1" t="inlineStr">
-        <is>
-          <t>Number of attendees: 240</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="inlineStr">
         <is>
-          <t>Number of voters: 95</t>
+          <t>Number of attendees: 241</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" s="1" t="inlineStr">
+        <is>
+          <t>Number of voters: 96</t>
         </is>
       </c>
     </row>
@@ -8211,7 +8243,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Registrees as of 24/04/2021 14:19</t>
+          <t>410E Registrees as of 26/04/2021 18:29</t>
         </is>
       </c>
     </row>
@@ -11796,7 +11828,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Registrees as of 24/04/2021 14:19</t>
+          <t>410W Registrees as of 26/04/2021 18:29</t>
         </is>
       </c>
     </row>
@@ -15972,7 +16004,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Voting details as of 24/04/2021 14:19</t>
+          <t>410E Voting details as of 26/04/2021 18:29</t>
         </is>
       </c>
     </row>
@@ -16349,7 +16381,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Voting details as of 24/04/2021 14:19</t>
+          <t>410W Voting details as of 26/04/2021 18:29</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Registree stats backup on Wed 28 Apr 2021 13:30:17 SAST
</commit_message>
<xml_diff>
--- a/static/docs/registrees_list.xlsx
+++ b/static/docs/registrees_list.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F245"/>
+  <dimension ref="A1:F247"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,7 +451,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>MD410 Registrees as of 26/04/2021 18:29</t>
+          <t>MD410 Registrees as of 28/04/2021 13:30</t>
         </is>
       </c>
     </row>
@@ -7530,17 +7530,17 @@
     <row r="223" ht="25" customHeight="1">
       <c r="A223" s="3" t="inlineStr">
         <is>
-          <t>du Toit</t>
+          <t>du Plooy</t>
         </is>
       </c>
       <c r="B223" s="3" t="inlineStr">
         <is>
-          <t>Desiree</t>
+          <t>Tammy</t>
         </is>
       </c>
       <c r="C223" s="3" t="inlineStr">
         <is>
-          <t>Ramsgate</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D223" s="3" t="inlineStr">
@@ -7562,22 +7562,22 @@
     <row r="224" ht="25" customHeight="1">
       <c r="A224" s="3" t="inlineStr">
         <is>
-          <t>stier</t>
+          <t>du Plooy</t>
         </is>
       </c>
       <c r="B224" s="3" t="inlineStr">
         <is>
-          <t>RORY</t>
+          <t>Marc</t>
         </is>
       </c>
       <c r="C224" s="3" t="inlineStr">
         <is>
-          <t>Deep South</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D224" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E224" s="3" t="inlineStr">
@@ -7587,24 +7587,24 @@
       </c>
       <c r="F224" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="225" ht="25" customHeight="1">
       <c r="A225" s="3" t="inlineStr">
         <is>
-          <t>tyler</t>
+          <t>du Toit</t>
         </is>
       </c>
       <c r="B225" s="3" t="inlineStr">
         <is>
-          <t>natascha</t>
+          <t>Desiree</t>
         </is>
       </c>
       <c r="C225" s="3" t="inlineStr">
         <is>
-          <t>Kensington</t>
+          <t>Ramsgate</t>
         </is>
       </c>
       <c r="D225" s="3" t="inlineStr">
@@ -7614,7 +7614,7 @@
       </c>
       <c r="E225" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F225" s="3" t="inlineStr">
@@ -7626,27 +7626,27 @@
     <row r="226" ht="25" customHeight="1">
       <c r="A226" s="3" t="inlineStr">
         <is>
-          <t>van Blerk</t>
+          <t>stier</t>
         </is>
       </c>
       <c r="B226" s="3" t="inlineStr">
         <is>
-          <t>Carl</t>
+          <t>RORY</t>
         </is>
       </c>
       <c r="C226" s="3" t="inlineStr">
         <is>
-          <t>Eden</t>
+          <t>Deep South</t>
         </is>
       </c>
       <c r="D226" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E226" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F226" s="3" t="inlineStr">
@@ -7658,17 +7658,17 @@
     <row r="227" ht="25" customHeight="1">
       <c r="A227" s="3" t="inlineStr">
         <is>
-          <t>van Heerden</t>
+          <t>tyler</t>
         </is>
       </c>
       <c r="B227" s="3" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>natascha</t>
         </is>
       </c>
       <c r="C227" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Kensington</t>
         </is>
       </c>
       <c r="D227" s="3" t="inlineStr">
@@ -7690,17 +7690,17 @@
     <row r="228" ht="25" customHeight="1">
       <c r="A228" s="3" t="inlineStr">
         <is>
-          <t>van Heerden</t>
+          <t>van Blerk</t>
         </is>
       </c>
       <c r="B228" s="3" t="inlineStr">
         <is>
-          <t>Sandy</t>
+          <t>Carl</t>
         </is>
       </c>
       <c r="C228" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Eden</t>
         </is>
       </c>
       <c r="D228" s="3" t="inlineStr">
@@ -7710,12 +7710,12 @@
       </c>
       <c r="E228" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F228" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -7727,22 +7727,22 @@
       </c>
       <c r="B229" s="3" t="inlineStr">
         <is>
-          <t>Craig</t>
+          <t>Sydney</t>
         </is>
       </c>
       <c r="C229" s="3" t="inlineStr">
         <is>
-          <t>East London Beacon Bay</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D229" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E229" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F229" s="3" t="inlineStr">
@@ -7759,12 +7759,12 @@
       </c>
       <c r="B230" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Sandy</t>
         </is>
       </c>
       <c r="C230" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D230" s="3" t="inlineStr">
@@ -7786,49 +7786,49 @@
     <row r="231" ht="25" customHeight="1">
       <c r="A231" s="3" t="inlineStr">
         <is>
-          <t>van Rensburg</t>
+          <t>van Heerden</t>
         </is>
       </c>
       <c r="B231" s="3" t="inlineStr">
         <is>
-          <t>Johan</t>
+          <t>Craig</t>
         </is>
       </c>
       <c r="C231" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>East London Beacon Bay</t>
         </is>
       </c>
       <c r="D231" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E231" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F231" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="232" ht="25" customHeight="1">
       <c r="A232" s="3" t="inlineStr">
         <is>
-          <t>van Rensburg</t>
+          <t>van Heerden</t>
         </is>
       </c>
       <c r="B232" s="3" t="inlineStr">
         <is>
-          <t>Anne</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C232" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D232" s="3" t="inlineStr">
@@ -7838,29 +7838,29 @@
       </c>
       <c r="E232" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F232" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="233" ht="25" customHeight="1">
       <c r="A233" s="3" t="inlineStr">
         <is>
-          <t>van Wulven</t>
+          <t>van Rensburg</t>
         </is>
       </c>
       <c r="B233" s="3" t="inlineStr">
         <is>
-          <t>Jeannie</t>
+          <t>Johan</t>
         </is>
       </c>
       <c r="C233" s="3" t="inlineStr">
         <is>
-          <t>Tygerberg Hills</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D233" s="3" t="inlineStr">
@@ -7882,17 +7882,17 @@
     <row r="234" ht="25" customHeight="1">
       <c r="A234" s="3" t="inlineStr">
         <is>
-          <t>van Wulven</t>
+          <t>van Rensburg</t>
         </is>
       </c>
       <c r="B234" s="3" t="inlineStr">
         <is>
-          <t>Alan</t>
+          <t>Anne</t>
         </is>
       </c>
       <c r="C234" s="3" t="inlineStr">
         <is>
-          <t>Tygerberg Hills</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D234" s="3" t="inlineStr">
@@ -7919,7 +7919,7 @@
       </c>
       <c r="B235" s="3" t="inlineStr">
         <is>
-          <t>Deon</t>
+          <t>Jeannie</t>
         </is>
       </c>
       <c r="C235" s="3" t="inlineStr">
@@ -7946,17 +7946,17 @@
     <row r="236" ht="25" customHeight="1">
       <c r="A236" s="3" t="inlineStr">
         <is>
-          <t>van Wyk</t>
+          <t>van Wulven</t>
         </is>
       </c>
       <c r="B236" s="3" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>Alan</t>
         </is>
       </c>
       <c r="C236" s="3" t="inlineStr">
         <is>
-          <t>North Durban</t>
+          <t>Tygerberg Hills</t>
         </is>
       </c>
       <c r="D236" s="3" t="inlineStr">
@@ -7971,24 +7971,24 @@
       </c>
       <c r="F236" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="237" ht="25" customHeight="1">
       <c r="A237" s="3" t="inlineStr">
         <is>
-          <t>van Wyk</t>
+          <t>van Wulven</t>
         </is>
       </c>
       <c r="B237" s="3" t="inlineStr">
         <is>
-          <t>Lindie</t>
+          <t>Deon</t>
         </is>
       </c>
       <c r="C237" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Tygerberg Hills</t>
         </is>
       </c>
       <c r="D237" s="3" t="inlineStr">
@@ -8003,7 +8003,7 @@
       </c>
       <c r="F237" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -8015,12 +8015,12 @@
       </c>
       <c r="B238" s="3" t="inlineStr">
         <is>
-          <t>Willem</t>
+          <t>Kim</t>
         </is>
       </c>
       <c r="C238" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>North Durban</t>
         </is>
       </c>
       <c r="D238" s="3" t="inlineStr">
@@ -8047,7 +8047,7 @@
       </c>
       <c r="B239" s="3" t="inlineStr">
         <is>
-          <t>Patricia</t>
+          <t>Lindie</t>
         </is>
       </c>
       <c r="C239" s="3" t="inlineStr">
@@ -8074,22 +8074,22 @@
     <row r="240" ht="25" customHeight="1">
       <c r="A240" s="3" t="inlineStr">
         <is>
-          <t>van der Merwe</t>
+          <t>van Wyk</t>
         </is>
       </c>
       <c r="B240" s="3" t="inlineStr">
         <is>
-          <t>Ingrid</t>
+          <t>Willem</t>
         </is>
       </c>
       <c r="C240" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D240" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E240" s="3" t="inlineStr">
@@ -8106,17 +8106,17 @@
     <row r="241" ht="25" customHeight="1">
       <c r="A241" s="3" t="inlineStr">
         <is>
-          <t>van der Westhuizen</t>
+          <t>van Wyk</t>
         </is>
       </c>
       <c r="B241" s="3" t="inlineStr">
         <is>
-          <t>Hennie</t>
+          <t>Patricia</t>
         </is>
       </c>
       <c r="C241" s="3" t="inlineStr">
         <is>
-          <t>Helderberg</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D241" s="3" t="inlineStr">
@@ -8126,39 +8126,39 @@
       </c>
       <c r="E241" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F241" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="242" ht="25" customHeight="1">
       <c r="A242" s="3" t="inlineStr">
         <is>
-          <t>von der Decken</t>
+          <t>van der Merwe</t>
         </is>
       </c>
       <c r="B242" s="3" t="inlineStr">
         <is>
-          <t>Brian</t>
+          <t>Ingrid</t>
         </is>
       </c>
       <c r="C242" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D242" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E242" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F242" s="3" t="inlineStr">
@@ -8170,46 +8170,110 @@
     <row r="243" ht="25" customHeight="1">
       <c r="A243" s="3" t="inlineStr">
         <is>
+          <t>van der Westhuizen</t>
+        </is>
+      </c>
+      <c r="B243" s="3" t="inlineStr">
+        <is>
+          <t>Hennie</t>
+        </is>
+      </c>
+      <c r="C243" s="3" t="inlineStr">
+        <is>
+          <t>Helderberg</t>
+        </is>
+      </c>
+      <c r="D243" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E243" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F243" s="3" t="inlineStr">
+        <is>
+          <t>410W</t>
+        </is>
+      </c>
+    </row>
+    <row r="244" ht="25" customHeight="1">
+      <c r="A244" s="3" t="inlineStr">
+        <is>
+          <t>von der Decken</t>
+        </is>
+      </c>
+      <c r="B244" s="3" t="inlineStr">
+        <is>
+          <t>Brian</t>
+        </is>
+      </c>
+      <c r="C244" s="3" t="inlineStr">
+        <is>
+          <t>King William's Town</t>
+        </is>
+      </c>
+      <c r="D244" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E244" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F244" s="3" t="inlineStr">
+        <is>
+          <t>410E</t>
+        </is>
+      </c>
+    </row>
+    <row r="245" ht="25" customHeight="1">
+      <c r="A245" s="3" t="inlineStr">
+        <is>
           <t>‘t Hart</t>
         </is>
       </c>
-      <c r="B243" s="3" t="inlineStr">
+      <c r="B245" s="3" t="inlineStr">
         <is>
           <t>Michelle</t>
         </is>
       </c>
-      <c r="C243" s="3" t="inlineStr">
+      <c r="C245" s="3" t="inlineStr">
         <is>
           <t>Benoni Lakes</t>
         </is>
       </c>
-      <c r="D243" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E243" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F243" s="3" t="inlineStr">
+      <c r="D245" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E245" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F245" s="3" t="inlineStr">
         <is>
           <t>410E</t>
         </is>
       </c>
     </row>
-    <row r="244">
-      <c r="A244" s="1" t="inlineStr">
-        <is>
-          <t>Number of attendees: 241</t>
-        </is>
-      </c>
-    </row>
-    <row r="245">
-      <c r="A245" s="1" t="inlineStr">
-        <is>
-          <t>Number of voters: 96</t>
+    <row r="246">
+      <c r="A246" s="1" t="inlineStr">
+        <is>
+          <t>Number of attendees: 243</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" s="1" t="inlineStr">
+        <is>
+          <t>Number of voters: 98</t>
         </is>
       </c>
     </row>
@@ -8243,7 +8307,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Registrees as of 26/04/2021 18:29</t>
+          <t>410E Registrees as of 28/04/2021 13:30</t>
         </is>
       </c>
     </row>
@@ -11828,7 +11892,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Registrees as of 26/04/2021 18:29</t>
+          <t>410W Registrees as of 28/04/2021 13:30</t>
         </is>
       </c>
     </row>
@@ -16004,7 +16068,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Voting details as of 26/04/2021 18:29</t>
+          <t>410E Voting details as of 28/04/2021 13:30</t>
         </is>
       </c>
     </row>
@@ -16381,7 +16445,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Voting details as of 26/04/2021 18:29</t>
+          <t>410W Voting details as of 28/04/2021 13:30</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Registree stats backup on Wed 28 Apr 2021 16:40:15 SAST
</commit_message>
<xml_diff>
--- a/static/docs/registrees_list.xlsx
+++ b/static/docs/registrees_list.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F247"/>
+  <dimension ref="A1:F248"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,7 +451,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>MD410 Registrees as of 28/04/2021 13:30</t>
+          <t>MD410 Registrees as of 28/04/2021 16:40</t>
         </is>
       </c>
     </row>
@@ -5450,17 +5450,17 @@
     <row r="158" ht="25" customHeight="1">
       <c r="A158" s="3" t="inlineStr">
         <is>
-          <t>Reniers</t>
+          <t>Rathbone Smyth</t>
         </is>
       </c>
       <c r="B158" s="3" t="inlineStr">
         <is>
-          <t>Hugo</t>
+          <t>Janine</t>
         </is>
       </c>
       <c r="C158" s="3" t="inlineStr">
         <is>
-          <t>Nelspruit</t>
+          <t>Vereeniging</t>
         </is>
       </c>
       <c r="D158" s="3" t="inlineStr">
@@ -5470,7 +5470,7 @@
       </c>
       <c r="E158" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F158" s="3" t="inlineStr">
@@ -5482,17 +5482,17 @@
     <row r="159" ht="25" customHeight="1">
       <c r="A159" s="3" t="inlineStr">
         <is>
-          <t>Roman</t>
+          <t>Reniers</t>
         </is>
       </c>
       <c r="B159" s="3" t="inlineStr">
         <is>
-          <t>Sandy</t>
+          <t>Hugo</t>
         </is>
       </c>
       <c r="C159" s="3" t="inlineStr">
         <is>
-          <t>Bergvliet</t>
+          <t>Nelspruit</t>
         </is>
       </c>
       <c r="D159" s="3" t="inlineStr">
@@ -5502,29 +5502,29 @@
       </c>
       <c r="E159" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F159" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="160" ht="25" customHeight="1">
       <c r="A160" s="3" t="inlineStr">
         <is>
-          <t>Rossouw</t>
+          <t>Roman</t>
         </is>
       </c>
       <c r="B160" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Sandy</t>
         </is>
       </c>
       <c r="C160" s="3" t="inlineStr">
         <is>
-          <t>Tokai</t>
+          <t>Bergvliet</t>
         </is>
       </c>
       <c r="D160" s="3" t="inlineStr">
@@ -5534,7 +5534,7 @@
       </c>
       <c r="E160" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F160" s="3" t="inlineStr">
@@ -5546,17 +5546,17 @@
     <row r="161" ht="25" customHeight="1">
       <c r="A161" s="3" t="inlineStr">
         <is>
-          <t>Rothner</t>
+          <t>Rossouw</t>
         </is>
       </c>
       <c r="B161" s="3" t="inlineStr">
         <is>
-          <t>Andrea</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C161" s="3" t="inlineStr">
         <is>
-          <t>Eden</t>
+          <t>Tokai</t>
         </is>
       </c>
       <c r="D161" s="3" t="inlineStr">
@@ -5566,7 +5566,7 @@
       </c>
       <c r="E161" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F161" s="3" t="inlineStr">
@@ -5578,17 +5578,17 @@
     <row r="162" ht="25" customHeight="1">
       <c r="A162" s="3" t="inlineStr">
         <is>
-          <t>Roux</t>
+          <t>Rothner</t>
         </is>
       </c>
       <c r="B162" s="3" t="inlineStr">
         <is>
-          <t>Anthonie Petrus</t>
+          <t>Andrea</t>
         </is>
       </c>
       <c r="C162" s="3" t="inlineStr">
         <is>
-          <t>Moorreesburg</t>
+          <t>Eden</t>
         </is>
       </c>
       <c r="D162" s="3" t="inlineStr">
@@ -5598,7 +5598,7 @@
       </c>
       <c r="E162" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F162" s="3" t="inlineStr">
@@ -5610,17 +5610,17 @@
     <row r="163" ht="25" customHeight="1">
       <c r="A163" s="3" t="inlineStr">
         <is>
-          <t>Russell</t>
+          <t>Roux</t>
         </is>
       </c>
       <c r="B163" s="3" t="inlineStr">
         <is>
-          <t>Ingrid</t>
+          <t>Anthonie Petrus</t>
         </is>
       </c>
       <c r="C163" s="3" t="inlineStr">
         <is>
-          <t>Fish Hoek</t>
+          <t>Moorreesburg</t>
         </is>
       </c>
       <c r="D163" s="3" t="inlineStr">
@@ -5642,27 +5642,27 @@
     <row r="164" ht="25" customHeight="1">
       <c r="A164" s="3" t="inlineStr">
         <is>
-          <t>SNYMAN</t>
+          <t>Russell</t>
         </is>
       </c>
       <c r="B164" s="3" t="inlineStr">
         <is>
-          <t>LYN</t>
+          <t>Ingrid</t>
         </is>
       </c>
       <c r="C164" s="3" t="inlineStr">
         <is>
-          <t>Deep South</t>
+          <t>Fish Hoek</t>
         </is>
       </c>
       <c r="D164" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E164" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F164" s="3" t="inlineStr">
@@ -5674,27 +5674,27 @@
     <row r="165" ht="25" customHeight="1">
       <c r="A165" s="3" t="inlineStr">
         <is>
-          <t>STEENBERG</t>
+          <t>SNYMAN</t>
         </is>
       </c>
       <c r="B165" s="3" t="inlineStr">
         <is>
-          <t>TIM</t>
+          <t>LYN</t>
         </is>
       </c>
       <c r="C165" s="3" t="inlineStr">
         <is>
-          <t>Wellington</t>
+          <t>Deep South</t>
         </is>
       </c>
       <c r="D165" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E165" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F165" s="3" t="inlineStr">
@@ -5706,17 +5706,17 @@
     <row r="166" ht="25" customHeight="1">
       <c r="A166" s="3" t="inlineStr">
         <is>
-          <t>Sabatier</t>
+          <t>STEENBERG</t>
         </is>
       </c>
       <c r="B166" s="3" t="inlineStr">
         <is>
-          <t>Rodney</t>
+          <t>TIM</t>
         </is>
       </c>
       <c r="C166" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Wellington</t>
         </is>
       </c>
       <c r="D166" s="3" t="inlineStr">
@@ -5731,24 +5731,24 @@
       </c>
       <c r="F166" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="167" ht="25" customHeight="1">
       <c r="A167" s="3" t="inlineStr">
         <is>
-          <t>Sampie</t>
+          <t>Sabatier</t>
         </is>
       </c>
       <c r="B167" s="3" t="inlineStr">
         <is>
-          <t>Sharon</t>
+          <t>Rodney</t>
         </is>
       </c>
       <c r="C167" s="3" t="inlineStr">
         <is>
-          <t>Bergvliet</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D167" s="3" t="inlineStr">
@@ -5763,24 +5763,24 @@
       </c>
       <c r="F167" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="168" ht="25" customHeight="1">
       <c r="A168" s="3" t="inlineStr">
         <is>
-          <t>Schatz</t>
+          <t>Sampie</t>
         </is>
       </c>
       <c r="B168" s="3" t="inlineStr">
         <is>
-          <t>Vera</t>
+          <t>Sharon</t>
         </is>
       </c>
       <c r="C168" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Bergvliet</t>
         </is>
       </c>
       <c r="D168" s="3" t="inlineStr">
@@ -5807,7 +5807,7 @@
       </c>
       <c r="B169" s="3" t="inlineStr">
         <is>
-          <t>Frank</t>
+          <t>Vera</t>
         </is>
       </c>
       <c r="C169" s="3" t="inlineStr">
@@ -5822,7 +5822,7 @@
       </c>
       <c r="E169" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F169" s="3" t="inlineStr">
@@ -5834,17 +5834,17 @@
     <row r="170" ht="25" customHeight="1">
       <c r="A170" s="3" t="inlineStr">
         <is>
-          <t>Searle</t>
+          <t>Schatz</t>
         </is>
       </c>
       <c r="B170" s="3" t="inlineStr">
         <is>
-          <t>Francis</t>
+          <t>Frank</t>
         </is>
       </c>
       <c r="C170" s="3" t="inlineStr">
         <is>
-          <t>Kouga</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D170" s="3" t="inlineStr">
@@ -5854,12 +5854,12 @@
       </c>
       <c r="E170" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F170" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -5871,7 +5871,7 @@
       </c>
       <c r="B171" s="3" t="inlineStr">
         <is>
-          <t>Gloria</t>
+          <t>Francis</t>
         </is>
       </c>
       <c r="C171" s="3" t="inlineStr">
@@ -5886,7 +5886,7 @@
       </c>
       <c r="E171" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F171" s="3" t="inlineStr">
@@ -5898,17 +5898,17 @@
     <row r="172" ht="25" customHeight="1">
       <c r="A172" s="3" t="inlineStr">
         <is>
-          <t>Sell</t>
+          <t>Searle</t>
         </is>
       </c>
       <c r="B172" s="3" t="inlineStr">
         <is>
-          <t>Ami</t>
+          <t>Gloria</t>
         </is>
       </c>
       <c r="C172" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Kouga</t>
         </is>
       </c>
       <c r="D172" s="3" t="inlineStr">
@@ -5923,24 +5923,24 @@
       </c>
       <c r="F172" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="173" ht="25" customHeight="1">
       <c r="A173" s="3" t="inlineStr">
         <is>
-          <t>Simpson</t>
+          <t>Sell</t>
         </is>
       </c>
       <c r="B173" s="3" t="inlineStr">
         <is>
-          <t>Beryl</t>
+          <t>Ami</t>
         </is>
       </c>
       <c r="C173" s="3" t="inlineStr">
         <is>
-          <t>Cape Town</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D173" s="3" t="inlineStr">
@@ -5962,17 +5962,17 @@
     <row r="174" ht="25" customHeight="1">
       <c r="A174" s="3" t="inlineStr">
         <is>
-          <t>Sircoulomb</t>
+          <t>Simpson</t>
         </is>
       </c>
       <c r="B174" s="3" t="inlineStr">
         <is>
-          <t>Kenlis</t>
+          <t>Beryl</t>
         </is>
       </c>
       <c r="C174" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Cape Town</t>
         </is>
       </c>
       <c r="D174" s="3" t="inlineStr">
@@ -5999,7 +5999,7 @@
       </c>
       <c r="B175" s="3" t="inlineStr">
         <is>
-          <t>Holger</t>
+          <t>Kenlis</t>
         </is>
       </c>
       <c r="C175" s="3" t="inlineStr">
@@ -6014,7 +6014,7 @@
       </c>
       <c r="E175" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F175" s="3" t="inlineStr">
@@ -6026,12 +6026,12 @@
     <row r="176" ht="25" customHeight="1">
       <c r="A176" s="3" t="inlineStr">
         <is>
-          <t>Smeer</t>
+          <t>Sircoulomb</t>
         </is>
       </c>
       <c r="B176" s="3" t="inlineStr">
         <is>
-          <t>Hennie</t>
+          <t>Holger</t>
         </is>
       </c>
       <c r="C176" s="3" t="inlineStr">
@@ -6041,12 +6041,12 @@
       </c>
       <c r="D176" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E176" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F176" s="3" t="inlineStr">
@@ -6058,22 +6058,22 @@
     <row r="177" ht="25" customHeight="1">
       <c r="A177" s="3" t="inlineStr">
         <is>
-          <t>Smit</t>
+          <t>Smeer</t>
         </is>
       </c>
       <c r="B177" s="3" t="inlineStr">
         <is>
-          <t>Sue</t>
+          <t>Hennie</t>
         </is>
       </c>
       <c r="C177" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D177" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E177" s="3" t="inlineStr">
@@ -6083,7 +6083,7 @@
       </c>
       <c r="F177" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -6095,12 +6095,12 @@
       </c>
       <c r="B178" s="3" t="inlineStr">
         <is>
-          <t>Herman</t>
+          <t>Sue</t>
         </is>
       </c>
       <c r="C178" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D178" s="3" t="inlineStr">
@@ -6115,7 +6115,7 @@
       </c>
       <c r="F178" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -6127,17 +6127,17 @@
       </c>
       <c r="B179" s="3" t="inlineStr">
         <is>
-          <t>Juanita</t>
+          <t>Herman</t>
         </is>
       </c>
       <c r="C179" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D179" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E179" s="3" t="inlineStr">
@@ -6147,29 +6147,29 @@
       </c>
       <c r="F179" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="180" ht="25" customHeight="1">
       <c r="A180" s="3" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Smit</t>
         </is>
       </c>
       <c r="B180" s="3" t="inlineStr">
         <is>
-          <t>Jeff</t>
+          <t>Juanita</t>
         </is>
       </c>
       <c r="C180" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D180" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E180" s="3" t="inlineStr">
@@ -6191,12 +6191,12 @@
       </c>
       <c r="B181" s="3" t="inlineStr">
         <is>
-          <t>Bennie</t>
+          <t>Jeff</t>
         </is>
       </c>
       <c r="C181" s="3" t="inlineStr">
         <is>
-          <t>Wellington</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D181" s="3" t="inlineStr">
@@ -6206,12 +6206,12 @@
       </c>
       <c r="E181" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F181" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -6223,12 +6223,12 @@
       </c>
       <c r="B182" s="3" t="inlineStr">
         <is>
-          <t>Carmen Dolores</t>
+          <t>Bennie</t>
         </is>
       </c>
       <c r="C182" s="3" t="inlineStr">
         <is>
-          <t>Tokai</t>
+          <t>Wellington</t>
         </is>
       </c>
       <c r="D182" s="3" t="inlineStr">
@@ -6238,7 +6238,7 @@
       </c>
       <c r="E182" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F182" s="3" t="inlineStr">
@@ -6255,7 +6255,7 @@
       </c>
       <c r="B183" s="3" t="inlineStr">
         <is>
-          <t>David John</t>
+          <t>Carmen Dolores</t>
         </is>
       </c>
       <c r="C183" s="3" t="inlineStr">
@@ -6282,17 +6282,17 @@
     <row r="184" ht="25" customHeight="1">
       <c r="A184" s="3" t="inlineStr">
         <is>
-          <t>Sochen</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="B184" s="3" t="inlineStr">
         <is>
-          <t>Diana</t>
+          <t>David John</t>
         </is>
       </c>
       <c r="C184" s="3" t="inlineStr">
         <is>
-          <t>Sea Point</t>
+          <t>Tokai</t>
         </is>
       </c>
       <c r="D184" s="3" t="inlineStr">
@@ -6302,7 +6302,7 @@
       </c>
       <c r="E184" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F184" s="3" t="inlineStr">
@@ -6314,49 +6314,49 @@
     <row r="185" ht="25" customHeight="1">
       <c r="A185" s="3" t="inlineStr">
         <is>
-          <t>Steyn</t>
+          <t>Sochen</t>
         </is>
       </c>
       <c r="B185" s="3" t="inlineStr">
         <is>
-          <t>Elna</t>
+          <t>Diana</t>
         </is>
       </c>
       <c r="C185" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Sea Point</t>
         </is>
       </c>
       <c r="D185" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E185" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F185" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="186" ht="25" customHeight="1">
       <c r="A186" s="3" t="inlineStr">
         <is>
-          <t>Strauss</t>
+          <t>Steyn</t>
         </is>
       </c>
       <c r="B186" s="3" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>Elna</t>
         </is>
       </c>
       <c r="C186" s="3" t="inlineStr">
         <is>
-          <t>Kuilsriver</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D186" s="3" t="inlineStr">
@@ -6371,29 +6371,29 @@
       </c>
       <c r="F186" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="187" ht="25" customHeight="1">
       <c r="A187" s="3" t="inlineStr">
         <is>
-          <t>Strydom</t>
+          <t>Strauss</t>
         </is>
       </c>
       <c r="B187" s="3" t="inlineStr">
         <is>
-          <t>Melinda Lee</t>
+          <t>Patrick</t>
         </is>
       </c>
       <c r="C187" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Kuilsriver</t>
         </is>
       </c>
       <c r="D187" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E187" s="3" t="inlineStr">
@@ -6403,24 +6403,24 @@
       </c>
       <c r="F187" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="188" ht="25" customHeight="1">
       <c r="A188" s="3" t="inlineStr">
         <is>
-          <t>Sturges</t>
+          <t>Strydom</t>
         </is>
       </c>
       <c r="B188" s="3" t="inlineStr">
         <is>
-          <t>Trevor</t>
+          <t>Melinda Lee</t>
         </is>
       </c>
       <c r="C188" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D188" s="3" t="inlineStr">
@@ -6442,17 +6442,17 @@
     <row r="189" ht="25" customHeight="1">
       <c r="A189" s="3" t="inlineStr">
         <is>
-          <t>Talbot</t>
+          <t>Sturges</t>
         </is>
       </c>
       <c r="B189" s="3" t="inlineStr">
         <is>
-          <t>Lauryn</t>
+          <t>Trevor</t>
         </is>
       </c>
       <c r="C189" s="3" t="inlineStr">
         <is>
-          <t>Benoni Lakes</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D189" s="3" t="inlineStr">
@@ -6474,17 +6474,17 @@
     <row r="190" ht="25" customHeight="1">
       <c r="A190" s="3" t="inlineStr">
         <is>
-          <t>Theron</t>
+          <t>Talbot</t>
         </is>
       </c>
       <c r="B190" s="3" t="inlineStr">
         <is>
-          <t>Pierre</t>
+          <t>Lauryn</t>
         </is>
       </c>
       <c r="C190" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Benoni Lakes</t>
         </is>
       </c>
       <c r="D190" s="3" t="inlineStr">
@@ -6511,7 +6511,7 @@
       </c>
       <c r="B191" s="3" t="inlineStr">
         <is>
-          <t>Moira</t>
+          <t>Pierre</t>
         </is>
       </c>
       <c r="C191" s="3" t="inlineStr">
@@ -6538,17 +6538,17 @@
     <row r="192" ht="25" customHeight="1">
       <c r="A192" s="3" t="inlineStr">
         <is>
-          <t>Townsend</t>
+          <t>Theron</t>
         </is>
       </c>
       <c r="B192" s="3" t="inlineStr">
         <is>
-          <t>Diane</t>
+          <t>Moira</t>
         </is>
       </c>
       <c r="C192" s="3" t="inlineStr">
         <is>
-          <t>Benoni Lakes</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D192" s="3" t="inlineStr">
@@ -6558,7 +6558,7 @@
       </c>
       <c r="E192" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F192" s="3" t="inlineStr">
@@ -6570,27 +6570,27 @@
     <row r="193" ht="25" customHeight="1">
       <c r="A193" s="3" t="inlineStr">
         <is>
-          <t>Toye</t>
+          <t>Townsend</t>
         </is>
       </c>
       <c r="B193" s="3" t="inlineStr">
         <is>
-          <t>Omolayo</t>
+          <t>Diane</t>
         </is>
       </c>
       <c r="C193" s="3" t="inlineStr">
         <is>
-          <t>The Wilds</t>
+          <t>Benoni Lakes</t>
         </is>
       </c>
       <c r="D193" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E193" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F193" s="3" t="inlineStr">
@@ -6602,22 +6602,22 @@
     <row r="194" ht="25" customHeight="1">
       <c r="A194" s="3" t="inlineStr">
         <is>
-          <t>Tshikala</t>
+          <t>Toye</t>
         </is>
       </c>
       <c r="B194" s="3" t="inlineStr">
         <is>
-          <t>David Alex</t>
+          <t>Omolayo</t>
         </is>
       </c>
       <c r="C194" s="3" t="inlineStr">
         <is>
-          <t>Athlone</t>
+          <t>The Wilds</t>
         </is>
       </c>
       <c r="D194" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E194" s="3" t="inlineStr">
@@ -6627,24 +6627,24 @@
       </c>
       <c r="F194" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="195" ht="25" customHeight="1">
       <c r="A195" s="3" t="inlineStr">
         <is>
-          <t>Tuckett</t>
+          <t>Tshikala</t>
         </is>
       </c>
       <c r="B195" s="3" t="inlineStr">
         <is>
-          <t>Alistair</t>
+          <t>David Alex</t>
         </is>
       </c>
       <c r="C195" s="3" t="inlineStr">
         <is>
-          <t>Roodepoort Clearwater Cyber</t>
+          <t>Athlone</t>
         </is>
       </c>
       <c r="D195" s="3" t="inlineStr">
@@ -6659,7 +6659,7 @@
       </c>
       <c r="F195" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -6671,7 +6671,7 @@
       </c>
       <c r="B196" s="3" t="inlineStr">
         <is>
-          <t>Rowan</t>
+          <t>Alistair</t>
         </is>
       </c>
       <c r="C196" s="3" t="inlineStr">
@@ -6686,7 +6686,7 @@
       </c>
       <c r="E196" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F196" s="3" t="inlineStr">
@@ -6703,7 +6703,7 @@
       </c>
       <c r="B197" s="3" t="inlineStr">
         <is>
-          <t>Gail</t>
+          <t>Rowan</t>
         </is>
       </c>
       <c r="C197" s="3" t="inlineStr">
@@ -6718,7 +6718,7 @@
       </c>
       <c r="E197" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F197" s="3" t="inlineStr">
@@ -6730,17 +6730,17 @@
     <row r="198" ht="25" customHeight="1">
       <c r="A198" s="3" t="inlineStr">
         <is>
-          <t>VAN BREDA</t>
+          <t>Tuckett</t>
         </is>
       </c>
       <c r="B198" s="3" t="inlineStr">
         <is>
-          <t>HILARY LISE</t>
+          <t>Gail</t>
         </is>
       </c>
       <c r="C198" s="3" t="inlineStr">
         <is>
-          <t>Cape Town</t>
+          <t>Roodepoort Clearwater Cyber</t>
         </is>
       </c>
       <c r="D198" s="3" t="inlineStr">
@@ -6755,39 +6755,39 @@
       </c>
       <c r="F198" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="199" ht="25" customHeight="1">
       <c r="A199" s="3" t="inlineStr">
         <is>
-          <t>VAN DER MERWE</t>
+          <t>VAN BREDA</t>
         </is>
       </c>
       <c r="B199" s="3" t="inlineStr">
         <is>
-          <t>PATRICIA</t>
+          <t>HILARY LISE</t>
         </is>
       </c>
       <c r="C199" s="3" t="inlineStr">
         <is>
-          <t>East London Port Rex</t>
+          <t>Cape Town</t>
         </is>
       </c>
       <c r="D199" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E199" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F199" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -6799,17 +6799,17 @@
       </c>
       <c r="B200" s="3" t="inlineStr">
         <is>
-          <t>MARINA</t>
+          <t>PATRICIA</t>
         </is>
       </c>
       <c r="C200" s="3" t="inlineStr">
         <is>
-          <t>Malmesbury</t>
+          <t>East London Port Rex</t>
         </is>
       </c>
       <c r="D200" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E200" s="3" t="inlineStr">
@@ -6819,56 +6819,56 @@
       </c>
       <c r="F200" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="201" ht="25" customHeight="1">
       <c r="A201" s="3" t="inlineStr">
         <is>
-          <t>Valadao</t>
+          <t>VAN DER MERWE</t>
         </is>
       </c>
       <c r="B201" s="3" t="inlineStr">
         <is>
-          <t>Tracy</t>
+          <t>MARINA</t>
         </is>
       </c>
       <c r="C201" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Malmesbury</t>
         </is>
       </c>
       <c r="D201" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E201" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F201" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="202" ht="25" customHeight="1">
       <c r="A202" s="3" t="inlineStr">
         <is>
-          <t>Van Niekerk</t>
+          <t>Valadao</t>
         </is>
       </c>
       <c r="B202" s="3" t="inlineStr">
         <is>
-          <t>Riaan</t>
+          <t>Tracy</t>
         </is>
       </c>
       <c r="C202" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D202" s="3" t="inlineStr">
@@ -6890,22 +6890,22 @@
     <row r="203" ht="25" customHeight="1">
       <c r="A203" s="3" t="inlineStr">
         <is>
-          <t>Van Nieuwenhuyzen</t>
+          <t>Van Niekerk</t>
         </is>
       </c>
       <c r="B203" s="3" t="inlineStr">
         <is>
-          <t>Hilgardt</t>
+          <t>Riaan</t>
         </is>
       </c>
       <c r="C203" s="3" t="inlineStr">
         <is>
-          <t>Worcester</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D203" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E203" s="3" t="inlineStr">
@@ -6915,24 +6915,24 @@
       </c>
       <c r="F203" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="204" ht="25" customHeight="1">
       <c r="A204" s="3" t="inlineStr">
         <is>
-          <t>Van Rensburg</t>
+          <t>Van Nieuwenhuyzen</t>
         </is>
       </c>
       <c r="B204" s="3" t="inlineStr">
         <is>
-          <t>Neville</t>
+          <t>Hilgardt</t>
         </is>
       </c>
       <c r="C204" s="3" t="inlineStr">
         <is>
-          <t>Moorreesburg</t>
+          <t>Worcester</t>
         </is>
       </c>
       <c r="D204" s="3" t="inlineStr">
@@ -6942,7 +6942,7 @@
       </c>
       <c r="E204" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F204" s="3" t="inlineStr">
@@ -6954,27 +6954,27 @@
     <row r="205" ht="25" customHeight="1">
       <c r="A205" s="3" t="inlineStr">
         <is>
-          <t>Van Romburgh</t>
+          <t>Van Rensburg</t>
         </is>
       </c>
       <c r="B205" s="3" t="inlineStr">
         <is>
-          <t>Lorna</t>
+          <t>Neville</t>
         </is>
       </c>
       <c r="C205" s="3" t="inlineStr">
         <is>
-          <t>Fish Hoek</t>
+          <t>Moorreesburg</t>
         </is>
       </c>
       <c r="D205" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E205" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F205" s="3" t="inlineStr">
@@ -6986,17 +6986,17 @@
     <row r="206" ht="25" customHeight="1">
       <c r="A206" s="3" t="inlineStr">
         <is>
-          <t>Van Wyk-Nelson</t>
+          <t>Van Romburgh</t>
         </is>
       </c>
       <c r="B206" s="3" t="inlineStr">
         <is>
-          <t>Edith</t>
+          <t>Lorna</t>
         </is>
       </c>
       <c r="C206" s="3" t="inlineStr">
         <is>
-          <t>Kuilsriver</t>
+          <t>Fish Hoek</t>
         </is>
       </c>
       <c r="D206" s="3" t="inlineStr">
@@ -7018,17 +7018,17 @@
     <row r="207" ht="25" customHeight="1">
       <c r="A207" s="3" t="inlineStr">
         <is>
-          <t>Van Zyl</t>
+          <t>Van Wyk-Nelson</t>
         </is>
       </c>
       <c r="B207" s="3" t="inlineStr">
         <is>
-          <t>Louis</t>
+          <t>Edith</t>
         </is>
       </c>
       <c r="C207" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Kuilsriver</t>
         </is>
       </c>
       <c r="D207" s="3" t="inlineStr">
@@ -7043,29 +7043,29 @@
       </c>
       <c r="F207" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="208" ht="25" customHeight="1">
       <c r="A208" s="3" t="inlineStr">
         <is>
-          <t>Van de Merwe</t>
+          <t>Van Zyl</t>
         </is>
       </c>
       <c r="B208" s="3" t="inlineStr">
         <is>
-          <t>Marina</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="C208" s="3" t="inlineStr">
         <is>
-          <t>Malmesbury</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D208" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E208" s="3" t="inlineStr">
@@ -7075,29 +7075,29 @@
       </c>
       <c r="F208" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="209" ht="25" customHeight="1">
       <c r="A209" s="3" t="inlineStr">
         <is>
-          <t>Venter</t>
+          <t>Van de Merwe</t>
         </is>
       </c>
       <c r="B209" s="3" t="inlineStr">
         <is>
-          <t>Louis</t>
+          <t>Marina</t>
         </is>
       </c>
       <c r="C209" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Malmesbury</t>
         </is>
       </c>
       <c r="D209" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E209" s="3" t="inlineStr">
@@ -7107,34 +7107,34 @@
       </c>
       <c r="F209" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="210" ht="25" customHeight="1">
       <c r="A210" s="3" t="inlineStr">
         <is>
-          <t>Volker</t>
+          <t>Venter</t>
         </is>
       </c>
       <c r="B210" s="3" t="inlineStr">
         <is>
-          <t>Russell</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="C210" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D210" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E210" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F210" s="3" t="inlineStr">
@@ -7146,96 +7146,96 @@
     <row r="211" ht="25" customHeight="1">
       <c r="A211" s="3" t="inlineStr">
         <is>
-          <t>Von Mollendorf</t>
+          <t>Volker</t>
         </is>
       </c>
       <c r="B211" s="3" t="inlineStr">
         <is>
-          <t>Rinette</t>
+          <t>Russell</t>
         </is>
       </c>
       <c r="C211" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>King William's Town</t>
         </is>
       </c>
       <c r="D211" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E211" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F211" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="212" ht="25" customHeight="1">
       <c r="A212" s="3" t="inlineStr">
         <is>
-          <t>Warman</t>
+          <t>Von Mollendorf</t>
         </is>
       </c>
       <c r="B212" s="3" t="inlineStr">
         <is>
-          <t>Alastair</t>
+          <t>Rinette</t>
         </is>
       </c>
       <c r="C212" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Durbanville</t>
         </is>
       </c>
       <c r="D212" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E212" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F212" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="213" ht="25" customHeight="1">
       <c r="A213" s="3" t="inlineStr">
         <is>
-          <t>Watson</t>
+          <t>Warman</t>
         </is>
       </c>
       <c r="B213" s="3" t="inlineStr">
         <is>
-          <t>Allan</t>
+          <t>Alastair</t>
         </is>
       </c>
       <c r="C213" s="3" t="inlineStr">
         <is>
-          <t>Sea Point</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D213" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E213" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F213" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -7247,22 +7247,22 @@
       </c>
       <c r="B214" s="3" t="inlineStr">
         <is>
-          <t>Alison</t>
+          <t>Allan</t>
         </is>
       </c>
       <c r="C214" s="3" t="inlineStr">
         <is>
-          <t>Sedgefield</t>
+          <t>Sea Point</t>
         </is>
       </c>
       <c r="D214" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E214" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F214" s="3" t="inlineStr">
@@ -7274,27 +7274,27 @@
     <row r="215" ht="25" customHeight="1">
       <c r="A215" s="3" t="inlineStr">
         <is>
-          <t>Williams</t>
+          <t>Watson</t>
         </is>
       </c>
       <c r="B215" s="3" t="inlineStr">
         <is>
-          <t>Johanna</t>
+          <t>Alison</t>
         </is>
       </c>
       <c r="C215" s="3" t="inlineStr">
         <is>
-          <t>Mitchells Plain</t>
+          <t>Sedgefield</t>
         </is>
       </c>
       <c r="D215" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E215" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F215" s="3" t="inlineStr">
@@ -7306,22 +7306,22 @@
     <row r="216" ht="25" customHeight="1">
       <c r="A216" s="3" t="inlineStr">
         <is>
-          <t>Wills</t>
+          <t>Williams</t>
         </is>
       </c>
       <c r="B216" s="3" t="inlineStr">
         <is>
-          <t>Geila</t>
+          <t>Johanna</t>
         </is>
       </c>
       <c r="C216" s="3" t="inlineStr">
         <is>
-          <t>Athlone</t>
+          <t>Mitchells Plain</t>
         </is>
       </c>
       <c r="D216" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E216" s="3" t="inlineStr">
@@ -7338,17 +7338,17 @@
     <row r="217" ht="25" customHeight="1">
       <c r="A217" s="3" t="inlineStr">
         <is>
-          <t>Wilter-Sturges</t>
+          <t>Wills</t>
         </is>
       </c>
       <c r="B217" s="3" t="inlineStr">
         <is>
-          <t>Meredith</t>
+          <t>Geila</t>
         </is>
       </c>
       <c r="C217" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Athlone</t>
         </is>
       </c>
       <c r="D217" s="3" t="inlineStr">
@@ -7363,24 +7363,24 @@
       </c>
       <c r="F217" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="218" ht="25" customHeight="1">
       <c r="A218" s="3" t="inlineStr">
         <is>
-          <t>Wright</t>
+          <t>Wilter-Sturges</t>
         </is>
       </c>
       <c r="B218" s="3" t="inlineStr">
         <is>
-          <t>Rocky</t>
+          <t>Meredith</t>
         </is>
       </c>
       <c r="C218" s="3" t="inlineStr">
         <is>
-          <t>Table View</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D218" s="3" t="inlineStr">
@@ -7390,29 +7390,29 @@
       </c>
       <c r="E218" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F218" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="219" ht="25" customHeight="1">
       <c r="A219" s="3" t="inlineStr">
         <is>
-          <t>Young</t>
+          <t>Wright</t>
         </is>
       </c>
       <c r="B219" s="3" t="inlineStr">
         <is>
-          <t>Judy</t>
+          <t>Rocky</t>
         </is>
       </c>
       <c r="C219" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>Table View</t>
         </is>
       </c>
       <c r="D219" s="3" t="inlineStr">
@@ -7422,7 +7422,7 @@
       </c>
       <c r="E219" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F219" s="3" t="inlineStr">
@@ -7434,17 +7434,17 @@
     <row r="220" ht="25" customHeight="1">
       <c r="A220" s="3" t="inlineStr">
         <is>
-          <t>de Kock</t>
+          <t>Young</t>
         </is>
       </c>
       <c r="B220" s="3" t="inlineStr">
         <is>
-          <t>Engela</t>
+          <t>Judy</t>
         </is>
       </c>
       <c r="C220" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Durbanville</t>
         </is>
       </c>
       <c r="D220" s="3" t="inlineStr">
@@ -7454,7 +7454,7 @@
       </c>
       <c r="E220" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F220" s="3" t="inlineStr">
@@ -7471,7 +7471,7 @@
       </c>
       <c r="B221" s="3" t="inlineStr">
         <is>
-          <t>Francois</t>
+          <t>Engela</t>
         </is>
       </c>
       <c r="C221" s="3" t="inlineStr">
@@ -7498,59 +7498,59 @@
     <row r="222" ht="25" customHeight="1">
       <c r="A222" s="3" t="inlineStr">
         <is>
-          <t>de Silva</t>
+          <t>de Kock</t>
         </is>
       </c>
       <c r="B222" s="3" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Francois</t>
         </is>
       </c>
       <c r="C222" s="3" t="inlineStr">
         <is>
-          <t>Edenvale</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D222" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E222" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F222" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="223" ht="25" customHeight="1">
       <c r="A223" s="3" t="inlineStr">
         <is>
-          <t>du Plooy</t>
+          <t>de Silva</t>
         </is>
       </c>
       <c r="B223" s="3" t="inlineStr">
         <is>
-          <t>Tammy</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="C223" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Edenvale</t>
         </is>
       </c>
       <c r="D223" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E223" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F223" s="3" t="inlineStr">
@@ -7567,7 +7567,7 @@
       </c>
       <c r="B224" s="3" t="inlineStr">
         <is>
-          <t>Marc</t>
+          <t>Tammy</t>
         </is>
       </c>
       <c r="C224" s="3" t="inlineStr">
@@ -7594,17 +7594,17 @@
     <row r="225" ht="25" customHeight="1">
       <c r="A225" s="3" t="inlineStr">
         <is>
-          <t>du Toit</t>
+          <t>du Plooy</t>
         </is>
       </c>
       <c r="B225" s="3" t="inlineStr">
         <is>
-          <t>Desiree</t>
+          <t>Marc</t>
         </is>
       </c>
       <c r="C225" s="3" t="inlineStr">
         <is>
-          <t>Ramsgate</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D225" s="3" t="inlineStr">
@@ -7626,22 +7626,22 @@
     <row r="226" ht="25" customHeight="1">
       <c r="A226" s="3" t="inlineStr">
         <is>
-          <t>stier</t>
+          <t>du Toit</t>
         </is>
       </c>
       <c r="B226" s="3" t="inlineStr">
         <is>
-          <t>RORY</t>
+          <t>Desiree</t>
         </is>
       </c>
       <c r="C226" s="3" t="inlineStr">
         <is>
-          <t>Deep South</t>
+          <t>Ramsgate</t>
         </is>
       </c>
       <c r="D226" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E226" s="3" t="inlineStr">
@@ -7651,56 +7651,56 @@
       </c>
       <c r="F226" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="227" ht="25" customHeight="1">
       <c r="A227" s="3" t="inlineStr">
         <is>
-          <t>tyler</t>
+          <t>stier</t>
         </is>
       </c>
       <c r="B227" s="3" t="inlineStr">
         <is>
-          <t>natascha</t>
+          <t>RORY</t>
         </is>
       </c>
       <c r="C227" s="3" t="inlineStr">
         <is>
-          <t>Kensington</t>
+          <t>Deep South</t>
         </is>
       </c>
       <c r="D227" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E227" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F227" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="228" ht="25" customHeight="1">
       <c r="A228" s="3" t="inlineStr">
         <is>
-          <t>van Blerk</t>
+          <t>tyler</t>
         </is>
       </c>
       <c r="B228" s="3" t="inlineStr">
         <is>
-          <t>Carl</t>
+          <t>natascha</t>
         </is>
       </c>
       <c r="C228" s="3" t="inlineStr">
         <is>
-          <t>Eden</t>
+          <t>Kensington</t>
         </is>
       </c>
       <c r="D228" s="3" t="inlineStr">
@@ -7715,24 +7715,24 @@
       </c>
       <c r="F228" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="229" ht="25" customHeight="1">
       <c r="A229" s="3" t="inlineStr">
         <is>
-          <t>van Heerden</t>
+          <t>van Blerk</t>
         </is>
       </c>
       <c r="B229" s="3" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Carl</t>
         </is>
       </c>
       <c r="C229" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Eden</t>
         </is>
       </c>
       <c r="D229" s="3" t="inlineStr">
@@ -7747,7 +7747,7 @@
       </c>
       <c r="F229" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -7759,7 +7759,7 @@
       </c>
       <c r="B230" s="3" t="inlineStr">
         <is>
-          <t>Sandy</t>
+          <t>Sydney</t>
         </is>
       </c>
       <c r="C230" s="3" t="inlineStr">
@@ -7774,7 +7774,7 @@
       </c>
       <c r="E230" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F230" s="3" t="inlineStr">
@@ -7791,17 +7791,17 @@
       </c>
       <c r="B231" s="3" t="inlineStr">
         <is>
-          <t>Craig</t>
+          <t>Sandy</t>
         </is>
       </c>
       <c r="C231" s="3" t="inlineStr">
         <is>
-          <t>East London Beacon Bay</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D231" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E231" s="3" t="inlineStr">
@@ -7823,17 +7823,17 @@
       </c>
       <c r="B232" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Craig</t>
         </is>
       </c>
       <c r="C232" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>East London Beacon Bay</t>
         </is>
       </c>
       <c r="D232" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E232" s="3" t="inlineStr">
@@ -7850,17 +7850,17 @@
     <row r="233" ht="25" customHeight="1">
       <c r="A233" s="3" t="inlineStr">
         <is>
-          <t>van Rensburg</t>
+          <t>van Heerden</t>
         </is>
       </c>
       <c r="B233" s="3" t="inlineStr">
         <is>
-          <t>Johan</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C233" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D233" s="3" t="inlineStr">
@@ -7870,12 +7870,12 @@
       </c>
       <c r="E233" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F233" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -7887,7 +7887,7 @@
       </c>
       <c r="B234" s="3" t="inlineStr">
         <is>
-          <t>Anne</t>
+          <t>Johan</t>
         </is>
       </c>
       <c r="C234" s="3" t="inlineStr">
@@ -7914,17 +7914,17 @@
     <row r="235" ht="25" customHeight="1">
       <c r="A235" s="3" t="inlineStr">
         <is>
-          <t>van Wulven</t>
+          <t>van Rensburg</t>
         </is>
       </c>
       <c r="B235" s="3" t="inlineStr">
         <is>
-          <t>Jeannie</t>
+          <t>Anne</t>
         </is>
       </c>
       <c r="C235" s="3" t="inlineStr">
         <is>
-          <t>Tygerberg Hills</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D235" s="3" t="inlineStr">
@@ -7951,7 +7951,7 @@
       </c>
       <c r="B236" s="3" t="inlineStr">
         <is>
-          <t>Alan</t>
+          <t>Jeannie</t>
         </is>
       </c>
       <c r="C236" s="3" t="inlineStr">
@@ -7983,7 +7983,7 @@
       </c>
       <c r="B237" s="3" t="inlineStr">
         <is>
-          <t>Deon</t>
+          <t>Alan</t>
         </is>
       </c>
       <c r="C237" s="3" t="inlineStr">
@@ -8010,17 +8010,17 @@
     <row r="238" ht="25" customHeight="1">
       <c r="A238" s="3" t="inlineStr">
         <is>
-          <t>van Wyk</t>
+          <t>van Wulven</t>
         </is>
       </c>
       <c r="B238" s="3" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>Deon</t>
         </is>
       </c>
       <c r="C238" s="3" t="inlineStr">
         <is>
-          <t>North Durban</t>
+          <t>Tygerberg Hills</t>
         </is>
       </c>
       <c r="D238" s="3" t="inlineStr">
@@ -8035,7 +8035,7 @@
       </c>
       <c r="F238" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -8047,12 +8047,12 @@
       </c>
       <c r="B239" s="3" t="inlineStr">
         <is>
-          <t>Lindie</t>
+          <t>Kim</t>
         </is>
       </c>
       <c r="C239" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>North Durban</t>
         </is>
       </c>
       <c r="D239" s="3" t="inlineStr">
@@ -8079,12 +8079,12 @@
       </c>
       <c r="B240" s="3" t="inlineStr">
         <is>
-          <t>Willem</t>
+          <t>Lindie</t>
         </is>
       </c>
       <c r="C240" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D240" s="3" t="inlineStr">
@@ -8111,12 +8111,12 @@
       </c>
       <c r="B241" s="3" t="inlineStr">
         <is>
-          <t>Patricia</t>
+          <t>Willem</t>
         </is>
       </c>
       <c r="C241" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D241" s="3" t="inlineStr">
@@ -8138,22 +8138,22 @@
     <row r="242" ht="25" customHeight="1">
       <c r="A242" s="3" t="inlineStr">
         <is>
-          <t>van der Merwe</t>
+          <t>van Wyk</t>
         </is>
       </c>
       <c r="B242" s="3" t="inlineStr">
         <is>
-          <t>Ingrid</t>
+          <t>Patricia</t>
         </is>
       </c>
       <c r="C242" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D242" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E242" s="3" t="inlineStr">
@@ -8170,49 +8170,49 @@
     <row r="243" ht="25" customHeight="1">
       <c r="A243" s="3" t="inlineStr">
         <is>
-          <t>van der Westhuizen</t>
+          <t>van der Merwe</t>
         </is>
       </c>
       <c r="B243" s="3" t="inlineStr">
         <is>
-          <t>Hennie</t>
+          <t>Ingrid</t>
         </is>
       </c>
       <c r="C243" s="3" t="inlineStr">
         <is>
-          <t>Helderberg</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D243" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E243" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F243" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="244" ht="25" customHeight="1">
       <c r="A244" s="3" t="inlineStr">
         <is>
-          <t>von der Decken</t>
+          <t>van der Westhuizen</t>
         </is>
       </c>
       <c r="B244" s="3" t="inlineStr">
         <is>
-          <t>Brian</t>
+          <t>Hennie</t>
         </is>
       </c>
       <c r="C244" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Helderberg</t>
         </is>
       </c>
       <c r="D244" s="3" t="inlineStr">
@@ -8227,51 +8227,83 @@
       </c>
       <c r="F244" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="245" ht="25" customHeight="1">
       <c r="A245" s="3" t="inlineStr">
         <is>
+          <t>von der Decken</t>
+        </is>
+      </c>
+      <c r="B245" s="3" t="inlineStr">
+        <is>
+          <t>Brian</t>
+        </is>
+      </c>
+      <c r="C245" s="3" t="inlineStr">
+        <is>
+          <t>King William's Town</t>
+        </is>
+      </c>
+      <c r="D245" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E245" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F245" s="3" t="inlineStr">
+        <is>
+          <t>410E</t>
+        </is>
+      </c>
+    </row>
+    <row r="246" ht="25" customHeight="1">
+      <c r="A246" s="3" t="inlineStr">
+        <is>
           <t>‘t Hart</t>
         </is>
       </c>
-      <c r="B245" s="3" t="inlineStr">
+      <c r="B246" s="3" t="inlineStr">
         <is>
           <t>Michelle</t>
         </is>
       </c>
-      <c r="C245" s="3" t="inlineStr">
+      <c r="C246" s="3" t="inlineStr">
         <is>
           <t>Benoni Lakes</t>
         </is>
       </c>
-      <c r="D245" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E245" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F245" s="3" t="inlineStr">
+      <c r="D246" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E246" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F246" s="3" t="inlineStr">
         <is>
           <t>410E</t>
-        </is>
-      </c>
-    </row>
-    <row r="246">
-      <c r="A246" s="1" t="inlineStr">
-        <is>
-          <t>Number of attendees: 243</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="inlineStr">
+        <is>
+          <t>Number of attendees: 244</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" s="1" t="inlineStr">
         <is>
           <t>Number of voters: 98</t>
         </is>
@@ -8307,7 +8339,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Registrees as of 28/04/2021 13:30</t>
+          <t>410E Registrees as of 28/04/2021 16:40</t>
         </is>
       </c>
     </row>
@@ -11892,7 +11924,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Registrees as of 28/04/2021 13:30</t>
+          <t>410W Registrees as of 28/04/2021 16:40</t>
         </is>
       </c>
     </row>
@@ -16068,7 +16100,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Voting details as of 28/04/2021 13:30</t>
+          <t>410E Voting details as of 28/04/2021 16:40</t>
         </is>
       </c>
     </row>
@@ -16445,7 +16477,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Voting details as of 28/04/2021 13:30</t>
+          <t>410W Voting details as of 28/04/2021 16:40</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Registree stats backup on Thu 29 Apr 2021 09:02:29 SAST
</commit_message>
<xml_diff>
--- a/static/docs/registrees_list.xlsx
+++ b/static/docs/registrees_list.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F248"/>
+  <dimension ref="A1:F249"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,7 +451,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>MD410 Registrees as of 28/04/2021 16:40</t>
+          <t>MD410 Registrees as of 29/04/2021 09:02</t>
         </is>
       </c>
     </row>
@@ -1502,7 +1502,7 @@
       </c>
       <c r="E34" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F34" s="3" t="inlineStr">
@@ -4030,7 +4030,7 @@
       </c>
       <c r="E113" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F113" s="3" t="inlineStr">
@@ -4874,17 +4874,17 @@
     <row r="140" ht="25" customHeight="1">
       <c r="A140" s="3" t="inlineStr">
         <is>
-          <t>Nel</t>
+          <t>Naude</t>
         </is>
       </c>
       <c r="B140" s="3" t="inlineStr">
         <is>
-          <t>Pieter</t>
+          <t>Nici</t>
         </is>
       </c>
       <c r="C140" s="3" t="inlineStr">
         <is>
-          <t>George</t>
+          <t>King William's Town</t>
         </is>
       </c>
       <c r="D140" s="3" t="inlineStr">
@@ -4894,12 +4894,12 @@
       </c>
       <c r="E140" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F140" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -4911,12 +4911,12 @@
       </c>
       <c r="B141" s="3" t="inlineStr">
         <is>
-          <t>Tillie</t>
+          <t>Pieter</t>
         </is>
       </c>
       <c r="C141" s="3" t="inlineStr">
         <is>
-          <t>Eden</t>
+          <t>George</t>
         </is>
       </c>
       <c r="D141" s="3" t="inlineStr">
@@ -4938,17 +4938,17 @@
     <row r="142" ht="25" customHeight="1">
       <c r="A142" s="3" t="inlineStr">
         <is>
-          <t>Newlands</t>
+          <t>Nel</t>
         </is>
       </c>
       <c r="B142" s="3" t="inlineStr">
         <is>
-          <t>Mike</t>
+          <t>Tillie</t>
         </is>
       </c>
       <c r="C142" s="3" t="inlineStr">
         <is>
-          <t>Port Alfred</t>
+          <t>Eden</t>
         </is>
       </c>
       <c r="D142" s="3" t="inlineStr">
@@ -4963,24 +4963,24 @@
       </c>
       <c r="F142" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="143" ht="25" customHeight="1">
       <c r="A143" s="3" t="inlineStr">
         <is>
-          <t>Ngobozana</t>
+          <t>Newlands</t>
         </is>
       </c>
       <c r="B143" s="3" t="inlineStr">
         <is>
-          <t>Sphiwe</t>
+          <t>Mike</t>
         </is>
       </c>
       <c r="C143" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Port Alfred</t>
         </is>
       </c>
       <c r="D143" s="3" t="inlineStr">
@@ -4990,7 +4990,7 @@
       </c>
       <c r="E143" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F143" s="3" t="inlineStr">
@@ -5002,17 +5002,17 @@
     <row r="144" ht="25" customHeight="1">
       <c r="A144" s="3" t="inlineStr">
         <is>
-          <t>Niehaus</t>
+          <t>Ngobozana</t>
         </is>
       </c>
       <c r="B144" s="3" t="inlineStr">
         <is>
-          <t>Angela</t>
+          <t>Sphiwe</t>
         </is>
       </c>
       <c r="C144" s="3" t="inlineStr">
         <is>
-          <t>Bergvliet</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D144" s="3" t="inlineStr">
@@ -5022,29 +5022,29 @@
       </c>
       <c r="E144" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F144" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="145" ht="25" customHeight="1">
       <c r="A145" s="3" t="inlineStr">
         <is>
-          <t>Oberholzer</t>
+          <t>Niehaus</t>
         </is>
       </c>
       <c r="B145" s="3" t="inlineStr">
         <is>
-          <t>PDG Bokkie</t>
+          <t>Angela</t>
         </is>
       </c>
       <c r="C145" s="3" t="inlineStr">
         <is>
-          <t>Uitenhage</t>
+          <t>Bergvliet</t>
         </is>
       </c>
       <c r="D145" s="3" t="inlineStr">
@@ -5054,29 +5054,29 @@
       </c>
       <c r="E145" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F145" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="146" ht="25" customHeight="1">
       <c r="A146" s="3" t="inlineStr">
         <is>
-          <t>PORTEOUS</t>
+          <t>Oberholzer</t>
         </is>
       </c>
       <c r="B146" s="3" t="inlineStr">
         <is>
-          <t>BRIAN</t>
+          <t>PDG Bokkie</t>
         </is>
       </c>
       <c r="C146" s="3" t="inlineStr">
         <is>
-          <t>Hibberdene</t>
+          <t>Uitenhage</t>
         </is>
       </c>
       <c r="D146" s="3" t="inlineStr">
@@ -5086,7 +5086,7 @@
       </c>
       <c r="E146" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F146" s="3" t="inlineStr">
@@ -5098,17 +5098,17 @@
     <row r="147" ht="25" customHeight="1">
       <c r="A147" s="3" t="inlineStr">
         <is>
-          <t>Paijmans</t>
+          <t>PORTEOUS</t>
         </is>
       </c>
       <c r="B147" s="3" t="inlineStr">
         <is>
-          <t>Bronwyn Anne</t>
+          <t>BRIAN</t>
         </is>
       </c>
       <c r="C147" s="3" t="inlineStr">
         <is>
-          <t>Cowies Hill</t>
+          <t>Hibberdene</t>
         </is>
       </c>
       <c r="D147" s="3" t="inlineStr">
@@ -5118,7 +5118,7 @@
       </c>
       <c r="E147" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F147" s="3" t="inlineStr">
@@ -5130,17 +5130,17 @@
     <row r="148" ht="25" customHeight="1">
       <c r="A148" s="3" t="inlineStr">
         <is>
-          <t>Pantoleon</t>
+          <t>Paijmans</t>
         </is>
       </c>
       <c r="B148" s="3" t="inlineStr">
         <is>
-          <t>Teresa</t>
+          <t>Bronwyn Anne</t>
         </is>
       </c>
       <c r="C148" s="3" t="inlineStr">
         <is>
-          <t>Vereeniging</t>
+          <t>Cowies Hill</t>
         </is>
       </c>
       <c r="D148" s="3" t="inlineStr">
@@ -5150,7 +5150,7 @@
       </c>
       <c r="E148" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F148" s="3" t="inlineStr">
@@ -5162,17 +5162,17 @@
     <row r="149" ht="25" customHeight="1">
       <c r="A149" s="3" t="inlineStr">
         <is>
-          <t>Peters</t>
+          <t>Pantoleon</t>
         </is>
       </c>
       <c r="B149" s="3" t="inlineStr">
         <is>
-          <t>Maureen</t>
+          <t>Teresa</t>
         </is>
       </c>
       <c r="C149" s="3" t="inlineStr">
         <is>
-          <t>Ceres</t>
+          <t>Vereeniging</t>
         </is>
       </c>
       <c r="D149" s="3" t="inlineStr">
@@ -5187,24 +5187,24 @@
       </c>
       <c r="F149" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="150" ht="25" customHeight="1">
       <c r="A150" s="3" t="inlineStr">
         <is>
-          <t>Pillay</t>
+          <t>Peters</t>
         </is>
       </c>
       <c r="B150" s="3" t="inlineStr">
         <is>
-          <t>Sundru</t>
+          <t>Maureen</t>
         </is>
       </c>
       <c r="C150" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>Ceres</t>
         </is>
       </c>
       <c r="D150" s="3" t="inlineStr">
@@ -5214,7 +5214,7 @@
       </c>
       <c r="E150" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F150" s="3" t="inlineStr">
@@ -5231,12 +5231,12 @@
       </c>
       <c r="B151" s="3" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>Sundru</t>
         </is>
       </c>
       <c r="C151" s="3" t="inlineStr">
         <is>
-          <t>Tygerberg Hills</t>
+          <t>Durbanville</t>
         </is>
       </c>
       <c r="D151" s="3" t="inlineStr">
@@ -5246,7 +5246,7 @@
       </c>
       <c r="E151" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F151" s="3" t="inlineStr">
@@ -5258,17 +5258,17 @@
     <row r="152" ht="25" customHeight="1">
       <c r="A152" s="3" t="inlineStr">
         <is>
-          <t>Polkinghorne</t>
+          <t>Pillay</t>
         </is>
       </c>
       <c r="B152" s="3" t="inlineStr">
         <is>
-          <t>Tracey</t>
+          <t>Patrick</t>
         </is>
       </c>
       <c r="C152" s="3" t="inlineStr">
         <is>
-          <t>Kensington</t>
+          <t>Tygerberg Hills</t>
         </is>
       </c>
       <c r="D152" s="3" t="inlineStr">
@@ -5278,12 +5278,12 @@
       </c>
       <c r="E152" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F152" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -5295,7 +5295,7 @@
       </c>
       <c r="B153" s="3" t="inlineStr">
         <is>
-          <t>Gavin</t>
+          <t>Tracey</t>
         </is>
       </c>
       <c r="C153" s="3" t="inlineStr">
@@ -5310,7 +5310,7 @@
       </c>
       <c r="E153" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F153" s="3" t="inlineStr">
@@ -5322,22 +5322,22 @@
     <row r="154" ht="25" customHeight="1">
       <c r="A154" s="3" t="inlineStr">
         <is>
-          <t>Pretorius</t>
+          <t>Polkinghorne</t>
         </is>
       </c>
       <c r="B154" s="3" t="inlineStr">
         <is>
-          <t>Sheldon Edmund</t>
+          <t>Gavin</t>
         </is>
       </c>
       <c r="C154" s="3" t="inlineStr">
         <is>
-          <t>Merriman</t>
+          <t>Kensington</t>
         </is>
       </c>
       <c r="D154" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E154" s="3" t="inlineStr">
@@ -5347,29 +5347,29 @@
       </c>
       <c r="F154" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="155" ht="25" customHeight="1">
       <c r="A155" s="3" t="inlineStr">
         <is>
-          <t>Ras</t>
+          <t>Pretorius</t>
         </is>
       </c>
       <c r="B155" s="3" t="inlineStr">
         <is>
-          <t>Mary-Anne</t>
+          <t>Sheldon Edmund</t>
         </is>
       </c>
       <c r="C155" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Merriman</t>
         </is>
       </c>
       <c r="D155" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E155" s="3" t="inlineStr">
@@ -5391,7 +5391,7 @@
       </c>
       <c r="B156" s="3" t="inlineStr">
         <is>
-          <t>Leon Jacobus</t>
+          <t>Mary-Anne</t>
         </is>
       </c>
       <c r="C156" s="3" t="inlineStr">
@@ -5418,22 +5418,22 @@
     <row r="157" ht="25" customHeight="1">
       <c r="A157" s="3" t="inlineStr">
         <is>
-          <t>Rashirai</t>
+          <t>Ras</t>
         </is>
       </c>
       <c r="B157" s="3" t="inlineStr">
         <is>
-          <t>Tabeth</t>
+          <t>Leon Jacobus</t>
         </is>
       </c>
       <c r="C157" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D157" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E157" s="3" t="inlineStr">
@@ -5443,29 +5443,29 @@
       </c>
       <c r="F157" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="158" ht="25" customHeight="1">
       <c r="A158" s="3" t="inlineStr">
         <is>
-          <t>Rathbone Smyth</t>
+          <t>Rashirai</t>
         </is>
       </c>
       <c r="B158" s="3" t="inlineStr">
         <is>
-          <t>Janine</t>
+          <t>Tabeth</t>
         </is>
       </c>
       <c r="C158" s="3" t="inlineStr">
         <is>
-          <t>Vereeniging</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D158" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E158" s="3" t="inlineStr">
@@ -5482,17 +5482,17 @@
     <row r="159" ht="25" customHeight="1">
       <c r="A159" s="3" t="inlineStr">
         <is>
-          <t>Reniers</t>
+          <t>Rathbone Smyth</t>
         </is>
       </c>
       <c r="B159" s="3" t="inlineStr">
         <is>
-          <t>Hugo</t>
+          <t>Janine</t>
         </is>
       </c>
       <c r="C159" s="3" t="inlineStr">
         <is>
-          <t>Nelspruit</t>
+          <t>Vereeniging</t>
         </is>
       </c>
       <c r="D159" s="3" t="inlineStr">
@@ -5502,7 +5502,7 @@
       </c>
       <c r="E159" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F159" s="3" t="inlineStr">
@@ -5514,17 +5514,17 @@
     <row r="160" ht="25" customHeight="1">
       <c r="A160" s="3" t="inlineStr">
         <is>
-          <t>Roman</t>
+          <t>Reniers</t>
         </is>
       </c>
       <c r="B160" s="3" t="inlineStr">
         <is>
-          <t>Sandy</t>
+          <t>Hugo</t>
         </is>
       </c>
       <c r="C160" s="3" t="inlineStr">
         <is>
-          <t>Bergvliet</t>
+          <t>Nelspruit</t>
         </is>
       </c>
       <c r="D160" s="3" t="inlineStr">
@@ -5534,29 +5534,29 @@
       </c>
       <c r="E160" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F160" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="161" ht="25" customHeight="1">
       <c r="A161" s="3" t="inlineStr">
         <is>
-          <t>Rossouw</t>
+          <t>Roman</t>
         </is>
       </c>
       <c r="B161" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Sandy</t>
         </is>
       </c>
       <c r="C161" s="3" t="inlineStr">
         <is>
-          <t>Tokai</t>
+          <t>Bergvliet</t>
         </is>
       </c>
       <c r="D161" s="3" t="inlineStr">
@@ -5566,7 +5566,7 @@
       </c>
       <c r="E161" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F161" s="3" t="inlineStr">
@@ -5578,17 +5578,17 @@
     <row r="162" ht="25" customHeight="1">
       <c r="A162" s="3" t="inlineStr">
         <is>
-          <t>Rothner</t>
+          <t>Rossouw</t>
         </is>
       </c>
       <c r="B162" s="3" t="inlineStr">
         <is>
-          <t>Andrea</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C162" s="3" t="inlineStr">
         <is>
-          <t>Eden</t>
+          <t>Tokai</t>
         </is>
       </c>
       <c r="D162" s="3" t="inlineStr">
@@ -5598,7 +5598,7 @@
       </c>
       <c r="E162" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F162" s="3" t="inlineStr">
@@ -5610,17 +5610,17 @@
     <row r="163" ht="25" customHeight="1">
       <c r="A163" s="3" t="inlineStr">
         <is>
-          <t>Roux</t>
+          <t>Rothner</t>
         </is>
       </c>
       <c r="B163" s="3" t="inlineStr">
         <is>
-          <t>Anthonie Petrus</t>
+          <t>Andrea</t>
         </is>
       </c>
       <c r="C163" s="3" t="inlineStr">
         <is>
-          <t>Moorreesburg</t>
+          <t>Eden</t>
         </is>
       </c>
       <c r="D163" s="3" t="inlineStr">
@@ -5630,7 +5630,7 @@
       </c>
       <c r="E163" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F163" s="3" t="inlineStr">
@@ -5642,17 +5642,17 @@
     <row r="164" ht="25" customHeight="1">
       <c r="A164" s="3" t="inlineStr">
         <is>
-          <t>Russell</t>
+          <t>Roux</t>
         </is>
       </c>
       <c r="B164" s="3" t="inlineStr">
         <is>
-          <t>Ingrid</t>
+          <t>Anthonie Petrus</t>
         </is>
       </c>
       <c r="C164" s="3" t="inlineStr">
         <is>
-          <t>Fish Hoek</t>
+          <t>Moorreesburg</t>
         </is>
       </c>
       <c r="D164" s="3" t="inlineStr">
@@ -5674,27 +5674,27 @@
     <row r="165" ht="25" customHeight="1">
       <c r="A165" s="3" t="inlineStr">
         <is>
-          <t>SNYMAN</t>
+          <t>Russell</t>
         </is>
       </c>
       <c r="B165" s="3" t="inlineStr">
         <is>
-          <t>LYN</t>
+          <t>Ingrid</t>
         </is>
       </c>
       <c r="C165" s="3" t="inlineStr">
         <is>
-          <t>Deep South</t>
+          <t>Fish Hoek</t>
         </is>
       </c>
       <c r="D165" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E165" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F165" s="3" t="inlineStr">
@@ -5706,27 +5706,27 @@
     <row r="166" ht="25" customHeight="1">
       <c r="A166" s="3" t="inlineStr">
         <is>
-          <t>STEENBERG</t>
+          <t>SNYMAN</t>
         </is>
       </c>
       <c r="B166" s="3" t="inlineStr">
         <is>
-          <t>TIM</t>
+          <t>LYN</t>
         </is>
       </c>
       <c r="C166" s="3" t="inlineStr">
         <is>
-          <t>Wellington</t>
+          <t>Deep South</t>
         </is>
       </c>
       <c r="D166" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E166" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F166" s="3" t="inlineStr">
@@ -5738,17 +5738,17 @@
     <row r="167" ht="25" customHeight="1">
       <c r="A167" s="3" t="inlineStr">
         <is>
-          <t>Sabatier</t>
+          <t>STEENBERG</t>
         </is>
       </c>
       <c r="B167" s="3" t="inlineStr">
         <is>
-          <t>Rodney</t>
+          <t>TIM</t>
         </is>
       </c>
       <c r="C167" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Wellington</t>
         </is>
       </c>
       <c r="D167" s="3" t="inlineStr">
@@ -5763,24 +5763,24 @@
       </c>
       <c r="F167" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="168" ht="25" customHeight="1">
       <c r="A168" s="3" t="inlineStr">
         <is>
-          <t>Sampie</t>
+          <t>Sabatier</t>
         </is>
       </c>
       <c r="B168" s="3" t="inlineStr">
         <is>
-          <t>Sharon</t>
+          <t>Rodney</t>
         </is>
       </c>
       <c r="C168" s="3" t="inlineStr">
         <is>
-          <t>Bergvliet</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D168" s="3" t="inlineStr">
@@ -5795,24 +5795,24 @@
       </c>
       <c r="F168" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="169" ht="25" customHeight="1">
       <c r="A169" s="3" t="inlineStr">
         <is>
-          <t>Schatz</t>
+          <t>Sampie</t>
         </is>
       </c>
       <c r="B169" s="3" t="inlineStr">
         <is>
-          <t>Vera</t>
+          <t>Sharon</t>
         </is>
       </c>
       <c r="C169" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Bergvliet</t>
         </is>
       </c>
       <c r="D169" s="3" t="inlineStr">
@@ -5839,7 +5839,7 @@
       </c>
       <c r="B170" s="3" t="inlineStr">
         <is>
-          <t>Frank</t>
+          <t>Vera</t>
         </is>
       </c>
       <c r="C170" s="3" t="inlineStr">
@@ -5854,7 +5854,7 @@
       </c>
       <c r="E170" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F170" s="3" t="inlineStr">
@@ -5866,17 +5866,17 @@
     <row r="171" ht="25" customHeight="1">
       <c r="A171" s="3" t="inlineStr">
         <is>
-          <t>Searle</t>
+          <t>Schatz</t>
         </is>
       </c>
       <c r="B171" s="3" t="inlineStr">
         <is>
-          <t>Francis</t>
+          <t>Frank</t>
         </is>
       </c>
       <c r="C171" s="3" t="inlineStr">
         <is>
-          <t>Kouga</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D171" s="3" t="inlineStr">
@@ -5886,12 +5886,12 @@
       </c>
       <c r="E171" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F171" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -5903,7 +5903,7 @@
       </c>
       <c r="B172" s="3" t="inlineStr">
         <is>
-          <t>Gloria</t>
+          <t>Francis</t>
         </is>
       </c>
       <c r="C172" s="3" t="inlineStr">
@@ -5918,7 +5918,7 @@
       </c>
       <c r="E172" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F172" s="3" t="inlineStr">
@@ -5930,17 +5930,17 @@
     <row r="173" ht="25" customHeight="1">
       <c r="A173" s="3" t="inlineStr">
         <is>
-          <t>Sell</t>
+          <t>Searle</t>
         </is>
       </c>
       <c r="B173" s="3" t="inlineStr">
         <is>
-          <t>Ami</t>
+          <t>Gloria</t>
         </is>
       </c>
       <c r="C173" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Kouga</t>
         </is>
       </c>
       <c r="D173" s="3" t="inlineStr">
@@ -5955,24 +5955,24 @@
       </c>
       <c r="F173" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="174" ht="25" customHeight="1">
       <c r="A174" s="3" t="inlineStr">
         <is>
-          <t>Simpson</t>
+          <t>Sell</t>
         </is>
       </c>
       <c r="B174" s="3" t="inlineStr">
         <is>
-          <t>Beryl</t>
+          <t>Ami</t>
         </is>
       </c>
       <c r="C174" s="3" t="inlineStr">
         <is>
-          <t>Cape Town</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D174" s="3" t="inlineStr">
@@ -5994,17 +5994,17 @@
     <row r="175" ht="25" customHeight="1">
       <c r="A175" s="3" t="inlineStr">
         <is>
-          <t>Sircoulomb</t>
+          <t>Simpson</t>
         </is>
       </c>
       <c r="B175" s="3" t="inlineStr">
         <is>
-          <t>Kenlis</t>
+          <t>Beryl</t>
         </is>
       </c>
       <c r="C175" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Cape Town</t>
         </is>
       </c>
       <c r="D175" s="3" t="inlineStr">
@@ -6031,7 +6031,7 @@
       </c>
       <c r="B176" s="3" t="inlineStr">
         <is>
-          <t>Holger</t>
+          <t>Kenlis</t>
         </is>
       </c>
       <c r="C176" s="3" t="inlineStr">
@@ -6046,7 +6046,7 @@
       </c>
       <c r="E176" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F176" s="3" t="inlineStr">
@@ -6058,12 +6058,12 @@
     <row r="177" ht="25" customHeight="1">
       <c r="A177" s="3" t="inlineStr">
         <is>
-          <t>Smeer</t>
+          <t>Sircoulomb</t>
         </is>
       </c>
       <c r="B177" s="3" t="inlineStr">
         <is>
-          <t>Hennie</t>
+          <t>Holger</t>
         </is>
       </c>
       <c r="C177" s="3" t="inlineStr">
@@ -6073,12 +6073,12 @@
       </c>
       <c r="D177" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E177" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F177" s="3" t="inlineStr">
@@ -6090,22 +6090,22 @@
     <row r="178" ht="25" customHeight="1">
       <c r="A178" s="3" t="inlineStr">
         <is>
-          <t>Smit</t>
+          <t>Smeer</t>
         </is>
       </c>
       <c r="B178" s="3" t="inlineStr">
         <is>
-          <t>Sue</t>
+          <t>Hennie</t>
         </is>
       </c>
       <c r="C178" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D178" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E178" s="3" t="inlineStr">
@@ -6115,7 +6115,7 @@
       </c>
       <c r="F178" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -6127,12 +6127,12 @@
       </c>
       <c r="B179" s="3" t="inlineStr">
         <is>
-          <t>Herman</t>
+          <t>Sue</t>
         </is>
       </c>
       <c r="C179" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D179" s="3" t="inlineStr">
@@ -6147,7 +6147,7 @@
       </c>
       <c r="F179" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -6159,17 +6159,17 @@
       </c>
       <c r="B180" s="3" t="inlineStr">
         <is>
-          <t>Juanita</t>
+          <t>Herman</t>
         </is>
       </c>
       <c r="C180" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D180" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E180" s="3" t="inlineStr">
@@ -6179,29 +6179,29 @@
       </c>
       <c r="F180" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="181" ht="25" customHeight="1">
       <c r="A181" s="3" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Smit</t>
         </is>
       </c>
       <c r="B181" s="3" t="inlineStr">
         <is>
-          <t>Jeff</t>
+          <t>Juanita</t>
         </is>
       </c>
       <c r="C181" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D181" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E181" s="3" t="inlineStr">
@@ -6223,12 +6223,12 @@
       </c>
       <c r="B182" s="3" t="inlineStr">
         <is>
-          <t>Bennie</t>
+          <t>Jeff</t>
         </is>
       </c>
       <c r="C182" s="3" t="inlineStr">
         <is>
-          <t>Wellington</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D182" s="3" t="inlineStr">
@@ -6238,12 +6238,12 @@
       </c>
       <c r="E182" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F182" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -6255,12 +6255,12 @@
       </c>
       <c r="B183" s="3" t="inlineStr">
         <is>
-          <t>Carmen Dolores</t>
+          <t>Bennie</t>
         </is>
       </c>
       <c r="C183" s="3" t="inlineStr">
         <is>
-          <t>Tokai</t>
+          <t>Wellington</t>
         </is>
       </c>
       <c r="D183" s="3" t="inlineStr">
@@ -6270,7 +6270,7 @@
       </c>
       <c r="E183" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F183" s="3" t="inlineStr">
@@ -6287,7 +6287,7 @@
       </c>
       <c r="B184" s="3" t="inlineStr">
         <is>
-          <t>David John</t>
+          <t>Carmen Dolores</t>
         </is>
       </c>
       <c r="C184" s="3" t="inlineStr">
@@ -6314,17 +6314,17 @@
     <row r="185" ht="25" customHeight="1">
       <c r="A185" s="3" t="inlineStr">
         <is>
-          <t>Sochen</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="B185" s="3" t="inlineStr">
         <is>
-          <t>Diana</t>
+          <t>David John</t>
         </is>
       </c>
       <c r="C185" s="3" t="inlineStr">
         <is>
-          <t>Sea Point</t>
+          <t>Tokai</t>
         </is>
       </c>
       <c r="D185" s="3" t="inlineStr">
@@ -6334,7 +6334,7 @@
       </c>
       <c r="E185" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F185" s="3" t="inlineStr">
@@ -6346,49 +6346,49 @@
     <row r="186" ht="25" customHeight="1">
       <c r="A186" s="3" t="inlineStr">
         <is>
-          <t>Steyn</t>
+          <t>Sochen</t>
         </is>
       </c>
       <c r="B186" s="3" t="inlineStr">
         <is>
-          <t>Elna</t>
+          <t>Diana</t>
         </is>
       </c>
       <c r="C186" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Sea Point</t>
         </is>
       </c>
       <c r="D186" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E186" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F186" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="187" ht="25" customHeight="1">
       <c r="A187" s="3" t="inlineStr">
         <is>
-          <t>Strauss</t>
+          <t>Steyn</t>
         </is>
       </c>
       <c r="B187" s="3" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>Elna</t>
         </is>
       </c>
       <c r="C187" s="3" t="inlineStr">
         <is>
-          <t>Kuilsriver</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D187" s="3" t="inlineStr">
@@ -6403,29 +6403,29 @@
       </c>
       <c r="F187" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="188" ht="25" customHeight="1">
       <c r="A188" s="3" t="inlineStr">
         <is>
-          <t>Strydom</t>
+          <t>Strauss</t>
         </is>
       </c>
       <c r="B188" s="3" t="inlineStr">
         <is>
-          <t>Melinda Lee</t>
+          <t>Patrick</t>
         </is>
       </c>
       <c r="C188" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Kuilsriver</t>
         </is>
       </c>
       <c r="D188" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E188" s="3" t="inlineStr">
@@ -6435,24 +6435,24 @@
       </c>
       <c r="F188" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="189" ht="25" customHeight="1">
       <c r="A189" s="3" t="inlineStr">
         <is>
-          <t>Sturges</t>
+          <t>Strydom</t>
         </is>
       </c>
       <c r="B189" s="3" t="inlineStr">
         <is>
-          <t>Trevor</t>
+          <t>Melinda Lee</t>
         </is>
       </c>
       <c r="C189" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D189" s="3" t="inlineStr">
@@ -6474,17 +6474,17 @@
     <row r="190" ht="25" customHeight="1">
       <c r="A190" s="3" t="inlineStr">
         <is>
-          <t>Talbot</t>
+          <t>Sturges</t>
         </is>
       </c>
       <c r="B190" s="3" t="inlineStr">
         <is>
-          <t>Lauryn</t>
+          <t>Trevor</t>
         </is>
       </c>
       <c r="C190" s="3" t="inlineStr">
         <is>
-          <t>Benoni Lakes</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D190" s="3" t="inlineStr">
@@ -6506,17 +6506,17 @@
     <row r="191" ht="25" customHeight="1">
       <c r="A191" s="3" t="inlineStr">
         <is>
-          <t>Theron</t>
+          <t>Talbot</t>
         </is>
       </c>
       <c r="B191" s="3" t="inlineStr">
         <is>
-          <t>Pierre</t>
+          <t>Lauryn</t>
         </is>
       </c>
       <c r="C191" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Benoni Lakes</t>
         </is>
       </c>
       <c r="D191" s="3" t="inlineStr">
@@ -6543,7 +6543,7 @@
       </c>
       <c r="B192" s="3" t="inlineStr">
         <is>
-          <t>Moira</t>
+          <t>Pierre</t>
         </is>
       </c>
       <c r="C192" s="3" t="inlineStr">
@@ -6570,17 +6570,17 @@
     <row r="193" ht="25" customHeight="1">
       <c r="A193" s="3" t="inlineStr">
         <is>
-          <t>Townsend</t>
+          <t>Theron</t>
         </is>
       </c>
       <c r="B193" s="3" t="inlineStr">
         <is>
-          <t>Diane</t>
+          <t>Moira</t>
         </is>
       </c>
       <c r="C193" s="3" t="inlineStr">
         <is>
-          <t>Benoni Lakes</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D193" s="3" t="inlineStr">
@@ -6590,7 +6590,7 @@
       </c>
       <c r="E193" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F193" s="3" t="inlineStr">
@@ -6602,27 +6602,27 @@
     <row r="194" ht="25" customHeight="1">
       <c r="A194" s="3" t="inlineStr">
         <is>
-          <t>Toye</t>
+          <t>Townsend</t>
         </is>
       </c>
       <c r="B194" s="3" t="inlineStr">
         <is>
-          <t>Omolayo</t>
+          <t>Diane</t>
         </is>
       </c>
       <c r="C194" s="3" t="inlineStr">
         <is>
-          <t>The Wilds</t>
+          <t>Benoni Lakes</t>
         </is>
       </c>
       <c r="D194" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E194" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F194" s="3" t="inlineStr">
@@ -6634,22 +6634,22 @@
     <row r="195" ht="25" customHeight="1">
       <c r="A195" s="3" t="inlineStr">
         <is>
-          <t>Tshikala</t>
+          <t>Toye</t>
         </is>
       </c>
       <c r="B195" s="3" t="inlineStr">
         <is>
-          <t>David Alex</t>
+          <t>Omolayo</t>
         </is>
       </c>
       <c r="C195" s="3" t="inlineStr">
         <is>
-          <t>Athlone</t>
+          <t>The Wilds</t>
         </is>
       </c>
       <c r="D195" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E195" s="3" t="inlineStr">
@@ -6659,24 +6659,24 @@
       </c>
       <c r="F195" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="196" ht="25" customHeight="1">
       <c r="A196" s="3" t="inlineStr">
         <is>
-          <t>Tuckett</t>
+          <t>Tshikala</t>
         </is>
       </c>
       <c r="B196" s="3" t="inlineStr">
         <is>
-          <t>Alistair</t>
+          <t>David Alex</t>
         </is>
       </c>
       <c r="C196" s="3" t="inlineStr">
         <is>
-          <t>Roodepoort Clearwater Cyber</t>
+          <t>Athlone</t>
         </is>
       </c>
       <c r="D196" s="3" t="inlineStr">
@@ -6691,7 +6691,7 @@
       </c>
       <c r="F196" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -6703,7 +6703,7 @@
       </c>
       <c r="B197" s="3" t="inlineStr">
         <is>
-          <t>Rowan</t>
+          <t>Alistair</t>
         </is>
       </c>
       <c r="C197" s="3" t="inlineStr">
@@ -6718,7 +6718,7 @@
       </c>
       <c r="E197" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F197" s="3" t="inlineStr">
@@ -6735,7 +6735,7 @@
       </c>
       <c r="B198" s="3" t="inlineStr">
         <is>
-          <t>Gail</t>
+          <t>Rowan</t>
         </is>
       </c>
       <c r="C198" s="3" t="inlineStr">
@@ -6750,7 +6750,7 @@
       </c>
       <c r="E198" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F198" s="3" t="inlineStr">
@@ -6762,17 +6762,17 @@
     <row r="199" ht="25" customHeight="1">
       <c r="A199" s="3" t="inlineStr">
         <is>
-          <t>VAN BREDA</t>
+          <t>Tuckett</t>
         </is>
       </c>
       <c r="B199" s="3" t="inlineStr">
         <is>
-          <t>HILARY LISE</t>
+          <t>Gail</t>
         </is>
       </c>
       <c r="C199" s="3" t="inlineStr">
         <is>
-          <t>Cape Town</t>
+          <t>Roodepoort Clearwater Cyber</t>
         </is>
       </c>
       <c r="D199" s="3" t="inlineStr">
@@ -6787,39 +6787,39 @@
       </c>
       <c r="F199" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="200" ht="25" customHeight="1">
       <c r="A200" s="3" t="inlineStr">
         <is>
-          <t>VAN DER MERWE</t>
+          <t>VAN BREDA</t>
         </is>
       </c>
       <c r="B200" s="3" t="inlineStr">
         <is>
-          <t>PATRICIA</t>
+          <t>HILARY LISE</t>
         </is>
       </c>
       <c r="C200" s="3" t="inlineStr">
         <is>
-          <t>East London Port Rex</t>
+          <t>Cape Town</t>
         </is>
       </c>
       <c r="D200" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E200" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F200" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -6831,17 +6831,17 @@
       </c>
       <c r="B201" s="3" t="inlineStr">
         <is>
-          <t>MARINA</t>
+          <t>PATRICIA</t>
         </is>
       </c>
       <c r="C201" s="3" t="inlineStr">
         <is>
-          <t>Malmesbury</t>
+          <t>East London Port Rex</t>
         </is>
       </c>
       <c r="D201" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E201" s="3" t="inlineStr">
@@ -6851,56 +6851,56 @@
       </c>
       <c r="F201" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="202" ht="25" customHeight="1">
       <c r="A202" s="3" t="inlineStr">
         <is>
-          <t>Valadao</t>
+          <t>VAN DER MERWE</t>
         </is>
       </c>
       <c r="B202" s="3" t="inlineStr">
         <is>
-          <t>Tracy</t>
+          <t>MARINA</t>
         </is>
       </c>
       <c r="C202" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Malmesbury</t>
         </is>
       </c>
       <c r="D202" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E202" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F202" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="203" ht="25" customHeight="1">
       <c r="A203" s="3" t="inlineStr">
         <is>
-          <t>Van Niekerk</t>
+          <t>Valadao</t>
         </is>
       </c>
       <c r="B203" s="3" t="inlineStr">
         <is>
-          <t>Riaan</t>
+          <t>Tracy</t>
         </is>
       </c>
       <c r="C203" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D203" s="3" t="inlineStr">
@@ -6922,22 +6922,22 @@
     <row r="204" ht="25" customHeight="1">
       <c r="A204" s="3" t="inlineStr">
         <is>
-          <t>Van Nieuwenhuyzen</t>
+          <t>Van Niekerk</t>
         </is>
       </c>
       <c r="B204" s="3" t="inlineStr">
         <is>
-          <t>Hilgardt</t>
+          <t>Riaan</t>
         </is>
       </c>
       <c r="C204" s="3" t="inlineStr">
         <is>
-          <t>Worcester</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D204" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E204" s="3" t="inlineStr">
@@ -6947,24 +6947,24 @@
       </c>
       <c r="F204" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="205" ht="25" customHeight="1">
       <c r="A205" s="3" t="inlineStr">
         <is>
-          <t>Van Rensburg</t>
+          <t>Van Nieuwenhuyzen</t>
         </is>
       </c>
       <c r="B205" s="3" t="inlineStr">
         <is>
-          <t>Neville</t>
+          <t>Hilgardt</t>
         </is>
       </c>
       <c r="C205" s="3" t="inlineStr">
         <is>
-          <t>Moorreesburg</t>
+          <t>Worcester</t>
         </is>
       </c>
       <c r="D205" s="3" t="inlineStr">
@@ -6974,7 +6974,7 @@
       </c>
       <c r="E205" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F205" s="3" t="inlineStr">
@@ -6986,27 +6986,27 @@
     <row r="206" ht="25" customHeight="1">
       <c r="A206" s="3" t="inlineStr">
         <is>
-          <t>Van Romburgh</t>
+          <t>Van Rensburg</t>
         </is>
       </c>
       <c r="B206" s="3" t="inlineStr">
         <is>
-          <t>Lorna</t>
+          <t>Neville</t>
         </is>
       </c>
       <c r="C206" s="3" t="inlineStr">
         <is>
-          <t>Fish Hoek</t>
+          <t>Moorreesburg</t>
         </is>
       </c>
       <c r="D206" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E206" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F206" s="3" t="inlineStr">
@@ -7018,17 +7018,17 @@
     <row r="207" ht="25" customHeight="1">
       <c r="A207" s="3" t="inlineStr">
         <is>
-          <t>Van Wyk-Nelson</t>
+          <t>Van Romburgh</t>
         </is>
       </c>
       <c r="B207" s="3" t="inlineStr">
         <is>
-          <t>Edith</t>
+          <t>Lorna</t>
         </is>
       </c>
       <c r="C207" s="3" t="inlineStr">
         <is>
-          <t>Kuilsriver</t>
+          <t>Fish Hoek</t>
         </is>
       </c>
       <c r="D207" s="3" t="inlineStr">
@@ -7050,17 +7050,17 @@
     <row r="208" ht="25" customHeight="1">
       <c r="A208" s="3" t="inlineStr">
         <is>
-          <t>Van Zyl</t>
+          <t>Van Wyk-Nelson</t>
         </is>
       </c>
       <c r="B208" s="3" t="inlineStr">
         <is>
-          <t>Louis</t>
+          <t>Edith</t>
         </is>
       </c>
       <c r="C208" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Kuilsriver</t>
         </is>
       </c>
       <c r="D208" s="3" t="inlineStr">
@@ -7075,29 +7075,29 @@
       </c>
       <c r="F208" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="209" ht="25" customHeight="1">
       <c r="A209" s="3" t="inlineStr">
         <is>
-          <t>Van de Merwe</t>
+          <t>Van Zyl</t>
         </is>
       </c>
       <c r="B209" s="3" t="inlineStr">
         <is>
-          <t>Marina</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="C209" s="3" t="inlineStr">
         <is>
-          <t>Malmesbury</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D209" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E209" s="3" t="inlineStr">
@@ -7107,29 +7107,29 @@
       </c>
       <c r="F209" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="210" ht="25" customHeight="1">
       <c r="A210" s="3" t="inlineStr">
         <is>
-          <t>Venter</t>
+          <t>Van de Merwe</t>
         </is>
       </c>
       <c r="B210" s="3" t="inlineStr">
         <is>
-          <t>Louis</t>
+          <t>Marina</t>
         </is>
       </c>
       <c r="C210" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Malmesbury</t>
         </is>
       </c>
       <c r="D210" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E210" s="3" t="inlineStr">
@@ -7139,34 +7139,34 @@
       </c>
       <c r="F210" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="211" ht="25" customHeight="1">
       <c r="A211" s="3" t="inlineStr">
         <is>
-          <t>Volker</t>
+          <t>Venter</t>
         </is>
       </c>
       <c r="B211" s="3" t="inlineStr">
         <is>
-          <t>Russell</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="C211" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D211" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E211" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F211" s="3" t="inlineStr">
@@ -7178,96 +7178,96 @@
     <row r="212" ht="25" customHeight="1">
       <c r="A212" s="3" t="inlineStr">
         <is>
-          <t>Von Mollendorf</t>
+          <t>Volker</t>
         </is>
       </c>
       <c r="B212" s="3" t="inlineStr">
         <is>
-          <t>Rinette</t>
+          <t>Russell</t>
         </is>
       </c>
       <c r="C212" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>King William's Town</t>
         </is>
       </c>
       <c r="D212" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E212" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F212" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="213" ht="25" customHeight="1">
       <c r="A213" s="3" t="inlineStr">
         <is>
-          <t>Warman</t>
+          <t>Von Mollendorf</t>
         </is>
       </c>
       <c r="B213" s="3" t="inlineStr">
         <is>
-          <t>Alastair</t>
+          <t>Rinette</t>
         </is>
       </c>
       <c r="C213" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Durbanville</t>
         </is>
       </c>
       <c r="D213" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E213" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F213" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="214" ht="25" customHeight="1">
       <c r="A214" s="3" t="inlineStr">
         <is>
-          <t>Watson</t>
+          <t>Warman</t>
         </is>
       </c>
       <c r="B214" s="3" t="inlineStr">
         <is>
-          <t>Allan</t>
+          <t>Alastair</t>
         </is>
       </c>
       <c r="C214" s="3" t="inlineStr">
         <is>
-          <t>Sea Point</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D214" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E214" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F214" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -7279,22 +7279,22 @@
       </c>
       <c r="B215" s="3" t="inlineStr">
         <is>
-          <t>Alison</t>
+          <t>Allan</t>
         </is>
       </c>
       <c r="C215" s="3" t="inlineStr">
         <is>
-          <t>Sedgefield</t>
+          <t>Sea Point</t>
         </is>
       </c>
       <c r="D215" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E215" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F215" s="3" t="inlineStr">
@@ -7306,27 +7306,27 @@
     <row r="216" ht="25" customHeight="1">
       <c r="A216" s="3" t="inlineStr">
         <is>
-          <t>Williams</t>
+          <t>Watson</t>
         </is>
       </c>
       <c r="B216" s="3" t="inlineStr">
         <is>
-          <t>Johanna</t>
+          <t>Alison</t>
         </is>
       </c>
       <c r="C216" s="3" t="inlineStr">
         <is>
-          <t>Mitchells Plain</t>
+          <t>Sedgefield</t>
         </is>
       </c>
       <c r="D216" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E216" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F216" s="3" t="inlineStr">
@@ -7338,22 +7338,22 @@
     <row r="217" ht="25" customHeight="1">
       <c r="A217" s="3" t="inlineStr">
         <is>
-          <t>Wills</t>
+          <t>Williams</t>
         </is>
       </c>
       <c r="B217" s="3" t="inlineStr">
         <is>
-          <t>Geila</t>
+          <t>Johanna</t>
         </is>
       </c>
       <c r="C217" s="3" t="inlineStr">
         <is>
-          <t>Athlone</t>
+          <t>Mitchells Plain</t>
         </is>
       </c>
       <c r="D217" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E217" s="3" t="inlineStr">
@@ -7370,17 +7370,17 @@
     <row r="218" ht="25" customHeight="1">
       <c r="A218" s="3" t="inlineStr">
         <is>
-          <t>Wilter-Sturges</t>
+          <t>Wills</t>
         </is>
       </c>
       <c r="B218" s="3" t="inlineStr">
         <is>
-          <t>Meredith</t>
+          <t>Geila</t>
         </is>
       </c>
       <c r="C218" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Athlone</t>
         </is>
       </c>
       <c r="D218" s="3" t="inlineStr">
@@ -7395,24 +7395,24 @@
       </c>
       <c r="F218" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="219" ht="25" customHeight="1">
       <c r="A219" s="3" t="inlineStr">
         <is>
-          <t>Wright</t>
+          <t>Wilter-Sturges</t>
         </is>
       </c>
       <c r="B219" s="3" t="inlineStr">
         <is>
-          <t>Rocky</t>
+          <t>Meredith</t>
         </is>
       </c>
       <c r="C219" s="3" t="inlineStr">
         <is>
-          <t>Table View</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D219" s="3" t="inlineStr">
@@ -7422,29 +7422,29 @@
       </c>
       <c r="E219" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F219" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="220" ht="25" customHeight="1">
       <c r="A220" s="3" t="inlineStr">
         <is>
-          <t>Young</t>
+          <t>Wright</t>
         </is>
       </c>
       <c r="B220" s="3" t="inlineStr">
         <is>
-          <t>Judy</t>
+          <t>Rocky</t>
         </is>
       </c>
       <c r="C220" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>Table View</t>
         </is>
       </c>
       <c r="D220" s="3" t="inlineStr">
@@ -7454,7 +7454,7 @@
       </c>
       <c r="E220" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F220" s="3" t="inlineStr">
@@ -7466,17 +7466,17 @@
     <row r="221" ht="25" customHeight="1">
       <c r="A221" s="3" t="inlineStr">
         <is>
-          <t>de Kock</t>
+          <t>Young</t>
         </is>
       </c>
       <c r="B221" s="3" t="inlineStr">
         <is>
-          <t>Engela</t>
+          <t>Judy</t>
         </is>
       </c>
       <c r="C221" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Durbanville</t>
         </is>
       </c>
       <c r="D221" s="3" t="inlineStr">
@@ -7486,7 +7486,7 @@
       </c>
       <c r="E221" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F221" s="3" t="inlineStr">
@@ -7503,7 +7503,7 @@
       </c>
       <c r="B222" s="3" t="inlineStr">
         <is>
-          <t>Francois</t>
+          <t>Engela</t>
         </is>
       </c>
       <c r="C222" s="3" t="inlineStr">
@@ -7530,59 +7530,59 @@
     <row r="223" ht="25" customHeight="1">
       <c r="A223" s="3" t="inlineStr">
         <is>
-          <t>de Silva</t>
+          <t>de Kock</t>
         </is>
       </c>
       <c r="B223" s="3" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Francois</t>
         </is>
       </c>
       <c r="C223" s="3" t="inlineStr">
         <is>
-          <t>Edenvale</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D223" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E223" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F223" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="224" ht="25" customHeight="1">
       <c r="A224" s="3" t="inlineStr">
         <is>
-          <t>du Plooy</t>
+          <t>de Silva</t>
         </is>
       </c>
       <c r="B224" s="3" t="inlineStr">
         <is>
-          <t>Tammy</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="C224" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Edenvale</t>
         </is>
       </c>
       <c r="D224" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E224" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F224" s="3" t="inlineStr">
@@ -7599,7 +7599,7 @@
       </c>
       <c r="B225" s="3" t="inlineStr">
         <is>
-          <t>Marc</t>
+          <t>Tammy</t>
         </is>
       </c>
       <c r="C225" s="3" t="inlineStr">
@@ -7626,17 +7626,17 @@
     <row r="226" ht="25" customHeight="1">
       <c r="A226" s="3" t="inlineStr">
         <is>
-          <t>du Toit</t>
+          <t>du Plooy</t>
         </is>
       </c>
       <c r="B226" s="3" t="inlineStr">
         <is>
-          <t>Desiree</t>
+          <t>Marc</t>
         </is>
       </c>
       <c r="C226" s="3" t="inlineStr">
         <is>
-          <t>Ramsgate</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D226" s="3" t="inlineStr">
@@ -7658,22 +7658,22 @@
     <row r="227" ht="25" customHeight="1">
       <c r="A227" s="3" t="inlineStr">
         <is>
-          <t>stier</t>
+          <t>du Toit</t>
         </is>
       </c>
       <c r="B227" s="3" t="inlineStr">
         <is>
-          <t>RORY</t>
+          <t>Desiree</t>
         </is>
       </c>
       <c r="C227" s="3" t="inlineStr">
         <is>
-          <t>Deep South</t>
+          <t>Ramsgate</t>
         </is>
       </c>
       <c r="D227" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E227" s="3" t="inlineStr">
@@ -7683,56 +7683,56 @@
       </c>
       <c r="F227" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="228" ht="25" customHeight="1">
       <c r="A228" s="3" t="inlineStr">
         <is>
-          <t>tyler</t>
+          <t>stier</t>
         </is>
       </c>
       <c r="B228" s="3" t="inlineStr">
         <is>
-          <t>natascha</t>
+          <t>RORY</t>
         </is>
       </c>
       <c r="C228" s="3" t="inlineStr">
         <is>
-          <t>Kensington</t>
+          <t>Deep South</t>
         </is>
       </c>
       <c r="D228" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E228" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F228" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="229" ht="25" customHeight="1">
       <c r="A229" s="3" t="inlineStr">
         <is>
-          <t>van Blerk</t>
+          <t>tyler</t>
         </is>
       </c>
       <c r="B229" s="3" t="inlineStr">
         <is>
-          <t>Carl</t>
+          <t>natascha</t>
         </is>
       </c>
       <c r="C229" s="3" t="inlineStr">
         <is>
-          <t>Eden</t>
+          <t>Kensington</t>
         </is>
       </c>
       <c r="D229" s="3" t="inlineStr">
@@ -7747,24 +7747,24 @@
       </c>
       <c r="F229" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="230" ht="25" customHeight="1">
       <c r="A230" s="3" t="inlineStr">
         <is>
-          <t>van Heerden</t>
+          <t>van Blerk</t>
         </is>
       </c>
       <c r="B230" s="3" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Carl</t>
         </is>
       </c>
       <c r="C230" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Eden</t>
         </is>
       </c>
       <c r="D230" s="3" t="inlineStr">
@@ -7779,7 +7779,7 @@
       </c>
       <c r="F230" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -7791,7 +7791,7 @@
       </c>
       <c r="B231" s="3" t="inlineStr">
         <is>
-          <t>Sandy</t>
+          <t>Sydney</t>
         </is>
       </c>
       <c r="C231" s="3" t="inlineStr">
@@ -7806,7 +7806,7 @@
       </c>
       <c r="E231" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F231" s="3" t="inlineStr">
@@ -7823,17 +7823,17 @@
       </c>
       <c r="B232" s="3" t="inlineStr">
         <is>
-          <t>Craig</t>
+          <t>Sandy</t>
         </is>
       </c>
       <c r="C232" s="3" t="inlineStr">
         <is>
-          <t>East London Beacon Bay</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D232" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E232" s="3" t="inlineStr">
@@ -7855,17 +7855,17 @@
       </c>
       <c r="B233" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Craig</t>
         </is>
       </c>
       <c r="C233" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>East London Beacon Bay</t>
         </is>
       </c>
       <c r="D233" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E233" s="3" t="inlineStr">
@@ -7882,17 +7882,17 @@
     <row r="234" ht="25" customHeight="1">
       <c r="A234" s="3" t="inlineStr">
         <is>
-          <t>van Rensburg</t>
+          <t>van Heerden</t>
         </is>
       </c>
       <c r="B234" s="3" t="inlineStr">
         <is>
-          <t>Johan</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C234" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D234" s="3" t="inlineStr">
@@ -7902,12 +7902,12 @@
       </c>
       <c r="E234" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F234" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -7919,7 +7919,7 @@
       </c>
       <c r="B235" s="3" t="inlineStr">
         <is>
-          <t>Anne</t>
+          <t>Johan</t>
         </is>
       </c>
       <c r="C235" s="3" t="inlineStr">
@@ -7946,17 +7946,17 @@
     <row r="236" ht="25" customHeight="1">
       <c r="A236" s="3" t="inlineStr">
         <is>
-          <t>van Wulven</t>
+          <t>van Rensburg</t>
         </is>
       </c>
       <c r="B236" s="3" t="inlineStr">
         <is>
-          <t>Jeannie</t>
+          <t>Anne</t>
         </is>
       </c>
       <c r="C236" s="3" t="inlineStr">
         <is>
-          <t>Tygerberg Hills</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D236" s="3" t="inlineStr">
@@ -7983,7 +7983,7 @@
       </c>
       <c r="B237" s="3" t="inlineStr">
         <is>
-          <t>Alan</t>
+          <t>Jeannie</t>
         </is>
       </c>
       <c r="C237" s="3" t="inlineStr">
@@ -7998,7 +7998,7 @@
       </c>
       <c r="E237" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F237" s="3" t="inlineStr">
@@ -8015,7 +8015,7 @@
       </c>
       <c r="B238" s="3" t="inlineStr">
         <is>
-          <t>Deon</t>
+          <t>Alan</t>
         </is>
       </c>
       <c r="C238" s="3" t="inlineStr">
@@ -8042,17 +8042,17 @@
     <row r="239" ht="25" customHeight="1">
       <c r="A239" s="3" t="inlineStr">
         <is>
-          <t>van Wyk</t>
+          <t>van Wulven</t>
         </is>
       </c>
       <c r="B239" s="3" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>Deon</t>
         </is>
       </c>
       <c r="C239" s="3" t="inlineStr">
         <is>
-          <t>North Durban</t>
+          <t>Tygerberg Hills</t>
         </is>
       </c>
       <c r="D239" s="3" t="inlineStr">
@@ -8067,7 +8067,7 @@
       </c>
       <c r="F239" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -8079,12 +8079,12 @@
       </c>
       <c r="B240" s="3" t="inlineStr">
         <is>
-          <t>Lindie</t>
+          <t>Kim</t>
         </is>
       </c>
       <c r="C240" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>North Durban</t>
         </is>
       </c>
       <c r="D240" s="3" t="inlineStr">
@@ -8111,12 +8111,12 @@
       </c>
       <c r="B241" s="3" t="inlineStr">
         <is>
-          <t>Willem</t>
+          <t>Lindie</t>
         </is>
       </c>
       <c r="C241" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D241" s="3" t="inlineStr">
@@ -8143,12 +8143,12 @@
       </c>
       <c r="B242" s="3" t="inlineStr">
         <is>
-          <t>Patricia</t>
+          <t>Willem</t>
         </is>
       </c>
       <c r="C242" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D242" s="3" t="inlineStr">
@@ -8170,22 +8170,22 @@
     <row r="243" ht="25" customHeight="1">
       <c r="A243" s="3" t="inlineStr">
         <is>
-          <t>van der Merwe</t>
+          <t>van Wyk</t>
         </is>
       </c>
       <c r="B243" s="3" t="inlineStr">
         <is>
-          <t>Ingrid</t>
+          <t>Patricia</t>
         </is>
       </c>
       <c r="C243" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D243" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E243" s="3" t="inlineStr">
@@ -8202,49 +8202,49 @@
     <row r="244" ht="25" customHeight="1">
       <c r="A244" s="3" t="inlineStr">
         <is>
-          <t>van der Westhuizen</t>
+          <t>van der Merwe</t>
         </is>
       </c>
       <c r="B244" s="3" t="inlineStr">
         <is>
-          <t>Hennie</t>
+          <t>Ingrid</t>
         </is>
       </c>
       <c r="C244" s="3" t="inlineStr">
         <is>
-          <t>Helderberg</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D244" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E244" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F244" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="245" ht="25" customHeight="1">
       <c r="A245" s="3" t="inlineStr">
         <is>
-          <t>von der Decken</t>
+          <t>van der Westhuizen</t>
         </is>
       </c>
       <c r="B245" s="3" t="inlineStr">
         <is>
-          <t>Brian</t>
+          <t>Hennie</t>
         </is>
       </c>
       <c r="C245" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Helderberg</t>
         </is>
       </c>
       <c r="D245" s="3" t="inlineStr">
@@ -8259,51 +8259,83 @@
       </c>
       <c r="F245" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="246" ht="25" customHeight="1">
       <c r="A246" s="3" t="inlineStr">
         <is>
+          <t>von der Decken</t>
+        </is>
+      </c>
+      <c r="B246" s="3" t="inlineStr">
+        <is>
+          <t>Brian</t>
+        </is>
+      </c>
+      <c r="C246" s="3" t="inlineStr">
+        <is>
+          <t>King William's Town</t>
+        </is>
+      </c>
+      <c r="D246" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E246" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F246" s="3" t="inlineStr">
+        <is>
+          <t>410E</t>
+        </is>
+      </c>
+    </row>
+    <row r="247" ht="25" customHeight="1">
+      <c r="A247" s="3" t="inlineStr">
+        <is>
           <t>‘t Hart</t>
         </is>
       </c>
-      <c r="B246" s="3" t="inlineStr">
+      <c r="B247" s="3" t="inlineStr">
         <is>
           <t>Michelle</t>
         </is>
       </c>
-      <c r="C246" s="3" t="inlineStr">
+      <c r="C247" s="3" t="inlineStr">
         <is>
           <t>Benoni Lakes</t>
         </is>
       </c>
-      <c r="D246" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E246" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F246" s="3" t="inlineStr">
+      <c r="D247" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E247" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F247" s="3" t="inlineStr">
         <is>
           <t>410E</t>
-        </is>
-      </c>
-    </row>
-    <row r="247">
-      <c r="A247" s="1" t="inlineStr">
-        <is>
-          <t>Number of attendees: 244</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="inlineStr">
+        <is>
+          <t>Number of attendees: 245</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" s="1" t="inlineStr">
         <is>
           <t>Number of voters: 98</t>
         </is>
@@ -8339,7 +8371,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Registrees as of 28/04/2021 16:40</t>
+          <t>410E Registrees as of 29/04/2021 09:02</t>
         </is>
       </c>
     </row>
@@ -11924,7 +11956,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Registrees as of 28/04/2021 16:40</t>
+          <t>410W Registrees as of 29/04/2021 09:02</t>
         </is>
       </c>
     </row>
@@ -12626,7 +12658,7 @@
       </c>
       <c r="E27" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -14030,7 +14062,7 @@
       </c>
       <c r="E79" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -14651,7 +14683,7 @@
       </c>
       <c r="E102" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -15974,7 +16006,7 @@
       </c>
       <c r="E151" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -16100,7 +16132,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Voting details as of 28/04/2021 16:40</t>
+          <t>410E Voting details as of 29/04/2021 09:02</t>
         </is>
       </c>
     </row>
@@ -16477,7 +16509,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Voting details as of 28/04/2021 16:40</t>
+          <t>410W Voting details as of 29/04/2021 09:02</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Registree stats backup on Fri 30 Apr 2021 11:19:53 SAST
</commit_message>
<xml_diff>
--- a/static/docs/registrees_list.xlsx
+++ b/static/docs/registrees_list.xlsx
@@ -451,7 +451,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>MD410 Registrees as of 30/04/2021 08:28</t>
+          <t>MD410 Registrees as of 30/04/2021 11:19</t>
         </is>
       </c>
     </row>
@@ -8403,7 +8403,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Registrees as of 30/04/2021 08:28</t>
+          <t>410E Registrees as of 30/04/2021 11:19</t>
         </is>
       </c>
     </row>
@@ -8646,7 +8646,7 @@
       </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -10239,7 +10239,7 @@
       </c>
       <c r="E69" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -11988,7 +11988,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Registrees as of 30/04/2021 08:28</t>
+          <t>410W Registrees as of 30/04/2021 11:19</t>
         </is>
       </c>
     </row>
@@ -16164,7 +16164,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Voting details as of 30/04/2021 08:28</t>
+          <t>410E Voting details as of 30/04/2021 11:19</t>
         </is>
       </c>
     </row>
@@ -16541,7 +16541,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Voting details as of 30/04/2021 08:28</t>
+          <t>410W Voting details as of 30/04/2021 11:19</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Registree stats backup on Fri 30 Apr 2021 13:35:17 SAST
</commit_message>
<xml_diff>
--- a/static/docs/registrees_list.xlsx
+++ b/static/docs/registrees_list.xlsx
@@ -451,7 +451,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>MD410 Registrees as of 30/04/2021 11:19</t>
+          <t>MD410 Registrees as of 30/04/2021 13:35</t>
         </is>
       </c>
     </row>
@@ -8403,7 +8403,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Registrees as of 30/04/2021 11:19</t>
+          <t>410E Registrees as of 30/04/2021 13:35</t>
         </is>
       </c>
     </row>
@@ -11988,7 +11988,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Registrees as of 30/04/2021 11:19</t>
+          <t>410W Registrees as of 30/04/2021 13:35</t>
         </is>
       </c>
     </row>
@@ -16164,7 +16164,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Voting details as of 30/04/2021 11:19</t>
+          <t>410E Voting details as of 30/04/2021 13:35</t>
         </is>
       </c>
     </row>
@@ -16541,7 +16541,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Voting details as of 30/04/2021 11:19</t>
+          <t>410W Voting details as of 30/04/2021 13:35</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Registree stats backup on Fri 30 Apr 2021 17:39:12 SAST
</commit_message>
<xml_diff>
--- a/static/docs/registrees_list.xlsx
+++ b/static/docs/registrees_list.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F250"/>
+  <dimension ref="A1:F251"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,7 +451,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>MD410 Registrees as of 30/04/2021 13:35</t>
+          <t>MD410 Registrees as of 30/04/2021 17:39</t>
         </is>
       </c>
     </row>
@@ -5258,17 +5258,17 @@
     <row r="152" ht="25" customHeight="1">
       <c r="A152" s="3" t="inlineStr">
         <is>
-          <t>Pillay</t>
+          <t>Piater</t>
         </is>
       </c>
       <c r="B152" s="3" t="inlineStr">
         <is>
-          <t>Sundru</t>
+          <t>Ivan</t>
         </is>
       </c>
       <c r="C152" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>East London Port Rex</t>
         </is>
       </c>
       <c r="D152" s="3" t="inlineStr">
@@ -5283,7 +5283,7 @@
       </c>
       <c r="F152" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -5295,12 +5295,12 @@
       </c>
       <c r="B153" s="3" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>Sundru</t>
         </is>
       </c>
       <c r="C153" s="3" t="inlineStr">
         <is>
-          <t>Tygerberg Hills</t>
+          <t>Durbanville</t>
         </is>
       </c>
       <c r="D153" s="3" t="inlineStr">
@@ -5322,17 +5322,17 @@
     <row r="154" ht="25" customHeight="1">
       <c r="A154" s="3" t="inlineStr">
         <is>
-          <t>Polkinghorne</t>
+          <t>Pillay</t>
         </is>
       </c>
       <c r="B154" s="3" t="inlineStr">
         <is>
-          <t>Tracey</t>
+          <t>Patrick</t>
         </is>
       </c>
       <c r="C154" s="3" t="inlineStr">
         <is>
-          <t>Kensington</t>
+          <t>Tygerberg Hills</t>
         </is>
       </c>
       <c r="D154" s="3" t="inlineStr">
@@ -5342,12 +5342,12 @@
       </c>
       <c r="E154" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F154" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -5359,7 +5359,7 @@
       </c>
       <c r="B155" s="3" t="inlineStr">
         <is>
-          <t>Gavin</t>
+          <t>Tracey</t>
         </is>
       </c>
       <c r="C155" s="3" t="inlineStr">
@@ -5374,7 +5374,7 @@
       </c>
       <c r="E155" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F155" s="3" t="inlineStr">
@@ -5386,22 +5386,22 @@
     <row r="156" ht="25" customHeight="1">
       <c r="A156" s="3" t="inlineStr">
         <is>
-          <t>Pretorius</t>
+          <t>Polkinghorne</t>
         </is>
       </c>
       <c r="B156" s="3" t="inlineStr">
         <is>
-          <t>Sheldon Edmund</t>
+          <t>Gavin</t>
         </is>
       </c>
       <c r="C156" s="3" t="inlineStr">
         <is>
-          <t>Merriman</t>
+          <t>Kensington</t>
         </is>
       </c>
       <c r="D156" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E156" s="3" t="inlineStr">
@@ -5411,29 +5411,29 @@
       </c>
       <c r="F156" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="157" ht="25" customHeight="1">
       <c r="A157" s="3" t="inlineStr">
         <is>
-          <t>Ras</t>
+          <t>Pretorius</t>
         </is>
       </c>
       <c r="B157" s="3" t="inlineStr">
         <is>
-          <t>Mary-Anne</t>
+          <t>Sheldon Edmund</t>
         </is>
       </c>
       <c r="C157" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Merriman</t>
         </is>
       </c>
       <c r="D157" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E157" s="3" t="inlineStr">
@@ -5455,7 +5455,7 @@
       </c>
       <c r="B158" s="3" t="inlineStr">
         <is>
-          <t>Leon Jacobus</t>
+          <t>Mary-Anne</t>
         </is>
       </c>
       <c r="C158" s="3" t="inlineStr">
@@ -5482,22 +5482,22 @@
     <row r="159" ht="25" customHeight="1">
       <c r="A159" s="3" t="inlineStr">
         <is>
-          <t>Rashirai</t>
+          <t>Ras</t>
         </is>
       </c>
       <c r="B159" s="3" t="inlineStr">
         <is>
-          <t>Tabeth</t>
+          <t>Leon Jacobus</t>
         </is>
       </c>
       <c r="C159" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D159" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E159" s="3" t="inlineStr">
@@ -5507,29 +5507,29 @@
       </c>
       <c r="F159" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="160" ht="25" customHeight="1">
       <c r="A160" s="3" t="inlineStr">
         <is>
-          <t>Rathbone Smyth</t>
+          <t>Rashirai</t>
         </is>
       </c>
       <c r="B160" s="3" t="inlineStr">
         <is>
-          <t>Janine</t>
+          <t>Tabeth</t>
         </is>
       </c>
       <c r="C160" s="3" t="inlineStr">
         <is>
-          <t>Vereeniging</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D160" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E160" s="3" t="inlineStr">
@@ -5546,17 +5546,17 @@
     <row r="161" ht="25" customHeight="1">
       <c r="A161" s="3" t="inlineStr">
         <is>
-          <t>Reniers</t>
+          <t>Rathbone Smyth</t>
         </is>
       </c>
       <c r="B161" s="3" t="inlineStr">
         <is>
-          <t>Hugo</t>
+          <t>Janine</t>
         </is>
       </c>
       <c r="C161" s="3" t="inlineStr">
         <is>
-          <t>Nelspruit</t>
+          <t>Vereeniging</t>
         </is>
       </c>
       <c r="D161" s="3" t="inlineStr">
@@ -5566,7 +5566,7 @@
       </c>
       <c r="E161" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F161" s="3" t="inlineStr">
@@ -5578,17 +5578,17 @@
     <row r="162" ht="25" customHeight="1">
       <c r="A162" s="3" t="inlineStr">
         <is>
-          <t>Roman</t>
+          <t>Reniers</t>
         </is>
       </c>
       <c r="B162" s="3" t="inlineStr">
         <is>
-          <t>Sandy</t>
+          <t>Hugo</t>
         </is>
       </c>
       <c r="C162" s="3" t="inlineStr">
         <is>
-          <t>Bergvliet</t>
+          <t>Nelspruit</t>
         </is>
       </c>
       <c r="D162" s="3" t="inlineStr">
@@ -5598,29 +5598,29 @@
       </c>
       <c r="E162" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F162" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="163" ht="25" customHeight="1">
       <c r="A163" s="3" t="inlineStr">
         <is>
-          <t>Rossouw</t>
+          <t>Roman</t>
         </is>
       </c>
       <c r="B163" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Sandy</t>
         </is>
       </c>
       <c r="C163" s="3" t="inlineStr">
         <is>
-          <t>Tokai</t>
+          <t>Bergvliet</t>
         </is>
       </c>
       <c r="D163" s="3" t="inlineStr">
@@ -5630,7 +5630,7 @@
       </c>
       <c r="E163" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F163" s="3" t="inlineStr">
@@ -5642,17 +5642,17 @@
     <row r="164" ht="25" customHeight="1">
       <c r="A164" s="3" t="inlineStr">
         <is>
-          <t>Rothner</t>
+          <t>Rossouw</t>
         </is>
       </c>
       <c r="B164" s="3" t="inlineStr">
         <is>
-          <t>Andrea</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C164" s="3" t="inlineStr">
         <is>
-          <t>Eden</t>
+          <t>Tokai</t>
         </is>
       </c>
       <c r="D164" s="3" t="inlineStr">
@@ -5662,7 +5662,7 @@
       </c>
       <c r="E164" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F164" s="3" t="inlineStr">
@@ -5674,17 +5674,17 @@
     <row r="165" ht="25" customHeight="1">
       <c r="A165" s="3" t="inlineStr">
         <is>
-          <t>Roux</t>
+          <t>Rothner</t>
         </is>
       </c>
       <c r="B165" s="3" t="inlineStr">
         <is>
-          <t>Anthonie Petrus</t>
+          <t>Andrea</t>
         </is>
       </c>
       <c r="C165" s="3" t="inlineStr">
         <is>
-          <t>Moorreesburg</t>
+          <t>Eden</t>
         </is>
       </c>
       <c r="D165" s="3" t="inlineStr">
@@ -5694,7 +5694,7 @@
       </c>
       <c r="E165" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F165" s="3" t="inlineStr">
@@ -5706,17 +5706,17 @@
     <row r="166" ht="25" customHeight="1">
       <c r="A166" s="3" t="inlineStr">
         <is>
-          <t>Russell</t>
+          <t>Roux</t>
         </is>
       </c>
       <c r="B166" s="3" t="inlineStr">
         <is>
-          <t>Ingrid</t>
+          <t>Anthonie Petrus</t>
         </is>
       </c>
       <c r="C166" s="3" t="inlineStr">
         <is>
-          <t>Fish Hoek</t>
+          <t>Moorreesburg</t>
         </is>
       </c>
       <c r="D166" s="3" t="inlineStr">
@@ -5738,27 +5738,27 @@
     <row r="167" ht="25" customHeight="1">
       <c r="A167" s="3" t="inlineStr">
         <is>
-          <t>SNYMAN</t>
+          <t>Russell</t>
         </is>
       </c>
       <c r="B167" s="3" t="inlineStr">
         <is>
-          <t>LYN</t>
+          <t>Ingrid</t>
         </is>
       </c>
       <c r="C167" s="3" t="inlineStr">
         <is>
-          <t>Deep South</t>
+          <t>Fish Hoek</t>
         </is>
       </c>
       <c r="D167" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E167" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F167" s="3" t="inlineStr">
@@ -5770,27 +5770,27 @@
     <row r="168" ht="25" customHeight="1">
       <c r="A168" s="3" t="inlineStr">
         <is>
-          <t>STEENBERG</t>
+          <t>SNYMAN</t>
         </is>
       </c>
       <c r="B168" s="3" t="inlineStr">
         <is>
-          <t>TIM</t>
+          <t>LYN</t>
         </is>
       </c>
       <c r="C168" s="3" t="inlineStr">
         <is>
-          <t>Wellington</t>
+          <t>Deep South</t>
         </is>
       </c>
       <c r="D168" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E168" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F168" s="3" t="inlineStr">
@@ -5802,17 +5802,17 @@
     <row r="169" ht="25" customHeight="1">
       <c r="A169" s="3" t="inlineStr">
         <is>
-          <t>Sabatier</t>
+          <t>STEENBERG</t>
         </is>
       </c>
       <c r="B169" s="3" t="inlineStr">
         <is>
-          <t>Rodney</t>
+          <t>TIM</t>
         </is>
       </c>
       <c r="C169" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Wellington</t>
         </is>
       </c>
       <c r="D169" s="3" t="inlineStr">
@@ -5827,24 +5827,24 @@
       </c>
       <c r="F169" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="170" ht="25" customHeight="1">
       <c r="A170" s="3" t="inlineStr">
         <is>
-          <t>Sampie</t>
+          <t>Sabatier</t>
         </is>
       </c>
       <c r="B170" s="3" t="inlineStr">
         <is>
-          <t>Sharon</t>
+          <t>Rodney</t>
         </is>
       </c>
       <c r="C170" s="3" t="inlineStr">
         <is>
-          <t>Bergvliet</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D170" s="3" t="inlineStr">
@@ -5859,24 +5859,24 @@
       </c>
       <c r="F170" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="171" ht="25" customHeight="1">
       <c r="A171" s="3" t="inlineStr">
         <is>
-          <t>Schatz</t>
+          <t>Sampie</t>
         </is>
       </c>
       <c r="B171" s="3" t="inlineStr">
         <is>
-          <t>Vera</t>
+          <t>Sharon</t>
         </is>
       </c>
       <c r="C171" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Bergvliet</t>
         </is>
       </c>
       <c r="D171" s="3" t="inlineStr">
@@ -5903,7 +5903,7 @@
       </c>
       <c r="B172" s="3" t="inlineStr">
         <is>
-          <t>Frank</t>
+          <t>Vera</t>
         </is>
       </c>
       <c r="C172" s="3" t="inlineStr">
@@ -5918,7 +5918,7 @@
       </c>
       <c r="E172" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F172" s="3" t="inlineStr">
@@ -5930,17 +5930,17 @@
     <row r="173" ht="25" customHeight="1">
       <c r="A173" s="3" t="inlineStr">
         <is>
-          <t>Searle</t>
+          <t>Schatz</t>
         </is>
       </c>
       <c r="B173" s="3" t="inlineStr">
         <is>
-          <t>Francis</t>
+          <t>Frank</t>
         </is>
       </c>
       <c r="C173" s="3" t="inlineStr">
         <is>
-          <t>Kouga</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D173" s="3" t="inlineStr">
@@ -5950,12 +5950,12 @@
       </c>
       <c r="E173" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F173" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -5967,7 +5967,7 @@
       </c>
       <c r="B174" s="3" t="inlineStr">
         <is>
-          <t>Gloria</t>
+          <t>Francis</t>
         </is>
       </c>
       <c r="C174" s="3" t="inlineStr">
@@ -5982,7 +5982,7 @@
       </c>
       <c r="E174" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F174" s="3" t="inlineStr">
@@ -5994,17 +5994,17 @@
     <row r="175" ht="25" customHeight="1">
       <c r="A175" s="3" t="inlineStr">
         <is>
-          <t>Sell</t>
+          <t>Searle</t>
         </is>
       </c>
       <c r="B175" s="3" t="inlineStr">
         <is>
-          <t>Ami</t>
+          <t>Gloria</t>
         </is>
       </c>
       <c r="C175" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Kouga</t>
         </is>
       </c>
       <c r="D175" s="3" t="inlineStr">
@@ -6019,24 +6019,24 @@
       </c>
       <c r="F175" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="176" ht="25" customHeight="1">
       <c r="A176" s="3" t="inlineStr">
         <is>
-          <t>Simpson</t>
+          <t>Sell</t>
         </is>
       </c>
       <c r="B176" s="3" t="inlineStr">
         <is>
-          <t>Beryl</t>
+          <t>Ami</t>
         </is>
       </c>
       <c r="C176" s="3" t="inlineStr">
         <is>
-          <t>Cape Town</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D176" s="3" t="inlineStr">
@@ -6058,17 +6058,17 @@
     <row r="177" ht="25" customHeight="1">
       <c r="A177" s="3" t="inlineStr">
         <is>
-          <t>Sircoulomb</t>
+          <t>Simpson</t>
         </is>
       </c>
       <c r="B177" s="3" t="inlineStr">
         <is>
-          <t>Kenlis</t>
+          <t>Beryl</t>
         </is>
       </c>
       <c r="C177" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Cape Town</t>
         </is>
       </c>
       <c r="D177" s="3" t="inlineStr">
@@ -6095,7 +6095,7 @@
       </c>
       <c r="B178" s="3" t="inlineStr">
         <is>
-          <t>Holger</t>
+          <t>Kenlis</t>
         </is>
       </c>
       <c r="C178" s="3" t="inlineStr">
@@ -6110,7 +6110,7 @@
       </c>
       <c r="E178" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F178" s="3" t="inlineStr">
@@ -6122,12 +6122,12 @@
     <row r="179" ht="25" customHeight="1">
       <c r="A179" s="3" t="inlineStr">
         <is>
-          <t>Smeer</t>
+          <t>Sircoulomb</t>
         </is>
       </c>
       <c r="B179" s="3" t="inlineStr">
         <is>
-          <t>Hennie</t>
+          <t>Holger</t>
         </is>
       </c>
       <c r="C179" s="3" t="inlineStr">
@@ -6137,12 +6137,12 @@
       </c>
       <c r="D179" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E179" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F179" s="3" t="inlineStr">
@@ -6154,22 +6154,22 @@
     <row r="180" ht="25" customHeight="1">
       <c r="A180" s="3" t="inlineStr">
         <is>
-          <t>Smit</t>
+          <t>Smeer</t>
         </is>
       </c>
       <c r="B180" s="3" t="inlineStr">
         <is>
-          <t>Sue</t>
+          <t>Hennie</t>
         </is>
       </c>
       <c r="C180" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D180" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E180" s="3" t="inlineStr">
@@ -6179,7 +6179,7 @@
       </c>
       <c r="F180" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -6191,12 +6191,12 @@
       </c>
       <c r="B181" s="3" t="inlineStr">
         <is>
-          <t>Herman</t>
+          <t>Sue</t>
         </is>
       </c>
       <c r="C181" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D181" s="3" t="inlineStr">
@@ -6211,7 +6211,7 @@
       </c>
       <c r="F181" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -6223,17 +6223,17 @@
       </c>
       <c r="B182" s="3" t="inlineStr">
         <is>
-          <t>Juanita</t>
+          <t>Herman</t>
         </is>
       </c>
       <c r="C182" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D182" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E182" s="3" t="inlineStr">
@@ -6243,29 +6243,29 @@
       </c>
       <c r="F182" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="183" ht="25" customHeight="1">
       <c r="A183" s="3" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Smit</t>
         </is>
       </c>
       <c r="B183" s="3" t="inlineStr">
         <is>
-          <t>Jeff</t>
+          <t>Juanita</t>
         </is>
       </c>
       <c r="C183" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D183" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E183" s="3" t="inlineStr">
@@ -6287,12 +6287,12 @@
       </c>
       <c r="B184" s="3" t="inlineStr">
         <is>
-          <t>Bennie</t>
+          <t>Jeff</t>
         </is>
       </c>
       <c r="C184" s="3" t="inlineStr">
         <is>
-          <t>Wellington</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D184" s="3" t="inlineStr">
@@ -6302,12 +6302,12 @@
       </c>
       <c r="E184" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F184" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -6319,12 +6319,12 @@
       </c>
       <c r="B185" s="3" t="inlineStr">
         <is>
-          <t>Carmen Dolores</t>
+          <t>Bennie</t>
         </is>
       </c>
       <c r="C185" s="3" t="inlineStr">
         <is>
-          <t>Tokai</t>
+          <t>Wellington</t>
         </is>
       </c>
       <c r="D185" s="3" t="inlineStr">
@@ -6334,7 +6334,7 @@
       </c>
       <c r="E185" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F185" s="3" t="inlineStr">
@@ -6351,7 +6351,7 @@
       </c>
       <c r="B186" s="3" t="inlineStr">
         <is>
-          <t>David John</t>
+          <t>Carmen Dolores</t>
         </is>
       </c>
       <c r="C186" s="3" t="inlineStr">
@@ -6378,17 +6378,17 @@
     <row r="187" ht="25" customHeight="1">
       <c r="A187" s="3" t="inlineStr">
         <is>
-          <t>Sochen</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="B187" s="3" t="inlineStr">
         <is>
-          <t>Diana</t>
+          <t>David John</t>
         </is>
       </c>
       <c r="C187" s="3" t="inlineStr">
         <is>
-          <t>Sea Point</t>
+          <t>Tokai</t>
         </is>
       </c>
       <c r="D187" s="3" t="inlineStr">
@@ -6398,7 +6398,7 @@
       </c>
       <c r="E187" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F187" s="3" t="inlineStr">
@@ -6410,49 +6410,49 @@
     <row r="188" ht="25" customHeight="1">
       <c r="A188" s="3" t="inlineStr">
         <is>
-          <t>Steyn</t>
+          <t>Sochen</t>
         </is>
       </c>
       <c r="B188" s="3" t="inlineStr">
         <is>
-          <t>Elna</t>
+          <t>Diana</t>
         </is>
       </c>
       <c r="C188" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Sea Point</t>
         </is>
       </c>
       <c r="D188" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E188" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F188" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="189" ht="25" customHeight="1">
       <c r="A189" s="3" t="inlineStr">
         <is>
-          <t>Strauss</t>
+          <t>Steyn</t>
         </is>
       </c>
       <c r="B189" s="3" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>Elna</t>
         </is>
       </c>
       <c r="C189" s="3" t="inlineStr">
         <is>
-          <t>Kuilsriver</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D189" s="3" t="inlineStr">
@@ -6467,29 +6467,29 @@
       </c>
       <c r="F189" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="190" ht="25" customHeight="1">
       <c r="A190" s="3" t="inlineStr">
         <is>
-          <t>Strydom</t>
+          <t>Strauss</t>
         </is>
       </c>
       <c r="B190" s="3" t="inlineStr">
         <is>
-          <t>Melinda Lee</t>
+          <t>Patrick</t>
         </is>
       </c>
       <c r="C190" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Kuilsriver</t>
         </is>
       </c>
       <c r="D190" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E190" s="3" t="inlineStr">
@@ -6499,24 +6499,24 @@
       </c>
       <c r="F190" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="191" ht="25" customHeight="1">
       <c r="A191" s="3" t="inlineStr">
         <is>
-          <t>Sturges</t>
+          <t>Strydom</t>
         </is>
       </c>
       <c r="B191" s="3" t="inlineStr">
         <is>
-          <t>Trevor</t>
+          <t>Melinda Lee</t>
         </is>
       </c>
       <c r="C191" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D191" s="3" t="inlineStr">
@@ -6538,17 +6538,17 @@
     <row r="192" ht="25" customHeight="1">
       <c r="A192" s="3" t="inlineStr">
         <is>
-          <t>Talbot</t>
+          <t>Sturges</t>
         </is>
       </c>
       <c r="B192" s="3" t="inlineStr">
         <is>
-          <t>Lauryn</t>
+          <t>Trevor</t>
         </is>
       </c>
       <c r="C192" s="3" t="inlineStr">
         <is>
-          <t>Benoni Lakes</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D192" s="3" t="inlineStr">
@@ -6570,17 +6570,17 @@
     <row r="193" ht="25" customHeight="1">
       <c r="A193" s="3" t="inlineStr">
         <is>
-          <t>Theron</t>
+          <t>Talbot</t>
         </is>
       </c>
       <c r="B193" s="3" t="inlineStr">
         <is>
-          <t>Pierre</t>
+          <t>Lauryn</t>
         </is>
       </c>
       <c r="C193" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Benoni Lakes</t>
         </is>
       </c>
       <c r="D193" s="3" t="inlineStr">
@@ -6607,7 +6607,7 @@
       </c>
       <c r="B194" s="3" t="inlineStr">
         <is>
-          <t>Moira</t>
+          <t>Pierre</t>
         </is>
       </c>
       <c r="C194" s="3" t="inlineStr">
@@ -6634,17 +6634,17 @@
     <row r="195" ht="25" customHeight="1">
       <c r="A195" s="3" t="inlineStr">
         <is>
-          <t>Townsend</t>
+          <t>Theron</t>
         </is>
       </c>
       <c r="B195" s="3" t="inlineStr">
         <is>
-          <t>Diane</t>
+          <t>Moira</t>
         </is>
       </c>
       <c r="C195" s="3" t="inlineStr">
         <is>
-          <t>Benoni Lakes</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D195" s="3" t="inlineStr">
@@ -6654,7 +6654,7 @@
       </c>
       <c r="E195" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F195" s="3" t="inlineStr">
@@ -6666,27 +6666,27 @@
     <row r="196" ht="25" customHeight="1">
       <c r="A196" s="3" t="inlineStr">
         <is>
-          <t>Toye</t>
+          <t>Townsend</t>
         </is>
       </c>
       <c r="B196" s="3" t="inlineStr">
         <is>
-          <t>Omolayo</t>
+          <t>Diane</t>
         </is>
       </c>
       <c r="C196" s="3" t="inlineStr">
         <is>
-          <t>The Wilds</t>
+          <t>Benoni Lakes</t>
         </is>
       </c>
       <c r="D196" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E196" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F196" s="3" t="inlineStr">
@@ -6698,22 +6698,22 @@
     <row r="197" ht="25" customHeight="1">
       <c r="A197" s="3" t="inlineStr">
         <is>
-          <t>Tshikala</t>
+          <t>Toye</t>
         </is>
       </c>
       <c r="B197" s="3" t="inlineStr">
         <is>
-          <t>David Alex</t>
+          <t>Omolayo</t>
         </is>
       </c>
       <c r="C197" s="3" t="inlineStr">
         <is>
-          <t>Athlone</t>
+          <t>The Wilds</t>
         </is>
       </c>
       <c r="D197" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E197" s="3" t="inlineStr">
@@ -6723,24 +6723,24 @@
       </c>
       <c r="F197" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="198" ht="25" customHeight="1">
       <c r="A198" s="3" t="inlineStr">
         <is>
-          <t>Tuckett</t>
+          <t>Tshikala</t>
         </is>
       </c>
       <c r="B198" s="3" t="inlineStr">
         <is>
-          <t>Alistair</t>
+          <t>David Alex</t>
         </is>
       </c>
       <c r="C198" s="3" t="inlineStr">
         <is>
-          <t>Roodepoort Clearwater Cyber</t>
+          <t>Athlone</t>
         </is>
       </c>
       <c r="D198" s="3" t="inlineStr">
@@ -6755,7 +6755,7 @@
       </c>
       <c r="F198" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -6767,7 +6767,7 @@
       </c>
       <c r="B199" s="3" t="inlineStr">
         <is>
-          <t>Rowan</t>
+          <t>Alistair</t>
         </is>
       </c>
       <c r="C199" s="3" t="inlineStr">
@@ -6782,7 +6782,7 @@
       </c>
       <c r="E199" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F199" s="3" t="inlineStr">
@@ -6799,7 +6799,7 @@
       </c>
       <c r="B200" s="3" t="inlineStr">
         <is>
-          <t>Gail</t>
+          <t>Rowan</t>
         </is>
       </c>
       <c r="C200" s="3" t="inlineStr">
@@ -6814,7 +6814,7 @@
       </c>
       <c r="E200" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F200" s="3" t="inlineStr">
@@ -6826,17 +6826,17 @@
     <row r="201" ht="25" customHeight="1">
       <c r="A201" s="3" t="inlineStr">
         <is>
-          <t>VAN BREDA</t>
+          <t>Tuckett</t>
         </is>
       </c>
       <c r="B201" s="3" t="inlineStr">
         <is>
-          <t>HILARY LISE</t>
+          <t>Gail</t>
         </is>
       </c>
       <c r="C201" s="3" t="inlineStr">
         <is>
-          <t>Cape Town</t>
+          <t>Roodepoort Clearwater Cyber</t>
         </is>
       </c>
       <c r="D201" s="3" t="inlineStr">
@@ -6851,39 +6851,39 @@
       </c>
       <c r="F201" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="202" ht="25" customHeight="1">
       <c r="A202" s="3" t="inlineStr">
         <is>
-          <t>VAN DER MERWE</t>
+          <t>VAN BREDA</t>
         </is>
       </c>
       <c r="B202" s="3" t="inlineStr">
         <is>
-          <t>PATRICIA</t>
+          <t>HILARY LISE</t>
         </is>
       </c>
       <c r="C202" s="3" t="inlineStr">
         <is>
-          <t>East London Port Rex</t>
+          <t>Cape Town</t>
         </is>
       </c>
       <c r="D202" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E202" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F202" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -6895,17 +6895,17 @@
       </c>
       <c r="B203" s="3" t="inlineStr">
         <is>
-          <t>MARINA</t>
+          <t>PATRICIA</t>
         </is>
       </c>
       <c r="C203" s="3" t="inlineStr">
         <is>
-          <t>Malmesbury</t>
+          <t>East London Port Rex</t>
         </is>
       </c>
       <c r="D203" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E203" s="3" t="inlineStr">
@@ -6915,56 +6915,56 @@
       </c>
       <c r="F203" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="204" ht="25" customHeight="1">
       <c r="A204" s="3" t="inlineStr">
         <is>
-          <t>Valadao</t>
+          <t>VAN DER MERWE</t>
         </is>
       </c>
       <c r="B204" s="3" t="inlineStr">
         <is>
-          <t>Tracy</t>
+          <t>MARINA</t>
         </is>
       </c>
       <c r="C204" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Malmesbury</t>
         </is>
       </c>
       <c r="D204" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E204" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F204" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="205" ht="25" customHeight="1">
       <c r="A205" s="3" t="inlineStr">
         <is>
-          <t>Van Niekerk</t>
+          <t>Valadao</t>
         </is>
       </c>
       <c r="B205" s="3" t="inlineStr">
         <is>
-          <t>Riaan</t>
+          <t>Tracy</t>
         </is>
       </c>
       <c r="C205" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D205" s="3" t="inlineStr">
@@ -6986,22 +6986,22 @@
     <row r="206" ht="25" customHeight="1">
       <c r="A206" s="3" t="inlineStr">
         <is>
-          <t>Van Nieuwenhuyzen</t>
+          <t>Van Niekerk</t>
         </is>
       </c>
       <c r="B206" s="3" t="inlineStr">
         <is>
-          <t>Hilgardt</t>
+          <t>Riaan</t>
         </is>
       </c>
       <c r="C206" s="3" t="inlineStr">
         <is>
-          <t>Worcester</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D206" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E206" s="3" t="inlineStr">
@@ -7011,24 +7011,24 @@
       </c>
       <c r="F206" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="207" ht="25" customHeight="1">
       <c r="A207" s="3" t="inlineStr">
         <is>
-          <t>Van Rensburg</t>
+          <t>Van Nieuwenhuyzen</t>
         </is>
       </c>
       <c r="B207" s="3" t="inlineStr">
         <is>
-          <t>Neville</t>
+          <t>Hilgardt</t>
         </is>
       </c>
       <c r="C207" s="3" t="inlineStr">
         <is>
-          <t>Moorreesburg</t>
+          <t>Worcester</t>
         </is>
       </c>
       <c r="D207" s="3" t="inlineStr">
@@ -7038,7 +7038,7 @@
       </c>
       <c r="E207" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F207" s="3" t="inlineStr">
@@ -7050,27 +7050,27 @@
     <row r="208" ht="25" customHeight="1">
       <c r="A208" s="3" t="inlineStr">
         <is>
-          <t>Van Romburgh</t>
+          <t>Van Rensburg</t>
         </is>
       </c>
       <c r="B208" s="3" t="inlineStr">
         <is>
-          <t>Lorna</t>
+          <t>Neville</t>
         </is>
       </c>
       <c r="C208" s="3" t="inlineStr">
         <is>
-          <t>Fish Hoek</t>
+          <t>Moorreesburg</t>
         </is>
       </c>
       <c r="D208" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E208" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F208" s="3" t="inlineStr">
@@ -7082,17 +7082,17 @@
     <row r="209" ht="25" customHeight="1">
       <c r="A209" s="3" t="inlineStr">
         <is>
-          <t>Van Wyk-Nelson</t>
+          <t>Van Romburgh</t>
         </is>
       </c>
       <c r="B209" s="3" t="inlineStr">
         <is>
-          <t>Edith</t>
+          <t>Lorna</t>
         </is>
       </c>
       <c r="C209" s="3" t="inlineStr">
         <is>
-          <t>Kuilsriver</t>
+          <t>Fish Hoek</t>
         </is>
       </c>
       <c r="D209" s="3" t="inlineStr">
@@ -7114,17 +7114,17 @@
     <row r="210" ht="25" customHeight="1">
       <c r="A210" s="3" t="inlineStr">
         <is>
-          <t>Van Zyl</t>
+          <t>Van Wyk-Nelson</t>
         </is>
       </c>
       <c r="B210" s="3" t="inlineStr">
         <is>
-          <t>Louis</t>
+          <t>Edith</t>
         </is>
       </c>
       <c r="C210" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Kuilsriver</t>
         </is>
       </c>
       <c r="D210" s="3" t="inlineStr">
@@ -7139,29 +7139,29 @@
       </c>
       <c r="F210" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="211" ht="25" customHeight="1">
       <c r="A211" s="3" t="inlineStr">
         <is>
-          <t>Van de Merwe</t>
+          <t>Van Zyl</t>
         </is>
       </c>
       <c r="B211" s="3" t="inlineStr">
         <is>
-          <t>Marina</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="C211" s="3" t="inlineStr">
         <is>
-          <t>Malmesbury</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D211" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E211" s="3" t="inlineStr">
@@ -7171,29 +7171,29 @@
       </c>
       <c r="F211" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="212" ht="25" customHeight="1">
       <c r="A212" s="3" t="inlineStr">
         <is>
-          <t>Venter</t>
+          <t>Van de Merwe</t>
         </is>
       </c>
       <c r="B212" s="3" t="inlineStr">
         <is>
-          <t>Louis</t>
+          <t>Marina</t>
         </is>
       </c>
       <c r="C212" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Malmesbury</t>
         </is>
       </c>
       <c r="D212" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E212" s="3" t="inlineStr">
@@ -7203,34 +7203,34 @@
       </c>
       <c r="F212" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="213" ht="25" customHeight="1">
       <c r="A213" s="3" t="inlineStr">
         <is>
-          <t>Volker</t>
+          <t>Venter</t>
         </is>
       </c>
       <c r="B213" s="3" t="inlineStr">
         <is>
-          <t>Russell</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="C213" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D213" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E213" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F213" s="3" t="inlineStr">
@@ -7242,96 +7242,96 @@
     <row r="214" ht="25" customHeight="1">
       <c r="A214" s="3" t="inlineStr">
         <is>
-          <t>Von Mollendorf</t>
+          <t>Volker</t>
         </is>
       </c>
       <c r="B214" s="3" t="inlineStr">
         <is>
-          <t>Rinette</t>
+          <t>Russell</t>
         </is>
       </c>
       <c r="C214" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>King William's Town</t>
         </is>
       </c>
       <c r="D214" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E214" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F214" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="215" ht="25" customHeight="1">
       <c r="A215" s="3" t="inlineStr">
         <is>
-          <t>Warman</t>
+          <t>Von Mollendorf</t>
         </is>
       </c>
       <c r="B215" s="3" t="inlineStr">
         <is>
-          <t>Alastair</t>
+          <t>Rinette</t>
         </is>
       </c>
       <c r="C215" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Durbanville</t>
         </is>
       </c>
       <c r="D215" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E215" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F215" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="216" ht="25" customHeight="1">
       <c r="A216" s="3" t="inlineStr">
         <is>
-          <t>Watson</t>
+          <t>Warman</t>
         </is>
       </c>
       <c r="B216" s="3" t="inlineStr">
         <is>
-          <t>Allan</t>
+          <t>Alastair</t>
         </is>
       </c>
       <c r="C216" s="3" t="inlineStr">
         <is>
-          <t>Sea Point</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D216" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E216" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F216" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -7343,22 +7343,22 @@
       </c>
       <c r="B217" s="3" t="inlineStr">
         <is>
-          <t>Alison</t>
+          <t>Allan</t>
         </is>
       </c>
       <c r="C217" s="3" t="inlineStr">
         <is>
-          <t>Sedgefield</t>
+          <t>Sea Point</t>
         </is>
       </c>
       <c r="D217" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E217" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F217" s="3" t="inlineStr">
@@ -7370,27 +7370,27 @@
     <row r="218" ht="25" customHeight="1">
       <c r="A218" s="3" t="inlineStr">
         <is>
-          <t>Williams</t>
+          <t>Watson</t>
         </is>
       </c>
       <c r="B218" s="3" t="inlineStr">
         <is>
-          <t>Johanna</t>
+          <t>Alison</t>
         </is>
       </c>
       <c r="C218" s="3" t="inlineStr">
         <is>
-          <t>Mitchells Plain</t>
+          <t>Sedgefield</t>
         </is>
       </c>
       <c r="D218" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E218" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F218" s="3" t="inlineStr">
@@ -7402,22 +7402,22 @@
     <row r="219" ht="25" customHeight="1">
       <c r="A219" s="3" t="inlineStr">
         <is>
-          <t>Wills</t>
+          <t>Williams</t>
         </is>
       </c>
       <c r="B219" s="3" t="inlineStr">
         <is>
-          <t>Geila</t>
+          <t>Johanna</t>
         </is>
       </c>
       <c r="C219" s="3" t="inlineStr">
         <is>
-          <t>Athlone</t>
+          <t>Mitchells Plain</t>
         </is>
       </c>
       <c r="D219" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E219" s="3" t="inlineStr">
@@ -7434,17 +7434,17 @@
     <row r="220" ht="25" customHeight="1">
       <c r="A220" s="3" t="inlineStr">
         <is>
-          <t>Wilter-Sturges</t>
+          <t>Wills</t>
         </is>
       </c>
       <c r="B220" s="3" t="inlineStr">
         <is>
-          <t>Meredith</t>
+          <t>Geila</t>
         </is>
       </c>
       <c r="C220" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Athlone</t>
         </is>
       </c>
       <c r="D220" s="3" t="inlineStr">
@@ -7459,24 +7459,24 @@
       </c>
       <c r="F220" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="221" ht="25" customHeight="1">
       <c r="A221" s="3" t="inlineStr">
         <is>
-          <t>Wright</t>
+          <t>Wilter-Sturges</t>
         </is>
       </c>
       <c r="B221" s="3" t="inlineStr">
         <is>
-          <t>Rocky</t>
+          <t>Meredith</t>
         </is>
       </c>
       <c r="C221" s="3" t="inlineStr">
         <is>
-          <t>Table View</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D221" s="3" t="inlineStr">
@@ -7486,29 +7486,29 @@
       </c>
       <c r="E221" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F221" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="222" ht="25" customHeight="1">
       <c r="A222" s="3" t="inlineStr">
         <is>
-          <t>Young</t>
+          <t>Wright</t>
         </is>
       </c>
       <c r="B222" s="3" t="inlineStr">
         <is>
-          <t>Judy</t>
+          <t>Rocky</t>
         </is>
       </c>
       <c r="C222" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>Table View</t>
         </is>
       </c>
       <c r="D222" s="3" t="inlineStr">
@@ -7518,7 +7518,7 @@
       </c>
       <c r="E222" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F222" s="3" t="inlineStr">
@@ -7530,17 +7530,17 @@
     <row r="223" ht="25" customHeight="1">
       <c r="A223" s="3" t="inlineStr">
         <is>
-          <t>de Kock</t>
+          <t>Young</t>
         </is>
       </c>
       <c r="B223" s="3" t="inlineStr">
         <is>
-          <t>Engela</t>
+          <t>Judy</t>
         </is>
       </c>
       <c r="C223" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Durbanville</t>
         </is>
       </c>
       <c r="D223" s="3" t="inlineStr">
@@ -7550,7 +7550,7 @@
       </c>
       <c r="E223" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F223" s="3" t="inlineStr">
@@ -7567,7 +7567,7 @@
       </c>
       <c r="B224" s="3" t="inlineStr">
         <is>
-          <t>Francois</t>
+          <t>Engela</t>
         </is>
       </c>
       <c r="C224" s="3" t="inlineStr">
@@ -7594,59 +7594,59 @@
     <row r="225" ht="25" customHeight="1">
       <c r="A225" s="3" t="inlineStr">
         <is>
-          <t>de Silva</t>
+          <t>de Kock</t>
         </is>
       </c>
       <c r="B225" s="3" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Francois</t>
         </is>
       </c>
       <c r="C225" s="3" t="inlineStr">
         <is>
-          <t>Edenvale</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D225" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E225" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F225" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="226" ht="25" customHeight="1">
       <c r="A226" s="3" t="inlineStr">
         <is>
-          <t>du Plooy</t>
+          <t>de Silva</t>
         </is>
       </c>
       <c r="B226" s="3" t="inlineStr">
         <is>
-          <t>Tammy</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="C226" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Edenvale</t>
         </is>
       </c>
       <c r="D226" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E226" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F226" s="3" t="inlineStr">
@@ -7663,7 +7663,7 @@
       </c>
       <c r="B227" s="3" t="inlineStr">
         <is>
-          <t>Marc</t>
+          <t>Tammy</t>
         </is>
       </c>
       <c r="C227" s="3" t="inlineStr">
@@ -7690,17 +7690,17 @@
     <row r="228" ht="25" customHeight="1">
       <c r="A228" s="3" t="inlineStr">
         <is>
-          <t>du Toit</t>
+          <t>du Plooy</t>
         </is>
       </c>
       <c r="B228" s="3" t="inlineStr">
         <is>
-          <t>Desiree</t>
+          <t>Marc</t>
         </is>
       </c>
       <c r="C228" s="3" t="inlineStr">
         <is>
-          <t>Ramsgate</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D228" s="3" t="inlineStr">
@@ -7722,22 +7722,22 @@
     <row r="229" ht="25" customHeight="1">
       <c r="A229" s="3" t="inlineStr">
         <is>
-          <t>stier</t>
+          <t>du Toit</t>
         </is>
       </c>
       <c r="B229" s="3" t="inlineStr">
         <is>
-          <t>RORY</t>
+          <t>Desiree</t>
         </is>
       </c>
       <c r="C229" s="3" t="inlineStr">
         <is>
-          <t>Deep South</t>
+          <t>Ramsgate</t>
         </is>
       </c>
       <c r="D229" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E229" s="3" t="inlineStr">
@@ -7747,56 +7747,56 @@
       </c>
       <c r="F229" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="230" ht="25" customHeight="1">
       <c r="A230" s="3" t="inlineStr">
         <is>
-          <t>tyler</t>
+          <t>stier</t>
         </is>
       </c>
       <c r="B230" s="3" t="inlineStr">
         <is>
-          <t>natascha</t>
+          <t>RORY</t>
         </is>
       </c>
       <c r="C230" s="3" t="inlineStr">
         <is>
-          <t>Kensington</t>
+          <t>Deep South</t>
         </is>
       </c>
       <c r="D230" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E230" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F230" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="231" ht="25" customHeight="1">
       <c r="A231" s="3" t="inlineStr">
         <is>
-          <t>van Blerk</t>
+          <t>tyler</t>
         </is>
       </c>
       <c r="B231" s="3" t="inlineStr">
         <is>
-          <t>Carl</t>
+          <t>natascha</t>
         </is>
       </c>
       <c r="C231" s="3" t="inlineStr">
         <is>
-          <t>Eden</t>
+          <t>Kensington</t>
         </is>
       </c>
       <c r="D231" s="3" t="inlineStr">
@@ -7811,24 +7811,24 @@
       </c>
       <c r="F231" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="232" ht="25" customHeight="1">
       <c r="A232" s="3" t="inlineStr">
         <is>
-          <t>van Heerden</t>
+          <t>van Blerk</t>
         </is>
       </c>
       <c r="B232" s="3" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Carl</t>
         </is>
       </c>
       <c r="C232" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Eden</t>
         </is>
       </c>
       <c r="D232" s="3" t="inlineStr">
@@ -7843,7 +7843,7 @@
       </c>
       <c r="F232" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -7855,7 +7855,7 @@
       </c>
       <c r="B233" s="3" t="inlineStr">
         <is>
-          <t>Sandy</t>
+          <t>Sydney</t>
         </is>
       </c>
       <c r="C233" s="3" t="inlineStr">
@@ -7870,7 +7870,7 @@
       </c>
       <c r="E233" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F233" s="3" t="inlineStr">
@@ -7887,17 +7887,17 @@
       </c>
       <c r="B234" s="3" t="inlineStr">
         <is>
-          <t>Craig</t>
+          <t>Sandy</t>
         </is>
       </c>
       <c r="C234" s="3" t="inlineStr">
         <is>
-          <t>East London Beacon Bay</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D234" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E234" s="3" t="inlineStr">
@@ -7919,17 +7919,17 @@
       </c>
       <c r="B235" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Craig</t>
         </is>
       </c>
       <c r="C235" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>East London Beacon Bay</t>
         </is>
       </c>
       <c r="D235" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E235" s="3" t="inlineStr">
@@ -7946,17 +7946,17 @@
     <row r="236" ht="25" customHeight="1">
       <c r="A236" s="3" t="inlineStr">
         <is>
-          <t>van Rensburg</t>
+          <t>van Heerden</t>
         </is>
       </c>
       <c r="B236" s="3" t="inlineStr">
         <is>
-          <t>Johan</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C236" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D236" s="3" t="inlineStr">
@@ -7966,12 +7966,12 @@
       </c>
       <c r="E236" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F236" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -7983,7 +7983,7 @@
       </c>
       <c r="B237" s="3" t="inlineStr">
         <is>
-          <t>Anne</t>
+          <t>Johan</t>
         </is>
       </c>
       <c r="C237" s="3" t="inlineStr">
@@ -8010,17 +8010,17 @@
     <row r="238" ht="25" customHeight="1">
       <c r="A238" s="3" t="inlineStr">
         <is>
-          <t>van Wulven</t>
+          <t>van Rensburg</t>
         </is>
       </c>
       <c r="B238" s="3" t="inlineStr">
         <is>
-          <t>Jeannie</t>
+          <t>Anne</t>
         </is>
       </c>
       <c r="C238" s="3" t="inlineStr">
         <is>
-          <t>Tygerberg Hills</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D238" s="3" t="inlineStr">
@@ -8030,7 +8030,7 @@
       </c>
       <c r="E238" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F238" s="3" t="inlineStr">
@@ -8047,7 +8047,7 @@
       </c>
       <c r="B239" s="3" t="inlineStr">
         <is>
-          <t>Alan</t>
+          <t>Jeannie</t>
         </is>
       </c>
       <c r="C239" s="3" t="inlineStr">
@@ -8062,7 +8062,7 @@
       </c>
       <c r="E239" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F239" s="3" t="inlineStr">
@@ -8079,7 +8079,7 @@
       </c>
       <c r="B240" s="3" t="inlineStr">
         <is>
-          <t>Deon</t>
+          <t>Alan</t>
         </is>
       </c>
       <c r="C240" s="3" t="inlineStr">
@@ -8106,17 +8106,17 @@
     <row r="241" ht="25" customHeight="1">
       <c r="A241" s="3" t="inlineStr">
         <is>
-          <t>van Wyk</t>
+          <t>van Wulven</t>
         </is>
       </c>
       <c r="B241" s="3" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>Deon</t>
         </is>
       </c>
       <c r="C241" s="3" t="inlineStr">
         <is>
-          <t>North Durban</t>
+          <t>Tygerberg Hills</t>
         </is>
       </c>
       <c r="D241" s="3" t="inlineStr">
@@ -8131,7 +8131,7 @@
       </c>
       <c r="F241" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -8143,12 +8143,12 @@
       </c>
       <c r="B242" s="3" t="inlineStr">
         <is>
-          <t>Lindie</t>
+          <t>Kim</t>
         </is>
       </c>
       <c r="C242" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>North Durban</t>
         </is>
       </c>
       <c r="D242" s="3" t="inlineStr">
@@ -8175,12 +8175,12 @@
       </c>
       <c r="B243" s="3" t="inlineStr">
         <is>
-          <t>Willem</t>
+          <t>Lindie</t>
         </is>
       </c>
       <c r="C243" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D243" s="3" t="inlineStr">
@@ -8207,12 +8207,12 @@
       </c>
       <c r="B244" s="3" t="inlineStr">
         <is>
-          <t>Patricia</t>
+          <t>Willem</t>
         </is>
       </c>
       <c r="C244" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D244" s="3" t="inlineStr">
@@ -8234,22 +8234,22 @@
     <row r="245" ht="25" customHeight="1">
       <c r="A245" s="3" t="inlineStr">
         <is>
-          <t>van der Merwe</t>
+          <t>van Wyk</t>
         </is>
       </c>
       <c r="B245" s="3" t="inlineStr">
         <is>
-          <t>Ingrid</t>
+          <t>Patricia</t>
         </is>
       </c>
       <c r="C245" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D245" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E245" s="3" t="inlineStr">
@@ -8266,49 +8266,49 @@
     <row r="246" ht="25" customHeight="1">
       <c r="A246" s="3" t="inlineStr">
         <is>
-          <t>van der Westhuizen</t>
+          <t>van der Merwe</t>
         </is>
       </c>
       <c r="B246" s="3" t="inlineStr">
         <is>
-          <t>Hennie</t>
+          <t>Ingrid</t>
         </is>
       </c>
       <c r="C246" s="3" t="inlineStr">
         <is>
-          <t>Helderberg</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D246" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E246" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F246" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="247" ht="25" customHeight="1">
       <c r="A247" s="3" t="inlineStr">
         <is>
-          <t>von der Decken</t>
+          <t>van der Westhuizen</t>
         </is>
       </c>
       <c r="B247" s="3" t="inlineStr">
         <is>
-          <t>Brian</t>
+          <t>Hennie</t>
         </is>
       </c>
       <c r="C247" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Helderberg</t>
         </is>
       </c>
       <c r="D247" s="3" t="inlineStr">
@@ -8323,51 +8323,83 @@
       </c>
       <c r="F247" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="248" ht="25" customHeight="1">
       <c r="A248" s="3" t="inlineStr">
         <is>
+          <t>von der Decken</t>
+        </is>
+      </c>
+      <c r="B248" s="3" t="inlineStr">
+        <is>
+          <t>Brian</t>
+        </is>
+      </c>
+      <c r="C248" s="3" t="inlineStr">
+        <is>
+          <t>King William's Town</t>
+        </is>
+      </c>
+      <c r="D248" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E248" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F248" s="3" t="inlineStr">
+        <is>
+          <t>410E</t>
+        </is>
+      </c>
+    </row>
+    <row r="249" ht="25" customHeight="1">
+      <c r="A249" s="3" t="inlineStr">
+        <is>
           <t>‘t Hart</t>
         </is>
       </c>
-      <c r="B248" s="3" t="inlineStr">
+      <c r="B249" s="3" t="inlineStr">
         <is>
           <t>Michelle</t>
         </is>
       </c>
-      <c r="C248" s="3" t="inlineStr">
+      <c r="C249" s="3" t="inlineStr">
         <is>
           <t>Benoni Lakes</t>
         </is>
       </c>
-      <c r="D248" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E248" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F248" s="3" t="inlineStr">
+      <c r="D249" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E249" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F249" s="3" t="inlineStr">
         <is>
           <t>410E</t>
-        </is>
-      </c>
-    </row>
-    <row r="249">
-      <c r="A249" s="1" t="inlineStr">
-        <is>
-          <t>Number of attendees: 246</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="inlineStr">
+        <is>
+          <t>Number of attendees: 247</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" s="1" t="inlineStr">
         <is>
           <t>Number of voters: 98</t>
         </is>
@@ -8403,7 +8435,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Registrees as of 30/04/2021 13:35</t>
+          <t>410E Registrees as of 30/04/2021 17:39</t>
         </is>
       </c>
     </row>
@@ -11988,7 +12020,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Registrees as of 30/04/2021 13:35</t>
+          <t>410W Registrees as of 30/04/2021 17:39</t>
         </is>
       </c>
     </row>
@@ -16164,7 +16196,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Voting details as of 30/04/2021 13:35</t>
+          <t>410E Voting details as of 30/04/2021 17:39</t>
         </is>
       </c>
     </row>
@@ -16541,7 +16573,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Voting details as of 30/04/2021 13:35</t>
+          <t>410W Voting details as of 30/04/2021 17:39</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Registree stats backup on Sat 01 May 2021 07:39:28 SAST
</commit_message>
<xml_diff>
--- a/static/docs/registrees_list.xlsx
+++ b/static/docs/registrees_list.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F253"/>
+  <dimension ref="A1:F254"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,7 +451,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>MD410 Registrees as of 30/04/2021 21:18</t>
+          <t>MD410 Registrees as of 01/05/2021 07:39</t>
         </is>
       </c>
     </row>
@@ -6154,22 +6154,22 @@
     <row r="180" ht="25" customHeight="1">
       <c r="A180" s="3" t="inlineStr">
         <is>
-          <t>Sircoulomb</t>
+          <t>Singh</t>
         </is>
       </c>
       <c r="B180" s="3" t="inlineStr">
         <is>
-          <t>Kenlis</t>
+          <t>Niroshni</t>
         </is>
       </c>
       <c r="C180" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>East Coast</t>
         </is>
       </c>
       <c r="D180" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E180" s="3" t="inlineStr">
@@ -6179,7 +6179,7 @@
       </c>
       <c r="F180" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -6191,7 +6191,7 @@
       </c>
       <c r="B181" s="3" t="inlineStr">
         <is>
-          <t>Holger</t>
+          <t>Kenlis</t>
         </is>
       </c>
       <c r="C181" s="3" t="inlineStr">
@@ -6206,7 +6206,7 @@
       </c>
       <c r="E181" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F181" s="3" t="inlineStr">
@@ -6218,12 +6218,12 @@
     <row r="182" ht="25" customHeight="1">
       <c r="A182" s="3" t="inlineStr">
         <is>
-          <t>Smeer</t>
+          <t>Sircoulomb</t>
         </is>
       </c>
       <c r="B182" s="3" t="inlineStr">
         <is>
-          <t>Hennie</t>
+          <t>Holger</t>
         </is>
       </c>
       <c r="C182" s="3" t="inlineStr">
@@ -6233,12 +6233,12 @@
       </c>
       <c r="D182" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E182" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F182" s="3" t="inlineStr">
@@ -6250,22 +6250,22 @@
     <row r="183" ht="25" customHeight="1">
       <c r="A183" s="3" t="inlineStr">
         <is>
-          <t>Smit</t>
+          <t>Smeer</t>
         </is>
       </c>
       <c r="B183" s="3" t="inlineStr">
         <is>
-          <t>Sue</t>
+          <t>Hennie</t>
         </is>
       </c>
       <c r="C183" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D183" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E183" s="3" t="inlineStr">
@@ -6275,7 +6275,7 @@
       </c>
       <c r="F183" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -6287,12 +6287,12 @@
       </c>
       <c r="B184" s="3" t="inlineStr">
         <is>
-          <t>Herman</t>
+          <t>Sue</t>
         </is>
       </c>
       <c r="C184" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D184" s="3" t="inlineStr">
@@ -6307,7 +6307,7 @@
       </c>
       <c r="F184" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -6319,17 +6319,17 @@
       </c>
       <c r="B185" s="3" t="inlineStr">
         <is>
-          <t>Juanita</t>
+          <t>Herman</t>
         </is>
       </c>
       <c r="C185" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D185" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E185" s="3" t="inlineStr">
@@ -6339,29 +6339,29 @@
       </c>
       <c r="F185" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="186" ht="25" customHeight="1">
       <c r="A186" s="3" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Smit</t>
         </is>
       </c>
       <c r="B186" s="3" t="inlineStr">
         <is>
-          <t>Jeff</t>
+          <t>Juanita</t>
         </is>
       </c>
       <c r="C186" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D186" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E186" s="3" t="inlineStr">
@@ -6383,12 +6383,12 @@
       </c>
       <c r="B187" s="3" t="inlineStr">
         <is>
-          <t>Bennie</t>
+          <t>Jeff</t>
         </is>
       </c>
       <c r="C187" s="3" t="inlineStr">
         <is>
-          <t>Wellington</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D187" s="3" t="inlineStr">
@@ -6398,12 +6398,12 @@
       </c>
       <c r="E187" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F187" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -6415,12 +6415,12 @@
       </c>
       <c r="B188" s="3" t="inlineStr">
         <is>
-          <t>Carmen Dolores</t>
+          <t>Bennie</t>
         </is>
       </c>
       <c r="C188" s="3" t="inlineStr">
         <is>
-          <t>Tokai</t>
+          <t>Wellington</t>
         </is>
       </c>
       <c r="D188" s="3" t="inlineStr">
@@ -6430,7 +6430,7 @@
       </c>
       <c r="E188" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F188" s="3" t="inlineStr">
@@ -6447,7 +6447,7 @@
       </c>
       <c r="B189" s="3" t="inlineStr">
         <is>
-          <t>David John</t>
+          <t>Carmen Dolores</t>
         </is>
       </c>
       <c r="C189" s="3" t="inlineStr">
@@ -6474,17 +6474,17 @@
     <row r="190" ht="25" customHeight="1">
       <c r="A190" s="3" t="inlineStr">
         <is>
-          <t>Sochen</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="B190" s="3" t="inlineStr">
         <is>
-          <t>Diana</t>
+          <t>David John</t>
         </is>
       </c>
       <c r="C190" s="3" t="inlineStr">
         <is>
-          <t>Sea Point</t>
+          <t>Tokai</t>
         </is>
       </c>
       <c r="D190" s="3" t="inlineStr">
@@ -6494,7 +6494,7 @@
       </c>
       <c r="E190" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F190" s="3" t="inlineStr">
@@ -6506,49 +6506,49 @@
     <row r="191" ht="25" customHeight="1">
       <c r="A191" s="3" t="inlineStr">
         <is>
-          <t>Steyn</t>
+          <t>Sochen</t>
         </is>
       </c>
       <c r="B191" s="3" t="inlineStr">
         <is>
-          <t>Elna</t>
+          <t>Diana</t>
         </is>
       </c>
       <c r="C191" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Sea Point</t>
         </is>
       </c>
       <c r="D191" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E191" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F191" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="192" ht="25" customHeight="1">
       <c r="A192" s="3" t="inlineStr">
         <is>
-          <t>Strauss</t>
+          <t>Steyn</t>
         </is>
       </c>
       <c r="B192" s="3" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>Elna</t>
         </is>
       </c>
       <c r="C192" s="3" t="inlineStr">
         <is>
-          <t>Kuilsriver</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D192" s="3" t="inlineStr">
@@ -6563,29 +6563,29 @@
       </c>
       <c r="F192" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="193" ht="25" customHeight="1">
       <c r="A193" s="3" t="inlineStr">
         <is>
-          <t>Strydom</t>
+          <t>Strauss</t>
         </is>
       </c>
       <c r="B193" s="3" t="inlineStr">
         <is>
-          <t>Melinda Lee</t>
+          <t>Patrick</t>
         </is>
       </c>
       <c r="C193" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Kuilsriver</t>
         </is>
       </c>
       <c r="D193" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E193" s="3" t="inlineStr">
@@ -6595,24 +6595,24 @@
       </c>
       <c r="F193" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="194" ht="25" customHeight="1">
       <c r="A194" s="3" t="inlineStr">
         <is>
-          <t>Sturges</t>
+          <t>Strydom</t>
         </is>
       </c>
       <c r="B194" s="3" t="inlineStr">
         <is>
-          <t>Trevor</t>
+          <t>Melinda Lee</t>
         </is>
       </c>
       <c r="C194" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D194" s="3" t="inlineStr">
@@ -6634,17 +6634,17 @@
     <row r="195" ht="25" customHeight="1">
       <c r="A195" s="3" t="inlineStr">
         <is>
-          <t>Talbot</t>
+          <t>Sturges</t>
         </is>
       </c>
       <c r="B195" s="3" t="inlineStr">
         <is>
-          <t>Lauryn</t>
+          <t>Trevor</t>
         </is>
       </c>
       <c r="C195" s="3" t="inlineStr">
         <is>
-          <t>Benoni Lakes</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D195" s="3" t="inlineStr">
@@ -6666,17 +6666,17 @@
     <row r="196" ht="25" customHeight="1">
       <c r="A196" s="3" t="inlineStr">
         <is>
-          <t>Theron</t>
+          <t>Talbot</t>
         </is>
       </c>
       <c r="B196" s="3" t="inlineStr">
         <is>
-          <t>Pierre</t>
+          <t>Lauryn</t>
         </is>
       </c>
       <c r="C196" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Benoni Lakes</t>
         </is>
       </c>
       <c r="D196" s="3" t="inlineStr">
@@ -6703,7 +6703,7 @@
       </c>
       <c r="B197" s="3" t="inlineStr">
         <is>
-          <t>Moira</t>
+          <t>Pierre</t>
         </is>
       </c>
       <c r="C197" s="3" t="inlineStr">
@@ -6730,17 +6730,17 @@
     <row r="198" ht="25" customHeight="1">
       <c r="A198" s="3" t="inlineStr">
         <is>
-          <t>Townsend</t>
+          <t>Theron</t>
         </is>
       </c>
       <c r="B198" s="3" t="inlineStr">
         <is>
-          <t>Diane</t>
+          <t>Moira</t>
         </is>
       </c>
       <c r="C198" s="3" t="inlineStr">
         <is>
-          <t>Benoni Lakes</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D198" s="3" t="inlineStr">
@@ -6750,7 +6750,7 @@
       </c>
       <c r="E198" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F198" s="3" t="inlineStr">
@@ -6762,27 +6762,27 @@
     <row r="199" ht="25" customHeight="1">
       <c r="A199" s="3" t="inlineStr">
         <is>
-          <t>Toye</t>
+          <t>Townsend</t>
         </is>
       </c>
       <c r="B199" s="3" t="inlineStr">
         <is>
-          <t>Omolayo</t>
+          <t>Diane</t>
         </is>
       </c>
       <c r="C199" s="3" t="inlineStr">
         <is>
-          <t>The Wilds</t>
+          <t>Benoni Lakes</t>
         </is>
       </c>
       <c r="D199" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E199" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F199" s="3" t="inlineStr">
@@ -6794,22 +6794,22 @@
     <row r="200" ht="25" customHeight="1">
       <c r="A200" s="3" t="inlineStr">
         <is>
-          <t>Tshikala</t>
+          <t>Toye</t>
         </is>
       </c>
       <c r="B200" s="3" t="inlineStr">
         <is>
-          <t>David Alex</t>
+          <t>Omolayo</t>
         </is>
       </c>
       <c r="C200" s="3" t="inlineStr">
         <is>
-          <t>Athlone</t>
+          <t>The Wilds</t>
         </is>
       </c>
       <c r="D200" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E200" s="3" t="inlineStr">
@@ -6819,24 +6819,24 @@
       </c>
       <c r="F200" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="201" ht="25" customHeight="1">
       <c r="A201" s="3" t="inlineStr">
         <is>
-          <t>Tuckett</t>
+          <t>Tshikala</t>
         </is>
       </c>
       <c r="B201" s="3" t="inlineStr">
         <is>
-          <t>Alistair</t>
+          <t>David Alex</t>
         </is>
       </c>
       <c r="C201" s="3" t="inlineStr">
         <is>
-          <t>Roodepoort Clearwater Cyber</t>
+          <t>Athlone</t>
         </is>
       </c>
       <c r="D201" s="3" t="inlineStr">
@@ -6851,7 +6851,7 @@
       </c>
       <c r="F201" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -6863,7 +6863,7 @@
       </c>
       <c r="B202" s="3" t="inlineStr">
         <is>
-          <t>Rowan</t>
+          <t>Alistair</t>
         </is>
       </c>
       <c r="C202" s="3" t="inlineStr">
@@ -6878,7 +6878,7 @@
       </c>
       <c r="E202" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F202" s="3" t="inlineStr">
@@ -6895,7 +6895,7 @@
       </c>
       <c r="B203" s="3" t="inlineStr">
         <is>
-          <t>Gail</t>
+          <t>Rowan</t>
         </is>
       </c>
       <c r="C203" s="3" t="inlineStr">
@@ -6910,7 +6910,7 @@
       </c>
       <c r="E203" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F203" s="3" t="inlineStr">
@@ -6922,17 +6922,17 @@
     <row r="204" ht="25" customHeight="1">
       <c r="A204" s="3" t="inlineStr">
         <is>
-          <t>VAN BREDA</t>
+          <t>Tuckett</t>
         </is>
       </c>
       <c r="B204" s="3" t="inlineStr">
         <is>
-          <t>HILARY LISE</t>
+          <t>Gail</t>
         </is>
       </c>
       <c r="C204" s="3" t="inlineStr">
         <is>
-          <t>Cape Town</t>
+          <t>Roodepoort Clearwater Cyber</t>
         </is>
       </c>
       <c r="D204" s="3" t="inlineStr">
@@ -6947,39 +6947,39 @@
       </c>
       <c r="F204" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="205" ht="25" customHeight="1">
       <c r="A205" s="3" t="inlineStr">
         <is>
-          <t>VAN DER MERWE</t>
+          <t>VAN BREDA</t>
         </is>
       </c>
       <c r="B205" s="3" t="inlineStr">
         <is>
-          <t>PATRICIA</t>
+          <t>HILARY LISE</t>
         </is>
       </c>
       <c r="C205" s="3" t="inlineStr">
         <is>
-          <t>East London Port Rex</t>
+          <t>Cape Town</t>
         </is>
       </c>
       <c r="D205" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E205" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F205" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -6991,17 +6991,17 @@
       </c>
       <c r="B206" s="3" t="inlineStr">
         <is>
-          <t>MARINA</t>
+          <t>PATRICIA</t>
         </is>
       </c>
       <c r="C206" s="3" t="inlineStr">
         <is>
-          <t>Malmesbury</t>
+          <t>East London Port Rex</t>
         </is>
       </c>
       <c r="D206" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E206" s="3" t="inlineStr">
@@ -7011,56 +7011,56 @@
       </c>
       <c r="F206" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="207" ht="25" customHeight="1">
       <c r="A207" s="3" t="inlineStr">
         <is>
-          <t>Valadao</t>
+          <t>VAN DER MERWE</t>
         </is>
       </c>
       <c r="B207" s="3" t="inlineStr">
         <is>
-          <t>Tracy</t>
+          <t>MARINA</t>
         </is>
       </c>
       <c r="C207" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Malmesbury</t>
         </is>
       </c>
       <c r="D207" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E207" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F207" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="208" ht="25" customHeight="1">
       <c r="A208" s="3" t="inlineStr">
         <is>
-          <t>Van Niekerk</t>
+          <t>Valadao</t>
         </is>
       </c>
       <c r="B208" s="3" t="inlineStr">
         <is>
-          <t>Riaan</t>
+          <t>Tracy</t>
         </is>
       </c>
       <c r="C208" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D208" s="3" t="inlineStr">
@@ -7082,22 +7082,22 @@
     <row r="209" ht="25" customHeight="1">
       <c r="A209" s="3" t="inlineStr">
         <is>
-          <t>Van Nieuwenhuyzen</t>
+          <t>Van Niekerk</t>
         </is>
       </c>
       <c r="B209" s="3" t="inlineStr">
         <is>
-          <t>Hilgardt</t>
+          <t>Riaan</t>
         </is>
       </c>
       <c r="C209" s="3" t="inlineStr">
         <is>
-          <t>Worcester</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D209" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E209" s="3" t="inlineStr">
@@ -7107,24 +7107,24 @@
       </c>
       <c r="F209" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="210" ht="25" customHeight="1">
       <c r="A210" s="3" t="inlineStr">
         <is>
-          <t>Van Rensburg</t>
+          <t>Van Nieuwenhuyzen</t>
         </is>
       </c>
       <c r="B210" s="3" t="inlineStr">
         <is>
-          <t>Neville</t>
+          <t>Hilgardt</t>
         </is>
       </c>
       <c r="C210" s="3" t="inlineStr">
         <is>
-          <t>Moorreesburg</t>
+          <t>Worcester</t>
         </is>
       </c>
       <c r="D210" s="3" t="inlineStr">
@@ -7134,7 +7134,7 @@
       </c>
       <c r="E210" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F210" s="3" t="inlineStr">
@@ -7146,27 +7146,27 @@
     <row r="211" ht="25" customHeight="1">
       <c r="A211" s="3" t="inlineStr">
         <is>
-          <t>Van Romburgh</t>
+          <t>Van Rensburg</t>
         </is>
       </c>
       <c r="B211" s="3" t="inlineStr">
         <is>
-          <t>Lorna</t>
+          <t>Neville</t>
         </is>
       </c>
       <c r="C211" s="3" t="inlineStr">
         <is>
-          <t>Fish Hoek</t>
+          <t>Moorreesburg</t>
         </is>
       </c>
       <c r="D211" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E211" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F211" s="3" t="inlineStr">
@@ -7178,17 +7178,17 @@
     <row r="212" ht="25" customHeight="1">
       <c r="A212" s="3" t="inlineStr">
         <is>
-          <t>Van Wyk-Nelson</t>
+          <t>Van Romburgh</t>
         </is>
       </c>
       <c r="B212" s="3" t="inlineStr">
         <is>
-          <t>Edith</t>
+          <t>Lorna</t>
         </is>
       </c>
       <c r="C212" s="3" t="inlineStr">
         <is>
-          <t>Kuilsriver</t>
+          <t>Fish Hoek</t>
         </is>
       </c>
       <c r="D212" s="3" t="inlineStr">
@@ -7210,17 +7210,17 @@
     <row r="213" ht="25" customHeight="1">
       <c r="A213" s="3" t="inlineStr">
         <is>
-          <t>Van Zyl</t>
+          <t>Van Wyk-Nelson</t>
         </is>
       </c>
       <c r="B213" s="3" t="inlineStr">
         <is>
-          <t>Louis</t>
+          <t>Edith</t>
         </is>
       </c>
       <c r="C213" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Kuilsriver</t>
         </is>
       </c>
       <c r="D213" s="3" t="inlineStr">
@@ -7235,29 +7235,29 @@
       </c>
       <c r="F213" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="214" ht="25" customHeight="1">
       <c r="A214" s="3" t="inlineStr">
         <is>
-          <t>Van de Merwe</t>
+          <t>Van Zyl</t>
         </is>
       </c>
       <c r="B214" s="3" t="inlineStr">
         <is>
-          <t>Marina</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="C214" s="3" t="inlineStr">
         <is>
-          <t>Malmesbury</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D214" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E214" s="3" t="inlineStr">
@@ -7267,29 +7267,29 @@
       </c>
       <c r="F214" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="215" ht="25" customHeight="1">
       <c r="A215" s="3" t="inlineStr">
         <is>
-          <t>Venter</t>
+          <t>Van de Merwe</t>
         </is>
       </c>
       <c r="B215" s="3" t="inlineStr">
         <is>
-          <t>Louis</t>
+          <t>Marina</t>
         </is>
       </c>
       <c r="C215" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Malmesbury</t>
         </is>
       </c>
       <c r="D215" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E215" s="3" t="inlineStr">
@@ -7299,34 +7299,34 @@
       </c>
       <c r="F215" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="216" ht="25" customHeight="1">
       <c r="A216" s="3" t="inlineStr">
         <is>
-          <t>Volker</t>
+          <t>Venter</t>
         </is>
       </c>
       <c r="B216" s="3" t="inlineStr">
         <is>
-          <t>Russell</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="C216" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D216" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E216" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F216" s="3" t="inlineStr">
@@ -7338,96 +7338,96 @@
     <row r="217" ht="25" customHeight="1">
       <c r="A217" s="3" t="inlineStr">
         <is>
-          <t>Von Mollendorf</t>
+          <t>Volker</t>
         </is>
       </c>
       <c r="B217" s="3" t="inlineStr">
         <is>
-          <t>Rinette</t>
+          <t>Russell</t>
         </is>
       </c>
       <c r="C217" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>King William's Town</t>
         </is>
       </c>
       <c r="D217" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E217" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F217" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="218" ht="25" customHeight="1">
       <c r="A218" s="3" t="inlineStr">
         <is>
-          <t>Warman</t>
+          <t>Von Mollendorf</t>
         </is>
       </c>
       <c r="B218" s="3" t="inlineStr">
         <is>
-          <t>Alastair</t>
+          <t>Rinette</t>
         </is>
       </c>
       <c r="C218" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Durbanville</t>
         </is>
       </c>
       <c r="D218" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E218" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F218" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="219" ht="25" customHeight="1">
       <c r="A219" s="3" t="inlineStr">
         <is>
-          <t>Watson</t>
+          <t>Warman</t>
         </is>
       </c>
       <c r="B219" s="3" t="inlineStr">
         <is>
-          <t>Allan</t>
+          <t>Alastair</t>
         </is>
       </c>
       <c r="C219" s="3" t="inlineStr">
         <is>
-          <t>Sea Point</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D219" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E219" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F219" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -7439,22 +7439,22 @@
       </c>
       <c r="B220" s="3" t="inlineStr">
         <is>
-          <t>Alison</t>
+          <t>Allan</t>
         </is>
       </c>
       <c r="C220" s="3" t="inlineStr">
         <is>
-          <t>Sedgefield</t>
+          <t>Sea Point</t>
         </is>
       </c>
       <c r="D220" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E220" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F220" s="3" t="inlineStr">
@@ -7466,27 +7466,27 @@
     <row r="221" ht="25" customHeight="1">
       <c r="A221" s="3" t="inlineStr">
         <is>
-          <t>Williams</t>
+          <t>Watson</t>
         </is>
       </c>
       <c r="B221" s="3" t="inlineStr">
         <is>
-          <t>Johanna</t>
+          <t>Alison</t>
         </is>
       </c>
       <c r="C221" s="3" t="inlineStr">
         <is>
-          <t>Mitchells Plain</t>
+          <t>Sedgefield</t>
         </is>
       </c>
       <c r="D221" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E221" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F221" s="3" t="inlineStr">
@@ -7498,22 +7498,22 @@
     <row r="222" ht="25" customHeight="1">
       <c r="A222" s="3" t="inlineStr">
         <is>
-          <t>Wills</t>
+          <t>Williams</t>
         </is>
       </c>
       <c r="B222" s="3" t="inlineStr">
         <is>
-          <t>Geila</t>
+          <t>Johanna</t>
         </is>
       </c>
       <c r="C222" s="3" t="inlineStr">
         <is>
-          <t>Athlone</t>
+          <t>Mitchells Plain</t>
         </is>
       </c>
       <c r="D222" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E222" s="3" t="inlineStr">
@@ -7530,17 +7530,17 @@
     <row r="223" ht="25" customHeight="1">
       <c r="A223" s="3" t="inlineStr">
         <is>
-          <t>Wilter-Sturges</t>
+          <t>Wills</t>
         </is>
       </c>
       <c r="B223" s="3" t="inlineStr">
         <is>
-          <t>Meredith</t>
+          <t>Geila</t>
         </is>
       </c>
       <c r="C223" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Athlone</t>
         </is>
       </c>
       <c r="D223" s="3" t="inlineStr">
@@ -7555,24 +7555,24 @@
       </c>
       <c r="F223" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="224" ht="25" customHeight="1">
       <c r="A224" s="3" t="inlineStr">
         <is>
-          <t>Wright</t>
+          <t>Wilter-Sturges</t>
         </is>
       </c>
       <c r="B224" s="3" t="inlineStr">
         <is>
-          <t>Rocky</t>
+          <t>Meredith</t>
         </is>
       </c>
       <c r="C224" s="3" t="inlineStr">
         <is>
-          <t>Table View</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D224" s="3" t="inlineStr">
@@ -7582,29 +7582,29 @@
       </c>
       <c r="E224" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F224" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="225" ht="25" customHeight="1">
       <c r="A225" s="3" t="inlineStr">
         <is>
-          <t>Young</t>
+          <t>Wright</t>
         </is>
       </c>
       <c r="B225" s="3" t="inlineStr">
         <is>
-          <t>Judy</t>
+          <t>Rocky</t>
         </is>
       </c>
       <c r="C225" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>Table View</t>
         </is>
       </c>
       <c r="D225" s="3" t="inlineStr">
@@ -7614,7 +7614,7 @@
       </c>
       <c r="E225" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F225" s="3" t="inlineStr">
@@ -7626,17 +7626,17 @@
     <row r="226" ht="25" customHeight="1">
       <c r="A226" s="3" t="inlineStr">
         <is>
-          <t>de Kock</t>
+          <t>Young</t>
         </is>
       </c>
       <c r="B226" s="3" t="inlineStr">
         <is>
-          <t>Engela</t>
+          <t>Judy</t>
         </is>
       </c>
       <c r="C226" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Durbanville</t>
         </is>
       </c>
       <c r="D226" s="3" t="inlineStr">
@@ -7646,7 +7646,7 @@
       </c>
       <c r="E226" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F226" s="3" t="inlineStr">
@@ -7663,7 +7663,7 @@
       </c>
       <c r="B227" s="3" t="inlineStr">
         <is>
-          <t>Francois</t>
+          <t>Engela</t>
         </is>
       </c>
       <c r="C227" s="3" t="inlineStr">
@@ -7690,59 +7690,59 @@
     <row r="228" ht="25" customHeight="1">
       <c r="A228" s="3" t="inlineStr">
         <is>
-          <t>de Silva</t>
+          <t>de Kock</t>
         </is>
       </c>
       <c r="B228" s="3" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Francois</t>
         </is>
       </c>
       <c r="C228" s="3" t="inlineStr">
         <is>
-          <t>Edenvale</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D228" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E228" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F228" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="229" ht="25" customHeight="1">
       <c r="A229" s="3" t="inlineStr">
         <is>
-          <t>du Plooy</t>
+          <t>de Silva</t>
         </is>
       </c>
       <c r="B229" s="3" t="inlineStr">
         <is>
-          <t>Tammy</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="C229" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Edenvale</t>
         </is>
       </c>
       <c r="D229" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E229" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F229" s="3" t="inlineStr">
@@ -7759,7 +7759,7 @@
       </c>
       <c r="B230" s="3" t="inlineStr">
         <is>
-          <t>Marc</t>
+          <t>Tammy</t>
         </is>
       </c>
       <c r="C230" s="3" t="inlineStr">
@@ -7786,17 +7786,17 @@
     <row r="231" ht="25" customHeight="1">
       <c r="A231" s="3" t="inlineStr">
         <is>
-          <t>du Toit</t>
+          <t>du Plooy</t>
         </is>
       </c>
       <c r="B231" s="3" t="inlineStr">
         <is>
-          <t>Desiree</t>
+          <t>Marc</t>
         </is>
       </c>
       <c r="C231" s="3" t="inlineStr">
         <is>
-          <t>Ramsgate</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D231" s="3" t="inlineStr">
@@ -7818,22 +7818,22 @@
     <row r="232" ht="25" customHeight="1">
       <c r="A232" s="3" t="inlineStr">
         <is>
-          <t>stier</t>
+          <t>du Toit</t>
         </is>
       </c>
       <c r="B232" s="3" t="inlineStr">
         <is>
-          <t>RORY</t>
+          <t>Desiree</t>
         </is>
       </c>
       <c r="C232" s="3" t="inlineStr">
         <is>
-          <t>Deep South</t>
+          <t>Ramsgate</t>
         </is>
       </c>
       <c r="D232" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E232" s="3" t="inlineStr">
@@ -7843,56 +7843,56 @@
       </c>
       <c r="F232" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="233" ht="25" customHeight="1">
       <c r="A233" s="3" t="inlineStr">
         <is>
-          <t>tyler</t>
+          <t>stier</t>
         </is>
       </c>
       <c r="B233" s="3" t="inlineStr">
         <is>
-          <t>natascha</t>
+          <t>RORY</t>
         </is>
       </c>
       <c r="C233" s="3" t="inlineStr">
         <is>
-          <t>Kensington</t>
+          <t>Deep South</t>
         </is>
       </c>
       <c r="D233" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E233" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F233" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="234" ht="25" customHeight="1">
       <c r="A234" s="3" t="inlineStr">
         <is>
-          <t>van Blerk</t>
+          <t>tyler</t>
         </is>
       </c>
       <c r="B234" s="3" t="inlineStr">
         <is>
-          <t>Carl</t>
+          <t>natascha</t>
         </is>
       </c>
       <c r="C234" s="3" t="inlineStr">
         <is>
-          <t>Eden</t>
+          <t>Kensington</t>
         </is>
       </c>
       <c r="D234" s="3" t="inlineStr">
@@ -7907,24 +7907,24 @@
       </c>
       <c r="F234" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="235" ht="25" customHeight="1">
       <c r="A235" s="3" t="inlineStr">
         <is>
-          <t>van Heerden</t>
+          <t>van Blerk</t>
         </is>
       </c>
       <c r="B235" s="3" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Carl</t>
         </is>
       </c>
       <c r="C235" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Eden</t>
         </is>
       </c>
       <c r="D235" s="3" t="inlineStr">
@@ -7939,7 +7939,7 @@
       </c>
       <c r="F235" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -7951,7 +7951,7 @@
       </c>
       <c r="B236" s="3" t="inlineStr">
         <is>
-          <t>Sandy</t>
+          <t>Sydney</t>
         </is>
       </c>
       <c r="C236" s="3" t="inlineStr">
@@ -7966,7 +7966,7 @@
       </c>
       <c r="E236" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F236" s="3" t="inlineStr">
@@ -7983,17 +7983,17 @@
       </c>
       <c r="B237" s="3" t="inlineStr">
         <is>
-          <t>Craig</t>
+          <t>Sandy</t>
         </is>
       </c>
       <c r="C237" s="3" t="inlineStr">
         <is>
-          <t>East London Beacon Bay</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D237" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E237" s="3" t="inlineStr">
@@ -8015,17 +8015,17 @@
       </c>
       <c r="B238" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Craig</t>
         </is>
       </c>
       <c r="C238" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>East London Beacon Bay</t>
         </is>
       </c>
       <c r="D238" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E238" s="3" t="inlineStr">
@@ -8042,17 +8042,17 @@
     <row r="239" ht="25" customHeight="1">
       <c r="A239" s="3" t="inlineStr">
         <is>
-          <t>van Rensburg</t>
+          <t>van Heerden</t>
         </is>
       </c>
       <c r="B239" s="3" t="inlineStr">
         <is>
-          <t>Johan</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C239" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D239" s="3" t="inlineStr">
@@ -8062,12 +8062,12 @@
       </c>
       <c r="E239" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F239" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -8079,7 +8079,7 @@
       </c>
       <c r="B240" s="3" t="inlineStr">
         <is>
-          <t>Anne</t>
+          <t>Johan</t>
         </is>
       </c>
       <c r="C240" s="3" t="inlineStr">
@@ -8106,17 +8106,17 @@
     <row r="241" ht="25" customHeight="1">
       <c r="A241" s="3" t="inlineStr">
         <is>
-          <t>van Wulven</t>
+          <t>van Rensburg</t>
         </is>
       </c>
       <c r="B241" s="3" t="inlineStr">
         <is>
-          <t>Jeannie</t>
+          <t>Anne</t>
         </is>
       </c>
       <c r="C241" s="3" t="inlineStr">
         <is>
-          <t>Tygerberg Hills</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D241" s="3" t="inlineStr">
@@ -8126,7 +8126,7 @@
       </c>
       <c r="E241" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F241" s="3" t="inlineStr">
@@ -8143,7 +8143,7 @@
       </c>
       <c r="B242" s="3" t="inlineStr">
         <is>
-          <t>Alan</t>
+          <t>Jeannie</t>
         </is>
       </c>
       <c r="C242" s="3" t="inlineStr">
@@ -8158,7 +8158,7 @@
       </c>
       <c r="E242" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F242" s="3" t="inlineStr">
@@ -8175,7 +8175,7 @@
       </c>
       <c r="B243" s="3" t="inlineStr">
         <is>
-          <t>Deon</t>
+          <t>Alan</t>
         </is>
       </c>
       <c r="C243" s="3" t="inlineStr">
@@ -8202,17 +8202,17 @@
     <row r="244" ht="25" customHeight="1">
       <c r="A244" s="3" t="inlineStr">
         <is>
-          <t>van Wyk</t>
+          <t>van Wulven</t>
         </is>
       </c>
       <c r="B244" s="3" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>Deon</t>
         </is>
       </c>
       <c r="C244" s="3" t="inlineStr">
         <is>
-          <t>North Durban</t>
+          <t>Tygerberg Hills</t>
         </is>
       </c>
       <c r="D244" s="3" t="inlineStr">
@@ -8227,7 +8227,7 @@
       </c>
       <c r="F244" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -8239,12 +8239,12 @@
       </c>
       <c r="B245" s="3" t="inlineStr">
         <is>
-          <t>Lindie</t>
+          <t>Kim</t>
         </is>
       </c>
       <c r="C245" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>North Durban</t>
         </is>
       </c>
       <c r="D245" s="3" t="inlineStr">
@@ -8271,12 +8271,12 @@
       </c>
       <c r="B246" s="3" t="inlineStr">
         <is>
-          <t>Willem</t>
+          <t>Lindie</t>
         </is>
       </c>
       <c r="C246" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D246" s="3" t="inlineStr">
@@ -8303,12 +8303,12 @@
       </c>
       <c r="B247" s="3" t="inlineStr">
         <is>
-          <t>Patricia</t>
+          <t>Willem</t>
         </is>
       </c>
       <c r="C247" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D247" s="3" t="inlineStr">
@@ -8330,22 +8330,22 @@
     <row r="248" ht="25" customHeight="1">
       <c r="A248" s="3" t="inlineStr">
         <is>
-          <t>van der Merwe</t>
+          <t>van Wyk</t>
         </is>
       </c>
       <c r="B248" s="3" t="inlineStr">
         <is>
-          <t>Ingrid</t>
+          <t>Patricia</t>
         </is>
       </c>
       <c r="C248" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D248" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E248" s="3" t="inlineStr">
@@ -8362,49 +8362,49 @@
     <row r="249" ht="25" customHeight="1">
       <c r="A249" s="3" t="inlineStr">
         <is>
-          <t>van der Westhuizen</t>
+          <t>van der Merwe</t>
         </is>
       </c>
       <c r="B249" s="3" t="inlineStr">
         <is>
-          <t>Hennie</t>
+          <t>Ingrid</t>
         </is>
       </c>
       <c r="C249" s="3" t="inlineStr">
         <is>
-          <t>Helderberg</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D249" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E249" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F249" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="250" ht="25" customHeight="1">
       <c r="A250" s="3" t="inlineStr">
         <is>
-          <t>von der Decken</t>
+          <t>van der Westhuizen</t>
         </is>
       </c>
       <c r="B250" s="3" t="inlineStr">
         <is>
-          <t>Brian</t>
+          <t>Hennie</t>
         </is>
       </c>
       <c r="C250" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Helderberg</t>
         </is>
       </c>
       <c r="D250" s="3" t="inlineStr">
@@ -8419,51 +8419,83 @@
       </c>
       <c r="F250" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="251" ht="25" customHeight="1">
       <c r="A251" s="3" t="inlineStr">
         <is>
+          <t>von der Decken</t>
+        </is>
+      </c>
+      <c r="B251" s="3" t="inlineStr">
+        <is>
+          <t>Brian</t>
+        </is>
+      </c>
+      <c r="C251" s="3" t="inlineStr">
+        <is>
+          <t>King William's Town</t>
+        </is>
+      </c>
+      <c r="D251" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E251" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F251" s="3" t="inlineStr">
+        <is>
+          <t>410E</t>
+        </is>
+      </c>
+    </row>
+    <row r="252" ht="25" customHeight="1">
+      <c r="A252" s="3" t="inlineStr">
+        <is>
           <t>‘t Hart</t>
         </is>
       </c>
-      <c r="B251" s="3" t="inlineStr">
+      <c r="B252" s="3" t="inlineStr">
         <is>
           <t>Michelle</t>
         </is>
       </c>
-      <c r="C251" s="3" t="inlineStr">
+      <c r="C252" s="3" t="inlineStr">
         <is>
           <t>Benoni Lakes</t>
         </is>
       </c>
-      <c r="D251" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E251" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F251" s="3" t="inlineStr">
+      <c r="D252" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E252" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F252" s="3" t="inlineStr">
         <is>
           <t>410E</t>
-        </is>
-      </c>
-    </row>
-    <row r="252">
-      <c r="A252" s="1" t="inlineStr">
-        <is>
-          <t>Number of attendees: 249</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="inlineStr">
+        <is>
+          <t>Number of attendees: 250</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" s="1" t="inlineStr">
         <is>
           <t>Number of voters: 98</t>
         </is>
@@ -8499,7 +8531,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Registrees as of 30/04/2021 21:18</t>
+          <t>410E Registrees as of 01/05/2021 07:39</t>
         </is>
       </c>
     </row>
@@ -12111,7 +12143,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Registrees as of 30/04/2021 21:18</t>
+          <t>410W Registrees as of 01/05/2021 07:39</t>
         </is>
       </c>
     </row>
@@ -16287,7 +16319,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Voting details as of 30/04/2021 21:18</t>
+          <t>410E Voting details as of 01/05/2021 07:39</t>
         </is>
       </c>
     </row>
@@ -16664,7 +16696,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Voting details as of 30/04/2021 21:18</t>
+          <t>410W Voting details as of 01/05/2021 07:39</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Registree stats backup on Sat 01 May 2021 08:09:32 SAST
</commit_message>
<xml_diff>
--- a/static/docs/registrees_list.xlsx
+++ b/static/docs/registrees_list.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F254"/>
+  <dimension ref="A1:F255"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,7 +451,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>MD410 Registrees as of 01/05/2021 07:39</t>
+          <t>MD410 Registrees as of 01/05/2021 08:09</t>
         </is>
       </c>
     </row>
@@ -4394,22 +4394,22 @@
     <row r="125" ht="25" customHeight="1">
       <c r="A125" s="3" t="inlineStr">
         <is>
-          <t>McDonald</t>
+          <t>Maweya</t>
         </is>
       </c>
       <c r="B125" s="3" t="inlineStr">
         <is>
-          <t>Rochelle</t>
+          <t>HLEKANI</t>
         </is>
       </c>
       <c r="C125" s="3" t="inlineStr">
         <is>
-          <t>Vereeniging</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D125" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E125" s="3" t="inlineStr">
@@ -4426,17 +4426,17 @@
     <row r="126" ht="25" customHeight="1">
       <c r="A126" s="3" t="inlineStr">
         <is>
-          <t>McPherson</t>
+          <t>McDonald</t>
         </is>
       </c>
       <c r="B126" s="3" t="inlineStr">
         <is>
-          <t>Stuart</t>
+          <t>Rochelle</t>
         </is>
       </c>
       <c r="C126" s="3" t="inlineStr">
         <is>
-          <t>Newlands</t>
+          <t>Vereeniging</t>
         </is>
       </c>
       <c r="D126" s="3" t="inlineStr">
@@ -4446,29 +4446,29 @@
       </c>
       <c r="E126" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F126" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="127" ht="25" customHeight="1">
       <c r="A127" s="3" t="inlineStr">
         <is>
-          <t>Mccullough</t>
+          <t>McPherson</t>
         </is>
       </c>
       <c r="B127" s="3" t="inlineStr">
         <is>
-          <t>David</t>
+          <t>Stuart</t>
         </is>
       </c>
       <c r="C127" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Newlands</t>
         </is>
       </c>
       <c r="D127" s="3" t="inlineStr">
@@ -4478,29 +4478,29 @@
       </c>
       <c r="E127" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F127" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="128" ht="25" customHeight="1">
       <c r="A128" s="3" t="inlineStr">
         <is>
-          <t>Meyer</t>
+          <t>Mccullough</t>
         </is>
       </c>
       <c r="B128" s="3" t="inlineStr">
         <is>
-          <t>Denis</t>
+          <t>David</t>
         </is>
       </c>
       <c r="C128" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D128" s="3" t="inlineStr">
@@ -4510,7 +4510,7 @@
       </c>
       <c r="E128" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F128" s="3" t="inlineStr">
@@ -4522,17 +4522,17 @@
     <row r="129" ht="25" customHeight="1">
       <c r="A129" s="3" t="inlineStr">
         <is>
-          <t>Michas</t>
+          <t>Meyer</t>
         </is>
       </c>
       <c r="B129" s="3" t="inlineStr">
         <is>
-          <t>Roy</t>
+          <t>Denis</t>
         </is>
       </c>
       <c r="C129" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D129" s="3" t="inlineStr">
@@ -4559,7 +4559,7 @@
       </c>
       <c r="B130" s="3" t="inlineStr">
         <is>
-          <t>Dawn</t>
+          <t>Roy</t>
         </is>
       </c>
       <c r="C130" s="3" t="inlineStr">
@@ -4574,7 +4574,7 @@
       </c>
       <c r="E130" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F130" s="3" t="inlineStr">
@@ -4586,17 +4586,17 @@
     <row r="131" ht="25" customHeight="1">
       <c r="A131" s="3" t="inlineStr">
         <is>
-          <t>Mills</t>
+          <t>Michas</t>
         </is>
       </c>
       <c r="B131" s="3" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>Dawn</t>
         </is>
       </c>
       <c r="C131" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D131" s="3" t="inlineStr">
@@ -4606,7 +4606,7 @@
       </c>
       <c r="E131" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F131" s="3" t="inlineStr">
@@ -4618,17 +4618,17 @@
     <row r="132" ht="25" customHeight="1">
       <c r="A132" s="3" t="inlineStr">
         <is>
-          <t>Mitchell</t>
+          <t>Mills</t>
         </is>
       </c>
       <c r="B132" s="3" t="inlineStr">
         <is>
-          <t>Alana</t>
+          <t>Patrick</t>
         </is>
       </c>
       <c r="C132" s="3" t="inlineStr">
         <is>
-          <t>Rustenburg</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D132" s="3" t="inlineStr">
@@ -4638,7 +4638,7 @@
       </c>
       <c r="E132" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F132" s="3" t="inlineStr">
@@ -4655,7 +4655,7 @@
       </c>
       <c r="B133" s="3" t="inlineStr">
         <is>
-          <t>Juan</t>
+          <t>Alana</t>
         </is>
       </c>
       <c r="C133" s="3" t="inlineStr">
@@ -4670,7 +4670,7 @@
       </c>
       <c r="E133" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F133" s="3" t="inlineStr">
@@ -4682,17 +4682,17 @@
     <row r="134" ht="25" customHeight="1">
       <c r="A134" s="3" t="inlineStr">
         <is>
-          <t>Mkhize</t>
+          <t>Mitchell</t>
         </is>
       </c>
       <c r="B134" s="3" t="inlineStr">
         <is>
-          <t>Virginia</t>
+          <t>Juan</t>
         </is>
       </c>
       <c r="C134" s="3" t="inlineStr">
         <is>
-          <t>Cape Town</t>
+          <t>Rustenburg</t>
         </is>
       </c>
       <c r="D134" s="3" t="inlineStr">
@@ -4702,34 +4702,34 @@
       </c>
       <c r="E134" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F134" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="135" ht="25" customHeight="1">
       <c r="A135" s="3" t="inlineStr">
         <is>
-          <t>Moeller</t>
+          <t>Mkhize</t>
         </is>
       </c>
       <c r="B135" s="3" t="inlineStr">
         <is>
-          <t>Frauke E.</t>
+          <t>Virginia</t>
         </is>
       </c>
       <c r="C135" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Cape Town</t>
         </is>
       </c>
       <c r="D135" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E135" s="3" t="inlineStr">
@@ -4746,22 +4746,22 @@
     <row r="136" ht="25" customHeight="1">
       <c r="A136" s="3" t="inlineStr">
         <is>
-          <t>Moodley</t>
+          <t>Moeller</t>
         </is>
       </c>
       <c r="B136" s="3" t="inlineStr">
         <is>
-          <t>Hansuya</t>
+          <t>Frauke E.</t>
         </is>
       </c>
       <c r="C136" s="3" t="inlineStr">
         <is>
-          <t>East Coast</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D136" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E136" s="3" t="inlineStr">
@@ -4771,24 +4771,24 @@
       </c>
       <c r="F136" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="137" ht="25" customHeight="1">
       <c r="A137" s="3" t="inlineStr">
         <is>
-          <t>Moses</t>
+          <t>Moodley</t>
         </is>
       </c>
       <c r="B137" s="3" t="inlineStr">
         <is>
-          <t>Bernadine</t>
+          <t>Hansuya</t>
         </is>
       </c>
       <c r="C137" s="3" t="inlineStr">
         <is>
-          <t>Cape Town</t>
+          <t>East Coast</t>
         </is>
       </c>
       <c r="D137" s="3" t="inlineStr">
@@ -4803,34 +4803,34 @@
       </c>
       <c r="F137" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="138" ht="25" customHeight="1">
       <c r="A138" s="3" t="inlineStr">
         <is>
-          <t>Mostert</t>
+          <t>Moses</t>
         </is>
       </c>
       <c r="B138" s="3" t="inlineStr">
         <is>
-          <t>Jacques</t>
+          <t>Bernadine</t>
         </is>
       </c>
       <c r="C138" s="3" t="inlineStr">
         <is>
-          <t>Merriman</t>
+          <t>Cape Town</t>
         </is>
       </c>
       <c r="D138" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E138" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F138" s="3" t="inlineStr">
@@ -4842,22 +4842,22 @@
     <row r="139" ht="25" customHeight="1">
       <c r="A139" s="3" t="inlineStr">
         <is>
-          <t>Murray</t>
+          <t>Mostert</t>
         </is>
       </c>
       <c r="B139" s="3" t="inlineStr">
         <is>
-          <t>Suzanne</t>
+          <t>Jacques</t>
         </is>
       </c>
       <c r="C139" s="3" t="inlineStr">
         <is>
-          <t>Vereeniging</t>
+          <t>Merriman</t>
         </is>
       </c>
       <c r="D139" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E139" s="3" t="inlineStr">
@@ -4867,7 +4867,7 @@
       </c>
       <c r="F139" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -4879,7 +4879,7 @@
       </c>
       <c r="B140" s="3" t="inlineStr">
         <is>
-          <t>Gary</t>
+          <t>Suzanne</t>
         </is>
       </c>
       <c r="C140" s="3" t="inlineStr">
@@ -4906,17 +4906,17 @@
     <row r="141" ht="25" customHeight="1">
       <c r="A141" s="3" t="inlineStr">
         <is>
-          <t>Myburg</t>
+          <t>Murray</t>
         </is>
       </c>
       <c r="B141" s="3" t="inlineStr">
         <is>
-          <t>Pieter</t>
+          <t>Gary</t>
         </is>
       </c>
       <c r="C141" s="3" t="inlineStr">
         <is>
-          <t>Wellington</t>
+          <t>Vereeniging</t>
         </is>
       </c>
       <c r="D141" s="3" t="inlineStr">
@@ -4926,34 +4926,34 @@
       </c>
       <c r="E141" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F141" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="142" ht="25" customHeight="1">
       <c r="A142" s="3" t="inlineStr">
         <is>
-          <t>Naude</t>
+          <t>Myburg</t>
         </is>
       </c>
       <c r="B142" s="3" t="inlineStr">
         <is>
-          <t>Cornette</t>
+          <t>Pieter</t>
         </is>
       </c>
       <c r="C142" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Wellington</t>
         </is>
       </c>
       <c r="D142" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E142" s="3" t="inlineStr">
@@ -4963,7 +4963,7 @@
       </c>
       <c r="F142" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -4975,17 +4975,17 @@
       </c>
       <c r="B143" s="3" t="inlineStr">
         <is>
-          <t>Nici</t>
+          <t>Cornette</t>
         </is>
       </c>
       <c r="C143" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D143" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E143" s="3" t="inlineStr">
@@ -5002,17 +5002,17 @@
     <row r="144" ht="25" customHeight="1">
       <c r="A144" s="3" t="inlineStr">
         <is>
-          <t>Nel</t>
+          <t>Naude</t>
         </is>
       </c>
       <c r="B144" s="3" t="inlineStr">
         <is>
-          <t>Pieter</t>
+          <t>Nici</t>
         </is>
       </c>
       <c r="C144" s="3" t="inlineStr">
         <is>
-          <t>George</t>
+          <t>King William's Town</t>
         </is>
       </c>
       <c r="D144" s="3" t="inlineStr">
@@ -5022,12 +5022,12 @@
       </c>
       <c r="E144" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F144" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -5039,12 +5039,12 @@
       </c>
       <c r="B145" s="3" t="inlineStr">
         <is>
-          <t>Tillie</t>
+          <t>Pieter</t>
         </is>
       </c>
       <c r="C145" s="3" t="inlineStr">
         <is>
-          <t>Eden</t>
+          <t>George</t>
         </is>
       </c>
       <c r="D145" s="3" t="inlineStr">
@@ -5066,17 +5066,17 @@
     <row r="146" ht="25" customHeight="1">
       <c r="A146" s="3" t="inlineStr">
         <is>
-          <t>Newlands</t>
+          <t>Nel</t>
         </is>
       </c>
       <c r="B146" s="3" t="inlineStr">
         <is>
-          <t>Mike</t>
+          <t>Tillie</t>
         </is>
       </c>
       <c r="C146" s="3" t="inlineStr">
         <is>
-          <t>Port Alfred</t>
+          <t>Eden</t>
         </is>
       </c>
       <c r="D146" s="3" t="inlineStr">
@@ -5091,24 +5091,24 @@
       </c>
       <c r="F146" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="147" ht="25" customHeight="1">
       <c r="A147" s="3" t="inlineStr">
         <is>
-          <t>Ngobozana</t>
+          <t>Newlands</t>
         </is>
       </c>
       <c r="B147" s="3" t="inlineStr">
         <is>
-          <t>Sphiwe</t>
+          <t>Mike</t>
         </is>
       </c>
       <c r="C147" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Port Alfred</t>
         </is>
       </c>
       <c r="D147" s="3" t="inlineStr">
@@ -5118,7 +5118,7 @@
       </c>
       <c r="E147" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F147" s="3" t="inlineStr">
@@ -5130,17 +5130,17 @@
     <row r="148" ht="25" customHeight="1">
       <c r="A148" s="3" t="inlineStr">
         <is>
-          <t>Niehaus</t>
+          <t>Ngobozana</t>
         </is>
       </c>
       <c r="B148" s="3" t="inlineStr">
         <is>
-          <t>Angela</t>
+          <t>Sphiwe</t>
         </is>
       </c>
       <c r="C148" s="3" t="inlineStr">
         <is>
-          <t>Bergvliet</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D148" s="3" t="inlineStr">
@@ -5150,29 +5150,29 @@
       </c>
       <c r="E148" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F148" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="149" ht="25" customHeight="1">
       <c r="A149" s="3" t="inlineStr">
         <is>
-          <t>Oberholzer</t>
+          <t>Niehaus</t>
         </is>
       </c>
       <c r="B149" s="3" t="inlineStr">
         <is>
-          <t>PDG Bokkie</t>
+          <t>Angela</t>
         </is>
       </c>
       <c r="C149" s="3" t="inlineStr">
         <is>
-          <t>Uitenhage</t>
+          <t>Bergvliet</t>
         </is>
       </c>
       <c r="D149" s="3" t="inlineStr">
@@ -5182,29 +5182,29 @@
       </c>
       <c r="E149" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F149" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="150" ht="25" customHeight="1">
       <c r="A150" s="3" t="inlineStr">
         <is>
-          <t>PORTEOUS</t>
+          <t>Oberholzer</t>
         </is>
       </c>
       <c r="B150" s="3" t="inlineStr">
         <is>
-          <t>BRIAN</t>
+          <t>PDG Bokkie</t>
         </is>
       </c>
       <c r="C150" s="3" t="inlineStr">
         <is>
-          <t>Hibberdene</t>
+          <t>Uitenhage</t>
         </is>
       </c>
       <c r="D150" s="3" t="inlineStr">
@@ -5214,7 +5214,7 @@
       </c>
       <c r="E150" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F150" s="3" t="inlineStr">
@@ -5226,17 +5226,17 @@
     <row r="151" ht="25" customHeight="1">
       <c r="A151" s="3" t="inlineStr">
         <is>
-          <t>Paijmans</t>
+          <t>PORTEOUS</t>
         </is>
       </c>
       <c r="B151" s="3" t="inlineStr">
         <is>
-          <t>Bronwyn Anne</t>
+          <t>BRIAN</t>
         </is>
       </c>
       <c r="C151" s="3" t="inlineStr">
         <is>
-          <t>Cowies Hill</t>
+          <t>Hibberdene</t>
         </is>
       </c>
       <c r="D151" s="3" t="inlineStr">
@@ -5246,7 +5246,7 @@
       </c>
       <c r="E151" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F151" s="3" t="inlineStr">
@@ -5258,17 +5258,17 @@
     <row r="152" ht="25" customHeight="1">
       <c r="A152" s="3" t="inlineStr">
         <is>
-          <t>Pantoleon</t>
+          <t>Paijmans</t>
         </is>
       </c>
       <c r="B152" s="3" t="inlineStr">
         <is>
-          <t>Teresa</t>
+          <t>Bronwyn Anne</t>
         </is>
       </c>
       <c r="C152" s="3" t="inlineStr">
         <is>
-          <t>Vereeniging</t>
+          <t>Cowies Hill</t>
         </is>
       </c>
       <c r="D152" s="3" t="inlineStr">
@@ -5278,7 +5278,7 @@
       </c>
       <c r="E152" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F152" s="3" t="inlineStr">
@@ -5290,17 +5290,17 @@
     <row r="153" ht="25" customHeight="1">
       <c r="A153" s="3" t="inlineStr">
         <is>
-          <t>Peters</t>
+          <t>Pantoleon</t>
         </is>
       </c>
       <c r="B153" s="3" t="inlineStr">
         <is>
-          <t>Maureen</t>
+          <t>Teresa</t>
         </is>
       </c>
       <c r="C153" s="3" t="inlineStr">
         <is>
-          <t>Ceres</t>
+          <t>Vereeniging</t>
         </is>
       </c>
       <c r="D153" s="3" t="inlineStr">
@@ -5315,24 +5315,24 @@
       </c>
       <c r="F153" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="154" ht="25" customHeight="1">
       <c r="A154" s="3" t="inlineStr">
         <is>
-          <t>Piater</t>
+          <t>Peters</t>
         </is>
       </c>
       <c r="B154" s="3" t="inlineStr">
         <is>
-          <t>Ivan</t>
+          <t>Maureen</t>
         </is>
       </c>
       <c r="C154" s="3" t="inlineStr">
         <is>
-          <t>East London Port Rex</t>
+          <t>Ceres</t>
         </is>
       </c>
       <c r="D154" s="3" t="inlineStr">
@@ -5342,29 +5342,29 @@
       </c>
       <c r="E154" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F154" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="155" ht="25" customHeight="1">
       <c r="A155" s="3" t="inlineStr">
         <is>
-          <t>Pillay</t>
+          <t>Piater</t>
         </is>
       </c>
       <c r="B155" s="3" t="inlineStr">
         <is>
-          <t>Sundru</t>
+          <t>Ivan</t>
         </is>
       </c>
       <c r="C155" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>East London Port Rex</t>
         </is>
       </c>
       <c r="D155" s="3" t="inlineStr">
@@ -5379,7 +5379,7 @@
       </c>
       <c r="F155" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -5391,12 +5391,12 @@
       </c>
       <c r="B156" s="3" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>Sundru</t>
         </is>
       </c>
       <c r="C156" s="3" t="inlineStr">
         <is>
-          <t>Tygerberg Hills</t>
+          <t>Durbanville</t>
         </is>
       </c>
       <c r="D156" s="3" t="inlineStr">
@@ -5418,17 +5418,17 @@
     <row r="157" ht="25" customHeight="1">
       <c r="A157" s="3" t="inlineStr">
         <is>
-          <t>Polkinghorne</t>
+          <t>Pillay</t>
         </is>
       </c>
       <c r="B157" s="3" t="inlineStr">
         <is>
-          <t>Tracey</t>
+          <t>Patrick</t>
         </is>
       </c>
       <c r="C157" s="3" t="inlineStr">
         <is>
-          <t>Kensington</t>
+          <t>Tygerberg Hills</t>
         </is>
       </c>
       <c r="D157" s="3" t="inlineStr">
@@ -5438,12 +5438,12 @@
       </c>
       <c r="E157" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F157" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -5455,7 +5455,7 @@
       </c>
       <c r="B158" s="3" t="inlineStr">
         <is>
-          <t>Gavin</t>
+          <t>Tracey</t>
         </is>
       </c>
       <c r="C158" s="3" t="inlineStr">
@@ -5470,7 +5470,7 @@
       </c>
       <c r="E158" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F158" s="3" t="inlineStr">
@@ -5482,22 +5482,22 @@
     <row r="159" ht="25" customHeight="1">
       <c r="A159" s="3" t="inlineStr">
         <is>
-          <t>Pretorius</t>
+          <t>Polkinghorne</t>
         </is>
       </c>
       <c r="B159" s="3" t="inlineStr">
         <is>
-          <t>Sheldon Edmund</t>
+          <t>Gavin</t>
         </is>
       </c>
       <c r="C159" s="3" t="inlineStr">
         <is>
-          <t>Merriman</t>
+          <t>Kensington</t>
         </is>
       </c>
       <c r="D159" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E159" s="3" t="inlineStr">
@@ -5507,29 +5507,29 @@
       </c>
       <c r="F159" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="160" ht="25" customHeight="1">
       <c r="A160" s="3" t="inlineStr">
         <is>
-          <t>Ras</t>
+          <t>Pretorius</t>
         </is>
       </c>
       <c r="B160" s="3" t="inlineStr">
         <is>
-          <t>Mary-Anne</t>
+          <t>Sheldon Edmund</t>
         </is>
       </c>
       <c r="C160" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Merriman</t>
         </is>
       </c>
       <c r="D160" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E160" s="3" t="inlineStr">
@@ -5551,7 +5551,7 @@
       </c>
       <c r="B161" s="3" t="inlineStr">
         <is>
-          <t>Leon Jacobus</t>
+          <t>Mary-Anne</t>
         </is>
       </c>
       <c r="C161" s="3" t="inlineStr">
@@ -5578,22 +5578,22 @@
     <row r="162" ht="25" customHeight="1">
       <c r="A162" s="3" t="inlineStr">
         <is>
-          <t>Rashirai</t>
+          <t>Ras</t>
         </is>
       </c>
       <c r="B162" s="3" t="inlineStr">
         <is>
-          <t>Tabeth</t>
+          <t>Leon Jacobus</t>
         </is>
       </c>
       <c r="C162" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D162" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E162" s="3" t="inlineStr">
@@ -5603,29 +5603,29 @@
       </c>
       <c r="F162" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="163" ht="25" customHeight="1">
       <c r="A163" s="3" t="inlineStr">
         <is>
-          <t>Rathbone Smyth</t>
+          <t>Rashirai</t>
         </is>
       </c>
       <c r="B163" s="3" t="inlineStr">
         <is>
-          <t>Janine</t>
+          <t>Tabeth</t>
         </is>
       </c>
       <c r="C163" s="3" t="inlineStr">
         <is>
-          <t>Vereeniging</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D163" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E163" s="3" t="inlineStr">
@@ -5642,17 +5642,17 @@
     <row r="164" ht="25" customHeight="1">
       <c r="A164" s="3" t="inlineStr">
         <is>
-          <t>Reniers</t>
+          <t>Rathbone Smyth</t>
         </is>
       </c>
       <c r="B164" s="3" t="inlineStr">
         <is>
-          <t>Hugo</t>
+          <t>Janine</t>
         </is>
       </c>
       <c r="C164" s="3" t="inlineStr">
         <is>
-          <t>Nelspruit</t>
+          <t>Vereeniging</t>
         </is>
       </c>
       <c r="D164" s="3" t="inlineStr">
@@ -5662,7 +5662,7 @@
       </c>
       <c r="E164" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F164" s="3" t="inlineStr">
@@ -5674,17 +5674,17 @@
     <row r="165" ht="25" customHeight="1">
       <c r="A165" s="3" t="inlineStr">
         <is>
-          <t>Roman</t>
+          <t>Reniers</t>
         </is>
       </c>
       <c r="B165" s="3" t="inlineStr">
         <is>
-          <t>Sandy</t>
+          <t>Hugo</t>
         </is>
       </c>
       <c r="C165" s="3" t="inlineStr">
         <is>
-          <t>Bergvliet</t>
+          <t>Nelspruit</t>
         </is>
       </c>
       <c r="D165" s="3" t="inlineStr">
@@ -5694,29 +5694,29 @@
       </c>
       <c r="E165" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F165" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="166" ht="25" customHeight="1">
       <c r="A166" s="3" t="inlineStr">
         <is>
-          <t>Rossouw</t>
+          <t>Roman</t>
         </is>
       </c>
       <c r="B166" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Sandy</t>
         </is>
       </c>
       <c r="C166" s="3" t="inlineStr">
         <is>
-          <t>Tokai</t>
+          <t>Bergvliet</t>
         </is>
       </c>
       <c r="D166" s="3" t="inlineStr">
@@ -5726,7 +5726,7 @@
       </c>
       <c r="E166" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F166" s="3" t="inlineStr">
@@ -5738,17 +5738,17 @@
     <row r="167" ht="25" customHeight="1">
       <c r="A167" s="3" t="inlineStr">
         <is>
-          <t>Rothner</t>
+          <t>Rossouw</t>
         </is>
       </c>
       <c r="B167" s="3" t="inlineStr">
         <is>
-          <t>Andrea</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C167" s="3" t="inlineStr">
         <is>
-          <t>Eden</t>
+          <t>Tokai</t>
         </is>
       </c>
       <c r="D167" s="3" t="inlineStr">
@@ -5758,7 +5758,7 @@
       </c>
       <c r="E167" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F167" s="3" t="inlineStr">
@@ -5770,17 +5770,17 @@
     <row r="168" ht="25" customHeight="1">
       <c r="A168" s="3" t="inlineStr">
         <is>
-          <t>Roux</t>
+          <t>Rothner</t>
         </is>
       </c>
       <c r="B168" s="3" t="inlineStr">
         <is>
-          <t>Anthonie Petrus</t>
+          <t>Andrea</t>
         </is>
       </c>
       <c r="C168" s="3" t="inlineStr">
         <is>
-          <t>Moorreesburg</t>
+          <t>Eden</t>
         </is>
       </c>
       <c r="D168" s="3" t="inlineStr">
@@ -5790,7 +5790,7 @@
       </c>
       <c r="E168" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F168" s="3" t="inlineStr">
@@ -5802,17 +5802,17 @@
     <row r="169" ht="25" customHeight="1">
       <c r="A169" s="3" t="inlineStr">
         <is>
-          <t>Russell</t>
+          <t>Roux</t>
         </is>
       </c>
       <c r="B169" s="3" t="inlineStr">
         <is>
-          <t>Ingrid</t>
+          <t>Anthonie Petrus</t>
         </is>
       </c>
       <c r="C169" s="3" t="inlineStr">
         <is>
-          <t>Fish Hoek</t>
+          <t>Moorreesburg</t>
         </is>
       </c>
       <c r="D169" s="3" t="inlineStr">
@@ -5834,27 +5834,27 @@
     <row r="170" ht="25" customHeight="1">
       <c r="A170" s="3" t="inlineStr">
         <is>
-          <t>SNYMAN</t>
+          <t>Russell</t>
         </is>
       </c>
       <c r="B170" s="3" t="inlineStr">
         <is>
-          <t>LYN</t>
+          <t>Ingrid</t>
         </is>
       </c>
       <c r="C170" s="3" t="inlineStr">
         <is>
-          <t>Deep South</t>
+          <t>Fish Hoek</t>
         </is>
       </c>
       <c r="D170" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E170" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F170" s="3" t="inlineStr">
@@ -5866,27 +5866,27 @@
     <row r="171" ht="25" customHeight="1">
       <c r="A171" s="3" t="inlineStr">
         <is>
-          <t>STEENBERG</t>
+          <t>SNYMAN</t>
         </is>
       </c>
       <c r="B171" s="3" t="inlineStr">
         <is>
-          <t>TIM</t>
+          <t>LYN</t>
         </is>
       </c>
       <c r="C171" s="3" t="inlineStr">
         <is>
-          <t>Wellington</t>
+          <t>Deep South</t>
         </is>
       </c>
       <c r="D171" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E171" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F171" s="3" t="inlineStr">
@@ -5898,17 +5898,17 @@
     <row r="172" ht="25" customHeight="1">
       <c r="A172" s="3" t="inlineStr">
         <is>
-          <t>Sabatier</t>
+          <t>STEENBERG</t>
         </is>
       </c>
       <c r="B172" s="3" t="inlineStr">
         <is>
-          <t>Rodney</t>
+          <t>TIM</t>
         </is>
       </c>
       <c r="C172" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Wellington</t>
         </is>
       </c>
       <c r="D172" s="3" t="inlineStr">
@@ -5923,24 +5923,24 @@
       </c>
       <c r="F172" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="173" ht="25" customHeight="1">
       <c r="A173" s="3" t="inlineStr">
         <is>
-          <t>Sampie</t>
+          <t>Sabatier</t>
         </is>
       </c>
       <c r="B173" s="3" t="inlineStr">
         <is>
-          <t>Sharon</t>
+          <t>Rodney</t>
         </is>
       </c>
       <c r="C173" s="3" t="inlineStr">
         <is>
-          <t>Bergvliet</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D173" s="3" t="inlineStr">
@@ -5955,24 +5955,24 @@
       </c>
       <c r="F173" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="174" ht="25" customHeight="1">
       <c r="A174" s="3" t="inlineStr">
         <is>
-          <t>Schatz</t>
+          <t>Sampie</t>
         </is>
       </c>
       <c r="B174" s="3" t="inlineStr">
         <is>
-          <t>Vera</t>
+          <t>Sharon</t>
         </is>
       </c>
       <c r="C174" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Bergvliet</t>
         </is>
       </c>
       <c r="D174" s="3" t="inlineStr">
@@ -5999,7 +5999,7 @@
       </c>
       <c r="B175" s="3" t="inlineStr">
         <is>
-          <t>Frank</t>
+          <t>Vera</t>
         </is>
       </c>
       <c r="C175" s="3" t="inlineStr">
@@ -6014,7 +6014,7 @@
       </c>
       <c r="E175" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F175" s="3" t="inlineStr">
@@ -6026,17 +6026,17 @@
     <row r="176" ht="25" customHeight="1">
       <c r="A176" s="3" t="inlineStr">
         <is>
-          <t>Searle</t>
+          <t>Schatz</t>
         </is>
       </c>
       <c r="B176" s="3" t="inlineStr">
         <is>
-          <t>Francis</t>
+          <t>Frank</t>
         </is>
       </c>
       <c r="C176" s="3" t="inlineStr">
         <is>
-          <t>Kouga</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D176" s="3" t="inlineStr">
@@ -6046,12 +6046,12 @@
       </c>
       <c r="E176" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F176" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -6063,7 +6063,7 @@
       </c>
       <c r="B177" s="3" t="inlineStr">
         <is>
-          <t>Gloria</t>
+          <t>Francis</t>
         </is>
       </c>
       <c r="C177" s="3" t="inlineStr">
@@ -6078,7 +6078,7 @@
       </c>
       <c r="E177" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F177" s="3" t="inlineStr">
@@ -6090,17 +6090,17 @@
     <row r="178" ht="25" customHeight="1">
       <c r="A178" s="3" t="inlineStr">
         <is>
-          <t>Sell</t>
+          <t>Searle</t>
         </is>
       </c>
       <c r="B178" s="3" t="inlineStr">
         <is>
-          <t>Ami</t>
+          <t>Gloria</t>
         </is>
       </c>
       <c r="C178" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Kouga</t>
         </is>
       </c>
       <c r="D178" s="3" t="inlineStr">
@@ -6115,24 +6115,24 @@
       </c>
       <c r="F178" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="179" ht="25" customHeight="1">
       <c r="A179" s="3" t="inlineStr">
         <is>
-          <t>Simpson</t>
+          <t>Sell</t>
         </is>
       </c>
       <c r="B179" s="3" t="inlineStr">
         <is>
-          <t>Beryl</t>
+          <t>Ami</t>
         </is>
       </c>
       <c r="C179" s="3" t="inlineStr">
         <is>
-          <t>Cape Town</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D179" s="3" t="inlineStr">
@@ -6154,22 +6154,22 @@
     <row r="180" ht="25" customHeight="1">
       <c r="A180" s="3" t="inlineStr">
         <is>
-          <t>Singh</t>
+          <t>Simpson</t>
         </is>
       </c>
       <c r="B180" s="3" t="inlineStr">
         <is>
-          <t>Niroshni</t>
+          <t>Beryl</t>
         </is>
       </c>
       <c r="C180" s="3" t="inlineStr">
         <is>
-          <t>East Coast</t>
+          <t>Cape Town</t>
         </is>
       </c>
       <c r="D180" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E180" s="3" t="inlineStr">
@@ -6179,29 +6179,29 @@
       </c>
       <c r="F180" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="181" ht="25" customHeight="1">
       <c r="A181" s="3" t="inlineStr">
         <is>
-          <t>Sircoulomb</t>
+          <t>Singh</t>
         </is>
       </c>
       <c r="B181" s="3" t="inlineStr">
         <is>
-          <t>Kenlis</t>
+          <t>Niroshni</t>
         </is>
       </c>
       <c r="C181" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>East Coast</t>
         </is>
       </c>
       <c r="D181" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E181" s="3" t="inlineStr">
@@ -6211,7 +6211,7 @@
       </c>
       <c r="F181" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -6223,7 +6223,7 @@
       </c>
       <c r="B182" s="3" t="inlineStr">
         <is>
-          <t>Holger</t>
+          <t>Kenlis</t>
         </is>
       </c>
       <c r="C182" s="3" t="inlineStr">
@@ -6238,7 +6238,7 @@
       </c>
       <c r="E182" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F182" s="3" t="inlineStr">
@@ -6250,12 +6250,12 @@
     <row r="183" ht="25" customHeight="1">
       <c r="A183" s="3" t="inlineStr">
         <is>
-          <t>Smeer</t>
+          <t>Sircoulomb</t>
         </is>
       </c>
       <c r="B183" s="3" t="inlineStr">
         <is>
-          <t>Hennie</t>
+          <t>Holger</t>
         </is>
       </c>
       <c r="C183" s="3" t="inlineStr">
@@ -6265,12 +6265,12 @@
       </c>
       <c r="D183" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E183" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F183" s="3" t="inlineStr">
@@ -6282,22 +6282,22 @@
     <row r="184" ht="25" customHeight="1">
       <c r="A184" s="3" t="inlineStr">
         <is>
-          <t>Smit</t>
+          <t>Smeer</t>
         </is>
       </c>
       <c r="B184" s="3" t="inlineStr">
         <is>
-          <t>Sue</t>
+          <t>Hennie</t>
         </is>
       </c>
       <c r="C184" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D184" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E184" s="3" t="inlineStr">
@@ -6307,7 +6307,7 @@
       </c>
       <c r="F184" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -6319,12 +6319,12 @@
       </c>
       <c r="B185" s="3" t="inlineStr">
         <is>
-          <t>Herman</t>
+          <t>Sue</t>
         </is>
       </c>
       <c r="C185" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D185" s="3" t="inlineStr">
@@ -6339,7 +6339,7 @@
       </c>
       <c r="F185" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -6351,17 +6351,17 @@
       </c>
       <c r="B186" s="3" t="inlineStr">
         <is>
-          <t>Juanita</t>
+          <t>Herman</t>
         </is>
       </c>
       <c r="C186" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D186" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E186" s="3" t="inlineStr">
@@ -6371,29 +6371,29 @@
       </c>
       <c r="F186" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="187" ht="25" customHeight="1">
       <c r="A187" s="3" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Smit</t>
         </is>
       </c>
       <c r="B187" s="3" t="inlineStr">
         <is>
-          <t>Jeff</t>
+          <t>Juanita</t>
         </is>
       </c>
       <c r="C187" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D187" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E187" s="3" t="inlineStr">
@@ -6415,12 +6415,12 @@
       </c>
       <c r="B188" s="3" t="inlineStr">
         <is>
-          <t>Bennie</t>
+          <t>Jeff</t>
         </is>
       </c>
       <c r="C188" s="3" t="inlineStr">
         <is>
-          <t>Wellington</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D188" s="3" t="inlineStr">
@@ -6430,12 +6430,12 @@
       </c>
       <c r="E188" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F188" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -6447,12 +6447,12 @@
       </c>
       <c r="B189" s="3" t="inlineStr">
         <is>
-          <t>Carmen Dolores</t>
+          <t>Bennie</t>
         </is>
       </c>
       <c r="C189" s="3" t="inlineStr">
         <is>
-          <t>Tokai</t>
+          <t>Wellington</t>
         </is>
       </c>
       <c r="D189" s="3" t="inlineStr">
@@ -6462,7 +6462,7 @@
       </c>
       <c r="E189" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F189" s="3" t="inlineStr">
@@ -6479,7 +6479,7 @@
       </c>
       <c r="B190" s="3" t="inlineStr">
         <is>
-          <t>David John</t>
+          <t>Carmen Dolores</t>
         </is>
       </c>
       <c r="C190" s="3" t="inlineStr">
@@ -6506,17 +6506,17 @@
     <row r="191" ht="25" customHeight="1">
       <c r="A191" s="3" t="inlineStr">
         <is>
-          <t>Sochen</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="B191" s="3" t="inlineStr">
         <is>
-          <t>Diana</t>
+          <t>David John</t>
         </is>
       </c>
       <c r="C191" s="3" t="inlineStr">
         <is>
-          <t>Sea Point</t>
+          <t>Tokai</t>
         </is>
       </c>
       <c r="D191" s="3" t="inlineStr">
@@ -6526,7 +6526,7 @@
       </c>
       <c r="E191" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F191" s="3" t="inlineStr">
@@ -6538,49 +6538,49 @@
     <row r="192" ht="25" customHeight="1">
       <c r="A192" s="3" t="inlineStr">
         <is>
-          <t>Steyn</t>
+          <t>Sochen</t>
         </is>
       </c>
       <c r="B192" s="3" t="inlineStr">
         <is>
-          <t>Elna</t>
+          <t>Diana</t>
         </is>
       </c>
       <c r="C192" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Sea Point</t>
         </is>
       </c>
       <c r="D192" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E192" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F192" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="193" ht="25" customHeight="1">
       <c r="A193" s="3" t="inlineStr">
         <is>
-          <t>Strauss</t>
+          <t>Steyn</t>
         </is>
       </c>
       <c r="B193" s="3" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>Elna</t>
         </is>
       </c>
       <c r="C193" s="3" t="inlineStr">
         <is>
-          <t>Kuilsriver</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D193" s="3" t="inlineStr">
@@ -6595,29 +6595,29 @@
       </c>
       <c r="F193" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="194" ht="25" customHeight="1">
       <c r="A194" s="3" t="inlineStr">
         <is>
-          <t>Strydom</t>
+          <t>Strauss</t>
         </is>
       </c>
       <c r="B194" s="3" t="inlineStr">
         <is>
-          <t>Melinda Lee</t>
+          <t>Patrick</t>
         </is>
       </c>
       <c r="C194" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Kuilsriver</t>
         </is>
       </c>
       <c r="D194" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E194" s="3" t="inlineStr">
@@ -6627,24 +6627,24 @@
       </c>
       <c r="F194" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="195" ht="25" customHeight="1">
       <c r="A195" s="3" t="inlineStr">
         <is>
-          <t>Sturges</t>
+          <t>Strydom</t>
         </is>
       </c>
       <c r="B195" s="3" t="inlineStr">
         <is>
-          <t>Trevor</t>
+          <t>Melinda Lee</t>
         </is>
       </c>
       <c r="C195" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D195" s="3" t="inlineStr">
@@ -6666,17 +6666,17 @@
     <row r="196" ht="25" customHeight="1">
       <c r="A196" s="3" t="inlineStr">
         <is>
-          <t>Talbot</t>
+          <t>Sturges</t>
         </is>
       </c>
       <c r="B196" s="3" t="inlineStr">
         <is>
-          <t>Lauryn</t>
+          <t>Trevor</t>
         </is>
       </c>
       <c r="C196" s="3" t="inlineStr">
         <is>
-          <t>Benoni Lakes</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D196" s="3" t="inlineStr">
@@ -6698,17 +6698,17 @@
     <row r="197" ht="25" customHeight="1">
       <c r="A197" s="3" t="inlineStr">
         <is>
-          <t>Theron</t>
+          <t>Talbot</t>
         </is>
       </c>
       <c r="B197" s="3" t="inlineStr">
         <is>
-          <t>Pierre</t>
+          <t>Lauryn</t>
         </is>
       </c>
       <c r="C197" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Benoni Lakes</t>
         </is>
       </c>
       <c r="D197" s="3" t="inlineStr">
@@ -6735,7 +6735,7 @@
       </c>
       <c r="B198" s="3" t="inlineStr">
         <is>
-          <t>Moira</t>
+          <t>Pierre</t>
         </is>
       </c>
       <c r="C198" s="3" t="inlineStr">
@@ -6762,17 +6762,17 @@
     <row r="199" ht="25" customHeight="1">
       <c r="A199" s="3" t="inlineStr">
         <is>
-          <t>Townsend</t>
+          <t>Theron</t>
         </is>
       </c>
       <c r="B199" s="3" t="inlineStr">
         <is>
-          <t>Diane</t>
+          <t>Moira</t>
         </is>
       </c>
       <c r="C199" s="3" t="inlineStr">
         <is>
-          <t>Benoni Lakes</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D199" s="3" t="inlineStr">
@@ -6782,7 +6782,7 @@
       </c>
       <c r="E199" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F199" s="3" t="inlineStr">
@@ -6794,27 +6794,27 @@
     <row r="200" ht="25" customHeight="1">
       <c r="A200" s="3" t="inlineStr">
         <is>
-          <t>Toye</t>
+          <t>Townsend</t>
         </is>
       </c>
       <c r="B200" s="3" t="inlineStr">
         <is>
-          <t>Omolayo</t>
+          <t>Diane</t>
         </is>
       </c>
       <c r="C200" s="3" t="inlineStr">
         <is>
-          <t>The Wilds</t>
+          <t>Benoni Lakes</t>
         </is>
       </c>
       <c r="D200" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E200" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F200" s="3" t="inlineStr">
@@ -6826,22 +6826,22 @@
     <row r="201" ht="25" customHeight="1">
       <c r="A201" s="3" t="inlineStr">
         <is>
-          <t>Tshikala</t>
+          <t>Toye</t>
         </is>
       </c>
       <c r="B201" s="3" t="inlineStr">
         <is>
-          <t>David Alex</t>
+          <t>Omolayo</t>
         </is>
       </c>
       <c r="C201" s="3" t="inlineStr">
         <is>
-          <t>Athlone</t>
+          <t>The Wilds</t>
         </is>
       </c>
       <c r="D201" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E201" s="3" t="inlineStr">
@@ -6851,24 +6851,24 @@
       </c>
       <c r="F201" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="202" ht="25" customHeight="1">
       <c r="A202" s="3" t="inlineStr">
         <is>
-          <t>Tuckett</t>
+          <t>Tshikala</t>
         </is>
       </c>
       <c r="B202" s="3" t="inlineStr">
         <is>
-          <t>Alistair</t>
+          <t>David Alex</t>
         </is>
       </c>
       <c r="C202" s="3" t="inlineStr">
         <is>
-          <t>Roodepoort Clearwater Cyber</t>
+          <t>Athlone</t>
         </is>
       </c>
       <c r="D202" s="3" t="inlineStr">
@@ -6883,7 +6883,7 @@
       </c>
       <c r="F202" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -6895,7 +6895,7 @@
       </c>
       <c r="B203" s="3" t="inlineStr">
         <is>
-          <t>Rowan</t>
+          <t>Alistair</t>
         </is>
       </c>
       <c r="C203" s="3" t="inlineStr">
@@ -6910,7 +6910,7 @@
       </c>
       <c r="E203" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F203" s="3" t="inlineStr">
@@ -6927,7 +6927,7 @@
       </c>
       <c r="B204" s="3" t="inlineStr">
         <is>
-          <t>Gail</t>
+          <t>Rowan</t>
         </is>
       </c>
       <c r="C204" s="3" t="inlineStr">
@@ -6942,7 +6942,7 @@
       </c>
       <c r="E204" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F204" s="3" t="inlineStr">
@@ -6954,17 +6954,17 @@
     <row r="205" ht="25" customHeight="1">
       <c r="A205" s="3" t="inlineStr">
         <is>
-          <t>VAN BREDA</t>
+          <t>Tuckett</t>
         </is>
       </c>
       <c r="B205" s="3" t="inlineStr">
         <is>
-          <t>HILARY LISE</t>
+          <t>Gail</t>
         </is>
       </c>
       <c r="C205" s="3" t="inlineStr">
         <is>
-          <t>Cape Town</t>
+          <t>Roodepoort Clearwater Cyber</t>
         </is>
       </c>
       <c r="D205" s="3" t="inlineStr">
@@ -6979,39 +6979,39 @@
       </c>
       <c r="F205" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="206" ht="25" customHeight="1">
       <c r="A206" s="3" t="inlineStr">
         <is>
-          <t>VAN DER MERWE</t>
+          <t>VAN BREDA</t>
         </is>
       </c>
       <c r="B206" s="3" t="inlineStr">
         <is>
-          <t>PATRICIA</t>
+          <t>HILARY LISE</t>
         </is>
       </c>
       <c r="C206" s="3" t="inlineStr">
         <is>
-          <t>East London Port Rex</t>
+          <t>Cape Town</t>
         </is>
       </c>
       <c r="D206" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E206" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F206" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -7023,17 +7023,17 @@
       </c>
       <c r="B207" s="3" t="inlineStr">
         <is>
-          <t>MARINA</t>
+          <t>PATRICIA</t>
         </is>
       </c>
       <c r="C207" s="3" t="inlineStr">
         <is>
-          <t>Malmesbury</t>
+          <t>East London Port Rex</t>
         </is>
       </c>
       <c r="D207" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E207" s="3" t="inlineStr">
@@ -7043,56 +7043,56 @@
       </c>
       <c r="F207" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="208" ht="25" customHeight="1">
       <c r="A208" s="3" t="inlineStr">
         <is>
-          <t>Valadao</t>
+          <t>VAN DER MERWE</t>
         </is>
       </c>
       <c r="B208" s="3" t="inlineStr">
         <is>
-          <t>Tracy</t>
+          <t>MARINA</t>
         </is>
       </c>
       <c r="C208" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Malmesbury</t>
         </is>
       </c>
       <c r="D208" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E208" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F208" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="209" ht="25" customHeight="1">
       <c r="A209" s="3" t="inlineStr">
         <is>
-          <t>Van Niekerk</t>
+          <t>Valadao</t>
         </is>
       </c>
       <c r="B209" s="3" t="inlineStr">
         <is>
-          <t>Riaan</t>
+          <t>Tracy</t>
         </is>
       </c>
       <c r="C209" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D209" s="3" t="inlineStr">
@@ -7114,22 +7114,22 @@
     <row r="210" ht="25" customHeight="1">
       <c r="A210" s="3" t="inlineStr">
         <is>
-          <t>Van Nieuwenhuyzen</t>
+          <t>Van Niekerk</t>
         </is>
       </c>
       <c r="B210" s="3" t="inlineStr">
         <is>
-          <t>Hilgardt</t>
+          <t>Riaan</t>
         </is>
       </c>
       <c r="C210" s="3" t="inlineStr">
         <is>
-          <t>Worcester</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D210" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E210" s="3" t="inlineStr">
@@ -7139,24 +7139,24 @@
       </c>
       <c r="F210" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="211" ht="25" customHeight="1">
       <c r="A211" s="3" t="inlineStr">
         <is>
-          <t>Van Rensburg</t>
+          <t>Van Nieuwenhuyzen</t>
         </is>
       </c>
       <c r="B211" s="3" t="inlineStr">
         <is>
-          <t>Neville</t>
+          <t>Hilgardt</t>
         </is>
       </c>
       <c r="C211" s="3" t="inlineStr">
         <is>
-          <t>Moorreesburg</t>
+          <t>Worcester</t>
         </is>
       </c>
       <c r="D211" s="3" t="inlineStr">
@@ -7166,7 +7166,7 @@
       </c>
       <c r="E211" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F211" s="3" t="inlineStr">
@@ -7178,27 +7178,27 @@
     <row r="212" ht="25" customHeight="1">
       <c r="A212" s="3" t="inlineStr">
         <is>
-          <t>Van Romburgh</t>
+          <t>Van Rensburg</t>
         </is>
       </c>
       <c r="B212" s="3" t="inlineStr">
         <is>
-          <t>Lorna</t>
+          <t>Neville</t>
         </is>
       </c>
       <c r="C212" s="3" t="inlineStr">
         <is>
-          <t>Fish Hoek</t>
+          <t>Moorreesburg</t>
         </is>
       </c>
       <c r="D212" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E212" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F212" s="3" t="inlineStr">
@@ -7210,17 +7210,17 @@
     <row r="213" ht="25" customHeight="1">
       <c r="A213" s="3" t="inlineStr">
         <is>
-          <t>Van Wyk-Nelson</t>
+          <t>Van Romburgh</t>
         </is>
       </c>
       <c r="B213" s="3" t="inlineStr">
         <is>
-          <t>Edith</t>
+          <t>Lorna</t>
         </is>
       </c>
       <c r="C213" s="3" t="inlineStr">
         <is>
-          <t>Kuilsriver</t>
+          <t>Fish Hoek</t>
         </is>
       </c>
       <c r="D213" s="3" t="inlineStr">
@@ -7242,17 +7242,17 @@
     <row r="214" ht="25" customHeight="1">
       <c r="A214" s="3" t="inlineStr">
         <is>
-          <t>Van Zyl</t>
+          <t>Van Wyk-Nelson</t>
         </is>
       </c>
       <c r="B214" s="3" t="inlineStr">
         <is>
-          <t>Louis</t>
+          <t>Edith</t>
         </is>
       </c>
       <c r="C214" s="3" t="inlineStr">
         <is>
-          <t>Centurion</t>
+          <t>Kuilsriver</t>
         </is>
       </c>
       <c r="D214" s="3" t="inlineStr">
@@ -7267,29 +7267,29 @@
       </c>
       <c r="F214" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="215" ht="25" customHeight="1">
       <c r="A215" s="3" t="inlineStr">
         <is>
-          <t>Van de Merwe</t>
+          <t>Van Zyl</t>
         </is>
       </c>
       <c r="B215" s="3" t="inlineStr">
         <is>
-          <t>Marina</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="C215" s="3" t="inlineStr">
         <is>
-          <t>Malmesbury</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="D215" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E215" s="3" t="inlineStr">
@@ -7299,29 +7299,29 @@
       </c>
       <c r="F215" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="216" ht="25" customHeight="1">
       <c r="A216" s="3" t="inlineStr">
         <is>
-          <t>Venter</t>
+          <t>Van de Merwe</t>
         </is>
       </c>
       <c r="B216" s="3" t="inlineStr">
         <is>
-          <t>Louis</t>
+          <t>Marina</t>
         </is>
       </c>
       <c r="C216" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Malmesbury</t>
         </is>
       </c>
       <c r="D216" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E216" s="3" t="inlineStr">
@@ -7331,34 +7331,34 @@
       </c>
       <c r="F216" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="217" ht="25" customHeight="1">
       <c r="A217" s="3" t="inlineStr">
         <is>
-          <t>Volker</t>
+          <t>Venter</t>
         </is>
       </c>
       <c r="B217" s="3" t="inlineStr">
         <is>
-          <t>Russell</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="C217" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D217" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E217" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F217" s="3" t="inlineStr">
@@ -7370,96 +7370,96 @@
     <row r="218" ht="25" customHeight="1">
       <c r="A218" s="3" t="inlineStr">
         <is>
-          <t>Von Mollendorf</t>
+          <t>Volker</t>
         </is>
       </c>
       <c r="B218" s="3" t="inlineStr">
         <is>
-          <t>Rinette</t>
+          <t>Russell</t>
         </is>
       </c>
       <c r="C218" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>King William's Town</t>
         </is>
       </c>
       <c r="D218" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E218" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F218" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="219" ht="25" customHeight="1">
       <c r="A219" s="3" t="inlineStr">
         <is>
-          <t>Warman</t>
+          <t>Von Mollendorf</t>
         </is>
       </c>
       <c r="B219" s="3" t="inlineStr">
         <is>
-          <t>Alastair</t>
+          <t>Rinette</t>
         </is>
       </c>
       <c r="C219" s="3" t="inlineStr">
         <is>
-          <t>Port Shepstone</t>
+          <t>Durbanville</t>
         </is>
       </c>
       <c r="D219" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E219" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F219" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="220" ht="25" customHeight="1">
       <c r="A220" s="3" t="inlineStr">
         <is>
-          <t>Watson</t>
+          <t>Warman</t>
         </is>
       </c>
       <c r="B220" s="3" t="inlineStr">
         <is>
-          <t>Allan</t>
+          <t>Alastair</t>
         </is>
       </c>
       <c r="C220" s="3" t="inlineStr">
         <is>
-          <t>Sea Point</t>
+          <t>Port Shepstone</t>
         </is>
       </c>
       <c r="D220" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E220" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F220" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -7471,22 +7471,22 @@
       </c>
       <c r="B221" s="3" t="inlineStr">
         <is>
-          <t>Alison</t>
+          <t>Allan</t>
         </is>
       </c>
       <c r="C221" s="3" t="inlineStr">
         <is>
-          <t>Sedgefield</t>
+          <t>Sea Point</t>
         </is>
       </c>
       <c r="D221" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E221" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F221" s="3" t="inlineStr">
@@ -7498,27 +7498,27 @@
     <row r="222" ht="25" customHeight="1">
       <c r="A222" s="3" t="inlineStr">
         <is>
-          <t>Williams</t>
+          <t>Watson</t>
         </is>
       </c>
       <c r="B222" s="3" t="inlineStr">
         <is>
-          <t>Johanna</t>
+          <t>Alison</t>
         </is>
       </c>
       <c r="C222" s="3" t="inlineStr">
         <is>
-          <t>Mitchells Plain</t>
+          <t>Sedgefield</t>
         </is>
       </c>
       <c r="D222" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E222" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F222" s="3" t="inlineStr">
@@ -7530,22 +7530,22 @@
     <row r="223" ht="25" customHeight="1">
       <c r="A223" s="3" t="inlineStr">
         <is>
-          <t>Wills</t>
+          <t>Williams</t>
         </is>
       </c>
       <c r="B223" s="3" t="inlineStr">
         <is>
-          <t>Geila</t>
+          <t>Johanna</t>
         </is>
       </c>
       <c r="C223" s="3" t="inlineStr">
         <is>
-          <t>Athlone</t>
+          <t>Mitchells Plain</t>
         </is>
       </c>
       <c r="D223" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E223" s="3" t="inlineStr">
@@ -7562,17 +7562,17 @@
     <row r="224" ht="25" customHeight="1">
       <c r="A224" s="3" t="inlineStr">
         <is>
-          <t>Wilter-Sturges</t>
+          <t>Wills</t>
         </is>
       </c>
       <c r="B224" s="3" t="inlineStr">
         <is>
-          <t>Meredith</t>
+          <t>Geila</t>
         </is>
       </c>
       <c r="C224" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Athlone</t>
         </is>
       </c>
       <c r="D224" s="3" t="inlineStr">
@@ -7587,24 +7587,24 @@
       </c>
       <c r="F224" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="225" ht="25" customHeight="1">
       <c r="A225" s="3" t="inlineStr">
         <is>
-          <t>Wright</t>
+          <t>Wilter-Sturges</t>
         </is>
       </c>
       <c r="B225" s="3" t="inlineStr">
         <is>
-          <t>Rocky</t>
+          <t>Meredith</t>
         </is>
       </c>
       <c r="C225" s="3" t="inlineStr">
         <is>
-          <t>Table View</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D225" s="3" t="inlineStr">
@@ -7614,29 +7614,29 @@
       </c>
       <c r="E225" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F225" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="226" ht="25" customHeight="1">
       <c r="A226" s="3" t="inlineStr">
         <is>
-          <t>Young</t>
+          <t>Wright</t>
         </is>
       </c>
       <c r="B226" s="3" t="inlineStr">
         <is>
-          <t>Judy</t>
+          <t>Rocky</t>
         </is>
       </c>
       <c r="C226" s="3" t="inlineStr">
         <is>
-          <t>Durbanville</t>
+          <t>Table View</t>
         </is>
       </c>
       <c r="D226" s="3" t="inlineStr">
@@ -7646,7 +7646,7 @@
       </c>
       <c r="E226" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F226" s="3" t="inlineStr">
@@ -7658,17 +7658,17 @@
     <row r="227" ht="25" customHeight="1">
       <c r="A227" s="3" t="inlineStr">
         <is>
-          <t>de Kock</t>
+          <t>Young</t>
         </is>
       </c>
       <c r="B227" s="3" t="inlineStr">
         <is>
-          <t>Engela</t>
+          <t>Judy</t>
         </is>
       </c>
       <c r="C227" s="3" t="inlineStr">
         <is>
-          <t>Swellendam</t>
+          <t>Durbanville</t>
         </is>
       </c>
       <c r="D227" s="3" t="inlineStr">
@@ -7678,7 +7678,7 @@
       </c>
       <c r="E227" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F227" s="3" t="inlineStr">
@@ -7695,7 +7695,7 @@
       </c>
       <c r="B228" s="3" t="inlineStr">
         <is>
-          <t>Francois</t>
+          <t>Engela</t>
         </is>
       </c>
       <c r="C228" s="3" t="inlineStr">
@@ -7722,59 +7722,59 @@
     <row r="229" ht="25" customHeight="1">
       <c r="A229" s="3" t="inlineStr">
         <is>
-          <t>de Silva</t>
+          <t>de Kock</t>
         </is>
       </c>
       <c r="B229" s="3" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Francois</t>
         </is>
       </c>
       <c r="C229" s="3" t="inlineStr">
         <is>
-          <t>Edenvale</t>
+          <t>Swellendam</t>
         </is>
       </c>
       <c r="D229" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E229" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F229" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="230" ht="25" customHeight="1">
       <c r="A230" s="3" t="inlineStr">
         <is>
-          <t>du Plooy</t>
+          <t>de Silva</t>
         </is>
       </c>
       <c r="B230" s="3" t="inlineStr">
         <is>
-          <t>Tammy</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="C230" s="3" t="inlineStr">
         <is>
-          <t>Alberton</t>
+          <t>Edenvale</t>
         </is>
       </c>
       <c r="D230" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E230" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F230" s="3" t="inlineStr">
@@ -7791,7 +7791,7 @@
       </c>
       <c r="B231" s="3" t="inlineStr">
         <is>
-          <t>Marc</t>
+          <t>Tammy</t>
         </is>
       </c>
       <c r="C231" s="3" t="inlineStr">
@@ -7818,17 +7818,17 @@
     <row r="232" ht="25" customHeight="1">
       <c r="A232" s="3" t="inlineStr">
         <is>
-          <t>du Toit</t>
+          <t>du Plooy</t>
         </is>
       </c>
       <c r="B232" s="3" t="inlineStr">
         <is>
-          <t>Desiree</t>
+          <t>Marc</t>
         </is>
       </c>
       <c r="C232" s="3" t="inlineStr">
         <is>
-          <t>Ramsgate</t>
+          <t>Alberton</t>
         </is>
       </c>
       <c r="D232" s="3" t="inlineStr">
@@ -7850,22 +7850,22 @@
     <row r="233" ht="25" customHeight="1">
       <c r="A233" s="3" t="inlineStr">
         <is>
-          <t>stier</t>
+          <t>du Toit</t>
         </is>
       </c>
       <c r="B233" s="3" t="inlineStr">
         <is>
-          <t>RORY</t>
+          <t>Desiree</t>
         </is>
       </c>
       <c r="C233" s="3" t="inlineStr">
         <is>
-          <t>Deep South</t>
+          <t>Ramsgate</t>
         </is>
       </c>
       <c r="D233" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E233" s="3" t="inlineStr">
@@ -7875,56 +7875,56 @@
       </c>
       <c r="F233" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="234" ht="25" customHeight="1">
       <c r="A234" s="3" t="inlineStr">
         <is>
-          <t>tyler</t>
+          <t>stier</t>
         </is>
       </c>
       <c r="B234" s="3" t="inlineStr">
         <is>
-          <t>natascha</t>
+          <t>RORY</t>
         </is>
       </c>
       <c r="C234" s="3" t="inlineStr">
         <is>
-          <t>Kensington</t>
+          <t>Deep South</t>
         </is>
       </c>
       <c r="D234" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E234" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F234" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="235" ht="25" customHeight="1">
       <c r="A235" s="3" t="inlineStr">
         <is>
-          <t>van Blerk</t>
+          <t>tyler</t>
         </is>
       </c>
       <c r="B235" s="3" t="inlineStr">
         <is>
-          <t>Carl</t>
+          <t>natascha</t>
         </is>
       </c>
       <c r="C235" s="3" t="inlineStr">
         <is>
-          <t>Eden</t>
+          <t>Kensington</t>
         </is>
       </c>
       <c r="D235" s="3" t="inlineStr">
@@ -7939,24 +7939,24 @@
       </c>
       <c r="F235" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="236" ht="25" customHeight="1">
       <c r="A236" s="3" t="inlineStr">
         <is>
-          <t>van Heerden</t>
+          <t>van Blerk</t>
         </is>
       </c>
       <c r="B236" s="3" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Carl</t>
         </is>
       </c>
       <c r="C236" s="3" t="inlineStr">
         <is>
-          <t>Wilro Park</t>
+          <t>Eden</t>
         </is>
       </c>
       <c r="D236" s="3" t="inlineStr">
@@ -7971,7 +7971,7 @@
       </c>
       <c r="F236" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -7983,7 +7983,7 @@
       </c>
       <c r="B237" s="3" t="inlineStr">
         <is>
-          <t>Sandy</t>
+          <t>Sydney</t>
         </is>
       </c>
       <c r="C237" s="3" t="inlineStr">
@@ -7998,7 +7998,7 @@
       </c>
       <c r="E237" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F237" s="3" t="inlineStr">
@@ -8015,17 +8015,17 @@
       </c>
       <c r="B238" s="3" t="inlineStr">
         <is>
-          <t>Craig</t>
+          <t>Sandy</t>
         </is>
       </c>
       <c r="C238" s="3" t="inlineStr">
         <is>
-          <t>East London Beacon Bay</t>
+          <t>Wilro Park</t>
         </is>
       </c>
       <c r="D238" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E238" s="3" t="inlineStr">
@@ -8047,17 +8047,17 @@
       </c>
       <c r="B239" s="3" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Craig</t>
         </is>
       </c>
       <c r="C239" s="3" t="inlineStr">
         <is>
-          <t>Pretoria South</t>
+          <t>East London Beacon Bay</t>
         </is>
       </c>
       <c r="D239" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E239" s="3" t="inlineStr">
@@ -8074,17 +8074,17 @@
     <row r="240" ht="25" customHeight="1">
       <c r="A240" s="3" t="inlineStr">
         <is>
-          <t>van Rensburg</t>
+          <t>van Heerden</t>
         </is>
       </c>
       <c r="B240" s="3" t="inlineStr">
         <is>
-          <t>Johan</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C240" s="3" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Pretoria South</t>
         </is>
       </c>
       <c r="D240" s="3" t="inlineStr">
@@ -8094,12 +8094,12 @@
       </c>
       <c r="E240" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F240" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
@@ -8111,7 +8111,7 @@
       </c>
       <c r="B241" s="3" t="inlineStr">
         <is>
-          <t>Anne</t>
+          <t>Johan</t>
         </is>
       </c>
       <c r="C241" s="3" t="inlineStr">
@@ -8138,17 +8138,17 @@
     <row r="242" ht="25" customHeight="1">
       <c r="A242" s="3" t="inlineStr">
         <is>
-          <t>van Wulven</t>
+          <t>van Rensburg</t>
         </is>
       </c>
       <c r="B242" s="3" t="inlineStr">
         <is>
-          <t>Jeannie</t>
+          <t>Anne</t>
         </is>
       </c>
       <c r="C242" s="3" t="inlineStr">
         <is>
-          <t>Tygerberg Hills</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="D242" s="3" t="inlineStr">
@@ -8158,7 +8158,7 @@
       </c>
       <c r="E242" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F242" s="3" t="inlineStr">
@@ -8175,7 +8175,7 @@
       </c>
       <c r="B243" s="3" t="inlineStr">
         <is>
-          <t>Alan</t>
+          <t>Jeannie</t>
         </is>
       </c>
       <c r="C243" s="3" t="inlineStr">
@@ -8190,7 +8190,7 @@
       </c>
       <c r="E243" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F243" s="3" t="inlineStr">
@@ -8207,7 +8207,7 @@
       </c>
       <c r="B244" s="3" t="inlineStr">
         <is>
-          <t>Deon</t>
+          <t>Alan</t>
         </is>
       </c>
       <c r="C244" s="3" t="inlineStr">
@@ -8234,17 +8234,17 @@
     <row r="245" ht="25" customHeight="1">
       <c r="A245" s="3" t="inlineStr">
         <is>
-          <t>van Wyk</t>
+          <t>van Wulven</t>
         </is>
       </c>
       <c r="B245" s="3" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>Deon</t>
         </is>
       </c>
       <c r="C245" s="3" t="inlineStr">
         <is>
-          <t>North Durban</t>
+          <t>Tygerberg Hills</t>
         </is>
       </c>
       <c r="D245" s="3" t="inlineStr">
@@ -8259,7 +8259,7 @@
       </c>
       <c r="F245" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
@@ -8271,12 +8271,12 @@
       </c>
       <c r="B246" s="3" t="inlineStr">
         <is>
-          <t>Lindie</t>
+          <t>Kim</t>
         </is>
       </c>
       <c r="C246" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>North Durban</t>
         </is>
       </c>
       <c r="D246" s="3" t="inlineStr">
@@ -8303,12 +8303,12 @@
       </c>
       <c r="B247" s="3" t="inlineStr">
         <is>
-          <t>Willem</t>
+          <t>Lindie</t>
         </is>
       </c>
       <c r="C247" s="3" t="inlineStr">
         <is>
-          <t>Midrand</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D247" s="3" t="inlineStr">
@@ -8335,12 +8335,12 @@
       </c>
       <c r="B248" s="3" t="inlineStr">
         <is>
-          <t>Patricia</t>
+          <t>Willem</t>
         </is>
       </c>
       <c r="C248" s="3" t="inlineStr">
         <is>
-          <t>Pretoria Jakaranda</t>
+          <t>Midrand</t>
         </is>
       </c>
       <c r="D248" s="3" t="inlineStr">
@@ -8362,22 +8362,22 @@
     <row r="249" ht="25" customHeight="1">
       <c r="A249" s="3" t="inlineStr">
         <is>
-          <t>van der Merwe</t>
+          <t>van Wyk</t>
         </is>
       </c>
       <c r="B249" s="3" t="inlineStr">
         <is>
-          <t>Ingrid</t>
+          <t>Patricia</t>
         </is>
       </c>
       <c r="C249" s="3" t="inlineStr">
         <is>
-          <t>Letaba Tzaneen</t>
+          <t>Pretoria Jakaranda</t>
         </is>
       </c>
       <c r="D249" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E249" s="3" t="inlineStr">
@@ -8394,49 +8394,49 @@
     <row r="250" ht="25" customHeight="1">
       <c r="A250" s="3" t="inlineStr">
         <is>
-          <t>van der Westhuizen</t>
+          <t>van der Merwe</t>
         </is>
       </c>
       <c r="B250" s="3" t="inlineStr">
         <is>
-          <t>Hennie</t>
+          <t>Ingrid</t>
         </is>
       </c>
       <c r="C250" s="3" t="inlineStr">
         <is>
-          <t>Helderberg</t>
+          <t>Letaba Tzaneen</t>
         </is>
       </c>
       <c r="D250" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E250" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F250" s="3" t="inlineStr">
         <is>
-          <t>410W</t>
+          <t>410E</t>
         </is>
       </c>
     </row>
     <row r="251" ht="25" customHeight="1">
       <c r="A251" s="3" t="inlineStr">
         <is>
-          <t>von der Decken</t>
+          <t>van der Westhuizen</t>
         </is>
       </c>
       <c r="B251" s="3" t="inlineStr">
         <is>
-          <t>Brian</t>
+          <t>Hennie</t>
         </is>
       </c>
       <c r="C251" s="3" t="inlineStr">
         <is>
-          <t>King William's Town</t>
+          <t>Helderberg</t>
         </is>
       </c>
       <c r="D251" s="3" t="inlineStr">
@@ -8451,51 +8451,83 @@
       </c>
       <c r="F251" s="3" t="inlineStr">
         <is>
-          <t>410E</t>
+          <t>410W</t>
         </is>
       </c>
     </row>
     <row r="252" ht="25" customHeight="1">
       <c r="A252" s="3" t="inlineStr">
         <is>
+          <t>von der Decken</t>
+        </is>
+      </c>
+      <c r="B252" s="3" t="inlineStr">
+        <is>
+          <t>Brian</t>
+        </is>
+      </c>
+      <c r="C252" s="3" t="inlineStr">
+        <is>
+          <t>King William's Town</t>
+        </is>
+      </c>
+      <c r="D252" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E252" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F252" s="3" t="inlineStr">
+        <is>
+          <t>410E</t>
+        </is>
+      </c>
+    </row>
+    <row r="253" ht="25" customHeight="1">
+      <c r="A253" s="3" t="inlineStr">
+        <is>
           <t>‘t Hart</t>
         </is>
       </c>
-      <c r="B252" s="3" t="inlineStr">
+      <c r="B253" s="3" t="inlineStr">
         <is>
           <t>Michelle</t>
         </is>
       </c>
-      <c r="C252" s="3" t="inlineStr">
+      <c r="C253" s="3" t="inlineStr">
         <is>
           <t>Benoni Lakes</t>
         </is>
       </c>
-      <c r="D252" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E252" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F252" s="3" t="inlineStr">
+      <c r="D253" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E253" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F253" s="3" t="inlineStr">
         <is>
           <t>410E</t>
-        </is>
-      </c>
-    </row>
-    <row r="253">
-      <c r="A253" s="1" t="inlineStr">
-        <is>
-          <t>Number of attendees: 250</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="inlineStr">
+        <is>
+          <t>Number of attendees: 251</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" s="1" t="inlineStr">
         <is>
           <t>Number of voters: 98</t>
         </is>
@@ -8531,7 +8563,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Registrees as of 01/05/2021 07:39</t>
+          <t>410E Registrees as of 01/05/2021 08:09</t>
         </is>
       </c>
     </row>
@@ -12143,7 +12175,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Registrees as of 01/05/2021 07:39</t>
+          <t>410W Registrees as of 01/05/2021 08:09</t>
         </is>
       </c>
     </row>
@@ -16319,7 +16351,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410E Voting details as of 01/05/2021 07:39</t>
+          <t>410E Voting details as of 01/05/2021 08:09</t>
         </is>
       </c>
     </row>
@@ -16696,7 +16728,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>410W Voting details as of 01/05/2021 07:39</t>
+          <t>410W Voting details as of 01/05/2021 08:09</t>
         </is>
       </c>
     </row>

</xml_diff>